<commit_message>
add CAD models: det-objective holders, filter wheel
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop-v2\parts-list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF99F25-5E86-4792-9550-6C6CB620D5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D1D7E8-FFF3-4DD5-9CE9-4B4E09C1DBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2171,8 +2171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C138" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
create galvo mount for 15-mm galvos Thorlabs QS15
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24450412-BA24-4F87-950D-8E9FAB90CF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E62078-DB90-4189-A3BE-15EEE8007E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="3444" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -671,43 +671,7 @@
     <t>Portmann Instruments</t>
   </si>
   <si>
-    <t>UQ-205-H80 10x20x80</t>
-  </si>
-  <si>
     <t>Whole-Mouse CNS Cuvettes</t>
-  </si>
-  <si>
-    <t>UQ-753-H100 40x40x100</t>
-  </si>
-  <si>
-    <t>UQ-205-H120 10x20x120</t>
-  </si>
-  <si>
-    <t>UQ-753-H120 40x40x120</t>
-  </si>
-  <si>
-    <t>UQ-751 20x20 mm</t>
-  </si>
-  <si>
-    <t>UQ-752 30x30</t>
-  </si>
-  <si>
-    <t>UQ-753 40x40</t>
-  </si>
-  <si>
-    <t>UQ-754 50x50</t>
-  </si>
-  <si>
-    <t>UQ-203 5x10x45</t>
-  </si>
-  <si>
-    <t>UQ-204 10x10x45</t>
-  </si>
-  <si>
-    <t>UQ-205 10x20x45</t>
-  </si>
-  <si>
-    <t>Standard cuvette for mouse brains &amp; CLARITY</t>
   </si>
   <si>
     <t>SUM</t>
@@ -1392,6 +1356,42 @@
   </si>
   <si>
     <t>Todo: Adapt the code and test this option.</t>
+  </si>
+  <si>
+    <t>UG-205-H80 10x20x80</t>
+  </si>
+  <si>
+    <t>UG-753-H100 40x40x100</t>
+  </si>
+  <si>
+    <t>UG-205-H120 10x20x120</t>
+  </si>
+  <si>
+    <t>UG-753-H120 40x40x120</t>
+  </si>
+  <si>
+    <t>UG-751 20x20 mm</t>
+  </si>
+  <si>
+    <t>UG-752 30x30</t>
+  </si>
+  <si>
+    <t>UG-753 40x40</t>
+  </si>
+  <si>
+    <t>UG-754 50x50</t>
+  </si>
+  <si>
+    <t>UG-203 5x10x45</t>
+  </si>
+  <si>
+    <t>UG-204 10x10x45</t>
+  </si>
+  <si>
+    <t>UG-205 10x20x45</t>
+  </si>
+  <si>
+    <t>Material: glass, RI=1.52. For quartz  (e.g. CLARITY imaging, RI=1.47), replace UG qwith UQ in the part name.</t>
   </si>
 </sst>
 </file>
@@ -2107,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B207" sqref="B207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,18 +2184,18 @@
         <v>12350</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="27" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="D5" s="27">
         <v>0</v>
@@ -2210,7 +2210,7 @@
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
       <c r="I5" s="27" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2221,24 +2221,24 @@
     </row>
     <row r="7" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
@@ -2254,7 +2254,7 @@
         <v>46</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="38" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -2262,7 +2262,7 @@
         <v>1008062</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C10" s="38" t="s">
         <v>16</v>
@@ -2279,15 +2279,15 @@
       </c>
       <c r="G10" s="53"/>
       <c r="I10" s="38" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="38" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="D11" s="38">
         <v>0</v>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="G11" s="53"/>
       <c r="I11" s="38" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2332,10 +2332,10 @@
         <v>5254</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2359,7 +2359,7 @@
         <v>520</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2383,10 +2383,10 @@
         <v>1807</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="I15" s="41" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2410,7 +2410,7 @@
         <v>132</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="H16" s="41" t="s">
         <v>13</v>
@@ -2437,10 +2437,10 @@
         <v>250</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="I17" s="41" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2464,13 +2464,13 @@
         <v>1807</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="H18" s="41" t="s">
         <v>13</v>
       </c>
       <c r="I18" s="41" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2494,10 +2494,10 @@
         <v>200</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="I19" s="41" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2521,10 +2521,10 @@
         <v>1939</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="I20" s="41" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2548,10 +2548,10 @@
         <v>110</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2575,10 +2575,10 @@
         <v>2450</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2589,7 +2589,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
@@ -2602,10 +2602,10 @@
         <v>4800</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2629,28 +2629,28 @@
         <v>870</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>84</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="D26" s="3">
         <v>2</v>
@@ -2663,21 +2663,21 @@
         <v>140</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>84</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="D27" s="3">
         <v>6</v>
@@ -2690,21 +2690,21 @@
         <v>216</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="54" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>84</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
@@ -2717,21 +2717,21 @@
         <v>43</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="54" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>84</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="D29" s="3">
         <v>1</v>
@@ -2744,21 +2744,21 @@
         <v>29</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="54" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -2771,21 +2771,21 @@
         <v>195</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="54" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
@@ -2798,7 +2798,7 @@
         <v>10</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="15" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2810,7 +2810,7 @@
     </row>
     <row r="33" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="36" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
@@ -2923,13 +2923,13 @@
     </row>
     <row r="40" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="42" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="B40" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C40" s="42" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="D40" s="41">
         <v>2</v>
@@ -2947,13 +2947,13 @@
     </row>
     <row r="41" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="42" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="B41" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C41" s="42" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="D41" s="41">
         <v>2</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>53</v>
@@ -3019,7 +3019,7 @@
         <v>46</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>57</v>
@@ -3027,13 +3027,13 @@
     </row>
     <row r="44" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="47" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="B44" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C44" s="47" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="D44" s="48">
         <v>0</v>
@@ -3049,10 +3049,10 @@
         <v>46</v>
       </c>
       <c r="H44" s="48" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="I44" s="48" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -3063,7 +3063,7 @@
         <v>84</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="D45" s="41">
         <v>2</v>
@@ -3076,21 +3076,21 @@
         <v>62</v>
       </c>
       <c r="H45" s="41" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="I45" s="41" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="B46" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D46" s="45">
         <v>10</v>
@@ -3103,21 +3103,21 @@
         <v>160</v>
       </c>
       <c r="H46" s="45" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="I46" s="45" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="B47" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="D47" s="45">
         <v>4</v>
@@ -3130,21 +3130,21 @@
         <v>164</v>
       </c>
       <c r="H47" s="45" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="I47" s="45" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="42" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="B48" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C48" s="42" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="D48" s="41">
         <v>2</v>
@@ -3157,21 +3157,21 @@
         <v>198</v>
       </c>
       <c r="H48" s="41" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="I48" s="41" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="B49" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="D49" s="45">
         <v>6</v>
@@ -3184,21 +3184,21 @@
         <v>1134</v>
       </c>
       <c r="H49" s="45" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="I49" s="45" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="44" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="B50" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="D50" s="45">
         <v>6</v>
@@ -3211,21 +3211,21 @@
         <v>660</v>
       </c>
       <c r="H50" s="45" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="I50" s="45" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="42" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="B51" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C51" s="42" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="D51" s="41">
         <v>4</v>
@@ -3238,21 +3238,21 @@
         <v>52</v>
       </c>
       <c r="H51" s="41" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="I51" s="41" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="42" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="B52" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C52" s="42" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="D52" s="41">
         <v>2</v>
@@ -3265,18 +3265,18 @@
         <v>16</v>
       </c>
       <c r="H52" s="41" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="42" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="B53" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C53" s="42" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="D53" s="41">
         <v>4</v>
@@ -3289,21 +3289,21 @@
         <v>28</v>
       </c>
       <c r="H53" s="41" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="I53" s="41" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="42" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="B54" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="D54" s="41">
         <v>6</v>
@@ -3316,21 +3316,21 @@
         <v>30</v>
       </c>
       <c r="H54" s="41" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="I54" s="41" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="42" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="B55" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C55" s="42" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="D55" s="41">
         <v>4</v>
@@ -3343,21 +3343,21 @@
         <v>24</v>
       </c>
       <c r="H55" s="41" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="I55" s="41" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="42" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="B56" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C56" s="42" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="D56" s="41">
         <v>4</v>
@@ -3370,21 +3370,21 @@
         <v>20</v>
       </c>
       <c r="H56" s="41" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="I56" s="41" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="42" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="B57" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C57" s="42" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D57" s="41">
         <v>2</v>
@@ -3397,18 +3397,18 @@
         <v>10</v>
       </c>
       <c r="H57" s="41" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="44" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="B58" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C58" s="44" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="D58" s="45">
         <v>2</v>
@@ -3421,21 +3421,21 @@
         <v>796</v>
       </c>
       <c r="H58" s="45" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="I58" s="45" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="44" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="B59" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C59" s="44" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="D59" s="45">
         <v>2</v>
@@ -3448,21 +3448,21 @@
         <v>52</v>
       </c>
       <c r="H59" s="45" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="I59" s="45" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="44" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="B60" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C60" s="44" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="D60" s="45">
         <v>2</v>
@@ -3475,21 +3475,21 @@
         <v>60</v>
       </c>
       <c r="H60" s="45" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="I60" s="45" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="42" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="B61" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C61" s="42" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="D61" s="41">
         <v>2</v>
@@ -3502,15 +3502,15 @@
         <v>72</v>
       </c>
       <c r="H61" s="41" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="I61" s="50" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="71" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="C62" s="42"/>
       <c r="E62" s="43"/>
@@ -3519,13 +3519,13 @@
     </row>
     <row r="63" spans="1:9" s="62" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="61" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="B63" s="62" t="s">
         <v>84</v>
       </c>
       <c r="C63" s="61" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="D63" s="62">
         <v>2</v>
@@ -3538,10 +3538,10 @@
         <v>3514</v>
       </c>
       <c r="H63" s="62" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="I63" s="65" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="62" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3550,18 +3550,18 @@
       <c r="E64" s="63"/>
       <c r="F64" s="64"/>
       <c r="I64" s="65" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
     </row>
     <row r="65" spans="1:10" s="62" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="61" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="B65" s="62" t="s">
         <v>84</v>
       </c>
       <c r="C65" s="61" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="D65" s="62">
         <v>2</v>
@@ -3574,19 +3574,19 @@
         <v>118</v>
       </c>
       <c r="H65" s="62" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="I65" s="65"/>
     </row>
     <row r="66" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="61" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="B66" s="62" t="s">
         <v>84</v>
       </c>
       <c r="C66" s="61" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="D66" s="62">
         <v>1</v>
@@ -3599,15 +3599,15 @@
         <v>495</v>
       </c>
       <c r="H66" s="62" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="I66" s="62" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
     </row>
     <row r="67" spans="1:10" s="67" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="70" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="C67" s="66"/>
       <c r="E67" s="68"/>
@@ -3615,13 +3615,13 @@
     </row>
     <row r="68" spans="1:10" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="66" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="B68" s="67" t="s">
         <v>84</v>
       </c>
       <c r="C68" s="66" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="D68" s="67">
         <v>2</v>
@@ -3634,21 +3634,21 @@
         <v>4208</v>
       </c>
       <c r="H68" s="67" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="I68" s="67" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
     </row>
     <row r="69" spans="1:10" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="66" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="B69" s="67" t="s">
         <v>84</v>
       </c>
       <c r="C69" s="66" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="D69" s="67">
         <v>2</v>
@@ -3661,18 +3661,18 @@
         <v>164</v>
       </c>
       <c r="H69" s="67" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
     </row>
     <row r="70" spans="1:10" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="66" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="B70" s="67" t="s">
         <v>84</v>
       </c>
       <c r="C70" s="66" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="D70" s="67">
         <v>1</v>
@@ -3685,21 +3685,21 @@
         <v>390</v>
       </c>
       <c r="H70" s="67" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="I70" s="67" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="42" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="B71" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="D71" s="41">
         <v>2</v>
@@ -3712,18 +3712,18 @@
         <v>50</v>
       </c>
       <c r="H71" s="41" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
     </row>
     <row r="72" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="51" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="B72" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="D72" s="41">
         <v>2</v>
@@ -3736,24 +3736,24 @@
         <v>70</v>
       </c>
       <c r="H72" s="41" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="I72" s="50" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="J72" s="52" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
     </row>
     <row r="73" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="42" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="B73" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="D73" s="41">
         <v>2</v>
@@ -3766,29 +3766,29 @@
         <v>184</v>
       </c>
       <c r="H73" s="41" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="I73" s="41" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
     </row>
     <row r="74" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="42" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="B74" s="41" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="C74" s="60" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="E74" s="43"/>
       <c r="F74" s="55"/>
       <c r="H74" s="41" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="I74" s="41" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
     </row>
     <row r="75" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -3811,7 +3811,7 @@
     </row>
     <row r="78" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
@@ -3832,18 +3832,18 @@
       <c r="E79" s="43"/>
       <c r="F79" s="55"/>
       <c r="I79" s="41" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
     </row>
     <row r="80" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="42" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="B80" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C80" s="42" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="D80" s="41">
         <v>1</v>
@@ -3858,13 +3858,13 @@
     </row>
     <row r="81" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="51" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="B81" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C81" s="42" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="D81" s="41">
         <v>2</v>
@@ -3879,13 +3879,13 @@
     </row>
     <row r="82" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="42" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="B82" s="41" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="C82" s="42" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="D82" s="41">
         <v>1</v>
@@ -3898,7 +3898,7 @@
         <v>10</v>
       </c>
       <c r="I82" s="41" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
     </row>
     <row r="83" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -3917,36 +3917,36 @@
       <c r="E83" s="43"/>
       <c r="F83" s="55"/>
       <c r="I83" s="41" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
     </row>
     <row r="84" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
     </row>
     <row r="85" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="E85" s="9"/>
       <c r="F85" s="9"/>
     </row>
     <row r="86" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
     </row>
     <row r="87" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>14</v>
@@ -3971,13 +3971,13 @@
     </row>
     <row r="88" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="D88" s="3">
         <v>1</v>
@@ -3999,13 +3999,13 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="D89" s="3">
         <v>1</v>
@@ -4026,47 +4026,47 @@
     </row>
     <row r="90" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="D90" s="3">
         <v>1</v>
       </c>
       <c r="I90" s="41" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
     </row>
     <row r="91" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="C91" s="72" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
     </row>
     <row r="92" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
     </row>
     <row r="93" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="42" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="B93" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="D93" s="41">
         <v>0</v>
@@ -4082,13 +4082,13 @@
     </row>
     <row r="94" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="42" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="B94" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C94" s="42" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="D94" s="41">
         <v>0</v>
@@ -4103,13 +4103,13 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="B95" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="D95" s="3">
         <v>0</v>
@@ -4124,13 +4124,13 @@
     </row>
     <row r="96" spans="1:10" s="22" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="23" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F96" s="58"/>
     </row>
     <row r="97" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="22" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="F97" s="58"/>
     </row>
@@ -4158,7 +4158,7 @@
         <v>13</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4185,7 +4185,7 @@
         <v>13</v>
       </c>
       <c r="I99" s="38" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4212,7 +4212,7 @@
         <v>13</v>
       </c>
       <c r="I100" s="38" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4239,7 +4239,7 @@
         <v>13</v>
       </c>
       <c r="I101" s="38" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4266,7 +4266,7 @@
         <v>13</v>
       </c>
       <c r="I102" s="38" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
     </row>
     <row r="103" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -4293,25 +4293,25 @@
         <v>13</v>
       </c>
       <c r="I103" s="38" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="30" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A104" s="29" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="E104" s="31"/>
       <c r="F104" s="31"/>
     </row>
     <row r="105" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="34" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="B105" s="32" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="C105" s="36" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D105" s="32">
         <v>1</v>
@@ -4327,10 +4327,10 @@
         <v>13</v>
       </c>
       <c r="H105" s="32" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="I105" s="32" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -4338,10 +4338,10 @@
         <v>11454</v>
       </c>
       <c r="B106" s="32" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="D106" s="3">
         <v>0</v>
@@ -4357,10 +4357,10 @@
         <v>13</v>
       </c>
       <c r="H106" s="32" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -4368,10 +4368,10 @@
         <v>11044</v>
       </c>
       <c r="B107" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="C107" s="37" t="s">
         <v>249</v>
-      </c>
-      <c r="C107" s="37" t="s">
-        <v>261</v>
       </c>
       <c r="D107" s="3">
         <v>0</v>
@@ -4387,21 +4387,21 @@
         <v>13</v>
       </c>
       <c r="H107" s="32" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B108" s="32" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="C108" s="37" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="D108" s="3">
         <v>0</v>
@@ -4417,21 +4417,21 @@
         <v>13</v>
       </c>
       <c r="H108" s="32" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="B109" s="32" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="C109" s="37" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="D109" s="3">
         <v>0</v>
@@ -4447,12 +4447,12 @@
         <v>13</v>
       </c>
       <c r="H109" s="32" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="30" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A110" s="29" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="E110" s="31"/>
       <c r="F110" s="31"/>
@@ -4536,18 +4536,18 @@
         <v>73</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="D130" s="3">
         <v>1</v>
@@ -4563,18 +4563,18 @@
         <v>73</v>
       </c>
       <c r="I130" s="3" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="D131" s="3">
         <v>1</v>
@@ -4590,18 +4590,18 @@
         <v>73</v>
       </c>
       <c r="I131" s="3" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="D132" s="3">
         <v>1</v>
@@ -4617,7 +4617,7 @@
         <v>73</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -4628,7 +4628,7 @@
         <v>72</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="D133" s="3">
         <v>1</v>
@@ -4670,13 +4670,13 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="D135" s="3">
         <v>1</v>
@@ -4716,15 +4716,15 @@
         <v>73</v>
       </c>
       <c r="I136" s="38" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
     </row>
     <row r="137" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="38" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="B137" s="38" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="C137" s="38" t="s">
         <v>81</v>
@@ -4743,7 +4743,7 @@
         <v>73</v>
       </c>
       <c r="I137" s="38" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
     </row>
     <row r="141" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -5968,6 +5968,9 @@
       <c r="A206" s="8" t="s">
         <v>209</v>
       </c>
+      <c r="B206" s="7" t="s">
+        <v>436</v>
+      </c>
       <c r="E206" s="9"/>
       <c r="F206" s="9"/>
     </row>
@@ -5976,7 +5979,7 @@
         <v>210</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>211</v>
+        <v>425</v>
       </c>
       <c r="D207" s="3">
         <v>0</v>
@@ -5989,7 +5992,7 @@
         <v>0</v>
       </c>
       <c r="I207" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.25">
@@ -5997,7 +6000,7 @@
         <v>210</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>213</v>
+        <v>426</v>
       </c>
       <c r="D208" s="3">
         <v>0</v>
@@ -6015,7 +6018,7 @@
         <v>210</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>214</v>
+        <v>427</v>
       </c>
       <c r="D209" s="3">
         <v>0</v>
@@ -6028,7 +6031,7 @@
         <v>0</v>
       </c>
       <c r="I209" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="210" spans="2:9" x14ac:dyDescent="0.25">
@@ -6036,7 +6039,7 @@
         <v>210</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>215</v>
+        <v>428</v>
       </c>
       <c r="D210" s="3">
         <v>0</v>
@@ -6054,7 +6057,7 @@
         <v>210</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>216</v>
+        <v>429</v>
       </c>
       <c r="D211" s="3">
         <v>0</v>
@@ -6072,7 +6075,7 @@
         <v>210</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>217</v>
+        <v>430</v>
       </c>
       <c r="D212" s="3">
         <v>0</v>
@@ -6090,7 +6093,7 @@
         <v>210</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>218</v>
+        <v>431</v>
       </c>
       <c r="D213" s="3">
         <v>0</v>
@@ -6108,7 +6111,7 @@
         <v>210</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>219</v>
+        <v>432</v>
       </c>
       <c r="D214" s="3">
         <v>0</v>
@@ -6126,7 +6129,7 @@
         <v>210</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>220</v>
+        <v>433</v>
       </c>
       <c r="D215" s="3">
         <v>0</v>
@@ -6144,7 +6147,7 @@
         <v>210</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>221</v>
+        <v>434</v>
       </c>
       <c r="D216" s="3">
         <v>6</v>
@@ -6162,7 +6165,7 @@
         <v>210</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>222</v>
+        <v>435</v>
       </c>
       <c r="D217" s="3">
         <v>10</v>
@@ -6174,13 +6177,10 @@
         <f t="shared" si="7"/>
         <v>1215</v>
       </c>
-      <c r="I217" s="3" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="220" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E220" s="21" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="F220" s="5">
         <f>SUM(F3:F218)</f>

</xml_diff>

<commit_message>
add excitation mirror bracket 3D printable; clean up parts list.
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF0CFCC-9529-4158-A9FE-ECB7CC199E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05B115D-0D9A-4771-9D9A-A06D730E507E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8976" yWindow="3876" windowWidth="32904" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10200" yWindow="3696" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="426">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -722,9 +722,6 @@
     <t>Alternative. FOV 29 mm diagonal</t>
   </si>
   <si>
-    <t>Detection: Filter wheels</t>
-  </si>
-  <si>
     <t>Detection: Lenses</t>
   </si>
   <si>
@@ -737,43 +734,10 @@
     <t>1.2x telecentric lens, F-mount, suitable for sensors up to 25 megapixel and with an image format of 32mm (diagonal).</t>
   </si>
   <si>
-    <t>0.9X, 28.7mm F-Mount PlatinumTL™ Telecentric Lens</t>
-  </si>
-  <si>
     <t>1.2x Lensagon T25M-12-155I</t>
   </si>
   <si>
-    <t>2x Lensagon TM42-10M-20-75</t>
-  </si>
-  <si>
-    <t>Edmund</t>
-  </si>
-  <si>
-    <t>62-902</t>
-  </si>
-  <si>
-    <t>2x telecentric lens with very flat FOV, designed by request of L.Sacconi. Default mount M42x0.75 (T-mount), needs F-mount adapter.</t>
-  </si>
-  <si>
-    <t>0.9x telecentric lens</t>
-  </si>
-  <si>
-    <t>0.5X, 28.7mm F-Mount PlatinumTL™ Telecentric Lens</t>
-  </si>
-  <si>
-    <t>62-912</t>
-  </si>
-  <si>
     <t>Camera assembly</t>
-  </si>
-  <si>
-    <t>3x Lensagon T25M-30-78</t>
-  </si>
-  <si>
-    <t>3x telecentric lens  is suitable for sensors up to 25 megapixel and with an image format of 32mm (diagonal).</t>
-  </si>
-  <si>
-    <t>Alternative. Moderate-cost 4-channel laser, with mature software and good support. Requires additional switching mechanism (flip mirror).</t>
   </si>
   <si>
     <t>Recommended. Includes switching module between 2 laser ports, controlled by TTL signal.</t>
@@ -842,9 +806,6 @@
     <t>Cable between the Chassis and the PC</t>
   </si>
   <si>
-    <t>Optional. Only if you need more than 4 laser lines.</t>
-  </si>
-  <si>
     <t>SH68-68-EPM Shielded Cable, 68 D-Type to 68 D-Type, 1M</t>
   </si>
   <si>
@@ -971,15 +932,6 @@
     <t>Linear stage for M3 mirror adjustment</t>
   </si>
   <si>
-    <t>AB90H</t>
-  </si>
-  <si>
-    <t>Slim Right-Angle Bracket with Counterbored Slots</t>
-  </si>
-  <si>
-    <t>Bracket for M3 mirror mounting on linear stage</t>
-  </si>
-  <si>
     <t>XRN-B1/M</t>
   </si>
   <si>
@@ -1245,12 +1197,6 @@
   </si>
   <si>
     <t>Robotis FR07-S101K Set</t>
-  </si>
-  <si>
-    <t>Option 1: Servo-driven filter wheel</t>
-  </si>
-  <si>
-    <t>Option 2: Motorized flip mount</t>
   </si>
   <si>
     <t>Deprecated 10mm Galvos</t>
@@ -1380,6 +1326,51 @@
   </si>
   <si>
     <t>varies</t>
+  </si>
+  <si>
+    <t>mirror-bracket.stl</t>
+  </si>
+  <si>
+    <t>Braket for M3 kinematic mirror mount</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bracket for M3 mirror mounting on linear stage. Folder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/custom-parts/excitation-mirror-bracket/</t>
+    </r>
+  </si>
+  <si>
+    <t>HW-KIT5</t>
+  </si>
+  <si>
+    <t>4-40 Cap Screw and Hardware Kit</t>
+  </si>
+  <si>
+    <t>Option 1: Servo-driven filter wheel. ONLY for telecentric lenses or long-WD objectives (&gt; 75 mm)</t>
+  </si>
+  <si>
+    <t>Option 2: Motorized flip mount ONLY for telecentric lenses or long-WD objectives (&gt; 75 mm)</t>
+  </si>
+  <si>
+    <t>Detection: Filter wheels (OPTIONAL)</t>
+  </si>
+  <si>
+    <t>IN PROGRESS</t>
+  </si>
+  <si>
+    <t>OPTIONAL. Only if you need more than 4 laser lines.</t>
+  </si>
+  <si>
+    <t>Alternative. Moderate-cost 4-channel laser, with mature software and good support. Requires switching mechanism or laser duplication.</t>
   </si>
 </sst>
 </file>
@@ -2083,15 +2074,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K218"/>
+  <dimension ref="A1:K205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D169" sqref="D169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="42.5546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="24.109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="86.77734375" style="3" customWidth="1"/>
     <col min="4" max="4" width="6.44140625" style="3" customWidth="1"/>
@@ -2162,7 +2153,7 @@
         <v>12350</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>224</v>
@@ -2216,7 +2207,7 @@
         <v>226</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
@@ -2232,7 +2223,7 @@
         <v>46</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="38" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -2257,7 +2248,7 @@
       </c>
       <c r="G10" s="50"/>
       <c r="I10" s="38" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -2265,7 +2256,7 @@
         <v>211</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="D11" s="38">
         <v>0</v>
@@ -2279,7 +2270,7 @@
       </c>
       <c r="G11" s="50"/>
       <c r="I11" s="38" t="s">
-        <v>245</v>
+        <v>425</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2310,10 +2301,10 @@
         <v>5254</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2337,7 +2328,7 @@
         <v>520</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2361,10 +2352,10 @@
         <v>1807</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="I15" s="41" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2388,7 +2379,7 @@
         <v>132</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="H16" s="41" t="s">
         <v>13</v>
@@ -2415,10 +2406,10 @@
         <v>250</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="I17" s="41" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2442,13 +2433,13 @@
         <v>1807</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="H18" s="41" t="s">
         <v>13</v>
       </c>
       <c r="I18" s="41" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2472,10 +2463,10 @@
         <v>200</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="I19" s="41" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2499,10 +2490,10 @@
         <v>1939</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="I20" s="41" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2526,10 +2517,10 @@
         <v>110</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2553,10 +2544,10 @@
         <v>2450</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2580,10 +2571,10 @@
         <v>4800</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2607,28 +2598,28 @@
         <v>870</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>83</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="D26" s="3">
         <v>2</v>
@@ -2641,21 +2632,21 @@
         <v>140</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>83</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="D27" s="3">
         <v>6</v>
@@ -2668,21 +2659,21 @@
         <v>216</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="51" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>83</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
@@ -2695,21 +2686,21 @@
         <v>43</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="51" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>83</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="D29" s="3">
         <v>1</v>
@@ -2722,21 +2713,21 @@
         <v>29</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="51" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -2749,21 +2740,21 @@
         <v>195</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="51" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
@@ -2776,7 +2767,7 @@
         <v>10</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="15" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2810,7 +2801,7 @@
     </row>
     <row r="36" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
@@ -2901,13 +2892,13 @@
     </row>
     <row r="40" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="42" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="B40" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C40" s="42" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="D40" s="41">
         <v>2</v>
@@ -2955,13 +2946,13 @@
     </row>
     <row r="42" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="42" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
       <c r="B42" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C42" s="42" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="D42" s="41">
         <v>2</v>
@@ -2982,10 +2973,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>53</v>
@@ -3026,14 +3017,14 @@
         <v>400</v>
       </c>
       <c r="F44" s="5">
-        <f t="shared" ref="F44:F73" si="2">E44*D44</f>
+        <f t="shared" ref="F44:F74" si="2">E44*D44</f>
         <v>800</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>46</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>57</v>
@@ -3047,7 +3038,7 @@
         <v>83</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="D45" s="41">
         <v>2</v>
@@ -3060,21 +3051,21 @@
         <v>62</v>
       </c>
       <c r="H45" s="41" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="I45" s="41" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="B46" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="D46" s="45">
         <v>10</v>
@@ -3087,21 +3078,21 @@
         <v>160</v>
       </c>
       <c r="H46" s="45" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="I46" s="45" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="B47" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="D47" s="45">
         <v>2</v>
@@ -3114,21 +3105,21 @@
         <v>82</v>
       </c>
       <c r="H47" s="45" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="I47" s="45" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="42" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="B48" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C48" s="42" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="D48" s="41">
         <v>2</v>
@@ -3141,21 +3132,21 @@
         <v>198</v>
       </c>
       <c r="H48" s="41" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="I48" s="41" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="B49" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="D49" s="45">
         <v>4</v>
@@ -3168,21 +3159,21 @@
         <v>756</v>
       </c>
       <c r="H49" s="45" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="I49" s="45" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="44" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="B50" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="D50" s="45">
         <v>4</v>
@@ -3195,21 +3186,21 @@
         <v>440</v>
       </c>
       <c r="H50" s="45" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="I50" s="45" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="42" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="B51" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C51" s="42" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="D51" s="41">
         <v>4</v>
@@ -3222,21 +3213,21 @@
         <v>52</v>
       </c>
       <c r="H51" s="41" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="I51" s="41" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="42" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="B52" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C52" s="42" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="D52" s="41">
         <v>2</v>
@@ -3249,7 +3240,7 @@
         <v>16</v>
       </c>
       <c r="H52" s="41" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -3273,21 +3264,21 @@
         <v>28</v>
       </c>
       <c r="H53" s="41" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="I53" s="41" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="42" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="B54" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="D54" s="41">
         <v>6</v>
@@ -3300,21 +3291,21 @@
         <v>30</v>
       </c>
       <c r="H54" s="41" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="I54" s="41" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="42" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="B55" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C55" s="42" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="D55" s="41">
         <v>4</v>
@@ -3327,21 +3318,21 @@
         <v>24</v>
       </c>
       <c r="H55" s="41" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="I55" s="41" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="42" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="B56" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C56" s="42" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="D56" s="41">
         <v>4</v>
@@ -3354,10 +3345,10 @@
         <v>20</v>
       </c>
       <c r="H56" s="41" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="I56" s="41" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -3381,18 +3372,18 @@
         <v>10</v>
       </c>
       <c r="H57" s="41" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="44" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="B58" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C58" s="44" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="D58" s="45">
         <v>2</v>
@@ -3405,48 +3396,48 @@
         <v>796</v>
       </c>
       <c r="H58" s="45" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="I58" s="45" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="44" t="s">
-        <v>304</v>
+        <v>415</v>
       </c>
       <c r="B59" s="41" t="s">
-        <v>83</v>
+        <v>317</v>
       </c>
       <c r="C59" s="44" t="s">
-        <v>305</v>
+        <v>416</v>
       </c>
       <c r="D59" s="45">
         <v>2</v>
       </c>
       <c r="E59" s="46">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="F59" s="53">
         <f t="shared" si="2"/>
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="H59" s="45" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="I59" s="45" t="s">
-        <v>306</v>
+        <v>417</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="44" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="B60" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C60" s="44" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="D60" s="45">
         <v>2</v>
@@ -3459,21 +3450,21 @@
         <v>60</v>
       </c>
       <c r="H60" s="45" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="I60" s="45" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="42" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="B61" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C61" s="42" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="D61" s="41">
         <v>2</v>
@@ -3486,15 +3477,15 @@
         <v>72</v>
       </c>
       <c r="H61" s="41" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I61" s="47" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="67" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="C62" s="42"/>
       <c r="E62" s="43"/>
@@ -3503,13 +3494,13 @@
     </row>
     <row r="63" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="57" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="B63" s="58" t="s">
         <v>83</v>
       </c>
       <c r="C63" s="57" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="D63" s="58">
         <v>0</v>
@@ -3522,10 +3513,10 @@
         <v>0</v>
       </c>
       <c r="H63" s="58" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I63" s="61" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3534,18 +3525,18 @@
       <c r="E64" s="59"/>
       <c r="F64" s="60"/>
       <c r="I64" s="61" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
     </row>
     <row r="65" spans="1:10" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="57" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="B65" s="58" t="s">
         <v>83</v>
       </c>
       <c r="C65" s="57" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="D65" s="58">
         <v>0</v>
@@ -3558,19 +3549,19 @@
         <v>0</v>
       </c>
       <c r="H65" s="58" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I65" s="61"/>
     </row>
     <row r="66" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="57" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="B66" s="58" t="s">
         <v>83</v>
       </c>
       <c r="C66" s="57" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="D66" s="58">
         <v>0</v>
@@ -3583,15 +3574,15 @@
         <v>0</v>
       </c>
       <c r="H66" s="58" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I66" s="58" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
     </row>
     <row r="67" spans="1:10" s="63" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="66" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="C67" s="62"/>
       <c r="E67" s="64"/>
@@ -3599,13 +3590,13 @@
     </row>
     <row r="68" spans="1:10" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="62" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="B68" s="63" t="s">
         <v>83</v>
       </c>
       <c r="C68" s="62" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="D68" s="63">
         <v>2</v>
@@ -3618,21 +3609,21 @@
         <v>4208</v>
       </c>
       <c r="H68" s="63" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I68" s="63" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
     </row>
     <row r="69" spans="1:10" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="62" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="B69" s="63" t="s">
         <v>83</v>
       </c>
       <c r="C69" s="62" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="D69" s="63">
         <v>2</v>
@@ -3645,18 +3636,18 @@
         <v>164</v>
       </c>
       <c r="H69" s="63" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
     </row>
     <row r="70" spans="1:10" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="62" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="B70" s="63" t="s">
         <v>83</v>
       </c>
       <c r="C70" s="62" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="D70" s="63">
         <v>1</v>
@@ -3669,21 +3660,21 @@
         <v>390</v>
       </c>
       <c r="H70" s="63" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="I70" s="63" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="42" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="B71" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="D71" s="41">
         <v>2</v>
@@ -3696,18 +3687,18 @@
         <v>50</v>
       </c>
       <c r="H71" s="41" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
     </row>
     <row r="72" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="48" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="B72" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="D72" s="41">
         <v>2</v>
@@ -3720,24 +3711,24 @@
         <v>70</v>
       </c>
       <c r="H72" s="41" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="I72" s="47" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="J72" s="49" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
     </row>
     <row r="73" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="42" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="B73" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="D73" s="41">
         <v>2</v>
@@ -3750,29 +3741,37 @@
         <v>184</v>
       </c>
       <c r="H73" s="41" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="I73" s="41" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
     </row>
     <row r="74" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="42" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="B74" s="41" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="C74" s="56" t="s">
-        <v>388</v>
-      </c>
-      <c r="E74" s="43"/>
-      <c r="F74" s="52"/>
+        <v>372</v>
+      </c>
+      <c r="D74" s="41">
+        <v>2</v>
+      </c>
+      <c r="E74" s="43">
+        <v>1</v>
+      </c>
+      <c r="F74" s="52">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="H74" s="41" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="I74" s="41" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
     </row>
     <row r="75" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -3795,7 +3794,7 @@
     </row>
     <row r="78" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
@@ -3816,18 +3815,18 @@
       <c r="E79" s="43"/>
       <c r="F79" s="52"/>
       <c r="I79" s="41" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
     </row>
     <row r="80" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="42" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="B80" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C80" s="42" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="D80" s="41">
         <v>1</v>
@@ -3842,13 +3841,13 @@
     </row>
     <row r="81" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="48" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="B81" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C81" s="42" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="D81" s="41">
         <v>2</v>
@@ -3863,13 +3862,13 @@
     </row>
     <row r="82" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="42" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="B82" s="41" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="C82" s="42" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="D82" s="41">
         <v>1</v>
@@ -3882,7 +3881,7 @@
         <v>10</v>
       </c>
       <c r="I82" s="41" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
     </row>
     <row r="83" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -3901,36 +3900,36 @@
       <c r="E83" s="43"/>
       <c r="F83" s="52"/>
       <c r="I83" s="41" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
     </row>
     <row r="84" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
-        <v>228</v>
+        <v>422</v>
       </c>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
     </row>
     <row r="85" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
-        <v>396</v>
+        <v>420</v>
       </c>
       <c r="E85" s="9"/>
       <c r="F85" s="9"/>
     </row>
     <row r="86" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
     </row>
     <row r="87" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>14</v>
@@ -3955,13 +3954,13 @@
     </row>
     <row r="88" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="D88" s="3">
         <v>1</v>
@@ -3983,13 +3982,13 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="D89" s="3">
         <v>1</v>
@@ -4010,47 +4009,47 @@
     </row>
     <row r="90" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="D90" s="3">
         <v>1</v>
       </c>
       <c r="I90" s="41" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
     </row>
     <row r="91" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
-        <v>397</v>
+        <v>421</v>
       </c>
       <c r="C91" s="68" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
     </row>
     <row r="92" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
     </row>
     <row r="93" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="42" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="B93" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="D93" s="41">
         <v>0</v>
@@ -4066,13 +4065,13 @@
     </row>
     <row r="94" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="42" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="B94" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C94" s="42" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="D94" s="41">
         <v>0</v>
@@ -4087,13 +4086,13 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="B95" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="D95" s="3">
         <v>0</v>
@@ -4282,20 +4281,20 @@
     </row>
     <row r="104" spans="1:9" s="30" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A104" s="29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E104" s="31"/>
       <c r="F104" s="31"/>
     </row>
     <row r="105" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="B105" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="B105" s="32" t="s">
-        <v>231</v>
-      </c>
       <c r="C105" s="36" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D105" s="32">
         <v>1</v>
@@ -4311,1856 +4310,1738 @@
         <v>13</v>
       </c>
       <c r="H105" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="I105" s="32" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="35" t="s">
+        <v>423</v>
+      </c>
+      <c r="B106" s="32"/>
+      <c r="H106" s="32"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="35"/>
+      <c r="B107" s="32"/>
+      <c r="C107" s="37"/>
+      <c r="H107" s="32"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B108" s="32"/>
+      <c r="C108" s="37"/>
+      <c r="H108" s="32"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="32"/>
+      <c r="C109" s="37"/>
+      <c r="H109" s="32"/>
+    </row>
+    <row r="110" spans="1:9" s="30" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A110" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="E110" s="31"/>
+      <c r="F110" s="31"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B111" s="32"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B112" s="32"/>
+    </row>
+    <row r="114" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A114" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E114" s="9"/>
+      <c r="F114" s="9"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D115" s="3">
+        <v>1</v>
+      </c>
+      <c r="E115" s="5">
+        <v>3582</v>
+      </c>
+      <c r="F115" s="5">
+        <f>E115*D115</f>
+        <v>3582</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D116" s="3">
+        <v>1</v>
+      </c>
+      <c r="E116" s="5">
+        <v>1630</v>
+      </c>
+      <c r="F116" s="5">
+        <f t="shared" ref="F116:F124" si="4">E116*D116</f>
+        <v>1630</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="I105" s="32" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="35">
-        <v>11454</v>
-      </c>
-      <c r="B106" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D106" s="3">
+      <c r="B117" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D117" s="3">
+        <v>1</v>
+      </c>
+      <c r="E117" s="5">
+        <v>886</v>
+      </c>
+      <c r="F117" s="5">
+        <f t="shared" si="4"/>
+        <v>886</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D118" s="3">
+        <v>1</v>
+      </c>
+      <c r="E118" s="5">
+        <v>163</v>
+      </c>
+      <c r="F118" s="5">
+        <f t="shared" si="4"/>
+        <v>163</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D119" s="3">
+        <v>1</v>
+      </c>
+      <c r="E119" s="5">
+        <v>11</v>
+      </c>
+      <c r="F119" s="5">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D120" s="3">
+        <v>1</v>
+      </c>
+      <c r="E120" s="5">
+        <v>520</v>
+      </c>
+      <c r="F120" s="5">
+        <f>E120*D120</f>
+        <v>520</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D121" s="3">
+        <v>1</v>
+      </c>
+      <c r="E121" s="5">
+        <v>193</v>
+      </c>
+      <c r="F121" s="5">
+        <f>E121*D121</f>
+        <v>193</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B122" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C122" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D122" s="38">
         <v>0</v>
       </c>
-      <c r="E106" s="5">
-        <v>5000</v>
-      </c>
-      <c r="F106" s="5">
-        <f>D106*E106</f>
-        <v>0</v>
-      </c>
-      <c r="G106" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H106" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="I106" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="35">
-        <v>11044</v>
-      </c>
-      <c r="B107" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="C107" s="37" t="s">
-        <v>243</v>
-      </c>
-      <c r="D107" s="3">
-        <v>0</v>
-      </c>
-      <c r="E107" s="5">
-        <v>9387</v>
-      </c>
-      <c r="F107" s="5">
-        <f>D107*E107</f>
-        <v>0</v>
-      </c>
-      <c r="G107" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H107" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="I107" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="B108" s="32" t="s">
-        <v>236</v>
-      </c>
-      <c r="C108" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="D108" s="3">
-        <v>0</v>
-      </c>
-      <c r="E108" s="5">
-        <v>2000</v>
-      </c>
-      <c r="F108" s="5">
-        <f t="shared" ref="F108:F109" si="4">D108*E108</f>
-        <v>0</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H108" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="I108" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="B109" s="32" t="s">
-        <v>236</v>
-      </c>
-      <c r="C109" s="37" t="s">
-        <v>240</v>
-      </c>
-      <c r="D109" s="3">
-        <v>0</v>
-      </c>
-      <c r="E109" s="5">
-        <v>2500</v>
-      </c>
-      <c r="F109" s="5">
+      <c r="E122" s="39">
+        <v>2800</v>
+      </c>
+      <c r="F122" s="39">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G109" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H109" s="32" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" s="30" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A110" s="29" t="s">
-        <v>336</v>
-      </c>
-      <c r="E110" s="31"/>
-      <c r="F110" s="31"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B111" s="32"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B112" s="32"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B113" s="32"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B114" s="32"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B115" s="32"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B116" s="32"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B117" s="32"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B118" s="32"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B119" s="32"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B120" s="32"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B121" s="32"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B122" s="32"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B123" s="32"/>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B124" s="32"/>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B125" s="32"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B126" s="32"/>
-    </row>
-    <row r="128" spans="1:6" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A128" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E128" s="9"/>
-      <c r="F128" s="9"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D129" s="3">
-        <v>1</v>
-      </c>
-      <c r="E129" s="5">
-        <v>3582</v>
-      </c>
-      <c r="F129" s="5">
-        <f>E129*D129</f>
-        <v>3582</v>
-      </c>
-      <c r="G129" s="3" t="s">
+      <c r="G122" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="I129" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D130" s="3">
-        <v>1</v>
-      </c>
-      <c r="E130" s="5">
-        <v>1630</v>
-      </c>
-      <c r="F130" s="5">
-        <f t="shared" ref="F130:F138" si="5">E130*D130</f>
-        <v>1630</v>
-      </c>
-      <c r="G130" s="3" t="s">
+      <c r="I122" s="38" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="41" t="s">
+        <v>407</v>
+      </c>
+      <c r="B123" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C123" s="41" t="s">
+        <v>408</v>
+      </c>
+      <c r="D123" s="41">
+        <v>10</v>
+      </c>
+      <c r="E123" s="52">
+        <v>12</v>
+      </c>
+      <c r="F123" s="52">
+        <f t="shared" si="4"/>
+        <v>120</v>
+      </c>
+      <c r="G123" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="I130" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="D131" s="3">
-        <v>1</v>
-      </c>
-      <c r="E131" s="5">
-        <v>886</v>
-      </c>
-      <c r="F131" s="5">
-        <f t="shared" si="5"/>
-        <v>886</v>
-      </c>
-      <c r="G131" s="3" t="s">
+      <c r="I123" s="41" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="41" t="s">
+        <v>409</v>
+      </c>
+      <c r="B124" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C124" s="41" t="s">
+        <v>410</v>
+      </c>
+      <c r="D124" s="41">
+        <v>1</v>
+      </c>
+      <c r="E124" s="52">
+        <v>14</v>
+      </c>
+      <c r="F124" s="52">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="G124" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="I131" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="D132" s="3">
-        <v>1</v>
-      </c>
-      <c r="E132" s="5">
-        <v>163</v>
-      </c>
-      <c r="F132" s="5">
-        <f t="shared" si="5"/>
-        <v>163</v>
-      </c>
-      <c r="G132" s="3" t="s">
+      <c r="I124" s="41" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D125" s="3">
+        <v>4</v>
+      </c>
+      <c r="E125" s="5">
+        <v>15.25</v>
+      </c>
+      <c r="F125" s="5">
+        <f>E125*D125</f>
+        <v>61</v>
+      </c>
+      <c r="G125" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="I132" s="3" t="s">
-        <v>260</v>
-      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D126" s="3">
+        <v>10</v>
+      </c>
+      <c r="E126" s="5">
+        <v>16.5</v>
+      </c>
+      <c r="F126" s="5">
+        <f>E126*D126</f>
+        <v>165</v>
+      </c>
+      <c r="G126" s="41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D127" s="3">
+        <v>10</v>
+      </c>
+      <c r="E127" s="5">
+        <v>24</v>
+      </c>
+      <c r="F127" s="5">
+        <f>E127*D127</f>
+        <v>240</v>
+      </c>
+      <c r="G127" s="41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D128" s="3">
+        <v>6</v>
+      </c>
+      <c r="E128" s="5">
+        <v>24</v>
+      </c>
+      <c r="F128" s="5">
+        <f>E128*D128</f>
+        <v>144</v>
+      </c>
+      <c r="G128" s="41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E129" s="52"/>
+      <c r="F129" s="52"/>
+    </row>
+    <row r="132" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A132" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C132" s="7"/>
+      <c r="E132" s="18"/>
+      <c r="F132" s="18"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>251</v>
+        <v>84</v>
       </c>
       <c r="D133" s="3">
         <v>1</v>
       </c>
       <c r="E133" s="5">
-        <v>11</v>
+        <v>488</v>
       </c>
       <c r="F133" s="5">
-        <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="G133" s="3" t="s">
-        <v>73</v>
+        <f t="shared" ref="F133:F154" si="5">E133*D133</f>
+        <v>488</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D134" s="3">
         <v>1</v>
       </c>
       <c r="E134" s="5">
-        <v>520</v>
+        <v>184</v>
       </c>
       <c r="F134" s="5">
-        <f>E134*D134</f>
-        <v>520</v>
-      </c>
-      <c r="G134" s="3" t="s">
-        <v>73</v>
+        <f t="shared" si="5"/>
+        <v>184</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>263</v>
+        <v>87</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>262</v>
+        <v>88</v>
       </c>
       <c r="D135" s="3">
         <v>1</v>
       </c>
       <c r="E135" s="5">
-        <v>193</v>
+        <v>76</v>
       </c>
       <c r="F135" s="5">
-        <f>E135*D135</f>
-        <v>193</v>
-      </c>
-      <c r="G135" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="B136" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="C136" s="38" t="s">
+        <f t="shared" si="5"/>
         <v>76</v>
       </c>
-      <c r="D136" s="38">
-        <v>0</v>
-      </c>
-      <c r="E136" s="39">
-        <v>2800</v>
-      </c>
-      <c r="F136" s="39">
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D136" s="3">
+        <v>1</v>
+      </c>
+      <c r="E136" s="5">
+        <v>184</v>
+      </c>
+      <c r="F136" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G136" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="I136" s="38" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="41" t="s">
-        <v>425</v>
-      </c>
-      <c r="B137" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C137" s="41" t="s">
-        <v>426</v>
-      </c>
-      <c r="D137" s="41">
-        <v>10</v>
-      </c>
-      <c r="E137" s="52">
-        <v>12</v>
-      </c>
-      <c r="F137" s="52">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D137" s="3">
+        <v>1</v>
+      </c>
+      <c r="E137" s="5">
+        <v>94.180155999999997</v>
+      </c>
+      <c r="F137" s="5">
         <f t="shared" si="5"/>
-        <v>120</v>
-      </c>
-      <c r="G137" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="I137" s="41" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="41" t="s">
-        <v>427</v>
-      </c>
-      <c r="B138" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C138" s="41" t="s">
-        <v>428</v>
-      </c>
-      <c r="D138" s="41">
-        <v>1</v>
-      </c>
-      <c r="E138" s="52">
-        <v>14</v>
-      </c>
-      <c r="F138" s="52">
+        <v>94.180155999999997</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D138" s="3">
+        <v>1</v>
+      </c>
+      <c r="E138" s="5">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="F138" s="5">
         <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="G138" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="I138" s="41" t="s">
-        <v>429</v>
+        <v>36.799999999999997</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="D139" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E139" s="5">
-        <v>15.25</v>
+        <v>21.21</v>
       </c>
       <c r="F139" s="5">
-        <f>E139*D139</f>
-        <v>61</v>
-      </c>
-      <c r="G139" s="41" t="s">
-        <v>73</v>
+        <f t="shared" si="5"/>
+        <v>42.42</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="D140" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E140" s="5">
-        <v>16.5</v>
+        <v>304.75</v>
       </c>
       <c r="F140" s="5">
-        <f>E140*D140</f>
-        <v>165</v>
-      </c>
-      <c r="G140" s="41" t="s">
-        <v>73</v>
+        <f t="shared" si="5"/>
+        <v>304.75</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
       <c r="D141" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E141" s="5">
-        <v>24</v>
+        <v>148.21</v>
       </c>
       <c r="F141" s="5">
-        <f>E141*D141</f>
-        <v>240</v>
-      </c>
-      <c r="G141" s="41" t="s">
-        <v>73</v>
+        <f t="shared" si="5"/>
+        <v>148.21</v>
+      </c>
+      <c r="I141" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>145</v>
+        <v>105</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>151</v>
+        <v>106</v>
       </c>
       <c r="D142" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E142" s="5">
-        <v>24</v>
+        <v>348.45</v>
       </c>
       <c r="F142" s="5">
-        <f>E142*D142</f>
-        <v>144</v>
-      </c>
-      <c r="G142" s="41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E143" s="52"/>
-      <c r="F143" s="52"/>
-    </row>
-    <row r="146" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C146" s="7"/>
-      <c r="E146" s="18"/>
-      <c r="F146" s="18"/>
+        <f t="shared" si="5"/>
+        <v>348.45</v>
+      </c>
+      <c r="I142" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D143" s="3">
+        <v>1</v>
+      </c>
+      <c r="E143" s="5">
+        <v>60.95</v>
+      </c>
+      <c r="F143" s="5">
+        <f t="shared" si="5"/>
+        <v>60.95</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D144" s="3">
+        <v>1</v>
+      </c>
+      <c r="E144" s="5">
+        <v>34.5</v>
+      </c>
+      <c r="F144" s="5">
+        <f t="shared" si="5"/>
+        <v>34.5</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D145" s="3">
+        <v>1</v>
+      </c>
+      <c r="E145" s="5">
+        <v>51.45</v>
+      </c>
+      <c r="F145" s="5">
+        <f t="shared" si="5"/>
+        <v>51.45</v>
+      </c>
+      <c r="I145" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D146" s="3">
+        <v>2</v>
+      </c>
+      <c r="E146" s="5">
+        <v>13.8</v>
+      </c>
+      <c r="F146" s="5">
+        <f t="shared" si="5"/>
+        <v>27.6</v>
+      </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="D147" s="3">
         <v>1</v>
       </c>
       <c r="E147" s="5">
-        <v>488</v>
+        <v>19.09</v>
       </c>
       <c r="F147" s="5">
-        <f t="shared" ref="F147:F168" si="6">E147*D147</f>
-        <v>488</v>
+        <f t="shared" si="5"/>
+        <v>19.09</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="D148" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E148" s="5">
-        <v>184</v>
+        <v>40.51</v>
       </c>
       <c r="F148" s="5">
+        <f t="shared" si="5"/>
+        <v>81.02</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D149" s="3">
+        <v>2</v>
+      </c>
+      <c r="E149" s="5">
+        <v>83.598116000000005</v>
+      </c>
+      <c r="F149" s="5">
+        <f t="shared" si="5"/>
+        <v>167.19623200000001</v>
+      </c>
+      <c r="I149" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D150" s="3">
+        <v>4</v>
+      </c>
+      <c r="E150" s="5">
+        <v>70.103999999999999</v>
+      </c>
+      <c r="F150" s="5">
+        <f t="shared" si="5"/>
+        <v>280.416</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A151" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D151" s="3">
+        <v>2</v>
+      </c>
+      <c r="E151" s="5">
+        <v>28.75</v>
+      </c>
+      <c r="F151" s="5">
+        <f t="shared" si="5"/>
+        <v>57.5</v>
+      </c>
+      <c r="I151" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D152" s="3">
+        <v>2</v>
+      </c>
+      <c r="E152" s="5">
+        <v>38.872799999999998</v>
+      </c>
+      <c r="F152" s="5">
+        <f t="shared" si="5"/>
+        <v>77.745599999999996</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B153" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D153" s="3">
+        <v>1</v>
+      </c>
+      <c r="E153" s="5">
+        <v>205</v>
+      </c>
+      <c r="F153" s="5">
+        <f t="shared" si="5"/>
+        <v>205</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B154" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D154" s="3">
+        <v>2</v>
+      </c>
+      <c r="E154" s="5">
+        <v>12</v>
+      </c>
+      <c r="F154" s="5">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A155" s="11"/>
+      <c r="B155" s="11"/>
+      <c r="C155" s="10"/>
+    </row>
+    <row r="156" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A156" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F156" s="9"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D157" s="3">
+        <v>4</v>
+      </c>
+      <c r="E157" s="5">
+        <v>16.5</v>
+      </c>
+      <c r="F157" s="5">
+        <f t="shared" ref="F157:F173" si="6">E157*D157</f>
+        <v>66</v>
+      </c>
+      <c r="I157" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D158" s="3">
+        <v>2</v>
+      </c>
+      <c r="E158" s="5">
+        <v>140</v>
+      </c>
+      <c r="F158" s="5">
+        <f t="shared" si="6"/>
+        <v>280</v>
+      </c>
+      <c r="I158" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D159" s="3">
+        <v>1</v>
+      </c>
+      <c r="E159" s="5">
+        <v>85.1</v>
+      </c>
+      <c r="F159" s="5">
+        <f t="shared" si="6"/>
+        <v>85.1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D160" s="3">
+        <v>2</v>
+      </c>
+      <c r="E160" s="5">
+        <v>32</v>
+      </c>
+      <c r="F160" s="5">
+        <f t="shared" si="6"/>
+        <v>64</v>
+      </c>
+      <c r="I160" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D161" s="3">
+        <v>2</v>
+      </c>
+      <c r="E161" s="5">
+        <v>51.58</v>
+      </c>
+      <c r="F161" s="5">
+        <f t="shared" si="6"/>
+        <v>103.16</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D162" s="3">
+        <v>1</v>
+      </c>
+      <c r="E162" s="5">
+        <v>60</v>
+      </c>
+      <c r="F162" s="5">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="I162" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D163" s="3">
+        <v>1</v>
+      </c>
+      <c r="E163" s="5">
+        <v>136.47999999999999</v>
+      </c>
+      <c r="F163" s="5">
+        <f t="shared" si="6"/>
+        <v>136.47999999999999</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D164" s="3">
+        <v>1</v>
+      </c>
+      <c r="E164" s="5">
+        <v>136.47999999999999</v>
+      </c>
+      <c r="F164" s="5">
+        <f t="shared" si="6"/>
+        <v>136.47999999999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D165" s="3">
+        <v>1</v>
+      </c>
+      <c r="E165" s="5">
+        <v>60.95</v>
+      </c>
+      <c r="F165" s="5">
+        <f t="shared" si="6"/>
+        <v>60.95</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D166" s="3">
+        <v>1</v>
+      </c>
+      <c r="E166" s="5">
+        <v>119.416</v>
+      </c>
+      <c r="F166" s="5">
+        <f t="shared" si="6"/>
+        <v>119.416</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D167" s="3">
+        <v>1</v>
+      </c>
+      <c r="E167" s="5">
+        <v>105.8</v>
+      </c>
+      <c r="F167" s="5">
+        <f t="shared" si="6"/>
+        <v>105.8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D168" s="3">
+        <v>2</v>
+      </c>
+      <c r="E168" s="5">
+        <v>119.6</v>
+      </c>
+      <c r="F168" s="5">
+        <f t="shared" si="6"/>
+        <v>239.2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D169" s="3">
+        <v>1</v>
+      </c>
+      <c r="E169" s="5">
+        <v>100</v>
+      </c>
+      <c r="F169" s="5">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D170" s="3">
+        <v>2</v>
+      </c>
+      <c r="E170" s="5">
+        <v>92</v>
+      </c>
+      <c r="F170" s="5">
         <f t="shared" si="6"/>
         <v>184</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A149" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D149" s="3">
-        <v>1</v>
-      </c>
-      <c r="E149" s="5">
-        <v>76</v>
-      </c>
-      <c r="F149" s="5">
-        <f t="shared" si="6"/>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A150" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B150" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D150" s="3">
-        <v>1</v>
-      </c>
-      <c r="E150" s="5">
-        <v>184</v>
-      </c>
-      <c r="F150" s="5">
-        <f t="shared" si="6"/>
-        <v>184</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A151" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B151" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C151" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D151" s="3">
-        <v>1</v>
-      </c>
-      <c r="E151" s="5">
-        <v>94.180155999999997</v>
-      </c>
-      <c r="F151" s="5">
-        <f t="shared" si="6"/>
-        <v>94.180155999999997</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A152" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C152" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D152" s="3">
-        <v>1</v>
-      </c>
-      <c r="E152" s="5">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="F152" s="5">
-        <f t="shared" si="6"/>
-        <v>36.799999999999997</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A153" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D153" s="3">
-        <v>2</v>
-      </c>
-      <c r="E153" s="5">
-        <v>21.21</v>
-      </c>
-      <c r="F153" s="5">
-        <f t="shared" si="6"/>
-        <v>42.42</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A154" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D154" s="3">
-        <v>1</v>
-      </c>
-      <c r="E154" s="5">
-        <v>304.75</v>
-      </c>
-      <c r="F154" s="5">
-        <f t="shared" si="6"/>
-        <v>304.75</v>
-      </c>
-      <c r="I154" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A155" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D155" s="3">
-        <v>1</v>
-      </c>
-      <c r="E155" s="5">
-        <v>148.21</v>
-      </c>
-      <c r="F155" s="5">
-        <f t="shared" si="6"/>
-        <v>148.21</v>
-      </c>
-      <c r="I155" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A156" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C156" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D156" s="3">
-        <v>1</v>
-      </c>
-      <c r="E156" s="5">
-        <v>348.45</v>
-      </c>
-      <c r="F156" s="5">
-        <f t="shared" si="6"/>
-        <v>348.45</v>
-      </c>
-      <c r="I156" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A157" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D157" s="3">
-        <v>1</v>
-      </c>
-      <c r="E157" s="5">
-        <v>60.95</v>
-      </c>
-      <c r="F157" s="5">
-        <f t="shared" si="6"/>
-        <v>60.95</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A158" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D158" s="3">
-        <v>1</v>
-      </c>
-      <c r="E158" s="5">
-        <v>34.5</v>
-      </c>
-      <c r="F158" s="5">
-        <f t="shared" si="6"/>
-        <v>34.5</v>
-      </c>
-      <c r="I158" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A159" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D159" s="3">
-        <v>1</v>
-      </c>
-      <c r="E159" s="5">
-        <v>51.45</v>
-      </c>
-      <c r="F159" s="5">
-        <f t="shared" si="6"/>
-        <v>51.45</v>
-      </c>
-      <c r="I159" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A160" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D160" s="3">
-        <v>2</v>
-      </c>
-      <c r="E160" s="5">
-        <v>13.8</v>
-      </c>
-      <c r="F160" s="5">
-        <f t="shared" si="6"/>
-        <v>27.6</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D161" s="3">
-        <v>1</v>
-      </c>
-      <c r="E161" s="5">
-        <v>19.09</v>
-      </c>
-      <c r="F161" s="5">
-        <f t="shared" si="6"/>
-        <v>19.09</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A162" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D162" s="3">
-        <v>2</v>
-      </c>
-      <c r="E162" s="5">
-        <v>40.51</v>
-      </c>
-      <c r="F162" s="5">
-        <f t="shared" si="6"/>
-        <v>81.02</v>
-      </c>
-      <c r="I162" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D163" s="3">
-        <v>2</v>
-      </c>
-      <c r="E163" s="5">
-        <v>83.598116000000005</v>
-      </c>
-      <c r="F163" s="5">
-        <f t="shared" si="6"/>
-        <v>167.19623200000001</v>
-      </c>
-      <c r="I163" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A164" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D164" s="3">
-        <v>4</v>
-      </c>
-      <c r="E164" s="5">
-        <v>70.103999999999999</v>
-      </c>
-      <c r="F164" s="5">
-        <f t="shared" si="6"/>
-        <v>280.416</v>
-      </c>
-      <c r="I164" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A165" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D165" s="3">
-        <v>2</v>
-      </c>
-      <c r="E165" s="5">
-        <v>28.75</v>
-      </c>
-      <c r="F165" s="5">
-        <f t="shared" si="6"/>
-        <v>57.5</v>
-      </c>
-      <c r="I165" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A166" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D166" s="3">
-        <v>2</v>
-      </c>
-      <c r="E166" s="5">
-        <v>38.872799999999998</v>
-      </c>
-      <c r="F166" s="5">
-        <f t="shared" si="6"/>
-        <v>77.745599999999996</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B167" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C167" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D167" s="3">
-        <v>1</v>
-      </c>
-      <c r="E167" s="5">
-        <v>205</v>
-      </c>
-      <c r="F167" s="5">
-        <f t="shared" si="6"/>
-        <v>205</v>
-      </c>
-      <c r="I167" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B168" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D168" s="3">
-        <v>2</v>
-      </c>
-      <c r="E168" s="5">
-        <v>12</v>
-      </c>
-      <c r="F168" s="5">
-        <f t="shared" si="6"/>
-        <v>24</v>
-      </c>
-      <c r="I168" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A169" s="11"/>
-      <c r="B169" s="11"/>
-      <c r="C169" s="10"/>
-    </row>
-    <row r="170" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A170" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F170" s="9"/>
-    </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>136</v>
+        <v>83</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
       <c r="D171" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E171" s="5">
-        <v>16.5</v>
+        <v>96.23</v>
       </c>
       <c r="F171" s="5">
-        <f t="shared" ref="F171:F186" si="7">E171*D171</f>
-        <v>66</v>
-      </c>
-      <c r="I171" s="3" t="s">
-        <v>138</v>
+        <f t="shared" si="6"/>
+        <v>96.23</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>140</v>
+        <v>83</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>141</v>
+        <v>176</v>
       </c>
       <c r="D172" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E172" s="5">
-        <v>140</v>
+        <v>102.44</v>
       </c>
       <c r="F172" s="5">
-        <f t="shared" si="7"/>
-        <v>280</v>
-      </c>
-      <c r="I172" s="3" t="s">
-        <v>142</v>
+        <f t="shared" si="6"/>
+        <v>102.44</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="D173" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E173" s="5">
-        <v>85.1</v>
+        <v>28</v>
       </c>
       <c r="F173" s="5">
-        <f t="shared" si="7"/>
-        <v>85.1</v>
+        <f t="shared" si="6"/>
+        <v>56</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A174" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="C174" s="3" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="D174" s="3">
-        <v>2</v>
-      </c>
-      <c r="E174" s="5">
-        <v>32</v>
-      </c>
-      <c r="F174" s="5">
-        <f t="shared" si="7"/>
-        <v>64</v>
-      </c>
-      <c r="I174" s="3" t="s">
-        <v>154</v>
+        <v>4</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A175" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="C175" s="3" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="D175" s="3">
-        <v>2</v>
-      </c>
-      <c r="E175" s="5">
-        <v>51.58</v>
-      </c>
-      <c r="F175" s="5">
-        <f t="shared" si="7"/>
-        <v>103.16</v>
+        <v>1</v>
+      </c>
+      <c r="I175" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A176" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="C176" s="3" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="D176" s="3">
         <v>1</v>
       </c>
-      <c r="E176" s="5">
-        <v>60</v>
-      </c>
-      <c r="F176" s="5">
-        <f t="shared" si="7"/>
-        <v>60</v>
-      </c>
-      <c r="I176" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A177" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D177" s="3">
-        <v>1</v>
-      </c>
-      <c r="E177" s="5">
-        <v>136.47999999999999</v>
-      </c>
-      <c r="F177" s="5">
-        <f t="shared" si="7"/>
-        <v>136.47999999999999</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A178" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B178" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D178" s="3">
-        <v>1</v>
-      </c>
-      <c r="E178" s="5">
-        <v>136.47999999999999</v>
-      </c>
-      <c r="F178" s="5">
-        <f t="shared" si="7"/>
-        <v>136.47999999999999</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A179" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C179" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D179" s="3">
-        <v>1</v>
-      </c>
-      <c r="E179" s="5">
-        <v>60.95</v>
-      </c>
-      <c r="F179" s="5">
-        <f t="shared" si="7"/>
-        <v>60.95</v>
-      </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A180" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C180" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D180" s="3">
-        <v>1</v>
-      </c>
-      <c r="E180" s="5">
-        <v>119.416</v>
-      </c>
-      <c r="F180" s="5">
-        <f t="shared" si="7"/>
-        <v>119.416</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A181" s="3" t="s">
-        <v>167</v>
-      </c>
+    </row>
+    <row r="180" spans="1:11" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A180" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C180" s="7"/>
+      <c r="E180" s="18"/>
+      <c r="F180" s="18"/>
+    </row>
+    <row r="181" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B181" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C181" s="3" t="s">
-        <v>168</v>
+        <v>184</v>
+      </c>
+      <c r="C181" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="D181" s="3">
         <v>1</v>
       </c>
-      <c r="E181" s="5">
-        <v>105.8</v>
-      </c>
-      <c r="F181" s="5">
-        <f t="shared" si="7"/>
-        <v>105.8</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A182" s="3" t="s">
-        <v>169</v>
-      </c>
+      <c r="G181" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I181" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J181" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K181" s="4"/>
+    </row>
+    <row r="182" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B182" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C182" s="3" t="s">
-        <v>170</v>
+        <v>184</v>
+      </c>
+      <c r="C182" s="19" t="s">
+        <v>189</v>
       </c>
       <c r="D182" s="3">
-        <v>2</v>
-      </c>
-      <c r="E182" s="5">
-        <v>119.6</v>
-      </c>
-      <c r="F182" s="5">
-        <f t="shared" si="7"/>
-        <v>239.2</v>
-      </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A183" s="3" t="s">
-        <v>171</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G182" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I182" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J182" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K182" s="4"/>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B183" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>172</v>
+        <v>184</v>
+      </c>
+      <c r="C183" s="19" t="s">
+        <v>190</v>
       </c>
       <c r="D183" s="3">
         <v>2</v>
       </c>
-      <c r="E183" s="5">
-        <v>92</v>
-      </c>
-      <c r="F183" s="5">
-        <f t="shared" si="7"/>
+      <c r="G183" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I183" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="J183" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B184" s="3" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A184" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="C184" s="3" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="D184" s="3">
         <v>1</v>
       </c>
-      <c r="E184" s="5">
-        <v>96.23</v>
-      </c>
-      <c r="F184" s="5">
-        <f t="shared" si="7"/>
-        <v>96.23</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A185" s="3" t="s">
-        <v>175</v>
-      </c>
+      <c r="G184" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="J184" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B185" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C185" s="3" t="s">
-        <v>176</v>
+        <v>184</v>
+      </c>
+      <c r="C185" s="19" t="s">
+        <v>194</v>
       </c>
       <c r="D185" s="3">
-        <v>1</v>
-      </c>
-      <c r="E185" s="5">
-        <v>102.44</v>
-      </c>
-      <c r="F185" s="5">
-        <f t="shared" si="7"/>
-        <v>102.44</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A186" s="3" t="s">
-        <v>177</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G185" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I185" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="J185" s="19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B186" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>178</v>
+        <v>184</v>
+      </c>
+      <c r="C186" s="19" t="s">
+        <v>198</v>
       </c>
       <c r="D186" s="3">
         <v>2</v>
       </c>
-      <c r="E186" s="5">
-        <v>28</v>
-      </c>
-      <c r="F186" s="5">
+      <c r="G186" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I186" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="J186" s="19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B187" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C187" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="D187" s="3">
+        <v>2</v>
+      </c>
+      <c r="G187" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I187" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="J187" s="19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B188" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D188" s="3">
+        <v>1</v>
+      </c>
+      <c r="G188" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="J188" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A189" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B189" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C189" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="D189" s="19">
+        <v>10</v>
+      </c>
+      <c r="F189" s="55"/>
+      <c r="G189" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="I189" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="J189" s="19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A191" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B191" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="E191" s="9"/>
+      <c r="F191" s="9"/>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B192" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="D192" s="3">
+        <v>0</v>
+      </c>
+      <c r="E192" s="5">
+        <v>518.5</v>
+      </c>
+      <c r="F192" s="5">
+        <f t="shared" ref="F192:F202" si="7">E192*D192</f>
+        <v>0</v>
+      </c>
+      <c r="I192" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="193" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B193" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="D193" s="3">
+        <v>0</v>
+      </c>
+      <c r="E193" s="5">
+        <v>764</v>
+      </c>
+      <c r="F193" s="5">
         <f t="shared" si="7"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C187" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D187" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C188" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D188" s="3">
-        <v>1</v>
-      </c>
-      <c r="I188" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C189" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="D189" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" spans="1:11" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A193" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C193" s="7"/>
-      <c r="E193" s="18"/>
-      <c r="F193" s="18"/>
-    </row>
-    <row r="194" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C194" s="19" t="s">
-        <v>185</v>
+        <v>206</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>396</v>
       </c>
       <c r="D194" s="3">
-        <v>1</v>
-      </c>
-      <c r="G194" s="3" t="s">
-        <v>186</v>
+        <v>0</v>
+      </c>
+      <c r="E194" s="5">
+        <v>816</v>
+      </c>
+      <c r="F194" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="I194" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J194" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="K194" s="4"/>
-    </row>
-    <row r="195" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="195" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C195" s="19" t="s">
-        <v>189</v>
+        <v>206</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>397</v>
       </c>
       <c r="D195" s="3">
-        <v>1</v>
-      </c>
-      <c r="G195" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="I195" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J195" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="K195" s="4"/>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E195" s="5">
+        <v>952</v>
+      </c>
+      <c r="F195" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C196" s="19" t="s">
-        <v>190</v>
+        <v>206</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>398</v>
       </c>
       <c r="D196" s="3">
-        <v>2</v>
-      </c>
-      <c r="G196" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="I196" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="J196" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E196" s="5">
+        <v>99.5</v>
+      </c>
+      <c r="F196" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>192</v>
+        <v>399</v>
       </c>
       <c r="D197" s="3">
-        <v>1</v>
-      </c>
-      <c r="G197" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="J197" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E197" s="5">
+        <v>128.5</v>
+      </c>
+      <c r="F197" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C198" s="19" t="s">
-        <v>194</v>
+        <v>206</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>400</v>
       </c>
       <c r="D198" s="3">
         <v>0</v>
       </c>
-      <c r="G198" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="I198" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="J198" s="19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E198" s="5">
+        <v>156</v>
+      </c>
+      <c r="F198" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C199" s="19" t="s">
-        <v>198</v>
+        <v>206</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>401</v>
       </c>
       <c r="D199" s="3">
-        <v>2</v>
-      </c>
-      <c r="G199" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="I199" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="J199" s="19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E199" s="5">
+        <v>184.5</v>
+      </c>
+      <c r="F199" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C200" s="19" t="s">
-        <v>200</v>
+        <v>206</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>402</v>
       </c>
       <c r="D200" s="3">
-        <v>2</v>
-      </c>
-      <c r="G200" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="I200" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="J200" s="19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E200" s="5">
+        <v>106.5</v>
+      </c>
+      <c r="F200" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>201</v>
+        <v>403</v>
       </c>
       <c r="D201" s="3">
-        <v>1</v>
-      </c>
-      <c r="G201" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="J201" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="202" spans="1:11" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A202" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="B202" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="C202" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="D202" s="19">
+        <v>6</v>
+      </c>
+      <c r="E201" s="5">
+        <v>106.5</v>
+      </c>
+      <c r="F201" s="5">
+        <f t="shared" si="7"/>
+        <v>639</v>
+      </c>
+    </row>
+    <row r="202" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B202" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="D202" s="3">
         <v>10</v>
       </c>
-      <c r="F202" s="55"/>
-      <c r="G202" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="I202" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="J202" s="19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="204" spans="1:11" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A204" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="B204" s="7" t="s">
-        <v>423</v>
-      </c>
-      <c r="E204" s="9"/>
-      <c r="F204" s="9"/>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B205" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C205" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="D205" s="3">
-        <v>0</v>
-      </c>
-      <c r="E205" s="5">
-        <v>518.5</v>
+      <c r="E202" s="5">
+        <v>121.5</v>
+      </c>
+      <c r="F202" s="5">
+        <f t="shared" si="7"/>
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="205" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E205" s="21" t="s">
+        <v>208</v>
       </c>
       <c r="F205" s="5">
-        <f t="shared" ref="F205:F215" si="8">E205*D205</f>
-        <v>0</v>
-      </c>
-      <c r="I205" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B206" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C206" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="D206" s="3">
-        <v>0</v>
-      </c>
-      <c r="E206" s="5">
-        <v>764</v>
-      </c>
-      <c r="F206" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B207" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C207" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="D207" s="3">
-        <v>0</v>
-      </c>
-      <c r="E207" s="5">
-        <v>816</v>
-      </c>
-      <c r="F207" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I207" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B208" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C208" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="D208" s="3">
-        <v>0</v>
-      </c>
-      <c r="E208" s="5">
-        <v>952</v>
-      </c>
-      <c r="F208" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B209" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C209" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="D209" s="3">
-        <v>0</v>
-      </c>
-      <c r="E209" s="5">
-        <v>99.5</v>
-      </c>
-      <c r="F209" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B210" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C210" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="D210" s="3">
-        <v>0</v>
-      </c>
-      <c r="E210" s="5">
-        <v>128.5</v>
-      </c>
-      <c r="F210" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B211" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="D211" s="3">
-        <v>0</v>
-      </c>
-      <c r="E211" s="5">
-        <v>156</v>
-      </c>
-      <c r="F211" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B212" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C212" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="D212" s="3">
-        <v>0</v>
-      </c>
-      <c r="E212" s="5">
-        <v>184.5</v>
-      </c>
-      <c r="F212" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B213" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C213" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="D213" s="3">
-        <v>0</v>
-      </c>
-      <c r="E213" s="5">
-        <v>106.5</v>
-      </c>
-      <c r="F213" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B214" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C214" s="3" t="s">
-        <v>421</v>
-      </c>
-      <c r="D214" s="3">
-        <v>6</v>
-      </c>
-      <c r="E214" s="5">
-        <v>106.5</v>
-      </c>
-      <c r="F214" s="5">
-        <f t="shared" si="8"/>
-        <v>639</v>
-      </c>
-    </row>
-    <row r="215" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B215" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="D215" s="3">
-        <v>10</v>
-      </c>
-      <c r="E215" s="5">
-        <v>121.5</v>
-      </c>
-      <c r="F215" s="5">
-        <f t="shared" si="8"/>
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="218" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E218" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="F218" s="5">
-        <f>SUM(F3:F216)</f>
-        <v>99059.533987999996</v>
+        <f>SUM(F3:F203)</f>
+        <v>99111.533987999996</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C108" r:id="rId1" xr:uid="{67732474-80B4-4B9F-B7F4-8404FF2C5C7F}"/>
-    <hyperlink ref="C105" r:id="rId2" xr:uid="{3BC0AF99-F679-46A9-B7F9-6A136F582C78}"/>
-    <hyperlink ref="C109" r:id="rId3" xr:uid="{45DA022D-F6DD-4A17-9406-F3AFCDB6F6B9}"/>
-    <hyperlink ref="C107" r:id="rId4" xr:uid="{F54B111C-4718-45BF-A954-B0E31DB7F5D0}"/>
+    <hyperlink ref="C105" r:id="rId1" xr:uid="{3BC0AF99-F679-46A9-B7F9-6A136F582C78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
laser cover model update
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05B115D-0D9A-4771-9D9A-A06D730E507E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13C9DBA-C156-42C5-9FF2-6F6792D1DB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="3696" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8352" yWindow="3984" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="426">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -947,24 +947,12 @@
     <t>Cage assembly</t>
   </si>
   <si>
-    <t>LCP03/M</t>
-  </si>
-  <si>
     <t>60 mm Blank Cage Plate, M4 Tap</t>
   </si>
   <si>
-    <t>GVS211/M</t>
-  </si>
-  <si>
-    <t>1D Large Beam (10 mm) Diameter Galvo System, Broadband Mirror (-E02), Metric, Power Supply Not Included</t>
-  </si>
-  <si>
     <t>Galvo assembly</t>
   </si>
   <si>
-    <t>Galvo cables must be ordered long (80 cm), and controller boards must be tuned accordingly, ask Thorlabs. Short (default) cables enforce placing the controller boards inside the housing, and they generate a lot of heat.</t>
-  </si>
-  <si>
     <t>ER4-P4</t>
   </si>
   <si>
@@ -974,9 +962,6 @@
     <t>Excitation obj mount</t>
   </si>
   <si>
-    <t>Needs modification, see LCP03M_modified.ipt</t>
-  </si>
-  <si>
     <t>SM2NFM</t>
   </si>
   <si>
@@ -992,33 +977,18 @@
     <t>Todo: design 3D-printable alternative</t>
   </si>
   <si>
-    <t>GPS011-EC</t>
-  </si>
-  <si>
     <t>1D or 2D Galvo System Linear Power Supply, 230 VAC</t>
   </si>
   <si>
-    <t>Power supply for 2 galvos. Voltage and plugs are country specific!</t>
-  </si>
-  <si>
     <t>The F-mount steel ring must be taken out and mounted into the modified LCP06M plate using screws.</t>
   </si>
   <si>
     <t>Needs modification (using lathe or mill), see LCP06M-Nikon-modified.ipt</t>
   </si>
   <si>
-    <t>Galvo bracket must be modified (using milling machine), see Galvo-bracket-modified.ipt</t>
-  </si>
-  <si>
     <t>3D printed</t>
   </si>
   <si>
-    <t>GCE001</t>
-  </si>
-  <si>
-    <t>Galvo Driver Card Cover</t>
-  </si>
-  <si>
     <t>Detection: Other components</t>
   </si>
   <si>
@@ -1199,9 +1169,6 @@
     <t>Robotis FR07-S101K Set</t>
   </si>
   <si>
-    <t>Deprecated 10mm Galvos</t>
-  </si>
-  <si>
     <t>QS15X-AG</t>
   </si>
   <si>
@@ -1214,13 +1181,7 @@
     <t>Command and Power Cables for QS15/20/30/45, SS, &amp; SP Series Galvo Scanners</t>
   </si>
   <si>
-    <t>GPWR15</t>
-  </si>
-  <si>
     <t>±15 V Power Supply for BLINK &amp; QS, SS, SP, &amp; XG Series Galvo Scanners</t>
-  </si>
-  <si>
-    <t>To be tested:</t>
   </si>
   <si>
     <t>Standard cables are 60 cm long. Sufficient?</t>
@@ -1372,12 +1333,51 @@
   <si>
     <t>Alternative. Moderate-cost 4-channel laser, with mature software and good support. Requires switching mechanism or laser duplication.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Preferred power supply for 2 galvos. Needs a simple adapter (3 wires), see Wiki. </t>
+  </si>
+  <si>
+    <t>Non-preferred (but offered by Thorlabs) Power supply for 2 galvos. Bare wires sticking around, unsafe!</t>
+  </si>
+  <si>
+    <t>Galvo heat sink assembled from sheets, each galvo requires 7 sheets</t>
+  </si>
+  <si>
+    <t>HeatSink-sheet-H2mm.pdf</t>
+  </si>
+  <si>
+    <t>LCP03/M, modified</t>
+  </si>
+  <si>
+    <t>Needs modification (machining), see  /custom-parts/galvo-assembly/15mm-galvo(Thorlabs-QS15)-mount/QS15-mount-modified-Thorlabs-CagePlate-LCP03.pdf</t>
+  </si>
+  <si>
+    <t>Claser-cut or water-jet cut from 2-mm Aluminum. See folder /custom-parts/galvo-assembly/15mm-galvo(Thorlabs-QS15)-mount/</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>Heat sink for galvo driver</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>TODO: find specific model</t>
+  </si>
+  <si>
+    <t>GPS011 (obsolete)</t>
+  </si>
+  <si>
+    <t>GPWR15 (unsafe)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1499,8 +1499,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1555,18 +1561,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1609,7 +1603,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -1675,18 +1669,9 @@
     <xf numFmtId="2" fontId="5" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="10" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="11" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Excel Built-in Heading 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -2074,10 +2059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K205"/>
+  <dimension ref="A1:K202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D169" sqref="D169"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2153,7 +2138,7 @@
         <v>12350</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>224</v>
@@ -2270,7 +2255,7 @@
       </c>
       <c r="G11" s="50"/>
       <c r="I11" s="38" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2301,10 +2286,10 @@
         <v>5254</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2328,7 +2313,7 @@
         <v>520</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2352,10 +2337,10 @@
         <v>1807</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="I15" s="41" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2379,7 +2364,7 @@
         <v>132</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="H16" s="41" t="s">
         <v>13</v>
@@ -2406,10 +2391,10 @@
         <v>250</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="I17" s="41" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2433,13 +2418,13 @@
         <v>1807</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="H18" s="41" t="s">
         <v>13</v>
       </c>
       <c r="I18" s="41" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2463,10 +2448,10 @@
         <v>200</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="I19" s="41" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -2490,10 +2475,10 @@
         <v>1939</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="I20" s="41" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2517,10 +2502,10 @@
         <v>110</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2544,10 +2529,10 @@
         <v>2450</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2571,10 +2556,10 @@
         <v>4800</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2598,28 +2583,28 @@
         <v>870</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>83</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="D26" s="3">
         <v>2</v>
@@ -2632,21 +2617,21 @@
         <v>140</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>83</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="D27" s="3">
         <v>6</v>
@@ -2659,21 +2644,21 @@
         <v>216</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="51" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>83</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
@@ -2686,21 +2671,21 @@
         <v>43</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="51" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>83</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="D29" s="3">
         <v>1</v>
@@ -2713,21 +2698,21 @@
         <v>29</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="51" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -2740,21 +2725,21 @@
         <v>195</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="51" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
@@ -2767,7 +2752,7 @@
         <v>10</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="15" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2946,7 +2931,7 @@
     </row>
     <row r="42" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="42" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="B42" s="41" t="s">
         <v>83</v>
@@ -2973,7 +2958,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>251</v>
@@ -3017,7 +3002,7 @@
         <v>400</v>
       </c>
       <c r="F44" s="5">
-        <f t="shared" ref="F44:F74" si="2">E44*D44</f>
+        <f t="shared" ref="F44:F71" si="2">E44*D44</f>
         <v>800</v>
       </c>
       <c r="G44" s="3" t="s">
@@ -3162,7 +3147,7 @@
         <v>269</v>
       </c>
       <c r="I49" s="45" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -3189,7 +3174,7 @@
         <v>269</v>
       </c>
       <c r="I50" s="45" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -3240,7 +3225,7 @@
         <v>16</v>
       </c>
       <c r="H52" s="41" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -3372,7 +3357,7 @@
         <v>10</v>
       </c>
       <c r="H57" s="41" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -3404,13 +3389,13 @@
     </row>
     <row r="59" spans="1:9" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="44" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="B59" s="41" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C59" s="44" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="D59" s="45">
         <v>2</v>
@@ -3426,7 +3411,7 @@
         <v>294</v>
       </c>
       <c r="I59" s="45" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -3458,13 +3443,13 @@
     </row>
     <row r="61" spans="1:9" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="42" t="s">
+        <v>417</v>
+      </c>
+      <c r="B61" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C61" s="42" t="s">
         <v>296</v>
-      </c>
-      <c r="B61" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C61" s="42" t="s">
-        <v>297</v>
       </c>
       <c r="D61" s="41">
         <v>2</v>
@@ -3477,691 +3462,748 @@
         <v>72</v>
       </c>
       <c r="H61" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I61" s="47" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="42" t="s">
+        <v>370</v>
+      </c>
+      <c r="B62" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C62" s="42" t="s">
+        <v>371</v>
+      </c>
+      <c r="D62" s="41">
+        <v>2</v>
+      </c>
+      <c r="E62" s="43">
+        <v>2104</v>
+      </c>
+      <c r="F62" s="52">
+        <f t="shared" ref="F62:F67" si="3">E62*D62</f>
+        <v>4208</v>
+      </c>
+      <c r="H62" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I62" s="41" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="42" t="s">
+        <v>372</v>
+      </c>
+      <c r="B63" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" s="42" t="s">
+        <v>373</v>
+      </c>
+      <c r="D63" s="41">
+        <v>2</v>
+      </c>
+      <c r="E63" s="43">
+        <v>82</v>
+      </c>
+      <c r="F63" s="52">
+        <f t="shared" si="3"/>
+        <v>164</v>
+      </c>
+      <c r="H63" s="41" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="59" t="s">
+        <v>424</v>
+      </c>
+      <c r="B64" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C64" s="42" t="s">
+        <v>306</v>
+      </c>
+      <c r="D64" s="41">
+        <v>1</v>
+      </c>
+      <c r="E64" s="43">
+        <v>495</v>
+      </c>
+      <c r="F64" s="52">
+        <f t="shared" si="3"/>
+        <v>495</v>
+      </c>
+      <c r="H64" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I64" s="41" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="59" t="s">
+        <v>425</v>
+      </c>
+      <c r="B65" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" s="42" t="s">
+        <v>374</v>
+      </c>
+      <c r="D65" s="41">
+        <v>0</v>
+      </c>
+      <c r="E65" s="43">
+        <v>390</v>
+      </c>
+      <c r="F65" s="52">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H65" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I65" s="41" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="42" t="s">
+        <v>416</v>
+      </c>
+      <c r="B66" s="41" t="s">
+        <v>420</v>
+      </c>
+      <c r="C66" s="42" t="s">
+        <v>415</v>
+      </c>
+      <c r="D66" s="41">
+        <v>14</v>
+      </c>
+      <c r="E66" s="43">
+        <v>20</v>
+      </c>
+      <c r="F66" s="52">
+        <f t="shared" si="3"/>
+        <v>280</v>
+      </c>
+      <c r="H66" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I66" s="47" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="58" t="s">
+        <v>422</v>
+      </c>
+      <c r="B67" s="41" t="s">
+        <v>363</v>
+      </c>
+      <c r="C67" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="D67" s="41">
+        <v>1</v>
+      </c>
+      <c r="E67" s="43">
+        <v>10</v>
+      </c>
+      <c r="F67" s="52">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="H67" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I67" s="41" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="42" t="s">
+        <v>298</v>
+      </c>
+      <c r="B68" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C68" s="42" t="s">
+        <v>299</v>
+      </c>
+      <c r="D68" s="41">
+        <v>2</v>
+      </c>
+      <c r="E68" s="43">
+        <v>25</v>
+      </c>
+      <c r="F68" s="52">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="H68" s="41" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="48" t="s">
+        <v>302</v>
+      </c>
+      <c r="B69" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" s="42" t="s">
+        <v>303</v>
+      </c>
+      <c r="D69" s="41">
+        <v>2</v>
+      </c>
+      <c r="E69" s="43">
+        <v>35</v>
+      </c>
+      <c r="F69" s="52">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H69" s="41" t="s">
         <v>300</v>
       </c>
-      <c r="I61" s="47" t="s">
+      <c r="I69" s="47" t="s">
+        <v>308</v>
+      </c>
+      <c r="J69" s="49" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="67" t="s">
-        <v>380</v>
-      </c>
-      <c r="C62" s="42"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="52"/>
-      <c r="I62" s="47"/>
-    </row>
-    <row r="63" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="57" t="s">
-        <v>298</v>
-      </c>
-      <c r="B63" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="C63" s="57" t="s">
-        <v>299</v>
-      </c>
-      <c r="D63" s="58">
-        <v>0</v>
-      </c>
-      <c r="E63" s="59">
-        <v>1757</v>
-      </c>
-      <c r="F63" s="60">
+    <row r="70" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="42" t="s">
+        <v>301</v>
+      </c>
+      <c r="B70" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" s="42" t="s">
+        <v>304</v>
+      </c>
+      <c r="D70" s="41">
+        <v>2</v>
+      </c>
+      <c r="E70" s="43">
+        <v>92</v>
+      </c>
+      <c r="F70" s="52">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H63" s="58" t="s">
+        <v>184</v>
+      </c>
+      <c r="H70" s="41" t="s">
         <v>300</v>
       </c>
-      <c r="I63" s="61" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="57"/>
-      <c r="C64" s="57"/>
-      <c r="E64" s="59"/>
-      <c r="F64" s="60"/>
-      <c r="I64" s="61" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="57" t="s">
-        <v>318</v>
-      </c>
-      <c r="B65" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="C65" s="57" t="s">
-        <v>319</v>
-      </c>
-      <c r="D65" s="58">
-        <v>0</v>
-      </c>
-      <c r="E65" s="59">
-        <v>59</v>
-      </c>
-      <c r="F65" s="60">
-        <f>E65*D65</f>
-        <v>0</v>
-      </c>
-      <c r="H65" s="58" t="s">
-        <v>300</v>
-      </c>
-      <c r="I65" s="61"/>
-    </row>
-    <row r="66" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="57" t="s">
-        <v>311</v>
-      </c>
-      <c r="B66" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="C66" s="57" t="s">
-        <v>312</v>
-      </c>
-      <c r="D66" s="58">
-        <v>0</v>
-      </c>
-      <c r="E66" s="59">
-        <v>495</v>
-      </c>
-      <c r="F66" s="60">
-        <f>E66*D66</f>
-        <v>0</v>
-      </c>
-      <c r="H66" s="58" t="s">
-        <v>300</v>
-      </c>
-      <c r="I66" s="58" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" s="63" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="66" t="s">
-        <v>387</v>
-      </c>
-      <c r="C67" s="62"/>
-      <c r="E67" s="64"/>
-      <c r="F67" s="65"/>
-    </row>
-    <row r="68" spans="1:10" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="62" t="s">
-        <v>381</v>
-      </c>
-      <c r="B68" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="C68" s="62" t="s">
-        <v>382</v>
-      </c>
-      <c r="D68" s="63">
-        <v>2</v>
-      </c>
-      <c r="E68" s="64">
-        <v>2104</v>
-      </c>
-      <c r="F68" s="65">
-        <f>E68*D68</f>
-        <v>4208</v>
-      </c>
-      <c r="H68" s="63" t="s">
-        <v>300</v>
-      </c>
-      <c r="I68" s="63" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="62" t="s">
-        <v>383</v>
-      </c>
-      <c r="B69" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="C69" s="62" t="s">
-        <v>384</v>
-      </c>
-      <c r="D69" s="63">
-        <v>2</v>
-      </c>
-      <c r="E69" s="64">
-        <v>82</v>
-      </c>
-      <c r="F69" s="65">
-        <f>E69*D69</f>
-        <v>164</v>
-      </c>
-      <c r="H69" s="63" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="62" t="s">
-        <v>385</v>
-      </c>
-      <c r="B70" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70" s="62" t="s">
-        <v>386</v>
-      </c>
-      <c r="D70" s="63">
-        <v>1</v>
-      </c>
-      <c r="E70" s="64">
-        <v>390</v>
-      </c>
-      <c r="F70" s="65">
-        <f>E70*D70</f>
-        <v>390</v>
-      </c>
-      <c r="H70" s="63" t="s">
-        <v>300</v>
-      </c>
-      <c r="I70" s="63" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I70" s="41" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="42" t="s">
-        <v>302</v>
+        <v>377</v>
       </c>
       <c r="B71" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C71" s="42" t="s">
-        <v>303</v>
+        <v>309</v>
+      </c>
+      <c r="C71" s="56" t="s">
+        <v>362</v>
       </c>
       <c r="D71" s="41">
         <v>2</v>
       </c>
       <c r="E71" s="43">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F71" s="52">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="H71" s="41" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="48" t="s">
-        <v>307</v>
-      </c>
-      <c r="B72" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C72" s="42" t="s">
-        <v>308</v>
-      </c>
-      <c r="D72" s="41">
-        <v>2</v>
-      </c>
-      <c r="E72" s="43">
-        <v>35</v>
-      </c>
-      <c r="F72" s="52">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="H72" s="41" t="s">
-        <v>304</v>
-      </c>
-      <c r="I72" s="47" t="s">
-        <v>315</v>
-      </c>
-      <c r="J72" s="49" t="s">
-        <v>310</v>
-      </c>
+      <c r="I71" s="41" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="42"/>
+      <c r="C72" s="42"/>
+      <c r="E72" s="43"/>
+      <c r="F72" s="52"/>
     </row>
     <row r="73" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="42" t="s">
-        <v>306</v>
-      </c>
-      <c r="B73" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C73" s="42" t="s">
-        <v>309</v>
-      </c>
-      <c r="D73" s="41">
-        <v>2</v>
-      </c>
-      <c r="E73" s="43">
-        <v>92</v>
-      </c>
-      <c r="F73" s="52">
-        <f t="shared" si="2"/>
-        <v>184</v>
-      </c>
-      <c r="H73" s="41" t="s">
-        <v>304</v>
-      </c>
-      <c r="I73" s="41" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="42" t="s">
-        <v>390</v>
-      </c>
-      <c r="B74" s="41" t="s">
-        <v>317</v>
-      </c>
-      <c r="C74" s="56" t="s">
-        <v>372</v>
-      </c>
-      <c r="D74" s="41">
-        <v>2</v>
-      </c>
-      <c r="E74" s="43">
-        <v>1</v>
-      </c>
-      <c r="F74" s="52">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="H74" s="41" t="s">
-        <v>304</v>
-      </c>
-      <c r="I74" s="41" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="42"/>
-      <c r="C75" s="42"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="52"/>
+      <c r="A73" s="42"/>
+      <c r="C73" s="42"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="52"/>
+    </row>
+    <row r="74" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="42"/>
+      <c r="C74" s="42"/>
+      <c r="E74" s="43"/>
+      <c r="F74" s="52"/>
+    </row>
+    <row r="75" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A75" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
     </row>
     <row r="76" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="42"/>
-      <c r="C76" s="42"/>
+      <c r="A76" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B76" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C76" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D76" s="41">
+        <v>1</v>
+      </c>
       <c r="E76" s="43"/>
       <c r="F76" s="52"/>
+      <c r="I76" s="41" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="77" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="42"/>
-      <c r="C77" s="42"/>
-      <c r="E77" s="43"/>
-      <c r="F77" s="52"/>
-    </row>
-    <row r="78" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
+      <c r="A77" s="42" t="s">
+        <v>326</v>
+      </c>
+      <c r="B77" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C77" s="42" t="s">
+        <v>327</v>
+      </c>
+      <c r="D77" s="41">
+        <v>1</v>
+      </c>
+      <c r="E77" s="43">
+        <v>63</v>
+      </c>
+      <c r="F77" s="52">
+        <f>D77*E77</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="48" t="s">
+        <v>331</v>
+      </c>
+      <c r="B78" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C78" s="42" t="s">
+        <v>332</v>
+      </c>
+      <c r="D78" s="41">
+        <v>2</v>
+      </c>
+      <c r="E78" s="43">
+        <v>69</v>
+      </c>
+      <c r="F78" s="52">
+        <f>D78*E78</f>
+        <v>138</v>
+      </c>
     </row>
     <row r="79" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="42" t="s">
-        <v>29</v>
+        <v>329</v>
       </c>
       <c r="B79" s="41" t="s">
+        <v>328</v>
+      </c>
+      <c r="C79" s="42" t="s">
+        <v>330</v>
+      </c>
+      <c r="D79" s="41">
+        <v>1</v>
+      </c>
+      <c r="E79" s="43">
+        <v>10</v>
+      </c>
+      <c r="F79" s="52">
+        <f>D79*E79</f>
+        <v>10</v>
+      </c>
+      <c r="I79" s="41" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B80" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C79" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="D79" s="41">
-        <v>1</v>
-      </c>
-      <c r="E79" s="43"/>
-      <c r="F79" s="52"/>
-      <c r="I79" s="41" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="42" t="s">
-        <v>336</v>
-      </c>
-      <c r="B80" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C80" s="42" t="s">
-        <v>337</v>
+      <c r="C80" s="41" t="s">
+        <v>26</v>
       </c>
       <c r="D80" s="41">
         <v>1</v>
       </c>
-      <c r="E80" s="43">
-        <v>63</v>
-      </c>
-      <c r="F80" s="52">
-        <f>D80*E80</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="48" t="s">
-        <v>341</v>
-      </c>
-      <c r="B81" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C81" s="42" t="s">
-        <v>342</v>
-      </c>
-      <c r="D81" s="41">
-        <v>2</v>
-      </c>
-      <c r="E81" s="43">
-        <v>69</v>
-      </c>
-      <c r="F81" s="52">
-        <f>D81*E81</f>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="42" t="s">
-        <v>339</v>
-      </c>
-      <c r="B82" s="41" t="s">
-        <v>338</v>
-      </c>
-      <c r="C82" s="42" t="s">
-        <v>340</v>
-      </c>
-      <c r="D82" s="41">
-        <v>1</v>
-      </c>
-      <c r="E82" s="43">
-        <v>10</v>
-      </c>
-      <c r="F82" s="52">
-        <f>D82*E82</f>
-        <v>10</v>
-      </c>
-      <c r="I82" s="41" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="B83" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="C83" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="D83" s="41">
-        <v>1</v>
-      </c>
-      <c r="E83" s="43"/>
-      <c r="F83" s="52"/>
-      <c r="I83" s="41" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="6" t="s">
-        <v>422</v>
-      </c>
-      <c r="E84" s="9"/>
-      <c r="F84" s="9"/>
-    </row>
-    <row r="85" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="8" t="s">
-        <v>420</v>
-      </c>
-      <c r="E85" s="9"/>
-      <c r="F85" s="9"/>
-    </row>
-    <row r="86" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="E86" s="9"/>
-      <c r="F86" s="9"/>
+      <c r="E80" s="43"/>
+      <c r="F80" s="52"/>
+      <c r="I80" s="41" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A81" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+    </row>
+    <row r="82" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+    </row>
+    <row r="83" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+    </row>
+    <row r="84" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" s="3">
+        <v>1</v>
+      </c>
+      <c r="E84" s="5">
+        <v>250</v>
+      </c>
+      <c r="F84" s="5">
+        <f>E84*D84</f>
+        <v>250</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J84" s="4"/>
+    </row>
+    <row r="85" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="D85" s="3">
+        <v>1</v>
+      </c>
+      <c r="E85" s="5">
+        <v>13</v>
+      </c>
+      <c r="F85" s="5">
+        <f>E85*D85</f>
+        <v>13</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J85" s="4"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="D86" s="3">
+        <v>1</v>
+      </c>
+      <c r="E86" s="5">
+        <v>43</v>
+      </c>
+      <c r="F86" s="5">
+        <f>E86*D86</f>
+        <v>43</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="87" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>373</v>
+        <v>309</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>14</v>
+        <v>368</v>
       </c>
       <c r="D87" s="3">
         <v>1</v>
       </c>
-      <c r="E87" s="5">
-        <v>250</v>
-      </c>
-      <c r="F87" s="5">
-        <f>E87*D87</f>
-        <v>250</v>
-      </c>
-      <c r="G87" s="3" t="s">
+      <c r="I87" s="41" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="C88" s="57" t="s">
+        <v>380</v>
+      </c>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+    </row>
+    <row r="89" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+    </row>
+    <row r="90" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="42" t="s">
+        <v>357</v>
+      </c>
+      <c r="B90" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C90" s="42" t="s">
+        <v>358</v>
+      </c>
+      <c r="D90" s="41">
+        <v>0</v>
+      </c>
+      <c r="E90" s="43">
+        <v>656</v>
+      </c>
+      <c r="F90" s="52">
+        <f>E90*D90</f>
+        <v>0</v>
+      </c>
+      <c r="I90" s="49"/>
+    </row>
+    <row r="91" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="42" t="s">
+        <v>355</v>
+      </c>
+      <c r="B91" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C91" s="42" t="s">
+        <v>356</v>
+      </c>
+      <c r="D91" s="41">
+        <v>0</v>
+      </c>
+      <c r="E91" s="43">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="F91" s="52">
+        <f>E91*D91</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="B92" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="D92" s="3">
+        <v>0</v>
+      </c>
+      <c r="E92" s="12">
+        <v>4.87</v>
+      </c>
+      <c r="F92" s="52">
+        <f>E92*D92</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" s="22" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="F93" s="54"/>
+    </row>
+    <row r="94" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="F94" s="54"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D95" s="3">
+        <v>1</v>
+      </c>
+      <c r="E95" s="5">
+        <v>1075</v>
+      </c>
+      <c r="F95" s="5">
+        <f t="shared" ref="F95:F100" si="4">E95*D95</f>
+        <v>1075</v>
+      </c>
+      <c r="G95" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H87" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J87" s="4"/>
-    </row>
-    <row r="88" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="D88" s="3">
-        <v>1</v>
-      </c>
-      <c r="E88" s="5">
+      <c r="I95" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B96" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C96" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D96" s="38">
+        <v>0</v>
+      </c>
+      <c r="E96" s="39">
+        <v>1350</v>
+      </c>
+      <c r="F96" s="39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G96" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="F88" s="5">
-        <f>E88*D88</f>
+      <c r="I96" s="38" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B97" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C97" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D97" s="38">
+        <v>0</v>
+      </c>
+      <c r="E97" s="39">
+        <v>1350</v>
+      </c>
+      <c r="F97" s="39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G97" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="G88" s="3" t="s">
+      <c r="I97" s="38" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B98" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C98" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D98" s="38">
+        <v>0</v>
+      </c>
+      <c r="E98" s="40">
+        <v>1445</v>
+      </c>
+      <c r="F98" s="39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G98" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H88" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J88" s="4"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="D89" s="3">
-        <v>1</v>
-      </c>
-      <c r="E89" s="5">
-        <v>43</v>
-      </c>
-      <c r="F89" s="5">
-        <f>E89*D89</f>
-        <v>43</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D90" s="3">
-        <v>1</v>
-      </c>
-      <c r="I90" s="41" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="8" t="s">
-        <v>421</v>
-      </c>
-      <c r="C91" s="68" t="s">
-        <v>393</v>
-      </c>
-      <c r="E91" s="9"/>
-      <c r="F91" s="9"/>
-    </row>
-    <row r="92" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="E92" s="9"/>
-      <c r="F92" s="9"/>
-    </row>
-    <row r="93" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="42" t="s">
-        <v>367</v>
-      </c>
-      <c r="B93" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C93" s="42" t="s">
-        <v>368</v>
-      </c>
-      <c r="D93" s="41">
-        <v>0</v>
-      </c>
-      <c r="E93" s="43">
-        <v>656</v>
-      </c>
-      <c r="F93" s="52">
-        <f>E93*D93</f>
-        <v>0</v>
-      </c>
-      <c r="I93" s="49"/>
-    </row>
-    <row r="94" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="42" t="s">
-        <v>365</v>
-      </c>
-      <c r="B94" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C94" s="42" t="s">
-        <v>366</v>
-      </c>
-      <c r="D94" s="41">
-        <v>0</v>
-      </c>
-      <c r="E94" s="43">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="F94" s="52">
-        <f>E94*D94</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="B95" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C95" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="D95" s="3">
-        <v>0</v>
-      </c>
-      <c r="E95" s="12">
-        <v>4.87</v>
-      </c>
-      <c r="F95" s="52">
-        <f>E95*D95</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" s="22" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="F96" s="54"/>
-    </row>
-    <row r="97" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="F97" s="54"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D98" s="3">
-        <v>1</v>
-      </c>
-      <c r="E98" s="5">
-        <v>1075</v>
-      </c>
-      <c r="F98" s="5">
-        <f t="shared" ref="F98:F103" si="3">E98*D98</f>
-        <v>1075</v>
-      </c>
-      <c r="G98" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I98" s="3" t="s">
-        <v>221</v>
+      <c r="I98" s="38" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="38" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B99" s="38" t="s">
         <v>59</v>
       </c>
       <c r="C99" s="38" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D99" s="38">
         <v>0</v>
       </c>
       <c r="E99" s="39">
-        <v>1350</v>
+        <v>1130</v>
       </c>
       <c r="F99" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G99" s="38" t="s">
@@ -4173,22 +4215,22 @@
     </row>
     <row r="100" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="38" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B100" s="38" t="s">
         <v>59</v>
       </c>
       <c r="C100" s="38" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D100" s="38">
         <v>0</v>
       </c>
       <c r="E100" s="39">
-        <v>1350</v>
+        <v>1130</v>
       </c>
       <c r="F100" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G100" s="38" t="s">
@@ -4198,426 +4240,417 @@
         <v>215</v>
       </c>
     </row>
-    <row r="101" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B101" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C101" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="D101" s="38">
-        <v>0</v>
-      </c>
-      <c r="E101" s="40">
-        <v>1445</v>
-      </c>
-      <c r="F101" s="39">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G101" s="38" t="s">
+    <row r="101" spans="1:9" s="30" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A101" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="E101" s="31"/>
+      <c r="F101" s="31"/>
+    </row>
+    <row r="102" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="B102" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="C102" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="D102" s="32">
+        <v>1</v>
+      </c>
+      <c r="E102" s="33">
+        <v>6734</v>
+      </c>
+      <c r="F102" s="33">
+        <f>D102*E102</f>
+        <v>6734</v>
+      </c>
+      <c r="G102" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I101" s="38" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="B102" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C102" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="D102" s="38">
-        <v>0</v>
-      </c>
-      <c r="E102" s="39">
-        <v>1130</v>
-      </c>
-      <c r="F102" s="39">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G102" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="I102" s="38" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="B103" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C103" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="D103" s="38">
-        <v>0</v>
-      </c>
-      <c r="E103" s="39">
-        <v>1130</v>
-      </c>
-      <c r="F103" s="39">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G103" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="I103" s="38" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" s="30" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A104" s="29" t="s">
-        <v>228</v>
-      </c>
-      <c r="E104" s="31"/>
-      <c r="F104" s="31"/>
-    </row>
-    <row r="105" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="34" t="s">
-        <v>229</v>
-      </c>
-      <c r="B105" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="C105" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D105" s="32">
-        <v>1</v>
-      </c>
-      <c r="E105" s="33">
-        <v>6734</v>
-      </c>
-      <c r="F105" s="33">
-        <f>D105*E105</f>
-        <v>6734</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H105" s="32" t="s">
+      <c r="H102" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="I105" s="32" t="s">
+      <c r="I102" s="32" t="s">
         <v>231</v>
       </c>
     </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="35" t="s">
+        <v>410</v>
+      </c>
+      <c r="B103" s="32"/>
+      <c r="H103" s="32"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="35"/>
+      <c r="B104" s="32"/>
+      <c r="C104" s="37"/>
+      <c r="H104" s="32"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="32"/>
+      <c r="C105" s="37"/>
+      <c r="H105" s="32"/>
+    </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="35" t="s">
-        <v>423</v>
-      </c>
       <c r="B106" s="32"/>
+      <c r="C106" s="37"/>
       <c r="H106" s="32"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="35"/>
-      <c r="B107" s="32"/>
-      <c r="C107" s="37"/>
-      <c r="H107" s="32"/>
+    <row r="107" spans="1:9" s="30" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A107" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="E107" s="31"/>
+      <c r="F107" s="31"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B108" s="32"/>
-      <c r="C108" s="37"/>
-      <c r="H108" s="32"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B109" s="32"/>
-      <c r="C109" s="37"/>
-      <c r="H109" s="32"/>
-    </row>
-    <row r="110" spans="1:9" s="30" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A110" s="29" t="s">
-        <v>320</v>
-      </c>
-      <c r="E110" s="31"/>
-      <c r="F110" s="31"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B111" s="32"/>
+    </row>
+    <row r="111" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A111" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B112" s="32"/>
-    </row>
-    <row r="114" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A114" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E114" s="9"/>
-      <c r="F114" s="9"/>
+      <c r="A112" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D112" s="3">
+        <v>1</v>
+      </c>
+      <c r="E112" s="5">
+        <v>3582</v>
+      </c>
+      <c r="F112" s="5">
+        <f>E112*D112</f>
+        <v>3582</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D113" s="3">
+        <v>1</v>
+      </c>
+      <c r="E113" s="5">
+        <v>1630</v>
+      </c>
+      <c r="F113" s="5">
+        <f t="shared" ref="F113:F121" si="5">E113*D113</f>
+        <v>1630</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D114" s="3">
+        <v>1</v>
+      </c>
+      <c r="E114" s="5">
+        <v>886</v>
+      </c>
+      <c r="F114" s="5">
+        <f t="shared" si="5"/>
+        <v>886</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>79</v>
+        <v>247</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>80</v>
+        <v>245</v>
       </c>
       <c r="D115" s="3">
         <v>1</v>
       </c>
       <c r="E115" s="5">
-        <v>3582</v>
+        <v>163</v>
       </c>
       <c r="F115" s="5">
-        <f>E115*D115</f>
-        <v>3582</v>
+        <f t="shared" si="5"/>
+        <v>163</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>73</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>243</v>
+        <v>74</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D116" s="3">
         <v>1</v>
       </c>
       <c r="E116" s="5">
-        <v>1630</v>
+        <v>11</v>
       </c>
       <c r="F116" s="5">
-        <f t="shared" ref="F116:F124" si="4">E116*D116</f>
-        <v>1630</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
       <c r="G116" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I116" s="3" t="s">
-        <v>240</v>
-      </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>242</v>
+        <v>77</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>241</v>
+        <v>78</v>
       </c>
       <c r="D117" s="3">
         <v>1</v>
       </c>
       <c r="E117" s="5">
-        <v>886</v>
+        <v>520</v>
       </c>
       <c r="F117" s="5">
-        <f t="shared" si="4"/>
-        <v>886</v>
+        <f>E117*D117</f>
+        <v>520</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I117" s="3" t="s">
-        <v>244</v>
-      </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="D118" s="3">
         <v>1</v>
       </c>
       <c r="E118" s="5">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="F118" s="5">
-        <f t="shared" si="4"/>
-        <v>163</v>
+        <f>E118*D118</f>
+        <v>193</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I118" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B119" s="3" t="s">
+    </row>
+    <row r="119" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B119" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C119" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="D119" s="3">
-        <v>1</v>
-      </c>
-      <c r="E119" s="5">
-        <v>11</v>
-      </c>
-      <c r="F119" s="5">
-        <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="G119" s="3" t="s">
+      <c r="C119" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D119" s="38">
+        <v>0</v>
+      </c>
+      <c r="E119" s="39">
+        <v>2800</v>
+      </c>
+      <c r="F119" s="39">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G119" s="38" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D120" s="3">
-        <v>1</v>
-      </c>
-      <c r="E120" s="5">
-        <v>520</v>
-      </c>
-      <c r="F120" s="5">
-        <f>E120*D120</f>
-        <v>520</v>
-      </c>
-      <c r="G120" s="3" t="s">
+      <c r="I119" s="38" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="41" t="s">
+        <v>394</v>
+      </c>
+      <c r="B120" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C120" s="41" t="s">
+        <v>395</v>
+      </c>
+      <c r="D120" s="41">
+        <v>10</v>
+      </c>
+      <c r="E120" s="52">
+        <v>12</v>
+      </c>
+      <c r="F120" s="52">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+      <c r="G120" s="41" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="D121" s="3">
-        <v>1</v>
-      </c>
-      <c r="E121" s="5">
-        <v>193</v>
-      </c>
-      <c r="F121" s="5">
-        <f>E121*D121</f>
-        <v>193</v>
-      </c>
-      <c r="G121" s="3" t="s">
+      <c r="I120" s="41" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="41" t="s">
+        <v>396</v>
+      </c>
+      <c r="B121" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C121" s="41" t="s">
+        <v>397</v>
+      </c>
+      <c r="D121" s="41">
+        <v>1</v>
+      </c>
+      <c r="E121" s="52">
+        <v>14</v>
+      </c>
+      <c r="F121" s="52">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="G121" s="41" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="B122" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="C122" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D122" s="38">
-        <v>0</v>
-      </c>
-      <c r="E122" s="39">
-        <v>2800</v>
-      </c>
-      <c r="F122" s="39">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G122" s="38" t="s">
+      <c r="I121" s="41" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D122" s="3">
+        <v>4</v>
+      </c>
+      <c r="E122" s="5">
+        <v>15.25</v>
+      </c>
+      <c r="F122" s="5">
+        <f>E122*D122</f>
+        <v>61</v>
+      </c>
+      <c r="G122" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="I122" s="38" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="41" t="s">
-        <v>407</v>
-      </c>
-      <c r="B123" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C123" s="41" t="s">
-        <v>408</v>
-      </c>
-      <c r="D123" s="41">
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D123" s="3">
         <v>10</v>
       </c>
-      <c r="E123" s="52">
-        <v>12</v>
-      </c>
-      <c r="F123" s="52">
-        <f t="shared" si="4"/>
-        <v>120</v>
+      <c r="E123" s="5">
+        <v>16.5</v>
+      </c>
+      <c r="F123" s="5">
+        <f>E123*D123</f>
+        <v>165</v>
       </c>
       <c r="G123" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="I123" s="41" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="41" t="s">
-        <v>409</v>
-      </c>
-      <c r="B124" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C124" s="41" t="s">
-        <v>410</v>
-      </c>
-      <c r="D124" s="41">
-        <v>1</v>
-      </c>
-      <c r="E124" s="52">
-        <v>14</v>
-      </c>
-      <c r="F124" s="52">
-        <f t="shared" si="4"/>
-        <v>14</v>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D124" s="3">
+        <v>10</v>
+      </c>
+      <c r="E124" s="5">
+        <v>24</v>
+      </c>
+      <c r="F124" s="5">
+        <f>E124*D124</f>
+        <v>240</v>
       </c>
       <c r="G124" s="41" t="s">
         <v>73</v>
-      </c>
-      <c r="I124" s="41" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -4628,1417 +4661,1345 @@
         <v>83</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D125" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E125" s="5">
-        <v>15.25</v>
+        <v>24</v>
       </c>
       <c r="F125" s="5">
         <f>E125*D125</f>
-        <v>61</v>
+        <v>144</v>
       </c>
       <c r="G125" s="41" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D126" s="3">
-        <v>10</v>
-      </c>
-      <c r="E126" s="5">
-        <v>16.5</v>
-      </c>
-      <c r="F126" s="5">
-        <f>E126*D126</f>
-        <v>165</v>
-      </c>
-      <c r="G126" s="41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D127" s="3">
-        <v>10</v>
-      </c>
-      <c r="E127" s="5">
-        <v>24</v>
-      </c>
-      <c r="F127" s="5">
-        <f>E127*D127</f>
-        <v>240</v>
-      </c>
-      <c r="G127" s="41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D128" s="3">
-        <v>6</v>
-      </c>
-      <c r="E128" s="5">
-        <v>24</v>
-      </c>
-      <c r="F128" s="5">
-        <f>E128*D128</f>
-        <v>144</v>
-      </c>
-      <c r="G128" s="41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E129" s="52"/>
-      <c r="F129" s="52"/>
-    </row>
-    <row r="132" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A132" s="8" t="s">
+    <row r="126" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E126" s="52"/>
+      <c r="F126" s="52"/>
+    </row>
+    <row r="129" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A129" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C132" s="7"/>
-      <c r="E132" s="18"/>
-      <c r="F132" s="18"/>
+      <c r="C129" s="7"/>
+      <c r="E129" s="18"/>
+      <c r="F129" s="18"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D130" s="3">
+        <v>1</v>
+      </c>
+      <c r="E130" s="5">
+        <v>488</v>
+      </c>
+      <c r="F130" s="5">
+        <f t="shared" ref="F130:F151" si="6">E130*D130</f>
+        <v>488</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D131" s="3">
+        <v>1</v>
+      </c>
+      <c r="E131" s="5">
+        <v>184</v>
+      </c>
+      <c r="F131" s="5">
+        <f t="shared" si="6"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D132" s="3">
+        <v>1</v>
+      </c>
+      <c r="E132" s="5">
+        <v>76</v>
+      </c>
+      <c r="F132" s="5">
+        <f t="shared" si="6"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D133" s="3">
         <v>1</v>
       </c>
       <c r="E133" s="5">
-        <v>488</v>
+        <v>184</v>
       </c>
       <c r="F133" s="5">
-        <f t="shared" ref="F133:F154" si="5">E133*D133</f>
-        <v>488</v>
+        <f t="shared" si="6"/>
+        <v>184</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D134" s="3">
         <v>1</v>
       </c>
       <c r="E134" s="5">
-        <v>184</v>
+        <v>94.180155999999997</v>
       </c>
       <c r="F134" s="5">
-        <f t="shared" si="5"/>
-        <v>184</v>
+        <f t="shared" si="6"/>
+        <v>94.180155999999997</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D135" s="3">
         <v>1</v>
       </c>
       <c r="E135" s="5">
-        <v>76</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="F135" s="5">
-        <f t="shared" si="5"/>
-        <v>76</v>
+        <f t="shared" si="6"/>
+        <v>36.799999999999997</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D136" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E136" s="5">
-        <v>184</v>
+        <v>21.21</v>
       </c>
       <c r="F136" s="5">
-        <f t="shared" si="5"/>
-        <v>184</v>
+        <f t="shared" si="6"/>
+        <v>42.42</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D137" s="3">
         <v>1</v>
       </c>
       <c r="E137" s="5">
-        <v>94.180155999999997</v>
+        <v>304.75</v>
       </c>
       <c r="F137" s="5">
-        <f t="shared" si="5"/>
-        <v>94.180155999999997</v>
+        <f t="shared" si="6"/>
+        <v>304.75</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D138" s="3">
         <v>1</v>
       </c>
       <c r="E138" s="5">
-        <v>36.799999999999997</v>
+        <v>148.21</v>
       </c>
       <c r="F138" s="5">
-        <f t="shared" si="5"/>
-        <v>36.799999999999997</v>
+        <f t="shared" si="6"/>
+        <v>148.21</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D139" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E139" s="5">
-        <v>21.21</v>
+        <v>348.45</v>
       </c>
       <c r="F139" s="5">
-        <f t="shared" si="5"/>
-        <v>42.42</v>
+        <f t="shared" si="6"/>
+        <v>348.45</v>
+      </c>
+      <c r="I139" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D140" s="3">
         <v>1</v>
       </c>
       <c r="E140" s="5">
-        <v>304.75</v>
+        <v>60.95</v>
       </c>
       <c r="F140" s="5">
-        <f t="shared" si="5"/>
-        <v>304.75</v>
-      </c>
-      <c r="I140" s="3" t="s">
-        <v>102</v>
+        <f t="shared" si="6"/>
+        <v>60.95</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D141" s="3">
         <v>1</v>
       </c>
       <c r="E141" s="5">
-        <v>148.21</v>
+        <v>34.5</v>
       </c>
       <c r="F141" s="5">
-        <f t="shared" si="5"/>
-        <v>148.21</v>
+        <f t="shared" si="6"/>
+        <v>34.5</v>
       </c>
       <c r="I141" s="3" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D142" s="3">
         <v>1</v>
       </c>
       <c r="E142" s="5">
-        <v>348.45</v>
+        <v>51.45</v>
       </c>
       <c r="F142" s="5">
-        <f t="shared" si="5"/>
-        <v>348.45</v>
+        <f t="shared" si="6"/>
+        <v>51.45</v>
       </c>
       <c r="I142" s="3" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="D143" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E143" s="5">
-        <v>60.95</v>
+        <v>13.8</v>
       </c>
       <c r="F143" s="5">
-        <f t="shared" si="5"/>
-        <v>60.95</v>
+        <f t="shared" si="6"/>
+        <v>27.6</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D144" s="3">
         <v>1</v>
       </c>
       <c r="E144" s="5">
-        <v>34.5</v>
+        <v>19.09</v>
       </c>
       <c r="F144" s="5">
-        <f t="shared" si="5"/>
-        <v>34.5</v>
-      </c>
-      <c r="I144" s="3" t="s">
-        <v>111</v>
+        <f t="shared" si="6"/>
+        <v>19.09</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D145" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E145" s="5">
-        <v>51.45</v>
+        <v>40.51</v>
       </c>
       <c r="F145" s="5">
-        <f t="shared" si="5"/>
-        <v>51.45</v>
+        <f t="shared" si="6"/>
+        <v>81.02</v>
       </c>
       <c r="I145" s="3" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D146" s="3">
         <v>2</v>
       </c>
       <c r="E146" s="5">
-        <v>13.8</v>
+        <v>83.598116000000005</v>
       </c>
       <c r="F146" s="5">
-        <f t="shared" si="5"/>
-        <v>27.6</v>
+        <f t="shared" si="6"/>
+        <v>167.19623200000001</v>
+      </c>
+      <c r="I146" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D147" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E147" s="5">
-        <v>19.09</v>
+        <v>70.103999999999999</v>
       </c>
       <c r="F147" s="5">
-        <f t="shared" si="5"/>
-        <v>19.09</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>280.416</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D148" s="3">
         <v>2</v>
       </c>
       <c r="E148" s="5">
-        <v>40.51</v>
+        <v>28.75</v>
       </c>
       <c r="F148" s="5">
-        <f t="shared" si="5"/>
-        <v>81.02</v>
-      </c>
-      <c r="I148" s="3" t="s">
-        <v>120</v>
+        <f t="shared" si="6"/>
+        <v>57.5</v>
+      </c>
+      <c r="I148" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D149" s="3">
         <v>2</v>
       </c>
       <c r="E149" s="5">
-        <v>83.598116000000005</v>
+        <v>38.872799999999998</v>
       </c>
       <c r="F149" s="5">
-        <f t="shared" si="5"/>
-        <v>167.19623200000001</v>
-      </c>
-      <c r="I149" s="3" t="s">
-        <v>111</v>
+        <f t="shared" si="6"/>
+        <v>77.745599999999996</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A150" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="B150" s="3" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="D150" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E150" s="5">
-        <v>70.103999999999999</v>
+        <v>205</v>
       </c>
       <c r="F150" s="5">
-        <f t="shared" si="5"/>
-        <v>280.416</v>
+        <f t="shared" si="6"/>
+        <v>205</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A151" s="3" t="s">
-        <v>125</v>
-      </c>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B151" s="3" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="D151" s="3">
         <v>2</v>
       </c>
       <c r="E151" s="5">
-        <v>28.75</v>
+        <v>12</v>
       </c>
       <c r="F151" s="5">
-        <f t="shared" si="5"/>
-        <v>57.5</v>
-      </c>
-      <c r="I151" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A152" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C152" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D152" s="3">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="I151" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A152" s="11"/>
+      <c r="B152" s="11"/>
+      <c r="C152" s="10"/>
+    </row>
+    <row r="153" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A153" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F153" s="9"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D154" s="3">
+        <v>4</v>
+      </c>
+      <c r="E154" s="5">
+        <v>16.5</v>
+      </c>
+      <c r="F154" s="5">
+        <f t="shared" ref="F154:F170" si="7">E154*D154</f>
+        <v>66</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D155" s="3">
         <v>2</v>
       </c>
-      <c r="E152" s="5">
-        <v>38.872799999999998</v>
-      </c>
-      <c r="F152" s="5">
-        <f t="shared" si="5"/>
-        <v>77.745599999999996</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B153" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D153" s="3">
-        <v>1</v>
-      </c>
-      <c r="E153" s="5">
-        <v>205</v>
-      </c>
-      <c r="F153" s="5">
-        <f t="shared" si="5"/>
-        <v>205</v>
-      </c>
-      <c r="I153" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B154" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D154" s="3">
-        <v>2</v>
-      </c>
-      <c r="E154" s="5">
-        <v>12</v>
-      </c>
-      <c r="F154" s="5">
-        <f t="shared" si="5"/>
-        <v>24</v>
-      </c>
-      <c r="I154" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A155" s="11"/>
-      <c r="B155" s="11"/>
-      <c r="C155" s="10"/>
-    </row>
-    <row r="156" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A156" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F156" s="9"/>
+      <c r="E155" s="5">
+        <v>140</v>
+      </c>
+      <c r="F155" s="5">
+        <f t="shared" si="7"/>
+        <v>280</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D156" s="3">
+        <v>1</v>
+      </c>
+      <c r="E156" s="5">
+        <v>85.1</v>
+      </c>
+      <c r="F156" s="5">
+        <f t="shared" si="7"/>
+        <v>85.1</v>
+      </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>136</v>
+        <v>83</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="D157" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E157" s="5">
-        <v>16.5</v>
+        <v>32</v>
       </c>
       <c r="F157" s="5">
-        <f t="shared" ref="F157:F173" si="6">E157*D157</f>
-        <v>66</v>
+        <f t="shared" si="7"/>
+        <v>64</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>140</v>
+        <v>83</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="D158" s="3">
         <v>2</v>
       </c>
       <c r="E158" s="5">
-        <v>140</v>
+        <v>51.58</v>
       </c>
       <c r="F158" s="5">
-        <f t="shared" si="6"/>
-        <v>280</v>
-      </c>
-      <c r="I158" s="3" t="s">
-        <v>142</v>
+        <f t="shared" si="7"/>
+        <v>103.16</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="D159" s="3">
         <v>1</v>
       </c>
       <c r="E159" s="5">
-        <v>85.1</v>
+        <v>60</v>
       </c>
       <c r="F159" s="5">
-        <f t="shared" si="6"/>
-        <v>85.1</v>
+        <f t="shared" si="7"/>
+        <v>60</v>
+      </c>
+      <c r="I159" s="3" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="D160" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E160" s="5">
-        <v>32</v>
+        <v>136.47999999999999</v>
       </c>
       <c r="F160" s="5">
-        <f t="shared" si="6"/>
-        <v>64</v>
-      </c>
-      <c r="I160" s="3" t="s">
-        <v>154</v>
+        <f t="shared" si="7"/>
+        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D161" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E161" s="5">
-        <v>51.58</v>
+        <v>136.47999999999999</v>
       </c>
       <c r="F161" s="5">
-        <f t="shared" si="6"/>
-        <v>103.16</v>
+        <f t="shared" si="7"/>
+        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D162" s="3">
         <v>1</v>
       </c>
       <c r="E162" s="5">
-        <v>60</v>
+        <v>60.95</v>
       </c>
       <c r="F162" s="5">
-        <f t="shared" si="6"/>
-        <v>60</v>
-      </c>
-      <c r="I162" s="3" t="s">
-        <v>159</v>
+        <f t="shared" si="7"/>
+        <v>60.95</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D163" s="3">
         <v>1</v>
       </c>
       <c r="E163" s="5">
-        <v>136.47999999999999</v>
+        <v>119.416</v>
       </c>
       <c r="F163" s="5">
-        <f t="shared" si="6"/>
-        <v>136.47999999999999</v>
+        <f t="shared" si="7"/>
+        <v>119.416</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D164" s="3">
         <v>1</v>
       </c>
       <c r="E164" s="5">
-        <v>136.47999999999999</v>
+        <v>105.8</v>
       </c>
       <c r="F164" s="5">
-        <f t="shared" si="6"/>
-        <v>136.47999999999999</v>
+        <f t="shared" si="7"/>
+        <v>105.8</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D165" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E165" s="5">
-        <v>60.95</v>
+        <v>119.6</v>
       </c>
       <c r="F165" s="5">
-        <f t="shared" si="6"/>
-        <v>60.95</v>
+        <f t="shared" si="7"/>
+        <v>239.2</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>165</v>
+        <v>405</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>166</v>
+        <v>406</v>
       </c>
       <c r="D166" s="3">
         <v>1</v>
       </c>
       <c r="E166" s="5">
-        <v>119.416</v>
+        <v>100</v>
       </c>
       <c r="F166" s="5">
-        <f t="shared" si="6"/>
-        <v>119.416</v>
+        <f t="shared" si="7"/>
+        <v>100</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D167" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E167" s="5">
-        <v>105.8</v>
+        <v>92</v>
       </c>
       <c r="F167" s="5">
-        <f t="shared" si="6"/>
-        <v>105.8</v>
+        <f t="shared" si="7"/>
+        <v>184</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D168" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E168" s="5">
-        <v>119.6</v>
+        <v>96.23</v>
       </c>
       <c r="F168" s="5">
-        <f t="shared" si="6"/>
-        <v>239.2</v>
+        <f t="shared" si="7"/>
+        <v>96.23</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>418</v>
+        <v>175</v>
       </c>
       <c r="B169" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>419</v>
+        <v>176</v>
       </c>
       <c r="D169" s="3">
         <v>1</v>
       </c>
       <c r="E169" s="5">
-        <v>100</v>
+        <v>102.44</v>
       </c>
       <c r="F169" s="5">
-        <f t="shared" si="6"/>
-        <v>100</v>
+        <f t="shared" si="7"/>
+        <v>102.44</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="D170" s="3">
         <v>2</v>
       </c>
       <c r="E170" s="5">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="F170" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C171" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D171" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C172" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D172" s="3">
+        <v>1</v>
+      </c>
+      <c r="I172" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C173" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D173" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A177" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C177" s="7"/>
+      <c r="E177" s="18"/>
+      <c r="F177" s="18"/>
+    </row>
+    <row r="178" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B178" s="3" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A171" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D171" s="3">
-        <v>1</v>
-      </c>
-      <c r="E171" s="5">
-        <v>96.23</v>
-      </c>
-      <c r="F171" s="5">
-        <f t="shared" si="6"/>
-        <v>96.23</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A172" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D172" s="3">
-        <v>1</v>
-      </c>
-      <c r="E172" s="5">
-        <v>102.44</v>
-      </c>
-      <c r="F172" s="5">
-        <f t="shared" si="6"/>
-        <v>102.44</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A173" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D173" s="3">
+      <c r="C178" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="D178" s="3">
+        <v>1</v>
+      </c>
+      <c r="G178" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I178" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J178" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K178" s="4"/>
+    </row>
+    <row r="179" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B179" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C179" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="D179" s="3">
+        <v>1</v>
+      </c>
+      <c r="G179" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I179" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J179" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K179" s="4"/>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B180" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C180" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="D180" s="3">
         <v>2</v>
       </c>
-      <c r="E173" s="5">
-        <v>28</v>
-      </c>
-      <c r="F173" s="5">
-        <f t="shared" si="6"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C174" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D174" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C175" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D175" s="3">
-        <v>1</v>
-      </c>
-      <c r="I175" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C176" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="D176" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="180" spans="1:11" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A180" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C180" s="7"/>
-      <c r="E180" s="18"/>
-      <c r="F180" s="18"/>
-    </row>
-    <row r="181" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G180" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I180" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="J180" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B181" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C181" s="19" t="s">
-        <v>185</v>
+      <c r="C181" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D181" s="3">
         <v>1</v>
       </c>
       <c r="G181" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="I181" s="3" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="J181" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="K181" s="4"/>
-    </row>
-    <row r="182" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B182" s="3" t="s">
         <v>184</v>
       </c>
       <c r="C182" s="19" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D182" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="I182" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J182" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="K182" s="4"/>
+        <v>196</v>
+      </c>
+      <c r="J182" s="19" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B183" s="3" t="s">
         <v>184</v>
       </c>
       <c r="C183" s="19" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D183" s="3">
         <v>2</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="I183" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="J183" s="3" t="s">
-        <v>188</v>
+        <v>199</v>
+      </c>
+      <c r="J183" s="19" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B184" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C184" s="3" t="s">
-        <v>192</v>
+      <c r="C184" s="19" t="s">
+        <v>200</v>
       </c>
       <c r="D184" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="J184" s="3" t="s">
-        <v>188</v>
+        <v>195</v>
+      </c>
+      <c r="I184" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="J184" s="19" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B185" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C185" s="19" t="s">
-        <v>194</v>
+      <c r="C185" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="D185" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G185" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="I185" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="J185" s="19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B186" s="3" t="s">
+      <c r="J185" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A186" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B186" s="19" t="s">
         <v>184</v>
       </c>
       <c r="C186" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="D186" s="3">
-        <v>2</v>
-      </c>
-      <c r="G186" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D186" s="19">
+        <v>10</v>
+      </c>
+      <c r="F186" s="55"/>
+      <c r="G186" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="I186" s="3" t="s">
-        <v>199</v>
+      <c r="I186" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="J186" s="19" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B187" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C187" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="D187" s="3">
-        <v>2</v>
-      </c>
-      <c r="G187" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="I187" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="J187" s="19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B188" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D188" s="3">
-        <v>1</v>
-      </c>
-      <c r="G188" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="J188" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="189" spans="1:11" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A189" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="B189" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="C189" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="D189" s="19">
-        <v>10</v>
-      </c>
-      <c r="F189" s="55"/>
-      <c r="G189" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="I189" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="J189" s="19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="191" spans="1:11" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A191" s="8" t="s">
+    <row r="188" spans="1:11" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A188" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="B191" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="E191" s="9"/>
-      <c r="F191" s="9"/>
+      <c r="B188" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="E188" s="9"/>
+      <c r="F188" s="9"/>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B189" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="D189" s="3">
+        <v>0</v>
+      </c>
+      <c r="E189" s="5">
+        <v>518.5</v>
+      </c>
+      <c r="F189" s="5">
+        <f t="shared" ref="F189:F199" si="8">E189*D189</f>
+        <v>0</v>
+      </c>
+      <c r="I189" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B190" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="D190" s="3">
+        <v>0</v>
+      </c>
+      <c r="E190" s="5">
+        <v>764</v>
+      </c>
+      <c r="F190" s="5">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B191" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="D191" s="3">
+        <v>0</v>
+      </c>
+      <c r="E191" s="5">
+        <v>816</v>
+      </c>
+      <c r="F191" s="5">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I191" s="3" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="D192" s="3">
         <v>0</v>
       </c>
       <c r="E192" s="5">
-        <v>518.5</v>
+        <v>952</v>
       </c>
       <c r="F192" s="5">
-        <f t="shared" ref="F192:F202" si="7">E192*D192</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="I192" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="193" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="193" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="D193" s="3">
         <v>0</v>
       </c>
       <c r="E193" s="5">
-        <v>764</v>
+        <v>99.5</v>
       </c>
       <c r="F193" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="D194" s="3">
         <v>0</v>
       </c>
       <c r="E194" s="5">
-        <v>816</v>
+        <v>128.5</v>
       </c>
       <c r="F194" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="I194" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="195" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="195" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="D195" s="3">
         <v>0</v>
       </c>
       <c r="E195" s="5">
-        <v>952</v>
+        <v>156</v>
       </c>
       <c r="F195" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="D196" s="3">
         <v>0</v>
       </c>
       <c r="E196" s="5">
-        <v>99.5</v>
+        <v>184.5</v>
       </c>
       <c r="F196" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="D197" s="3">
         <v>0</v>
       </c>
       <c r="E197" s="5">
-        <v>128.5</v>
+        <v>106.5</v>
       </c>
       <c r="F197" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="D198" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E198" s="5">
-        <v>156</v>
+        <v>106.5</v>
       </c>
       <c r="F198" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199" spans="2:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>639</v>
+      </c>
+    </row>
+    <row r="199" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="D199" s="3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E199" s="5">
-        <v>184.5</v>
+        <v>121.5</v>
       </c>
       <c r="F199" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B200" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C200" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D200" s="3">
-        <v>0</v>
-      </c>
-      <c r="E200" s="5">
-        <v>106.5</v>
-      </c>
-      <c r="F200" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B201" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C201" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="D201" s="3">
-        <v>6</v>
-      </c>
-      <c r="E201" s="5">
-        <v>106.5</v>
-      </c>
-      <c r="F201" s="5">
-        <f t="shared" si="7"/>
-        <v>639</v>
-      </c>
-    </row>
-    <row r="202" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B202" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="D202" s="3">
-        <v>10</v>
-      </c>
-      <c r="E202" s="5">
-        <v>121.5</v>
+        <f t="shared" si="8"/>
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="202" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E202" s="21" t="s">
+        <v>208</v>
       </c>
       <c r="F202" s="5">
-        <f t="shared" si="7"/>
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="205" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E205" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="F205" s="5">
-        <f>SUM(F3:F203)</f>
-        <v>99111.533987999996</v>
+        <f>SUM(F3:F200)</f>
+        <v>99506.533987999996</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C105" r:id="rId1" xr:uid="{3BC0AF99-F679-46A9-B7F9-6A136F582C78}"/>
+    <hyperlink ref="C102" r:id="rId1" xr:uid="{3BC0AF99-F679-46A9-B7F9-6A136F582C78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
galvo fans with 60 mm cage mounts
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13C9DBA-C156-42C5-9FF2-6F6792D1DB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9268E1-B5D2-4C90-83A7-E1A3CFD11ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8352" yWindow="3984" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8652" yWindow="4272" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="437">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -1259,9 +1259,6 @@
     <t>UG-205 10x20x45</t>
   </si>
   <si>
-    <t>Material: glass, RI=1.52. For quartz  (e.g. CLARITY imaging, RI=1.47), replace UG qwith UQ in the part name.</t>
-  </si>
-  <si>
     <t>Depending on the laser control interface (Oxxius: SMB).</t>
   </si>
   <si>
@@ -1371,6 +1368,42 @@
   </si>
   <si>
     <t>GPWR15 (unsafe)</t>
+  </si>
+  <si>
+    <t>Material: glass, RI=1.52. For quartz  (e.g. CLARITY imaging, RI=1.47), replace UG with UQ in the part name.</t>
+  </si>
+  <si>
+    <t>Fan-mount-modified-Thorlabs-CagePlate-LCP03.ipt</t>
+  </si>
+  <si>
+    <t>Fan mount for galvos</t>
+  </si>
+  <si>
+    <t>3D printed or machined</t>
+  </si>
+  <si>
+    <t>5912-412JHHU</t>
+  </si>
+  <si>
+    <t>Barrel connector for galvo fan</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Cooling of the galvo is essential</t>
+  </si>
+  <si>
+    <t>Fan for galvo: 40x40x25mm, 12V DC, 0.25A, dust-protected (IP rating 68)</t>
+  </si>
+  <si>
+    <t>Power connector for two fans</t>
+  </si>
+  <si>
+    <t>12V, 1A power supply, barrel jack connector</t>
+  </si>
+  <si>
+    <t>Power supply for the galvo fans</t>
   </si>
 </sst>
 </file>
@@ -2059,10 +2092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K202"/>
+  <dimension ref="A1:K206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2255,7 +2288,7 @@
       </c>
       <c r="G11" s="50"/>
       <c r="I11" s="38" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2931,7 +2964,7 @@
     </row>
     <row r="42" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="42" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B42" s="41" t="s">
         <v>83</v>
@@ -2958,7 +2991,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>251</v>
@@ -3002,7 +3035,7 @@
         <v>400</v>
       </c>
       <c r="F44" s="5">
-        <f t="shared" ref="F44:F71" si="2">E44*D44</f>
+        <f t="shared" ref="F44:F75" si="2">E44*D44</f>
         <v>800</v>
       </c>
       <c r="G44" s="3" t="s">
@@ -3147,7 +3180,7 @@
         <v>269</v>
       </c>
       <c r="I49" s="45" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -3174,7 +3207,7 @@
         <v>269</v>
       </c>
       <c r="I50" s="45" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -3389,13 +3422,13 @@
     </row>
     <row r="59" spans="1:9" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="44" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B59" s="41" t="s">
         <v>309</v>
       </c>
       <c r="C59" s="44" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D59" s="45">
         <v>2</v>
@@ -3411,7 +3444,7 @@
         <v>294</v>
       </c>
       <c r="I59" s="45" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -3443,7 +3476,7 @@
     </row>
     <row r="61" spans="1:9" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="42" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B61" s="41" t="s">
         <v>83</v>
@@ -3465,7 +3498,7 @@
         <v>297</v>
       </c>
       <c r="I61" s="47" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -3485,7 +3518,7 @@
         <v>2104</v>
       </c>
       <c r="F62" s="52">
-        <f t="shared" ref="F62:F67" si="3">E62*D62</f>
+        <f t="shared" ref="F62:F71" si="3">E62*D62</f>
         <v>4208</v>
       </c>
       <c r="H62" s="41" t="s">
@@ -3521,7 +3554,7 @@
     </row>
     <row r="64" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="59" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B64" s="41" t="s">
         <v>83</v>
@@ -3543,12 +3576,12 @@
         <v>297</v>
       </c>
       <c r="I64" s="41" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="65" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="59" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B65" s="41" t="s">
         <v>83</v>
@@ -3570,18 +3603,18 @@
         <v>297</v>
       </c>
       <c r="I65" s="41" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="42" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B66" s="41" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C66" s="42" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D66" s="41">
         <v>14</v>
@@ -3597,18 +3630,18 @@
         <v>297</v>
       </c>
       <c r="I66" s="47" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="67" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="58" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B67" s="41" t="s">
         <v>363</v>
       </c>
       <c r="C67" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D67" s="41">
         <v>1</v>
@@ -3624,236 +3657,259 @@
         <v>297</v>
       </c>
       <c r="I67" s="41" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="68" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="42" t="s">
-        <v>298</v>
+        <v>426</v>
       </c>
       <c r="B68" s="41" t="s">
-        <v>83</v>
+        <v>309</v>
       </c>
       <c r="C68" s="42" t="s">
-        <v>299</v>
+        <v>427</v>
       </c>
       <c r="D68" s="41">
         <v>2</v>
       </c>
       <c r="E68" s="43">
+        <v>5</v>
+      </c>
+      <c r="F68" s="52">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="H68" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I68" s="41" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="42" t="s">
+        <v>429</v>
+      </c>
+      <c r="B69" s="41" t="s">
+        <v>363</v>
+      </c>
+      <c r="C69" s="42" t="s">
+        <v>433</v>
+      </c>
+      <c r="D69" s="41">
+        <v>2</v>
+      </c>
+      <c r="E69" s="43">
+        <v>62</v>
+      </c>
+      <c r="F69" s="52">
+        <f t="shared" si="3"/>
+        <v>124</v>
+      </c>
+      <c r="H69" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I69" s="41" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="47" t="s">
+        <v>431</v>
+      </c>
+      <c r="B70" s="41" t="s">
+        <v>363</v>
+      </c>
+      <c r="C70" s="42" t="s">
+        <v>430</v>
+      </c>
+      <c r="D70" s="41">
+        <v>1</v>
+      </c>
+      <c r="E70" s="43">
+        <v>2</v>
+      </c>
+      <c r="F70" s="52">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="H70" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I70" s="41" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="47" t="s">
+        <v>431</v>
+      </c>
+      <c r="B71" s="41" t="s">
+        <v>363</v>
+      </c>
+      <c r="C71" s="42" t="s">
+        <v>435</v>
+      </c>
+      <c r="D71" s="41">
+        <v>1</v>
+      </c>
+      <c r="E71" s="43">
+        <v>15</v>
+      </c>
+      <c r="F71" s="52">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="H71" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I71" s="41" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="42" t="s">
+        <v>298</v>
+      </c>
+      <c r="B72" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C72" s="42" t="s">
+        <v>299</v>
+      </c>
+      <c r="D72" s="41">
+        <v>2</v>
+      </c>
+      <c r="E72" s="43">
         <v>25</v>
       </c>
-      <c r="F68" s="52">
+      <c r="F72" s="52">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="H68" s="41" t="s">
+      <c r="H72" s="41" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="69" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="48" t="s">
+    <row r="73" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="48" t="s">
         <v>302</v>
       </c>
-      <c r="B69" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C69" s="42" t="s">
+      <c r="B73" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C73" s="42" t="s">
         <v>303</v>
       </c>
-      <c r="D69" s="41">
+      <c r="D73" s="41">
         <v>2</v>
       </c>
-      <c r="E69" s="43">
+      <c r="E73" s="43">
         <v>35</v>
       </c>
-      <c r="F69" s="52">
+      <c r="F73" s="52">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="H69" s="41" t="s">
+      <c r="H73" s="41" t="s">
         <v>300</v>
       </c>
-      <c r="I69" s="47" t="s">
+      <c r="I73" s="47" t="s">
         <v>308</v>
       </c>
-      <c r="J69" s="49" t="s">
+      <c r="J73" s="49" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="42" t="s">
+    <row r="74" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="42" t="s">
         <v>301</v>
       </c>
-      <c r="B70" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70" s="42" t="s">
+      <c r="B74" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C74" s="42" t="s">
         <v>304</v>
       </c>
-      <c r="D70" s="41">
+      <c r="D74" s="41">
         <v>2</v>
       </c>
-      <c r="E70" s="43">
+      <c r="E74" s="43">
         <v>92</v>
       </c>
-      <c r="F70" s="52">
+      <c r="F74" s="52">
         <f t="shared" si="2"/>
         <v>184</v>
       </c>
-      <c r="H70" s="41" t="s">
+      <c r="H74" s="41" t="s">
         <v>300</v>
       </c>
-      <c r="I70" s="41" t="s">
+      <c r="I74" s="41" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="71" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="42" t="s">
+    <row r="75" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="42" t="s">
         <v>377</v>
       </c>
-      <c r="B71" s="41" t="s">
+      <c r="B75" s="41" t="s">
         <v>309</v>
       </c>
-      <c r="C71" s="56" t="s">
+      <c r="C75" s="56" t="s">
         <v>362</v>
       </c>
-      <c r="D71" s="41">
+      <c r="D75" s="41">
         <v>2</v>
       </c>
-      <c r="E71" s="43">
-        <v>1</v>
-      </c>
-      <c r="F71" s="52">
+      <c r="E75" s="43">
+        <v>1</v>
+      </c>
+      <c r="F75" s="52">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H71" s="41" t="s">
+      <c r="H75" s="41" t="s">
         <v>300</v>
       </c>
-      <c r="I71" s="41" t="s">
+      <c r="I75" s="41" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="72" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="42"/>
-      <c r="C72" s="42"/>
-      <c r="E72" s="43"/>
-      <c r="F72" s="52"/>
-    </row>
-    <row r="73" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="42"/>
-      <c r="C73" s="42"/>
-      <c r="E73" s="43"/>
-      <c r="F73" s="52"/>
-    </row>
-    <row r="74" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="42"/>
-      <c r="C74" s="42"/>
-      <c r="E74" s="43"/>
-      <c r="F74" s="52"/>
-    </row>
-    <row r="75" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-    </row>
     <row r="76" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="B76" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="C76" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="D76" s="41">
-        <v>1</v>
-      </c>
+      <c r="A76" s="42"/>
+      <c r="C76" s="42"/>
       <c r="E76" s="43"/>
       <c r="F76" s="52"/>
-      <c r="I76" s="41" t="s">
-        <v>334</v>
-      </c>
     </row>
     <row r="77" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="42" t="s">
-        <v>326</v>
-      </c>
-      <c r="B77" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C77" s="42" t="s">
-        <v>327</v>
-      </c>
-      <c r="D77" s="41">
-        <v>1</v>
-      </c>
-      <c r="E77" s="43">
-        <v>63</v>
-      </c>
-      <c r="F77" s="52">
-        <f>D77*E77</f>
-        <v>63</v>
-      </c>
+      <c r="A77" s="42"/>
+      <c r="C77" s="42"/>
+      <c r="E77" s="43"/>
+      <c r="F77" s="52"/>
     </row>
     <row r="78" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="48" t="s">
-        <v>331</v>
-      </c>
-      <c r="B78" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C78" s="42" t="s">
-        <v>332</v>
-      </c>
-      <c r="D78" s="41">
-        <v>2</v>
-      </c>
-      <c r="E78" s="43">
-        <v>69</v>
-      </c>
-      <c r="F78" s="52">
-        <f>D78*E78</f>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="42" t="s">
-        <v>329</v>
-      </c>
-      <c r="B79" s="41" t="s">
-        <v>328</v>
-      </c>
-      <c r="C79" s="42" t="s">
-        <v>330</v>
-      </c>
-      <c r="D79" s="41">
-        <v>1</v>
-      </c>
-      <c r="E79" s="43">
-        <v>10</v>
-      </c>
-      <c r="F79" s="52">
-        <f>D79*E79</f>
-        <v>10</v>
-      </c>
-      <c r="I79" s="41" t="s">
-        <v>333</v>
-      </c>
+      <c r="A78" s="42"/>
+      <c r="C78" s="42"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="52"/>
+    </row>
+    <row r="79" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A79" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
     </row>
     <row r="80" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="41" t="s">
-        <v>25</v>
+      <c r="A80" s="42" t="s">
+        <v>29</v>
       </c>
       <c r="B80" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C80" s="41" t="s">
-        <v>26</v>
+      <c r="C80" s="42" t="s">
+        <v>24</v>
       </c>
       <c r="D80" s="41">
         <v>1</v>
@@ -3864,370 +3920,347 @@
         <v>334</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="6" t="s">
-        <v>409</v>
-      </c>
-      <c r="E81" s="9"/>
-      <c r="F81" s="9"/>
-    </row>
-    <row r="82" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="8" t="s">
+    <row r="81" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="42" t="s">
+        <v>326</v>
+      </c>
+      <c r="B81" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C81" s="42" t="s">
+        <v>327</v>
+      </c>
+      <c r="D81" s="41">
+        <v>1</v>
+      </c>
+      <c r="E81" s="43">
+        <v>63</v>
+      </c>
+      <c r="F81" s="52">
+        <f>D81*E81</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="48" t="s">
+        <v>331</v>
+      </c>
+      <c r="B82" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C82" s="42" t="s">
+        <v>332</v>
+      </c>
+      <c r="D82" s="41">
+        <v>2</v>
+      </c>
+      <c r="E82" s="43">
+        <v>69</v>
+      </c>
+      <c r="F82" s="52">
+        <f>D82*E82</f>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="42" t="s">
+        <v>329</v>
+      </c>
+      <c r="B83" s="41" t="s">
+        <v>328</v>
+      </c>
+      <c r="C83" s="42" t="s">
+        <v>330</v>
+      </c>
+      <c r="D83" s="41">
+        <v>1</v>
+      </c>
+      <c r="E83" s="43">
+        <v>10</v>
+      </c>
+      <c r="F83" s="52">
+        <f>D83*E83</f>
+        <v>10</v>
+      </c>
+      <c r="I83" s="41" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B84" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D84" s="41">
+        <v>1</v>
+      </c>
+      <c r="E84" s="43"/>
+      <c r="F84" s="52"/>
+      <c r="I84" s="41" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A85" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+    </row>
+    <row r="86" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+    </row>
+    <row r="87" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+    </row>
+    <row r="88" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" s="3">
+        <v>1</v>
+      </c>
+      <c r="E88" s="5">
+        <v>250</v>
+      </c>
+      <c r="F88" s="5">
+        <f>E88*D88</f>
+        <v>250</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J88" s="4"/>
+    </row>
+    <row r="89" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="D89" s="3">
+        <v>1</v>
+      </c>
+      <c r="E89" s="5">
+        <v>13</v>
+      </c>
+      <c r="F89" s="5">
+        <f>E89*D89</f>
+        <v>13</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J89" s="4"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="D90" s="3">
+        <v>1</v>
+      </c>
+      <c r="E90" s="5">
+        <v>43</v>
+      </c>
+      <c r="F90" s="5">
+        <f>E90*D90</f>
+        <v>43</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D91" s="3">
+        <v>1</v>
+      </c>
+      <c r="I91" s="41" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="E82" s="9"/>
-      <c r="F82" s="9"/>
-    </row>
-    <row r="83" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
-    </row>
-    <row r="84" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D84" s="3">
-        <v>1</v>
-      </c>
-      <c r="E84" s="5">
-        <v>250</v>
-      </c>
-      <c r="F84" s="5">
-        <f>E84*D84</f>
-        <v>250</v>
-      </c>
-      <c r="G84" s="3" t="s">
+      <c r="C92" s="57" t="s">
+        <v>380</v>
+      </c>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+    </row>
+    <row r="93" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+    </row>
+    <row r="94" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="42" t="s">
+        <v>357</v>
+      </c>
+      <c r="B94" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C94" s="42" t="s">
+        <v>358</v>
+      </c>
+      <c r="D94" s="41">
+        <v>0</v>
+      </c>
+      <c r="E94" s="43">
+        <v>656</v>
+      </c>
+      <c r="F94" s="52">
+        <f>E94*D94</f>
+        <v>0</v>
+      </c>
+      <c r="I94" s="49"/>
+    </row>
+    <row r="95" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="42" t="s">
+        <v>355</v>
+      </c>
+      <c r="B95" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C95" s="42" t="s">
+        <v>356</v>
+      </c>
+      <c r="D95" s="41">
+        <v>0</v>
+      </c>
+      <c r="E95" s="43">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="F95" s="52">
+        <f>E95*D95</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="B96" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="D96" s="3">
+        <v>0</v>
+      </c>
+      <c r="E96" s="12">
+        <v>4.87</v>
+      </c>
+      <c r="F96" s="52">
+        <f>E96*D96</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="22" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="F97" s="54"/>
+    </row>
+    <row r="98" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="F98" s="54"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D99" s="3">
+        <v>1</v>
+      </c>
+      <c r="E99" s="5">
+        <v>1075</v>
+      </c>
+      <c r="F99" s="5">
+        <f t="shared" ref="F99:F104" si="4">E99*D99</f>
+        <v>1075</v>
+      </c>
+      <c r="G99" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H84" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J84" s="4"/>
-    </row>
-    <row r="85" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="D85" s="3">
-        <v>1</v>
-      </c>
-      <c r="E85" s="5">
-        <v>13</v>
-      </c>
-      <c r="F85" s="5">
-        <f>E85*D85</f>
-        <v>13</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J85" s="4"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="D86" s="3">
-        <v>1</v>
-      </c>
-      <c r="E86" s="5">
-        <v>43</v>
-      </c>
-      <c r="F86" s="5">
-        <f>E86*D86</f>
-        <v>43</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="D87" s="3">
-        <v>1</v>
-      </c>
-      <c r="I87" s="41" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="C88" s="57" t="s">
-        <v>380</v>
-      </c>
-      <c r="E88" s="9"/>
-      <c r="F88" s="9"/>
-    </row>
-    <row r="89" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="E89" s="9"/>
-      <c r="F89" s="9"/>
-    </row>
-    <row r="90" spans="1:10" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="42" t="s">
-        <v>357</v>
-      </c>
-      <c r="B90" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C90" s="42" t="s">
-        <v>358</v>
-      </c>
-      <c r="D90" s="41">
-        <v>0</v>
-      </c>
-      <c r="E90" s="43">
-        <v>656</v>
-      </c>
-      <c r="F90" s="52">
-        <f>E90*D90</f>
-        <v>0</v>
-      </c>
-      <c r="I90" s="49"/>
-    </row>
-    <row r="91" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="42" t="s">
-        <v>355</v>
-      </c>
-      <c r="B91" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C91" s="42" t="s">
-        <v>356</v>
-      </c>
-      <c r="D91" s="41">
-        <v>0</v>
-      </c>
-      <c r="E91" s="43">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="F91" s="52">
-        <f>E91*D91</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="B92" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="D92" s="3">
-        <v>0</v>
-      </c>
-      <c r="E92" s="12">
-        <v>4.87</v>
-      </c>
-      <c r="F92" s="52">
-        <f>E92*D92</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" s="22" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="F93" s="54"/>
-    </row>
-    <row r="94" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="F94" s="54"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D95" s="3">
-        <v>1</v>
-      </c>
-      <c r="E95" s="5">
-        <v>1075</v>
-      </c>
-      <c r="F95" s="5">
-        <f t="shared" ref="F95:F100" si="4">E95*D95</f>
-        <v>1075</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I95" s="3" t="s">
+      <c r="I99" s="3" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="B96" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C96" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D96" s="38">
-        <v>0</v>
-      </c>
-      <c r="E96" s="39">
-        <v>1350</v>
-      </c>
-      <c r="F96" s="39">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G96" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="I96" s="38" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="B97" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C97" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="D97" s="38">
-        <v>0</v>
-      </c>
-      <c r="E97" s="39">
-        <v>1350</v>
-      </c>
-      <c r="F97" s="39">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G97" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="I97" s="38" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B98" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C98" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="D98" s="38">
-        <v>0</v>
-      </c>
-      <c r="E98" s="40">
-        <v>1445</v>
-      </c>
-      <c r="F98" s="39">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G98" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="I98" s="38" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="B99" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C99" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="D99" s="38">
-        <v>0</v>
-      </c>
-      <c r="E99" s="39">
-        <v>1130</v>
-      </c>
-      <c r="F99" s="39">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G99" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="I99" s="38" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="38" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B100" s="38" t="s">
         <v>59</v>
       </c>
       <c r="C100" s="38" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D100" s="38">
         <v>0</v>
       </c>
       <c r="E100" s="39">
-        <v>1130</v>
+        <v>1350</v>
       </c>
       <c r="F100" s="39">
         <f t="shared" si="4"/>
@@ -4240,1496 +4273,1527 @@
         <v>215</v>
       </c>
     </row>
-    <row r="101" spans="1:9" s="30" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A101" s="29" t="s">
+    <row r="101" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B101" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C101" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D101" s="38">
+        <v>0</v>
+      </c>
+      <c r="E101" s="39">
+        <v>1350</v>
+      </c>
+      <c r="F101" s="39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G101" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="I101" s="38" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B102" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C102" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D102" s="38">
+        <v>0</v>
+      </c>
+      <c r="E102" s="40">
+        <v>1445</v>
+      </c>
+      <c r="F102" s="39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G102" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="I102" s="38" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B103" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C103" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D103" s="38">
+        <v>0</v>
+      </c>
+      <c r="E103" s="39">
+        <v>1130</v>
+      </c>
+      <c r="F103" s="39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G103" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="I103" s="38" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B104" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C104" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D104" s="38">
+        <v>0</v>
+      </c>
+      <c r="E104" s="39">
+        <v>1130</v>
+      </c>
+      <c r="F104" s="39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G104" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="I104" s="38" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" s="30" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A105" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="E101" s="31"/>
-      <c r="F101" s="31"/>
-    </row>
-    <row r="102" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="34" t="s">
+      <c r="E105" s="31"/>
+      <c r="F105" s="31"/>
+    </row>
+    <row r="106" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="B102" s="32" t="s">
+      <c r="B106" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="C102" s="36" t="s">
+      <c r="C106" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="D102" s="32">
-        <v>1</v>
-      </c>
-      <c r="E102" s="33">
+      <c r="D106" s="32">
+        <v>1</v>
+      </c>
+      <c r="E106" s="33">
         <v>6734</v>
       </c>
-      <c r="F102" s="33">
-        <f>D102*E102</f>
+      <c r="F106" s="33">
+        <f>D106*E106</f>
         <v>6734</v>
       </c>
-      <c r="G102" s="3" t="s">
+      <c r="G106" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H102" s="32" t="s">
+      <c r="H106" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="I102" s="32" t="s">
+      <c r="I106" s="32" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="35" t="s">
-        <v>410</v>
-      </c>
-      <c r="B103" s="32"/>
-      <c r="H103" s="32"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="35"/>
-      <c r="B104" s="32"/>
-      <c r="C104" s="37"/>
-      <c r="H104" s="32"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B105" s="32"/>
-      <c r="C105" s="37"/>
-      <c r="H105" s="32"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B106" s="32"/>
-      <c r="C106" s="37"/>
-      <c r="H106" s="32"/>
-    </row>
-    <row r="107" spans="1:9" s="30" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A107" s="29" t="s">
-        <v>310</v>
-      </c>
-      <c r="E107" s="31"/>
-      <c r="F107" s="31"/>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="35" t="s">
+        <v>409</v>
+      </c>
+      <c r="B107" s="32"/>
+      <c r="H107" s="32"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="35"/>
       <c r="B108" s="32"/>
+      <c r="C108" s="37"/>
+      <c r="H108" s="32"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B109" s="32"/>
-    </row>
-    <row r="111" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A111" s="6" t="s">
+      <c r="C109" s="37"/>
+      <c r="H109" s="32"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B110" s="32"/>
+      <c r="C110" s="37"/>
+      <c r="H110" s="32"/>
+    </row>
+    <row r="111" spans="1:9" s="30" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A111" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="E111" s="31"/>
+      <c r="F111" s="31"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B112" s="32"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="32"/>
+    </row>
+    <row r="115" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A115" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E111" s="9"/>
-      <c r="F111" s="9"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
+      <c r="E115" s="9"/>
+      <c r="F115" s="9"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B116" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C116" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D112" s="3">
-        <v>1</v>
-      </c>
-      <c r="E112" s="5">
+      <c r="D116" s="3">
+        <v>1</v>
+      </c>
+      <c r="E116" s="5">
         <v>3582</v>
       </c>
-      <c r="F112" s="5">
-        <f>E112*D112</f>
+      <c r="F116" s="5">
+        <f>E116*D116</f>
         <v>3582</v>
       </c>
-      <c r="G112" s="3" t="s">
+      <c r="G116" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I112" s="3" t="s">
+      <c r="I116" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B117" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="C117" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D113" s="3">
-        <v>1</v>
-      </c>
-      <c r="E113" s="5">
+      <c r="D117" s="3">
+        <v>1</v>
+      </c>
+      <c r="E117" s="5">
         <v>1630</v>
       </c>
-      <c r="F113" s="5">
-        <f t="shared" ref="F113:F121" si="5">E113*D113</f>
+      <c r="F117" s="5">
+        <f t="shared" ref="F117:F125" si="5">E117*D117</f>
         <v>1630</v>
       </c>
-      <c r="G113" s="3" t="s">
+      <c r="G117" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I113" s="3" t="s">
+      <c r="I117" s="3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B118" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C118" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="D114" s="3">
-        <v>1</v>
-      </c>
-      <c r="E114" s="5">
+      <c r="D118" s="3">
+        <v>1</v>
+      </c>
+      <c r="E118" s="5">
         <v>886</v>
       </c>
-      <c r="F114" s="5">
+      <c r="F118" s="5">
         <f t="shared" si="5"/>
         <v>886</v>
       </c>
-      <c r="G114" s="3" t="s">
+      <c r="G118" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I114" s="3" t="s">
+      <c r="I118" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B119" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C119" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D115" s="3">
-        <v>1</v>
-      </c>
-      <c r="E115" s="5">
+      <c r="D119" s="3">
+        <v>1</v>
+      </c>
+      <c r="E119" s="5">
         <v>163</v>
       </c>
-      <c r="F115" s="5">
+      <c r="F119" s="5">
         <f t="shared" si="5"/>
         <v>163</v>
       </c>
-      <c r="G115" s="3" t="s">
+      <c r="G119" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I115" s="3" t="s">
+      <c r="I119" s="3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B120" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C120" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="D116" s="3">
-        <v>1</v>
-      </c>
-      <c r="E116" s="5">
+      <c r="D120" s="3">
+        <v>1</v>
+      </c>
+      <c r="E120" s="5">
         <v>11</v>
       </c>
-      <c r="F116" s="5">
+      <c r="F120" s="5">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="G116" s="3" t="s">
+      <c r="G120" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B121" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C121" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D117" s="3">
-        <v>1</v>
-      </c>
-      <c r="E117" s="5">
+      <c r="D121" s="3">
+        <v>1</v>
+      </c>
+      <c r="E121" s="5">
         <v>520</v>
       </c>
-      <c r="F117" s="5">
-        <f>E117*D117</f>
+      <c r="F121" s="5">
+        <f>E121*D121</f>
         <v>520</v>
       </c>
-      <c r="G117" s="3" t="s">
+      <c r="G121" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B122" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C122" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="D118" s="3">
-        <v>1</v>
-      </c>
-      <c r="E118" s="5">
+      <c r="D122" s="3">
+        <v>1</v>
+      </c>
+      <c r="E122" s="5">
         <v>193</v>
       </c>
-      <c r="F118" s="5">
-        <f>E118*D118</f>
+      <c r="F122" s="5">
+        <f>E122*D122</f>
         <v>193</v>
       </c>
-      <c r="G118" s="3" t="s">
+      <c r="G122" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="119" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="38" t="s">
+    <row r="123" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B119" s="38" t="s">
+      <c r="B123" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C119" s="38" t="s">
+      <c r="C123" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D119" s="38">
+      <c r="D123" s="38">
         <v>0</v>
       </c>
-      <c r="E119" s="39">
+      <c r="E123" s="39">
         <v>2800</v>
       </c>
-      <c r="F119" s="39">
+      <c r="F123" s="39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G119" s="38" t="s">
+      <c r="G123" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="I119" s="38" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="41" t="s">
+      <c r="I123" s="38" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="41" t="s">
+        <v>393</v>
+      </c>
+      <c r="B124" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C124" s="41" t="s">
         <v>394</v>
       </c>
-      <c r="B120" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C120" s="41" t="s">
-        <v>395</v>
-      </c>
-      <c r="D120" s="41">
+      <c r="D124" s="41">
         <v>10</v>
       </c>
-      <c r="E120" s="52">
+      <c r="E124" s="52">
         <v>12</v>
       </c>
-      <c r="F120" s="52">
+      <c r="F124" s="52">
         <f t="shared" si="5"/>
         <v>120</v>
       </c>
-      <c r="G120" s="41" t="s">
+      <c r="G124" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="I120" s="41" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="41" t="s">
+      <c r="I124" s="41" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="41" t="s">
+        <v>395</v>
+      </c>
+      <c r="B125" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C125" s="41" t="s">
         <v>396</v>
       </c>
-      <c r="B121" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C121" s="41" t="s">
-        <v>397</v>
-      </c>
-      <c r="D121" s="41">
-        <v>1</v>
-      </c>
-      <c r="E121" s="52">
+      <c r="D125" s="41">
+        <v>1</v>
+      </c>
+      <c r="E125" s="52">
         <v>14</v>
       </c>
-      <c r="F121" s="52">
+      <c r="F125" s="52">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="G121" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="I121" s="41" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D122" s="3">
-        <v>4</v>
-      </c>
-      <c r="E122" s="5">
-        <v>15.25</v>
-      </c>
-      <c r="F122" s="5">
-        <f>E122*D122</f>
-        <v>61</v>
-      </c>
-      <c r="G122" s="41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D123" s="3">
-        <v>10</v>
-      </c>
-      <c r="E123" s="5">
-        <v>16.5</v>
-      </c>
-      <c r="F123" s="5">
-        <f>E123*D123</f>
-        <v>165</v>
-      </c>
-      <c r="G123" s="41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D124" s="3">
-        <v>10</v>
-      </c>
-      <c r="E124" s="5">
-        <v>24</v>
-      </c>
-      <c r="F124" s="5">
-        <f>E124*D124</f>
-        <v>240</v>
-      </c>
-      <c r="G124" s="41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D125" s="3">
-        <v>6</v>
-      </c>
-      <c r="E125" s="5">
-        <v>24</v>
-      </c>
-      <c r="F125" s="5">
-        <f>E125*D125</f>
-        <v>144</v>
-      </c>
       <c r="G125" s="41" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E126" s="52"/>
-      <c r="F126" s="52"/>
-    </row>
-    <row r="129" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="8" t="s">
+      <c r="I125" s="41" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D126" s="3">
+        <v>4</v>
+      </c>
+      <c r="E126" s="5">
+        <v>15.25</v>
+      </c>
+      <c r="F126" s="5">
+        <f>E126*D126</f>
+        <v>61</v>
+      </c>
+      <c r="G126" s="41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D127" s="3">
+        <v>10</v>
+      </c>
+      <c r="E127" s="5">
+        <v>16.5</v>
+      </c>
+      <c r="F127" s="5">
+        <f>E127*D127</f>
+        <v>165</v>
+      </c>
+      <c r="G127" s="41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D128" s="3">
+        <v>10</v>
+      </c>
+      <c r="E128" s="5">
+        <v>24</v>
+      </c>
+      <c r="F128" s="5">
+        <f>E128*D128</f>
+        <v>240</v>
+      </c>
+      <c r="G128" s="41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D129" s="3">
+        <v>6</v>
+      </c>
+      <c r="E129" s="5">
+        <v>24</v>
+      </c>
+      <c r="F129" s="5">
+        <f>E129*D129</f>
+        <v>144</v>
+      </c>
+      <c r="G129" s="41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E130" s="52"/>
+      <c r="F130" s="52"/>
+    </row>
+    <row r="133" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A133" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C129" s="7"/>
-      <c r="E129" s="18"/>
-      <c r="F129" s="18"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="3" t="s">
+      <c r="C133" s="7"/>
+      <c r="E133" s="18"/>
+      <c r="F133" s="18"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B130" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C130" s="3" t="s">
+      <c r="B134" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C134" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D130" s="3">
-        <v>1</v>
-      </c>
-      <c r="E130" s="5">
+      <c r="D134" s="3">
+        <v>1</v>
+      </c>
+      <c r="E134" s="5">
         <v>488</v>
       </c>
-      <c r="F130" s="5">
-        <f t="shared" ref="F130:F151" si="6">E130*D130</f>
+      <c r="F134" s="5">
+        <f t="shared" ref="F134:F155" si="6">E134*D134</f>
         <v>488</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B131" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C131" s="3" t="s">
+      <c r="B135" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C135" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D131" s="3">
-        <v>1</v>
-      </c>
-      <c r="E131" s="5">
+      <c r="D135" s="3">
+        <v>1</v>
+      </c>
+      <c r="E135" s="5">
         <v>184</v>
       </c>
-      <c r="F131" s="5">
+      <c r="F135" s="5">
         <f t="shared" si="6"/>
         <v>184</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="s">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B132" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C132" s="3" t="s">
+      <c r="B136" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C136" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D132" s="3">
-        <v>1</v>
-      </c>
-      <c r="E132" s="5">
+      <c r="D136" s="3">
+        <v>1</v>
+      </c>
+      <c r="E136" s="5">
         <v>76</v>
       </c>
-      <c r="F132" s="5">
+      <c r="F136" s="5">
         <f t="shared" si="6"/>
         <v>76</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="3" t="s">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B133" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C133" s="3" t="s">
+      <c r="B137" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C137" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D133" s="3">
-        <v>1</v>
-      </c>
-      <c r="E133" s="5">
+      <c r="D137" s="3">
+        <v>1</v>
+      </c>
+      <c r="E137" s="5">
         <v>184</v>
       </c>
-      <c r="F133" s="5">
+      <c r="F137" s="5">
         <f t="shared" si="6"/>
         <v>184</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="3" t="s">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B134" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C134" s="3" t="s">
+      <c r="B138" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C138" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D134" s="3">
-        <v>1</v>
-      </c>
-      <c r="E134" s="5">
+      <c r="D138" s="3">
+        <v>1</v>
+      </c>
+      <c r="E138" s="5">
         <v>94.180155999999997</v>
       </c>
-      <c r="F134" s="5">
+      <c r="F138" s="5">
         <f t="shared" si="6"/>
         <v>94.180155999999997</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A135" s="3" t="s">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B135" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C135" s="3" t="s">
+      <c r="B139" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C139" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D135" s="3">
-        <v>1</v>
-      </c>
-      <c r="E135" s="5">
+      <c r="D139" s="3">
+        <v>1</v>
+      </c>
+      <c r="E139" s="5">
         <v>36.799999999999997</v>
       </c>
-      <c r="F135" s="5">
+      <c r="F139" s="5">
         <f t="shared" si="6"/>
         <v>36.799999999999997</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" s="3" t="s">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B136" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C136" s="3" t="s">
+      <c r="B140" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C140" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D136" s="3">
+      <c r="D140" s="3">
         <v>2</v>
       </c>
-      <c r="E136" s="5">
+      <c r="E140" s="5">
         <v>21.21</v>
       </c>
-      <c r="F136" s="5">
+      <c r="F140" s="5">
         <f t="shared" si="6"/>
         <v>42.42</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B137" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C137" s="3" t="s">
+      <c r="B141" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C141" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D137" s="3">
-        <v>1</v>
-      </c>
-      <c r="E137" s="5">
+      <c r="D141" s="3">
+        <v>1</v>
+      </c>
+      <c r="E141" s="5">
         <v>304.75</v>
       </c>
-      <c r="F137" s="5">
+      <c r="F141" s="5">
         <f t="shared" si="6"/>
         <v>304.75</v>
       </c>
-      <c r="I137" s="3" t="s">
+      <c r="I141" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="3" t="s">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B138" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C138" s="3" t="s">
+      <c r="B142" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C142" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D138" s="3">
-        <v>1</v>
-      </c>
-      <c r="E138" s="5">
+      <c r="D142" s="3">
+        <v>1</v>
+      </c>
+      <c r="E142" s="5">
         <v>148.21</v>
       </c>
-      <c r="F138" s="5">
+      <c r="F142" s="5">
         <f t="shared" si="6"/>
         <v>148.21</v>
       </c>
-      <c r="I138" s="3" t="s">
+      <c r="I142" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A139" s="3" t="s">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B139" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C139" s="3" t="s">
+      <c r="B143" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C143" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D139" s="3">
-        <v>1</v>
-      </c>
-      <c r="E139" s="5">
+      <c r="D143" s="3">
+        <v>1</v>
+      </c>
+      <c r="E143" s="5">
         <v>348.45</v>
       </c>
-      <c r="F139" s="5">
+      <c r="F143" s="5">
         <f t="shared" si="6"/>
         <v>348.45</v>
       </c>
-      <c r="I139" s="3" t="s">
+      <c r="I143" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A140" s="3" t="s">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B140" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C140" s="3" t="s">
+      <c r="B144" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C144" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D140" s="3">
-        <v>1</v>
-      </c>
-      <c r="E140" s="5">
+      <c r="D144" s="3">
+        <v>1</v>
+      </c>
+      <c r="E144" s="5">
         <v>60.95</v>
       </c>
-      <c r="F140" s="5">
+      <c r="F144" s="5">
         <f t="shared" si="6"/>
         <v>60.95</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A141" s="3" t="s">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B141" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C141" s="3" t="s">
+      <c r="B145" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C145" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D141" s="3">
-        <v>1</v>
-      </c>
-      <c r="E141" s="5">
+      <c r="D145" s="3">
+        <v>1</v>
+      </c>
+      <c r="E145" s="5">
         <v>34.5</v>
       </c>
-      <c r="F141" s="5">
+      <c r="F145" s="5">
         <f t="shared" si="6"/>
         <v>34.5</v>
       </c>
-      <c r="I141" s="3" t="s">
+      <c r="I145" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A142" s="3" t="s">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B142" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C142" s="3" t="s">
+      <c r="B146" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C146" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D142" s="3">
-        <v>1</v>
-      </c>
-      <c r="E142" s="5">
+      <c r="D146" s="3">
+        <v>1</v>
+      </c>
+      <c r="E146" s="5">
         <v>51.45</v>
       </c>
-      <c r="F142" s="5">
+      <c r="F146" s="5">
         <f t="shared" si="6"/>
         <v>51.45</v>
       </c>
-      <c r="I142" s="3" t="s">
+      <c r="I146" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A143" s="3" t="s">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B143" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C143" s="3" t="s">
+      <c r="B147" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C147" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D143" s="3">
+      <c r="D147" s="3">
         <v>2</v>
       </c>
-      <c r="E143" s="5">
+      <c r="E147" s="5">
         <v>13.8</v>
       </c>
-      <c r="F143" s="5">
+      <c r="F147" s="5">
         <f t="shared" si="6"/>
         <v>27.6</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A144" s="3" t="s">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B144" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C144" s="3" t="s">
+      <c r="B148" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C148" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D144" s="3">
-        <v>1</v>
-      </c>
-      <c r="E144" s="5">
+      <c r="D148" s="3">
+        <v>1</v>
+      </c>
+      <c r="E148" s="5">
         <v>19.09</v>
       </c>
-      <c r="F144" s="5">
+      <c r="F148" s="5">
         <f t="shared" si="6"/>
         <v>19.09</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A145" s="3" t="s">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B145" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C145" s="3" t="s">
+      <c r="B149" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C149" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D145" s="3">
+      <c r="D149" s="3">
         <v>2</v>
       </c>
-      <c r="E145" s="5">
+      <c r="E149" s="5">
         <v>40.51</v>
       </c>
-      <c r="F145" s="5">
+      <c r="F149" s="5">
         <f t="shared" si="6"/>
         <v>81.02</v>
       </c>
-      <c r="I145" s="3" t="s">
+      <c r="I149" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A146" s="3" t="s">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B146" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C146" s="3" t="s">
+      <c r="B150" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C150" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D146" s="3">
+      <c r="D150" s="3">
         <v>2</v>
       </c>
-      <c r="E146" s="5">
+      <c r="E150" s="5">
         <v>83.598116000000005</v>
       </c>
-      <c r="F146" s="5">
+      <c r="F150" s="5">
         <f t="shared" si="6"/>
         <v>167.19623200000001</v>
       </c>
-      <c r="I146" s="3" t="s">
+      <c r="I150" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A147" s="3" t="s">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B147" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C147" s="3" t="s">
+      <c r="B151" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C151" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D147" s="3">
+      <c r="D151" s="3">
         <v>4</v>
       </c>
-      <c r="E147" s="5">
+      <c r="E151" s="5">
         <v>70.103999999999999</v>
       </c>
-      <c r="F147" s="5">
+      <c r="F151" s="5">
         <f t="shared" si="6"/>
         <v>280.416</v>
       </c>
-      <c r="I147" s="3" t="s">
+      <c r="I151" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A148" s="3" t="s">
+    <row r="152" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A152" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B148" s="3" t="s">
+      <c r="B152" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C148" s="3" t="s">
+      <c r="C152" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D148" s="3">
+      <c r="D152" s="3">
         <v>2</v>
       </c>
-      <c r="E148" s="5">
+      <c r="E152" s="5">
         <v>28.75</v>
       </c>
-      <c r="F148" s="5">
+      <c r="F152" s="5">
         <f t="shared" si="6"/>
         <v>57.5</v>
       </c>
-      <c r="I148" s="4" t="s">
+      <c r="I152" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A149" s="3" t="s">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B149" s="3" t="s">
+      <c r="B153" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C149" s="3" t="s">
+      <c r="C153" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D149" s="3">
+      <c r="D153" s="3">
         <v>2</v>
       </c>
-      <c r="E149" s="5">
+      <c r="E153" s="5">
         <v>38.872799999999998</v>
       </c>
-      <c r="F149" s="5">
+      <c r="F153" s="5">
         <f t="shared" si="6"/>
         <v>77.745599999999996</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B150" s="3" t="s">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B154" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C150" s="3" t="s">
+      <c r="C154" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D150" s="3">
-        <v>1</v>
-      </c>
-      <c r="E150" s="5">
+      <c r="D154" s="3">
+        <v>1</v>
+      </c>
+      <c r="E154" s="5">
         <v>205</v>
       </c>
-      <c r="F150" s="5">
+      <c r="F154" s="5">
         <f t="shared" si="6"/>
         <v>205</v>
       </c>
-      <c r="I150" s="3" t="s">
+      <c r="I154" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B151" s="3" t="s">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B155" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C151" s="3" t="s">
+      <c r="C155" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D151" s="3">
+      <c r="D155" s="3">
         <v>2</v>
       </c>
-      <c r="E151" s="5">
+      <c r="E155" s="5">
         <v>12</v>
       </c>
-      <c r="F151" s="5">
+      <c r="F155" s="5">
         <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="I151" s="3" t="s">
+      <c r="I155" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A152" s="11"/>
-      <c r="B152" s="11"/>
-      <c r="C152" s="10"/>
-    </row>
-    <row r="153" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A153" s="8" t="s">
+    <row r="156" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A156" s="11"/>
+      <c r="B156" s="11"/>
+      <c r="C156" s="10"/>
+    </row>
+    <row r="157" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A157" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="F153" s="9"/>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A154" s="3" t="s">
+      <c r="F157" s="9"/>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B154" s="3" t="s">
+      <c r="B158" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C154" s="3" t="s">
+      <c r="C158" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D154" s="3">
+      <c r="D158" s="3">
         <v>4</v>
       </c>
-      <c r="E154" s="5">
+      <c r="E158" s="5">
         <v>16.5</v>
       </c>
-      <c r="F154" s="5">
-        <f t="shared" ref="F154:F170" si="7">E154*D154</f>
+      <c r="F158" s="5">
+        <f t="shared" ref="F158:F174" si="7">E158*D158</f>
         <v>66</v>
       </c>
-      <c r="I154" s="3" t="s">
+      <c r="I158" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A155" s="3" t="s">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B155" s="3" t="s">
+      <c r="B159" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C155" s="3" t="s">
+      <c r="C159" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D155" s="3">
+      <c r="D159" s="3">
         <v>2</v>
       </c>
-      <c r="E155" s="5">
+      <c r="E159" s="5">
         <v>140</v>
       </c>
-      <c r="F155" s="5">
+      <c r="F159" s="5">
         <f t="shared" si="7"/>
         <v>280</v>
       </c>
-      <c r="I155" s="3" t="s">
+      <c r="I159" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A156" s="3" t="s">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B156" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C156" s="3" t="s">
+      <c r="B160" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C160" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D156" s="3">
-        <v>1</v>
-      </c>
-      <c r="E156" s="5">
+      <c r="D160" s="3">
+        <v>1</v>
+      </c>
+      <c r="E160" s="5">
         <v>85.1</v>
       </c>
-      <c r="F156" s="5">
+      <c r="F160" s="5">
         <f t="shared" si="7"/>
         <v>85.1</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A157" s="3" t="s">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B157" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C157" s="3" t="s">
+      <c r="B161" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C161" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D157" s="3">
+      <c r="D161" s="3">
         <v>2</v>
       </c>
-      <c r="E157" s="5">
+      <c r="E161" s="5">
         <v>32</v>
       </c>
-      <c r="F157" s="5">
+      <c r="F161" s="5">
         <f t="shared" si="7"/>
         <v>64</v>
       </c>
-      <c r="I157" s="3" t="s">
+      <c r="I161" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A158" s="3" t="s">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B158" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C158" s="3" t="s">
+      <c r="B162" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C162" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D158" s="3">
+      <c r="D162" s="3">
         <v>2</v>
       </c>
-      <c r="E158" s="5">
+      <c r="E162" s="5">
         <v>51.58</v>
       </c>
-      <c r="F158" s="5">
+      <c r="F162" s="5">
         <f t="shared" si="7"/>
         <v>103.16</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A159" s="3" t="s">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B159" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C159" s="3" t="s">
+      <c r="B163" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C163" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D159" s="3">
-        <v>1</v>
-      </c>
-      <c r="E159" s="5">
+      <c r="D163" s="3">
+        <v>1</v>
+      </c>
+      <c r="E163" s="5">
         <v>60</v>
       </c>
-      <c r="F159" s="5">
+      <c r="F163" s="5">
         <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="I159" s="3" t="s">
+      <c r="I163" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A160" s="3" t="s">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B160" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C160" s="3" t="s">
+      <c r="B164" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C164" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D160" s="3">
-        <v>1</v>
-      </c>
-      <c r="E160" s="5">
+      <c r="D164" s="3">
+        <v>1</v>
+      </c>
+      <c r="E164" s="5">
         <v>136.47999999999999</v>
       </c>
-      <c r="F160" s="5">
+      <c r="F164" s="5">
         <f t="shared" si="7"/>
         <v>136.47999999999999</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B161" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C161" s="3" t="s">
+      <c r="B165" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C165" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D161" s="3">
-        <v>1</v>
-      </c>
-      <c r="E161" s="5">
+      <c r="D165" s="3">
+        <v>1</v>
+      </c>
+      <c r="E165" s="5">
         <v>136.47999999999999</v>
       </c>
-      <c r="F161" s="5">
+      <c r="F165" s="5">
         <f t="shared" si="7"/>
         <v>136.47999999999999</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A162" s="3" t="s">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B162" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C162" s="3" t="s">
+      <c r="B166" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C166" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D162" s="3">
-        <v>1</v>
-      </c>
-      <c r="E162" s="5">
+      <c r="D166" s="3">
+        <v>1</v>
+      </c>
+      <c r="E166" s="5">
         <v>60.95</v>
       </c>
-      <c r="F162" s="5">
+      <c r="F166" s="5">
         <f t="shared" si="7"/>
         <v>60.95</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B163" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C163" s="3" t="s">
+      <c r="B167" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C167" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D163" s="3">
-        <v>1</v>
-      </c>
-      <c r="E163" s="5">
+      <c r="D167" s="3">
+        <v>1</v>
+      </c>
+      <c r="E167" s="5">
         <v>119.416</v>
       </c>
-      <c r="F163" s="5">
+      <c r="F167" s="5">
         <f t="shared" si="7"/>
         <v>119.416</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A164" s="3" t="s">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B164" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C164" s="3" t="s">
+      <c r="B168" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C168" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D164" s="3">
-        <v>1</v>
-      </c>
-      <c r="E164" s="5">
+      <c r="D168" s="3">
+        <v>1</v>
+      </c>
+      <c r="E168" s="5">
         <v>105.8</v>
       </c>
-      <c r="F164" s="5">
+      <c r="F168" s="5">
         <f t="shared" si="7"/>
         <v>105.8</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A165" s="3" t="s">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B165" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C165" s="3" t="s">
+      <c r="B169" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C169" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D165" s="3">
+      <c r="D169" s="3">
         <v>2</v>
       </c>
-      <c r="E165" s="5">
+      <c r="E169" s="5">
         <v>119.6</v>
       </c>
-      <c r="F165" s="5">
+      <c r="F169" s="5">
         <f t="shared" si="7"/>
         <v>239.2</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A166" s="3" t="s">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C170" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="B166" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="D166" s="3">
-        <v>1</v>
-      </c>
-      <c r="E166" s="5">
+      <c r="D170" s="3">
+        <v>1</v>
+      </c>
+      <c r="E170" s="5">
         <v>100</v>
       </c>
-      <c r="F166" s="5">
+      <c r="F170" s="5">
         <f t="shared" si="7"/>
         <v>100</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A167" s="3" t="s">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B167" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C167" s="3" t="s">
+      <c r="B171" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C171" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D167" s="3">
+      <c r="D171" s="3">
         <v>2</v>
       </c>
-      <c r="E167" s="5">
+      <c r="E171" s="5">
         <v>92</v>
       </c>
-      <c r="F167" s="5">
+      <c r="F171" s="5">
         <f t="shared" si="7"/>
         <v>184</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B168" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C168" s="3" t="s">
+      <c r="B172" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C172" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D168" s="3">
-        <v>1</v>
-      </c>
-      <c r="E168" s="5">
+      <c r="D172" s="3">
+        <v>1</v>
+      </c>
+      <c r="E172" s="5">
         <v>96.23</v>
       </c>
-      <c r="F168" s="5">
+      <c r="F172" s="5">
         <f t="shared" si="7"/>
         <v>96.23</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A169" s="3" t="s">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B169" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C169" s="3" t="s">
+      <c r="B173" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C173" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D169" s="3">
-        <v>1</v>
-      </c>
-      <c r="E169" s="5">
+      <c r="D173" s="3">
+        <v>1</v>
+      </c>
+      <c r="E173" s="5">
         <v>102.44</v>
       </c>
-      <c r="F169" s="5">
+      <c r="F173" s="5">
         <f t="shared" si="7"/>
         <v>102.44</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A170" s="3" t="s">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B170" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C170" s="3" t="s">
+      <c r="B174" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C174" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D170" s="3">
+      <c r="D174" s="3">
         <v>2</v>
       </c>
-      <c r="E170" s="5">
+      <c r="E174" s="5">
         <v>28</v>
       </c>
-      <c r="F170" s="5">
+      <c r="F174" s="5">
         <f t="shared" si="7"/>
         <v>56</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C171" s="3" t="s">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C175" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D171" s="3">
+      <c r="D175" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C172" s="3" t="s">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C176" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D172" s="3">
-        <v>1</v>
-      </c>
-      <c r="I172" s="3" t="s">
+      <c r="D176" s="3">
+        <v>1</v>
+      </c>
+      <c r="I176" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C173" s="3" t="s">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C177" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D173" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="1:11" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A177" s="8" t="s">
+      <c r="D177" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A181" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="C177" s="7"/>
-      <c r="E177" s="18"/>
-      <c r="F177" s="18"/>
-    </row>
-    <row r="178" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B178" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C178" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="D178" s="3">
-        <v>1</v>
-      </c>
-      <c r="G178" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="I178" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J178" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="K178" s="4"/>
-    </row>
-    <row r="179" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B179" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C179" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="D179" s="3">
-        <v>1</v>
-      </c>
-      <c r="G179" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="I179" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J179" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="K179" s="4"/>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B180" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C180" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="D180" s="3">
-        <v>2</v>
-      </c>
-      <c r="G180" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="I180" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="J180" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B181" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C181" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D181" s="3">
-        <v>1</v>
-      </c>
-      <c r="G181" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="J181" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C181" s="7"/>
+      <c r="E181" s="18"/>
+      <c r="F181" s="18"/>
+    </row>
+    <row r="182" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B182" s="3" t="s">
         <v>184</v>
       </c>
       <c r="C182" s="19" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D182" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="I182" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="J182" s="19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="J182" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K182" s="4"/>
+    </row>
+    <row r="183" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B183" s="3" t="s">
         <v>184</v>
       </c>
       <c r="C183" s="19" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D183" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="I183" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="J183" s="19" t="s">
-        <v>197</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="J183" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K183" s="4"/>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B184" s="3" t="s">
         <v>184</v>
       </c>
       <c r="C184" s="19" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D184" s="3">
         <v>2</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="I184" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="J184" s="19" t="s">
-        <v>197</v>
+        <v>191</v>
+      </c>
+      <c r="J184" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.25">
@@ -5737,269 +5801,346 @@
         <v>184</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D185" s="3">
         <v>1</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J185" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="186" spans="1:11" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A186" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="B186" s="19" t="s">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B186" s="3" t="s">
         <v>184</v>
       </c>
       <c r="C186" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="D186" s="19">
-        <v>10</v>
-      </c>
-      <c r="F186" s="55"/>
-      <c r="G186" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="D186" s="3">
+        <v>0</v>
+      </c>
+      <c r="G186" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="I186" s="4" t="s">
-        <v>204</v>
+      <c r="I186" s="3" t="s">
+        <v>196</v>
       </c>
       <c r="J186" s="19" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="188" spans="1:11" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A188" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="B188" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="E188" s="9"/>
-      <c r="F188" s="9"/>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B187" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C187" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="D187" s="3">
+        <v>2</v>
+      </c>
+      <c r="G187" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I187" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="J187" s="19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B188" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C188" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="D188" s="3">
+        <v>2</v>
+      </c>
+      <c r="G188" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I188" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="J188" s="19" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B189" s="3" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>381</v>
+        <v>201</v>
       </c>
       <c r="D189" s="3">
-        <v>0</v>
-      </c>
-      <c r="E189" s="5">
-        <v>518.5</v>
-      </c>
-      <c r="F189" s="5">
-        <f t="shared" ref="F189:F199" si="8">E189*D189</f>
-        <v>0</v>
-      </c>
-      <c r="I189" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B190" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C190" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="D190" s="3">
-        <v>0</v>
-      </c>
-      <c r="E190" s="5">
-        <v>764</v>
-      </c>
-      <c r="F190" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B191" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="D191" s="3">
-        <v>0</v>
-      </c>
-      <c r="E191" s="5">
-        <v>816</v>
-      </c>
-      <c r="F191" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I191" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B192" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="D192" s="3">
-        <v>0</v>
-      </c>
-      <c r="E192" s="5">
-        <v>952</v>
-      </c>
-      <c r="F192" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G189" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="J189" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A190" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B190" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C190" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="D190" s="19">
+        <v>10</v>
+      </c>
+      <c r="F190" s="55"/>
+      <c r="G190" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="I190" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="J190" s="19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A192" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B192" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="E192" s="9"/>
+      <c r="F192" s="9"/>
+    </row>
+    <row r="193" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D193" s="3">
         <v>0</v>
       </c>
       <c r="E193" s="5">
-        <v>99.5</v>
+        <v>518.5</v>
       </c>
       <c r="F193" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="F193:F203" si="8">E193*D193</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I193" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="194" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D194" s="3">
         <v>0</v>
       </c>
       <c r="E194" s="5">
-        <v>128.5</v>
+        <v>764</v>
       </c>
       <c r="F194" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D195" s="3">
         <v>0</v>
       </c>
       <c r="E195" s="5">
-        <v>156</v>
+        <v>816</v>
       </c>
       <c r="F195" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I195" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="196" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D196" s="3">
         <v>0</v>
       </c>
       <c r="E196" s="5">
-        <v>184.5</v>
+        <v>952</v>
       </c>
       <c r="F196" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D197" s="3">
         <v>0</v>
       </c>
       <c r="E197" s="5">
-        <v>106.5</v>
+        <v>99.5</v>
       </c>
       <c r="F197" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D198" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E198" s="5">
-        <v>106.5</v>
+        <v>128.5</v>
       </c>
       <c r="F198" s="5">
         <f t="shared" si="8"/>
-        <v>639</v>
-      </c>
-    </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D199" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E199" s="5">
-        <v>121.5</v>
+        <v>156</v>
       </c>
       <c r="F199" s="5">
         <f t="shared" si="8"/>
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="202" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E202" s="21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B200" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="D200" s="3">
+        <v>0</v>
+      </c>
+      <c r="E200" s="5">
+        <v>184.5</v>
+      </c>
+      <c r="F200" s="5">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B201" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D201" s="3">
+        <v>4</v>
+      </c>
+      <c r="E201" s="5">
+        <v>25</v>
+      </c>
+      <c r="F201" s="5">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="202" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B202" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D202" s="3">
+        <v>4</v>
+      </c>
+      <c r="E202" s="5">
+        <v>28</v>
+      </c>
+      <c r="F202" s="5">
+        <f t="shared" si="8"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="203" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B203" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="D203" s="3">
+        <v>6</v>
+      </c>
+      <c r="E203" s="5">
+        <v>121.5</v>
+      </c>
+      <c r="F203" s="5">
+        <f t="shared" si="8"/>
+        <v>729</v>
+      </c>
+    </row>
+    <row r="206" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E206" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="F202" s="5">
-        <f>SUM(F3:F200)</f>
-        <v>99506.533987999996</v>
+      <c r="F206" s="5">
+        <f>SUM(F3:F204)</f>
+        <v>98744.533987999996</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C102" r:id="rId1" xr:uid="{3BC0AF99-F679-46A9-B7F9-6A136F582C78}"/>
+    <hyperlink ref="C106" r:id="rId1" xr:uid="{3BC0AF99-F679-46A9-B7F9-6A136F582C78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
detection path model: add ZWO EFW-Mini filter wheel
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\GitHub-public\benchtop-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B6534A-1202-4442-92EF-AF6A682FC1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="34560" windowHeight="18690" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Options" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1598,7 +1597,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1920,12 +1919,12 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="4" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Excel Built-in Heading 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Excel Built-in Note" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Excel Built-in Heading 1" xfId="3"/>
+    <cellStyle name="Excel Built-in Note" xfId="4"/>
+    <cellStyle name="Explanatory Text 2" xfId="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2304,29 +2303,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="86.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="31.77734375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="69.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="21.109375" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.6640625" style="3"/>
+    <col min="1" max="1" width="42.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="86.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="69.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2355,15 +2354,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -2390,27 +2389,27 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>178</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>187</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>193</v>
       </c>
@@ -2434,14 +2433,14 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -2468,7 +2467,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>21</v>
       </c>
@@ -2495,7 +2494,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>23</v>
       </c>
@@ -2522,7 +2521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>395</v>
       </c>
@@ -2549,7 +2548,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>26</v>
       </c>
@@ -2579,7 +2578,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>27</v>
       </c>
@@ -2606,7 +2605,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>29</v>
       </c>
@@ -2633,7 +2632,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
@@ -2660,7 +2659,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
@@ -2687,7 +2686,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>35</v>
       </c>
@@ -2714,7 +2713,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
@@ -2741,14 +2740,14 @@
         <v>275</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>297</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>292</v>
       </c>
@@ -2775,7 +2774,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>295</v>
       </c>
@@ -2802,7 +2801,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="41" t="s">
         <v>299</v>
       </c>
@@ -2829,7 +2828,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="41" t="s">
         <v>302</v>
       </c>
@@ -2856,7 +2855,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="41" t="s">
         <v>305</v>
       </c>
@@ -2883,7 +2882,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="41" t="s">
         <v>310</v>
       </c>
@@ -2907,21 +2906,21 @@
         <v>311</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="15" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
     </row>
-    <row r="29" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>459</v>
       </c>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C30" s="3" t="s">
         <v>39</v>
       </c>
@@ -2936,14 +2935,14 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>211</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -2970,7 +2969,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>45</v>
       </c>
@@ -3000,7 +2999,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>48</v>
       </c>
@@ -3027,7 +3026,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="33" t="s">
         <v>232</v>
       </c>
@@ -3054,7 +3053,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>81</v>
       </c>
@@ -3081,7 +3080,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="33" t="s">
         <v>340</v>
       </c>
@@ -3108,7 +3107,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>341</v>
       </c>
@@ -3137,7 +3136,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="24">
         <v>91863</v>
       </c>
@@ -3167,7 +3166,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>169</v>
       </c>
@@ -3200,7 +3199,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
         <v>261</v>
       </c>
@@ -3233,7 +3232,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="33" t="s">
         <v>260</v>
       </c>
@@ -3263,7 +3262,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="33" t="s">
         <v>327</v>
       </c>
@@ -3293,7 +3292,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="33" t="s">
         <v>76</v>
       </c>
@@ -3323,7 +3322,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="35" t="s">
         <v>214</v>
       </c>
@@ -3353,7 +3352,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="35" t="s">
         <v>220</v>
       </c>
@@ -3383,7 +3382,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="33" t="s">
         <v>222</v>
       </c>
@@ -3413,7 +3412,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="35" t="s">
         <v>226</v>
       </c>
@@ -3443,7 +3442,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="35" t="s">
         <v>229</v>
       </c>
@@ -3473,7 +3472,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="33" t="s">
         <v>235</v>
       </c>
@@ -3503,7 +3502,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="33" t="s">
         <v>245</v>
       </c>
@@ -3530,7 +3529,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="33" t="s">
         <v>185</v>
       </c>
@@ -3560,7 +3559,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="33" t="s">
         <v>237</v>
       </c>
@@ -3590,7 +3589,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="33" t="s">
         <v>241</v>
       </c>
@@ -3620,7 +3619,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="33" t="s">
         <v>243</v>
       </c>
@@ -3650,7 +3649,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="33" t="s">
         <v>183</v>
       </c>
@@ -3677,7 +3676,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="35" t="s">
         <v>247</v>
       </c>
@@ -3707,7 +3706,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="35" t="s">
         <v>342</v>
       </c>
@@ -3737,7 +3736,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="35" t="s">
         <v>250</v>
       </c>
@@ -3767,7 +3766,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="33" t="s">
         <v>352</v>
       </c>
@@ -3797,7 +3796,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="33" t="s">
         <v>320</v>
       </c>
@@ -3827,7 +3826,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="33" t="s">
         <v>322</v>
       </c>
@@ -3854,7 +3853,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="47" t="s">
         <v>359</v>
       </c>
@@ -3884,7 +3883,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="47" t="s">
         <v>360</v>
       </c>
@@ -3914,7 +3913,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="33" t="s">
         <v>351</v>
       </c>
@@ -3944,7 +3943,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="46" t="s">
         <v>357</v>
       </c>
@@ -3974,32 +3973,32 @@
         <v>358</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="33"/>
       <c r="C68" s="33"/>
       <c r="E68" s="34"/>
       <c r="F68" s="42"/>
     </row>
-    <row r="69" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="33"/>
       <c r="C69" s="33"/>
       <c r="E69" s="34"/>
       <c r="F69" s="42"/>
     </row>
-    <row r="70" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="33"/>
       <c r="C70" s="33"/>
       <c r="E70" s="34"/>
       <c r="F70" s="42"/>
     </row>
-    <row r="71" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>283</v>
       </c>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
     </row>
-    <row r="72" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="33" t="s">
         <v>26</v>
       </c>
@@ -4018,7 +4017,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="73" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="33" t="s">
         <v>284</v>
       </c>
@@ -4039,7 +4038,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="39" t="s">
         <v>289</v>
       </c>
@@ -4060,7 +4059,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="32" t="s">
         <v>23</v>
       </c>
@@ -4079,21 +4078,21 @@
         <v>291</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>486</v>
       </c>
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
     </row>
-    <row r="77" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
         <v>487</v>
       </c>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
     </row>
-    <row r="78" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>490</v>
       </c>
@@ -4118,7 +4117,7 @@
       </c>
       <c r="J78" s="4"/>
     </row>
-    <row r="79" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>492</v>
       </c>
@@ -4143,7 +4142,7 @@
       </c>
       <c r="J79" s="4"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="70" t="s">
         <v>496</v>
       </c>
@@ -4167,7 +4166,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>498</v>
       </c>
@@ -4189,7 +4188,7 @@
       </c>
       <c r="I81" s="32"/>
     </row>
-    <row r="82" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="70" t="s">
         <v>405</v>
       </c>
@@ -4213,19 +4212,19 @@
         <v>500</v>
       </c>
     </row>
-    <row r="83" spans="1:9" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="75" t="s">
         <v>181</v>
       </c>
       <c r="F83" s="44"/>
     </row>
-    <row r="84" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="21" t="s">
         <v>182</v>
       </c>
       <c r="F84" s="44"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>412</v>
       </c>
@@ -4252,14 +4251,14 @@
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" s="26" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="25" t="s">
         <v>414</v>
       </c>
       <c r="E86" s="27"/>
       <c r="F86" s="27"/>
     </row>
-    <row r="87" spans="1:9" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="30" t="s">
         <v>374</v>
       </c>
@@ -4286,7 +4285,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="31" t="s">
         <v>375</v>
       </c>
@@ -4314,7 +4313,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="31" t="s">
         <v>379</v>
       </c>
@@ -4342,7 +4341,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>381</v>
       </c>
@@ -4370,7 +4369,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>382</v>
       </c>
@@ -4395,7 +4394,7 @@
       </c>
       <c r="H91" s="28"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>385</v>
       </c>
@@ -4420,14 +4419,14 @@
       </c>
       <c r="H92" s="28"/>
     </row>
-    <row r="93" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" s="26" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="25" t="s">
         <v>415</v>
       </c>
       <c r="E93" s="27"/>
       <c r="F93" s="27"/>
     </row>
-    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>397</v>
       </c>
@@ -4454,7 +4453,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>419</v>
       </c>
@@ -4478,7 +4477,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>421</v>
       </c>
@@ -4505,7 +4504,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>430</v>
       </c>
@@ -4531,7 +4530,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>423</v>
       </c>
@@ -4558,7 +4557,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>427</v>
       </c>
@@ -4585,7 +4584,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>408</v>
       </c>
@@ -4612,7 +4611,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>367</v>
       </c>
@@ -4633,14 +4632,14 @@
         <v>436</v>
       </c>
     </row>
-    <row r="102" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>56</v>
       </c>
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>64</v>
       </c>
@@ -4667,7 +4666,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>202</v>
       </c>
@@ -4694,7 +4693,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>201</v>
       </c>
@@ -4721,7 +4720,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>206</v>
       </c>
@@ -4748,7 +4747,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>59</v>
       </c>
@@ -4772,7 +4771,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>62</v>
       </c>
@@ -4796,7 +4795,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>209</v>
       </c>
@@ -4820,7 +4819,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="32" t="s">
         <v>334</v>
       </c>
@@ -4847,7 +4846,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="111" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="32" t="s">
         <v>336</v>
       </c>
@@ -4874,7 +4873,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>129</v>
       </c>
@@ -4898,7 +4897,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>131</v>
       </c>
@@ -4922,7 +4921,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>133</v>
       </c>
@@ -4946,7 +4945,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>129</v>
       </c>
@@ -4970,22 +4969,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E116" s="42"/>
       <c r="F116" s="42"/>
     </row>
-    <row r="118" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="11"/>
       <c r="B118" s="11"/>
       <c r="C118" s="10"/>
     </row>
-    <row r="119" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
         <v>119</v>
       </c>
       <c r="F119" s="9"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>120</v>
       </c>
@@ -5009,7 +5008,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>127</v>
       </c>
@@ -5030,7 +5029,7 @@
         <v>85.1</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>136</v>
       </c>
@@ -5054,7 +5053,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>139</v>
       </c>
@@ -5075,7 +5074,7 @@
         <v>103.16</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>141</v>
       </c>
@@ -5099,7 +5098,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>144</v>
       </c>
@@ -5120,7 +5119,7 @@
         <v>136.47999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>144</v>
       </c>
@@ -5141,7 +5140,7 @@
         <v>136.47999999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>147</v>
       </c>
@@ -5162,7 +5161,7 @@
         <v>60.95</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>149</v>
       </c>
@@ -5183,7 +5182,7 @@
         <v>119.416</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>151</v>
       </c>
@@ -5204,7 +5203,7 @@
         <v>105.8</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>153</v>
       </c>
@@ -5225,7 +5224,7 @@
         <v>239.2</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>345</v>
       </c>
@@ -5246,7 +5245,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>155</v>
       </c>
@@ -5267,7 +5266,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>157</v>
       </c>
@@ -5288,7 +5287,7 @@
         <v>96.23</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>159</v>
       </c>
@@ -5309,7 +5308,7 @@
         <v>102.44</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>161</v>
       </c>
@@ -5330,7 +5329,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C136" s="3" t="s">
         <v>163</v>
       </c>
@@ -5338,7 +5337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C137" s="3" t="s">
         <v>164</v>
       </c>
@@ -5349,7 +5348,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C138" s="3" t="s">
         <v>166</v>
       </c>
@@ -5357,7 +5356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
         <v>174</v>
       </c>
@@ -5367,7 +5366,7 @@
       <c r="E140" s="9"/>
       <c r="F140" s="9"/>
     </row>
-    <row r="141" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141" s="70"/>
       <c r="B141" s="70" t="s">
         <v>167</v>
@@ -5396,7 +5395,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="142" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B142" s="70" t="s">
         <v>175</v>
       </c>
@@ -5417,7 +5416,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="143" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B143" s="70" t="s">
         <v>175</v>
       </c>
@@ -5438,7 +5437,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="144" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B144" s="70" t="s">
         <v>175</v>
       </c>
@@ -5459,7 +5458,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="145" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B145" s="70" t="s">
         <v>175</v>
       </c>
@@ -5480,7 +5479,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="148" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E148" s="20" t="s">
         <v>177</v>
       </c>
@@ -5492,12 +5491,12 @@
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C87" r:id="rId1" display="Mitutoyo Plan Apo Brightfield and Darkfield, 2X" xr:uid="{3D527150-CD66-4BE5-B185-85CFF78C5CA5}"/>
-    <hyperlink ref="C88" r:id="rId2" display="Plan Apo" xr:uid="{E97E73FC-AE1E-4348-9424-88ED8BD705E0}"/>
-    <hyperlink ref="C89" r:id="rId3" display="Plan Apo" xr:uid="{D8344794-7BA0-4E50-AD86-C3517128EA92}"/>
-    <hyperlink ref="C90" r:id="rId4" display="Plan Apo Brightfield and Darkfield " xr:uid="{46B4BB89-8C51-4E18-A88E-F41D266DC652}"/>
-    <hyperlink ref="C94" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{54BFEC5E-01BD-448D-BEB4-DF34719378D8}"/>
-    <hyperlink ref="C78" r:id="rId6" xr:uid="{2D54C350-F085-4610-AC01-B5FF1DBBAFA1}"/>
+    <hyperlink ref="C87" r:id="rId1" display="Mitutoyo Plan Apo Brightfield and Darkfield, 2X"/>
+    <hyperlink ref="C88" r:id="rId2" display="Plan Apo"/>
+    <hyperlink ref="C89" r:id="rId3" display="Plan Apo"/>
+    <hyperlink ref="C90" r:id="rId4" display="Plan Apo Brightfield and Darkfield "/>
+    <hyperlink ref="C94" r:id="rId5" display="MT-1 Accessory Tube Lens"/>
+    <hyperlink ref="C78" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
@@ -5505,24 +5504,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="47.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5551,14 +5550,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="7" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>178</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:9" s="63" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="63" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="63">
         <v>1008062</v>
       </c>
@@ -5582,7 +5581,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="63" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="63" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="63" t="s">
         <v>180</v>
       </c>
@@ -5603,7 +5602,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="52" t="s">
         <v>461</v>
       </c>
@@ -5617,15 +5616,15 @@
         <v>462</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>464</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="52" t="s">
         <v>189</v>
       </c>
@@ -5646,16 +5645,16 @@
         <v>465</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:9" s="26" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>416</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
     </row>
-    <row r="12" spans="1:9" s="52" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="52" t="s">
         <v>397</v>
       </c>
@@ -5685,7 +5684,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="52" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="52" t="s">
         <v>400</v>
       </c>
@@ -5715,7 +5714,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="52" t="s">
         <v>402</v>
       </c>
@@ -5745,7 +5744,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="52" t="s">
         <v>405</v>
       </c>
@@ -5775,7 +5774,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="56" t="s">
         <v>287</v>
       </c>
@@ -5805,21 +5804,21 @@
         <v>441</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>484</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>485</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:10" s="70" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="70" t="s">
         <v>314</v>
       </c>
@@ -5847,7 +5846,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" s="70" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="70" t="s">
         <v>315</v>
       </c>
@@ -5875,7 +5874,7 @@
       </c>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" s="70" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="70" t="s">
         <v>317</v>
       </c>
@@ -5902,7 +5901,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="70" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
         <v>329</v>
       </c>
@@ -5921,21 +5920,21 @@
         <v>328</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>439</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:10" s="61" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="61" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="60" t="s">
         <v>440</v>
       </c>
       <c r="E25" s="62"/>
       <c r="F25" s="62"/>
     </row>
-    <row r="26" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="56" t="s">
         <v>362</v>
       </c>
@@ -5965,7 +5964,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="56" t="s">
         <v>365</v>
       </c>
@@ -5995,7 +5994,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="56" t="s">
         <v>341</v>
       </c>
@@ -6025,7 +6024,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="56" t="s">
         <v>391</v>
       </c>
@@ -6052,7 +6051,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="56" t="s">
         <v>392</v>
       </c>
@@ -6082,7 +6081,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="59" t="s">
         <v>367</v>
       </c>
@@ -6112,7 +6111,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="59" t="s">
         <v>367</v>
       </c>
@@ -6142,7 +6141,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="56" t="s">
         <v>257</v>
       </c>
@@ -6169,14 +6168,14 @@
         <v>438</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>56</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
     </row>
-    <row r="38" spans="1:9" s="63" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="63" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="63" t="s">
         <v>60</v>
       </c>
@@ -6203,7 +6202,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>66</v>
       </c>
@@ -6211,7 +6210,7 @@
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
     </row>
-    <row r="43" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="52" t="s">
         <v>67</v>
       </c>
@@ -6232,7 +6231,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="52" t="s">
         <v>70</v>
       </c>
@@ -6253,7 +6252,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="52" t="s">
         <v>72</v>
       </c>
@@ -6274,7 +6273,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="52" t="s">
         <v>74</v>
       </c>
@@ -6295,7 +6294,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="52" t="s">
         <v>77</v>
       </c>
@@ -6316,7 +6315,7 @@
         <v>94.180155999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="52" t="s">
         <v>79</v>
       </c>
@@ -6337,7 +6336,7 @@
         <v>36.799999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="52" t="s">
         <v>83</v>
       </c>
@@ -6358,7 +6357,7 @@
         <v>42.42</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="52" t="s">
         <v>85</v>
       </c>
@@ -6382,7 +6381,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="52" t="s">
         <v>88</v>
       </c>
@@ -6406,7 +6405,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="52" t="s">
         <v>90</v>
       </c>
@@ -6430,7 +6429,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="52" t="s">
         <v>92</v>
       </c>
@@ -6451,7 +6450,7 @@
         <v>60.95</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="52" t="s">
         <v>94</v>
       </c>
@@ -6475,7 +6474,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="52" t="s">
         <v>97</v>
       </c>
@@ -6499,7 +6498,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="52" t="s">
         <v>99</v>
       </c>
@@ -6520,7 +6519,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="52" t="s">
         <v>101</v>
       </c>
@@ -6541,7 +6540,7 @@
         <v>19.09</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="52" t="s">
         <v>103</v>
       </c>
@@ -6565,7 +6564,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="52" t="s">
         <v>106</v>
       </c>
@@ -6589,7 +6588,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="52" t="s">
         <v>108</v>
       </c>
@@ -6613,7 +6612,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="52" t="s">
         <v>110</v>
       </c>
@@ -6637,7 +6636,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="52" t="s">
         <v>114</v>
       </c>
@@ -6658,7 +6657,7 @@
         <v>77.745599999999996</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B63" s="52" t="s">
         <v>116</v>
       </c>
@@ -6679,7 +6678,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B64" s="52" t="s">
         <v>116</v>
       </c>
@@ -6700,13 +6699,13 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>445</v>
       </c>
       <c r="F66" s="9"/>
     </row>
-    <row r="67" spans="1:10" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="52" t="s">
         <v>124</v>
       </c>
@@ -6730,7 +6729,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>446</v>
       </c>
@@ -6754,7 +6753,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>453</v>
       </c>
@@ -6778,13 +6777,13 @@
         <v>454</v>
       </c>
     </row>
-    <row r="71" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>455</v>
       </c>
       <c r="F71" s="9"/>
     </row>
-    <row r="72" spans="1:10" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="52" t="s">
         <v>456</v>
       </c>
@@ -6793,7 +6792,7 @@
       <c r="F72" s="55"/>
       <c r="J72" s="68"/>
     </row>
-    <row r="73" spans="1:10" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="52" t="s">
         <v>457</v>
       </c>
@@ -6802,13 +6801,13 @@
       <c r="F73" s="55"/>
       <c r="J73" s="68"/>
     </row>
-    <row r="74" spans="1:10" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C74" s="68"/>
       <c r="E74" s="55"/>
       <c r="F74" s="55"/>
       <c r="J74" s="68"/>
     </row>
-    <row r="75" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>174</v>
       </c>
@@ -6818,7 +6817,7 @@
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
     </row>
-    <row r="76" spans="1:10" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="73" t="s">
         <v>466</v>
       </c>
@@ -6842,7 +6841,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="73" t="s">
         <v>469</v>
       </c>
@@ -6863,7 +6862,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="78" spans="1:10" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="73" t="s">
         <v>471</v>
       </c>
@@ -6887,7 +6886,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="73" t="s">
         <v>473</v>
       </c>
@@ -6908,7 +6907,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="73" t="s">
         <v>482</v>
       </c>
@@ -6929,7 +6928,7 @@
         <v>99.5</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="73" t="s">
         <v>475</v>
       </c>
@@ -6950,7 +6949,7 @@
         <v>128.5</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="73" t="s">
         <v>477</v>
       </c>
@@ -6971,7 +6970,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="73" t="s">
         <v>479</v>
       </c>
@@ -6994,8 +6993,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" xr:uid="{47E90902-2781-43B8-B25D-BA619CD65758}"/>
-    <hyperlink ref="C13" r:id="rId2" xr:uid="{FD011529-5D8C-44BA-8321-CE0ABF6601E4}"/>
+    <hyperlink ref="C12" r:id="rId1"/>
+    <hyperlink ref="C13" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -7003,12 +7002,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
remove workstation from the BOM, can be procured/reused independently.
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\GitHub-public\benchtop-hardware\Benchtop\parts-list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB27C5D-16E7-42C1-A427-422B62805AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="34560" windowHeight="18690" tabRatio="500"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Options" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="501">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -1445,9 +1446,6 @@
   </si>
   <si>
     <t>Nikon objective mount</t>
-  </si>
-  <si>
-    <t>Recommendations: at least 64 GB RAM, 2 TB SSD drive</t>
   </si>
   <si>
     <r>
@@ -1477,18 +1475,12 @@
     <t>Toptica</t>
   </si>
   <si>
-    <t>50000?</t>
-  </si>
-  <si>
     <t>Dual-fiber output option</t>
   </si>
   <si>
     <t>Cameras</t>
   </si>
   <si>
-    <t>FOV 29 mm diagonal, can be challenging for detection optics to priovide high resolution in the corners</t>
-  </si>
-  <si>
     <t>UG-205-H80</t>
   </si>
   <si>
@@ -1592,12 +1584,21 @@
   </si>
   <si>
     <t>Adapters for both sides of the ZWO EFW Mini filter, which has T-mount threads (M42)</t>
+  </si>
+  <si>
+    <t>Recommendations: at least 64 GB RAM, 2 TB SSD drive, 2 PCIex8 slots</t>
+  </si>
+  <si>
+    <t>SOFTWARE not yet compatible! Can be done on request. FOV 29 mm diagonal.</t>
+  </si>
+  <si>
+    <t>One module serves both arms, fiber switching mechanism built-in.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1832,7 +1833,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -1917,14 +1918,15 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="4" applyFont="1"/>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Excel Built-in Heading 1" xfId="3"/>
-    <cellStyle name="Excel Built-in Note" xfId="4"/>
-    <cellStyle name="Explanatory Text 2" xfId="1"/>
+    <cellStyle name="Excel Built-in Heading 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Excel Built-in Note" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2303,29 +2305,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="86.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="31.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="69.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.7109375" style="3"/>
+    <col min="1" max="1" width="42.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="86.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="69.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="21.109375" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2354,15 +2356,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -2389,27 +2391,27 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>178</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>187</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>193</v>
       </c>
@@ -2433,14 +2435,14 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -2467,7 +2469,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>21</v>
       </c>
@@ -2494,7 +2496,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>23</v>
       </c>
@@ -2521,7 +2523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>395</v>
       </c>
@@ -2548,7 +2550,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
         <v>26</v>
       </c>
@@ -2578,7 +2580,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>27</v>
       </c>
@@ -2605,7 +2607,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>29</v>
       </c>
@@ -2632,7 +2634,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
@@ -2659,7 +2661,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
@@ -2686,7 +2688,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>35</v>
       </c>
@@ -2713,7 +2715,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
@@ -2740,14 +2742,14 @@
         <v>275</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>297</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>292</v>
       </c>
@@ -2774,7 +2776,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>295</v>
       </c>
@@ -2801,7 +2803,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
         <v>299</v>
       </c>
@@ -2828,7 +2830,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
         <v>302</v>
       </c>
@@ -2855,7 +2857,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
         <v>305</v>
       </c>
@@ -2882,7 +2884,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
         <v>310</v>
       </c>
@@ -2906,43 +2908,42 @@
         <v>311</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="15" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
     </row>
-    <row r="29" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>459</v>
+        <v>498</v>
       </c>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
       </c>
-      <c r="E30" s="5">
-        <v>8000</v>
+      <c r="E30" s="5" t="s">
+        <v>341</v>
       </c>
       <c r="F30" s="5">
-        <f>E30*D30</f>
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>211</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -2969,7 +2970,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>45</v>
       </c>
@@ -2999,7 +3000,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>48</v>
       </c>
@@ -3026,7 +3027,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="33" t="s">
         <v>232</v>
       </c>
@@ -3053,7 +3054,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>81</v>
       </c>
@@ -3080,7 +3081,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
         <v>340</v>
       </c>
@@ -3107,7 +3108,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>341</v>
       </c>
@@ -3136,7 +3137,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="24">
         <v>91863</v>
       </c>
@@ -3166,7 +3167,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>169</v>
       </c>
@@ -3199,7 +3200,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
         <v>261</v>
       </c>
@@ -3232,7 +3233,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="33" t="s">
         <v>260</v>
       </c>
@@ -3262,7 +3263,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
         <v>327</v>
       </c>
@@ -3292,7 +3293,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="33" t="s">
         <v>76</v>
       </c>
@@ -3322,7 +3323,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
         <v>214</v>
       </c>
@@ -3352,7 +3353,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="35" t="s">
         <v>220</v>
       </c>
@@ -3382,7 +3383,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
         <v>222</v>
       </c>
@@ -3412,7 +3413,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="35" t="s">
         <v>226</v>
       </c>
@@ -3442,7 +3443,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
         <v>229</v>
       </c>
@@ -3472,7 +3473,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
         <v>235</v>
       </c>
@@ -3502,7 +3503,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="33" t="s">
         <v>245</v>
       </c>
@@ -3529,7 +3530,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="33" t="s">
         <v>185</v>
       </c>
@@ -3559,7 +3560,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="33" t="s">
         <v>237</v>
       </c>
@@ -3589,7 +3590,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="33" t="s">
         <v>241</v>
       </c>
@@ -3619,7 +3620,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="33" t="s">
         <v>243</v>
       </c>
@@ -3649,7 +3650,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="33" t="s">
         <v>183</v>
       </c>
@@ -3676,7 +3677,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="35" t="s">
         <v>247</v>
       </c>
@@ -3706,7 +3707,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="35" t="s">
         <v>342</v>
       </c>
@@ -3736,7 +3737,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="35" t="s">
         <v>250</v>
       </c>
@@ -3766,7 +3767,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="33" t="s">
         <v>352</v>
       </c>
@@ -3796,7 +3797,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="33" t="s">
         <v>320</v>
       </c>
@@ -3826,7 +3827,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="33" t="s">
         <v>322</v>
       </c>
@@ -3853,7 +3854,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="47" t="s">
         <v>359</v>
       </c>
@@ -3883,7 +3884,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="47" t="s">
         <v>360</v>
       </c>
@@ -3913,7 +3914,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="33" t="s">
         <v>351</v>
       </c>
@@ -3943,7 +3944,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="46" t="s">
         <v>357</v>
       </c>
@@ -3973,32 +3974,32 @@
         <v>358</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="33"/>
       <c r="C68" s="33"/>
       <c r="E68" s="34"/>
       <c r="F68" s="42"/>
     </row>
-    <row r="69" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="33"/>
       <c r="C69" s="33"/>
       <c r="E69" s="34"/>
       <c r="F69" s="42"/>
     </row>
-    <row r="70" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="33"/>
       <c r="C70" s="33"/>
       <c r="E70" s="34"/>
       <c r="F70" s="42"/>
     </row>
-    <row r="71" spans="1:10" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>283</v>
       </c>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
     </row>
-    <row r="72" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="33" t="s">
         <v>26</v>
       </c>
@@ -4017,7 +4018,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="73" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
         <v>284</v>
       </c>
@@ -4038,7 +4039,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="39" t="s">
         <v>289</v>
       </c>
@@ -4059,7 +4060,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="32" t="s">
         <v>23</v>
       </c>
@@ -4078,29 +4079,29 @@
         <v>291</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
     </row>
-    <row r="77" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
     </row>
-    <row r="78" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C78" s="51" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D78" s="3">
         <v>1</v>
@@ -4113,19 +4114,19 @@
         <v>200</v>
       </c>
       <c r="I78" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="J78" s="4"/>
+    </row>
+    <row r="79" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
         <v>489</v>
-      </c>
-      <c r="J78" s="4"/>
-    </row>
-    <row r="79" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>492</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>268</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D79" s="3">
         <v>5</v>
@@ -4138,19 +4139,19 @@
         <v>5</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J79" s="4"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="70" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D80" s="3">
         <v>1</v>
@@ -4163,18 +4164,18 @@
         <v>26</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D81" s="3">
         <v>1</v>
@@ -4188,7 +4189,7 @@
       </c>
       <c r="I81" s="32"/>
     </row>
-    <row r="82" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="70" t="s">
         <v>405</v>
       </c>
@@ -4209,22 +4210,22 @@
         <v>48</v>
       </c>
       <c r="I82" s="32" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="75" t="s">
         <v>181</v>
       </c>
       <c r="F83" s="44"/>
     </row>
-    <row r="84" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="21" t="s">
         <v>182</v>
       </c>
       <c r="F84" s="44"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>412</v>
       </c>
@@ -4251,14 +4252,14 @@
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="1:9" s="26" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A86" s="25" t="s">
         <v>414</v>
       </c>
       <c r="E86" s="27"/>
       <c r="F86" s="27"/>
     </row>
-    <row r="87" spans="1:9" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="30" t="s">
         <v>374</v>
       </c>
@@ -4285,7 +4286,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="31" t="s">
         <v>375</v>
       </c>
@@ -4313,7 +4314,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="31" t="s">
         <v>379</v>
       </c>
@@ -4341,7 +4342,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>381</v>
       </c>
@@ -4369,7 +4370,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>382</v>
       </c>
@@ -4394,7 +4395,7 @@
       </c>
       <c r="H91" s="28"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>385</v>
       </c>
@@ -4419,14 +4420,14 @@
       </c>
       <c r="H92" s="28"/>
     </row>
-    <row r="93" spans="1:9" s="26" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A93" s="25" t="s">
         <v>415</v>
       </c>
       <c r="E93" s="27"/>
       <c r="F93" s="27"/>
     </row>
-    <row r="94" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>397</v>
       </c>
@@ -4453,7 +4454,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>419</v>
       </c>
@@ -4477,7 +4478,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>421</v>
       </c>
@@ -4504,7 +4505,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>430</v>
       </c>
@@ -4530,7 +4531,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>423</v>
       </c>
@@ -4557,7 +4558,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>427</v>
       </c>
@@ -4584,7 +4585,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>408</v>
       </c>
@@ -4611,7 +4612,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>367</v>
       </c>
@@ -4632,14 +4633,14 @@
         <v>436</v>
       </c>
     </row>
-    <row r="102" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
         <v>56</v>
       </c>
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>64</v>
       </c>
@@ -4666,7 +4667,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>202</v>
       </c>
@@ -4693,7 +4694,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>201</v>
       </c>
@@ -4720,7 +4721,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>206</v>
       </c>
@@ -4747,7 +4748,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>59</v>
       </c>
@@ -4771,7 +4772,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>62</v>
       </c>
@@ -4795,7 +4796,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>209</v>
       </c>
@@ -4819,7 +4820,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="32" t="s">
         <v>334</v>
       </c>
@@ -4846,7 +4847,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="111" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="32" t="s">
         <v>336</v>
       </c>
@@ -4873,7 +4874,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>129</v>
       </c>
@@ -4897,7 +4898,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>131</v>
       </c>
@@ -4921,7 +4922,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>133</v>
       </c>
@@ -4945,7 +4946,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>129</v>
       </c>
@@ -4969,22 +4970,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E116" s="42"/>
       <c r="F116" s="42"/>
     </row>
-    <row r="118" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="11"/>
       <c r="B118" s="11"/>
       <c r="C118" s="10"/>
     </row>
-    <row r="119" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="8" t="s">
         <v>119</v>
       </c>
       <c r="F119" s="9"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>120</v>
       </c>
@@ -5008,7 +5009,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>127</v>
       </c>
@@ -5029,7 +5030,7 @@
         <v>85.1</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>136</v>
       </c>
@@ -5053,7 +5054,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>139</v>
       </c>
@@ -5074,7 +5075,7 @@
         <v>103.16</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>141</v>
       </c>
@@ -5098,7 +5099,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>144</v>
       </c>
@@ -5119,7 +5120,7 @@
         <v>136.47999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>144</v>
       </c>
@@ -5140,7 +5141,7 @@
         <v>136.47999999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>147</v>
       </c>
@@ -5161,7 +5162,7 @@
         <v>60.95</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>149</v>
       </c>
@@ -5182,7 +5183,7 @@
         <v>119.416</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>151</v>
       </c>
@@ -5203,7 +5204,7 @@
         <v>105.8</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>153</v>
       </c>
@@ -5224,7 +5225,7 @@
         <v>239.2</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>345</v>
       </c>
@@ -5245,7 +5246,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>155</v>
       </c>
@@ -5266,7 +5267,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>157</v>
       </c>
@@ -5287,7 +5288,7 @@
         <v>96.23</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>159</v>
       </c>
@@ -5308,7 +5309,7 @@
         <v>102.44</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>161</v>
       </c>
@@ -5329,7 +5330,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C136" s="3" t="s">
         <v>163</v>
       </c>
@@ -5337,7 +5338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C137" s="3" t="s">
         <v>164</v>
       </c>
@@ -5348,7 +5349,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C138" s="3" t="s">
         <v>166</v>
       </c>
@@ -5356,7 +5357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="8" t="s">
         <v>174</v>
       </c>
@@ -5366,7 +5367,7 @@
       <c r="E140" s="9"/>
       <c r="F140" s="9"/>
     </row>
-    <row r="141" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="70"/>
       <c r="B141" s="70" t="s">
         <v>167</v>
@@ -5385,7 +5386,7 @@
         <v>160</v>
       </c>
       <c r="G141" s="70" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="H141" s="70"/>
       <c r="I141" s="70" t="s">
@@ -5395,7 +5396,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="142" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B142" s="70" t="s">
         <v>175</v>
       </c>
@@ -5413,10 +5414,10 @@
         <v>662</v>
       </c>
       <c r="G142" s="70" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.2">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B143" s="70" t="s">
         <v>175</v>
       </c>
@@ -5434,10 +5435,10 @@
         <v>100</v>
       </c>
       <c r="G143" s="70" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.2">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B144" s="70" t="s">
         <v>175</v>
       </c>
@@ -5455,10 +5456,10 @@
         <v>112</v>
       </c>
       <c r="G144" s="70" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="145" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.2">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="145" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B145" s="70" t="s">
         <v>175</v>
       </c>
@@ -5476,27 +5477,27 @@
         <v>729</v>
       </c>
       <c r="G145" s="70" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="148" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="148" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E148" s="20" t="s">
         <v>177</v>
       </c>
       <c r="F148" s="5">
         <f>SUM(F3:F146)</f>
-        <v>93866.255999999994</v>
+        <v>85866.255999999994</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C87" r:id="rId1" display="Mitutoyo Plan Apo Brightfield and Darkfield, 2X"/>
-    <hyperlink ref="C88" r:id="rId2" display="Plan Apo"/>
-    <hyperlink ref="C89" r:id="rId3" display="Plan Apo"/>
-    <hyperlink ref="C90" r:id="rId4" display="Plan Apo Brightfield and Darkfield "/>
-    <hyperlink ref="C94" r:id="rId5" display="MT-1 Accessory Tube Lens"/>
-    <hyperlink ref="C78" r:id="rId6"/>
+    <hyperlink ref="C87" r:id="rId1" display="Mitutoyo Plan Apo Brightfield and Darkfield, 2X" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C88" r:id="rId2" display="Plan Apo" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C89" r:id="rId3" display="Plan Apo" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C90" r:id="rId4" display="Plan Apo Brightfield and Darkfield " xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C94" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C78" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
@@ -5504,24 +5505,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="47.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5550,14 +5552,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="7" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>178</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:9" s="63" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="63" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="63">
         <v>1008062</v>
       </c>
@@ -5570,7 +5572,7 @@
       <c r="D3" s="63">
         <v>1</v>
       </c>
-      <c r="E3" s="64">
+      <c r="E3" s="76">
         <v>7400</v>
       </c>
       <c r="F3" s="64">
@@ -5578,10 +5580,10 @@
         <v>7400</v>
       </c>
       <c r="I3" s="63" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="63" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="63" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="63" t="s">
         <v>180</v>
       </c>
@@ -5591,7 +5593,7 @@
       <c r="D4" s="63">
         <v>1</v>
       </c>
-      <c r="E4" s="64">
+      <c r="E4" s="76">
         <v>20000</v>
       </c>
       <c r="F4" s="64">
@@ -5602,29 +5604,35 @@
         <v>347</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="52" t="s">
+        <v>460</v>
+      </c>
+      <c r="C5" s="52" t="s">
         <v>461</v>
       </c>
-      <c r="C5" s="52" t="s">
-        <v>463</v>
-      </c>
       <c r="D5" s="52">
         <v>1</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="52">
+        <v>50000</v>
+      </c>
+      <c r="F5" s="52">
+        <v>50000</v>
+      </c>
+      <c r="I5" s="52" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>462</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>464</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B8" s="52" t="s">
         <v>189</v>
       </c>
@@ -5642,19 +5650,19 @@
         <v>25000</v>
       </c>
       <c r="I8" s="52" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:9" s="26" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>416</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
     </row>
-    <row r="12" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="52" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="52" t="s">
         <v>397</v>
       </c>
@@ -5684,7 +5692,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="52" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="52" t="s">
         <v>400</v>
       </c>
@@ -5714,7 +5722,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
         <v>402</v>
       </c>
@@ -5744,7 +5752,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
         <v>405</v>
       </c>
@@ -5774,7 +5782,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="56" t="s">
         <v>287</v>
       </c>
@@ -5804,21 +5812,21 @@
         <v>441</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:10" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="70" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="70" t="s">
         <v>314</v>
       </c>
@@ -5846,7 +5854,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="70" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="70" t="s">
         <v>315</v>
       </c>
@@ -5874,7 +5882,7 @@
       </c>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" s="70" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="70" t="s">
         <v>317</v>
       </c>
@@ -5901,7 +5909,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="70" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="70" t="s">
         <v>329</v>
       </c>
@@ -5920,21 +5928,21 @@
         <v>328</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>439</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:10" s="61" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" s="61" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
         <v>440</v>
       </c>
       <c r="E25" s="62"/>
       <c r="F25" s="62"/>
     </row>
-    <row r="26" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="56" t="s">
         <v>362</v>
       </c>
@@ -5964,7 +5972,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="56" t="s">
         <v>365</v>
       </c>
@@ -5994,7 +6002,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="56" t="s">
         <v>341</v>
       </c>
@@ -6024,7 +6032,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
         <v>391</v>
       </c>
@@ -6051,7 +6059,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="56" t="s">
         <v>392</v>
       </c>
@@ -6081,7 +6089,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="59" t="s">
         <v>367</v>
       </c>
@@ -6111,7 +6119,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="59" t="s">
         <v>367</v>
       </c>
@@ -6141,7 +6149,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" s="53" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="56" t="s">
         <v>257</v>
       </c>
@@ -6168,14 +6176,14 @@
         <v>438</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>56</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
     </row>
-    <row r="38" spans="1:9" s="63" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" s="63" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="63" t="s">
         <v>60</v>
       </c>
@@ -6202,7 +6210,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>66</v>
       </c>
@@ -6210,7 +6218,7 @@
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
     </row>
-    <row r="43" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="52" t="s">
         <v>67</v>
       </c>
@@ -6231,7 +6239,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="52" t="s">
         <v>70</v>
       </c>
@@ -6252,7 +6260,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="52" t="s">
         <v>72</v>
       </c>
@@ -6273,7 +6281,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="52" t="s">
         <v>74</v>
       </c>
@@ -6294,7 +6302,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="52" t="s">
         <v>77</v>
       </c>
@@ -6315,7 +6323,7 @@
         <v>94.180155999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="52" t="s">
         <v>79</v>
       </c>
@@ -6336,7 +6344,7 @@
         <v>36.799999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="52" t="s">
         <v>83</v>
       </c>
@@ -6357,7 +6365,7 @@
         <v>42.42</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="52" t="s">
         <v>85</v>
       </c>
@@ -6381,7 +6389,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="52" t="s">
         <v>88</v>
       </c>
@@ -6405,7 +6413,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="52" t="s">
         <v>90</v>
       </c>
@@ -6429,7 +6437,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="52" t="s">
         <v>92</v>
       </c>
@@ -6450,7 +6458,7 @@
         <v>60.95</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="52" t="s">
         <v>94</v>
       </c>
@@ -6474,7 +6482,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="52" t="s">
         <v>97</v>
       </c>
@@ -6498,7 +6506,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="52" t="s">
         <v>99</v>
       </c>
@@ -6519,7 +6527,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="52" t="s">
         <v>101</v>
       </c>
@@ -6540,7 +6548,7 @@
         <v>19.09</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="52" t="s">
         <v>103</v>
       </c>
@@ -6564,7 +6572,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="52" t="s">
         <v>106</v>
       </c>
@@ -6588,7 +6596,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="52" t="s">
         <v>108</v>
       </c>
@@ -6612,7 +6620,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="52" t="s">
         <v>110</v>
       </c>
@@ -6636,7 +6644,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="52" t="s">
         <v>114</v>
       </c>
@@ -6657,7 +6665,7 @@
         <v>77.745599999999996</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B63" s="52" t="s">
         <v>116</v>
       </c>
@@ -6678,7 +6686,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B64" s="52" t="s">
         <v>116</v>
       </c>
@@ -6699,13 +6707,13 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
         <v>445</v>
       </c>
       <c r="F66" s="9"/>
     </row>
-    <row r="67" spans="1:10" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="52" t="s">
         <v>124</v>
       </c>
@@ -6729,7 +6737,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>446</v>
       </c>
@@ -6753,7 +6761,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>453</v>
       </c>
@@ -6777,13 +6785,13 @@
         <v>454</v>
       </c>
     </row>
-    <row r="71" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
         <v>455</v>
       </c>
       <c r="F71" s="9"/>
     </row>
-    <row r="72" spans="1:10" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="52" t="s">
         <v>456</v>
       </c>
@@ -6792,7 +6800,7 @@
       <c r="F72" s="55"/>
       <c r="J72" s="68"/>
     </row>
-    <row r="73" spans="1:10" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="52" t="s">
         <v>457</v>
       </c>
@@ -6801,13 +6809,13 @@
       <c r="F73" s="55"/>
       <c r="J73" s="68"/>
     </row>
-    <row r="74" spans="1:10" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C74" s="68"/>
       <c r="E74" s="55"/>
       <c r="F74" s="55"/>
       <c r="J74" s="68"/>
     </row>
-    <row r="75" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
         <v>174</v>
       </c>
@@ -6817,15 +6825,15 @@
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
     </row>
-    <row r="76" spans="1:10" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="73" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B76" s="73" t="s">
         <v>175</v>
       </c>
       <c r="C76" s="73" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D76" s="73">
         <v>1</v>
@@ -6841,15 +6849,15 @@
         <v>176</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="73" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B77" s="73" t="s">
         <v>175</v>
       </c>
       <c r="C77" s="73" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D77" s="73">
         <v>1</v>
@@ -6862,15 +6870,15 @@
         <v>764</v>
       </c>
     </row>
-    <row r="78" spans="1:10" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="73" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B78" s="73" t="s">
         <v>175</v>
       </c>
       <c r="C78" s="73" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D78" s="73">
         <v>1</v>
@@ -6886,15 +6894,15 @@
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="73" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B79" s="73" t="s">
         <v>175</v>
       </c>
       <c r="C79" s="73" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D79" s="73">
         <v>1</v>
@@ -6907,15 +6915,15 @@
         <v>952</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="73" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B80" s="73" t="s">
         <v>175</v>
       </c>
       <c r="C80" s="73" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="D80" s="73">
         <v>1</v>
@@ -6928,15 +6936,15 @@
         <v>99.5</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="73" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B81" s="73" t="s">
         <v>175</v>
       </c>
       <c r="C81" s="73" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D81" s="73">
         <v>1</v>
@@ -6949,15 +6957,15 @@
         <v>128.5</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="73" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B82" s="73" t="s">
         <v>175</v>
       </c>
       <c r="C82" s="73" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D82" s="73">
         <v>1</v>
@@ -6970,15 +6978,15 @@
         <v>156</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" s="73" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="73" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B83" s="73" t="s">
         <v>175</v>
       </c>
       <c r="C83" s="73" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D83" s="73">
         <v>1</v>
@@ -6993,8 +7001,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1"/>
-    <hyperlink ref="C13" r:id="rId2"/>
+    <hyperlink ref="C12" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C13" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -7002,12 +7010,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
add 20x objective, adjust total cost
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB27C5D-16E7-42C1-A427-422B62805AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AA2EBB-783C-4678-B2A5-565AF1D788B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5952" yWindow="3864" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="506">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -1593,6 +1593,21 @@
   </si>
   <si>
     <t>One module serves both arms, fiber switching mechanism built-in.</t>
+  </si>
+  <si>
+    <t>Works best with the Mitutoyo MT-1 tube lens. Optional.</t>
+  </si>
+  <si>
+    <t>378-847</t>
+  </si>
+  <si>
+    <t>Mitutoyo</t>
+  </si>
+  <si>
+    <t>Mitutoyo G Plan APO 20X/t3,5</t>
+  </si>
+  <si>
+    <t>Corrected for 3.5 mm of glass (n1.52). Thread is unusual, but fits SM1.</t>
   </si>
 </sst>
 </file>
@@ -2306,10 +2321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J148"/>
+  <dimension ref="A1:J149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4276,7 +4291,7 @@
         <v>912</v>
       </c>
       <c r="F87" s="29">
-        <f t="shared" ref="F87:F92" si="4">E87*D87</f>
+        <f t="shared" ref="F87:F93" si="4">E87*D87</f>
         <v>912</v>
       </c>
       <c r="G87" s="3" t="s">
@@ -4325,21 +4340,21 @@
         <v>378</v>
       </c>
       <c r="D89" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" s="5">
         <v>1540</v>
       </c>
       <c r="F89" s="29">
         <f t="shared" si="4"/>
-        <v>1540</v>
+        <v>0</v>
       </c>
       <c r="G89" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H89" s="28"/>
       <c r="I89" s="3" t="s">
-        <v>434</v>
+        <v>501</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -4370,754 +4385,761 @@
         <v>434</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
-        <v>382</v>
+    <row r="91" spans="1:9" s="70" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="70" t="s">
+        <v>502</v>
       </c>
       <c r="B91" s="28" t="s">
-        <v>268</v>
-      </c>
-      <c r="C91" s="50" t="s">
-        <v>383</v>
-      </c>
-      <c r="D91" s="3">
-        <v>4</v>
-      </c>
-      <c r="E91" s="5">
-        <v>1</v>
+        <v>503</v>
+      </c>
+      <c r="C91" s="51" t="s">
+        <v>504</v>
+      </c>
+      <c r="D91" s="70">
+        <v>0</v>
+      </c>
+      <c r="E91" s="71">
+        <v>3670</v>
       </c>
       <c r="F91" s="29">
         <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="G91" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G91" s="70" t="s">
         <v>13</v>
       </c>
       <c r="H91" s="28"/>
+      <c r="I91" s="70" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>68</v>
+        <v>268</v>
       </c>
       <c r="C92" s="50" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D92" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E92" s="5">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="F92" s="29">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="G92" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H92" s="28"/>
     </row>
-    <row r="93" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A93" s="25" t="s">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="B93" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C93" s="50" t="s">
+        <v>386</v>
+      </c>
+      <c r="D93" s="3">
+        <v>1</v>
+      </c>
+      <c r="E93" s="5">
+        <v>60</v>
+      </c>
+      <c r="F93" s="29">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H93" s="28"/>
+    </row>
+    <row r="94" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A94" s="25" t="s">
         <v>415</v>
       </c>
-      <c r="E93" s="27"/>
-      <c r="F93" s="27"/>
-    </row>
-    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="3" t="s">
+      <c r="E94" s="27"/>
+      <c r="F94" s="27"/>
+    </row>
+    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="B94" s="28" t="s">
+      <c r="B95" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="C94" s="51" t="s">
+      <c r="C95" s="51" t="s">
         <v>417</v>
       </c>
-      <c r="D94" s="3">
-        <v>1</v>
-      </c>
-      <c r="E94" s="5">
+      <c r="D95" s="3">
+        <v>1</v>
+      </c>
+      <c r="E95" s="5">
         <v>752</v>
-      </c>
-      <c r="F94" s="5">
-        <f>D94*E94</f>
-        <v>752</v>
-      </c>
-      <c r="G94" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I94" s="3" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="B95" s="28" t="s">
-        <v>268</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="D95" s="3">
-        <v>1</v>
-      </c>
-      <c r="E95" s="5">
-        <v>1</v>
       </c>
       <c r="F95" s="5">
         <f>D95*E95</f>
-        <v>1</v>
+        <v>752</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="I95" s="3" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B96" s="28" t="s">
-        <v>68</v>
+        <v>268</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D96" s="3">
         <v>1</v>
       </c>
       <c r="E96" s="5">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="F96" s="5">
         <f>D96*E96</f>
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="G96" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I96" s="3" t="s">
-        <v>426</v>
-      </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="B97" s="28" t="s">
-        <v>268</v>
+        <v>68</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="D97" s="3">
         <v>1</v>
       </c>
       <c r="E97" s="5">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="F97" s="5">
-        <v>1</v>
+        <f>D97*E97</f>
+        <v>36</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="B98" s="28" t="s">
-        <v>68</v>
+        <v>268</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="D98" s="3">
         <v>1</v>
       </c>
       <c r="E98" s="5">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="F98" s="5">
-        <f>D98*E98</f>
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B99" s="28" t="s">
         <v>68</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D99" s="3">
         <v>1</v>
       </c>
       <c r="E99" s="5">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="F99" s="5">
         <f>D99*E99</f>
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="G99" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>408</v>
+        <v>427</v>
       </c>
       <c r="B100" s="28" t="s">
         <v>68</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>409</v>
+        <v>428</v>
       </c>
       <c r="D100" s="3">
         <v>1</v>
       </c>
       <c r="E100" s="5">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="F100" s="5">
         <f>D100*E100</f>
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="G100" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A101" s="4" t="s">
-        <v>367</v>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>408</v>
       </c>
       <c r="B101" s="28" t="s">
-        <v>435</v>
+        <v>68</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>384</v>
+        <v>409</v>
+      </c>
+      <c r="D101" s="3">
+        <v>1</v>
+      </c>
+      <c r="E101" s="5">
+        <v>112</v>
       </c>
       <c r="F101" s="5">
         <f>D101*E101</f>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I101" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="B102" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="F102" s="5">
+        <f>D102*E102</f>
+        <v>0</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I102" s="3" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="102" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A102" s="6" t="s">
+    <row r="103" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A103" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E102" s="9"/>
-      <c r="F102" s="9"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D103" s="3">
-        <v>1</v>
-      </c>
-      <c r="E103" s="5">
-        <v>3582</v>
-      </c>
-      <c r="F103" s="5">
-        <f t="shared" ref="F103:F115" si="5">E103*D103</f>
-        <v>3582</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I103" s="3" t="s">
-        <v>197</v>
-      </c>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>202</v>
+        <v>64</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C104" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D104" s="3">
+        <v>1</v>
+      </c>
+      <c r="E104" s="5">
+        <v>3582</v>
+      </c>
+      <c r="F104" s="5">
+        <f t="shared" ref="F104:F116" si="5">E104*D104</f>
+        <v>3582</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C105" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D104" s="3">
-        <v>1</v>
-      </c>
-      <c r="E104" s="5">
+      <c r="D105" s="3">
+        <v>1</v>
+      </c>
+      <c r="E105" s="5">
         <v>1630</v>
       </c>
-      <c r="F104" s="5">
+      <c r="F105" s="5">
         <f t="shared" si="5"/>
         <v>1630</v>
       </c>
-      <c r="G104" s="3" t="s">
+      <c r="G105" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I104" s="3" t="s">
+      <c r="I105" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B106" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="C106" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="D105" s="3">
-        <v>1</v>
-      </c>
-      <c r="E105" s="5">
+      <c r="D106" s="3">
+        <v>1</v>
+      </c>
+      <c r="E106" s="5">
         <v>886</v>
       </c>
-      <c r="F105" s="5">
+      <c r="F106" s="5">
         <f t="shared" si="5"/>
         <v>886</v>
       </c>
-      <c r="G105" s="3" t="s">
+      <c r="G106" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I105" s="3" t="s">
+      <c r="I106" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D106" s="3">
-        <v>1</v>
-      </c>
-      <c r="E106" s="5">
+      <c r="D107" s="3">
+        <v>1</v>
+      </c>
+      <c r="E107" s="5">
         <v>163</v>
       </c>
-      <c r="F106" s="5">
+      <c r="F107" s="5">
         <f t="shared" si="5"/>
         <v>163</v>
       </c>
-      <c r="G106" s="3" t="s">
+      <c r="G107" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I106" s="3" t="s">
+      <c r="I107" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B108" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D107" s="3">
-        <v>1</v>
-      </c>
-      <c r="E107" s="5">
+      <c r="D108" s="3">
+        <v>1</v>
+      </c>
+      <c r="E108" s="5">
         <v>11</v>
       </c>
-      <c r="F107" s="5">
+      <c r="F108" s="5">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="G107" s="3" t="s">
+      <c r="G108" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B109" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D108" s="3">
-        <v>1</v>
-      </c>
-      <c r="E108" s="5">
+      <c r="D109" s="3">
+        <v>1</v>
+      </c>
+      <c r="E109" s="5">
         <v>520</v>
       </c>
-      <c r="F108" s="5">
+      <c r="F109" s="5">
         <f t="shared" si="5"/>
         <v>520</v>
       </c>
-      <c r="G108" s="3" t="s">
+      <c r="G109" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B110" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="C110" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D109" s="3">
-        <v>1</v>
-      </c>
-      <c r="E109" s="5">
+      <c r="D110" s="3">
+        <v>1</v>
+      </c>
+      <c r="E110" s="5">
         <v>193</v>
       </c>
-      <c r="F109" s="5">
+      <c r="F110" s="5">
         <f t="shared" si="5"/>
         <v>193</v>
       </c>
-      <c r="G109" s="3" t="s">
+      <c r="G110" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="32" t="s">
+    <row r="111" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="32" t="s">
         <v>334</v>
       </c>
-      <c r="B110" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C110" s="32" t="s">
+      <c r="B111" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C111" s="32" t="s">
         <v>335</v>
       </c>
-      <c r="D110" s="32">
+      <c r="D111" s="32">
         <v>10</v>
       </c>
-      <c r="E110" s="42">
+      <c r="E111" s="42">
         <v>12</v>
       </c>
-      <c r="F110" s="42">
+      <c r="F111" s="42">
         <f t="shared" si="5"/>
         <v>120</v>
       </c>
-      <c r="G110" s="32" t="s">
+      <c r="G111" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="I110" s="32" t="s">
+      <c r="I111" s="32" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="111" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="32" t="s">
+    <row r="112" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="32" t="s">
         <v>336</v>
       </c>
-      <c r="B111" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C111" s="32" t="s">
+      <c r="B112" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C112" s="32" t="s">
         <v>337</v>
       </c>
-      <c r="D111" s="32">
-        <v>1</v>
-      </c>
-      <c r="E111" s="42">
+      <c r="D112" s="32">
+        <v>1</v>
+      </c>
+      <c r="E112" s="42">
         <v>14</v>
       </c>
-      <c r="F111" s="42">
+      <c r="F112" s="42">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="G111" s="32" t="s">
+      <c r="G112" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="I111" s="32" t="s">
+      <c r="I112" s="32" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B112" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C112" s="3" t="s">
+      <c r="B113" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D112" s="3">
+      <c r="D113" s="3">
         <v>4</v>
       </c>
-      <c r="E112" s="5">
+      <c r="E113" s="5">
         <v>15.25</v>
       </c>
-      <c r="F112" s="5">
+      <c r="F113" s="5">
         <f t="shared" si="5"/>
         <v>61</v>
       </c>
-      <c r="G112" s="32" t="s">
+      <c r="G113" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B113" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C113" s="3" t="s">
+      <c r="B114" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D113" s="3">
+      <c r="D114" s="3">
         <v>10</v>
       </c>
-      <c r="E113" s="5">
+      <c r="E114" s="5">
         <v>16.5</v>
       </c>
-      <c r="F113" s="5">
+      <c r="F114" s="5">
         <f t="shared" si="5"/>
         <v>165</v>
       </c>
-      <c r="G113" s="32" t="s">
+      <c r="G114" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B114" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C114" s="3" t="s">
+      <c r="B115" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D115" s="3">
         <v>10</v>
       </c>
-      <c r="E114" s="5">
+      <c r="E115" s="5">
         <v>24</v>
       </c>
-      <c r="F114" s="5">
+      <c r="F115" s="5">
         <f t="shared" si="5"/>
         <v>240</v>
       </c>
-      <c r="G114" s="32" t="s">
+      <c r="G115" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B115" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C115" s="3" t="s">
+      <c r="B116" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C116" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D116" s="3">
         <v>6</v>
       </c>
-      <c r="E115" s="5">
+      <c r="E116" s="5">
         <v>24</v>
       </c>
-      <c r="F115" s="5">
+      <c r="F116" s="5">
         <f t="shared" si="5"/>
         <v>144</v>
       </c>
-      <c r="G115" s="32" t="s">
+      <c r="G116" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E116" s="42"/>
-      <c r="F116" s="42"/>
-    </row>
-    <row r="118" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="11"/>
-      <c r="B118" s="11"/>
-      <c r="C118" s="10"/>
-    </row>
-    <row r="119" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="8" t="s">
+    <row r="117" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E117" s="42"/>
+      <c r="F117" s="42"/>
+    </row>
+    <row r="119" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A119" s="11"/>
+      <c r="B119" s="11"/>
+      <c r="C119" s="10"/>
+    </row>
+    <row r="120" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A120" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="F119" s="9"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D120" s="3">
-        <v>4</v>
-      </c>
-      <c r="E120" s="5">
-        <v>16.5</v>
-      </c>
-      <c r="F120" s="5">
-        <f t="shared" ref="F120:F135" si="6">E120*D120</f>
-        <v>66</v>
-      </c>
-      <c r="I120" s="3" t="s">
-        <v>123</v>
-      </c>
+      <c r="F120" s="9"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D121" s="3">
+        <v>4</v>
+      </c>
+      <c r="E121" s="5">
+        <v>16.5</v>
+      </c>
+      <c r="F121" s="5">
+        <f t="shared" ref="F121:F136" si="6">E121*D121</f>
+        <v>66</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B121" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C121" s="3" t="s">
+      <c r="B122" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C122" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D121" s="3">
-        <v>1</v>
-      </c>
-      <c r="E121" s="5">
+      <c r="D122" s="3">
+        <v>1</v>
+      </c>
+      <c r="E122" s="5">
         <v>85.1</v>
       </c>
-      <c r="F121" s="5">
+      <c r="F122" s="5">
         <f t="shared" si="6"/>
         <v>85.1</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="3" t="s">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B122" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C122" s="3" t="s">
+      <c r="B123" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C123" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D122" s="3">
+      <c r="D123" s="3">
         <v>2</v>
       </c>
-      <c r="E122" s="5">
+      <c r="E123" s="5">
         <v>32</v>
       </c>
-      <c r="F122" s="5">
+      <c r="F123" s="5">
         <f t="shared" si="6"/>
         <v>64</v>
       </c>
-      <c r="I122" s="3" t="s">
+      <c r="I123" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B123" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C123" s="3" t="s">
+      <c r="B124" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C124" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D123" s="3">
+      <c r="D124" s="3">
         <v>2</v>
       </c>
-      <c r="E123" s="5">
+      <c r="E124" s="5">
         <v>51.58</v>
       </c>
-      <c r="F123" s="5">
+      <c r="F124" s="5">
         <f t="shared" si="6"/>
         <v>103.16</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B124" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C124" s="3" t="s">
+      <c r="B125" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D124" s="3">
-        <v>1</v>
-      </c>
-      <c r="E124" s="5">
+      <c r="D125" s="3">
+        <v>1</v>
+      </c>
+      <c r="E125" s="5">
         <v>60</v>
       </c>
-      <c r="F124" s="5">
+      <c r="F125" s="5">
         <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="I124" s="3" t="s">
+      <c r="I125" s="3" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D125" s="3">
-        <v>1</v>
-      </c>
-      <c r="E125" s="5">
-        <v>136.47999999999999</v>
-      </c>
-      <c r="F125" s="5">
-        <f t="shared" si="6"/>
-        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -5128,7 +5150,7 @@
         <v>68</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D126" s="3">
         <v>1</v>
@@ -5143,278 +5165,278 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D127" s="3">
         <v>1</v>
       </c>
       <c r="E127" s="5">
-        <v>60.95</v>
+        <v>136.47999999999999</v>
       </c>
       <c r="F127" s="5">
         <f t="shared" si="6"/>
-        <v>60.95</v>
+        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D128" s="3">
         <v>1</v>
       </c>
       <c r="E128" s="5">
-        <v>119.416</v>
+        <v>60.95</v>
       </c>
       <c r="F128" s="5">
         <f t="shared" si="6"/>
-        <v>119.416</v>
+        <v>60.95</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D129" s="3">
         <v>1</v>
       </c>
       <c r="E129" s="5">
-        <v>105.8</v>
+        <v>119.416</v>
       </c>
       <c r="F129" s="5">
         <f t="shared" si="6"/>
-        <v>105.8</v>
+        <v>119.416</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D130" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E130" s="5">
-        <v>119.6</v>
+        <v>105.8</v>
       </c>
       <c r="F130" s="5">
         <f t="shared" si="6"/>
-        <v>239.2</v>
+        <v>105.8</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>345</v>
+        <v>153</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>346</v>
+        <v>154</v>
       </c>
       <c r="D131" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E131" s="5">
-        <v>100</v>
+        <v>119.6</v>
       </c>
       <c r="F131" s="5">
         <f t="shared" si="6"/>
-        <v>100</v>
+        <v>239.2</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>155</v>
+        <v>345</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>156</v>
+        <v>346</v>
       </c>
       <c r="D132" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E132" s="5">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F132" s="5">
         <f t="shared" si="6"/>
-        <v>184</v>
+        <v>100</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D133" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E133" s="5">
-        <v>96.23</v>
+        <v>92</v>
       </c>
       <c r="F133" s="5">
         <f t="shared" si="6"/>
-        <v>96.23</v>
+        <v>184</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D134" s="3">
         <v>1</v>
       </c>
       <c r="E134" s="5">
-        <v>102.44</v>
+        <v>96.23</v>
       </c>
       <c r="F134" s="5">
         <f t="shared" si="6"/>
-        <v>102.44</v>
+        <v>96.23</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D135" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E135" s="5">
-        <v>28</v>
+        <v>102.44</v>
       </c>
       <c r="F135" s="5">
         <f t="shared" si="6"/>
+        <v>102.44</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D136" s="3">
+        <v>2</v>
+      </c>
+      <c r="E136" s="5">
+        <v>28</v>
+      </c>
+      <c r="F136" s="5">
+        <f t="shared" si="6"/>
         <v>56</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C136" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D136" s="3">
-        <v>4</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C137" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D137" s="3">
-        <v>1</v>
-      </c>
-      <c r="I137" s="3" t="s">
-        <v>165</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C138" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D138" s="3">
+        <v>1</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C139" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D138" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="8" t="s">
+      <c r="D139" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A141" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B140" s="7" t="s">
+      <c r="B141" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="E140" s="9"/>
-      <c r="F140" s="9"/>
-    </row>
-    <row r="141" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="70"/>
-      <c r="B141" s="70" t="s">
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+    </row>
+    <row r="142" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="70"/>
+      <c r="B142" s="70" t="s">
         <v>167</v>
       </c>
-      <c r="C141" s="72" t="s">
+      <c r="C142" s="72" t="s">
         <v>172</v>
       </c>
-      <c r="D141" s="70">
+      <c r="D142" s="70">
         <v>4</v>
       </c>
-      <c r="E141" s="70">
+      <c r="E142" s="70">
         <v>40</v>
       </c>
-      <c r="F141" s="70">
-        <f>E141*D141</f>
+      <c r="F142" s="70">
+        <f>E142*D142</f>
         <v>160</v>
       </c>
-      <c r="G141" s="70" t="s">
+      <c r="G142" s="70" t="s">
         <v>478</v>
       </c>
-      <c r="H141" s="70"/>
-      <c r="I141" s="70" t="s">
+      <c r="H142" s="70"/>
+      <c r="I142" s="70" t="s">
         <v>173</v>
       </c>
-      <c r="J141" s="72" t="s">
+      <c r="J142" s="72" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="70" t="s">
-        <v>175</v>
-      </c>
-      <c r="C142" s="70" t="s">
-        <v>413</v>
-      </c>
-      <c r="D142" s="70">
-        <v>2</v>
-      </c>
-      <c r="E142" s="71">
-        <v>331</v>
-      </c>
-      <c r="F142" s="71">
-        <f>E142*D142</f>
-        <v>662</v>
-      </c>
-      <c r="G142" s="70" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="143" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.25">
@@ -5422,17 +5444,17 @@
         <v>175</v>
       </c>
       <c r="C143" s="70" t="s">
-        <v>330</v>
+        <v>413</v>
       </c>
       <c r="D143" s="70">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E143" s="71">
-        <v>25</v>
+        <v>331</v>
       </c>
       <c r="F143" s="71">
         <f>E143*D143</f>
-        <v>100</v>
+        <v>662</v>
       </c>
       <c r="G143" s="70" t="s">
         <v>477</v>
@@ -5443,17 +5465,17 @@
         <v>175</v>
       </c>
       <c r="C144" s="70" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D144" s="70">
         <v>4</v>
       </c>
       <c r="E144" s="71">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F144" s="71">
         <f>E144*D144</f>
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G144" s="70" t="s">
         <v>477</v>
@@ -5464,29 +5486,50 @@
         <v>175</v>
       </c>
       <c r="C145" s="70" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D145" s="70">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E145" s="71">
-        <v>121.5</v>
+        <v>28</v>
       </c>
       <c r="F145" s="71">
         <f>E145*D145</f>
-        <v>729</v>
+        <v>112</v>
       </c>
       <c r="G145" s="70" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="148" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E148" s="20" t="s">
+    <row r="146" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B146" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="C146" s="70" t="s">
+        <v>332</v>
+      </c>
+      <c r="D146" s="70">
+        <v>6</v>
+      </c>
+      <c r="E146" s="71">
+        <v>121.5</v>
+      </c>
+      <c r="F146" s="71">
+        <f>E146*D146</f>
+        <v>729</v>
+      </c>
+      <c r="G146" s="70" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="149" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E149" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="F148" s="5">
-        <f>SUM(F3:F146)</f>
-        <v>85866.255999999994</v>
+      <c r="F149" s="5">
+        <f>SUM(F3:F147)</f>
+        <v>84327.255999999994</v>
       </c>
     </row>
   </sheetData>
@@ -5496,11 +5539,12 @@
     <hyperlink ref="C88" r:id="rId2" display="Plan Apo" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="C89" r:id="rId3" display="Plan Apo" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="C90" r:id="rId4" display="Plan Apo Brightfield and Darkfield " xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C94" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C95" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="C78" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C91" r:id="rId7" xr:uid="{3002EF90-377A-4FAD-A836-B22D0D243A96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add 1:1 relay lenses
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AA2EBB-783C-4678-B2A5-565AF1D788B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F9FFD2-ABEC-40CF-B39C-A7E5E8171C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5952" yWindow="3864" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="509">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -1608,6 +1608,15 @@
   </si>
   <si>
     <t>Corrected for 3.5 mm of glass (n1.52). Thread is unusual, but fits SM1.</t>
+  </si>
+  <si>
+    <t>f=100 mm, Ø1" Achromatic Doublet, SM1-Threaded Mount, ARC: 400-700 nm</t>
+  </si>
+  <si>
+    <t>A 1:1 relay from ETL to galvo</t>
+  </si>
+  <si>
+    <t>Lenses L2, L3 in the design view</t>
   </si>
 </sst>
 </file>
@@ -2321,20 +2330,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J149"/>
+  <dimension ref="A1:J150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I92" sqref="I92"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.5546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="24.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="86.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="81.77734375" style="3" customWidth="1"/>
     <col min="4" max="4" width="6.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="5" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="31.6640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="69.33203125" style="3" customWidth="1"/>
@@ -3169,7 +3178,7 @@
         <v>400</v>
       </c>
       <c r="F40" s="5">
-        <f t="shared" ref="F40:F67" si="3">E40*D40</f>
+        <f t="shared" ref="F40:F68" si="3">E40*D40</f>
         <v>800</v>
       </c>
       <c r="G40" s="3" t="s">
@@ -3428,572 +3437,596 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="35" t="s">
+    <row r="49" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>506</v>
+      </c>
+      <c r="D49" s="32">
+        <v>4</v>
+      </c>
+      <c r="E49" s="34">
+        <v>104</v>
+      </c>
+      <c r="F49" s="42">
+        <f t="shared" si="3"/>
+        <v>416</v>
+      </c>
+      <c r="G49" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="H49" s="32" t="s">
+        <v>507</v>
+      </c>
+      <c r="I49" s="32" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="B49" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C49" s="35" t="s">
+      <c r="B50" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="D49" s="36">
+      <c r="D50" s="36">
         <v>4</v>
       </c>
-      <c r="E49" s="37">
+      <c r="E50" s="37">
         <v>189</v>
       </c>
-      <c r="F49" s="43">
+      <c r="F50" s="43">
         <f t="shared" si="3"/>
         <v>756</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="G50" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H49" s="36" t="s">
+      <c r="H50" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="I49" s="36" t="s">
+      <c r="I50" s="36" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="35" t="s">
+    <row r="51" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="35" t="s">
         <v>229</v>
       </c>
-      <c r="B50" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C50" s="35" t="s">
+      <c r="B51" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="35" t="s">
         <v>230</v>
       </c>
-      <c r="D50" s="36">
+      <c r="D51" s="36">
         <v>4</v>
       </c>
-      <c r="E50" s="37">
+      <c r="E51" s="37">
         <v>110</v>
       </c>
-      <c r="F50" s="43">
+      <c r="F51" s="43">
         <f t="shared" si="3"/>
         <v>440</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="G51" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H50" s="36" t="s">
+      <c r="H51" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="I50" s="36" t="s">
+      <c r="I51" s="36" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="33" t="s">
+    <row r="52" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="B51" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C51" s="33" t="s">
+      <c r="B52" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="D51" s="32">
+      <c r="D52" s="32">
         <v>4</v>
       </c>
-      <c r="E51" s="34">
+      <c r="E52" s="34">
         <v>13</v>
       </c>
-      <c r="F51" s="42">
+      <c r="F52" s="42">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="G52" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H51" s="32" t="s">
+      <c r="H52" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="I51" s="32" t="s">
+      <c r="I52" s="32" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
+    <row r="53" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
         <v>245</v>
       </c>
-      <c r="B52" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52" s="33" t="s">
+      <c r="B53" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D52" s="32">
+      <c r="D53" s="32">
         <v>2</v>
       </c>
-      <c r="E52" s="34">
+      <c r="E53" s="34">
         <v>8</v>
       </c>
-      <c r="F52" s="42">
+      <c r="F53" s="42">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G53" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H52" s="32" t="s">
+      <c r="H53" s="32" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="33" t="s">
+    <row r="54" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="B53" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C53" s="33" t="s">
+      <c r="B54" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="D53" s="32">
+      <c r="D54" s="32">
         <v>4</v>
       </c>
-      <c r="E53" s="34">
+      <c r="E54" s="34">
         <v>7</v>
       </c>
-      <c r="F53" s="42">
+      <c r="F54" s="42">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="G54" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H53" s="32" t="s">
+      <c r="H54" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="I53" s="32" t="s">
+      <c r="I54" s="32" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
+    <row r="55" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
         <v>237</v>
       </c>
-      <c r="B54" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C54" s="33" t="s">
+      <c r="B55" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C55" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="D54" s="32">
+      <c r="D55" s="32">
         <v>6</v>
       </c>
-      <c r="E54" s="34">
+      <c r="E55" s="34">
         <v>5</v>
       </c>
-      <c r="F54" s="42">
+      <c r="F55" s="42">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="G54" s="3" t="s">
+      <c r="G55" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H54" s="32" t="s">
+      <c r="H55" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="I54" s="32" t="s">
+      <c r="I55" s="32" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="33" t="s">
+    <row r="56" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
         <v>241</v>
       </c>
-      <c r="B55" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C55" s="33" t="s">
+      <c r="B56" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="D55" s="32">
+      <c r="D56" s="32">
         <v>4</v>
       </c>
-      <c r="E55" s="34">
+      <c r="E56" s="34">
         <v>6</v>
       </c>
-      <c r="F55" s="42">
+      <c r="F56" s="42">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="G56" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H55" s="32" t="s">
+      <c r="H56" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="I55" s="32" t="s">
+      <c r="I56" s="32" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="33" t="s">
+    <row r="57" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
         <v>243</v>
       </c>
-      <c r="B56" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C56" s="33" t="s">
+      <c r="B57" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57" s="33" t="s">
         <v>244</v>
       </c>
-      <c r="D56" s="32">
+      <c r="D57" s="32">
         <v>4</v>
       </c>
-      <c r="E56" s="34">
+      <c r="E57" s="34">
         <v>5</v>
       </c>
-      <c r="F56" s="42">
+      <c r="F57" s="42">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G57" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H56" s="32" t="s">
+      <c r="H57" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="I56" s="32" t="s">
+      <c r="I57" s="32" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
+    <row r="58" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="B57" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C57" s="33" t="s">
+      <c r="B58" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="D57" s="32">
+      <c r="D58" s="32">
         <v>2</v>
       </c>
-      <c r="E57" s="34">
+      <c r="E58" s="34">
         <v>5</v>
       </c>
-      <c r="F57" s="42">
+      <c r="F58" s="42">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G58" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H57" s="32" t="s">
+      <c r="H58" s="32" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="35" t="s">
+    <row r="59" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="35" t="s">
         <v>247</v>
       </c>
-      <c r="B58" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C58" s="35" t="s">
+      <c r="B59" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="35" t="s">
         <v>248</v>
       </c>
-      <c r="D58" s="36">
+      <c r="D59" s="36">
         <v>2</v>
       </c>
-      <c r="E58" s="37">
+      <c r="E59" s="37">
         <v>398</v>
       </c>
-      <c r="F58" s="43">
+      <c r="F59" s="43">
         <f t="shared" si="3"/>
         <v>796</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="G59" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H58" s="36" t="s">
+      <c r="H59" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="I58" s="36" t="s">
+      <c r="I59" s="36" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="35" t="s">
+    <row r="60" spans="1:9" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="35" t="s">
         <v>342</v>
       </c>
-      <c r="B59" s="32" t="s">
+      <c r="B60" s="32" t="s">
         <v>437</v>
       </c>
-      <c r="C59" s="35" t="s">
+      <c r="C60" s="35" t="s">
         <v>343</v>
       </c>
-      <c r="D59" s="36">
+      <c r="D60" s="36">
         <v>2</v>
       </c>
-      <c r="E59" s="37">
-        <v>1</v>
-      </c>
-      <c r="F59" s="43">
+      <c r="E60" s="37">
+        <v>1</v>
+      </c>
+      <c r="F60" s="43">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="G59" s="3" t="s">
+      <c r="G60" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H59" s="36" t="s">
+      <c r="H60" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="I59" s="36" t="s">
+      <c r="I60" s="36" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="35" t="s">
+    <row r="61" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="35" t="s">
         <v>250</v>
       </c>
-      <c r="B60" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C60" s="35" t="s">
+      <c r="B61" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" s="35" t="s">
         <v>251</v>
       </c>
-      <c r="D60" s="36">
+      <c r="D61" s="36">
         <v>2</v>
       </c>
-      <c r="E60" s="37">
+      <c r="E61" s="37">
         <v>30</v>
       </c>
-      <c r="F60" s="43">
+      <c r="F61" s="43">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H60" s="36" t="s">
+      <c r="H61" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="I60" s="36" t="s">
+      <c r="I61" s="36" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="33" t="s">
+    <row r="62" spans="1:9" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="33" t="s">
         <v>352</v>
       </c>
-      <c r="B61" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C61" s="33" t="s">
+      <c r="B62" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="33" t="s">
         <v>255</v>
       </c>
-      <c r="D61" s="32">
+      <c r="D62" s="32">
         <v>2</v>
       </c>
-      <c r="E61" s="34">
+      <c r="E62" s="34">
         <v>36</v>
       </c>
-      <c r="F61" s="42">
+      <c r="F62" s="42">
         <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="G61" s="3" t="s">
+      <c r="G62" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H61" s="32" t="s">
+      <c r="H62" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="I61" s="38" t="s">
+      <c r="I62" s="38" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="33" t="s">
+    <row r="63" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="33" t="s">
         <v>320</v>
       </c>
-      <c r="B62" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C62" s="33" t="s">
+      <c r="B63" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C63" s="33" t="s">
         <v>321</v>
       </c>
-      <c r="D62" s="32">
+      <c r="D63" s="32">
         <v>2</v>
       </c>
-      <c r="E62" s="34">
+      <c r="E63" s="34">
         <v>2104</v>
       </c>
-      <c r="F62" s="42">
+      <c r="F63" s="42">
         <f t="shared" si="3"/>
         <v>4208</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="G63" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H62" s="32" t="s">
+      <c r="H63" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="I62" s="32" t="s">
+      <c r="I63" s="32" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="33" t="s">
+    <row r="64" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="33" t="s">
         <v>322</v>
       </c>
-      <c r="B63" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C63" s="33" t="s">
+      <c r="B64" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" s="33" t="s">
         <v>323</v>
       </c>
-      <c r="D63" s="32">
+      <c r="D64" s="32">
         <v>2</v>
       </c>
-      <c r="E63" s="34">
+      <c r="E64" s="34">
         <v>82</v>
       </c>
-      <c r="F63" s="42">
+      <c r="F64" s="42">
         <f t="shared" si="3"/>
         <v>164</v>
       </c>
-      <c r="G63" s="3" t="s">
+      <c r="G64" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H63" s="32" t="s">
+      <c r="H64" s="32" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="47" t="s">
+    <row r="65" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="47" t="s">
         <v>359</v>
       </c>
-      <c r="B64" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C64" s="33" t="s">
+      <c r="B65" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="33" t="s">
         <v>265</v>
       </c>
-      <c r="D64" s="32">
-        <v>1</v>
-      </c>
-      <c r="E64" s="34">
+      <c r="D65" s="32">
+        <v>1</v>
+      </c>
+      <c r="E65" s="34">
         <v>495</v>
       </c>
-      <c r="F64" s="42">
+      <c r="F65" s="42">
         <f t="shared" si="3"/>
         <v>495</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="G65" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H64" s="32" t="s">
+      <c r="H65" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="I64" s="32" t="s">
+      <c r="I65" s="32" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="47" t="s">
+    <row r="66" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="47" t="s">
         <v>360</v>
       </c>
-      <c r="B65" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C65" s="33" t="s">
+      <c r="B66" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C66" s="33" t="s">
         <v>324</v>
       </c>
-      <c r="D65" s="32">
+      <c r="D66" s="32">
         <v>0</v>
       </c>
-      <c r="E65" s="34">
+      <c r="E66" s="34">
         <v>390</v>
       </c>
-      <c r="F65" s="42">
+      <c r="F66" s="42">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="G66" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H65" s="32" t="s">
+      <c r="H66" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="I65" s="32" t="s">
+      <c r="I66" s="32" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="33" t="s">
+    <row r="67" spans="1:10" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="33" t="s">
         <v>351</v>
       </c>
-      <c r="B66" s="32" t="s">
+      <c r="B67" s="32" t="s">
         <v>355</v>
       </c>
-      <c r="C66" s="33" t="s">
+      <c r="C67" s="33" t="s">
         <v>350</v>
       </c>
-      <c r="D66" s="32">
+      <c r="D67" s="32">
         <v>14</v>
       </c>
-      <c r="E66" s="34">
+      <c r="E67" s="34">
         <v>20</v>
       </c>
-      <c r="F66" s="42">
+      <c r="F67" s="42">
         <f t="shared" si="3"/>
         <v>280</v>
       </c>
-      <c r="G66" s="3" t="s">
+      <c r="G67" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H66" s="32" t="s">
+      <c r="H67" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="I66" s="38" t="s">
+      <c r="I67" s="38" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="46" t="s">
+    <row r="68" spans="1:10" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="46" t="s">
         <v>357</v>
       </c>
-      <c r="B67" s="32" t="s">
+      <c r="B68" s="32" t="s">
         <v>313</v>
       </c>
-      <c r="C67" s="33" t="s">
+      <c r="C68" s="33" t="s">
         <v>356</v>
       </c>
-      <c r="D67" s="32">
-        <v>1</v>
-      </c>
-      <c r="E67" s="34">
+      <c r="D68" s="32">
+        <v>1</v>
+      </c>
+      <c r="E68" s="34">
         <v>10</v>
       </c>
-      <c r="F67" s="42">
+      <c r="F68" s="42">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="G67" s="3" t="s">
+      <c r="G68" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H67" s="32" t="s">
+      <c r="H68" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="I67" s="32" t="s">
+      <c r="I68" s="32" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="33"/>
-      <c r="C68" s="33"/>
-      <c r="E68" s="34"/>
-      <c r="F68" s="42"/>
     </row>
     <row r="69" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="33"/>
@@ -4007,1160 +4040,1145 @@
       <c r="E70" s="34"/>
       <c r="F70" s="42"/>
     </row>
-    <row r="71" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="6" t="s">
+    <row r="71" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="33"/>
+      <c r="C71" s="33"/>
+      <c r="E71" s="34"/>
+      <c r="F71" s="42"/>
+    </row>
+    <row r="72" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A72" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-    </row>
-    <row r="72" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B72" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C72" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D72" s="32">
-        <v>1</v>
-      </c>
-      <c r="E72" s="34"/>
-      <c r="F72" s="42"/>
-      <c r="I72" s="32" t="s">
-        <v>291</v>
-      </c>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
     </row>
     <row r="73" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C73" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D73" s="32">
+        <v>1</v>
+      </c>
+      <c r="E73" s="34"/>
+      <c r="F73" s="42"/>
+      <c r="I73" s="32" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="33" t="s">
         <v>284</v>
       </c>
-      <c r="B73" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C73" s="33" t="s">
+      <c r="B74" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C74" s="33" t="s">
         <v>285</v>
       </c>
-      <c r="D73" s="32">
-        <v>1</v>
-      </c>
-      <c r="E73" s="34">
+      <c r="D74" s="32">
+        <v>1</v>
+      </c>
+      <c r="E74" s="34">
         <v>63</v>
-      </c>
-      <c r="F73" s="42">
-        <f>D73*E73</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="39" t="s">
-        <v>289</v>
-      </c>
-      <c r="B74" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C74" s="33" t="s">
-        <v>290</v>
-      </c>
-      <c r="D74" s="32">
-        <v>2</v>
-      </c>
-      <c r="E74" s="34">
-        <v>69</v>
       </c>
       <c r="F74" s="42">
         <f>D74*E74</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="39" t="s">
+        <v>289</v>
+      </c>
+      <c r="B75" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C75" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="D75" s="32">
+        <v>2</v>
+      </c>
+      <c r="E75" s="34">
+        <v>69</v>
+      </c>
+      <c r="F75" s="42">
+        <f>D75*E75</f>
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="32" t="s">
+    <row r="76" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B75" s="32" t="s">
+      <c r="B76" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C75" s="32" t="s">
+      <c r="C76" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D75" s="32">
-        <v>1</v>
-      </c>
-      <c r="E75" s="34"/>
-      <c r="F75" s="42"/>
-      <c r="I75" s="32" t="s">
+      <c r="D76" s="32">
+        <v>1</v>
+      </c>
+      <c r="E76" s="34"/>
+      <c r="F76" s="42"/>
+      <c r="I76" s="32" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="6" t="s">
+    <row r="77" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A77" s="6" t="s">
         <v>483</v>
-      </c>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9"/>
-    </row>
-    <row r="77" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
-        <v>484</v>
       </c>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
     </row>
-    <row r="78" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="C78" s="51" t="s">
-        <v>485</v>
-      </c>
-      <c r="D78" s="3">
-        <v>1</v>
-      </c>
-      <c r="E78" s="5">
-        <v>200</v>
-      </c>
-      <c r="F78" s="5">
-        <f>E78*D78</f>
-        <v>200</v>
-      </c>
-      <c r="I78" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="J78" s="4"/>
+    <row r="78" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
     </row>
     <row r="79" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C79" s="51" t="s">
+        <v>485</v>
+      </c>
+      <c r="D79" s="3">
+        <v>1</v>
+      </c>
+      <c r="E79" s="5">
+        <v>200</v>
+      </c>
+      <c r="F79" s="5">
+        <f>E79*D79</f>
+        <v>200</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="J79" s="4"/>
+    </row>
+    <row r="80" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B80" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C80" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="D79" s="3">
+      <c r="D80" s="3">
         <v>5</v>
       </c>
-      <c r="E79" s="5">
-        <v>1</v>
-      </c>
-      <c r="F79" s="71">
-        <f>E79*D79</f>
-        <v>5</v>
-      </c>
-      <c r="I79" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="J79" s="4"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="70" t="s">
-        <v>493</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="D80" s="3">
-        <v>1</v>
-      </c>
       <c r="E80" s="5">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="F80" s="71">
         <f>E80*D80</f>
+        <v>5</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="J80" s="4"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="70" t="s">
+        <v>493</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="D81" s="3">
+        <v>1</v>
+      </c>
+      <c r="E81" s="5">
         <v>26</v>
-      </c>
-      <c r="I80" s="3" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="D81" s="3">
-        <v>1</v>
-      </c>
-      <c r="E81" s="5">
-        <v>37</v>
       </c>
       <c r="F81" s="71">
         <f>E81*D81</f>
+        <v>26</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="D82" s="3">
+        <v>1</v>
+      </c>
+      <c r="E82" s="5">
         <v>37</v>
-      </c>
-      <c r="I81" s="32"/>
-    </row>
-    <row r="82" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="70" t="s">
-        <v>405</v>
-      </c>
-      <c r="B82" s="70" t="s">
-        <v>68</v>
-      </c>
-      <c r="C82" s="70" t="s">
-        <v>404</v>
-      </c>
-      <c r="D82" s="70">
-        <v>2</v>
-      </c>
-      <c r="E82" s="71">
-        <v>24</v>
       </c>
       <c r="F82" s="71">
         <f>E82*D82</f>
+        <v>37</v>
+      </c>
+      <c r="I82" s="32"/>
+    </row>
+    <row r="83" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="70" t="s">
+        <v>405</v>
+      </c>
+      <c r="B83" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="C83" s="70" t="s">
+        <v>404</v>
+      </c>
+      <c r="D83" s="70">
+        <v>2</v>
+      </c>
+      <c r="E83" s="71">
+        <v>24</v>
+      </c>
+      <c r="F83" s="71">
+        <f>E83*D83</f>
         <v>48</v>
       </c>
-      <c r="I82" s="32" t="s">
+      <c r="I83" s="32" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="83" spans="1:9" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="75" t="s">
+    <row r="84" spans="1:9" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="75" t="s">
         <v>181</v>
       </c>
-      <c r="F83" s="44"/>
-    </row>
-    <row r="84" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="21" t="s">
+      <c r="F84" s="44"/>
+    </row>
+    <row r="85" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="F84" s="44"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+      <c r="F85" s="44"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B86" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C86" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="D85" s="3">
-        <v>1</v>
-      </c>
-      <c r="E85" s="5">
+      <c r="D86" s="3">
+        <v>1</v>
+      </c>
+      <c r="E86" s="5">
         <v>625</v>
       </c>
-      <c r="F85" s="5">
-        <f>E85*D85</f>
+      <c r="F86" s="5">
+        <f>E86*D86</f>
         <v>625</v>
       </c>
-      <c r="G85" s="3" t="s">
+      <c r="G86" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I85" s="3" t="s">
+      <c r="I86" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="25" t="s">
+    <row r="87" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A87" s="25" t="s">
         <v>414</v>
       </c>
-      <c r="E86" s="27"/>
-      <c r="F86" s="27"/>
-    </row>
-    <row r="87" spans="1:9" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="30" t="s">
+      <c r="E87" s="27"/>
+      <c r="F87" s="27"/>
+    </row>
+    <row r="88" spans="1:9" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="30" t="s">
         <v>374</v>
-      </c>
-      <c r="B87" s="28" t="s">
-        <v>373</v>
-      </c>
-      <c r="C87" s="48" t="s">
-        <v>376</v>
-      </c>
-      <c r="D87" s="28">
-        <v>1</v>
-      </c>
-      <c r="E87" s="29">
-        <v>912</v>
-      </c>
-      <c r="F87" s="29">
-        <f t="shared" ref="F87:F93" si="4">E87*D87</f>
-        <v>912</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I87" s="28" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="31" t="s">
-        <v>375</v>
       </c>
       <c r="B88" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="C88" s="49" t="s">
+      <c r="C88" s="48" t="s">
+        <v>376</v>
+      </c>
+      <c r="D88" s="28">
+        <v>1</v>
+      </c>
+      <c r="E88" s="29">
+        <v>912</v>
+      </c>
+      <c r="F88" s="29">
+        <f t="shared" ref="F88:F94" si="4">E88*D88</f>
+        <v>912</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I88" s="28" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="31" t="s">
+        <v>375</v>
+      </c>
+      <c r="B89" s="28" t="s">
+        <v>373</v>
+      </c>
+      <c r="C89" s="49" t="s">
         <v>377</v>
       </c>
-      <c r="D88" s="3">
-        <v>1</v>
-      </c>
-      <c r="E88" s="5">
+      <c r="D89" s="3">
+        <v>1</v>
+      </c>
+      <c r="E89" s="5">
         <v>837</v>
       </c>
-      <c r="F88" s="29">
+      <c r="F89" s="29">
         <f t="shared" si="4"/>
         <v>837</v>
       </c>
-      <c r="G88" s="3" t="s">
+      <c r="G89" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H88" s="28"/>
-      <c r="I88" s="3" t="s">
+      <c r="H89" s="28"/>
+      <c r="I89" s="3" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="31" t="s">
+    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="B89" s="28" t="s">
+      <c r="B90" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="C89" s="49" t="s">
+      <c r="C90" s="49" t="s">
         <v>378</v>
       </c>
-      <c r="D89" s="3">
+      <c r="D90" s="3">
         <v>0</v>
       </c>
-      <c r="E89" s="5">
+      <c r="E90" s="5">
         <v>1540</v>
       </c>
-      <c r="F89" s="29">
+      <c r="F90" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G89" s="3" t="s">
+      <c r="G90" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H89" s="28"/>
-      <c r="I89" s="3" t="s">
+      <c r="H90" s="28"/>
+      <c r="I90" s="3" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
+    <row r="91" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="B90" s="28" t="s">
+      <c r="B91" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="C90" s="49" t="s">
+      <c r="C91" s="49" t="s">
         <v>380</v>
       </c>
-      <c r="D90" s="3">
-        <v>1</v>
-      </c>
-      <c r="E90" s="5">
+      <c r="D91" s="3">
+        <v>1</v>
+      </c>
+      <c r="E91" s="5">
         <v>1026</v>
       </c>
-      <c r="F90" s="29">
+      <c r="F91" s="29">
         <f t="shared" si="4"/>
         <v>1026</v>
       </c>
-      <c r="G90" s="3" t="s">
+      <c r="G91" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H90" s="28"/>
-      <c r="I90" s="3" t="s">
+      <c r="H91" s="28"/>
+      <c r="I91" s="3" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="91" spans="1:9" s="70" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="70" t="s">
+    <row r="92" spans="1:9" s="70" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="70" t="s">
         <v>502</v>
       </c>
-      <c r="B91" s="28" t="s">
+      <c r="B92" s="28" t="s">
         <v>503</v>
       </c>
-      <c r="C91" s="51" t="s">
+      <c r="C92" s="51" t="s">
         <v>504</v>
       </c>
-      <c r="D91" s="70">
+      <c r="D92" s="70">
         <v>0</v>
       </c>
-      <c r="E91" s="71">
+      <c r="E92" s="71">
         <v>3670</v>
       </c>
-      <c r="F91" s="29">
+      <c r="F92" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G91" s="70" t="s">
+      <c r="G92" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="H91" s="28"/>
-      <c r="I91" s="70" t="s">
+      <c r="H92" s="28"/>
+      <c r="I92" s="70" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="B92" s="28" t="s">
+      <c r="B93" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="C92" s="50" t="s">
+      <c r="C93" s="50" t="s">
         <v>383</v>
       </c>
-      <c r="D92" s="3">
+      <c r="D93" s="3">
         <v>5</v>
       </c>
-      <c r="E92" s="5">
-        <v>1</v>
-      </c>
-      <c r="F92" s="29">
+      <c r="E93" s="5">
+        <v>1</v>
+      </c>
+      <c r="F93" s="29">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="G92" s="3" t="s">
+      <c r="G93" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H92" s="28"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
+      <c r="H93" s="28"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="B93" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C93" s="50" t="s">
+      <c r="B94" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C94" s="50" t="s">
         <v>386</v>
       </c>
-      <c r="D93" s="3">
-        <v>1</v>
-      </c>
-      <c r="E93" s="5">
+      <c r="D94" s="3">
+        <v>1</v>
+      </c>
+      <c r="E94" s="5">
         <v>60</v>
       </c>
-      <c r="F93" s="29">
+      <c r="F94" s="29">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="G93" s="3" t="s">
+      <c r="G94" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H93" s="28"/>
-    </row>
-    <row r="94" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A94" s="25" t="s">
+      <c r="H94" s="28"/>
+    </row>
+    <row r="95" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A95" s="25" t="s">
         <v>415</v>
       </c>
-      <c r="E94" s="27"/>
-      <c r="F94" s="27"/>
-    </row>
-    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="3" t="s">
+      <c r="E95" s="27"/>
+      <c r="F95" s="27"/>
+    </row>
+    <row r="96" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="B95" s="28" t="s">
+      <c r="B96" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="C95" s="51" t="s">
+      <c r="C96" s="51" t="s">
         <v>417</v>
       </c>
-      <c r="D95" s="3">
-        <v>1</v>
-      </c>
-      <c r="E95" s="5">
+      <c r="D96" s="3">
+        <v>1</v>
+      </c>
+      <c r="E96" s="5">
         <v>752</v>
-      </c>
-      <c r="F95" s="5">
-        <f>D95*E95</f>
-        <v>752</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I95" s="3" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="B96" s="28" t="s">
-        <v>268</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="D96" s="3">
-        <v>1</v>
-      </c>
-      <c r="E96" s="5">
-        <v>1</v>
       </c>
       <c r="F96" s="5">
         <f>D96*E96</f>
-        <v>1</v>
+        <v>752</v>
       </c>
       <c r="G96" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="I96" s="3" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B97" s="28" t="s">
-        <v>68</v>
+        <v>268</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D97" s="3">
         <v>1</v>
       </c>
       <c r="E97" s="5">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="F97" s="5">
         <f>D97*E97</f>
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I97" s="3" t="s">
-        <v>426</v>
-      </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="B98" s="28" t="s">
-        <v>268</v>
+        <v>68</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="D98" s="3">
         <v>1</v>
       </c>
       <c r="E98" s="5">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="F98" s="5">
-        <v>1</v>
+        <f>D98*E98</f>
+        <v>36</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="B99" s="28" t="s">
-        <v>68</v>
+        <v>268</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="D99" s="3">
         <v>1</v>
       </c>
       <c r="E99" s="5">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="F99" s="5">
-        <f>D99*E99</f>
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="G99" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B100" s="28" t="s">
         <v>68</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D100" s="3">
         <v>1</v>
       </c>
       <c r="E100" s="5">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="F100" s="5">
         <f>D100*E100</f>
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="G100" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>408</v>
+        <v>427</v>
       </c>
       <c r="B101" s="28" t="s">
         <v>68</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>409</v>
+        <v>428</v>
       </c>
       <c r="D101" s="3">
         <v>1</v>
       </c>
       <c r="E101" s="5">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="F101" s="5">
         <f>D101*E101</f>
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="4" t="s">
-        <v>367</v>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>408</v>
       </c>
       <c r="B102" s="28" t="s">
-        <v>435</v>
+        <v>68</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>384</v>
+        <v>409</v>
+      </c>
+      <c r="D102" s="3">
+        <v>1</v>
+      </c>
+      <c r="E102" s="5">
+        <v>112</v>
       </c>
       <c r="F102" s="5">
         <f>D102*E102</f>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="G102" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I102" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="B103" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="F103" s="5">
+        <f>D103*E103</f>
+        <v>0</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I103" s="3" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="103" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A103" s="6" t="s">
+    <row r="104" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A104" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E103" s="9"/>
-      <c r="F103" s="9"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D104" s="3">
-        <v>1</v>
-      </c>
-      <c r="E104" s="5">
-        <v>3582</v>
-      </c>
-      <c r="F104" s="5">
-        <f t="shared" ref="F104:F116" si="5">E104*D104</f>
-        <v>3582</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I104" s="3" t="s">
-        <v>197</v>
-      </c>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>202</v>
+        <v>64</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C105" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D105" s="3">
+        <v>1</v>
+      </c>
+      <c r="E105" s="5">
+        <v>3582</v>
+      </c>
+      <c r="F105" s="5">
+        <f t="shared" ref="F105:F117" si="5">E105*D105</f>
+        <v>3582</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D105" s="3">
-        <v>1</v>
-      </c>
-      <c r="E105" s="5">
+      <c r="D106" s="3">
+        <v>1</v>
+      </c>
+      <c r="E106" s="5">
         <v>1630</v>
       </c>
-      <c r="F105" s="5">
+      <c r="F106" s="5">
         <f t="shared" si="5"/>
         <v>1630</v>
       </c>
-      <c r="G105" s="3" t="s">
+      <c r="G106" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I105" s="3" t="s">
+      <c r="I106" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="D106" s="3">
-        <v>1</v>
-      </c>
-      <c r="E106" s="5">
+      <c r="D107" s="3">
+        <v>1</v>
+      </c>
+      <c r="E107" s="5">
         <v>886</v>
       </c>
-      <c r="F106" s="5">
+      <c r="F107" s="5">
         <f t="shared" si="5"/>
         <v>886</v>
       </c>
-      <c r="G106" s="3" t="s">
+      <c r="G107" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I106" s="3" t="s">
+      <c r="I107" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B108" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D107" s="3">
-        <v>1</v>
-      </c>
-      <c r="E107" s="5">
+      <c r="D108" s="3">
+        <v>1</v>
+      </c>
+      <c r="E108" s="5">
         <v>163</v>
       </c>
-      <c r="F107" s="5">
+      <c r="F108" s="5">
         <f t="shared" si="5"/>
         <v>163</v>
       </c>
-      <c r="G107" s="3" t="s">
+      <c r="G108" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I107" s="3" t="s">
+      <c r="I108" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B109" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D108" s="3">
-        <v>1</v>
-      </c>
-      <c r="E108" s="5">
+      <c r="D109" s="3">
+        <v>1</v>
+      </c>
+      <c r="E109" s="5">
         <v>11</v>
       </c>
-      <c r="F108" s="5">
+      <c r="F109" s="5">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="G108" s="3" t="s">
+      <c r="G109" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B110" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="C110" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D109" s="3">
-        <v>1</v>
-      </c>
-      <c r="E109" s="5">
+      <c r="D110" s="3">
+        <v>1</v>
+      </c>
+      <c r="E110" s="5">
         <v>520</v>
       </c>
-      <c r="F109" s="5">
+      <c r="F110" s="5">
         <f t="shared" si="5"/>
         <v>520</v>
       </c>
-      <c r="G109" s="3" t="s">
+      <c r="G110" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B111" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="C111" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D110" s="3">
-        <v>1</v>
-      </c>
-      <c r="E110" s="5">
+      <c r="D111" s="3">
+        <v>1</v>
+      </c>
+      <c r="E111" s="5">
         <v>193</v>
       </c>
-      <c r="F110" s="5">
+      <c r="F111" s="5">
         <f t="shared" si="5"/>
         <v>193</v>
       </c>
-      <c r="G110" s="3" t="s">
+      <c r="G111" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="111" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="32" t="s">
+    <row r="112" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="32" t="s">
         <v>334</v>
       </c>
-      <c r="B111" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C111" s="32" t="s">
+      <c r="B112" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C112" s="32" t="s">
         <v>335</v>
       </c>
-      <c r="D111" s="32">
+      <c r="D112" s="32">
         <v>10</v>
       </c>
-      <c r="E111" s="42">
+      <c r="E112" s="42">
         <v>12</v>
       </c>
-      <c r="F111" s="42">
+      <c r="F112" s="42">
         <f t="shared" si="5"/>
         <v>120</v>
       </c>
-      <c r="G111" s="32" t="s">
+      <c r="G112" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="I111" s="32" t="s">
+      <c r="I112" s="32" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="112" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="32" t="s">
+    <row r="113" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="32" t="s">
         <v>336</v>
       </c>
-      <c r="B112" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C112" s="32" t="s">
+      <c r="B113" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C113" s="32" t="s">
         <v>337</v>
       </c>
-      <c r="D112" s="32">
-        <v>1</v>
-      </c>
-      <c r="E112" s="42">
+      <c r="D113" s="32">
+        <v>1</v>
+      </c>
+      <c r="E113" s="42">
         <v>14</v>
       </c>
-      <c r="F112" s="42">
+      <c r="F113" s="42">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="G112" s="32" t="s">
+      <c r="G113" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="I112" s="32" t="s">
+      <c r="I113" s="32" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B113" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C113" s="3" t="s">
+      <c r="B114" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D113" s="3">
+      <c r="D114" s="3">
         <v>4</v>
       </c>
-      <c r="E113" s="5">
+      <c r="E114" s="5">
         <v>15.25</v>
       </c>
-      <c r="F113" s="5">
+      <c r="F114" s="5">
         <f t="shared" si="5"/>
         <v>61</v>
       </c>
-      <c r="G113" s="32" t="s">
+      <c r="G114" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B114" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C114" s="3" t="s">
+      <c r="B115" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D115" s="3">
         <v>10</v>
       </c>
-      <c r="E114" s="5">
+      <c r="E115" s="5">
         <v>16.5</v>
       </c>
-      <c r="F114" s="5">
+      <c r="F115" s="5">
         <f t="shared" si="5"/>
         <v>165</v>
       </c>
-      <c r="G114" s="32" t="s">
+      <c r="G115" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B115" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C115" s="3" t="s">
+      <c r="B116" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C116" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D116" s="3">
         <v>10</v>
       </c>
-      <c r="E115" s="5">
+      <c r="E116" s="5">
         <v>24</v>
       </c>
-      <c r="F115" s="5">
+      <c r="F116" s="5">
         <f t="shared" si="5"/>
         <v>240</v>
       </c>
-      <c r="G115" s="32" t="s">
+      <c r="G116" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B116" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C116" s="3" t="s">
+      <c r="B117" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C117" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D116" s="3">
+      <c r="D117" s="3">
         <v>6</v>
       </c>
-      <c r="E116" s="5">
+      <c r="E117" s="5">
         <v>24</v>
       </c>
-      <c r="F116" s="5">
+      <c r="F117" s="5">
         <f t="shared" si="5"/>
         <v>144</v>
       </c>
-      <c r="G116" s="32" t="s">
+      <c r="G117" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="117" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E117" s="42"/>
-      <c r="F117" s="42"/>
-    </row>
-    <row r="119" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="11"/>
-      <c r="B119" s="11"/>
-      <c r="C119" s="10"/>
-    </row>
-    <row r="120" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A120" s="8" t="s">
+    <row r="118" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E118" s="42"/>
+      <c r="F118" s="42"/>
+    </row>
+    <row r="120" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A120" s="11"/>
+      <c r="B120" s="11"/>
+      <c r="C120" s="10"/>
+    </row>
+    <row r="121" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A121" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="F120" s="9"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D121" s="3">
-        <v>4</v>
-      </c>
-      <c r="E121" s="5">
-        <v>16.5</v>
-      </c>
-      <c r="F121" s="5">
-        <f t="shared" ref="F121:F136" si="6">E121*D121</f>
-        <v>66</v>
-      </c>
-      <c r="I121" s="3" t="s">
-        <v>123</v>
-      </c>
+      <c r="F121" s="9"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D122" s="3">
+        <v>4</v>
+      </c>
+      <c r="E122" s="5">
+        <v>16.5</v>
+      </c>
+      <c r="F122" s="5">
+        <f t="shared" ref="F122:F137" si="6">E122*D122</f>
+        <v>66</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B122" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C122" s="3" t="s">
+      <c r="B123" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C123" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D122" s="3">
-        <v>1</v>
-      </c>
-      <c r="E122" s="5">
+      <c r="D123" s="3">
+        <v>1</v>
+      </c>
+      <c r="E123" s="5">
         <v>85.1</v>
       </c>
-      <c r="F122" s="5">
+      <c r="F123" s="5">
         <f t="shared" si="6"/>
         <v>85.1</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B123" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C123" s="3" t="s">
+      <c r="B124" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C124" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D123" s="3">
+      <c r="D124" s="3">
         <v>2</v>
       </c>
-      <c r="E123" s="5">
+      <c r="E124" s="5">
         <v>32</v>
       </c>
-      <c r="F123" s="5">
+      <c r="F124" s="5">
         <f t="shared" si="6"/>
         <v>64</v>
       </c>
-      <c r="I123" s="3" t="s">
+      <c r="I124" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B124" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C124" s="3" t="s">
+      <c r="B125" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D124" s="3">
+      <c r="D125" s="3">
         <v>2</v>
       </c>
-      <c r="E124" s="5">
+      <c r="E125" s="5">
         <v>51.58</v>
       </c>
-      <c r="F124" s="5">
+      <c r="F125" s="5">
         <f t="shared" si="6"/>
         <v>103.16</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="3" t="s">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B125" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C125" s="3" t="s">
+      <c r="B126" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C126" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D125" s="3">
-        <v>1</v>
-      </c>
-      <c r="E125" s="5">
+      <c r="D126" s="3">
+        <v>1</v>
+      </c>
+      <c r="E126" s="5">
         <v>60</v>
       </c>
-      <c r="F125" s="5">
+      <c r="F126" s="5">
         <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="I125" s="3" t="s">
+      <c r="I126" s="3" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D126" s="3">
-        <v>1</v>
-      </c>
-      <c r="E126" s="5">
-        <v>136.47999999999999</v>
-      </c>
-      <c r="F126" s="5">
-        <f t="shared" si="6"/>
-        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -5171,7 +5189,7 @@
         <v>68</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D127" s="3">
         <v>1</v>
@@ -5186,278 +5204,278 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D128" s="3">
         <v>1</v>
       </c>
       <c r="E128" s="5">
-        <v>60.95</v>
+        <v>136.47999999999999</v>
       </c>
       <c r="F128" s="5">
         <f t="shared" si="6"/>
-        <v>60.95</v>
+        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D129" s="3">
         <v>1</v>
       </c>
       <c r="E129" s="5">
-        <v>119.416</v>
+        <v>60.95</v>
       </c>
       <c r="F129" s="5">
         <f t="shared" si="6"/>
-        <v>119.416</v>
+        <v>60.95</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D130" s="3">
         <v>1</v>
       </c>
       <c r="E130" s="5">
-        <v>105.8</v>
+        <v>119.416</v>
       </c>
       <c r="F130" s="5">
         <f t="shared" si="6"/>
-        <v>105.8</v>
+        <v>119.416</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D131" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E131" s="5">
-        <v>119.6</v>
+        <v>105.8</v>
       </c>
       <c r="F131" s="5">
         <f t="shared" si="6"/>
-        <v>239.2</v>
+        <v>105.8</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>345</v>
+        <v>153</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>346</v>
+        <v>154</v>
       </c>
       <c r="D132" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E132" s="5">
-        <v>100</v>
+        <v>119.6</v>
       </c>
       <c r="F132" s="5">
         <f t="shared" si="6"/>
-        <v>100</v>
+        <v>239.2</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>155</v>
+        <v>345</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>156</v>
+        <v>346</v>
       </c>
       <c r="D133" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E133" s="5">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F133" s="5">
         <f t="shared" si="6"/>
-        <v>184</v>
+        <v>100</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D134" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E134" s="5">
-        <v>96.23</v>
+        <v>92</v>
       </c>
       <c r="F134" s="5">
         <f t="shared" si="6"/>
-        <v>96.23</v>
+        <v>184</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D135" s="3">
         <v>1</v>
       </c>
       <c r="E135" s="5">
-        <v>102.44</v>
+        <v>96.23</v>
       </c>
       <c r="F135" s="5">
         <f t="shared" si="6"/>
-        <v>102.44</v>
+        <v>96.23</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D136" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E136" s="5">
-        <v>28</v>
+        <v>102.44</v>
       </c>
       <c r="F136" s="5">
         <f t="shared" si="6"/>
+        <v>102.44</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D137" s="3">
+        <v>2</v>
+      </c>
+      <c r="E137" s="5">
+        <v>28</v>
+      </c>
+      <c r="F137" s="5">
+        <f t="shared" si="6"/>
         <v>56</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C137" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D137" s="3">
-        <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C138" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D138" s="3">
-        <v>1</v>
-      </c>
-      <c r="I138" s="3" t="s">
-        <v>165</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C139" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D139" s="3">
+        <v>1</v>
+      </c>
+      <c r="I139" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C140" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D139" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A141" s="8" t="s">
+      <c r="D140" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A142" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B141" s="7" t="s">
+      <c r="B142" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="E141" s="9"/>
-      <c r="F141" s="9"/>
-    </row>
-    <row r="142" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="70"/>
-      <c r="B142" s="70" t="s">
+      <c r="E142" s="9"/>
+      <c r="F142" s="9"/>
+    </row>
+    <row r="143" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="70"/>
+      <c r="B143" s="70" t="s">
         <v>167</v>
       </c>
-      <c r="C142" s="72" t="s">
+      <c r="C143" s="72" t="s">
         <v>172</v>
       </c>
-      <c r="D142" s="70">
+      <c r="D143" s="70">
         <v>4</v>
       </c>
-      <c r="E142" s="70">
+      <c r="E143" s="70">
         <v>40</v>
       </c>
-      <c r="F142" s="70">
-        <f>E142*D142</f>
+      <c r="F143" s="70">
+        <f>E143*D143</f>
         <v>160</v>
       </c>
-      <c r="G142" s="70" t="s">
+      <c r="G143" s="70" t="s">
         <v>478</v>
       </c>
-      <c r="H142" s="70"/>
-      <c r="I142" s="70" t="s">
+      <c r="H143" s="70"/>
+      <c r="I143" s="70" t="s">
         <v>173</v>
       </c>
-      <c r="J142" s="72" t="s">
+      <c r="J143" s="72" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="70" t="s">
-        <v>175</v>
-      </c>
-      <c r="C143" s="70" t="s">
-        <v>413</v>
-      </c>
-      <c r="D143" s="70">
-        <v>2</v>
-      </c>
-      <c r="E143" s="71">
-        <v>331</v>
-      </c>
-      <c r="F143" s="71">
-        <f>E143*D143</f>
-        <v>662</v>
-      </c>
-      <c r="G143" s="70" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="144" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.25">
@@ -5465,17 +5483,17 @@
         <v>175</v>
       </c>
       <c r="C144" s="70" t="s">
-        <v>330</v>
+        <v>413</v>
       </c>
       <c r="D144" s="70">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E144" s="71">
-        <v>25</v>
+        <v>331</v>
       </c>
       <c r="F144" s="71">
         <f>E144*D144</f>
-        <v>100</v>
+        <v>662</v>
       </c>
       <c r="G144" s="70" t="s">
         <v>477</v>
@@ -5486,17 +5504,17 @@
         <v>175</v>
       </c>
       <c r="C145" s="70" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D145" s="70">
         <v>4</v>
       </c>
       <c r="E145" s="71">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F145" s="71">
         <f>E145*D145</f>
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G145" s="70" t="s">
         <v>477</v>
@@ -5507,41 +5525,62 @@
         <v>175</v>
       </c>
       <c r="C146" s="70" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D146" s="70">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E146" s="71">
-        <v>121.5</v>
+        <v>28</v>
       </c>
       <c r="F146" s="71">
         <f>E146*D146</f>
-        <v>729</v>
+        <v>112</v>
       </c>
       <c r="G146" s="70" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="149" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E149" s="20" t="s">
+    <row r="147" spans="2:7" s="70" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="C147" s="70" t="s">
+        <v>332</v>
+      </c>
+      <c r="D147" s="70">
+        <v>6</v>
+      </c>
+      <c r="E147" s="71">
+        <v>121.5</v>
+      </c>
+      <c r="F147" s="71">
+        <f>E147*D147</f>
+        <v>729</v>
+      </c>
+      <c r="G147" s="70" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="150" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E150" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="F149" s="5">
-        <f>SUM(F3:F147)</f>
-        <v>84327.255999999994</v>
+      <c r="F150" s="5">
+        <f>SUM(F3:F148)</f>
+        <v>84743.255999999994</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C87" r:id="rId1" display="Mitutoyo Plan Apo Brightfield and Darkfield, 2X" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C88" r:id="rId2" display="Plan Apo" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C89" r:id="rId3" display="Plan Apo" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C90" r:id="rId4" display="Plan Apo Brightfield and Darkfield " xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C95" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C78" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C91" r:id="rId7" xr:uid="{3002EF90-377A-4FAD-A836-B22D0D243A96}"/>
+    <hyperlink ref="C88" r:id="rId1" display="Mitutoyo Plan Apo Brightfield and Darkfield, 2X" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C89" r:id="rId2" display="Plan Apo" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C90" r:id="rId3" display="Plan Apo" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C91" r:id="rId4" display="Plan Apo Brightfield and Darkfield " xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C96" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C79" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C92" r:id="rId7" xr:uid="{3002EF90-377A-4FAD-A836-B22D0D243A96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>

</xml_diff>

<commit_message>
GPS011 price and part number
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDD223E-8A13-4AC6-847E-45E7CF3139D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CE05DE-6B8B-4481-8653-4ADF58A10A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -797,9 +797,6 @@
     <t>Adapter with External SM2 Threads and Nikon Female F-Mount Ring</t>
   </si>
   <si>
-    <t>1D or 2D Galvo System Linear Power Supply, 230 VAC</t>
-  </si>
-  <si>
     <t>3D printed</t>
   </si>
   <si>
@@ -1092,9 +1089,6 @@
   </si>
   <si>
     <t>TODO: find specific model</t>
-  </si>
-  <si>
-    <t>GPS011 (obsolete)</t>
   </si>
   <si>
     <t>GPWR15 (unsafe)</t>
@@ -1647,6 +1641,12 @@
   </si>
   <si>
     <t>mirror-bracket.ipt</t>
+  </si>
+  <si>
+    <t>1D or 2D Galvo System Linear Power Supply, 110 or 230 VAC (EU or US option)</t>
+  </si>
+  <si>
+    <t>GPS011-EU/US</t>
   </si>
 </sst>
 </file>
@@ -1748,12 +1748,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1831,6 +1825,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1973,49 +1974,49 @@
     <xf numFmtId="2" fontId="5" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="14" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="15" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="4" applyFont="1"/>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Excel Built-in Heading 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2405,8 +2406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2482,7 +2483,7 @@
         <v>12350</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>182</v>
@@ -2547,7 +2548,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
@@ -2560,10 +2561,10 @@
         <v>6500</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -2587,10 +2588,10 @@
         <v>2250</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I11" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -2614,7 +2615,7 @@
         <v>160</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H12" s="32" t="s">
         <v>13</v>
@@ -2622,13 +2623,13 @@
     </row>
     <row r="13" spans="1:9" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D13" s="32">
         <v>1</v>
@@ -2641,10 +2642,10 @@
         <v>250</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I13" s="32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -2668,13 +2669,13 @@
         <v>2250</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H14" s="32" t="s">
         <v>13</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -2698,10 +2699,10 @@
         <v>230</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -2725,21 +2726,21 @@
         <v>2425</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I16" s="32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B17" s="32" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D17" s="32">
         <v>1</v>
@@ -2751,11 +2752,11 @@
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="G17" s="67" t="s">
-        <v>265</v>
+      <c r="G17" s="66" t="s">
+        <v>264</v>
       </c>
       <c r="I17" s="32" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2779,10 +2780,10 @@
         <v>150</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2806,10 +2807,10 @@
         <v>3000</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2833,10 +2834,10 @@
         <v>5800</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2860,28 +2861,28 @@
         <v>1100</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>280</v>
       </c>
       <c r="D23" s="3">
         <v>2</v>
@@ -2894,21 +2895,21 @@
         <v>140</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>283</v>
       </c>
       <c r="D24" s="3">
         <v>6</v>
@@ -2921,21 +2922,21 @@
         <v>216</v>
       </c>
       <c r="G24" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>287</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
@@ -2948,21 +2949,21 @@
         <v>43</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
+        <v>288</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>290</v>
       </c>
       <c r="D26" s="3">
         <v>1</v>
@@ -2975,21 +2976,21 @@
         <v>29</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
+        <v>291</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="C27" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>294</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
@@ -3002,21 +3003,21 @@
         <v>195</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
@@ -3029,7 +3030,7 @@
         <v>10</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="15" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3041,7 +3042,7 @@
     </row>
     <row r="30" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
@@ -3054,7 +3055,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F31" s="5">
         <v>0</v>
@@ -3207,7 +3208,7 @@
     </row>
     <row r="39" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="33" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B39" s="32" t="s">
         <v>65</v>
@@ -3234,7 +3235,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>201</v>
@@ -3266,7 +3267,7 @@
         <v>91863</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>50</v>
@@ -3293,13 +3294,13 @@
     </row>
     <row r="42" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D42" s="3">
         <v>2</v>
@@ -3318,79 +3319,79 @@
         <v>249</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="75" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="74" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="74" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="73" t="s">
         <v>251</v>
       </c>
-      <c r="B43" s="75" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="76" t="s">
+      <c r="B43" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="75" t="s">
         <v>252</v>
       </c>
-      <c r="D43" s="75">
+      <c r="D43" s="74">
         <v>0</v>
       </c>
-      <c r="E43" s="77">
+      <c r="E43" s="76">
         <v>40</v>
       </c>
-      <c r="F43" s="78">
+      <c r="F43" s="77">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G43" s="79" t="s">
+      <c r="G43" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="H43" s="75" t="s">
+      <c r="H43" s="74" t="s">
         <v>249</v>
       </c>
-      <c r="I43" s="80" t="s">
-        <v>493</v>
-      </c>
-      <c r="J43" s="81"/>
-    </row>
-    <row r="44" spans="1:10" s="75" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="76" t="s">
+      <c r="I43" s="79" t="s">
+        <v>491</v>
+      </c>
+      <c r="J43" s="80"/>
+    </row>
+    <row r="44" spans="1:10" s="74" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="75" t="s">
         <v>250</v>
       </c>
-      <c r="B44" s="75" t="s">
-        <v>65</v>
-      </c>
-      <c r="C44" s="76" t="s">
+      <c r="B44" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="75" t="s">
         <v>253</v>
       </c>
-      <c r="D44" s="75">
+      <c r="D44" s="74">
         <v>0</v>
       </c>
-      <c r="E44" s="77">
+      <c r="E44" s="76">
         <v>92</v>
       </c>
-      <c r="F44" s="78">
+      <c r="F44" s="77">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G44" s="79" t="s">
+      <c r="G44" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="H44" s="75" t="s">
+      <c r="H44" s="74" t="s">
         <v>249</v>
       </c>
-      <c r="I44" s="80" t="s">
-        <v>492</v>
+      <c r="I44" s="79" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="33" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D45" s="32">
         <v>2</v>
@@ -3409,7 +3410,7 @@
         <v>249</v>
       </c>
       <c r="I45" s="32" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3540,7 +3541,7 @@
         <v>65</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D50" s="32">
         <v>4</v>
@@ -3552,14 +3553,14 @@
         <f t="shared" si="3"/>
         <v>416</v>
       </c>
-      <c r="G50" s="67" t="s">
+      <c r="G50" s="66" t="s">
         <v>41</v>
       </c>
       <c r="H50" s="32" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="I50" s="32" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -3589,7 +3590,7 @@
         <v>219</v>
       </c>
       <c r="I51" s="36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -3619,7 +3620,7 @@
         <v>219</v>
       </c>
       <c r="I52" s="36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3858,13 +3859,13 @@
     </row>
     <row r="61" spans="1:9" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="35" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B61" s="38" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C61" s="35" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D61" s="36">
         <v>2</v>
@@ -3883,7 +3884,7 @@
         <v>244</v>
       </c>
       <c r="I61" s="36" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -3918,13 +3919,13 @@
     </row>
     <row r="63" spans="1:9" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="45" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B63" s="38" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C63" s="33" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D63" s="32">
         <v>2</v>
@@ -3936,55 +3937,55 @@
         <f t="shared" ref="F63" si="4">E63*D63</f>
         <v>600</v>
       </c>
-      <c r="G63" s="67" t="s">
+      <c r="G63" s="66" t="s">
         <v>41</v>
       </c>
       <c r="H63" s="32" t="s">
         <v>246</v>
       </c>
       <c r="I63" s="38" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="74" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="33" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" s="75" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="33" t="s">
-        <v>498</v>
-      </c>
-      <c r="B64" s="75" t="s">
-        <v>65</v>
-      </c>
-      <c r="C64" s="76" t="s">
-        <v>486</v>
-      </c>
-      <c r="D64" s="75">
+      <c r="B64" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" s="75" t="s">
+        <v>484</v>
+      </c>
+      <c r="D64" s="74">
         <v>0</v>
       </c>
-      <c r="E64" s="77">
+      <c r="E64" s="76">
         <v>36</v>
       </c>
-      <c r="F64" s="78">
+      <c r="F64" s="77">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G64" s="79" t="s">
+      <c r="G64" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="H64" s="75" t="s">
+      <c r="H64" s="74" t="s">
         <v>246</v>
       </c>
-      <c r="I64" s="75" t="s">
-        <v>497</v>
+      <c r="I64" s="74" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="33" t="s">
+        <v>306</v>
+      </c>
+      <c r="B65" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C65" s="33" t="s">
         <v>307</v>
-      </c>
-      <c r="B65" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C65" s="33" t="s">
-        <v>308</v>
       </c>
       <c r="D65" s="32">
         <v>2</v>
@@ -4003,18 +4004,18 @@
         <v>246</v>
       </c>
       <c r="I65" s="32" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="33" t="s">
+        <v>308</v>
+      </c>
+      <c r="B66" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C66" s="33" t="s">
         <v>309</v>
-      </c>
-      <c r="B66" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C66" s="33" t="s">
-        <v>310</v>
       </c>
       <c r="D66" s="32">
         <v>2</v>
@@ -4034,24 +4035,24 @@
       </c>
     </row>
     <row r="67" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="46" t="s">
-        <v>341</v>
+      <c r="A67" s="44" t="s">
+        <v>518</v>
       </c>
       <c r="B67" s="32" t="s">
         <v>65</v>
       </c>
       <c r="C67" s="33" t="s">
-        <v>254</v>
+        <v>517</v>
       </c>
       <c r="D67" s="32">
         <v>1</v>
       </c>
       <c r="E67" s="34">
-        <v>495</v>
+        <v>520</v>
       </c>
       <c r="F67" s="41">
         <f t="shared" si="3"/>
-        <v>495</v>
+        <v>520</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>41</v>
@@ -4060,48 +4061,48 @@
         <v>246</v>
       </c>
       <c r="I67" s="32" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="46" t="s">
-        <v>342</v>
-      </c>
-      <c r="B68" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C68" s="33" t="s">
-        <v>311</v>
-      </c>
-      <c r="D68" s="32">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="74" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="86" t="s">
+        <v>340</v>
+      </c>
+      <c r="B68" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" s="75" t="s">
+        <v>310</v>
+      </c>
+      <c r="D68" s="74">
         <v>0</v>
       </c>
-      <c r="E68" s="34">
+      <c r="E68" s="76">
         <v>390</v>
       </c>
-      <c r="F68" s="41">
+      <c r="F68" s="77">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G68" s="3" t="s">
+      <c r="G68" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="H68" s="32" t="s">
+      <c r="H68" s="74" t="s">
         <v>246</v>
       </c>
-      <c r="I68" s="32" t="s">
-        <v>334</v>
+      <c r="I68" s="74" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="45" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B69" s="38" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D69" s="32">
         <v>14</v>
@@ -4120,18 +4121,18 @@
         <v>246</v>
       </c>
       <c r="I69" s="38" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="45" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C70" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D70" s="32">
         <v>1</v>
@@ -4150,7 +4151,7 @@
         <v>246</v>
       </c>
       <c r="I70" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -4173,7 +4174,7 @@
     </row>
     <row r="74" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E74" s="9"/>
       <c r="F74" s="9"/>
@@ -4194,18 +4195,18 @@
       <c r="E75" s="34"/>
       <c r="F75" s="41"/>
       <c r="I75" s="32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="B76" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C76" s="33" t="s">
         <v>271</v>
-      </c>
-      <c r="B76" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C76" s="33" t="s">
-        <v>272</v>
       </c>
       <c r="D76" s="32">
         <v>1</v>
@@ -4220,13 +4221,13 @@
     </row>
     <row r="77" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
+        <v>275</v>
+      </c>
+      <c r="B77" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C77" s="33" t="s">
         <v>276</v>
-      </c>
-      <c r="B77" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C77" s="33" t="s">
-        <v>277</v>
       </c>
       <c r="D77" s="32">
         <v>2</v>
@@ -4255,32 +4256,32 @@
       <c r="E78" s="34"/>
       <c r="F78" s="41"/>
       <c r="I78" s="32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
     </row>
     <row r="80" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
     </row>
     <row r="81" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="C81" s="48" t="s">
-        <v>457</v>
+        <v>458</v>
+      </c>
+      <c r="C81" s="47" t="s">
+        <v>455</v>
       </c>
       <c r="D81" s="3">
         <v>1</v>
@@ -4293,19 +4294,19 @@
         <v>200</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="J81" s="4"/>
     </row>
     <row r="82" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D82" s="3">
         <v>5</v>
@@ -4313,24 +4314,24 @@
       <c r="E82" s="5">
         <v>1</v>
       </c>
-      <c r="F82" s="68">
+      <c r="F82" s="67">
         <f>E82*D82</f>
         <v>5</v>
       </c>
       <c r="I82" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="J82" s="4"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="66" t="s">
         <v>463</v>
       </c>
-      <c r="J82" s="4"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="67" t="s">
-        <v>465</v>
-      </c>
       <c r="B83" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D83" s="3">
         <v>1</v>
@@ -4338,23 +4339,23 @@
       <c r="E83" s="5">
         <v>26</v>
       </c>
-      <c r="F83" s="68">
+      <c r="F83" s="67">
         <f>E83*D83</f>
         <v>26</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D84" s="3">
         <v>1</v>
@@ -4362,38 +4363,38 @@
       <c r="E84" s="5">
         <v>37</v>
       </c>
-      <c r="F84" s="68">
+      <c r="F84" s="67">
         <f>E84*D84</f>
         <v>37</v>
       </c>
       <c r="I84" s="32"/>
     </row>
-    <row r="85" spans="1:10" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="67" t="s">
-        <v>386</v>
-      </c>
-      <c r="B85" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="C85" s="67" t="s">
-        <v>385</v>
-      </c>
-      <c r="D85" s="67">
+    <row r="85" spans="1:10" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="66" t="s">
+        <v>384</v>
+      </c>
+      <c r="B85" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="C85" s="66" t="s">
+        <v>383</v>
+      </c>
+      <c r="D85" s="66">
         <v>2</v>
       </c>
-      <c r="E85" s="68">
+      <c r="E85" s="67">
         <v>24</v>
       </c>
-      <c r="F85" s="68">
+      <c r="F85" s="67">
         <f>E85*D85</f>
         <v>48</v>
       </c>
       <c r="I85" s="32" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="86" spans="1:10" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="72" t="s">
+      <c r="A86" s="71" t="s">
         <v>172</v>
       </c>
       <c r="F86" s="43"/>
@@ -4406,13 +4407,13 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D88" s="3">
         <v>1</v>
@@ -4433,20 +4434,20 @@
     </row>
     <row r="89" spans="1:10" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A89" s="25" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E89" s="27"/>
       <c r="F89" s="27"/>
     </row>
     <row r="90" spans="1:10" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="30" t="s">
+        <v>354</v>
+      </c>
+      <c r="B90" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="C90" s="83" t="s">
         <v>356</v>
-      </c>
-      <c r="B90" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="C90" s="84" t="s">
-        <v>358</v>
       </c>
       <c r="D90" s="28">
         <v>1</v>
@@ -4462,18 +4463,18 @@
         <v>13</v>
       </c>
       <c r="I90" s="28" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="B91" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="C91" s="84" t="s">
         <v>357</v>
-      </c>
-      <c r="B91" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="C91" s="85" t="s">
-        <v>359</v>
       </c>
       <c r="D91" s="3">
         <v>1</v>
@@ -4490,18 +4491,18 @@
       </c>
       <c r="H91" s="28"/>
       <c r="I91" s="3" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="31" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="C92" s="85" t="s">
-        <v>360</v>
+        <v>353</v>
+      </c>
+      <c r="C92" s="84" t="s">
+        <v>358</v>
       </c>
       <c r="D92" s="3">
         <v>0</v>
@@ -4518,18 +4519,18 @@
       </c>
       <c r="H92" s="28"/>
       <c r="I92" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B93" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="C93" s="85" t="s">
-        <v>362</v>
+        <v>353</v>
+      </c>
+      <c r="C93" s="84" t="s">
+        <v>360</v>
       </c>
       <c r="D93" s="3">
         <v>1</v>
@@ -4546,46 +4547,46 @@
       </c>
       <c r="H93" s="28"/>
       <c r="I93" s="3" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" s="67" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="67" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" s="66" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="66" t="s">
+        <v>472</v>
+      </c>
+      <c r="B94" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="C94" s="85" t="s">
         <v>474</v>
       </c>
-      <c r="B94" s="28" t="s">
-        <v>475</v>
-      </c>
-      <c r="C94" s="86" t="s">
-        <v>476</v>
-      </c>
-      <c r="D94" s="67">
+      <c r="D94" s="66">
         <v>0</v>
       </c>
-      <c r="E94" s="68">
+      <c r="E94" s="67">
         <v>3670</v>
       </c>
       <c r="F94" s="29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G94" s="67" t="s">
+      <c r="G94" s="66" t="s">
         <v>13</v>
       </c>
       <c r="H94" s="28"/>
-      <c r="I94" s="67" t="s">
-        <v>477</v>
+      <c r="I94" s="66" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B95" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="C95" s="47" t="s">
-        <v>365</v>
+        <v>254</v>
+      </c>
+      <c r="C95" s="46" t="s">
+        <v>363</v>
       </c>
       <c r="D95" s="3">
         <v>5</v>
@@ -4604,13 +4605,13 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B96" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C96" s="47" t="s">
-        <v>367</v>
+      <c r="C96" s="46" t="s">
+        <v>365</v>
       </c>
       <c r="D96" s="3">
         <v>1</v>
@@ -4629,20 +4630,20 @@
     </row>
     <row r="97" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A97" s="25" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E97" s="27"/>
       <c r="F97" s="27"/>
     </row>
     <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B98" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="C98" s="83" t="s">
-        <v>398</v>
+        <v>353</v>
+      </c>
+      <c r="C98" s="82" t="s">
+        <v>396</v>
       </c>
       <c r="D98" s="3">
         <v>1</v>
@@ -4651,25 +4652,25 @@
         <v>752</v>
       </c>
       <c r="F98" s="5">
-        <f>D98*E98</f>
+        <f t="shared" ref="F98:F103" si="6">D98*E98</f>
         <v>752</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B99" s="28" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D99" s="3">
         <v>1</v>
@@ -4678,7 +4679,7 @@
         <v>1</v>
       </c>
       <c r="F99" s="5">
-        <f>D99*E99</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G99" s="3" t="s">
@@ -4687,13 +4688,13 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B100" s="28" t="s">
         <v>65</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D100" s="3">
         <v>1</v>
@@ -4702,25 +4703,25 @@
         <v>36</v>
       </c>
       <c r="F100" s="5">
-        <f>D100*E100</f>
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
       <c r="G100" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B101" s="28" t="s">
         <v>65</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D101" s="3">
         <v>1</v>
@@ -4729,25 +4730,25 @@
         <v>65</v>
       </c>
       <c r="F101" s="5">
-        <f>D101*E101</f>
+        <f t="shared" si="6"/>
         <v>65</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B102" s="28" t="s">
         <v>65</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D102" s="3">
         <v>1</v>
@@ -4756,25 +4757,25 @@
         <v>32</v>
       </c>
       <c r="F102" s="5">
-        <f>D102*E102</f>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="G102" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B103" s="28" t="s">
         <v>65</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D103" s="3">
         <v>1</v>
@@ -4783,14 +4784,14 @@
         <v>112</v>
       </c>
       <c r="F103" s="5">
-        <f>D103*E103</f>
+        <f t="shared" si="6"/>
         <v>112</v>
       </c>
       <c r="G103" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4817,7 +4818,7 @@
         <v>3582</v>
       </c>
       <c r="F105" s="5">
-        <f t="shared" ref="F105:F117" si="6">E105*D105</f>
+        <f t="shared" ref="F105:F117" si="7">E105*D105</f>
         <v>3582</v>
       </c>
       <c r="G105" s="3" t="s">
@@ -4844,7 +4845,7 @@
         <v>1630</v>
       </c>
       <c r="F106" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1630</v>
       </c>
       <c r="G106" s="3" t="s">
@@ -4871,7 +4872,7 @@
         <v>886</v>
       </c>
       <c r="F107" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>886</v>
       </c>
       <c r="G107" s="3" t="s">
@@ -4898,7 +4899,7 @@
         <v>163</v>
       </c>
       <c r="F108" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>163</v>
       </c>
       <c r="G108" s="3" t="s">
@@ -4925,7 +4926,7 @@
         <v>11</v>
       </c>
       <c r="F109" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="G109" s="3" t="s">
@@ -4949,7 +4950,7 @@
         <v>520</v>
       </c>
       <c r="F110" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>520</v>
       </c>
       <c r="G110" s="3" t="s">
@@ -4973,7 +4974,7 @@
         <v>193</v>
       </c>
       <c r="F111" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>193</v>
       </c>
       <c r="G111" s="3" t="s">
@@ -4982,13 +4983,13 @@
     </row>
     <row r="112" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="32" t="s">
+        <v>319</v>
+      </c>
+      <c r="B112" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C112" s="32" t="s">
         <v>320</v>
-      </c>
-      <c r="B112" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C112" s="32" t="s">
-        <v>321</v>
       </c>
       <c r="D112" s="32">
         <v>10</v>
@@ -4997,25 +4998,25 @@
         <v>12</v>
       </c>
       <c r="F112" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>120</v>
       </c>
       <c r="G112" s="32" t="s">
         <v>55</v>
       </c>
       <c r="I112" s="32" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="113" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="B113" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C113" s="32" t="s">
         <v>322</v>
-      </c>
-      <c r="B113" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C113" s="32" t="s">
-        <v>323</v>
       </c>
       <c r="D113" s="32">
         <v>1</v>
@@ -5024,14 +5025,14 @@
         <v>14</v>
       </c>
       <c r="F113" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
       <c r="G113" s="32" t="s">
         <v>55</v>
       </c>
       <c r="I113" s="32" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -5051,7 +5052,7 @@
         <v>15.25</v>
       </c>
       <c r="F114" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>61</v>
       </c>
       <c r="G114" s="32" t="s">
@@ -5075,7 +5076,7 @@
         <v>16.5</v>
       </c>
       <c r="F115" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>165</v>
       </c>
       <c r="G115" s="32" t="s">
@@ -5099,7 +5100,7 @@
         <v>24</v>
       </c>
       <c r="F116" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="G116" s="32" t="s">
@@ -5123,7 +5124,7 @@
         <v>24</v>
       </c>
       <c r="F117" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>144</v>
       </c>
       <c r="G117" s="32" t="s">
@@ -5162,7 +5163,7 @@
         <v>16.5</v>
       </c>
       <c r="F122" s="5">
-        <f t="shared" ref="F122:F137" si="7">E122*D122</f>
+        <f t="shared" ref="F122:F137" si="8">E122*D122</f>
         <v>66</v>
       </c>
       <c r="I122" s="3" t="s">
@@ -5186,7 +5187,7 @@
         <v>85.1</v>
       </c>
       <c r="F123" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>85.1</v>
       </c>
     </row>
@@ -5207,7 +5208,7 @@
         <v>32</v>
       </c>
       <c r="F124" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>64</v>
       </c>
       <c r="I124" s="3" t="s">
@@ -5231,7 +5232,7 @@
         <v>51.58</v>
       </c>
       <c r="F125" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>103.16</v>
       </c>
     </row>
@@ -5252,7 +5253,7 @@
         <v>60</v>
       </c>
       <c r="F126" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>60</v>
       </c>
       <c r="I126" s="3" t="s">
@@ -5276,7 +5277,7 @@
         <v>136.47999999999999</v>
       </c>
       <c r="F127" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>136.47999999999999</v>
       </c>
     </row>
@@ -5297,7 +5298,7 @@
         <v>136.47999999999999</v>
       </c>
       <c r="F128" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>136.47999999999999</v>
       </c>
     </row>
@@ -5318,7 +5319,7 @@
         <v>60.95</v>
       </c>
       <c r="F129" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>60.95</v>
       </c>
     </row>
@@ -5339,7 +5340,7 @@
         <v>119.416</v>
       </c>
       <c r="F130" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>119.416</v>
       </c>
     </row>
@@ -5360,7 +5361,7 @@
         <v>105.8</v>
       </c>
       <c r="F131" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>105.8</v>
       </c>
     </row>
@@ -5381,19 +5382,19 @@
         <v>119.6</v>
       </c>
       <c r="F132" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>239.2</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C133" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>331</v>
       </c>
       <c r="D133" s="3">
         <v>1</v>
@@ -5402,7 +5403,7 @@
         <v>100</v>
       </c>
       <c r="F133" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
     </row>
@@ -5423,7 +5424,7 @@
         <v>92</v>
       </c>
       <c r="F134" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>184</v>
       </c>
     </row>
@@ -5444,7 +5445,7 @@
         <v>96.23</v>
       </c>
       <c r="F135" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>96.23</v>
       </c>
     </row>
@@ -5465,7 +5466,7 @@
         <v>102.44</v>
       </c>
       <c r="F136" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>102.44</v>
       </c>
     </row>
@@ -5486,7 +5487,7 @@
         <v>28</v>
       </c>
       <c r="F137" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>56</v>
       </c>
     </row>
@@ -5522,202 +5523,202 @@
         <v>165</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E142" s="9"/>
       <c r="F142" s="9"/>
     </row>
-    <row r="143" spans="1:10" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="67"/>
-      <c r="B143" s="67" t="s">
-        <v>503</v>
-      </c>
-      <c r="C143" s="69" t="s">
+    <row r="143" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="66"/>
+      <c r="B143" s="66" t="s">
+        <v>501</v>
+      </c>
+      <c r="C143" s="68" t="s">
         <v>164</v>
       </c>
-      <c r="D143" s="67">
+      <c r="D143" s="66">
         <v>4</v>
       </c>
-      <c r="E143" s="67">
+      <c r="E143" s="66">
         <v>40</v>
       </c>
-      <c r="F143" s="67">
+      <c r="F143" s="66">
         <f>E143*D143</f>
         <v>160</v>
       </c>
-      <c r="G143" s="67" t="s">
-        <v>501</v>
-      </c>
-      <c r="H143" s="67" t="s">
-        <v>502</v>
-      </c>
-      <c r="I143" s="67" t="s">
+      <c r="G143" s="66" t="s">
+        <v>499</v>
+      </c>
+      <c r="H143" s="66" t="s">
         <v>500</v>
       </c>
-      <c r="J143" s="69"/>
-    </row>
-    <row r="144" spans="1:10" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="67" t="s">
+      <c r="I143" s="66" t="s">
+        <v>498</v>
+      </c>
+      <c r="J143" s="68"/>
+    </row>
+    <row r="144" spans="1:10" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="C144" s="67" t="s">
-        <v>394</v>
-      </c>
-      <c r="D144" s="67">
+      <c r="C144" s="66" t="s">
+        <v>392</v>
+      </c>
+      <c r="D144" s="66">
         <v>2</v>
       </c>
-      <c r="E144" s="68">
+      <c r="E144" s="67">
         <v>331</v>
       </c>
-      <c r="F144" s="68">
+      <c r="F144" s="67">
         <f>E144*D144</f>
         <v>662</v>
       </c>
-      <c r="G144" s="67" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="67" t="s">
+      <c r="G144" s="66" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B145" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="C145" s="67" t="s">
-        <v>316</v>
-      </c>
-      <c r="D145" s="67">
+      <c r="C145" s="66" t="s">
+        <v>315</v>
+      </c>
+      <c r="D145" s="66">
         <v>4</v>
       </c>
-      <c r="E145" s="68">
+      <c r="E145" s="67">
         <v>25</v>
       </c>
-      <c r="F145" s="68">
+      <c r="F145" s="67">
         <f>E145*D145</f>
         <v>100</v>
       </c>
-      <c r="G145" s="67" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="67" t="s">
+      <c r="G145" s="66" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B146" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="C146" s="67" t="s">
-        <v>317</v>
-      </c>
-      <c r="D146" s="67">
+      <c r="C146" s="66" t="s">
+        <v>316</v>
+      </c>
+      <c r="D146" s="66">
         <v>4</v>
       </c>
-      <c r="E146" s="68">
+      <c r="E146" s="67">
         <v>28</v>
       </c>
-      <c r="F146" s="68">
+      <c r="F146" s="67">
         <f>E146*D146</f>
         <v>112</v>
       </c>
-      <c r="G146" s="67" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="67" t="s">
+      <c r="G146" s="66" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="C147" s="67" t="s">
-        <v>318</v>
-      </c>
-      <c r="D147" s="67">
+      <c r="C147" s="66" t="s">
+        <v>317</v>
+      </c>
+      <c r="D147" s="66">
         <v>6</v>
       </c>
-      <c r="E147" s="68">
+      <c r="E147" s="67">
         <v>121.5</v>
       </c>
-      <c r="F147" s="68">
+      <c r="F147" s="67">
         <f>E147*D147</f>
         <v>729</v>
       </c>
-      <c r="G147" s="67" t="s">
-        <v>504</v>
+      <c r="G147" s="66" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E150" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="F150" s="82">
+      <c r="F150" s="81">
         <f>SUM(F3:F148)</f>
-        <v>93310.255999999994</v>
+        <v>93335.255999999994</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="4" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B154" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="C154" s="4" t="s">
         <v>506</v>
-      </c>
-      <c r="C154" s="4" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B155" s="3">
         <v>1</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B156" s="3">
         <v>14</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B157" s="3">
         <v>2</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B158" s="3">
         <v>2</v>
       </c>
-      <c r="C158" s="67" t="s">
-        <v>509</v>
+      <c r="C158" s="66" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B159" s="3">
         <v>2</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -5791,621 +5792,621 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:9" s="60" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="60">
+    <row r="3" spans="1:9" s="59" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="59">
         <v>1008062</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="59" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="60">
-        <v>1</v>
-      </c>
-      <c r="E3" s="73">
+      <c r="D3" s="59">
+        <v>1</v>
+      </c>
+      <c r="E3" s="72">
         <v>7400</v>
       </c>
-      <c r="F3" s="61">
+      <c r="F3" s="60">
         <f>E3*D3</f>
         <v>7400</v>
       </c>
-      <c r="I3" s="60" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="60" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B4" s="60" t="s">
+      <c r="I3" s="59" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="59" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B4" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="60">
-        <v>1</v>
-      </c>
-      <c r="E4" s="73">
+      <c r="D4" s="59">
+        <v>1</v>
+      </c>
+      <c r="E4" s="72">
         <v>20000</v>
       </c>
-      <c r="F4" s="61">
+      <c r="F4" s="60">
         <f>D4*E4</f>
         <v>20000</v>
       </c>
-      <c r="I4" s="60" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B5" s="49" t="s">
-        <v>434</v>
-      </c>
-      <c r="C5" s="49" t="s">
-        <v>435</v>
-      </c>
-      <c r="D5" s="49">
-        <v>1</v>
-      </c>
-      <c r="E5" s="49">
+      <c r="I4" s="59" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B5" s="48" t="s">
+        <v>432</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>433</v>
+      </c>
+      <c r="D5" s="48">
+        <v>1</v>
+      </c>
+      <c r="E5" s="48">
         <v>50000</v>
       </c>
-      <c r="F5" s="49">
+      <c r="F5" s="48">
         <v>50000</v>
       </c>
-      <c r="I5" s="49" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+      <c r="I5" s="48" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B8" s="49" t="s">
+    <row r="8" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B8" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="48" t="s">
         <v>181</v>
       </c>
-      <c r="D8" s="49">
-        <v>1</v>
-      </c>
-      <c r="E8" s="52">
+      <c r="D8" s="48">
+        <v>1</v>
+      </c>
+      <c r="E8" s="51">
         <v>25000</v>
       </c>
-      <c r="F8" s="52">
+      <c r="F8" s="51">
         <f>D8*E8</f>
         <v>25000</v>
       </c>
-      <c r="I8" s="49" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+      <c r="I8" s="48" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" s="26" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
     </row>
-    <row r="12" spans="1:9" s="49" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="49" t="s">
-        <v>378</v>
-      </c>
-      <c r="B12" s="50" t="s">
-        <v>355</v>
-      </c>
-      <c r="C12" s="51" t="s">
-        <v>377</v>
-      </c>
-      <c r="D12" s="49">
-        <v>1</v>
-      </c>
-      <c r="E12" s="52">
+    <row r="12" spans="1:9" s="48" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="48" t="s">
+        <v>376</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>353</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>375</v>
+      </c>
+      <c r="D12" s="48">
+        <v>1</v>
+      </c>
+      <c r="E12" s="51">
         <v>525</v>
       </c>
-      <c r="F12" s="52">
+      <c r="F12" s="51">
         <f>D12*E12</f>
         <v>525</v>
       </c>
-      <c r="G12" s="49" t="s">
+      <c r="G12" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="49" t="s">
-        <v>417</v>
-      </c>
-      <c r="I12" s="49" t="s">
+      <c r="H12" s="48" t="s">
+        <v>415</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="48" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="48" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" s="49" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="49" t="s">
-        <v>381</v>
-      </c>
-      <c r="B13" s="50" t="s">
-        <v>355</v>
-      </c>
-      <c r="C13" s="51" t="s">
-        <v>380</v>
-      </c>
-      <c r="D13" s="49">
-        <v>1</v>
-      </c>
-      <c r="E13" s="52">
+      <c r="B13" s="49" t="s">
+        <v>353</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>378</v>
+      </c>
+      <c r="D13" s="48">
+        <v>1</v>
+      </c>
+      <c r="E13" s="51">
         <v>214</v>
       </c>
-      <c r="F13" s="52">
+      <c r="F13" s="51">
         <f t="shared" ref="F13:F15" si="0">D13*E13</f>
         <v>214</v>
       </c>
-      <c r="G13" s="49" t="s">
+      <c r="G13" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="49" t="s">
-        <v>417</v>
-      </c>
-      <c r="I13" s="49" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="49" t="s">
-        <v>383</v>
-      </c>
-      <c r="B14" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="49" t="s">
+      <c r="H13" s="48" t="s">
+        <v>415</v>
+      </c>
+      <c r="I13" s="48" t="s">
         <v>382</v>
       </c>
-      <c r="D14" s="49">
-        <v>1</v>
-      </c>
-      <c r="E14" s="52">
+    </row>
+    <row r="14" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="48" t="s">
+        <v>381</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>380</v>
+      </c>
+      <c r="D14" s="48">
+        <v>1</v>
+      </c>
+      <c r="E14" s="51">
         <v>23</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="51">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="G14" s="49" t="s">
+      <c r="G14" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="49" t="s">
-        <v>417</v>
-      </c>
-      <c r="I14" s="49" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
-        <v>386</v>
-      </c>
-      <c r="B15" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="49" t="s">
+      <c r="H14" s="48" t="s">
+        <v>415</v>
+      </c>
+      <c r="I14" s="48" t="s">
         <v>385</v>
       </c>
-      <c r="D15" s="49">
-        <v>1</v>
-      </c>
-      <c r="E15" s="52">
+    </row>
+    <row r="15" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="48" t="s">
+        <v>384</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>383</v>
+      </c>
+      <c r="D15" s="48">
+        <v>1</v>
+      </c>
+      <c r="E15" s="51">
         <v>23</v>
       </c>
-      <c r="F15" s="52">
+      <c r="F15" s="51">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="49" t="s">
-        <v>417</v>
-      </c>
-      <c r="I15" s="49" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="50" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
+      <c r="H15" s="48" t="s">
+        <v>415</v>
+      </c>
+      <c r="I15" s="48" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="52" t="s">
+        <v>273</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>272</v>
+      </c>
+      <c r="C16" s="52" t="s">
         <v>274</v>
       </c>
-      <c r="B16" s="50" t="s">
-        <v>273</v>
-      </c>
-      <c r="C16" s="53" t="s">
-        <v>275</v>
-      </c>
-      <c r="D16" s="50">
-        <v>1</v>
-      </c>
-      <c r="E16" s="54">
+      <c r="D16" s="49">
+        <v>1</v>
+      </c>
+      <c r="E16" s="53">
         <v>2</v>
       </c>
-      <c r="F16" s="55">
+      <c r="F16" s="54">
         <f>D16*E16</f>
         <v>2</v>
       </c>
-      <c r="G16" s="49" t="s">
+      <c r="G16" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="50" t="s">
-        <v>418</v>
-      </c>
-      <c r="I16" s="50" t="s">
+      <c r="H16" s="49" t="s">
         <v>416</v>
+      </c>
+      <c r="I16" s="49" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:10" s="67" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="67" t="s">
-        <v>301</v>
-      </c>
-      <c r="B19" s="67" t="s">
+    <row r="19" spans="1:10" s="66" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="66" t="s">
         <v>300</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="B19" s="66" t="s">
+        <v>299</v>
+      </c>
+      <c r="C19" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="67">
-        <v>1</v>
-      </c>
-      <c r="E19" s="68">
+      <c r="D19" s="66">
+        <v>1</v>
+      </c>
+      <c r="E19" s="67">
         <v>250</v>
       </c>
-      <c r="F19" s="68">
+      <c r="F19" s="67">
         <f>E19*D19</f>
         <v>250</v>
       </c>
-      <c r="G19" s="67" t="s">
+      <c r="G19" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="67" t="s">
+      <c r="H19" s="66" t="s">
         <v>15</v>
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" s="67" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="67" t="s">
-        <v>302</v>
-      </c>
-      <c r="B20" s="67" t="s">
-        <v>300</v>
-      </c>
-      <c r="C20" s="67" t="s">
-        <v>306</v>
-      </c>
-      <c r="D20" s="67">
-        <v>1</v>
-      </c>
-      <c r="E20" s="68">
+    <row r="20" spans="1:10" s="66" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="66" t="s">
+        <v>301</v>
+      </c>
+      <c r="B20" s="66" t="s">
+        <v>299</v>
+      </c>
+      <c r="C20" s="66" t="s">
+        <v>305</v>
+      </c>
+      <c r="D20" s="66">
+        <v>1</v>
+      </c>
+      <c r="E20" s="67">
         <v>13</v>
       </c>
-      <c r="F20" s="68">
+      <c r="F20" s="67">
         <f>E20*D20</f>
         <v>13</v>
       </c>
-      <c r="G20" s="67" t="s">
+      <c r="G20" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="67" t="s">
+      <c r="H20" s="66" t="s">
         <v>15</v>
       </c>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" s="67" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="67" t="s">
-        <v>304</v>
-      </c>
-      <c r="B21" s="67" t="s">
-        <v>300</v>
-      </c>
-      <c r="C21" s="67" t="s">
+    <row r="21" spans="1:10" s="66" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="66" t="s">
         <v>303</v>
       </c>
-      <c r="D21" s="67">
-        <v>1</v>
-      </c>
-      <c r="E21" s="68">
+      <c r="B21" s="66" t="s">
+        <v>299</v>
+      </c>
+      <c r="C21" s="66" t="s">
+        <v>302</v>
+      </c>
+      <c r="D21" s="66">
+        <v>1</v>
+      </c>
+      <c r="E21" s="67">
         <v>43</v>
       </c>
-      <c r="F21" s="68">
+      <c r="F21" s="67">
         <f>E21*D21</f>
         <v>43</v>
       </c>
-      <c r="G21" s="67" t="s">
+      <c r="G21" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="67" t="s">
+      <c r="H21" s="66" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="67" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="67" t="s">
-        <v>315</v>
-      </c>
-      <c r="B22" s="67" t="s">
-        <v>255</v>
-      </c>
-      <c r="C22" s="67" t="s">
-        <v>305</v>
-      </c>
-      <c r="D22" s="67">
-        <v>1</v>
-      </c>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
+    <row r="22" spans="1:10" s="66" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="66" t="s">
+        <v>314</v>
+      </c>
+      <c r="B22" s="66" t="s">
+        <v>254</v>
+      </c>
+      <c r="C22" s="66" t="s">
+        <v>304</v>
+      </c>
+      <c r="D22" s="66">
+        <v>1</v>
+      </c>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
       <c r="I22" s="32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:10" s="58" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="s">
-        <v>415</v>
-      </c>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-    </row>
-    <row r="26" spans="1:10" s="50" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
-        <v>344</v>
-      </c>
-      <c r="B26" s="50" t="s">
-        <v>255</v>
-      </c>
-      <c r="C26" s="53" t="s">
-        <v>345</v>
-      </c>
-      <c r="D26" s="50">
+    <row r="25" spans="1:10" s="57" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="s">
+        <v>413</v>
+      </c>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+    </row>
+    <row r="26" spans="1:10" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="52" t="s">
+        <v>342</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>254</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>343</v>
+      </c>
+      <c r="D26" s="49">
         <v>2</v>
       </c>
-      <c r="E26" s="54">
+      <c r="E26" s="53">
         <v>5</v>
       </c>
-      <c r="F26" s="55">
+      <c r="F26" s="54">
         <f t="shared" ref="F26:F33" si="1">E26*D26</f>
         <v>10</v>
       </c>
-      <c r="G26" s="50" t="s">
+      <c r="G26" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="H26" s="50" t="s">
-        <v>413</v>
-      </c>
-      <c r="I26" s="50" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="50" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
-        <v>347</v>
-      </c>
-      <c r="B27" s="50" t="s">
-        <v>300</v>
-      </c>
-      <c r="C27" s="53" t="s">
-        <v>351</v>
-      </c>
-      <c r="D27" s="50">
+      <c r="H26" s="49" t="s">
+        <v>411</v>
+      </c>
+      <c r="I26" s="49" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="52" t="s">
+        <v>345</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>299</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>349</v>
+      </c>
+      <c r="D27" s="49">
         <v>2</v>
       </c>
-      <c r="E27" s="54">
+      <c r="E27" s="53">
         <v>62</v>
       </c>
-      <c r="F27" s="55">
+      <c r="F27" s="54">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-      <c r="G27" s="50" t="s">
+      <c r="G27" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="H27" s="50" t="s">
-        <v>413</v>
-      </c>
-      <c r="I27" s="50" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="50" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="53" t="s">
-        <v>327</v>
-      </c>
-      <c r="B28" s="50" t="s">
-        <v>368</v>
-      </c>
-      <c r="C28" s="53" t="s">
-        <v>369</v>
-      </c>
-      <c r="D28" s="50">
+      <c r="H27" s="49" t="s">
+        <v>411</v>
+      </c>
+      <c r="I27" s="49" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="52" t="s">
+        <v>326</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>366</v>
+      </c>
+      <c r="C28" s="52" t="s">
+        <v>367</v>
+      </c>
+      <c r="D28" s="49">
         <v>8</v>
       </c>
-      <c r="E28" s="54">
-        <v>1</v>
-      </c>
-      <c r="F28" s="55">
+      <c r="E28" s="53">
+        <v>1</v>
+      </c>
+      <c r="F28" s="54">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G28" s="50" t="s">
+      <c r="G28" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="H28" s="50" t="s">
-        <v>413</v>
-      </c>
-      <c r="I28" s="50" t="s">
+      <c r="H28" s="49" t="s">
+        <v>411</v>
+      </c>
+      <c r="I28" s="49" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="52" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" s="50" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="53" t="s">
-        <v>372</v>
-      </c>
-      <c r="B29" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="53" t="s">
-        <v>371</v>
-      </c>
-      <c r="D29" s="50">
+      <c r="B29" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="52" t="s">
+        <v>369</v>
+      </c>
+      <c r="D29" s="49">
         <v>6</v>
       </c>
-      <c r="E29" s="54">
+      <c r="E29" s="53">
         <v>6</v>
       </c>
-      <c r="F29" s="55">
+      <c r="F29" s="54">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="G29" s="50" t="s">
+      <c r="G29" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="H29" s="50" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="50" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="53" t="s">
-        <v>373</v>
-      </c>
-      <c r="B30" s="50" t="s">
-        <v>255</v>
-      </c>
-      <c r="C30" s="53" t="s">
-        <v>374</v>
-      </c>
-      <c r="D30" s="50">
+      <c r="H29" s="49" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="52" t="s">
+        <v>371</v>
+      </c>
+      <c r="B30" s="49" t="s">
+        <v>254</v>
+      </c>
+      <c r="C30" s="52" t="s">
+        <v>372</v>
+      </c>
+      <c r="D30" s="49">
         <v>2</v>
       </c>
-      <c r="E30" s="54">
-        <v>1</v>
-      </c>
-      <c r="F30" s="55">
+      <c r="E30" s="53">
+        <v>1</v>
+      </c>
+      <c r="F30" s="54">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G30" s="50" t="s">
+      <c r="G30" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="50" t="s">
-        <v>413</v>
-      </c>
-      <c r="I30" s="50" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="50" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="56" t="s">
-        <v>349</v>
-      </c>
-      <c r="B31" s="50" t="s">
-        <v>300</v>
-      </c>
-      <c r="C31" s="53" t="s">
-        <v>348</v>
-      </c>
-      <c r="D31" s="50">
-        <v>1</v>
-      </c>
-      <c r="E31" s="54">
+      <c r="H30" s="49" t="s">
+        <v>411</v>
+      </c>
+      <c r="I30" s="49" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="55" t="s">
+        <v>347</v>
+      </c>
+      <c r="B31" s="49" t="s">
+        <v>299</v>
+      </c>
+      <c r="C31" s="52" t="s">
+        <v>346</v>
+      </c>
+      <c r="D31" s="49">
+        <v>1</v>
+      </c>
+      <c r="E31" s="53">
         <v>2</v>
       </c>
-      <c r="F31" s="55">
+      <c r="F31" s="54">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G31" s="50" t="s">
+      <c r="G31" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="H31" s="50" t="s">
-        <v>413</v>
-      </c>
-      <c r="I31" s="50" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="50" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="56" t="s">
-        <v>349</v>
-      </c>
-      <c r="B32" s="50" t="s">
-        <v>300</v>
-      </c>
-      <c r="C32" s="53" t="s">
-        <v>353</v>
-      </c>
-      <c r="D32" s="50">
-        <v>1</v>
-      </c>
-      <c r="E32" s="54">
+      <c r="H31" s="49" t="s">
+        <v>411</v>
+      </c>
+      <c r="I31" s="49" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="55" t="s">
+        <v>347</v>
+      </c>
+      <c r="B32" s="49" t="s">
+        <v>299</v>
+      </c>
+      <c r="C32" s="52" t="s">
+        <v>351</v>
+      </c>
+      <c r="D32" s="49">
+        <v>1</v>
+      </c>
+      <c r="E32" s="53">
         <v>15</v>
       </c>
-      <c r="F32" s="55">
+      <c r="F32" s="54">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G32" s="50" t="s">
+      <c r="G32" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="H32" s="50" t="s">
-        <v>413</v>
-      </c>
-      <c r="I32" s="50" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="50" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="53" t="s">
+      <c r="H32" s="49" t="s">
+        <v>411</v>
+      </c>
+      <c r="I32" s="49" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="52" t="s">
         <v>247</v>
       </c>
-      <c r="B33" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="53" t="s">
+      <c r="B33" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="52" t="s">
         <v>248</v>
       </c>
-      <c r="D33" s="50">
+      <c r="D33" s="49">
         <v>2</v>
       </c>
-      <c r="E33" s="54">
+      <c r="E33" s="53">
         <v>25</v>
       </c>
-      <c r="F33" s="55">
+      <c r="F33" s="54">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="G33" s="50" t="s">
+      <c r="G33" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="H33" s="50" t="s">
-        <v>413</v>
+      <c r="H33" s="49" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -6415,31 +6416,31 @@
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
     </row>
-    <row r="38" spans="1:9" s="60" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="60" t="s">
+    <row r="38" spans="1:9" s="59" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="60" t="s">
+      <c r="B38" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="60" t="s">
+      <c r="C38" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="60">
-        <v>1</v>
-      </c>
-      <c r="E38" s="61">
+      <c r="D38" s="59">
+        <v>1</v>
+      </c>
+      <c r="E38" s="60">
         <v>2800</v>
       </c>
-      <c r="F38" s="61">
+      <c r="F38" s="60">
         <f>E38*D38</f>
         <v>2800</v>
       </c>
-      <c r="G38" s="60" t="s">
+      <c r="G38" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="I38" s="60" t="s">
-        <v>419</v>
+      <c r="I38" s="59" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -6450,783 +6451,783 @@
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
     </row>
-    <row r="43" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="49" t="s">
+    <row r="43" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="B43" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="49" t="s">
+      <c r="B43" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="D43" s="49">
-        <v>1</v>
-      </c>
-      <c r="E43" s="52">
+      <c r="D43" s="48">
+        <v>1</v>
+      </c>
+      <c r="E43" s="51">
         <v>488</v>
       </c>
-      <c r="F43" s="52">
+      <c r="F43" s="51">
         <f t="shared" ref="F43:F64" si="2">E43*D43</f>
         <v>488</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="49" t="s">
+    <row r="44" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A44" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C44" s="49" t="s">
+      <c r="B44" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="49">
-        <v>1</v>
-      </c>
-      <c r="E44" s="52">
+      <c r="D44" s="48">
+        <v>1</v>
+      </c>
+      <c r="E44" s="51">
         <v>184</v>
       </c>
-      <c r="F44" s="52">
+      <c r="F44" s="51">
         <f t="shared" si="2"/>
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="49" t="s">
+    <row r="45" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="B45" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="49" t="s">
+      <c r="B45" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="49">
-        <v>1</v>
-      </c>
-      <c r="E45" s="52">
+      <c r="D45" s="48">
+        <v>1</v>
+      </c>
+      <c r="E45" s="51">
         <v>76</v>
       </c>
-      <c r="F45" s="52">
+      <c r="F45" s="51">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="49" t="s">
+    <row r="46" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A46" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="B46" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="49" t="s">
+      <c r="B46" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="49">
-        <v>1</v>
-      </c>
-      <c r="E46" s="52">
+      <c r="D46" s="48">
+        <v>1</v>
+      </c>
+      <c r="E46" s="51">
         <v>184</v>
       </c>
-      <c r="F46" s="52">
+      <c r="F46" s="51">
         <f t="shared" si="2"/>
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="49" t="s">
+    <row r="47" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="49" t="s">
+      <c r="B47" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="D47" s="49">
-        <v>1</v>
-      </c>
-      <c r="E47" s="52">
+      <c r="D47" s="48">
+        <v>1</v>
+      </c>
+      <c r="E47" s="51">
         <v>94.180155999999997</v>
       </c>
-      <c r="F47" s="52">
+      <c r="F47" s="51">
         <f t="shared" si="2"/>
         <v>94.180155999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="49" t="s">
+    <row r="48" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A48" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="B48" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="49" t="s">
+      <c r="B48" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="D48" s="49">
-        <v>1</v>
-      </c>
-      <c r="E48" s="52">
+      <c r="D48" s="48">
+        <v>1</v>
+      </c>
+      <c r="E48" s="51">
         <v>36.799999999999997</v>
       </c>
-      <c r="F48" s="52">
+      <c r="F48" s="51">
         <f t="shared" si="2"/>
         <v>36.799999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A49" s="49" t="s">
+    <row r="49" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A49" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" s="49" t="s">
+      <c r="B49" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="D49" s="49">
+      <c r="D49" s="48">
         <v>2</v>
       </c>
-      <c r="E49" s="52">
+      <c r="E49" s="51">
         <v>21.21</v>
       </c>
-      <c r="F49" s="52">
+      <c r="F49" s="51">
         <f t="shared" si="2"/>
         <v>42.42</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="49" t="s">
+    <row r="50" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A50" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="B50" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C50" s="49" t="s">
+      <c r="B50" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="D50" s="49">
-        <v>1</v>
-      </c>
-      <c r="E50" s="52">
+      <c r="D50" s="48">
+        <v>1</v>
+      </c>
+      <c r="E50" s="51">
         <v>304.75</v>
       </c>
-      <c r="F50" s="52">
+      <c r="F50" s="51">
         <f t="shared" si="2"/>
         <v>304.75</v>
       </c>
-      <c r="I50" s="49" t="s">
+      <c r="I50" s="48" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A51" s="49" t="s">
+    <row r="51" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A51" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="49" t="s">
+      <c r="B51" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="D51" s="49">
-        <v>1</v>
-      </c>
-      <c r="E51" s="52">
+      <c r="D51" s="48">
+        <v>1</v>
+      </c>
+      <c r="E51" s="51">
         <v>148.21</v>
       </c>
-      <c r="F51" s="52">
+      <c r="F51" s="51">
         <f t="shared" si="2"/>
         <v>148.21</v>
       </c>
-      <c r="I51" s="49" t="s">
+      <c r="I51" s="48" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="49" t="s">
+    <row r="52" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A52" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C52" s="49" t="s">
+      <c r="B52" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="49">
-        <v>1</v>
-      </c>
-      <c r="E52" s="52">
+      <c r="D52" s="48">
+        <v>1</v>
+      </c>
+      <c r="E52" s="51">
         <v>348.45</v>
       </c>
-      <c r="F52" s="52">
+      <c r="F52" s="51">
         <f t="shared" si="2"/>
         <v>348.45</v>
       </c>
-      <c r="I52" s="49" t="s">
+      <c r="I52" s="48" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="49" t="s">
+    <row r="53" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A53" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" s="49" t="s">
+      <c r="B53" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="49">
-        <v>1</v>
-      </c>
-      <c r="E53" s="52">
+      <c r="D53" s="48">
+        <v>1</v>
+      </c>
+      <c r="E53" s="51">
         <v>60.95</v>
       </c>
-      <c r="F53" s="52">
+      <c r="F53" s="51">
         <f t="shared" si="2"/>
         <v>60.95</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="49" t="s">
+    <row r="54" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A54" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C54" s="49" t="s">
+      <c r="B54" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="49">
-        <v>1</v>
-      </c>
-      <c r="E54" s="52">
+      <c r="D54" s="48">
+        <v>1</v>
+      </c>
+      <c r="E54" s="51">
         <v>34.5</v>
       </c>
-      <c r="F54" s="52">
+      <c r="F54" s="51">
         <f t="shared" si="2"/>
         <v>34.5</v>
       </c>
-      <c r="I54" s="49" t="s">
+      <c r="I54" s="48" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="49" t="s">
+    <row r="55" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A55" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="B55" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C55" s="49" t="s">
+      <c r="B55" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="D55" s="49">
-        <v>1</v>
-      </c>
-      <c r="E55" s="52">
+      <c r="D55" s="48">
+        <v>1</v>
+      </c>
+      <c r="E55" s="51">
         <v>51.45</v>
       </c>
-      <c r="F55" s="52">
+      <c r="F55" s="51">
         <f t="shared" si="2"/>
         <v>51.45</v>
       </c>
-      <c r="I55" s="49" t="s">
+      <c r="I55" s="48" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="49" t="s">
+    <row r="56" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A56" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="B56" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C56" s="49" t="s">
+      <c r="B56" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="49">
+      <c r="D56" s="48">
         <v>2</v>
       </c>
-      <c r="E56" s="52">
+      <c r="E56" s="51">
         <v>13.8</v>
       </c>
-      <c r="F56" s="52">
+      <c r="F56" s="51">
         <f t="shared" si="2"/>
         <v>27.6</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A57" s="49" t="s">
+    <row r="57" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A57" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="B57" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57" s="49" t="s">
+      <c r="B57" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="D57" s="49">
-        <v>1</v>
-      </c>
-      <c r="E57" s="52">
+      <c r="D57" s="48">
+        <v>1</v>
+      </c>
+      <c r="E57" s="51">
         <v>19.09</v>
       </c>
-      <c r="F57" s="52">
+      <c r="F57" s="51">
         <f t="shared" si="2"/>
         <v>19.09</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A58" s="49" t="s">
+    <row r="58" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A58" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="B58" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58" s="49" t="s">
+      <c r="B58" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="D58" s="49">
+      <c r="D58" s="48">
         <v>2</v>
       </c>
-      <c r="E58" s="52">
+      <c r="E58" s="51">
         <v>40.51</v>
       </c>
-      <c r="F58" s="52">
+      <c r="F58" s="51">
         <f t="shared" si="2"/>
         <v>81.02</v>
       </c>
-      <c r="I58" s="49" t="s">
+      <c r="I58" s="48" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A59" s="49" t="s">
+    <row r="59" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A59" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="B59" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C59" s="49" t="s">
+      <c r="B59" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="D59" s="49">
+      <c r="D59" s="48">
         <v>2</v>
       </c>
-      <c r="E59" s="52">
+      <c r="E59" s="51">
         <v>83.598116000000005</v>
       </c>
-      <c r="F59" s="52">
+      <c r="F59" s="51">
         <f t="shared" si="2"/>
         <v>167.19623200000001</v>
       </c>
-      <c r="I59" s="49" t="s">
+      <c r="I59" s="48" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="49" t="s">
+    <row r="60" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A60" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="B60" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C60" s="49" t="s">
+      <c r="B60" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="D60" s="49">
+      <c r="D60" s="48">
         <v>4</v>
       </c>
-      <c r="E60" s="52">
+      <c r="E60" s="51">
         <v>70.103999999999999</v>
       </c>
-      <c r="F60" s="52">
+      <c r="F60" s="51">
         <f t="shared" si="2"/>
         <v>280.416</v>
       </c>
-      <c r="I60" s="49" t="s">
+      <c r="I60" s="48" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A61" s="49" t="s">
+    <row r="61" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A61" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="B61" s="49" t="s">
+      <c r="B61" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="C61" s="49" t="s">
+      <c r="C61" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="D61" s="49">
+      <c r="D61" s="48">
         <v>2</v>
       </c>
-      <c r="E61" s="52">
+      <c r="E61" s="51">
         <v>28.75</v>
       </c>
-      <c r="F61" s="52">
+      <c r="F61" s="51">
         <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
-      <c r="I61" s="62" t="s">
+      <c r="I61" s="61" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A62" s="49" t="s">
+    <row r="62" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A62" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="B62" s="49" t="s">
+      <c r="B62" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="C62" s="49" t="s">
+      <c r="C62" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="D62" s="49">
+      <c r="D62" s="48">
         <v>2</v>
       </c>
-      <c r="E62" s="52">
+      <c r="E62" s="51">
         <v>38.872799999999998</v>
       </c>
-      <c r="F62" s="52">
+      <c r="F62" s="51">
         <f t="shared" si="2"/>
         <v>77.745599999999996</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B63" s="49" t="s">
+    <row r="63" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B63" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="C63" s="49" t="s">
+      <c r="C63" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="D63" s="49">
-        <v>1</v>
-      </c>
-      <c r="E63" s="52">
+      <c r="D63" s="48">
+        <v>1</v>
+      </c>
+      <c r="E63" s="51">
         <v>205</v>
       </c>
-      <c r="F63" s="52">
+      <c r="F63" s="51">
         <f t="shared" si="2"/>
         <v>205</v>
       </c>
-      <c r="I63" s="49" t="s">
+      <c r="I63" s="48" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B64" s="49" t="s">
+    <row r="64" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B64" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="C64" s="49" t="s">
+      <c r="C64" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="D64" s="49">
+      <c r="D64" s="48">
         <v>2</v>
       </c>
-      <c r="E64" s="52">
+      <c r="E64" s="51">
         <v>12</v>
       </c>
-      <c r="F64" s="52">
+      <c r="F64" s="51">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="I64" s="49" t="s">
+      <c r="I64" s="48" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F66" s="9"/>
     </row>
-    <row r="67" spans="1:10" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="49" t="s">
+    <row r="67" spans="1:10" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A67" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="B67" s="49" t="s">
+      <c r="B67" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="C67" s="49" t="s">
+      <c r="C67" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="D67" s="49">
+      <c r="D67" s="48">
         <v>2</v>
       </c>
-      <c r="E67" s="52">
+      <c r="E67" s="51">
         <v>140</v>
       </c>
-      <c r="F67" s="52">
+      <c r="F67" s="51">
         <f>E67*D67</f>
         <v>280</v>
       </c>
-      <c r="I67" s="49" t="s">
-        <v>425</v>
+      <c r="I67" s="48" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>419</v>
+      </c>
+      <c r="B68" s="62" t="s">
+        <v>420</v>
+      </c>
+      <c r="C68" s="62" t="s">
         <v>421</v>
       </c>
-      <c r="B68" s="63" t="s">
-        <v>422</v>
-      </c>
-      <c r="C68" s="63" t="s">
-        <v>423</v>
-      </c>
-      <c r="D68" s="63">
+      <c r="D68" s="62">
         <v>2</v>
       </c>
-      <c r="E68" s="64">
+      <c r="E68" s="63">
         <v>84</v>
       </c>
       <c r="F68">
         <f>D68*E68</f>
         <v>168</v>
       </c>
-      <c r="I68" s="63" t="s">
-        <v>424</v>
+      <c r="I68" s="62" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>428</v>
-      </c>
-      <c r="B69" s="63" t="s">
-        <v>427</v>
-      </c>
-      <c r="C69" s="63" t="s">
         <v>426</v>
       </c>
-      <c r="D69" s="63">
-        <v>1</v>
-      </c>
-      <c r="E69" s="64">
+      <c r="B69" s="62" t="s">
+        <v>425</v>
+      </c>
+      <c r="C69" s="62" t="s">
+        <v>424</v>
+      </c>
+      <c r="D69" s="62">
+        <v>1</v>
+      </c>
+      <c r="E69" s="63">
         <v>54</v>
       </c>
       <c r="F69">
         <f>D69*E69</f>
         <v>54</v>
       </c>
-      <c r="I69" s="63" t="s">
-        <v>429</v>
+      <c r="I69" s="62" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="F71" s="9"/>
+    </row>
+    <row r="72" spans="1:10" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A72" s="48" t="s">
+        <v>429</v>
+      </c>
+      <c r="C72" s="64"/>
+      <c r="E72" s="51"/>
+      <c r="F72" s="51"/>
+      <c r="J72" s="64"/>
+    </row>
+    <row r="73" spans="1:10" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A73" s="48" t="s">
         <v>430</v>
       </c>
-      <c r="F71" s="9"/>
-    </row>
-    <row r="72" spans="1:10" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A72" s="49" t="s">
-        <v>431</v>
-      </c>
-      <c r="C72" s="65"/>
-      <c r="E72" s="52"/>
-      <c r="F72" s="52"/>
-      <c r="J72" s="65"/>
-    </row>
-    <row r="73" spans="1:10" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="49" t="s">
-        <v>432</v>
-      </c>
-      <c r="C73" s="65"/>
-      <c r="E73" s="52"/>
-      <c r="F73" s="52"/>
-      <c r="J73" s="65"/>
-    </row>
-    <row r="74" spans="1:10" s="49" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="C74" s="65"/>
-      <c r="E74" s="52"/>
-      <c r="F74" s="52"/>
-      <c r="J74" s="65"/>
+      <c r="C73" s="64"/>
+      <c r="E73" s="51"/>
+      <c r="F73" s="51"/>
+      <c r="J73" s="64"/>
+    </row>
+    <row r="74" spans="1:10" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C74" s="64"/>
+      <c r="E74" s="51"/>
+      <c r="F74" s="51"/>
+      <c r="J74" s="64"/>
     </row>
     <row r="75" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
         <v>165</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
     </row>
-    <row r="76" spans="1:10" s="70" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="70" t="s">
-        <v>437</v>
-      </c>
-      <c r="B76" s="70" t="s">
+    <row r="76" spans="1:10" s="69" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A76" s="69" t="s">
+        <v>435</v>
+      </c>
+      <c r="B76" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="C76" s="70" t="s">
-        <v>438</v>
-      </c>
-      <c r="D76" s="70">
-        <v>1</v>
-      </c>
-      <c r="E76" s="71">
+      <c r="C76" s="69" t="s">
+        <v>436</v>
+      </c>
+      <c r="D76" s="69">
+        <v>1</v>
+      </c>
+      <c r="E76" s="70">
         <v>518.5</v>
       </c>
-      <c r="F76" s="71">
+      <c r="F76" s="70">
         <f t="shared" ref="F76:F83" si="3">E76*D76</f>
         <v>518.5</v>
       </c>
-      <c r="I76" s="70" t="s">
+      <c r="I76" s="69" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="70" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A77" s="70" t="s">
-        <v>440</v>
-      </c>
-      <c r="B77" s="70" t="s">
+    <row r="77" spans="1:10" s="69" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A77" s="69" t="s">
+        <v>438</v>
+      </c>
+      <c r="B77" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="C77" s="70" t="s">
-        <v>439</v>
-      </c>
-      <c r="D77" s="70">
-        <v>1</v>
-      </c>
-      <c r="E77" s="71">
+      <c r="C77" s="69" t="s">
+        <v>437</v>
+      </c>
+      <c r="D77" s="69">
+        <v>1</v>
+      </c>
+      <c r="E77" s="70">
         <v>764</v>
       </c>
-      <c r="F77" s="71">
+      <c r="F77" s="70">
         <f t="shared" si="3"/>
         <v>764</v>
       </c>
     </row>
-    <row r="78" spans="1:10" s="70" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A78" s="70" t="s">
-        <v>442</v>
-      </c>
-      <c r="B78" s="70" t="s">
+    <row r="78" spans="1:10" s="69" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A78" s="69" t="s">
+        <v>440</v>
+      </c>
+      <c r="B78" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="C78" s="70" t="s">
-        <v>441</v>
-      </c>
-      <c r="D78" s="70">
-        <v>1</v>
-      </c>
-      <c r="E78" s="71">
+      <c r="C78" s="69" t="s">
+        <v>439</v>
+      </c>
+      <c r="D78" s="69">
+        <v>1</v>
+      </c>
+      <c r="E78" s="70">
         <v>816</v>
       </c>
-      <c r="F78" s="71">
+      <c r="F78" s="70">
         <f t="shared" si="3"/>
         <v>816</v>
       </c>
-      <c r="I78" s="70" t="s">
+      <c r="I78" s="69" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="70" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A79" s="70" t="s">
-        <v>444</v>
-      </c>
-      <c r="B79" s="70" t="s">
+    <row r="79" spans="1:10" s="69" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A79" s="69" t="s">
+        <v>442</v>
+      </c>
+      <c r="B79" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="C79" s="70" t="s">
-        <v>443</v>
-      </c>
-      <c r="D79" s="70">
-        <v>1</v>
-      </c>
-      <c r="E79" s="71">
+      <c r="C79" s="69" t="s">
+        <v>441</v>
+      </c>
+      <c r="D79" s="69">
+        <v>1</v>
+      </c>
+      <c r="E79" s="70">
         <v>952</v>
       </c>
-      <c r="F79" s="71">
+      <c r="F79" s="70">
         <f t="shared" si="3"/>
         <v>952</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="70" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A80" s="70" t="s">
-        <v>451</v>
-      </c>
-      <c r="B80" s="70" t="s">
+    <row r="80" spans="1:10" s="69" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A80" s="69" t="s">
+        <v>449</v>
+      </c>
+      <c r="B80" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="C80" s="70" t="s">
-        <v>452</v>
-      </c>
-      <c r="D80" s="70">
-        <v>1</v>
-      </c>
-      <c r="E80" s="71">
+      <c r="C80" s="69" t="s">
+        <v>450</v>
+      </c>
+      <c r="D80" s="69">
+        <v>1</v>
+      </c>
+      <c r="E80" s="70">
         <v>99.5</v>
       </c>
-      <c r="F80" s="71">
+      <c r="F80" s="70">
         <f t="shared" si="3"/>
         <v>99.5</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="70" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A81" s="70" t="s">
-        <v>446</v>
-      </c>
-      <c r="B81" s="70" t="s">
+    <row r="81" spans="1:6" s="69" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A81" s="69" t="s">
+        <v>444</v>
+      </c>
+      <c r="B81" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="C81" s="70" t="s">
-        <v>445</v>
-      </c>
-      <c r="D81" s="70">
-        <v>1</v>
-      </c>
-      <c r="E81" s="71">
+      <c r="C81" s="69" t="s">
+        <v>443</v>
+      </c>
+      <c r="D81" s="69">
+        <v>1</v>
+      </c>
+      <c r="E81" s="70">
         <v>128.5</v>
       </c>
-      <c r="F81" s="71">
+      <c r="F81" s="70">
         <f t="shared" si="3"/>
         <v>128.5</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="70" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A82" s="70" t="s">
-        <v>448</v>
-      </c>
-      <c r="B82" s="70" t="s">
+    <row r="82" spans="1:6" s="69" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A82" s="69" t="s">
+        <v>446</v>
+      </c>
+      <c r="B82" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="C82" s="70" t="s">
-        <v>447</v>
-      </c>
-      <c r="D82" s="70">
-        <v>1</v>
-      </c>
-      <c r="E82" s="71">
+      <c r="C82" s="69" t="s">
+        <v>445</v>
+      </c>
+      <c r="D82" s="69">
+        <v>1</v>
+      </c>
+      <c r="E82" s="70">
         <v>156</v>
       </c>
-      <c r="F82" s="71">
+      <c r="F82" s="70">
         <f t="shared" si="3"/>
         <v>156</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="70" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A83" s="70" t="s">
-        <v>450</v>
-      </c>
-      <c r="B83" s="70" t="s">
+    <row r="83" spans="1:6" s="69" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A83" s="69" t="s">
+        <v>448</v>
+      </c>
+      <c r="B83" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="C83" s="70" t="s">
-        <v>449</v>
-      </c>
-      <c r="D83" s="70">
-        <v>1</v>
-      </c>
-      <c r="E83" s="71">
+      <c r="C83" s="69" t="s">
+        <v>447</v>
+      </c>
+      <c r="D83" s="69">
+        <v>1</v>
+      </c>
+      <c r="E83" s="70">
         <v>184.5</v>
       </c>
-      <c r="F83" s="71">
+      <c r="F83" s="70">
         <f t="shared" si="3"/>
         <v>184.5</v>
       </c>

</xml_diff>

<commit_message>
v4-5 upgrade parts list
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB9E735-7DA6-46FB-9C65-9E8009EF0111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7F9232-9BE3-4DF5-91FA-8BEF246CF774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6336" yWindow="4560" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="530">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -1265,12 +1265,6 @@
     <t>Adapter for SM2 lens tube, attached to SM2 retaining ring</t>
   </si>
   <si>
-    <t>SM2L30</t>
-  </si>
-  <si>
-    <t>SM2 Lens Tube, 3" Thread Depth</t>
-  </si>
-  <si>
     <t>SM2E60</t>
   </si>
   <si>
@@ -1278,9 +1272,6 @@
   </si>
   <si>
     <t>Tube lens is inserted inside this tube</t>
-  </si>
-  <si>
-    <t>Objective is mounted on this tube using M2M40S adapter. Filter is mounted inside.</t>
   </si>
   <si>
     <t>SM2M20</t>
@@ -1705,12 +1696,18 @@
   <si>
     <t>Total:</t>
   </si>
+  <si>
+    <t>SM2 coupler to rotate the filter wheel and fix it at desired angle the with retaining ring</t>
+  </si>
+  <si>
+    <t>3D printed (SLS)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1887,6 +1884,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -2026,7 +2030,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyFont="1"/>
@@ -2078,6 +2081,7 @@
     <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Excel Built-in Heading 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2465,10 +2469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J173"/>
+  <dimension ref="A1:J172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F150" sqref="F150"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2609,7 +2613,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
@@ -2687,10 +2691,10 @@
         <v>372</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="D13" s="31">
         <v>1</v>
@@ -2795,13 +2799,13 @@
     </row>
     <row r="17" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B17" s="31" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D17" s="31">
         <v>1</v>
@@ -2813,11 +2817,11 @@
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="G17" s="65" t="s">
+      <c r="G17" s="64" t="s">
         <v>262</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3103,7 +3107,7 @@
     </row>
     <row r="30" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
@@ -3324,11 +3328,11 @@
       </c>
     </row>
     <row r="41" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="88">
+      <c r="A41" s="87">
         <v>91863</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>50</v>
@@ -3350,18 +3354,18 @@
         <v>220</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="D42" s="3">
         <v>2</v>
@@ -3380,11 +3384,11 @@
         <v>247</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="84" t="s">
+      <c r="A43" s="83" t="s">
         <v>249</v>
       </c>
       <c r="B43" s="37" t="s">
@@ -3396,10 +3400,10 @@
       <c r="D43" s="37">
         <v>0</v>
       </c>
-      <c r="E43" s="85">
+      <c r="E43" s="84">
         <v>40</v>
       </c>
-      <c r="F43" s="86">
+      <c r="F43" s="85">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3410,9 +3414,9 @@
         <v>247</v>
       </c>
       <c r="I43" s="37" t="s">
-        <v>518</v>
-      </c>
-      <c r="J43" s="87"/>
+        <v>515</v>
+      </c>
+      <c r="J43" s="86"/>
     </row>
     <row r="44" spans="1:10" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="44" t="s">
@@ -3427,10 +3431,10 @@
       <c r="D44" s="37">
         <v>0</v>
       </c>
-      <c r="E44" s="85">
+      <c r="E44" s="84">
         <v>92</v>
       </c>
-      <c r="F44" s="86">
+      <c r="F44" s="85">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3441,7 +3445,7 @@
         <v>247</v>
       </c>
       <c r="I44" s="37" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3602,7 +3606,7 @@
         <v>64</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D50" s="31">
         <v>4</v>
@@ -3614,14 +3618,14 @@
         <f t="shared" si="3"/>
         <v>416</v>
       </c>
-      <c r="G50" s="65" t="s">
+      <c r="G50" s="64" t="s">
         <v>41</v>
       </c>
       <c r="H50" s="31" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="I50" s="31" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -3919,11 +3923,11 @@
       </c>
     </row>
     <row r="61" spans="1:9" s="35" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="83" t="s">
-        <v>506</v>
+      <c r="A61" s="82" t="s">
+        <v>503</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C61" s="34" t="s">
         <v>325</v>
@@ -3980,13 +3984,13 @@
     </row>
     <row r="63" spans="1:9" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="44" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D63" s="31">
         <v>2</v>
@@ -3998,44 +4002,44 @@
         <f t="shared" ref="F63" si="4">E63*D63</f>
         <v>600</v>
       </c>
-      <c r="G63" s="65" t="s">
+      <c r="G63" s="64" t="s">
         <v>41</v>
       </c>
       <c r="H63" s="31" t="s">
         <v>244</v>
       </c>
       <c r="I63" s="37" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" s="72" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="32" t="s">
-        <v>490</v>
-      </c>
-      <c r="B64" s="72" t="s">
-        <v>64</v>
-      </c>
-      <c r="C64" s="73" t="s">
-        <v>481</v>
-      </c>
-      <c r="D64" s="72">
+        <v>487</v>
+      </c>
+      <c r="B64" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="C64" s="72" t="s">
+        <v>478</v>
+      </c>
+      <c r="D64" s="71">
         <v>0</v>
       </c>
-      <c r="E64" s="74">
+      <c r="E64" s="73">
         <v>36</v>
       </c>
-      <c r="F64" s="75">
+      <c r="F64" s="74">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G64" s="76" t="s">
+      <c r="G64" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="H64" s="72" t="s">
+      <c r="H64" s="71" t="s">
         <v>244</v>
       </c>
-      <c r="I64" s="72" t="s">
-        <v>489</v>
+      <c r="I64" s="71" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -4065,7 +4069,7 @@
         <v>244</v>
       </c>
       <c r="I65" s="31" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -4097,13 +4101,13 @@
     </row>
     <row r="67" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="43" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B67" s="31" t="s">
         <v>64</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D67" s="31">
         <v>1</v>
@@ -4125,33 +4129,33 @@
         <v>330</v>
       </c>
     </row>
-    <row r="68" spans="1:9" s="72" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="82" t="s">
+    <row r="68" spans="1:9" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="81" t="s">
         <v>338</v>
       </c>
-      <c r="B68" s="72" t="s">
-        <v>64</v>
-      </c>
-      <c r="C68" s="73" t="s">
+      <c r="B68" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="C68" s="72" t="s">
         <v>308</v>
       </c>
-      <c r="D68" s="72">
+      <c r="D68" s="71">
         <v>0</v>
       </c>
-      <c r="E68" s="74">
+      <c r="E68" s="73">
         <v>390</v>
       </c>
-      <c r="F68" s="75">
+      <c r="F68" s="74">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G68" s="76" t="s">
+      <c r="G68" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="H68" s="72" t="s">
+      <c r="H68" s="71" t="s">
         <v>244</v>
       </c>
-      <c r="I68" s="72" t="s">
+      <c r="I68" s="71" t="s">
         <v>331</v>
       </c>
     </row>
@@ -4160,7 +4164,7 @@
         <v>333</v>
       </c>
       <c r="B69" s="37" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C69" s="32" t="s">
         <v>332</v>
@@ -4322,27 +4326,27 @@
     </row>
     <row r="79" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
     </row>
     <row r="80" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
     </row>
     <row r="81" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="C81" s="46" t="s">
         <v>453</v>
+      </c>
+      <c r="C81" s="93" t="s">
+        <v>450</v>
       </c>
       <c r="D81" s="3">
         <v>1</v>
@@ -4355,19 +4359,19 @@
         <v>200</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="J81" s="4"/>
     </row>
     <row r="82" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>252</v>
+        <v>529</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D82" s="4">
         <v>5</v>
@@ -4380,18 +4384,18 @@
         <v>5</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="65" t="s">
-        <v>460</v>
+      <c r="A83" s="64" t="s">
+        <v>457</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D83" s="3">
         <v>1</v>
@@ -4399,23 +4403,23 @@
       <c r="E83" s="5">
         <v>26</v>
       </c>
-      <c r="F83" s="66">
+      <c r="F83" s="65">
         <f>E83*D83</f>
         <v>26</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D84" s="3">
         <v>1</v>
@@ -4423,38 +4427,40 @@
       <c r="E84" s="5">
         <v>37</v>
       </c>
-      <c r="F84" s="66">
+      <c r="F84" s="65">
         <f>E84*D84</f>
         <v>37</v>
       </c>
-      <c r="I84" s="31"/>
-    </row>
-    <row r="85" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="65" t="s">
+      <c r="I84" s="64" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="64" t="s">
         <v>382</v>
       </c>
-      <c r="B85" s="65" t="s">
-        <v>64</v>
-      </c>
-      <c r="C85" s="65" t="s">
+      <c r="B85" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="C85" s="64" t="s">
         <v>381</v>
       </c>
-      <c r="D85" s="65">
+      <c r="D85" s="64">
         <v>2</v>
       </c>
-      <c r="E85" s="66">
+      <c r="E85" s="65">
         <v>24</v>
       </c>
-      <c r="F85" s="66">
+      <c r="F85" s="65">
         <f>E85*D85</f>
         <v>48</v>
       </c>
       <c r="I85" s="31" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="86" spans="1:10" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="70" t="s">
+      <c r="A86" s="69" t="s">
         <v>170</v>
       </c>
       <c r="F86" s="42"/>
@@ -4506,7 +4512,7 @@
       <c r="B90" s="27" t="s">
         <v>351</v>
       </c>
-      <c r="C90" s="79" t="s">
+      <c r="C90" s="78" t="s">
         <v>354</v>
       </c>
       <c r="D90" s="27">
@@ -4523,7 +4529,7 @@
         <v>13</v>
       </c>
       <c r="I90" s="27" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -4533,7 +4539,7 @@
       <c r="B91" s="27" t="s">
         <v>351</v>
       </c>
-      <c r="C91" s="80" t="s">
+      <c r="C91" s="79" t="s">
         <v>355</v>
       </c>
       <c r="D91" s="3">
@@ -4551,7 +4557,7 @@
       </c>
       <c r="H91" s="27"/>
       <c r="I91" s="3" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -4561,7 +4567,7 @@
       <c r="B92" s="27" t="s">
         <v>351</v>
       </c>
-      <c r="C92" s="80" t="s">
+      <c r="C92" s="79" t="s">
         <v>356</v>
       </c>
       <c r="D92" s="3">
@@ -4579,7 +4585,7 @@
       </c>
       <c r="H92" s="27"/>
       <c r="I92" s="3" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -4589,7 +4595,7 @@
       <c r="B93" s="27" t="s">
         <v>351</v>
       </c>
-      <c r="C93" s="80" t="s">
+      <c r="C93" s="79" t="s">
         <v>358</v>
       </c>
       <c r="D93" s="3">
@@ -4607,45 +4613,45 @@
       </c>
       <c r="H93" s="27"/>
       <c r="I93" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" s="65" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="65" t="s">
-        <v>469</v>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" s="64" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="64" t="s">
+        <v>466</v>
       </c>
       <c r="B94" s="27" t="s">
-        <v>470</v>
-      </c>
-      <c r="C94" s="81" t="s">
-        <v>471</v>
-      </c>
-      <c r="D94" s="65">
+        <v>467</v>
+      </c>
+      <c r="C94" s="80" t="s">
+        <v>468</v>
+      </c>
+      <c r="D94" s="64">
         <v>0</v>
       </c>
-      <c r="E94" s="66">
+      <c r="E94" s="65">
         <v>3670</v>
       </c>
       <c r="F94" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G94" s="65" t="s">
+      <c r="G94" s="64" t="s">
         <v>13</v>
       </c>
       <c r="H94" s="27"/>
-      <c r="I94" s="65" t="s">
-        <v>472</v>
+      <c r="I94" s="64" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="95" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="B95" s="89" t="s">
+      <c r="B95" s="88" t="s">
         <v>252</v>
       </c>
-      <c r="C95" s="90" t="s">
+      <c r="C95" s="89" t="s">
         <v>361</v>
       </c>
       <c r="D95" s="4">
@@ -4654,14 +4660,14 @@
       <c r="E95" s="20">
         <v>1</v>
       </c>
-      <c r="F95" s="91">
+      <c r="F95" s="90">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="G95" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H95" s="89"/>
+      <c r="H95" s="88"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
@@ -4702,7 +4708,7 @@
       <c r="B98" s="27" t="s">
         <v>351</v>
       </c>
-      <c r="C98" s="78" t="s">
+      <c r="C98" s="77" t="s">
         <v>394</v>
       </c>
       <c r="D98" s="3">
@@ -4712,7 +4718,7 @@
         <v>752</v>
       </c>
       <c r="F98" s="5">
-        <f t="shared" ref="F98:F103" si="6">D98*E98</f>
+        <f t="shared" ref="F98:F102" si="6">D98*E98</f>
         <v>752</v>
       </c>
       <c r="G98" s="3" t="s">
@@ -4726,7 +4732,7 @@
       <c r="A99" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="B99" s="89" t="s">
+      <c r="B99" s="88" t="s">
         <v>252</v>
       </c>
       <c r="C99" s="4" t="s">
@@ -4760,234 +4766,231 @@
         <v>1</v>
       </c>
       <c r="E100" s="5">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="F100" s="5">
         <f t="shared" si="6"/>
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="G100" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B101" s="27" t="s">
         <v>64</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D101" s="3">
         <v>1</v>
       </c>
       <c r="E101" s="5">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="F101" s="5">
         <f t="shared" si="6"/>
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>404</v>
+        <v>385</v>
       </c>
       <c r="B102" s="27" t="s">
         <v>64</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
       <c r="D102" s="3">
         <v>1</v>
       </c>
       <c r="E102" s="5">
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="F102" s="5">
         <f t="shared" si="6"/>
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="G102" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="B103" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D103" s="3">
-        <v>1</v>
-      </c>
-      <c r="E103" s="5">
-        <v>112</v>
-      </c>
-      <c r="F103" s="5">
-        <f t="shared" si="6"/>
-        <v>112</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I103" s="3" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="104" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A104" s="6" t="s">
+    <row r="103" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A103" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E104" s="9"/>
-      <c r="F104" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D104" s="3">
+        <v>1</v>
+      </c>
+      <c r="E104" s="5">
+        <v>3582</v>
+      </c>
+      <c r="F104" s="5">
+        <f t="shared" ref="F104:F116" si="7">E104*D104</f>
+        <v>3582</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>60</v>
+        <v>191</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>61</v>
+        <v>194</v>
       </c>
       <c r="D105" s="3">
         <v>1</v>
       </c>
       <c r="E105" s="5">
-        <v>3582</v>
+        <v>1630</v>
       </c>
       <c r="F105" s="5">
-        <f t="shared" ref="F105:F117" si="7">E105*D105</f>
-        <v>3582</v>
+        <f t="shared" si="7"/>
+        <v>1630</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>54</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D106" s="3">
         <v>1</v>
       </c>
       <c r="E106" s="5">
-        <v>1630</v>
+        <v>886</v>
       </c>
       <c r="F106" s="5">
         <f t="shared" si="7"/>
-        <v>1630</v>
+        <v>886</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>54</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D107" s="3">
         <v>1</v>
       </c>
       <c r="E107" s="5">
-        <v>886</v>
+        <v>163</v>
       </c>
       <c r="F107" s="5">
         <f t="shared" si="7"/>
-        <v>886</v>
+        <v>163</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>54</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>195</v>
+        <v>55</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D108" s="3">
         <v>1</v>
       </c>
       <c r="E108" s="5">
-        <v>163</v>
+        <v>11</v>
       </c>
       <c r="F108" s="5">
         <f t="shared" si="7"/>
-        <v>163</v>
+        <v>11</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I108" s="3" t="s">
-        <v>196</v>
-      </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>187</v>
+        <v>59</v>
       </c>
       <c r="D109" s="3">
         <v>1</v>
       </c>
       <c r="E109" s="5">
-        <v>11</v>
+        <v>520</v>
       </c>
       <c r="F109" s="5">
         <f t="shared" si="7"/>
-        <v>11</v>
+        <v>520</v>
       </c>
       <c r="G109" s="3" t="s">
         <v>54</v>
@@ -4995,125 +4998,125 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>58</v>
+        <v>198</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="D110" s="3">
         <v>1</v>
       </c>
       <c r="E110" s="5">
-        <v>520</v>
+        <v>193</v>
       </c>
       <c r="F110" s="5">
         <f t="shared" si="7"/>
-        <v>520</v>
+        <v>193</v>
       </c>
       <c r="G110" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D111" s="3">
-        <v>1</v>
-      </c>
-      <c r="E111" s="5">
-        <v>193</v>
-      </c>
-      <c r="F111" s="5">
+    <row r="111" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="31" t="s">
+        <v>317</v>
+      </c>
+      <c r="B111" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C111" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="D111" s="31">
+        <v>10</v>
+      </c>
+      <c r="E111" s="40">
+        <v>12</v>
+      </c>
+      <c r="F111" s="40">
         <f t="shared" si="7"/>
-        <v>193</v>
-      </c>
-      <c r="G111" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G111" s="31" t="s">
         <v>54</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="31" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B112" s="31" t="s">
         <v>64</v>
       </c>
       <c r="C112" s="31" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D112" s="31">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E112" s="40">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F112" s="40">
         <f t="shared" si="7"/>
-        <v>120</v>
+        <v>14</v>
       </c>
       <c r="G112" s="31" t="s">
         <v>54</v>
       </c>
       <c r="I112" s="31" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="31" t="s">
-        <v>319</v>
-      </c>
-      <c r="B113" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C113" s="31" t="s">
-        <v>320</v>
-      </c>
-      <c r="D113" s="31">
-        <v>1</v>
-      </c>
-      <c r="E113" s="40">
-        <v>14</v>
-      </c>
-      <c r="F113" s="40">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D113" s="3">
+        <v>4</v>
+      </c>
+      <c r="E113" s="5">
+        <v>15.25</v>
+      </c>
+      <c r="F113" s="5">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="G113" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="I113" s="31" t="s">
-        <v>321</v>
-      </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D114" s="3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E114" s="5">
-        <v>15.25</v>
+        <v>16.5</v>
       </c>
       <c r="F114" s="5">
         <f t="shared" si="7"/>
-        <v>61</v>
+        <v>165</v>
       </c>
       <c r="G114" s="31" t="s">
         <v>54</v>
@@ -5121,23 +5124,23 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D115" s="3">
         <v>10</v>
       </c>
       <c r="E115" s="5">
-        <v>16.5</v>
+        <v>24</v>
       </c>
       <c r="F115" s="5">
         <f t="shared" si="7"/>
-        <v>165</v>
+        <v>240</v>
       </c>
       <c r="G115" s="31" t="s">
         <v>54</v>
@@ -5145,179 +5148,176 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D116" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E116" s="5">
         <v>24</v>
       </c>
       <c r="F116" s="5">
         <f t="shared" si="7"/>
-        <v>240</v>
+        <v>144</v>
       </c>
       <c r="G116" s="31" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D117" s="3">
-        <v>6</v>
-      </c>
-      <c r="E117" s="5">
-        <v>24</v>
-      </c>
-      <c r="F117" s="5">
-        <f t="shared" si="7"/>
-        <v>144</v>
-      </c>
-      <c r="G117" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E118" s="40"/>
-      <c r="F118" s="40"/>
-    </row>
-    <row r="120" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A120" s="11"/>
-      <c r="B120" s="11"/>
-      <c r="C120" s="10"/>
-    </row>
-    <row r="121" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A121" s="8" t="s">
+    <row r="117" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E117" s="40"/>
+      <c r="F117" s="40"/>
+    </row>
+    <row r="119" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A119" s="11"/>
+      <c r="B119" s="11"/>
+      <c r="C119" s="10"/>
+    </row>
+    <row r="120" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A120" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F121" s="9"/>
+      <c r="F120" s="9"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D121" s="3">
+        <v>4</v>
+      </c>
+      <c r="E121" s="5">
+        <v>16.5</v>
+      </c>
+      <c r="F121" s="5">
+        <f t="shared" ref="F121:F136" si="8">E121*D121</f>
+        <v>66</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>117</v>
+        <v>64</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D122" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E122" s="5">
-        <v>16.5</v>
+        <v>85.1</v>
       </c>
       <c r="F122" s="5">
-        <f t="shared" ref="F122:F137" si="8">E122*D122</f>
-        <v>66</v>
-      </c>
-      <c r="I122" s="3" t="s">
-        <v>119</v>
+        <f t="shared" si="8"/>
+        <v>85.1</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D123" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E123" s="5">
-        <v>85.1</v>
+        <v>32</v>
       </c>
       <c r="F123" s="5">
         <f t="shared" si="8"/>
-        <v>85.1</v>
+        <v>64</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D124" s="3">
         <v>2</v>
       </c>
       <c r="E124" s="5">
-        <v>32</v>
+        <v>51.58</v>
       </c>
       <c r="F124" s="5">
         <f t="shared" si="8"/>
-        <v>64</v>
-      </c>
-      <c r="I124" s="3" t="s">
-        <v>134</v>
+        <v>103.16</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D125" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E125" s="5">
-        <v>51.58</v>
+        <v>60</v>
       </c>
       <c r="F125" s="5">
         <f t="shared" si="8"/>
-        <v>103.16</v>
+        <v>60</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D126" s="3">
         <v>1</v>
       </c>
       <c r="E126" s="5">
-        <v>60</v>
+        <v>136.47999999999999</v>
       </c>
       <c r="F126" s="5">
         <f t="shared" si="8"/>
-        <v>60</v>
-      </c>
-      <c r="I126" s="3" t="s">
-        <v>139</v>
+        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -5328,7 +5328,7 @@
         <v>64</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D127" s="3">
         <v>1</v>
@@ -5343,412 +5343,402 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D128" s="3">
         <v>1</v>
       </c>
       <c r="E128" s="5">
-        <v>136.47999999999999</v>
+        <v>60.95</v>
       </c>
       <c r="F128" s="5">
         <f t="shared" si="8"/>
-        <v>136.47999999999999</v>
+        <v>60.95</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D129" s="3">
         <v>1</v>
       </c>
       <c r="E129" s="5">
-        <v>60.95</v>
+        <v>119.416</v>
       </c>
       <c r="F129" s="5">
         <f t="shared" si="8"/>
-        <v>60.95</v>
+        <v>119.416</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D130" s="3">
         <v>1</v>
       </c>
       <c r="E130" s="5">
-        <v>119.416</v>
+        <v>105.8</v>
       </c>
       <c r="F130" s="5">
         <f t="shared" si="8"/>
-        <v>119.416</v>
+        <v>105.8</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D131" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E131" s="5">
-        <v>105.8</v>
+        <v>119.6</v>
       </c>
       <c r="F131" s="5">
         <f t="shared" si="8"/>
-        <v>105.8</v>
+        <v>239.2</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>149</v>
+        <v>327</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>150</v>
+        <v>328</v>
       </c>
       <c r="D132" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E132" s="5">
-        <v>119.6</v>
+        <v>100</v>
       </c>
       <c r="F132" s="5">
         <f t="shared" si="8"/>
-        <v>239.2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>327</v>
+        <v>151</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>328</v>
+        <v>152</v>
       </c>
       <c r="D133" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E133" s="5">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F133" s="5">
         <f t="shared" si="8"/>
-        <v>100</v>
+        <v>184</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D134" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E134" s="5">
-        <v>92</v>
+        <v>96.23</v>
       </c>
       <c r="F134" s="5">
         <f t="shared" si="8"/>
-        <v>184</v>
+        <v>96.23</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D135" s="3">
         <v>1</v>
       </c>
       <c r="E135" s="5">
-        <v>96.23</v>
+        <v>102.44</v>
       </c>
       <c r="F135" s="5">
         <f t="shared" si="8"/>
-        <v>96.23</v>
+        <v>102.44</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D136" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E136" s="5">
-        <v>102.44</v>
+        <v>28</v>
       </c>
       <c r="F136" s="5">
         <f t="shared" si="8"/>
-        <v>102.44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="C137" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D137" s="3">
-        <v>2</v>
-      </c>
-      <c r="E137" s="5">
-        <v>28</v>
-      </c>
-      <c r="F137" s="5">
-        <f t="shared" si="8"/>
-        <v>56</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C138" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D138" s="3">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C139" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D139" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A141" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+    </row>
+    <row r="142" spans="1:10" s="63" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="64"/>
+      <c r="B142" s="64" t="s">
+        <v>492</v>
+      </c>
+      <c r="C142" s="66" t="s">
+        <v>163</v>
+      </c>
+      <c r="D142" s="64">
+        <v>4</v>
+      </c>
+      <c r="E142" s="64">
+        <v>40</v>
+      </c>
+      <c r="F142" s="64">
+        <f>E142*D142</f>
         <v>160</v>
       </c>
-      <c r="D139" s="3">
-        <v>1</v>
-      </c>
-      <c r="I139" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C140" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D140" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A142" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B142" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="E142" s="9"/>
-      <c r="F142" s="9"/>
+      <c r="G142" s="64" t="s">
+        <v>490</v>
+      </c>
+      <c r="H142" s="64" t="s">
+        <v>491</v>
+      </c>
+      <c r="I142" s="64" t="s">
+        <v>489</v>
+      </c>
+      <c r="J142" s="66"/>
     </row>
     <row r="143" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="65"/>
-      <c r="B143" s="65" t="s">
-        <v>495</v>
-      </c>
-      <c r="C143" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="D143" s="65">
-        <v>4</v>
+      <c r="B143" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="C143" s="64" t="s">
+        <v>390</v>
+      </c>
+      <c r="D143" s="64">
+        <v>2</v>
       </c>
       <c r="E143" s="65">
-        <v>40</v>
+        <v>331</v>
       </c>
       <c r="F143" s="65">
         <f>E143*D143</f>
-        <v>160</v>
-      </c>
-      <c r="G143" s="65" t="s">
+        <v>662</v>
+      </c>
+      <c r="G143" s="64" t="s">
         <v>493</v>
       </c>
-      <c r="H143" s="65" t="s">
+    </row>
+    <row r="144" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="C144" s="64" t="s">
+        <v>313</v>
+      </c>
+      <c r="D144" s="64">
+        <v>4</v>
+      </c>
+      <c r="E144" s="65">
+        <v>25</v>
+      </c>
+      <c r="F144" s="65">
+        <f>E144*D144</f>
+        <v>100</v>
+      </c>
+      <c r="G144" s="64" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B145" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="C145" s="64" t="s">
+        <v>314</v>
+      </c>
+      <c r="D145" s="64">
+        <v>4</v>
+      </c>
+      <c r="E145" s="65">
+        <v>28</v>
+      </c>
+      <c r="F145" s="65">
+        <f>E145*D145</f>
+        <v>112</v>
+      </c>
+      <c r="G145" s="64" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B146" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="C146" s="64" t="s">
+        <v>315</v>
+      </c>
+      <c r="D146" s="64">
+        <v>6</v>
+      </c>
+      <c r="E146" s="65">
+        <v>121.5</v>
+      </c>
+      <c r="F146" s="65">
+        <f>E146*D146</f>
+        <v>729</v>
+      </c>
+      <c r="G146" s="64" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E149" s="76" t="s">
+        <v>527</v>
+      </c>
+      <c r="F149" s="92">
+        <f>SUM(F3:F147)</f>
+        <v>93299.255999999994</v>
+      </c>
+      <c r="G149" s="3" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A152" s="91" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A153" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="B153" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="I143" s="65" t="s">
-        <v>492</v>
-      </c>
-      <c r="J143" s="67"/>
-    </row>
-    <row r="144" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="65" t="s">
-        <v>165</v>
-      </c>
-      <c r="C144" s="65" t="s">
-        <v>390</v>
-      </c>
-      <c r="D144" s="65">
-        <v>2</v>
-      </c>
-      <c r="E144" s="66">
-        <v>331</v>
-      </c>
-      <c r="F144" s="66">
-        <f>E144*D144</f>
-        <v>662</v>
-      </c>
-      <c r="G144" s="65" t="s">
+      <c r="C153" s="4" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="145" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="65" t="s">
-        <v>165</v>
-      </c>
-      <c r="C145" s="65" t="s">
-        <v>313</v>
-      </c>
-      <c r="D145" s="65">
-        <v>4</v>
-      </c>
-      <c r="E145" s="66">
-        <v>25</v>
-      </c>
-      <c r="F145" s="66">
-        <f>E145*D145</f>
-        <v>100</v>
-      </c>
-      <c r="G145" s="65" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="65" t="s">
-        <v>165</v>
-      </c>
-      <c r="C146" s="65" t="s">
-        <v>314</v>
-      </c>
-      <c r="D146" s="65">
-        <v>4</v>
-      </c>
-      <c r="E146" s="66">
-        <v>28</v>
-      </c>
-      <c r="F146" s="66">
-        <f>E146*D146</f>
-        <v>112</v>
-      </c>
-      <c r="G146" s="65" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="65" t="s">
-        <v>165</v>
-      </c>
-      <c r="C147" s="65" t="s">
-        <v>315</v>
-      </c>
-      <c r="D147" s="65">
-        <v>6</v>
-      </c>
-      <c r="E147" s="66">
-        <v>121.5</v>
-      </c>
-      <c r="F147" s="66">
-        <f>E147*D147</f>
-        <v>729</v>
-      </c>
-      <c r="G147" s="65" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E150" s="77" t="s">
-        <v>530</v>
-      </c>
-      <c r="F150" s="93">
-        <f>SUM(F3:F148)</f>
-        <v>93335.255999999994</v>
-      </c>
-      <c r="G150" s="3" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A153" s="92" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A154" s="4" t="s">
-        <v>501</v>
-      </c>
-      <c r="B154" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="C154" s="4" t="s">
-        <v>499</v>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="B154" s="3">
+        <v>1</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>510</v>
+        <v>495</v>
       </c>
       <c r="B155" s="3">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B156" s="3">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -5758,103 +5748,103 @@
       <c r="B157" s="3">
         <v>2</v>
       </c>
-      <c r="C157" s="3" t="s">
-        <v>502</v>
+      <c r="C157" s="64" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B158" s="3">
         <v>2</v>
       </c>
-      <c r="C158" s="65" t="s">
+      <c r="C158" s="3" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A161" s="91" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A162" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="C162" s="4" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="B163" s="3">
+        <v>2</v>
+      </c>
+      <c r="C163" s="3" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A159" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="B159" s="3">
-        <v>2</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A162" s="92" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A163" s="4" t="s">
-        <v>501</v>
-      </c>
-      <c r="B163" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="C163" s="4" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
-        <v>516</v>
+        <v>360</v>
       </c>
       <c r="B164" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>360</v>
+        <v>396</v>
       </c>
       <c r="B165" s="3">
+        <v>1</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A168" s="91" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A169" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="64" t="s">
+        <v>518</v>
+      </c>
+      <c r="B170" s="3">
         <v>5</v>
       </c>
-      <c r="C165" s="3" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="B166" s="3">
-        <v>1</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A169" s="92" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A170" s="4" t="s">
-        <v>501</v>
-      </c>
-      <c r="B170" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="C170" s="4" t="s">
-        <v>499</v>
+      <c r="C170" s="3" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="65" t="s">
-        <v>521</v>
+      <c r="A171" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="B171" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C171" s="3" t="s">
         <v>523</v>
@@ -5862,24 +5852,13 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B172" s="3">
-        <v>3</v>
+        <v>524</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>324</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" s="3" t="s">
-        <v>527</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>
@@ -5953,102 +5932,102 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:9" s="58" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="58">
+    <row r="3" spans="1:9" s="57" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="57">
         <v>1008062</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="57" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="58">
-        <v>1</v>
-      </c>
-      <c r="E3" s="71">
+      <c r="D3" s="57">
+        <v>1</v>
+      </c>
+      <c r="E3" s="70">
         <v>7400</v>
       </c>
-      <c r="F3" s="59">
+      <c r="F3" s="58">
         <f>E3*D3</f>
         <v>7400</v>
       </c>
-      <c r="I3" s="58" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="58" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B4" s="58" t="s">
+      <c r="I3" s="57" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="57" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B4" s="57" t="s">
         <v>169</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="D4" s="58">
-        <v>1</v>
-      </c>
-      <c r="E4" s="71">
+      <c r="D4" s="57">
+        <v>1</v>
+      </c>
+      <c r="E4" s="70">
         <v>20000</v>
       </c>
-      <c r="F4" s="59">
+      <c r="F4" s="58">
         <f>D4*E4</f>
         <v>20000</v>
       </c>
-      <c r="I4" s="58" t="s">
+      <c r="I4" s="57" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B5" s="47" t="s">
-        <v>430</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>431</v>
-      </c>
-      <c r="D5" s="47">
-        <v>1</v>
-      </c>
-      <c r="E5" s="47">
+    <row r="5" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B5" s="46" t="s">
+        <v>427</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>428</v>
+      </c>
+      <c r="D5" s="46">
+        <v>1</v>
+      </c>
+      <c r="E5" s="46">
         <v>50000</v>
       </c>
-      <c r="F5" s="47">
+      <c r="F5" s="46">
         <v>50000</v>
       </c>
-      <c r="I5" s="47" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+      <c r="I5" s="46" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B8" s="47" t="s">
+    <row r="8" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B8" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="46" t="s">
         <v>179</v>
       </c>
-      <c r="D8" s="47">
-        <v>1</v>
-      </c>
-      <c r="E8" s="50">
+      <c r="D8" s="46">
+        <v>1</v>
+      </c>
+      <c r="E8" s="49">
         <v>25000</v>
       </c>
-      <c r="F8" s="50">
+      <c r="F8" s="49">
         <f>D8*E8</f>
         <v>25000</v>
       </c>
-      <c r="I8" s="47" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+      <c r="I8" s="46" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" s="25" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>393</v>
@@ -6056,518 +6035,518 @@
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
     </row>
-    <row r="12" spans="1:9" s="47" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="47" t="s">
+    <row r="12" spans="1:9" s="46" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="46" t="s">
         <v>374</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="47" t="s">
         <v>351</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="48" t="s">
         <v>373</v>
       </c>
-      <c r="D12" s="47">
-        <v>1</v>
-      </c>
-      <c r="E12" s="50">
+      <c r="D12" s="46">
+        <v>1</v>
+      </c>
+      <c r="E12" s="49">
         <v>525</v>
       </c>
-      <c r="F12" s="50">
+      <c r="F12" s="49">
         <f>D12*E12</f>
         <v>525</v>
       </c>
-      <c r="G12" s="47" t="s">
+      <c r="G12" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="47" t="s">
-        <v>413</v>
-      </c>
-      <c r="I12" s="47" t="s">
+      <c r="H12" s="46" t="s">
+        <v>410</v>
+      </c>
+      <c r="I12" s="46" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="47" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="47" t="s">
+    <row r="13" spans="1:9" s="46" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="46" t="s">
         <v>377</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="47" t="s">
         <v>351</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="48" t="s">
         <v>376</v>
       </c>
-      <c r="D13" s="47">
-        <v>1</v>
-      </c>
-      <c r="E13" s="50">
+      <c r="D13" s="46">
+        <v>1</v>
+      </c>
+      <c r="E13" s="49">
         <v>214</v>
       </c>
-      <c r="F13" s="50">
+      <c r="F13" s="49">
         <f t="shared" ref="F13:F15" si="0">D13*E13</f>
         <v>214</v>
       </c>
-      <c r="G13" s="47" t="s">
+      <c r="G13" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="47" t="s">
-        <v>413</v>
-      </c>
-      <c r="I13" s="47" t="s">
+      <c r="H13" s="46" t="s">
+        <v>410</v>
+      </c>
+      <c r="I13" s="46" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+    <row r="14" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="s">
         <v>379</v>
       </c>
-      <c r="B14" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="47" t="s">
+      <c r="B14" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="46" t="s">
         <v>378</v>
       </c>
-      <c r="D14" s="47">
-        <v>1</v>
-      </c>
-      <c r="E14" s="50">
+      <c r="D14" s="46">
+        <v>1</v>
+      </c>
+      <c r="E14" s="49">
         <v>23</v>
       </c>
-      <c r="F14" s="50">
+      <c r="F14" s="49">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="G14" s="47" t="s">
+      <c r="G14" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="47" t="s">
-        <v>413</v>
-      </c>
-      <c r="I14" s="47" t="s">
+      <c r="H14" s="46" t="s">
+        <v>410</v>
+      </c>
+      <c r="I14" s="46" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+    <row r="15" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="46" t="s">
         <v>382</v>
       </c>
-      <c r="B15" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="47" t="s">
+      <c r="B15" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="46" t="s">
         <v>381</v>
       </c>
-      <c r="D15" s="47">
-        <v>1</v>
-      </c>
-      <c r="E15" s="50">
+      <c r="D15" s="46">
+        <v>1</v>
+      </c>
+      <c r="E15" s="49">
         <v>23</v>
       </c>
-      <c r="F15" s="50">
+      <c r="F15" s="49">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="G15" s="47" t="s">
+      <c r="G15" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="47" t="s">
-        <v>413</v>
-      </c>
-      <c r="I15" s="47" t="s">
+      <c r="H15" s="46" t="s">
+        <v>410</v>
+      </c>
+      <c r="I15" s="46" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+    <row r="16" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="50" t="s">
         <v>271</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="47" t="s">
         <v>270</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="50" t="s">
         <v>272</v>
       </c>
-      <c r="D16" s="48">
-        <v>1</v>
-      </c>
-      <c r="E16" s="52">
+      <c r="D16" s="47">
+        <v>1</v>
+      </c>
+      <c r="E16" s="51">
         <v>2</v>
       </c>
-      <c r="F16" s="53">
+      <c r="F16" s="52">
         <f>D16*E16</f>
         <v>2</v>
       </c>
-      <c r="G16" s="47" t="s">
+      <c r="G16" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="48" t="s">
-        <v>414</v>
-      </c>
-      <c r="I16" s="48" t="s">
-        <v>412</v>
+      <c r="H16" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="I16" s="47" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:10" s="65" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="65" t="s">
+    <row r="19" spans="1:10" s="64" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="64" t="s">
         <v>298</v>
       </c>
-      <c r="B19" s="65" t="s">
+      <c r="B19" s="64" t="s">
         <v>297</v>
       </c>
-      <c r="C19" s="65" t="s">
+      <c r="C19" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="65">
-        <v>1</v>
-      </c>
-      <c r="E19" s="66">
+      <c r="D19" s="64">
+        <v>1</v>
+      </c>
+      <c r="E19" s="65">
         <v>250</v>
       </c>
-      <c r="F19" s="66">
+      <c r="F19" s="65">
         <f>E19*D19</f>
         <v>250</v>
       </c>
-      <c r="G19" s="65" t="s">
+      <c r="G19" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="65" t="s">
+      <c r="H19" s="64" t="s">
         <v>15</v>
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" s="65" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="65" t="s">
+    <row r="20" spans="1:10" s="64" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="64" t="s">
         <v>299</v>
       </c>
-      <c r="B20" s="65" t="s">
+      <c r="B20" s="64" t="s">
         <v>297</v>
       </c>
-      <c r="C20" s="65" t="s">
+      <c r="C20" s="64" t="s">
         <v>303</v>
       </c>
-      <c r="D20" s="65">
-        <v>1</v>
-      </c>
-      <c r="E20" s="66">
+      <c r="D20" s="64">
+        <v>1</v>
+      </c>
+      <c r="E20" s="65">
         <v>13</v>
       </c>
-      <c r="F20" s="66">
+      <c r="F20" s="65">
         <f>E20*D20</f>
         <v>13</v>
       </c>
-      <c r="G20" s="65" t="s">
+      <c r="G20" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="65" t="s">
+      <c r="H20" s="64" t="s">
         <v>15</v>
       </c>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" s="65" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="65" t="s">
+    <row r="21" spans="1:10" s="64" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="64" t="s">
         <v>301</v>
       </c>
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="64" t="s">
         <v>297</v>
       </c>
-      <c r="C21" s="65" t="s">
+      <c r="C21" s="64" t="s">
         <v>300</v>
       </c>
-      <c r="D21" s="65">
-        <v>1</v>
-      </c>
-      <c r="E21" s="66">
+      <c r="D21" s="64">
+        <v>1</v>
+      </c>
+      <c r="E21" s="65">
         <v>43</v>
       </c>
-      <c r="F21" s="66">
+      <c r="F21" s="65">
         <f>E21*D21</f>
         <v>43</v>
       </c>
-      <c r="G21" s="65" t="s">
+      <c r="G21" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="65" t="s">
+      <c r="H21" s="64" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="65" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="65" t="s">
+    <row r="22" spans="1:10" s="64" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="64" t="s">
         <v>312</v>
       </c>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="64" t="s">
         <v>252</v>
       </c>
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="64" t="s">
         <v>302</v>
       </c>
-      <c r="D22" s="65">
-        <v>1</v>
-      </c>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
+      <c r="D22" s="64">
+        <v>1</v>
+      </c>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
       <c r="I22" s="31" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:10" s="56" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="55" t="s">
-        <v>411</v>
-      </c>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-    </row>
-    <row r="26" spans="1:10" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="51" t="s">
+    <row r="25" spans="1:10" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="54" t="s">
+        <v>408</v>
+      </c>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+    </row>
+    <row r="26" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="50" t="s">
         <v>340</v>
       </c>
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="47" t="s">
         <v>252</v>
       </c>
-      <c r="C26" s="51" t="s">
+      <c r="C26" s="50" t="s">
         <v>341</v>
       </c>
-      <c r="D26" s="48">
+      <c r="D26" s="47">
         <v>2</v>
       </c>
-      <c r="E26" s="52">
+      <c r="E26" s="51">
         <v>5</v>
       </c>
-      <c r="F26" s="53">
+      <c r="F26" s="52">
         <f t="shared" ref="F26:F33" si="1">E26*D26</f>
         <v>10</v>
       </c>
-      <c r="G26" s="48" t="s">
+      <c r="G26" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="H26" s="48" t="s">
-        <v>409</v>
-      </c>
-      <c r="I26" s="48" t="s">
+      <c r="H26" s="47" t="s">
+        <v>406</v>
+      </c>
+      <c r="I26" s="47" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="51" t="s">
+    <row r="27" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="50" t="s">
         <v>343</v>
       </c>
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="47" t="s">
         <v>297</v>
       </c>
-      <c r="C27" s="51" t="s">
+      <c r="C27" s="50" t="s">
         <v>347</v>
       </c>
-      <c r="D27" s="48">
+      <c r="D27" s="47">
         <v>2</v>
       </c>
-      <c r="E27" s="52">
+      <c r="E27" s="51">
         <v>62</v>
       </c>
-      <c r="F27" s="53">
+      <c r="F27" s="52">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-      <c r="G27" s="48" t="s">
+      <c r="G27" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="H27" s="48" t="s">
-        <v>409</v>
-      </c>
-      <c r="I27" s="48" t="s">
+      <c r="H27" s="47" t="s">
+        <v>406</v>
+      </c>
+      <c r="I27" s="47" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="51" t="s">
+    <row r="28" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="50" t="s">
         <v>324</v>
       </c>
-      <c r="B28" s="48" t="s">
+      <c r="B28" s="47" t="s">
         <v>364</v>
       </c>
-      <c r="C28" s="51" t="s">
+      <c r="C28" s="50" t="s">
         <v>365</v>
       </c>
-      <c r="D28" s="48">
+      <c r="D28" s="47">
         <v>8</v>
       </c>
-      <c r="E28" s="52">
-        <v>1</v>
-      </c>
-      <c r="F28" s="53">
+      <c r="E28" s="51">
+        <v>1</v>
+      </c>
+      <c r="F28" s="52">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G28" s="48" t="s">
+      <c r="G28" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="H28" s="48" t="s">
-        <v>409</v>
-      </c>
-      <c r="I28" s="48" t="s">
+      <c r="H28" s="47" t="s">
+        <v>406</v>
+      </c>
+      <c r="I28" s="47" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="51" t="s">
+    <row r="29" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="50" t="s">
         <v>368</v>
       </c>
-      <c r="B29" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="51" t="s">
+      <c r="B29" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="50" t="s">
         <v>367</v>
       </c>
-      <c r="D29" s="48">
+      <c r="D29" s="47">
         <v>6</v>
       </c>
-      <c r="E29" s="52">
+      <c r="E29" s="51">
         <v>6</v>
       </c>
-      <c r="F29" s="53">
+      <c r="F29" s="52">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="G29" s="48" t="s">
+      <c r="G29" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="H29" s="48" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
+      <c r="H29" s="47" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="50" t="s">
         <v>369</v>
       </c>
-      <c r="B30" s="48" t="s">
+      <c r="B30" s="47" t="s">
         <v>252</v>
       </c>
-      <c r="C30" s="51" t="s">
+      <c r="C30" s="50" t="s">
         <v>370</v>
       </c>
-      <c r="D30" s="48">
+      <c r="D30" s="47">
         <v>2</v>
       </c>
-      <c r="E30" s="52">
-        <v>1</v>
-      </c>
-      <c r="F30" s="53">
+      <c r="E30" s="51">
+        <v>1</v>
+      </c>
+      <c r="F30" s="52">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G30" s="48" t="s">
+      <c r="G30" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="48" t="s">
-        <v>409</v>
-      </c>
-      <c r="I30" s="48" t="s">
+      <c r="H30" s="47" t="s">
+        <v>406</v>
+      </c>
+      <c r="I30" s="47" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="s">
+    <row r="31" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="47" t="s">
         <v>297</v>
       </c>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="50" t="s">
         <v>344</v>
       </c>
-      <c r="D31" s="48">
-        <v>1</v>
-      </c>
-      <c r="E31" s="52">
+      <c r="D31" s="47">
+        <v>1</v>
+      </c>
+      <c r="E31" s="51">
         <v>2</v>
       </c>
-      <c r="F31" s="53">
+      <c r="F31" s="52">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G31" s="48" t="s">
+      <c r="G31" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="H31" s="48" t="s">
-        <v>409</v>
-      </c>
-      <c r="I31" s="48" t="s">
+      <c r="H31" s="47" t="s">
+        <v>406</v>
+      </c>
+      <c r="I31" s="47" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="54" t="s">
+    <row r="32" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="47" t="s">
         <v>297</v>
       </c>
-      <c r="C32" s="51" t="s">
+      <c r="C32" s="50" t="s">
         <v>349</v>
       </c>
-      <c r="D32" s="48">
-        <v>1</v>
-      </c>
-      <c r="E32" s="52">
+      <c r="D32" s="47">
+        <v>1</v>
+      </c>
+      <c r="E32" s="51">
         <v>15</v>
       </c>
-      <c r="F32" s="53">
+      <c r="F32" s="52">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G32" s="48" t="s">
+      <c r="G32" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="H32" s="48" t="s">
-        <v>409</v>
-      </c>
-      <c r="I32" s="48" t="s">
+      <c r="H32" s="47" t="s">
+        <v>406</v>
+      </c>
+      <c r="I32" s="47" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="48" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="51" t="s">
+    <row r="33" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="50" t="s">
         <v>245</v>
       </c>
-      <c r="B33" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="51" t="s">
+      <c r="B33" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="50" t="s">
         <v>246</v>
       </c>
-      <c r="D33" s="48">
+      <c r="D33" s="47">
         <v>2</v>
       </c>
-      <c r="E33" s="52">
+      <c r="E33" s="51">
         <v>25</v>
       </c>
-      <c r="F33" s="53">
+      <c r="F33" s="52">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="G33" s="48" t="s">
+      <c r="G33" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="H33" s="48" t="s">
-        <v>409</v>
+      <c r="H33" s="47" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -6577,31 +6556,31 @@
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
     </row>
-    <row r="38" spans="1:9" s="58" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="58" t="s">
+    <row r="38" spans="1:9" s="57" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="58" t="s">
+      <c r="B38" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="58" t="s">
+      <c r="C38" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="58">
-        <v>1</v>
-      </c>
-      <c r="E38" s="59">
+      <c r="D38" s="57">
+        <v>1</v>
+      </c>
+      <c r="E38" s="58">
         <v>2800</v>
       </c>
-      <c r="F38" s="59">
+      <c r="F38" s="58">
         <f>E38*D38</f>
         <v>2800</v>
       </c>
-      <c r="G38" s="58" t="s">
+      <c r="G38" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="I38" s="58" t="s">
-        <v>415</v>
+      <c r="I38" s="57" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -6612,602 +6591,602 @@
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
     </row>
-    <row r="43" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="47" t="s">
+    <row r="43" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="B43" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C43" s="47" t="s">
+      <c r="B43" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="D43" s="47">
-        <v>1</v>
-      </c>
-      <c r="E43" s="50">
+      <c r="D43" s="46">
+        <v>1</v>
+      </c>
+      <c r="E43" s="49">
         <v>488</v>
       </c>
-      <c r="F43" s="50">
+      <c r="F43" s="49">
         <f t="shared" ref="F43:F64" si="2">E43*D43</f>
         <v>488</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="47" t="s">
+    <row r="44" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A44" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="47" t="s">
+      <c r="B44" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="47">
-        <v>1</v>
-      </c>
-      <c r="E44" s="50">
+      <c r="D44" s="46">
+        <v>1</v>
+      </c>
+      <c r="E44" s="49">
         <v>184</v>
       </c>
-      <c r="F44" s="50">
+      <c r="F44" s="49">
         <f t="shared" si="2"/>
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="47" t="s">
+    <row r="45" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="47" t="s">
+      <c r="B45" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="47">
-        <v>1</v>
-      </c>
-      <c r="E45" s="50">
+      <c r="D45" s="46">
+        <v>1</v>
+      </c>
+      <c r="E45" s="49">
         <v>76</v>
       </c>
-      <c r="F45" s="50">
+      <c r="F45" s="49">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="47" t="s">
+    <row r="46" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A46" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C46" s="47" t="s">
+      <c r="B46" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="47">
-        <v>1</v>
-      </c>
-      <c r="E46" s="50">
+      <c r="D46" s="46">
+        <v>1</v>
+      </c>
+      <c r="E46" s="49">
         <v>184</v>
       </c>
-      <c r="F46" s="50">
+      <c r="F46" s="49">
         <f t="shared" si="2"/>
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="47" t="s">
+    <row r="47" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="B47" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="47" t="s">
+      <c r="B47" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="D47" s="47">
-        <v>1</v>
-      </c>
-      <c r="E47" s="50">
+      <c r="D47" s="46">
+        <v>1</v>
+      </c>
+      <c r="E47" s="49">
         <v>94.180155999999997</v>
       </c>
-      <c r="F47" s="50">
+      <c r="F47" s="49">
         <f t="shared" si="2"/>
         <v>94.180155999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="47" t="s">
+    <row r="48" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A48" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" s="47" t="s">
+      <c r="B48" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="47">
-        <v>1</v>
-      </c>
-      <c r="E48" s="50">
+      <c r="D48" s="46">
+        <v>1</v>
+      </c>
+      <c r="E48" s="49">
         <v>36.799999999999997</v>
       </c>
-      <c r="F48" s="50">
+      <c r="F48" s="49">
         <f t="shared" si="2"/>
         <v>36.799999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A49" s="47" t="s">
+    <row r="49" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A49" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="B49" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" s="47" t="s">
+      <c r="B49" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="D49" s="47">
+      <c r="D49" s="46">
         <v>2</v>
       </c>
-      <c r="E49" s="50">
+      <c r="E49" s="49">
         <v>21.21</v>
       </c>
-      <c r="F49" s="50">
+      <c r="F49" s="49">
         <f t="shared" si="2"/>
         <v>42.42</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="47" t="s">
+    <row r="50" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A50" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="B50" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C50" s="47" t="s">
+      <c r="B50" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="47">
-        <v>1</v>
-      </c>
-      <c r="E50" s="50">
+      <c r="D50" s="46">
+        <v>1</v>
+      </c>
+      <c r="E50" s="49">
         <v>304.75</v>
       </c>
-      <c r="F50" s="50">
+      <c r="F50" s="49">
         <f t="shared" si="2"/>
         <v>304.75</v>
       </c>
-      <c r="I50" s="47" t="s">
+      <c r="I50" s="46" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A51" s="47" t="s">
+    <row r="51" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A51" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C51" s="47" t="s">
+      <c r="B51" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="47">
-        <v>1</v>
-      </c>
-      <c r="E51" s="50">
+      <c r="D51" s="46">
+        <v>1</v>
+      </c>
+      <c r="E51" s="49">
         <v>148.21</v>
       </c>
-      <c r="F51" s="50">
+      <c r="F51" s="49">
         <f t="shared" si="2"/>
         <v>148.21</v>
       </c>
-      <c r="I51" s="47" t="s">
+      <c r="I51" s="46" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="47" t="s">
+    <row r="52" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A52" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B52" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C52" s="47" t="s">
+      <c r="B52" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="D52" s="47">
-        <v>1</v>
-      </c>
-      <c r="E52" s="50">
+      <c r="D52" s="46">
+        <v>1</v>
+      </c>
+      <c r="E52" s="49">
         <v>348.45</v>
       </c>
-      <c r="F52" s="50">
+      <c r="F52" s="49">
         <f t="shared" si="2"/>
         <v>348.45</v>
       </c>
-      <c r="I52" s="47" t="s">
+      <c r="I52" s="46" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="47" t="s">
+    <row r="53" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A53" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="B53" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C53" s="47" t="s">
+      <c r="B53" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="D53" s="47">
-        <v>1</v>
-      </c>
-      <c r="E53" s="50">
+      <c r="D53" s="46">
+        <v>1</v>
+      </c>
+      <c r="E53" s="49">
         <v>60.95</v>
       </c>
-      <c r="F53" s="50">
+      <c r="F53" s="49">
         <f t="shared" si="2"/>
         <v>60.95</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="47" t="s">
+    <row r="54" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A54" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" s="47" t="s">
+      <c r="B54" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="D54" s="47">
-        <v>1</v>
-      </c>
-      <c r="E54" s="50">
+      <c r="D54" s="46">
+        <v>1</v>
+      </c>
+      <c r="E54" s="49">
         <v>34.5</v>
       </c>
-      <c r="F54" s="50">
+      <c r="F54" s="49">
         <f t="shared" si="2"/>
         <v>34.5</v>
       </c>
-      <c r="I54" s="47" t="s">
+      <c r="I54" s="46" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="47" t="s">
+    <row r="55" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A55" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C55" s="47" t="s">
+      <c r="B55" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="47">
-        <v>1</v>
-      </c>
-      <c r="E55" s="50">
+      <c r="D55" s="46">
+        <v>1</v>
+      </c>
+      <c r="E55" s="49">
         <v>51.45</v>
       </c>
-      <c r="F55" s="50">
+      <c r="F55" s="49">
         <f t="shared" si="2"/>
         <v>51.45</v>
       </c>
-      <c r="I55" s="47" t="s">
+      <c r="I55" s="46" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="47" t="s">
+    <row r="56" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A56" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C56" s="47" t="s">
+      <c r="B56" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="D56" s="47">
+      <c r="D56" s="46">
         <v>2</v>
       </c>
-      <c r="E56" s="50">
+      <c r="E56" s="49">
         <v>13.8</v>
       </c>
-      <c r="F56" s="50">
+      <c r="F56" s="49">
         <f t="shared" si="2"/>
         <v>27.6</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A57" s="47" t="s">
+    <row r="57" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A57" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C57" s="47" t="s">
+      <c r="B57" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="D57" s="47">
-        <v>1</v>
-      </c>
-      <c r="E57" s="50">
+      <c r="D57" s="46">
+        <v>1</v>
+      </c>
+      <c r="E57" s="49">
         <v>19.09</v>
       </c>
-      <c r="F57" s="50">
+      <c r="F57" s="49">
         <f t="shared" si="2"/>
         <v>19.09</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A58" s="47" t="s">
+    <row r="58" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A58" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="47" t="s">
+      <c r="B58" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="D58" s="47">
+      <c r="D58" s="46">
         <v>2</v>
       </c>
-      <c r="E58" s="50">
+      <c r="E58" s="49">
         <v>40.51</v>
       </c>
-      <c r="F58" s="50">
+      <c r="F58" s="49">
         <f t="shared" si="2"/>
         <v>81.02</v>
       </c>
-      <c r="I58" s="47" t="s">
+      <c r="I58" s="46" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A59" s="47" t="s">
+    <row r="59" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A59" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="B59" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C59" s="47" t="s">
+      <c r="B59" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="D59" s="47">
+      <c r="D59" s="46">
         <v>2</v>
       </c>
-      <c r="E59" s="50">
+      <c r="E59" s="49">
         <v>83.598116000000005</v>
       </c>
-      <c r="F59" s="50">
+      <c r="F59" s="49">
         <f t="shared" si="2"/>
         <v>167.19623200000001</v>
       </c>
-      <c r="I59" s="47" t="s">
+      <c r="I59" s="46" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="47" t="s">
+    <row r="60" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A60" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="B60" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C60" s="47" t="s">
+      <c r="B60" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="D60" s="47">
+      <c r="D60" s="46">
         <v>4</v>
       </c>
-      <c r="E60" s="50">
+      <c r="E60" s="49">
         <v>70.103999999999999</v>
       </c>
-      <c r="F60" s="50">
+      <c r="F60" s="49">
         <f t="shared" si="2"/>
         <v>280.416</v>
       </c>
-      <c r="I60" s="47" t="s">
+      <c r="I60" s="46" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A61" s="47" t="s">
+    <row r="61" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A61" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="B61" s="47" t="s">
+      <c r="B61" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="C61" s="47" t="s">
+      <c r="C61" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="D61" s="47">
+      <c r="D61" s="46">
         <v>2</v>
       </c>
-      <c r="E61" s="50">
+      <c r="E61" s="49">
         <v>28.75</v>
       </c>
-      <c r="F61" s="50">
+      <c r="F61" s="49">
         <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
-      <c r="I61" s="60" t="s">
+      <c r="I61" s="59" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A62" s="47" t="s">
+    <row r="62" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A62" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="B62" s="47" t="s">
+      <c r="B62" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="C62" s="47" t="s">
+      <c r="C62" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="D62" s="47">
+      <c r="D62" s="46">
         <v>2</v>
       </c>
-      <c r="E62" s="50">
+      <c r="E62" s="49">
         <v>38.872799999999998</v>
       </c>
-      <c r="F62" s="50">
+      <c r="F62" s="49">
         <f t="shared" si="2"/>
         <v>77.745599999999996</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B63" s="47" t="s">
+    <row r="63" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B63" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="C63" s="47" t="s">
+      <c r="C63" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="D63" s="47">
-        <v>1</v>
-      </c>
-      <c r="E63" s="50">
+      <c r="D63" s="46">
+        <v>1</v>
+      </c>
+      <c r="E63" s="49">
         <v>205</v>
       </c>
-      <c r="F63" s="50">
+      <c r="F63" s="49">
         <f t="shared" si="2"/>
         <v>205</v>
       </c>
-      <c r="I63" s="47" t="s">
+      <c r="I63" s="46" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B64" s="47" t="s">
+    <row r="64" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B64" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="C64" s="47" t="s">
+      <c r="C64" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="D64" s="47">
+      <c r="D64" s="46">
         <v>2</v>
       </c>
-      <c r="E64" s="50">
+      <c r="E64" s="49">
         <v>12</v>
       </c>
-      <c r="F64" s="50">
+      <c r="F64" s="49">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="I64" s="47" t="s">
+      <c r="I64" s="46" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F66" s="9"/>
     </row>
-    <row r="67" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="47" t="s">
+    <row r="67" spans="1:10" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A67" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="B67" s="47" t="s">
+      <c r="B67" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="C67" s="47" t="s">
+      <c r="C67" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="D67" s="47">
+      <c r="D67" s="46">
         <v>2</v>
       </c>
-      <c r="E67" s="50">
+      <c r="E67" s="49">
         <v>140</v>
       </c>
-      <c r="F67" s="50">
+      <c r="F67" s="49">
         <f>E67*D67</f>
         <v>280</v>
       </c>
-      <c r="I67" s="47" t="s">
-        <v>421</v>
+      <c r="I67" s="46" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>417</v>
-      </c>
-      <c r="B68" s="61" t="s">
-        <v>418</v>
-      </c>
-      <c r="C68" s="61" t="s">
-        <v>419</v>
-      </c>
-      <c r="D68" s="61">
+        <v>414</v>
+      </c>
+      <c r="B68" s="60" t="s">
+        <v>415</v>
+      </c>
+      <c r="C68" s="60" t="s">
+        <v>416</v>
+      </c>
+      <c r="D68" s="60">
         <v>2</v>
       </c>
-      <c r="E68" s="62">
+      <c r="E68" s="61">
         <v>84</v>
       </c>
       <c r="F68">
         <f>D68*E68</f>
         <v>168</v>
       </c>
-      <c r="I68" s="61" t="s">
-        <v>420</v>
+      <c r="I68" s="60" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>424</v>
-      </c>
-      <c r="B69" s="61" t="s">
-        <v>423</v>
-      </c>
-      <c r="C69" s="61" t="s">
-        <v>422</v>
-      </c>
-      <c r="D69" s="61">
-        <v>1</v>
-      </c>
-      <c r="E69" s="62">
+        <v>421</v>
+      </c>
+      <c r="B69" s="60" t="s">
+        <v>420</v>
+      </c>
+      <c r="C69" s="60" t="s">
+        <v>419</v>
+      </c>
+      <c r="D69" s="60">
+        <v>1</v>
+      </c>
+      <c r="E69" s="61">
         <v>54</v>
       </c>
       <c r="F69">
         <f>D69*E69</f>
         <v>54</v>
       </c>
-      <c r="I69" s="61" t="s">
-        <v>425</v>
+      <c r="I69" s="60" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="F71" s="9"/>
     </row>
-    <row r="72" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A72" s="47" t="s">
-        <v>427</v>
-      </c>
-      <c r="C72" s="63"/>
-      <c r="E72" s="50"/>
-      <c r="F72" s="50"/>
-      <c r="J72" s="63"/>
-    </row>
-    <row r="73" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="47" t="s">
-        <v>428</v>
-      </c>
-      <c r="C73" s="63"/>
-      <c r="E73" s="50"/>
-      <c r="F73" s="50"/>
-      <c r="J73" s="63"/>
-    </row>
-    <row r="74" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="C74" s="63"/>
-      <c r="E74" s="50"/>
-      <c r="F74" s="50"/>
-      <c r="J74" s="63"/>
+    <row r="72" spans="1:10" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A72" s="46" t="s">
+        <v>424</v>
+      </c>
+      <c r="C72" s="62"/>
+      <c r="E72" s="49"/>
+      <c r="F72" s="49"/>
+      <c r="J72" s="62"/>
+    </row>
+    <row r="73" spans="1:10" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A73" s="46" t="s">
+        <v>425</v>
+      </c>
+      <c r="C73" s="62"/>
+      <c r="E73" s="49"/>
+      <c r="F73" s="49"/>
+      <c r="J73" s="62"/>
+    </row>
+    <row r="74" spans="1:10" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C74" s="62"/>
+      <c r="E74" s="49"/>
+      <c r="F74" s="49"/>
+      <c r="J74" s="62"/>
     </row>
     <row r="75" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
@@ -7219,176 +7198,176 @@
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
     </row>
-    <row r="76" spans="1:10" s="68" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="68" t="s">
-        <v>433</v>
-      </c>
-      <c r="B76" s="68" t="s">
+    <row r="76" spans="1:10" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A76" s="67" t="s">
+        <v>430</v>
+      </c>
+      <c r="B76" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="C76" s="68" t="s">
-        <v>434</v>
-      </c>
-      <c r="D76" s="68">
-        <v>1</v>
-      </c>
-      <c r="E76" s="69">
+      <c r="C76" s="67" t="s">
+        <v>431</v>
+      </c>
+      <c r="D76" s="67">
+        <v>1</v>
+      </c>
+      <c r="E76" s="68">
         <v>518.5</v>
       </c>
-      <c r="F76" s="69">
+      <c r="F76" s="68">
         <f t="shared" ref="F76:F83" si="3">E76*D76</f>
         <v>518.5</v>
       </c>
-      <c r="I76" s="68" t="s">
+      <c r="I76" s="67" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="68" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A77" s="68" t="s">
-        <v>436</v>
-      </c>
-      <c r="B77" s="68" t="s">
+    <row r="77" spans="1:10" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A77" s="67" t="s">
+        <v>433</v>
+      </c>
+      <c r="B77" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="C77" s="68" t="s">
-        <v>435</v>
-      </c>
-      <c r="D77" s="68">
-        <v>1</v>
-      </c>
-      <c r="E77" s="69">
+      <c r="C77" s="67" t="s">
+        <v>432</v>
+      </c>
+      <c r="D77" s="67">
+        <v>1</v>
+      </c>
+      <c r="E77" s="68">
         <v>764</v>
       </c>
-      <c r="F77" s="69">
+      <c r="F77" s="68">
         <f t="shared" si="3"/>
         <v>764</v>
       </c>
     </row>
-    <row r="78" spans="1:10" s="68" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A78" s="68" t="s">
-        <v>438</v>
-      </c>
-      <c r="B78" s="68" t="s">
+    <row r="78" spans="1:10" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A78" s="67" t="s">
+        <v>435</v>
+      </c>
+      <c r="B78" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="C78" s="68" t="s">
-        <v>437</v>
-      </c>
-      <c r="D78" s="68">
-        <v>1</v>
-      </c>
-      <c r="E78" s="69">
+      <c r="C78" s="67" t="s">
+        <v>434</v>
+      </c>
+      <c r="D78" s="67">
+        <v>1</v>
+      </c>
+      <c r="E78" s="68">
         <v>816</v>
       </c>
-      <c r="F78" s="69">
+      <c r="F78" s="68">
         <f t="shared" si="3"/>
         <v>816</v>
       </c>
-      <c r="I78" s="68" t="s">
+      <c r="I78" s="67" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="68" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A79" s="68" t="s">
-        <v>440</v>
-      </c>
-      <c r="B79" s="68" t="s">
+    <row r="79" spans="1:10" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A79" s="67" t="s">
+        <v>437</v>
+      </c>
+      <c r="B79" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="C79" s="68" t="s">
-        <v>439</v>
-      </c>
-      <c r="D79" s="68">
-        <v>1</v>
-      </c>
-      <c r="E79" s="69">
+      <c r="C79" s="67" t="s">
+        <v>436</v>
+      </c>
+      <c r="D79" s="67">
+        <v>1</v>
+      </c>
+      <c r="E79" s="68">
         <v>952</v>
       </c>
-      <c r="F79" s="69">
+      <c r="F79" s="68">
         <f t="shared" si="3"/>
         <v>952</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="68" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A80" s="68" t="s">
-        <v>447</v>
-      </c>
-      <c r="B80" s="68" t="s">
+    <row r="80" spans="1:10" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A80" s="67" t="s">
+        <v>444</v>
+      </c>
+      <c r="B80" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="C80" s="68" t="s">
-        <v>448</v>
-      </c>
-      <c r="D80" s="68">
-        <v>1</v>
-      </c>
-      <c r="E80" s="69">
+      <c r="C80" s="67" t="s">
+        <v>445</v>
+      </c>
+      <c r="D80" s="67">
+        <v>1</v>
+      </c>
+      <c r="E80" s="68">
         <v>99.5</v>
       </c>
-      <c r="F80" s="69">
+      <c r="F80" s="68">
         <f t="shared" si="3"/>
         <v>99.5</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="68" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A81" s="68" t="s">
-        <v>442</v>
-      </c>
-      <c r="B81" s="68" t="s">
+    <row r="81" spans="1:6" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A81" s="67" t="s">
+        <v>439</v>
+      </c>
+      <c r="B81" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="C81" s="68" t="s">
-        <v>441</v>
-      </c>
-      <c r="D81" s="68">
-        <v>1</v>
-      </c>
-      <c r="E81" s="69">
+      <c r="C81" s="67" t="s">
+        <v>438</v>
+      </c>
+      <c r="D81" s="67">
+        <v>1</v>
+      </c>
+      <c r="E81" s="68">
         <v>128.5</v>
       </c>
-      <c r="F81" s="69">
+      <c r="F81" s="68">
         <f t="shared" si="3"/>
         <v>128.5</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="68" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A82" s="68" t="s">
-        <v>444</v>
-      </c>
-      <c r="B82" s="68" t="s">
+    <row r="82" spans="1:6" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A82" s="67" t="s">
+        <v>441</v>
+      </c>
+      <c r="B82" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="C82" s="68" t="s">
-        <v>443</v>
-      </c>
-      <c r="D82" s="68">
-        <v>1</v>
-      </c>
-      <c r="E82" s="69">
+      <c r="C82" s="67" t="s">
+        <v>440</v>
+      </c>
+      <c r="D82" s="67">
+        <v>1</v>
+      </c>
+      <c r="E82" s="68">
         <v>156</v>
       </c>
-      <c r="F82" s="69">
+      <c r="F82" s="68">
         <f t="shared" si="3"/>
         <v>156</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="68" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A83" s="68" t="s">
-        <v>446</v>
-      </c>
-      <c r="B83" s="68" t="s">
+    <row r="83" spans="1:6" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A83" s="67" t="s">
+        <v>443</v>
+      </c>
+      <c r="B83" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="C83" s="68" t="s">
-        <v>445</v>
-      </c>
-      <c r="D83" s="68">
-        <v>1</v>
-      </c>
-      <c r="E83" s="69">
+      <c r="C83" s="67" t="s">
+        <v>442</v>
+      </c>
+      <c r="D83" s="67">
+        <v>1</v>
+      </c>
+      <c r="E83" s="68">
         <v>184.5</v>
       </c>
-      <c r="F83" s="69">
+      <c r="F83" s="68">
         <f t="shared" si="3"/>
         <v>184.5</v>
       </c>

</xml_diff>

<commit_message>
ETL driver modification link
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E93D38-1BD4-47D5-8BA8-EAC260B57F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C91E6B-60F4-42E8-A7F3-0BCC8821F950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7188" yWindow="7704" windowWidth="34560" windowHeight="15864" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,9 +170,6 @@
     <t xml:space="preserve">Optotune Lens Driver EL-E-4i </t>
   </si>
   <si>
-    <t>Have to be modified: BNC cables need to be soldered</t>
-  </si>
-  <si>
     <t>88-941</t>
   </si>
   <si>
@@ -1711,12 +1708,15 @@
   <si>
     <t>Table mounting for the Y axis (two parallel LS-100 servo actuators Dual-LS100-FTP)</t>
   </si>
+  <si>
+    <t>Have to be modified: BNC cables need to be soldered: see https://github.com/mesoSPIM/mesoSPIM-hardware-documentation/wiki/mesoSPIM_preparing_ETL_drivers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1850,30 +1850,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
@@ -1895,6 +1871,12 @@
     </font>
     <font>
       <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="10"/>
       <name val="Arial"/>
@@ -1986,7 +1968,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -2070,27 +2052,25 @@
     <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Excel Built-in Heading 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2480,8 +2460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92:C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2557,10 +2537,10 @@
         <v>12350</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2571,24 +2551,24 @@
     </row>
     <row r="6" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
@@ -2604,7 +2584,7 @@
         <v>41</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2622,7 +2602,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
@@ -2635,10 +2615,10 @@
         <v>6500</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -2662,10 +2642,10 @@
         <v>2250</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I11" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -2689,7 +2669,7 @@
         <v>160</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H12" s="31" t="s">
         <v>13</v>
@@ -2697,13 +2677,13 @@
     </row>
     <row r="13" spans="1:9" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D13" s="31">
         <v>1</v>
@@ -2716,10 +2696,10 @@
         <v>250</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -2743,13 +2723,13 @@
         <v>2250</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>13</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -2773,10 +2753,10 @@
         <v>230</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -2800,21 +2780,21 @@
         <v>2425</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B17" s="31" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D17" s="31">
         <v>1</v>
@@ -2827,10 +2807,10 @@
         <v>3000</v>
       </c>
       <c r="G17" s="64" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2854,10 +2834,10 @@
         <v>150</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2881,10 +2861,10 @@
         <v>3000</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2895,7 +2875,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
@@ -2908,10 +2888,10 @@
         <v>5800</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2935,21 +2915,21 @@
         <v>1100</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="64" t="s">
+        <v>529</v>
+      </c>
+      <c r="B22" s="64" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="64" t="s">
         <v>530</v>
-      </c>
-      <c r="B22" s="64" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="64" t="s">
-        <v>531</v>
       </c>
       <c r="D22" s="64">
         <v>4</v>
@@ -2962,28 +2942,28 @@
         <v>108</v>
       </c>
       <c r="G22" s="64" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I22" s="64" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>277</v>
       </c>
       <c r="D24" s="3">
         <v>2</v>
@@ -2996,21 +2976,21 @@
         <v>140</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>280</v>
       </c>
       <c r="D25" s="3">
         <v>6</v>
@@ -3023,21 +3003,21 @@
         <v>216</v>
       </c>
       <c r="G25" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>281</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>283</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>284</v>
       </c>
       <c r="D26" s="3">
         <v>1</v>
@@ -3050,21 +3030,21 @@
         <v>43</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="39" t="s">
+        <v>285</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>287</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
@@ -3077,21 +3057,21 @@
         <v>29</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="39" t="s">
+        <v>288</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="C28" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>291</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
@@ -3104,21 +3084,21 @@
         <v>195</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D29" s="3">
         <v>1</v>
@@ -3131,7 +3111,7 @@
         <v>10</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="15" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3143,7 +3123,7 @@
     </row>
     <row r="31" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
@@ -3156,7 +3136,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F32" s="5">
         <v>0</v>
@@ -3164,7 +3144,7 @@
     </row>
     <row r="34" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
@@ -3196,45 +3176,45 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="4">
         <v>2</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="20">
         <v>280</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="20">
         <f t="shared" si="2"/>
         <v>560</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>45</v>
+        <v>532</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D37" s="3">
         <v>2</v>
@@ -3255,13 +3235,13 @@
     </row>
     <row r="38" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="32" t="s">
         <v>221</v>
-      </c>
-      <c r="B38" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="32" t="s">
-        <v>222</v>
       </c>
       <c r="D38" s="31">
         <v>2</v>
@@ -3282,13 +3262,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="D39" s="3">
         <v>2</v>
@@ -3309,13 +3289,13 @@
     </row>
     <row r="40" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D40" s="31">
         <v>2</v>
@@ -3336,13 +3316,13 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D41" s="3">
         <v>1</v>
@@ -3360,18 +3340,18 @@
         <v>42</v>
       </c>
       <c r="I41" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="83">
+        <v>91863</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="87">
-        <v>91863</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="D42" s="4">
         <v>2</v>
@@ -3387,21 +3367,21 @@
         <v>41</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D43" s="3">
         <v>2</v>
@@ -3417,29 +3397,29 @@
         <v>41</v>
       </c>
       <c r="H43" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="83" t="s">
+      <c r="A44" s="79" t="s">
+        <v>248</v>
+      </c>
+      <c r="B44" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="44" t="s">
         <v>249</v>
-      </c>
-      <c r="B44" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="44" t="s">
-        <v>250</v>
       </c>
       <c r="D44" s="37">
         <v>0</v>
       </c>
-      <c r="E44" s="84">
+      <c r="E44" s="80">
         <v>40</v>
       </c>
-      <c r="F44" s="85">
+      <c r="F44" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3447,30 +3427,30 @@
         <v>41</v>
       </c>
       <c r="H44" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I44" s="37" t="s">
-        <v>515</v>
-      </c>
-      <c r="J44" s="86"/>
+        <v>514</v>
+      </c>
+      <c r="J44" s="82"/>
     </row>
     <row r="45" spans="1:10" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="44" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D45" s="37">
         <v>0</v>
       </c>
-      <c r="E45" s="84">
+      <c r="E45" s="80">
         <v>92</v>
       </c>
-      <c r="F45" s="85">
+      <c r="F45" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3478,21 +3458,21 @@
         <v>41</v>
       </c>
       <c r="H45" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I45" s="37" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="44" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C46" s="43" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D46" s="31">
         <v>2</v>
@@ -3508,21 +3488,21 @@
         <v>41</v>
       </c>
       <c r="H46" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I46" s="31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="47" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D47" s="31">
         <v>2</v>
@@ -3538,21 +3518,21 @@
         <v>41</v>
       </c>
       <c r="H47" s="31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I47" s="31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="B48" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="34" t="s">
         <v>203</v>
-      </c>
-      <c r="B48" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" s="34" t="s">
-        <v>204</v>
       </c>
       <c r="D48" s="35">
         <v>10</v>
@@ -3568,21 +3548,21 @@
         <v>41</v>
       </c>
       <c r="H48" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I48" s="35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="34" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" s="34" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D49" s="35">
         <v>2</v>
@@ -3598,21 +3578,21 @@
         <v>41</v>
       </c>
       <c r="H49" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I49" s="35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B50" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="32" t="s">
         <v>211</v>
-      </c>
-      <c r="B50" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C50" s="32" t="s">
-        <v>212</v>
       </c>
       <c r="D50" s="31">
         <v>2</v>
@@ -3628,21 +3608,21 @@
         <v>41</v>
       </c>
       <c r="H50" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="I50" s="31" t="s">
         <v>213</v>
-      </c>
-      <c r="I50" s="31" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D51" s="31">
         <v>4</v>
@@ -3658,21 +3638,21 @@
         <v>41</v>
       </c>
       <c r="H51" s="31" t="s">
+        <v>470</v>
+      </c>
+      <c r="I51" s="31" t="s">
         <v>471</v>
-      </c>
-      <c r="I51" s="31" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="34" t="s">
+        <v>214</v>
+      </c>
+      <c r="B52" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="34" t="s">
         <v>215</v>
-      </c>
-      <c r="B52" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C52" s="34" t="s">
-        <v>216</v>
       </c>
       <c r="D52" s="35">
         <v>4</v>
@@ -3688,21 +3668,21 @@
         <v>41</v>
       </c>
       <c r="H52" s="35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I52" s="35" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="B53" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="34" t="s">
         <v>218</v>
-      </c>
-      <c r="B53" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C53" s="34" t="s">
-        <v>219</v>
       </c>
       <c r="D53" s="35">
         <v>4</v>
@@ -3718,21 +3698,21 @@
         <v>41</v>
       </c>
       <c r="H53" s="35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I53" s="35" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="B54" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="32" t="s">
         <v>224</v>
-      </c>
-      <c r="B54" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" s="32" t="s">
-        <v>225</v>
       </c>
       <c r="D54" s="31">
         <v>4</v>
@@ -3748,21 +3728,21 @@
         <v>41</v>
       </c>
       <c r="H54" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I54" s="31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="B55" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="32" t="s">
         <v>234</v>
-      </c>
-      <c r="B55" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C55" s="32" t="s">
-        <v>235</v>
       </c>
       <c r="D55" s="31">
         <v>2</v>
@@ -3778,18 +3758,18 @@
         <v>41</v>
       </c>
       <c r="H55" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="32" t="s">
         <v>174</v>
-      </c>
-      <c r="B56" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C56" s="32" t="s">
-        <v>175</v>
       </c>
       <c r="D56" s="31">
         <v>4</v>
@@ -3805,21 +3785,21 @@
         <v>41</v>
       </c>
       <c r="H56" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I56" s="31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="B57" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" s="32" t="s">
         <v>226</v>
-      </c>
-      <c r="B57" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C57" s="32" t="s">
-        <v>227</v>
       </c>
       <c r="D57" s="31">
         <v>6</v>
@@ -3835,21 +3815,21 @@
         <v>41</v>
       </c>
       <c r="H57" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I57" s="31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B58" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" s="32" t="s">
         <v>230</v>
-      </c>
-      <c r="B58" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="32" t="s">
-        <v>231</v>
       </c>
       <c r="D58" s="31">
         <v>4</v>
@@ -3865,21 +3845,21 @@
         <v>41</v>
       </c>
       <c r="H58" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I58" s="31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="B59" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" s="32" t="s">
         <v>232</v>
-      </c>
-      <c r="B59" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C59" s="32" t="s">
-        <v>233</v>
       </c>
       <c r="D59" s="31">
         <v>4</v>
@@ -3895,21 +3875,21 @@
         <v>41</v>
       </c>
       <c r="H59" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I59" s="31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="B60" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" s="32" t="s">
         <v>172</v>
-      </c>
-      <c r="B60" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C60" s="32" t="s">
-        <v>173</v>
       </c>
       <c r="D60" s="31">
         <v>2</v>
@@ -3925,18 +3905,18 @@
         <v>41</v>
       </c>
       <c r="H60" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="B61" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="34" t="s">
         <v>236</v>
-      </c>
-      <c r="B61" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" s="34" t="s">
-        <v>237</v>
       </c>
       <c r="D61" s="35">
         <v>2</v>
@@ -3952,21 +3932,21 @@
         <v>41</v>
       </c>
       <c r="H61" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I61" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="35" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="82" t="s">
-        <v>503</v>
+      <c r="A62" s="78" t="s">
+        <v>502</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C62" s="34" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D62" s="35">
         <v>2</v>
@@ -3982,21 +3962,21 @@
         <v>41</v>
       </c>
       <c r="H62" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I62" s="35" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="B63" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C63" s="34" t="s">
         <v>239</v>
-      </c>
-      <c r="B63" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C63" s="34" t="s">
-        <v>240</v>
       </c>
       <c r="D63" s="35">
         <v>2</v>
@@ -4012,21 +3992,21 @@
         <v>41</v>
       </c>
       <c r="H63" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I63" s="35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="44" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D64" s="31">
         <v>2</v>
@@ -4042,21 +4022,21 @@
         <v>41</v>
       </c>
       <c r="H64" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I64" s="37" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="32" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B65" s="71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C65" s="72" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D65" s="71">
         <v>0</v>
@@ -4072,21 +4052,21 @@
         <v>41</v>
       </c>
       <c r="H65" s="71" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I65" s="71" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="B66" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" s="32" t="s">
         <v>304</v>
-      </c>
-      <c r="B66" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="32" t="s">
-        <v>305</v>
       </c>
       <c r="D66" s="31">
         <v>2</v>
@@ -4102,21 +4082,21 @@
         <v>41</v>
       </c>
       <c r="H66" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I66" s="31" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="B67" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C67" s="32" t="s">
         <v>306</v>
-      </c>
-      <c r="B67" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C67" s="32" t="s">
-        <v>307</v>
       </c>
       <c r="D67" s="31">
         <v>2</v>
@@ -4132,18 +4112,18 @@
         <v>41</v>
       </c>
       <c r="H67" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="43" t="s">
+        <v>503</v>
+      </c>
+      <c r="B68" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" s="32" t="s">
         <v>504</v>
-      </c>
-      <c r="B68" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C68" s="32" t="s">
-        <v>505</v>
       </c>
       <c r="D68" s="31">
         <v>1</v>
@@ -4159,21 +4139,21 @@
         <v>41</v>
       </c>
       <c r="H68" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I68" s="31" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="81" t="s">
-        <v>338</v>
+      <c r="A69" s="77" t="s">
+        <v>337</v>
       </c>
       <c r="B69" s="71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C69" s="72" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D69" s="71">
         <v>0</v>
@@ -4189,21 +4169,21 @@
         <v>41</v>
       </c>
       <c r="H69" s="71" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I69" s="71" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="44" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B70" s="37" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C70" s="32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D70" s="31">
         <v>14</v>
@@ -4219,21 +4199,21 @@
         <v>41</v>
       </c>
       <c r="H70" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I70" s="37" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="31" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D71" s="31">
         <v>1</v>
@@ -4249,10 +4229,10 @@
         <v>41</v>
       </c>
       <c r="H71" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I71" s="31" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -4275,7 +4255,7 @@
     </row>
     <row r="75" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
@@ -4296,18 +4276,18 @@
       <c r="E76" s="33"/>
       <c r="F76" s="40"/>
       <c r="I76" s="31" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="B77" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C77" s="32" t="s">
         <v>268</v>
-      </c>
-      <c r="B77" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C77" s="32" t="s">
-        <v>269</v>
       </c>
       <c r="D77" s="31">
         <v>1</v>
@@ -4322,13 +4302,13 @@
     </row>
     <row r="78" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="38" t="s">
+        <v>272</v>
+      </c>
+      <c r="B78" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C78" s="32" t="s">
         <v>273</v>
-      </c>
-      <c r="B78" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C78" s="32" t="s">
-        <v>274</v>
       </c>
       <c r="D78" s="31">
         <v>2</v>
@@ -4357,32 +4337,32 @@
       <c r="E79" s="33"/>
       <c r="F79" s="40"/>
       <c r="I79" s="31" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="80" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
     </row>
     <row r="81" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
     </row>
     <row r="82" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="B82" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="C82" s="93" t="s">
-        <v>450</v>
+      <c r="C82" s="89" t="s">
+        <v>449</v>
       </c>
       <c r="D82" s="3">
         <v>1</v>
@@ -4395,19 +4375,19 @@
         <v>200</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J82" s="4"/>
     </row>
     <row r="83" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D83" s="4">
         <v>5</v>
@@ -4420,18 +4400,18 @@
         <v>5</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="64" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D84" s="3">
         <v>1</v>
@@ -4444,18 +4424,18 @@
         <v>26</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>459</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>460</v>
       </c>
       <c r="D85" s="3">
         <v>1</v>
@@ -4468,18 +4448,18 @@
         <v>37</v>
       </c>
       <c r="I85" s="64" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="86" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="64" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B86" s="64" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C86" s="64" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D86" s="64">
         <v>2</v>
@@ -4492,30 +4472,30 @@
         <v>48</v>
       </c>
       <c r="I86" s="31" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="87" spans="1:10" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="69" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F87" s="42"/>
     </row>
     <row r="88" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F88" s="42"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D89" s="3">
         <v>1</v>
@@ -4531,25 +4511,25 @@
         <v>13</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="90" spans="1:10" s="25" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A90" s="24" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E90" s="26"/>
       <c r="F90" s="26"/>
     </row>
-    <row r="91" spans="1:10" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="29" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>351</v>
-      </c>
-      <c r="C91" s="78" t="s">
-        <v>354</v>
+        <v>350</v>
+      </c>
+      <c r="C91" s="90" t="s">
+        <v>353</v>
       </c>
       <c r="D91" s="27">
         <v>1</v>
@@ -4565,18 +4545,18 @@
         <v>13</v>
       </c>
       <c r="I91" s="27" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="30" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B92" s="27" t="s">
-        <v>351</v>
-      </c>
-      <c r="C92" s="79" t="s">
-        <v>355</v>
+        <v>350</v>
+      </c>
+      <c r="C92" s="91" t="s">
+        <v>354</v>
       </c>
       <c r="D92" s="3">
         <v>1</v>
@@ -4593,18 +4573,18 @@
       </c>
       <c r="H92" s="27"/>
       <c r="I92" s="3" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="30" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B93" s="27" t="s">
-        <v>351</v>
-      </c>
-      <c r="C93" s="79" t="s">
-        <v>356</v>
+        <v>350</v>
+      </c>
+      <c r="C93" s="91" t="s">
+        <v>355</v>
       </c>
       <c r="D93" s="3">
         <v>0</v>
@@ -4621,18 +4601,18 @@
       </c>
       <c r="H93" s="27"/>
       <c r="I93" s="3" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B94" s="27" t="s">
-        <v>351</v>
-      </c>
-      <c r="C94" s="79" t="s">
-        <v>358</v>
+        <v>350</v>
+      </c>
+      <c r="C94" s="91" t="s">
+        <v>357</v>
       </c>
       <c r="D94" s="3">
         <v>1</v>
@@ -4649,18 +4629,18 @@
       </c>
       <c r="H94" s="27"/>
       <c r="I94" s="3" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" s="64" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="64" t="s">
+        <v>465</v>
+      </c>
+      <c r="B95" s="27" t="s">
         <v>466</v>
       </c>
-      <c r="B95" s="27" t="s">
+      <c r="C95" s="91" t="s">
         <v>467</v>
-      </c>
-      <c r="C95" s="80" t="s">
-        <v>468</v>
       </c>
       <c r="D95" s="64">
         <v>0</v>
@@ -4677,18 +4657,18 @@
       </c>
       <c r="H95" s="27"/>
       <c r="I95" s="64" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="96" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B96" s="84" t="s">
+        <v>251</v>
+      </c>
+      <c r="C96" s="85" t="s">
         <v>360</v>
-      </c>
-      <c r="B96" s="88" t="s">
-        <v>252</v>
-      </c>
-      <c r="C96" s="89" t="s">
-        <v>361</v>
       </c>
       <c r="D96" s="4">
         <v>5</v>
@@ -4696,24 +4676,24 @@
       <c r="E96" s="20">
         <v>1</v>
       </c>
-      <c r="F96" s="90">
+      <c r="F96" s="86">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="G96" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H96" s="88"/>
+      <c r="H96" s="84"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B97" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C97" s="45" t="s">
         <v>362</v>
-      </c>
-      <c r="B97" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C97" s="45" t="s">
-        <v>363</v>
       </c>
       <c r="D97" s="3">
         <v>1</v>
@@ -4732,20 +4712,20 @@
     </row>
     <row r="98" spans="1:9" s="25" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A98" s="24" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E98" s="26"/>
       <c r="F98" s="26"/>
     </row>
-    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B99" s="27" t="s">
-        <v>351</v>
-      </c>
-      <c r="C99" s="77" t="s">
-        <v>394</v>
+        <v>350</v>
+      </c>
+      <c r="C99" s="91" t="s">
+        <v>393</v>
       </c>
       <c r="D99" s="3">
         <v>1</v>
@@ -4761,18 +4741,18 @@
         <v>13</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="B100" s="84" t="s">
+        <v>251</v>
+      </c>
+      <c r="C100" s="4" t="s">
         <v>396</v>
-      </c>
-      <c r="B100" s="88" t="s">
-        <v>252</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>397</v>
       </c>
       <c r="D100" s="4">
         <v>1</v>
@@ -4790,13 +4770,13 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B101" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>398</v>
-      </c>
-      <c r="B101" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>399</v>
       </c>
       <c r="D101" s="3">
         <v>1</v>
@@ -4812,18 +4792,18 @@
         <v>13</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B102" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C102" s="3" t="s">
         <v>401</v>
-      </c>
-      <c r="B102" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>402</v>
       </c>
       <c r="D102" s="3">
         <v>1</v>
@@ -4839,18 +4819,18 @@
         <v>13</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B103" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C103" s="3" t="s">
         <v>385</v>
-      </c>
-      <c r="B103" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>386</v>
       </c>
       <c r="D103" s="3">
         <v>1</v>
@@ -4866,25 +4846,25 @@
         <v>13</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E104" s="9"/>
       <c r="F104" s="9"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C105" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D105" s="3">
         <v>1</v>
@@ -4897,21 +4877,21 @@
         <v>3582</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D106" s="3">
         <v>1</v>
@@ -4924,21 +4904,21 @@
         <v>1630</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D107" s="3">
         <v>1</v>
@@ -4951,21 +4931,21 @@
         <v>886</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D108" s="3">
         <v>1</v>
@@ -4978,21 +4958,21 @@
         <v>163</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D109" s="3">
         <v>1</v>
@@ -5005,18 +4985,18 @@
         <v>11</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C110" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="D110" s="3">
         <v>1</v>
@@ -5029,18 +5009,18 @@
         <v>520</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D111" s="3">
         <v>1</v>
@@ -5053,18 +5033,18 @@
         <v>193</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="31" t="s">
+        <v>316</v>
+      </c>
+      <c r="B112" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C112" s="31" t="s">
         <v>317</v>
-      </c>
-      <c r="B112" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C112" s="31" t="s">
-        <v>318</v>
       </c>
       <c r="D112" s="31">
         <v>10</v>
@@ -5077,21 +5057,21 @@
         <v>120</v>
       </c>
       <c r="G112" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I112" s="31" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="113" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="B113" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C113" s="31" t="s">
         <v>319</v>
-      </c>
-      <c r="B113" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C113" s="31" t="s">
-        <v>320</v>
       </c>
       <c r="D113" s="31">
         <v>1</v>
@@ -5104,21 +5084,21 @@
         <v>14</v>
       </c>
       <c r="G113" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I113" s="31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="D114" s="3">
         <v>4</v>
@@ -5131,18 +5111,18 @@
         <v>61</v>
       </c>
       <c r="G114" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="D115" s="3">
         <v>10</v>
@@ -5155,18 +5135,18 @@
         <v>165</v>
       </c>
       <c r="G115" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C116" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="D116" s="3">
         <v>10</v>
@@ -5179,18 +5159,18 @@
         <v>240</v>
       </c>
       <c r="G116" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D117" s="3">
         <v>6</v>
@@ -5203,7 +5183,7 @@
         <v>144</v>
       </c>
       <c r="G117" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="118" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -5217,19 +5197,19 @@
     </row>
     <row r="121" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F121" s="9"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B122" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="C122" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="D122" s="3">
         <v>4</v>
@@ -5242,18 +5222,18 @@
         <v>66</v>
       </c>
       <c r="I122" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C123" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="D123" s="3">
         <v>1</v>
@@ -5268,13 +5248,13 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C124" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="D124" s="3">
         <v>2</v>
@@ -5287,18 +5267,18 @@
         <v>64</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="D125" s="3">
         <v>2</v>
@@ -5313,13 +5293,13 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C126" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="D126" s="3">
         <v>1</v>
@@ -5332,18 +5312,18 @@
         <v>60</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C127" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="D127" s="3">
         <v>1</v>
@@ -5358,13 +5338,13 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D128" s="3">
         <v>1</v>
@@ -5379,13 +5359,13 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="D129" s="3">
         <v>1</v>
@@ -5400,13 +5380,13 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C130" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="D130" s="3">
         <v>1</v>
@@ -5421,13 +5401,13 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C131" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="D131" s="3">
         <v>1</v>
@@ -5442,13 +5422,13 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C132" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="D132" s="3">
         <v>2</v>
@@ -5463,13 +5443,13 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C133" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>328</v>
       </c>
       <c r="D133" s="3">
         <v>1</v>
@@ -5484,13 +5464,13 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C134" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D134" s="3">
         <v>2</v>
@@ -5505,13 +5485,13 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C135" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="D135" s="3">
         <v>1</v>
@@ -5526,13 +5506,13 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C136" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="D136" s="3">
         <v>1</v>
@@ -5547,13 +5527,13 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C137" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C137" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="D137" s="3">
         <v>2</v>
@@ -5568,7 +5548,7 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C138" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D138" s="3">
         <v>4</v>
@@ -5576,18 +5556,18 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C139" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D139" s="3">
+        <v>1</v>
+      </c>
+      <c r="I139" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="D139" s="3">
-        <v>1</v>
-      </c>
-      <c r="I139" s="3" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C140" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D140" s="3">
         <v>1</v>
@@ -5595,10 +5575,10 @@
     </row>
     <row r="142" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E142" s="9"/>
       <c r="F142" s="9"/>
@@ -5606,10 +5586,10 @@
     <row r="143" spans="1:10" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="64"/>
       <c r="B143" s="64" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C143" s="66" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D143" s="64">
         <v>4</v>
@@ -5622,22 +5602,22 @@
         <v>160</v>
       </c>
       <c r="G143" s="64" t="s">
+        <v>489</v>
+      </c>
+      <c r="H143" s="64" t="s">
         <v>490</v>
       </c>
-      <c r="H143" s="64" t="s">
-        <v>491</v>
-      </c>
       <c r="I143" s="64" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J143" s="66"/>
     </row>
     <row r="144" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B144" s="64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C144" s="64" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D144" s="64">
         <v>2</v>
@@ -5650,15 +5630,15 @@
         <v>662</v>
       </c>
       <c r="G144" s="64" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="145" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B145" s="64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C145" s="64" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D145" s="64">
         <v>4</v>
@@ -5671,15 +5651,15 @@
         <v>100</v>
       </c>
       <c r="G145" s="64" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="146" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B146" s="64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C146" s="64" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D146" s="64">
         <v>4</v>
@@ -5692,15 +5672,15 @@
         <v>112</v>
       </c>
       <c r="G146" s="64" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="147" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B147" s="64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C147" s="64" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D147" s="64">
         <v>6</v>
@@ -5713,188 +5693,188 @@
         <v>729</v>
       </c>
       <c r="G147" s="64" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E150" s="76" t="s">
-        <v>527</v>
-      </c>
-      <c r="F150" s="92">
+        <v>526</v>
+      </c>
+      <c r="F150" s="88">
         <f>SUM(F3:F148)</f>
         <v>93407.255999999994</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A153" s="91" t="s">
-        <v>506</v>
+      <c r="A153" s="87" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B155" s="3">
         <v>1</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B156" s="3">
         <v>14</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B157" s="3">
         <v>2</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B158" s="3">
         <v>2</v>
       </c>
       <c r="C158" s="64" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B159" s="3">
         <v>2</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A162" s="91" t="s">
-        <v>512</v>
+      <c r="A162" s="87" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A163" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B164" s="3">
         <v>2</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B165" s="3">
         <v>5</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B166" s="3">
         <v>1</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A169" s="91" t="s">
-        <v>519</v>
+      <c r="A169" s="87" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A170" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="64" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B171" s="3">
         <v>5</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B172" s="3">
         <v>3</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C173" s="3" t="s">
         <v>524</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>525</v>
       </c>
     </row>
   </sheetData>
@@ -5963,7 +5943,7 @@
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -5973,7 +5953,7 @@
         <v>1008062</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C3" s="57" t="s">
         <v>16</v>
@@ -5989,15 +5969,15 @@
         <v>7400</v>
       </c>
       <c r="I3" s="57" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="57" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="57" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D4" s="57">
         <v>1</v>
@@ -6010,15 +5990,15 @@
         <v>20000</v>
       </c>
       <c r="I4" s="57" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="46" t="s">
+        <v>426</v>
+      </c>
+      <c r="C5" s="46" t="s">
         <v>427</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>428</v>
       </c>
       <c r="D5" s="46">
         <v>1</v>
@@ -6030,23 +6010,23 @@
         <v>50000</v>
       </c>
       <c r="I5" s="46" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B8" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="46" t="s">
         <v>178</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>179</v>
       </c>
       <c r="D8" s="46">
         <v>1</v>
@@ -6059,27 +6039,27 @@
         <v>25000</v>
       </c>
       <c r="I8" s="46" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" s="25" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:9" s="46" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="46" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B12" s="47" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D12" s="46">
         <v>1</v>
@@ -6095,21 +6075,21 @@
         <v>13</v>
       </c>
       <c r="H12" s="46" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I12" s="46" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="46" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B13" s="47" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D13" s="46">
         <v>1</v>
@@ -6125,21 +6105,21 @@
         <v>13</v>
       </c>
       <c r="H13" s="46" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I13" s="46" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B14" s="47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D14" s="46">
         <v>1</v>
@@ -6155,21 +6135,21 @@
         <v>13</v>
       </c>
       <c r="H14" s="46" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I14" s="46" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="46" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D15" s="46">
         <v>1</v>
@@ -6185,21 +6165,21 @@
         <v>13</v>
       </c>
       <c r="H15" s="46" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I15" s="46" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
+        <v>270</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C16" s="50" t="s">
         <v>271</v>
-      </c>
-      <c r="B16" s="47" t="s">
-        <v>270</v>
-      </c>
-      <c r="C16" s="50" t="s">
-        <v>272</v>
       </c>
       <c r="D16" s="47">
         <v>1</v>
@@ -6215,32 +6195,32 @@
         <v>13</v>
       </c>
       <c r="H16" s="47" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I16" s="47" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:10" s="64" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="64" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B19" s="64" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C19" s="64" t="s">
         <v>14</v>
@@ -6265,13 +6245,13 @@
     </row>
     <row r="20" spans="1:10" s="64" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="64" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B20" s="64" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C20" s="64" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D20" s="64">
         <v>1</v>
@@ -6293,13 +6273,13 @@
     </row>
     <row r="21" spans="1:10" s="64" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="64" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B21" s="64" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C21" s="64" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D21" s="64">
         <v>1</v>
@@ -6320,13 +6300,13 @@
     </row>
     <row r="22" spans="1:10" s="64" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="64" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B22" s="64" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C22" s="64" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D22" s="64">
         <v>1</v>
@@ -6334,32 +6314,32 @@
       <c r="E22" s="65"/>
       <c r="F22" s="65"/>
       <c r="I22" s="31" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:10" s="55" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="54" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E25" s="56"/>
       <c r="F25" s="56"/>
     </row>
     <row r="26" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="50" t="s">
+        <v>339</v>
+      </c>
+      <c r="B26" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="C26" s="50" t="s">
         <v>340</v>
-      </c>
-      <c r="B26" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="C26" s="50" t="s">
-        <v>341</v>
       </c>
       <c r="D26" s="47">
         <v>2</v>
@@ -6375,21 +6355,21 @@
         <v>41</v>
       </c>
       <c r="H26" s="47" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I26" s="47" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="50" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B27" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D27" s="47">
         <v>2</v>
@@ -6405,21 +6385,21 @@
         <v>41</v>
       </c>
       <c r="H27" s="47" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I27" s="47" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="50" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B28" s="47" t="s">
+        <v>363</v>
+      </c>
+      <c r="C28" s="50" t="s">
         <v>364</v>
-      </c>
-      <c r="C28" s="50" t="s">
-        <v>365</v>
       </c>
       <c r="D28" s="47">
         <v>8</v>
@@ -6435,21 +6415,21 @@
         <v>41</v>
       </c>
       <c r="H28" s="47" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I28" s="47" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="50" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B29" s="47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D29" s="47">
         <v>6</v>
@@ -6465,18 +6445,18 @@
         <v>41</v>
       </c>
       <c r="H29" s="47" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="50" t="s">
+        <v>368</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="C30" s="50" t="s">
         <v>369</v>
-      </c>
-      <c r="B30" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="C30" s="50" t="s">
-        <v>370</v>
       </c>
       <c r="D30" s="47">
         <v>2</v>
@@ -6492,21 +6472,21 @@
         <v>41</v>
       </c>
       <c r="H30" s="47" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I30" s="47" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B31" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D31" s="47">
         <v>1</v>
@@ -6522,21 +6502,21 @@
         <v>41</v>
       </c>
       <c r="H31" s="47" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I31" s="47" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B32" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D32" s="47">
         <v>1</v>
@@ -6552,21 +6532,21 @@
         <v>41</v>
       </c>
       <c r="H32" s="47" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I32" s="47" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="50" t="s">
+        <v>244</v>
+      </c>
+      <c r="B33" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="50" t="s">
         <v>245</v>
-      </c>
-      <c r="B33" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="50" t="s">
-        <v>246</v>
       </c>
       <c r="D33" s="47">
         <v>2</v>
@@ -6582,25 +6562,25 @@
         <v>41</v>
       </c>
       <c r="H33" s="47" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:9" s="57" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="57" t="s">
         <v>56</v>
-      </c>
-      <c r="B38" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="57" t="s">
-        <v>57</v>
       </c>
       <c r="D38" s="57">
         <v>1</v>
@@ -6613,15 +6593,15 @@
         <v>2800</v>
       </c>
       <c r="G38" s="57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I38" s="57" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" s="7"/>
       <c r="E42" s="18"/>
@@ -6629,13 +6609,13 @@
     </row>
     <row r="43" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="46" t="s">
         <v>64</v>
-      </c>
-      <c r="C43" s="46" t="s">
-        <v>65</v>
       </c>
       <c r="D43" s="46">
         <v>1</v>
@@ -6650,13 +6630,13 @@
     </row>
     <row r="44" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="46" t="s">
         <v>66</v>
-      </c>
-      <c r="B44" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="46" t="s">
-        <v>67</v>
       </c>
       <c r="D44" s="46">
         <v>1</v>
@@ -6671,13 +6651,13 @@
     </row>
     <row r="45" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="46" t="s">
         <v>68</v>
-      </c>
-      <c r="B45" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="46" t="s">
-        <v>69</v>
       </c>
       <c r="D45" s="46">
         <v>1</v>
@@ -6692,13 +6672,13 @@
     </row>
     <row r="46" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="46" t="s">
         <v>70</v>
-      </c>
-      <c r="B46" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C46" s="46" t="s">
-        <v>71</v>
       </c>
       <c r="D46" s="46">
         <v>1</v>
@@ -6713,13 +6693,13 @@
     </row>
     <row r="47" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="46" t="s">
         <v>73</v>
-      </c>
-      <c r="B47" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="46" t="s">
-        <v>74</v>
       </c>
       <c r="D47" s="46">
         <v>1</v>
@@ -6734,13 +6714,13 @@
     </row>
     <row r="48" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="46" t="s">
         <v>75</v>
-      </c>
-      <c r="B48" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" s="46" t="s">
-        <v>76</v>
       </c>
       <c r="D48" s="46">
         <v>1</v>
@@ -6755,13 +6735,13 @@
     </row>
     <row r="49" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="46" t="s">
         <v>79</v>
-      </c>
-      <c r="B49" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" s="46" t="s">
-        <v>80</v>
       </c>
       <c r="D49" s="46">
         <v>2</v>
@@ -6776,13 +6756,13 @@
     </row>
     <row r="50" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="46" t="s">
         <v>81</v>
-      </c>
-      <c r="B50" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C50" s="46" t="s">
-        <v>82</v>
       </c>
       <c r="D50" s="46">
         <v>1</v>
@@ -6795,18 +6775,18 @@
         <v>304.75</v>
       </c>
       <c r="I50" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" s="46" t="s">
         <v>84</v>
-      </c>
-      <c r="B51" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C51" s="46" t="s">
-        <v>85</v>
       </c>
       <c r="D51" s="46">
         <v>1</v>
@@ -6819,18 +6799,18 @@
         <v>148.21</v>
       </c>
       <c r="I51" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="46" t="s">
         <v>86</v>
-      </c>
-      <c r="B52" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C52" s="46" t="s">
-        <v>87</v>
       </c>
       <c r="D52" s="46">
         <v>1</v>
@@ -6843,18 +6823,18 @@
         <v>348.45</v>
       </c>
       <c r="I52" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="46" t="s">
         <v>88</v>
-      </c>
-      <c r="B53" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C53" s="46" t="s">
-        <v>89</v>
       </c>
       <c r="D53" s="46">
         <v>1</v>
@@ -6869,13 +6849,13 @@
     </row>
     <row r="54" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="46" t="s">
         <v>90</v>
-      </c>
-      <c r="B54" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" s="46" t="s">
-        <v>91</v>
       </c>
       <c r="D54" s="46">
         <v>1</v>
@@ -6888,18 +6868,18 @@
         <v>34.5</v>
       </c>
       <c r="I54" s="46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="46" t="s">
         <v>93</v>
-      </c>
-      <c r="B55" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C55" s="46" t="s">
-        <v>94</v>
       </c>
       <c r="D55" s="46">
         <v>1</v>
@@ -6912,18 +6892,18 @@
         <v>51.45</v>
       </c>
       <c r="I55" s="46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="46" t="s">
         <v>95</v>
-      </c>
-      <c r="B56" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C56" s="46" t="s">
-        <v>96</v>
       </c>
       <c r="D56" s="46">
         <v>2</v>
@@ -6938,13 +6918,13 @@
     </row>
     <row r="57" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" s="46" t="s">
         <v>97</v>
-      </c>
-      <c r="B57" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C57" s="46" t="s">
-        <v>98</v>
       </c>
       <c r="D57" s="46">
         <v>1</v>
@@ -6959,13 +6939,13 @@
     </row>
     <row r="58" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" s="46" t="s">
         <v>99</v>
-      </c>
-      <c r="B58" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="46" t="s">
-        <v>100</v>
       </c>
       <c r="D58" s="46">
         <v>2</v>
@@ -6978,18 +6958,18 @@
         <v>81.02</v>
       </c>
       <c r="I58" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" s="46" t="s">
         <v>102</v>
-      </c>
-      <c r="B59" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C59" s="46" t="s">
-        <v>103</v>
       </c>
       <c r="D59" s="46">
         <v>2</v>
@@ -7002,18 +6982,18 @@
         <v>167.19623200000001</v>
       </c>
       <c r="I59" s="46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" s="46" t="s">
         <v>104</v>
-      </c>
-      <c r="B60" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C60" s="46" t="s">
-        <v>105</v>
       </c>
       <c r="D60" s="46">
         <v>4</v>
@@ -7026,18 +7006,18 @@
         <v>280.416</v>
       </c>
       <c r="I60" s="46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="B61" s="46" t="s">
+      <c r="C61" s="46" t="s">
         <v>107</v>
-      </c>
-      <c r="C61" s="46" t="s">
-        <v>108</v>
       </c>
       <c r="D61" s="46">
         <v>2</v>
@@ -7050,18 +7030,18 @@
         <v>57.5</v>
       </c>
       <c r="I61" s="59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" s="46" t="s">
         <v>110</v>
-      </c>
-      <c r="B62" s="46" t="s">
-        <v>107</v>
-      </c>
-      <c r="C62" s="46" t="s">
-        <v>111</v>
       </c>
       <c r="D62" s="46">
         <v>2</v>
@@ -7076,10 +7056,10 @@
     </row>
     <row r="63" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B63" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C63" s="46" t="s">
         <v>112</v>
-      </c>
-      <c r="C63" s="46" t="s">
-        <v>113</v>
       </c>
       <c r="D63" s="46">
         <v>1</v>
@@ -7092,15 +7072,15 @@
         <v>205</v>
       </c>
       <c r="I63" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B64" s="46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C64" s="46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D64" s="46">
         <v>2</v>
@@ -7113,24 +7093,24 @@
         <v>24</v>
       </c>
       <c r="I64" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F66" s="9"/>
     </row>
     <row r="67" spans="1:10" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="B67" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="B67" s="46" t="s">
+      <c r="C67" s="46" t="s">
         <v>121</v>
-      </c>
-      <c r="C67" s="46" t="s">
-        <v>122</v>
       </c>
       <c r="D67" s="46">
         <v>2</v>
@@ -7143,18 +7123,18 @@
         <v>280</v>
       </c>
       <c r="I67" s="46" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>413</v>
+      </c>
+      <c r="B68" s="60" t="s">
         <v>414</v>
       </c>
-      <c r="B68" s="60" t="s">
+      <c r="C68" s="60" t="s">
         <v>415</v>
-      </c>
-      <c r="C68" s="60" t="s">
-        <v>416</v>
       </c>
       <c r="D68" s="60">
         <v>2</v>
@@ -7167,18 +7147,18 @@
         <v>168</v>
       </c>
       <c r="I68" s="60" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B69" s="60" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C69" s="60" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D69" s="60">
         <v>1</v>
@@ -7191,18 +7171,18 @@
         <v>54</v>
       </c>
       <c r="I69" s="60" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F71" s="9"/>
     </row>
     <row r="72" spans="1:10" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="46" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C72" s="62"/>
       <c r="E72" s="49"/>
@@ -7211,7 +7191,7 @@
     </row>
     <row r="73" spans="1:10" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="46" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C73" s="62"/>
       <c r="E73" s="49"/>
@@ -7226,23 +7206,23 @@
     </row>
     <row r="75" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
     </row>
     <row r="76" spans="1:10" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="67" t="s">
+        <v>429</v>
+      </c>
+      <c r="B76" s="67" t="s">
+        <v>164</v>
+      </c>
+      <c r="C76" s="67" t="s">
         <v>430</v>
-      </c>
-      <c r="B76" s="67" t="s">
-        <v>165</v>
-      </c>
-      <c r="C76" s="67" t="s">
-        <v>431</v>
       </c>
       <c r="D76" s="67">
         <v>1</v>
@@ -7255,18 +7235,18 @@
         <v>518.5</v>
       </c>
       <c r="I76" s="67" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:10" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="67" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B77" s="67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C77" s="67" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D77" s="67">
         <v>1</v>
@@ -7281,13 +7261,13 @@
     </row>
     <row r="78" spans="1:10" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="67" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B78" s="67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C78" s="67" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D78" s="67">
         <v>1</v>
@@ -7300,18 +7280,18 @@
         <v>816</v>
       </c>
       <c r="I78" s="67" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:10" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="67" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B79" s="67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C79" s="67" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D79" s="67">
         <v>1</v>
@@ -7326,13 +7306,13 @@
     </row>
     <row r="80" spans="1:10" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="67" t="s">
+        <v>443</v>
+      </c>
+      <c r="B80" s="67" t="s">
+        <v>164</v>
+      </c>
+      <c r="C80" s="67" t="s">
         <v>444</v>
-      </c>
-      <c r="B80" s="67" t="s">
-        <v>165</v>
-      </c>
-      <c r="C80" s="67" t="s">
-        <v>445</v>
       </c>
       <c r="D80" s="67">
         <v>1</v>
@@ -7347,13 +7327,13 @@
     </row>
     <row r="81" spans="1:6" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="67" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B81" s="67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C81" s="67" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D81" s="67">
         <v>1</v>
@@ -7368,13 +7348,13 @@
     </row>
     <row r="82" spans="1:6" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="67" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B82" s="67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C82" s="67" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D82" s="67">
         <v>1</v>
@@ -7389,13 +7369,13 @@
     </row>
     <row r="83" spans="1:6" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="67" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B83" s="67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C83" s="67" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D83" s="67">
         <v>1</v>

</xml_diff>

<commit_message>
change from BD to M series Mitutoyo objectives
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33331E9-254E-4EF6-BF42-53D685DB38B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D0EA47-A77E-4E92-8B09-6F02043FF557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9552" yWindow="6468" windowWidth="30132" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7836" yWindow="9624" windowWidth="30132" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="543">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -1112,39 +1112,9 @@
     <t>Edmund Optics</t>
   </si>
   <si>
-    <t>18-402</t>
-  </si>
-  <si>
-    <t>18-403</t>
-  </si>
-  <si>
-    <t>Mitutoyo Plan Apo Brightfield and Darkfield, 2X/0.055</t>
-  </si>
-  <si>
-    <t>Mitutoyo Plan Apo Brightfield and Darkfield, 5X/0.14</t>
-  </si>
-  <si>
-    <t>Mitutoyo Plan Apo Brightfield and Darkfield 7.5X/0.21</t>
-  </si>
-  <si>
-    <t>18-404</t>
-  </si>
-  <si>
-    <t>Mitutoyo Plan Apo Brightfield and Darkfield 10x/0.28</t>
-  </si>
-  <si>
-    <t>18-405</t>
-  </si>
-  <si>
     <t>Mitutoyo-BD-black-ring.ipt</t>
   </si>
   <si>
-    <t>M2M40S</t>
-  </si>
-  <si>
-    <t>SM2 adapter for Mitutoyo objectives</t>
-  </si>
-  <si>
     <t>Hardware store</t>
   </si>
   <si>
@@ -1263,12 +1233,6 @@
   </si>
   <si>
     <t>Extends the SM2E60 and mounts to the SM2NFM2</t>
-  </si>
-  <si>
-    <t>Works better with Olympus SWTLU-C tube lens</t>
-  </si>
-  <si>
-    <t>Works best with the Mitutoyo MT-1 tube lens</t>
   </si>
   <si>
     <t>Galvo assembly: OPTIONAL</t>
@@ -1469,19 +1433,7 @@
     <t>One module serves both arms, fiber switching mechanism built-in.</t>
   </si>
   <si>
-    <t>Works best with the Mitutoyo MT-1 tube lens. Optional.</t>
-  </si>
-  <si>
-    <t>378-847</t>
-  </si>
-  <si>
-    <t>Mitutoyo</t>
-  </si>
-  <si>
     <t>Mitutoyo G Plan APO 20X/t3,5</t>
-  </si>
-  <si>
-    <t>Corrected for 3.5 mm of glass (n1.52). Thread is unusual, but fits SM1.</t>
   </si>
   <si>
     <t>f=100 mm, Ø1" Achromatic Doublet, SM1-Threaded Mount, ARC: 400-700 nm</t>
@@ -1727,44 +1679,74 @@
     <t>Includes switching module between 2 laser ports, controlled by TTL signal. The 405nm is NOT included!</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Back cover for the Mitutoyo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>BD</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> objectives</t>
-    </r>
-  </si>
-  <si>
-    <t>Only needed for BD-series objectives.</t>
-  </si>
-  <si>
     <t>Connects the Chassis to the PC. Can be replaced with more modern two-port PCIe-8362 for a higher price.</t>
   </si>
   <si>
     <t>The signal generation card, 8 analog and 8 digital channels. Potentially replaceable with two NI-PCIe-6323 cards (and no chassis), but this needs testing and possibly software changes.</t>
+  </si>
+  <si>
+    <t>59-875</t>
+  </si>
+  <si>
+    <t>Mitutoyo M Plan Apo, 2X/0.055</t>
+  </si>
+  <si>
+    <t>Mitutoyo M Plan Apo, 5X/0.14</t>
+  </si>
+  <si>
+    <t>Mitutoyo M Plan Apo 7.5X/0.21</t>
+  </si>
+  <si>
+    <t>59-876</t>
+  </si>
+  <si>
+    <t>66-383</t>
+  </si>
+  <si>
+    <t>Mitutoyo M Plan Apo 10x/0.28</t>
+  </si>
+  <si>
+    <t>59-877</t>
+  </si>
+  <si>
+    <t>58-175</t>
+  </si>
+  <si>
+    <t>Works best with the Mitutoyo MT-1 tube lens.  Thread M26 x 36TPI</t>
+  </si>
+  <si>
+    <t>Works better with Olympus SWTLU-C tube lens.  Thread M26 x 36TPI</t>
+  </si>
+  <si>
+    <t>SM1A27</t>
+  </si>
+  <si>
+    <t>Adapter with External SM1 Threads and Internal M26 x 0.706 (36 TPI) Threads</t>
+  </si>
+  <si>
+    <t>SM2A6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Adapter with External SM2 Threads and Internal SM1 Threads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adapter from objective to ZWO filter wheel, part 1 </t>
+  </si>
+  <si>
+    <t>Adapter from objective to ZWO filter wheel, part 2</t>
+  </si>
+  <si>
+    <t>Not ideal (requires gluing it to SM2 ring), would be better to have all metal (cutom) part. TODO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrected for 3.5 mm of glass (n1.52). Thread M26 x 36TPI. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1936,13 +1918,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -2038,7 +2013,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -2116,11 +2091,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -2145,10 +2118,11 @@
     <xf numFmtId="1" fontId="5" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Excel Built-in Heading 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2536,10 +2510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J177"/>
+  <dimension ref="A1:J174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I110" sqref="I110"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I97" sqref="I97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,8 +2522,8 @@
     <col min="2" max="2" width="24.109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="81.77734375" style="3" customWidth="1"/>
     <col min="4" max="4" width="6.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" style="75" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="75" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" style="73" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="73" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="24" style="3" customWidth="1"/>
     <col min="9" max="9" width="69.33203125" style="3" customWidth="1"/>
@@ -2557,12 +2531,12 @@
     <col min="11" max="16384" width="8.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="98" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
-        <v>536</v>
-      </c>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
+    <row r="1" spans="1:9" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="95" t="s">
+        <v>520</v>
+      </c>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2577,11 +2551,11 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="74" t="s">
-        <v>530</v>
-      </c>
-      <c r="F2" s="74" t="s">
-        <v>529</v>
+      <c r="E2" s="72" t="s">
+        <v>514</v>
+      </c>
+      <c r="F2" s="72" t="s">
+        <v>513</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -2597,8 +2571,8 @@
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -2613,10 +2587,10 @@
       <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="75">
+      <c r="E4" s="73">
         <v>12350</v>
       </c>
-      <c r="F4" s="75">
+      <c r="F4" s="73">
         <f>E4*D4</f>
         <v>12350</v>
       </c>
@@ -2631,21 +2605,21 @@
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
-      <c r="E5" s="77"/>
+      <c r="E5" s="75"/>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
     </row>
     <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -2657,10 +2631,10 @@
       <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="75">
+      <c r="E8" s="73">
         <v>25000</v>
       </c>
-      <c r="F8" s="75">
+      <c r="F8" s="73">
         <f>D8*E8</f>
         <v>25000</v>
       </c>
@@ -2668,15 +2642,15 @@
         <v>41</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>537</v>
+        <v>521</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
     </row>
     <row r="10" spans="1:9" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
@@ -2686,15 +2660,15 @@
         <v>19</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="D10" s="54">
         <v>0</v>
       </c>
-      <c r="E10" s="78">
+      <c r="E10" s="76">
         <v>6500</v>
       </c>
-      <c r="F10" s="78">
+      <c r="F10" s="76">
         <f t="shared" ref="F10:F26" si="0">E10*D10</f>
         <v>0</v>
       </c>
@@ -2718,7 +2692,7 @@
       <c r="D11" s="44">
         <v>0</v>
       </c>
-      <c r="E11" s="79">
+      <c r="E11" s="77">
         <v>2250</v>
       </c>
       <c r="F11" s="57">
@@ -2745,7 +2719,7 @@
       <c r="D12" s="44">
         <v>0</v>
       </c>
-      <c r="E12" s="79">
+      <c r="E12" s="77">
         <v>160</v>
       </c>
       <c r="F12" s="57">
@@ -2761,18 +2735,18 @@
     </row>
     <row r="13" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>535</v>
+        <v>519</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="D13" s="44">
         <v>1</v>
       </c>
-      <c r="E13" s="79">
+      <c r="E13" s="77">
         <v>160</v>
       </c>
       <c r="F13" s="57">
@@ -2783,7 +2757,7 @@
         <v>258</v>
       </c>
       <c r="I13" s="44" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2799,7 +2773,7 @@
       <c r="D14" s="44">
         <v>0</v>
       </c>
-      <c r="E14" s="79">
+      <c r="E14" s="77">
         <v>2250</v>
       </c>
       <c r="F14" s="57">
@@ -2829,7 +2803,7 @@
       <c r="D15" s="44">
         <v>0</v>
       </c>
-      <c r="E15" s="79">
+      <c r="E15" s="77">
         <v>230</v>
       </c>
       <c r="F15" s="57">
@@ -2856,7 +2830,7 @@
       <c r="D16" s="44">
         <v>0</v>
       </c>
-      <c r="E16" s="79">
+      <c r="E16" s="77">
         <v>2425</v>
       </c>
       <c r="F16" s="57">
@@ -2872,18 +2846,18 @@
     </row>
     <row r="17" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="B17" s="44" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="D17" s="44">
         <v>0</v>
       </c>
-      <c r="E17" s="79">
+      <c r="E17" s="77">
         <v>3000</v>
       </c>
       <c r="F17" s="57">
@@ -2894,7 +2868,7 @@
         <v>258</v>
       </c>
       <c r="I17" s="44" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2910,10 +2884,10 @@
       <c r="D18" s="54">
         <v>0</v>
       </c>
-      <c r="E18" s="80">
+      <c r="E18" s="78">
         <v>150</v>
       </c>
-      <c r="F18" s="78">
+      <c r="F18" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2925,7 +2899,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="71" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="54" t="s">
@@ -2937,10 +2911,10 @@
       <c r="D19" s="54">
         <v>0</v>
       </c>
-      <c r="E19" s="80">
+      <c r="E19" s="78">
         <v>3000</v>
       </c>
-      <c r="F19" s="78">
+      <c r="F19" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2953,26 +2927,26 @@
     </row>
     <row r="20" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>528</v>
+        <v>512</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
       </c>
-      <c r="E20" s="81">
+      <c r="E20" s="79">
         <v>19965</v>
       </c>
-      <c r="F20" s="82">
+      <c r="F20" s="80">
         <f t="shared" si="0"/>
         <v>19965</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>532</v>
+        <v>516</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -2980,8 +2954,8 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="75"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="73"/>
     </row>
     <row r="22" spans="1:9" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="54" t="s">
@@ -2996,10 +2970,10 @@
       <c r="D22" s="54">
         <v>0</v>
       </c>
-      <c r="E22" s="80">
+      <c r="E22" s="78">
         <v>5800</v>
       </c>
-      <c r="F22" s="78">
+      <c r="F22" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3011,7 +2985,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="71" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="54" t="s">
@@ -3023,10 +2997,10 @@
       <c r="D23" s="54">
         <v>0</v>
       </c>
-      <c r="E23" s="78">
+      <c r="E23" s="76">
         <v>1100</v>
       </c>
-      <c r="F23" s="78">
+      <c r="F23" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3039,49 +3013,49 @@
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>527</v>
+        <v>511</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
       </c>
-      <c r="E24" s="82">
+      <c r="E24" s="80">
         <v>6900</v>
       </c>
-      <c r="F24" s="82">
+      <c r="F24" s="80">
         <f t="shared" si="0"/>
         <v>6900</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>533</v>
+        <v>517</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
     </row>
     <row r="26" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="51" t="s">
-        <v>521</v>
+        <v>505</v>
       </c>
       <c r="B26" s="51" t="s">
         <v>63</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>522</v>
+        <v>506</v>
       </c>
       <c r="D26" s="51">
         <v>4</v>
       </c>
-      <c r="E26" s="75">
+      <c r="E26" s="73">
         <v>27</v>
       </c>
-      <c r="F26" s="75">
+      <c r="F26" s="73">
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
@@ -3089,15 +3063,15 @@
         <v>258</v>
       </c>
       <c r="I26" s="51" t="s">
-        <v>523</v>
+        <v>507</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="E27" s="76"/>
-      <c r="F27" s="76"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -3112,10 +3086,10 @@
       <c r="D28" s="3">
         <v>2</v>
       </c>
-      <c r="E28" s="75">
+      <c r="E28" s="73">
         <v>70</v>
       </c>
-      <c r="F28" s="75">
+      <c r="F28" s="73">
         <f t="shared" ref="F28:F33" si="1">E28*D28</f>
         <v>140</v>
       </c>
@@ -3139,10 +3113,10 @@
       <c r="D29" s="3">
         <v>6</v>
       </c>
-      <c r="E29" s="75">
+      <c r="E29" s="73">
         <v>36</v>
       </c>
-      <c r="F29" s="75">
+      <c r="F29" s="73">
         <f t="shared" si="1"/>
         <v>216</v>
       </c>
@@ -3166,10 +3140,10 @@
       <c r="D30" s="3">
         <v>1</v>
       </c>
-      <c r="E30" s="75">
+      <c r="E30" s="73">
         <v>43</v>
       </c>
-      <c r="F30" s="75">
+      <c r="F30" s="73">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
@@ -3193,10 +3167,10 @@
       <c r="D31" s="3">
         <v>1</v>
       </c>
-      <c r="E31" s="75">
+      <c r="E31" s="73">
         <v>29</v>
       </c>
-      <c r="F31" s="75">
+      <c r="F31" s="73">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
@@ -3220,10 +3194,10 @@
       <c r="D32" s="3">
         <v>1</v>
       </c>
-      <c r="E32" s="75">
+      <c r="E32" s="73">
         <v>195</v>
       </c>
-      <c r="F32" s="75">
+      <c r="F32" s="73">
         <f t="shared" si="1"/>
         <v>195</v>
       </c>
@@ -3247,10 +3221,10 @@
       <c r="D33" s="3">
         <v>1</v>
       </c>
-      <c r="E33" s="75">
+      <c r="E33" s="73">
         <v>10</v>
       </c>
-      <c r="F33" s="75">
+      <c r="F33" s="73">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -3262,15 +3236,15 @@
       <c r="A34" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="84"/>
-      <c r="F34" s="84"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="82"/>
     </row>
     <row r="35" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>456</v>
-      </c>
-      <c r="E35" s="84"/>
-      <c r="F35" s="84"/>
+        <v>444</v>
+      </c>
+      <c r="E35" s="82"/>
+      <c r="F35" s="82"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C36" s="3" t="s">
@@ -3279,10 +3253,10 @@
       <c r="D36" s="3">
         <v>1</v>
       </c>
-      <c r="E36" s="75" t="s">
+      <c r="E36" s="73" t="s">
         <v>319</v>
       </c>
-      <c r="F36" s="75">
+      <c r="F36" s="73">
         <v>0</v>
       </c>
     </row>
@@ -3290,8 +3264,8 @@
       <c r="A38" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="E38" s="76"/>
-      <c r="F38" s="76"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
@@ -3306,10 +3280,10 @@
       <c r="D39" s="3">
         <v>2</v>
       </c>
-      <c r="E39" s="75">
+      <c r="E39" s="73">
         <v>780</v>
       </c>
-      <c r="F39" s="75">
+      <c r="F39" s="73">
         <f t="shared" ref="F39:F44" si="2">E39*D39</f>
         <v>1560</v>
       </c>
@@ -3333,10 +3307,10 @@
       <c r="D40" s="4">
         <v>2</v>
       </c>
-      <c r="E40" s="82">
+      <c r="E40" s="80">
         <v>280</v>
       </c>
-      <c r="F40" s="82">
+      <c r="F40" s="80">
         <f t="shared" si="2"/>
         <v>560</v>
       </c>
@@ -3347,7 +3321,7 @@
         <v>42</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3363,10 +3337,10 @@
       <c r="D41" s="3">
         <v>2</v>
       </c>
-      <c r="E41" s="75">
+      <c r="E41" s="73">
         <v>85</v>
       </c>
-      <c r="F41" s="75">
+      <c r="F41" s="73">
         <f t="shared" si="2"/>
         <v>170</v>
       </c>
@@ -3390,10 +3364,10 @@
       <c r="D42" s="23">
         <v>2</v>
       </c>
-      <c r="E42" s="85">
+      <c r="E42" s="83">
         <v>13</v>
       </c>
-      <c r="F42" s="86">
+      <c r="F42" s="84">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
@@ -3417,10 +3391,10 @@
       <c r="D43" s="3">
         <v>2</v>
       </c>
-      <c r="E43" s="75">
+      <c r="E43" s="73">
         <v>17</v>
       </c>
-      <c r="F43" s="75">
+      <c r="F43" s="73">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
@@ -3444,10 +3418,10 @@
       <c r="D44" s="23">
         <v>2</v>
       </c>
-      <c r="E44" s="85">
+      <c r="E44" s="83">
         <v>18</v>
       </c>
-      <c r="F44" s="86">
+      <c r="F44" s="84">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
@@ -3471,10 +3445,10 @@
       <c r="D45" s="3">
         <v>1</v>
       </c>
-      <c r="E45" s="75">
+      <c r="E45" s="73">
         <v>30</v>
       </c>
-      <c r="F45" s="75">
+      <c r="F45" s="73">
         <v>30</v>
       </c>
       <c r="G45" s="3" t="s">
@@ -3492,7 +3466,7 @@
         <v>91863</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>49</v>
@@ -3500,10 +3474,10 @@
       <c r="D46" s="4">
         <v>2</v>
       </c>
-      <c r="E46" s="82">
+      <c r="E46" s="80">
         <v>400</v>
       </c>
-      <c r="F46" s="82">
+      <c r="F46" s="80">
         <f t="shared" ref="F46:F75" si="3">E46*D46</f>
         <v>800</v>
       </c>
@@ -3514,26 +3488,26 @@
         <v>216</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>509</v>
+        <v>493</v>
       </c>
     </row>
     <row r="47" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>475</v>
+        <v>459</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>501</v>
-      </c>
-      <c r="C47" s="97" t="s">
-        <v>474</v>
+        <v>485</v>
+      </c>
+      <c r="C47" s="94" t="s">
+        <v>458</v>
       </c>
       <c r="D47" s="4">
         <v>2</v>
       </c>
-      <c r="E47" s="82">
+      <c r="E47" s="80">
         <v>300</v>
       </c>
-      <c r="F47" s="82">
+      <c r="F47" s="80">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
@@ -3544,7 +3518,7 @@
         <v>243</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3560,10 +3534,10 @@
       <c r="D48" s="27">
         <v>0</v>
       </c>
-      <c r="E48" s="87">
+      <c r="E48" s="85">
         <v>40</v>
       </c>
-      <c r="F48" s="88">
+      <c r="F48" s="86">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3574,7 +3548,7 @@
         <v>243</v>
       </c>
       <c r="I48" s="27" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
       <c r="J48" s="64"/>
     </row>
@@ -3591,10 +3565,10 @@
       <c r="D49" s="27">
         <v>0</v>
       </c>
-      <c r="E49" s="87">
+      <c r="E49" s="85">
         <v>92</v>
       </c>
-      <c r="F49" s="88">
+      <c r="F49" s="86">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3605,7 +3579,7 @@
         <v>243</v>
       </c>
       <c r="I49" s="27" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3621,10 +3595,10 @@
       <c r="D50" s="23">
         <v>2</v>
       </c>
-      <c r="E50" s="85">
-        <v>1</v>
-      </c>
-      <c r="F50" s="86">
+      <c r="E50" s="83">
+        <v>1</v>
+      </c>
+      <c r="F50" s="84">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
@@ -3651,10 +3625,10 @@
       <c r="D51" s="23">
         <v>2</v>
       </c>
-      <c r="E51" s="85">
+      <c r="E51" s="83">
         <v>31</v>
       </c>
-      <c r="F51" s="86">
+      <c r="F51" s="84">
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
@@ -3681,10 +3655,10 @@
       <c r="D52" s="26">
         <v>10</v>
       </c>
-      <c r="E52" s="89">
+      <c r="E52" s="87">
         <v>16</v>
       </c>
-      <c r="F52" s="90">
+      <c r="F52" s="88">
         <f t="shared" si="3"/>
         <v>160</v>
       </c>
@@ -3711,10 +3685,10 @@
       <c r="D53" s="26">
         <v>2</v>
       </c>
-      <c r="E53" s="89">
+      <c r="E53" s="87">
         <v>41</v>
       </c>
-      <c r="F53" s="90">
+      <c r="F53" s="88">
         <f t="shared" si="3"/>
         <v>82</v>
       </c>
@@ -3741,10 +3715,10 @@
       <c r="D54" s="23">
         <v>2</v>
       </c>
-      <c r="E54" s="85">
+      <c r="E54" s="83">
         <v>99</v>
       </c>
-      <c r="F54" s="86">
+      <c r="F54" s="84">
         <f t="shared" si="3"/>
         <v>198</v>
       </c>
@@ -3766,15 +3740,15 @@
         <v>63</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="D55" s="23">
         <v>4</v>
       </c>
-      <c r="E55" s="85">
+      <c r="E55" s="83">
         <v>104</v>
       </c>
-      <c r="F55" s="86">
+      <c r="F55" s="84">
         <f t="shared" si="3"/>
         <v>416</v>
       </c>
@@ -3782,10 +3756,10 @@
         <v>41</v>
       </c>
       <c r="H55" s="23" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3801,10 +3775,10 @@
       <c r="D56" s="26">
         <v>4</v>
       </c>
-      <c r="E56" s="89">
+      <c r="E56" s="87">
         <v>189</v>
       </c>
-      <c r="F56" s="90">
+      <c r="F56" s="88">
         <f t="shared" si="3"/>
         <v>756</v>
       </c>
@@ -3831,10 +3805,10 @@
       <c r="D57" s="26">
         <v>4</v>
       </c>
-      <c r="E57" s="89">
+      <c r="E57" s="87">
         <v>110</v>
       </c>
-      <c r="F57" s="90">
+      <c r="F57" s="88">
         <f t="shared" si="3"/>
         <v>440</v>
       </c>
@@ -3861,10 +3835,10 @@
       <c r="D58" s="23">
         <v>4</v>
       </c>
-      <c r="E58" s="85">
+      <c r="E58" s="83">
         <v>13</v>
       </c>
-      <c r="F58" s="86">
+      <c r="F58" s="84">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
@@ -3891,10 +3865,10 @@
       <c r="D59" s="23">
         <v>2</v>
       </c>
-      <c r="E59" s="85">
+      <c r="E59" s="83">
         <v>8</v>
       </c>
-      <c r="F59" s="86">
+      <c r="F59" s="84">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
@@ -3918,10 +3892,10 @@
       <c r="D60" s="23">
         <v>4</v>
       </c>
-      <c r="E60" s="85">
+      <c r="E60" s="83">
         <v>7</v>
       </c>
-      <c r="F60" s="86">
+      <c r="F60" s="84">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
@@ -3948,10 +3922,10 @@
       <c r="D61" s="23">
         <v>6</v>
       </c>
-      <c r="E61" s="85">
+      <c r="E61" s="83">
         <v>5</v>
       </c>
-      <c r="F61" s="86">
+      <c r="F61" s="84">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
@@ -3978,10 +3952,10 @@
       <c r="D62" s="23">
         <v>4</v>
       </c>
-      <c r="E62" s="85">
+      <c r="E62" s="83">
         <v>6</v>
       </c>
-      <c r="F62" s="86">
+      <c r="F62" s="84">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
@@ -4008,10 +3982,10 @@
       <c r="D63" s="23">
         <v>4</v>
       </c>
-      <c r="E63" s="85">
+      <c r="E63" s="83">
         <v>5</v>
       </c>
-      <c r="F63" s="86">
+      <c r="F63" s="84">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
@@ -4038,10 +4012,10 @@
       <c r="D64" s="23">
         <v>2</v>
       </c>
-      <c r="E64" s="85">
+      <c r="E64" s="83">
         <v>5</v>
       </c>
-      <c r="F64" s="86">
+      <c r="F64" s="84">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -4065,10 +4039,10 @@
       <c r="D65" s="26">
         <v>2</v>
       </c>
-      <c r="E65" s="89">
+      <c r="E65" s="87">
         <v>398</v>
       </c>
-      <c r="F65" s="90">
+      <c r="F65" s="88">
         <f t="shared" si="3"/>
         <v>796</v>
       </c>
@@ -4084,10 +4058,10 @@
     </row>
     <row r="66" spans="1:9" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="62" t="s">
-        <v>497</v>
+        <v>481</v>
       </c>
       <c r="B66" s="27" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="C66" s="25" t="s">
         <v>320</v>
@@ -4095,10 +4069,10 @@
       <c r="D66" s="26">
         <v>2</v>
       </c>
-      <c r="E66" s="89">
+      <c r="E66" s="87">
         <v>150</v>
       </c>
-      <c r="F66" s="90">
+      <c r="F66" s="88">
         <f t="shared" si="3"/>
         <v>300</v>
       </c>
@@ -4125,10 +4099,10 @@
       <c r="D67" s="26">
         <v>2</v>
       </c>
-      <c r="E67" s="89">
+      <c r="E67" s="87">
         <v>30</v>
       </c>
-      <c r="F67" s="90">
+      <c r="F67" s="88">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
@@ -4144,21 +4118,21 @@
     </row>
     <row r="68" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="31" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="B68" s="27" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="C68" s="24" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
       <c r="D68" s="23">
         <v>2</v>
       </c>
-      <c r="E68" s="85">
+      <c r="E68" s="83">
         <v>300</v>
       </c>
-      <c r="F68" s="86">
+      <c r="F68" s="84">
         <f t="shared" ref="F68" si="4">E68*D68</f>
         <v>600</v>
       </c>
@@ -4169,26 +4143,26 @@
         <v>240</v>
       </c>
       <c r="I68" s="27" t="s">
-        <v>479</v>
+        <v>463</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="24" t="s">
-        <v>481</v>
+        <v>465</v>
       </c>
       <c r="B69" s="58" t="s">
         <v>63</v>
       </c>
       <c r="C69" s="59" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="D69" s="58">
         <v>0</v>
       </c>
-      <c r="E69" s="91">
+      <c r="E69" s="89">
         <v>36</v>
       </c>
-      <c r="F69" s="92">
+      <c r="F69" s="90">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4199,7 +4173,7 @@
         <v>240</v>
       </c>
       <c r="I69" s="58" t="s">
-        <v>480</v>
+        <v>464</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -4215,10 +4189,10 @@
       <c r="D70" s="23">
         <v>2</v>
       </c>
-      <c r="E70" s="85">
+      <c r="E70" s="83">
         <v>2104</v>
       </c>
-      <c r="F70" s="86">
+      <c r="F70" s="84">
         <f t="shared" si="3"/>
         <v>4208</v>
       </c>
@@ -4229,7 +4203,7 @@
         <v>240</v>
       </c>
       <c r="I70" s="23" t="s">
-        <v>478</v>
+        <v>462</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -4245,10 +4219,10 @@
       <c r="D71" s="23">
         <v>2</v>
       </c>
-      <c r="E71" s="85">
+      <c r="E71" s="83">
         <v>82</v>
       </c>
-      <c r="F71" s="86">
+      <c r="F71" s="84">
         <f t="shared" si="3"/>
         <v>164</v>
       </c>
@@ -4261,21 +4235,21 @@
     </row>
     <row r="72" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="30" t="s">
-        <v>498</v>
+        <v>482</v>
       </c>
       <c r="B72" s="23" t="s">
         <v>63</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>499</v>
+        <v>483</v>
       </c>
       <c r="D72" s="23">
         <v>1</v>
       </c>
-      <c r="E72" s="85">
+      <c r="E72" s="83">
         <v>520</v>
       </c>
-      <c r="F72" s="86">
+      <c r="F72" s="84">
         <f t="shared" si="3"/>
         <v>520</v>
       </c>
@@ -4302,10 +4276,10 @@
       <c r="D73" s="58">
         <v>0</v>
       </c>
-      <c r="E73" s="91">
+      <c r="E73" s="89">
         <v>390</v>
       </c>
-      <c r="F73" s="92">
+      <c r="F73" s="90">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4324,7 +4298,7 @@
         <v>328</v>
       </c>
       <c r="B74" s="27" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="C74" s="24" t="s">
         <v>327</v>
@@ -4332,10 +4306,10 @@
       <c r="D74" s="23">
         <v>14</v>
       </c>
-      <c r="E74" s="85">
+      <c r="E74" s="83">
         <v>20</v>
       </c>
-      <c r="F74" s="86">
+      <c r="F74" s="84">
         <f t="shared" si="3"/>
         <v>280</v>
       </c>
@@ -4362,10 +4336,10 @@
       <c r="D75" s="23">
         <v>1</v>
       </c>
-      <c r="E75" s="85">
+      <c r="E75" s="83">
         <v>10</v>
       </c>
-      <c r="F75" s="86">
+      <c r="F75" s="84">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -4379,864 +4353,924 @@
         <v>332</v>
       </c>
     </row>
-    <row r="76" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="24"/>
-      <c r="C76" s="24"/>
-      <c r="E76" s="85"/>
-      <c r="F76" s="86"/>
+    <row r="76" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E76" s="74"/>
+      <c r="F76" s="74"/>
     </row>
     <row r="77" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="24"/>
-      <c r="C77" s="24"/>
-      <c r="E77" s="85"/>
-      <c r="F77" s="86"/>
+      <c r="A77" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B77" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D77" s="23">
+        <v>1</v>
+      </c>
+      <c r="E77" s="83"/>
+      <c r="F77" s="84"/>
+      <c r="I77" s="23" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="78" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="24"/>
-      <c r="C78" s="24"/>
-      <c r="E78" s="85"/>
-      <c r="F78" s="86"/>
-    </row>
-    <row r="79" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="E79" s="76"/>
-      <c r="F79" s="76"/>
+      <c r="A78" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="B78" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C78" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="D78" s="23">
+        <v>1</v>
+      </c>
+      <c r="E78" s="83">
+        <v>63</v>
+      </c>
+      <c r="F78" s="84">
+        <f>D78*E78</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="B79" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="D79" s="23">
+        <v>2</v>
+      </c>
+      <c r="E79" s="83">
+        <v>69</v>
+      </c>
+      <c r="F79" s="84">
+        <f>D79*E79</f>
+        <v>138</v>
+      </c>
     </row>
     <row r="80" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="24" t="s">
-        <v>24</v>
+      <c r="A80" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="B80" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C80" s="24" t="s">
-        <v>21</v>
+      <c r="C80" s="23" t="s">
+        <v>23</v>
       </c>
       <c r="D80" s="23">
         <v>1</v>
       </c>
-      <c r="E80" s="85"/>
-      <c r="F80" s="86"/>
+      <c r="E80" s="83"/>
+      <c r="F80" s="84"/>
       <c r="I80" s="23" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="B81" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C81" s="24" t="s">
-        <v>264</v>
-      </c>
-      <c r="D81" s="23">
-        <v>1</v>
-      </c>
-      <c r="E81" s="85">
-        <v>63</v>
-      </c>
-      <c r="F81" s="86">
-        <f>D81*E81</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="28" t="s">
-        <v>268</v>
-      </c>
-      <c r="B82" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C82" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="D82" s="23">
+    <row r="81" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="E81" s="74"/>
+      <c r="F81" s="74"/>
+    </row>
+    <row r="82" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="E82" s="74"/>
+      <c r="F82" s="74"/>
+    </row>
+    <row r="83" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C83" s="69" t="s">
+        <v>432</v>
+      </c>
+      <c r="D83" s="3">
+        <v>1</v>
+      </c>
+      <c r="E83" s="73">
+        <v>200</v>
+      </c>
+      <c r="F83" s="73">
+        <f>E83*D83</f>
+        <v>200</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="J83" s="4"/>
+    </row>
+    <row r="84" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="D84" s="4">
+        <v>5</v>
+      </c>
+      <c r="E84" s="80">
+        <v>1</v>
+      </c>
+      <c r="F84" s="80">
+        <f>E84*D84</f>
+        <v>5</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="51" t="s">
+        <v>439</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="D85" s="3">
+        <v>1</v>
+      </c>
+      <c r="E85" s="73">
+        <v>26</v>
+      </c>
+      <c r="F85" s="73">
+        <f>E85*D85</f>
+        <v>26</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="D86" s="3">
+        <v>1</v>
+      </c>
+      <c r="E86" s="73">
+        <v>37</v>
+      </c>
+      <c r="F86" s="73">
+        <f>E86*D86</f>
+        <v>37</v>
+      </c>
+      <c r="I86" s="51" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="51" t="s">
+        <v>366</v>
+      </c>
+      <c r="B87" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="C87" s="51" t="s">
+        <v>365</v>
+      </c>
+      <c r="D87" s="51">
         <v>2</v>
       </c>
-      <c r="E82" s="85">
-        <v>69</v>
-      </c>
-      <c r="F82" s="86">
-        <f>D82*E82</f>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B83" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C83" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D83" s="23">
-        <v>1</v>
-      </c>
-      <c r="E83" s="85"/>
-      <c r="F83" s="86"/>
-      <c r="I83" s="23" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="E84" s="76"/>
-      <c r="F84" s="76"/>
-    </row>
-    <row r="85" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
+      <c r="E87" s="73">
+        <v>24</v>
+      </c>
+      <c r="F87" s="73">
+        <f>E87*D87</f>
+        <v>48</v>
+      </c>
+      <c r="I87" s="23" t="s">
         <v>443</v>
       </c>
-      <c r="E85" s="76"/>
-      <c r="F85" s="76"/>
-    </row>
-    <row r="86" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="C86" s="70" t="s">
-        <v>444</v>
-      </c>
-      <c r="D86" s="3">
-        <v>1</v>
-      </c>
-      <c r="E86" s="75">
-        <v>200</v>
-      </c>
-      <c r="F86" s="75">
-        <f>E86*D86</f>
-        <v>200</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="J86" s="4"/>
-    </row>
-    <row r="87" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="4" t="s">
-        <v>510</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>520</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="D87" s="4">
-        <v>5</v>
-      </c>
-      <c r="E87" s="82">
-        <v>1</v>
-      </c>
-      <c r="F87" s="82">
-        <f>E87*D87</f>
-        <v>5</v>
-      </c>
-      <c r="I87" s="4" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="51" t="s">
-        <v>451</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="D88" s="3">
-        <v>1</v>
-      </c>
-      <c r="E88" s="75">
-        <v>26</v>
-      </c>
-      <c r="F88" s="75">
-        <f>E88*D88</f>
-        <v>26</v>
-      </c>
-      <c r="I88" s="3" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D89" s="3">
-        <v>1</v>
-      </c>
-      <c r="E89" s="75">
-        <v>37</v>
-      </c>
-      <c r="F89" s="75">
-        <f>E89*D89</f>
-        <v>37</v>
-      </c>
-      <c r="I89" s="51" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="51" t="s">
-        <v>376</v>
-      </c>
-      <c r="B90" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="C90" s="51" t="s">
+    </row>
+    <row r="88" spans="1:10" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="E88" s="91"/>
+      <c r="F88" s="91"/>
+    </row>
+    <row r="89" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="E89" s="91"/>
+      <c r="F89" s="91"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="D90" s="3">
+        <v>1</v>
+      </c>
+      <c r="E90" s="73">
+        <v>625</v>
+      </c>
+      <c r="F90" s="73">
+        <f>E90*D90</f>
+        <v>625</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A91" s="17" t="s">
         <v>375</v>
       </c>
-      <c r="D90" s="51">
-        <v>2</v>
-      </c>
-      <c r="E90" s="75">
-        <v>24</v>
-      </c>
-      <c r="F90" s="75">
-        <f>E90*D90</f>
-        <v>48</v>
-      </c>
-      <c r="I90" s="23" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="56" t="s">
-        <v>169</v>
-      </c>
-      <c r="E91" s="93"/>
-      <c r="F91" s="93"/>
-    </row>
-    <row r="92" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="E92" s="93"/>
-      <c r="F92" s="93"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>382</v>
+      <c r="E91" s="92"/>
+      <c r="F91" s="92"/>
+    </row>
+    <row r="92" spans="1:10" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="B92" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="C92" s="97" t="s">
+        <v>525</v>
+      </c>
+      <c r="D92" s="20">
+        <v>1</v>
+      </c>
+      <c r="E92" s="93">
+        <v>900</v>
+      </c>
+      <c r="F92" s="93">
+        <f t="shared" ref="F92:F98" si="5">E92*D92</f>
+        <v>900</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I92" s="20" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="B93" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="C93" s="98" t="s">
+        <v>526</v>
       </c>
       <c r="D93" s="3">
         <v>1</v>
       </c>
-      <c r="E93" s="75">
-        <v>625</v>
-      </c>
-      <c r="F93" s="75">
-        <f>E93*D93</f>
-        <v>625</v>
+      <c r="E93" s="73">
+        <v>767</v>
+      </c>
+      <c r="F93" s="93">
+        <f t="shared" si="5"/>
+        <v>767</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="H93" s="20"/>
       <c r="I93" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A94" s="17" t="s">
-        <v>385</v>
-      </c>
-      <c r="E94" s="94"/>
-      <c r="F94" s="94"/>
-    </row>
-    <row r="95" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="21" t="s">
-        <v>347</v>
+        <v>533</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="22" t="s">
+        <v>529</v>
+      </c>
+      <c r="B94" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="C94" s="98" t="s">
+        <v>527</v>
+      </c>
+      <c r="D94" s="3">
+        <v>0</v>
+      </c>
+      <c r="E94" s="73">
+        <v>1540</v>
+      </c>
+      <c r="F94" s="93">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H94" s="20"/>
+      <c r="I94" s="3" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="3" t="s">
+        <v>531</v>
       </c>
       <c r="B95" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="C95" s="71" t="s">
-        <v>349</v>
-      </c>
-      <c r="D95" s="20">
-        <v>1</v>
-      </c>
-      <c r="E95" s="95">
-        <v>912</v>
-      </c>
-      <c r="F95" s="95">
-        <f t="shared" ref="F95:F101" si="5">E95*D95</f>
-        <v>912</v>
+      <c r="C95" s="98" t="s">
+        <v>530</v>
+      </c>
+      <c r="D95" s="3">
+        <v>1</v>
+      </c>
+      <c r="E95" s="73">
+        <v>877</v>
+      </c>
+      <c r="F95" s="93">
+        <f t="shared" si="5"/>
+        <v>877</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I95" s="20" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="22" t="s">
-        <v>348</v>
+      <c r="H95" s="20"/>
+      <c r="I95" s="3" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="51" t="s">
+        <v>532</v>
       </c>
       <c r="B96" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="C96" s="72" t="s">
-        <v>350</v>
-      </c>
-      <c r="D96" s="3">
-        <v>1</v>
-      </c>
-      <c r="E96" s="75">
-        <v>837</v>
-      </c>
-      <c r="F96" s="95">
-        <f t="shared" si="5"/>
-        <v>837</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H96" s="20"/>
-      <c r="I96" s="3" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="22" t="s">
-        <v>352</v>
-      </c>
-      <c r="B97" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="C97" s="72" t="s">
-        <v>351</v>
-      </c>
-      <c r="D97" s="3">
+      <c r="C96" s="98" t="s">
+        <v>447</v>
+      </c>
+      <c r="D96" s="51">
         <v>0</v>
       </c>
-      <c r="E97" s="75">
-        <v>1540</v>
-      </c>
-      <c r="F97" s="95">
+      <c r="E96" s="73">
+        <v>4700</v>
+      </c>
+      <c r="F96" s="93">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G97" s="3" t="s">
+      <c r="G96" s="51" t="s">
         <v>13</v>
       </c>
+      <c r="H96" s="20"/>
+      <c r="I96" s="51" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="51" t="s">
+        <v>535</v>
+      </c>
+      <c r="B97" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C97" s="51" t="s">
+        <v>536</v>
+      </c>
+      <c r="D97" s="51">
+        <v>1</v>
+      </c>
+      <c r="E97" s="73">
+        <v>20</v>
+      </c>
+      <c r="F97" s="93">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="G97" s="51" t="s">
+        <v>13</v>
+      </c>
       <c r="H97" s="20"/>
-      <c r="I97" s="3" t="s">
-        <v>459</v>
+      <c r="I97" s="51" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>354</v>
+        <v>537</v>
       </c>
       <c r="B98" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="C98" s="72" t="s">
-        <v>353</v>
+        <v>63</v>
+      </c>
+      <c r="C98" s="32" t="s">
+        <v>538</v>
       </c>
       <c r="D98" s="3">
         <v>1</v>
       </c>
-      <c r="E98" s="75">
-        <v>1026</v>
-      </c>
-      <c r="F98" s="95">
+      <c r="E98" s="73">
+        <v>25</v>
+      </c>
+      <c r="F98" s="93">
         <f t="shared" si="5"/>
-        <v>1026</v>
+        <v>25</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H98" s="20"/>
-      <c r="I98" s="3" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="51" t="s">
-        <v>460</v>
-      </c>
-      <c r="B99" s="20" t="s">
-        <v>461</v>
-      </c>
-      <c r="C99" s="72" t="s">
-        <v>462</v>
-      </c>
-      <c r="D99" s="51">
-        <v>0</v>
-      </c>
-      <c r="E99" s="75">
-        <v>3670</v>
-      </c>
-      <c r="F99" s="95">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G99" s="51" t="s">
+      <c r="I98" s="51" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A99" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="E99" s="92"/>
+      <c r="F99" s="92"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B100" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="C100" s="70" t="s">
+        <v>378</v>
+      </c>
+      <c r="D100" s="3">
+        <v>1</v>
+      </c>
+      <c r="E100" s="73">
+        <v>752</v>
+      </c>
+      <c r="F100" s="73">
+        <f t="shared" ref="F100:F104" si="6">D100*E100</f>
+        <v>752</v>
+      </c>
+      <c r="G100" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H99" s="20"/>
-      <c r="I99" s="51" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="B100" s="66" t="s">
+      <c r="I100" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B101" s="66" t="s">
         <v>248</v>
       </c>
-      <c r="C100" s="67" t="s">
-        <v>538</v>
-      </c>
-      <c r="D100" s="4">
-        <v>5</v>
-      </c>
-      <c r="E100" s="82">
-        <v>1</v>
-      </c>
-      <c r="F100" s="96">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="G100" s="4" t="s">
+      <c r="C101" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="D101" s="4">
+        <v>1</v>
+      </c>
+      <c r="E101" s="80">
+        <v>1</v>
+      </c>
+      <c r="F101" s="80">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G101" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H100" s="66"/>
-      <c r="I100" s="4" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="B101" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C101" s="32" t="s">
-        <v>357</v>
-      </c>
-      <c r="D101" s="3">
-        <v>1</v>
-      </c>
-      <c r="E101" s="75">
-        <v>60</v>
-      </c>
-      <c r="F101" s="95">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="G101" s="3" t="s">
+      <c r="I101" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="D102" s="3">
+        <v>1</v>
+      </c>
+      <c r="E102" s="73">
+        <v>65</v>
+      </c>
+      <c r="F102" s="73">
+        <f t="shared" si="6"/>
+        <v>65</v>
+      </c>
+      <c r="G102" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H101" s="20"/>
-    </row>
-    <row r="102" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A102" s="17" t="s">
-        <v>386</v>
-      </c>
-      <c r="E102" s="94"/>
-      <c r="F102" s="94"/>
+      <c r="I102" s="3" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>368</v>
+        <v>385</v>
       </c>
       <c r="B103" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="C103" s="72" t="s">
-        <v>388</v>
+        <v>63</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>386</v>
       </c>
       <c r="D103" s="3">
         <v>1</v>
       </c>
-      <c r="E103" s="75">
-        <v>752</v>
-      </c>
-      <c r="F103" s="75">
-        <f t="shared" ref="F103:F107" si="6">D103*E103</f>
-        <v>752</v>
+      <c r="E103" s="73">
+        <v>32</v>
+      </c>
+      <c r="F103" s="73">
+        <f t="shared" si="6"/>
+        <v>32</v>
       </c>
       <c r="G103" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="B104" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="D104" s="4">
-        <v>1</v>
-      </c>
-      <c r="E104" s="82">
-        <v>1</v>
-      </c>
-      <c r="F104" s="82">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B104" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="D104" s="3">
+        <v>1</v>
+      </c>
+      <c r="E104" s="73">
+        <v>112</v>
+      </c>
+      <c r="F104" s="73">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="G104" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G104" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="B105" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="D105" s="3">
-        <v>1</v>
-      </c>
-      <c r="E105" s="75">
-        <v>65</v>
-      </c>
-      <c r="F105" s="75">
-        <f t="shared" si="6"/>
-        <v>65</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I105" s="3" t="s">
-        <v>394</v>
-      </c>
+      <c r="I104" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A105" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E105" s="74"/>
+      <c r="F105" s="74"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="B106" s="20" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>396</v>
+        <v>60</v>
       </c>
       <c r="D106" s="3">
         <v>1</v>
       </c>
-      <c r="E106" s="75">
-        <v>32</v>
-      </c>
-      <c r="F106" s="75">
-        <f t="shared" si="6"/>
-        <v>32</v>
+      <c r="E106" s="73">
+        <v>3582</v>
+      </c>
+      <c r="F106" s="73">
+        <f t="shared" ref="F106:F118" si="7">E106*D106</f>
+        <v>3582</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>397</v>
+        <v>523</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="B107" s="20" t="s">
-        <v>63</v>
+        <v>188</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>380</v>
+        <v>190</v>
       </c>
       <c r="D107" s="3">
         <v>1</v>
       </c>
-      <c r="E107" s="75">
-        <v>112</v>
-      </c>
-      <c r="F107" s="75">
-        <f t="shared" si="6"/>
-        <v>112</v>
+      <c r="E107" s="73">
+        <v>1630</v>
+      </c>
+      <c r="F107" s="73">
+        <f t="shared" si="7"/>
+        <v>1630</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A108" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E108" s="76"/>
-      <c r="F108" s="76"/>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D108" s="3">
+        <v>1</v>
+      </c>
+      <c r="E108" s="73">
+        <v>886</v>
+      </c>
+      <c r="F108" s="73">
+        <f t="shared" si="7"/>
+        <v>886</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>59</v>
+        <v>191</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>60</v>
+        <v>189</v>
       </c>
       <c r="D109" s="3">
         <v>1</v>
       </c>
-      <c r="E109" s="75">
-        <v>3582</v>
-      </c>
-      <c r="F109" s="75">
-        <f t="shared" ref="F109:F121" si="7">E109*D109</f>
-        <v>3582</v>
+      <c r="E109" s="73">
+        <v>163</v>
+      </c>
+      <c r="F109" s="73">
+        <f t="shared" si="7"/>
+        <v>163</v>
       </c>
       <c r="G109" s="3" t="s">
         <v>53</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>541</v>
+        <v>192</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>188</v>
+        <v>54</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D110" s="3">
         <v>1</v>
       </c>
-      <c r="E110" s="75">
-        <v>1630</v>
-      </c>
-      <c r="F110" s="75">
+      <c r="E110" s="73">
+        <v>11</v>
+      </c>
+      <c r="F110" s="73">
         <f t="shared" si="7"/>
-        <v>1630</v>
+        <v>11</v>
       </c>
       <c r="G110" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I110" s="3" t="s">
-        <v>185</v>
-      </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>187</v>
+        <v>57</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>186</v>
+        <v>58</v>
       </c>
       <c r="D111" s="3">
         <v>1</v>
       </c>
-      <c r="E111" s="75">
-        <v>886</v>
-      </c>
-      <c r="F111" s="75">
+      <c r="E111" s="73">
+        <v>520</v>
+      </c>
+      <c r="F111" s="73">
         <f t="shared" si="7"/>
-        <v>886</v>
+        <v>520</v>
       </c>
       <c r="G111" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I111" s="3" t="s">
-        <v>540</v>
-      </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D112" s="3">
         <v>1</v>
       </c>
-      <c r="E112" s="75">
-        <v>163</v>
-      </c>
-      <c r="F112" s="75">
+      <c r="E112" s="73">
+        <v>193</v>
+      </c>
+      <c r="F112" s="73">
         <f t="shared" si="7"/>
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="G112" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I112" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D113" s="3">
-        <v>1</v>
-      </c>
-      <c r="E113" s="75">
-        <v>11</v>
-      </c>
-      <c r="F113" s="75">
+    </row>
+    <row r="113" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="23" t="s">
+        <v>312</v>
+      </c>
+      <c r="B113" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C113" s="23" t="s">
+        <v>313</v>
+      </c>
+      <c r="D113" s="23">
+        <v>10</v>
+      </c>
+      <c r="E113" s="84">
+        <v>12</v>
+      </c>
+      <c r="F113" s="84">
         <f t="shared" si="7"/>
-        <v>11</v>
-      </c>
-      <c r="G113" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G113" s="23" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D114" s="3">
-        <v>1</v>
-      </c>
-      <c r="E114" s="75">
-        <v>520</v>
-      </c>
-      <c r="F114" s="75">
+      <c r="I113" s="23" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="23" t="s">
+        <v>314</v>
+      </c>
+      <c r="B114" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C114" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="D114" s="23">
+        <v>1</v>
+      </c>
+      <c r="E114" s="84">
+        <v>14</v>
+      </c>
+      <c r="F114" s="84">
         <f t="shared" si="7"/>
-        <v>520</v>
-      </c>
-      <c r="G114" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G114" s="23" t="s">
         <v>53</v>
+      </c>
+      <c r="I114" s="23" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>193</v>
+        <v>125</v>
       </c>
       <c r="D115" s="3">
-        <v>1</v>
-      </c>
-      <c r="E115" s="75">
-        <v>193</v>
-      </c>
-      <c r="F115" s="75">
+        <v>4</v>
+      </c>
+      <c r="E115" s="73">
+        <v>15.25</v>
+      </c>
+      <c r="F115" s="73">
         <f t="shared" si="7"/>
-        <v>193</v>
-      </c>
-      <c r="G115" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G115" s="23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="116" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="23" t="s">
-        <v>312</v>
-      </c>
-      <c r="B116" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C116" s="23" t="s">
-        <v>313</v>
-      </c>
-      <c r="D116" s="23">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D116" s="3">
         <v>10</v>
       </c>
-      <c r="E116" s="86">
-        <v>12</v>
-      </c>
-      <c r="F116" s="86">
+      <c r="E116" s="73">
+        <v>16.5</v>
+      </c>
+      <c r="F116" s="73">
         <f t="shared" si="7"/>
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="G116" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="I116" s="23" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="23" t="s">
-        <v>314</v>
-      </c>
-      <c r="B117" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C117" s="23" t="s">
-        <v>315</v>
-      </c>
-      <c r="D117" s="23">
-        <v>1</v>
-      </c>
-      <c r="E117" s="86">
-        <v>14</v>
-      </c>
-      <c r="F117" s="86">
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D117" s="3">
+        <v>10</v>
+      </c>
+      <c r="E117" s="73">
+        <v>24</v>
+      </c>
+      <c r="F117" s="73">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>240</v>
       </c>
       <c r="G117" s="23" t="s">
         <v>53</v>
-      </c>
-      <c r="I117" s="23" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -5247,789 +5281,717 @@
         <v>63</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D118" s="3">
-        <v>4</v>
-      </c>
-      <c r="E118" s="75">
-        <v>15.25</v>
-      </c>
-      <c r="F118" s="75">
+        <v>6</v>
+      </c>
+      <c r="E118" s="73">
+        <v>24</v>
+      </c>
+      <c r="F118" s="73">
         <f t="shared" si="7"/>
-        <v>61</v>
+        <v>144</v>
       </c>
       <c r="G118" s="23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D119" s="3">
-        <v>10</v>
-      </c>
-      <c r="E119" s="75">
+    <row r="119" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E119" s="84"/>
+      <c r="F119" s="84"/>
+    </row>
+    <row r="121" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A121" s="10"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="9"/>
+    </row>
+    <row r="122" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A122" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E122" s="74"/>
+      <c r="F122" s="74"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D123" s="3">
+        <v>4</v>
+      </c>
+      <c r="E123" s="73">
         <v>16.5</v>
       </c>
-      <c r="F119" s="75">
-        <f t="shared" si="7"/>
-        <v>165</v>
-      </c>
-      <c r="G119" s="23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D120" s="3">
-        <v>10</v>
-      </c>
-      <c r="E120" s="75">
-        <v>24</v>
-      </c>
-      <c r="F120" s="75">
-        <f t="shared" si="7"/>
-        <v>240</v>
-      </c>
-      <c r="G120" s="23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D121" s="3">
-        <v>6</v>
-      </c>
-      <c r="E121" s="75">
-        <v>24</v>
-      </c>
-      <c r="F121" s="75">
-        <f t="shared" si="7"/>
-        <v>144</v>
-      </c>
-      <c r="G121" s="23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E122" s="86"/>
-      <c r="F122" s="86"/>
-    </row>
-    <row r="124" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A124" s="10"/>
-      <c r="B124" s="10"/>
-      <c r="C124" s="9"/>
-    </row>
-    <row r="125" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E125" s="76"/>
-      <c r="F125" s="76"/>
+      <c r="F123" s="73">
+        <f t="shared" ref="F123:F138" si="8">E123*D123</f>
+        <v>66</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D124" s="3">
+        <v>1</v>
+      </c>
+      <c r="E124" s="73">
+        <v>85.1</v>
+      </c>
+      <c r="F124" s="73">
+        <f t="shared" si="8"/>
+        <v>85.1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D125" s="3">
+        <v>2</v>
+      </c>
+      <c r="E125" s="73">
+        <v>32</v>
+      </c>
+      <c r="F125" s="73">
+        <f t="shared" si="8"/>
+        <v>64</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="D126" s="3">
-        <v>4</v>
-      </c>
-      <c r="E126" s="75">
-        <v>16.5</v>
-      </c>
-      <c r="F126" s="75">
-        <f t="shared" ref="F126:F141" si="8">E126*D126</f>
-        <v>66</v>
-      </c>
-      <c r="I126" s="3" t="s">
-        <v>118</v>
+        <v>2</v>
+      </c>
+      <c r="E126" s="73">
+        <v>51.58</v>
+      </c>
+      <c r="F126" s="73">
+        <f t="shared" si="8"/>
+        <v>103.16</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="D127" s="3">
         <v>1</v>
       </c>
-      <c r="E127" s="75">
-        <v>85.1</v>
-      </c>
-      <c r="F127" s="75">
+      <c r="E127" s="73">
+        <v>60</v>
+      </c>
+      <c r="F127" s="73">
         <f t="shared" si="8"/>
-        <v>85.1</v>
+        <v>60</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D128" s="3">
-        <v>2</v>
-      </c>
-      <c r="E128" s="75">
-        <v>32</v>
-      </c>
-      <c r="F128" s="75">
-        <f t="shared" si="8"/>
-        <v>64</v>
-      </c>
-      <c r="I128" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D129" s="3">
-        <v>2</v>
-      </c>
-      <c r="E129" s="75">
-        <v>51.58</v>
-      </c>
-      <c r="F129" s="75">
-        <f t="shared" si="8"/>
-        <v>103.16</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D130" s="3">
-        <v>1</v>
-      </c>
-      <c r="E130" s="75">
-        <v>60</v>
-      </c>
-      <c r="F130" s="75">
-        <f t="shared" si="8"/>
-        <v>60</v>
-      </c>
-      <c r="I130" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D131" s="3">
-        <v>1</v>
-      </c>
-      <c r="E131" s="75">
+        <v>1</v>
+      </c>
+      <c r="E128" s="73">
         <v>136.47999999999999</v>
       </c>
-      <c r="F131" s="75">
+      <c r="F128" s="73">
         <f t="shared" si="8"/>
         <v>136.47999999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="s">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B132" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C132" s="3" t="s">
+      <c r="B129" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D132" s="3">
-        <v>1</v>
-      </c>
-      <c r="E132" s="75">
+      <c r="D129" s="3">
+        <v>1</v>
+      </c>
+      <c r="E129" s="73">
         <v>136.47999999999999</v>
       </c>
-      <c r="F132" s="75">
+      <c r="F129" s="73">
         <f t="shared" si="8"/>
         <v>136.47999999999999</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="3" t="s">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B133" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C133" s="3" t="s">
+      <c r="B130" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C130" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D133" s="3">
-        <v>1</v>
-      </c>
-      <c r="E133" s="75">
+      <c r="D130" s="3">
+        <v>1</v>
+      </c>
+      <c r="E130" s="73">
         <v>60.95</v>
       </c>
-      <c r="F133" s="75">
+      <c r="F130" s="73">
         <f t="shared" si="8"/>
         <v>60.95</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="3" t="s">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B134" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C134" s="3" t="s">
+      <c r="B131" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C131" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D134" s="3">
-        <v>1</v>
-      </c>
-      <c r="E134" s="75">
+      <c r="D131" s="3">
+        <v>1</v>
+      </c>
+      <c r="E131" s="73">
         <v>119.416</v>
       </c>
-      <c r="F134" s="75">
+      <c r="F131" s="73">
         <f t="shared" si="8"/>
         <v>119.416</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A135" s="3" t="s">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B135" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C135" s="3" t="s">
+      <c r="B132" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C132" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D135" s="3">
-        <v>1</v>
-      </c>
-      <c r="E135" s="75">
+      <c r="D132" s="3">
+        <v>1</v>
+      </c>
+      <c r="E132" s="73">
         <v>105.8</v>
       </c>
-      <c r="F135" s="75">
+      <c r="F132" s="73">
         <f t="shared" si="8"/>
         <v>105.8</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" s="3" t="s">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B136" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C136" s="3" t="s">
+      <c r="B133" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C133" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D136" s="3">
+      <c r="D133" s="3">
         <v>2</v>
       </c>
-      <c r="E136" s="75">
+      <c r="E133" s="73">
         <v>119.6</v>
       </c>
-      <c r="F136" s="75">
+      <c r="F133" s="73">
         <f t="shared" si="8"/>
         <v>239.2</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="B137" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C137" s="3" t="s">
+      <c r="B134" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C134" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="D137" s="3">
-        <v>1</v>
-      </c>
-      <c r="E137" s="75">
+      <c r="D134" s="3">
+        <v>1</v>
+      </c>
+      <c r="E134" s="73">
         <v>100</v>
       </c>
-      <c r="F137" s="75">
+      <c r="F134" s="73">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D135" s="3">
+        <v>2</v>
+      </c>
+      <c r="E135" s="73">
+        <v>92</v>
+      </c>
+      <c r="F135" s="73">
+        <f t="shared" si="8"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D136" s="3">
+        <v>1</v>
+      </c>
+      <c r="E136" s="73">
+        <v>96.23</v>
+      </c>
+      <c r="F136" s="73">
+        <f t="shared" si="8"/>
+        <v>96.23</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D137" s="3">
+        <v>1</v>
+      </c>
+      <c r="E137" s="73">
+        <v>102.44</v>
+      </c>
+      <c r="F137" s="73">
+        <f t="shared" si="8"/>
+        <v>102.44</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="D138" s="3">
         <v>2</v>
       </c>
-      <c r="E138" s="75">
-        <v>92</v>
-      </c>
-      <c r="F138" s="75">
-        <f t="shared" si="8"/>
-        <v>184</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A139" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D139" s="3">
-        <v>1</v>
-      </c>
-      <c r="E139" s="75">
-        <v>96.23</v>
-      </c>
-      <c r="F139" s="75">
-        <f t="shared" si="8"/>
-        <v>96.23</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A140" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D140" s="3">
-        <v>1</v>
-      </c>
-      <c r="E140" s="75">
-        <v>102.44</v>
-      </c>
-      <c r="F140" s="75">
-        <f t="shared" si="8"/>
-        <v>102.44</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A141" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D141" s="3">
-        <v>2</v>
-      </c>
-      <c r="E141" s="75">
+      <c r="E138" s="73">
         <v>28</v>
       </c>
-      <c r="F141" s="75">
+      <c r="F138" s="73">
         <f t="shared" si="8"/>
         <v>56</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C142" s="3" t="s">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C139" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D142" s="3">
+      <c r="D139" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C143" s="3" t="s">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C140" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D143" s="3">
-        <v>1</v>
-      </c>
-      <c r="I143" s="3" t="s">
+      <c r="D140" s="3">
+        <v>1</v>
+      </c>
+      <c r="I140" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C144" s="3" t="s">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C141" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D144" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="7" t="s">
+      <c r="D141" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A143" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B146" s="6" t="s">
+      <c r="B143" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="E146" s="76"/>
-      <c r="F146" s="76"/>
-    </row>
-    <row r="147" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="51"/>
+      <c r="E143" s="74"/>
+      <c r="F143" s="74"/>
+    </row>
+    <row r="144" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="51"/>
+      <c r="B144" s="51" t="s">
+        <v>470</v>
+      </c>
+      <c r="C144" s="53" t="s">
+        <v>162</v>
+      </c>
+      <c r="D144" s="51">
+        <v>4</v>
+      </c>
+      <c r="E144" s="73">
+        <v>40</v>
+      </c>
+      <c r="F144" s="73">
+        <f>E144*D144</f>
+        <v>160</v>
+      </c>
+      <c r="G144" s="51" t="s">
+        <v>468</v>
+      </c>
+      <c r="H144" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="I144" s="51" t="s">
+        <v>467</v>
+      </c>
+      <c r="J144" s="53"/>
+    </row>
+    <row r="145" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B145" s="51" t="s">
+        <v>164</v>
+      </c>
+      <c r="C145" s="51" t="s">
+        <v>374</v>
+      </c>
+      <c r="D145" s="51">
+        <v>2</v>
+      </c>
+      <c r="E145" s="73">
+        <v>331</v>
+      </c>
+      <c r="F145" s="73">
+        <f>E145*D145</f>
+        <v>662</v>
+      </c>
+      <c r="G145" s="51" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B146" s="51" t="s">
+        <v>164</v>
+      </c>
+      <c r="C146" s="51" t="s">
+        <v>308</v>
+      </c>
+      <c r="D146" s="51">
+        <v>4</v>
+      </c>
+      <c r="E146" s="73">
+        <v>25</v>
+      </c>
+      <c r="F146" s="73">
+        <f>E146*D146</f>
+        <v>100</v>
+      </c>
+      <c r="G146" s="51" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B147" s="51" t="s">
-        <v>486</v>
-      </c>
-      <c r="C147" s="53" t="s">
-        <v>162</v>
+        <v>164</v>
+      </c>
+      <c r="C147" s="51" t="s">
+        <v>309</v>
       </c>
       <c r="D147" s="51">
         <v>4</v>
       </c>
-      <c r="E147" s="75">
-        <v>40</v>
-      </c>
-      <c r="F147" s="75">
+      <c r="E147" s="73">
+        <v>28</v>
+      </c>
+      <c r="F147" s="73">
         <f>E147*D147</f>
-        <v>160</v>
+        <v>112</v>
       </c>
       <c r="G147" s="51" t="s">
-        <v>484</v>
-      </c>
-      <c r="H147" s="51" t="s">
-        <v>485</v>
-      </c>
-      <c r="I147" s="51" t="s">
-        <v>483</v>
-      </c>
-      <c r="J147" s="53"/>
-    </row>
-    <row r="148" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B148" s="51" t="s">
         <v>164</v>
       </c>
       <c r="C148" s="51" t="s">
-        <v>384</v>
+        <v>310</v>
       </c>
       <c r="D148" s="51">
+        <v>6</v>
+      </c>
+      <c r="E148" s="73">
+        <v>121.5</v>
+      </c>
+      <c r="F148" s="73">
+        <f>E148*D148</f>
+        <v>729</v>
+      </c>
+      <c r="G148" s="51" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E151" s="68" t="s">
+        <v>502</v>
+      </c>
+      <c r="F151" s="68">
+        <f>SUM(F3:F149)</f>
+        <v>94066.255999999994</v>
+      </c>
+      <c r="G151" s="3" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E153" s="73"/>
+      <c r="F153" s="73"/>
+    </row>
+    <row r="155" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A155" s="67" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A156" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="C156" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B157" s="3">
+        <v>14</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="B158" s="3">
         <v>2</v>
       </c>
-      <c r="E148" s="75">
-        <v>331</v>
-      </c>
-      <c r="F148" s="75">
-        <f>E148*D148</f>
-        <v>662</v>
-      </c>
-      <c r="G148" s="51" t="s">
+      <c r="C158" s="3" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="B159" s="3">
+        <v>2</v>
+      </c>
+      <c r="C159" s="51" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="149" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="51" t="s">
-        <v>164</v>
-      </c>
-      <c r="C149" s="51" t="s">
-        <v>308</v>
-      </c>
-      <c r="D149" s="51">
-        <v>4</v>
-      </c>
-      <c r="E149" s="75">
-        <v>25</v>
-      </c>
-      <c r="F149" s="75">
-        <f>E149*D149</f>
-        <v>100</v>
-      </c>
-      <c r="G149" s="51" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B150" s="51" t="s">
-        <v>164</v>
-      </c>
-      <c r="C150" s="51" t="s">
-        <v>309</v>
-      </c>
-      <c r="D150" s="51">
-        <v>4</v>
-      </c>
-      <c r="E150" s="75">
-        <v>28</v>
-      </c>
-      <c r="F150" s="75">
-        <f>E150*D150</f>
-        <v>112</v>
-      </c>
-      <c r="G150" s="51" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="151" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="51" t="s">
-        <v>164</v>
-      </c>
-      <c r="C151" s="51" t="s">
-        <v>310</v>
-      </c>
-      <c r="D151" s="51">
-        <v>6</v>
-      </c>
-      <c r="E151" s="75">
-        <v>121.5</v>
-      </c>
-      <c r="F151" s="75">
-        <f>E151*D151</f>
-        <v>729</v>
-      </c>
-      <c r="G151" s="51" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="154" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E154" s="69" t="s">
-        <v>518</v>
-      </c>
-      <c r="F154" s="69">
-        <f>SUM(F3:F152)</f>
-        <v>94317.255999999994</v>
-      </c>
-      <c r="G154" s="3" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E156" s="75"/>
-      <c r="F156" s="75"/>
-    </row>
-    <row r="158" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A158" s="68" t="s">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B160" s="3">
+        <v>2</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A163" s="67" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A164" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="C164" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B165" s="3">
+        <v>2</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A166" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B166" s="3">
+        <v>5</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B167" s="3">
+        <v>1</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A170" s="67" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A171" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="C171" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="51" t="s">
+        <v>494</v>
+      </c>
+      <c r="B172" s="3">
+        <v>5</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B173" s="3">
+        <v>3</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="159" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A159" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="B159" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="C159" s="4" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A160" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="B160" s="3">
-        <v>14</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="B161" s="3">
-        <v>2</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="3" t="s">
-        <v>494</v>
-      </c>
-      <c r="B162" s="3">
-        <v>2</v>
-      </c>
-      <c r="C162" s="51" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="B163" s="3">
-        <v>2</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A166" s="68" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A167" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="B167" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="C167" s="4" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="B168" s="3">
-        <v>2</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A169" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="B169" s="3">
-        <v>5</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="B170" s="3">
-        <v>1</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A173" s="68" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A174" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="B174" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="C174" s="4" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="51" t="s">
-        <v>510</v>
-      </c>
-      <c r="B175" s="3">
-        <v>5</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B176" s="3">
-        <v>3</v>
-      </c>
-      <c r="C176" s="3" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="3" t="s">
-        <v>516</v>
-      </c>
-      <c r="B177" s="3" t="s">
+      <c r="B174" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="C177" s="3" t="s">
-        <v>517</v>
+      <c r="C174" s="3" t="s">
+        <v>501</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C95" r:id="rId1" display="Mitutoyo Plan Apo Brightfield and Darkfield, 2X" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C96" r:id="rId2" display="Plan Apo" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C97" r:id="rId3" display="Plan Apo" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C98" r:id="rId4" display="Plan Apo Brightfield and Darkfield " xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C103" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C86" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C99" r:id="rId7" xr:uid="{3002EF90-377A-4FAD-A836-B22D0D243A96}"/>
+    <hyperlink ref="C92" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C93" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C94" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C95" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C100" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C83" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C96" r:id="rId7" xr:uid="{3002EF90-377A-4FAD-A836-B22D0D243A96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
@@ -6112,7 +6074,7 @@
         <v>7400</v>
       </c>
       <c r="I3" s="44" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6138,10 +6100,10 @@
     </row>
     <row r="5" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="D5" s="33">
         <v>1</v>
@@ -6153,13 +6115,13 @@
         <v>50000</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -6182,27 +6144,27 @@
         <v>25000</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:9" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B12" s="34" t="s">
         <v>346</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="D12" s="33">
         <v>1</v>
@@ -6218,21 +6180,21 @@
         <v>13</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>346</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="D13" s="33">
         <v>1</v>
@@ -6248,21 +6210,21 @@
         <v>13</v>
       </c>
       <c r="H13" s="33" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="I13" s="33" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>63</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="D14" s="33">
         <v>1</v>
@@ -6278,21 +6240,21 @@
         <v>13</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="I14" s="33" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>63</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="D15" s="33">
         <v>1</v>
@@ -6308,10 +6270,10 @@
         <v>13</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="I15" s="33" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6338,22 +6300,22 @@
         <v>13</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="I16" s="34" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -6462,14 +6424,14 @@
     </row>
     <row r="24" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" s="42" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
@@ -6498,7 +6460,7 @@
         <v>41</v>
       </c>
       <c r="H26" s="34" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="I26" s="34" t="s">
         <v>337</v>
@@ -6528,7 +6490,7 @@
         <v>41</v>
       </c>
       <c r="H27" s="34" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="I27" s="34" t="s">
         <v>341</v>
@@ -6539,10 +6501,10 @@
         <v>319</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="D28" s="34">
         <v>8</v>
@@ -6558,21 +6520,21 @@
         <v>41</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="I28" s="34" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B29" s="34" t="s">
         <v>63</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="D29" s="34">
         <v>6</v>
@@ -6588,18 +6550,18 @@
         <v>41</v>
       </c>
       <c r="H29" s="34" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="B30" s="34" t="s">
         <v>248</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="D30" s="34">
         <v>2</v>
@@ -6615,10 +6577,10 @@
         <v>41</v>
       </c>
       <c r="H30" s="34" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="I30" s="34" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6645,7 +6607,7 @@
         <v>41</v>
       </c>
       <c r="H31" s="34" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="I31" s="34" t="s">
         <v>343</v>
@@ -6675,7 +6637,7 @@
         <v>41</v>
       </c>
       <c r="H32" s="34" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="I32" s="34" t="s">
         <v>345</v>
@@ -6705,7 +6667,7 @@
         <v>41</v>
       </c>
       <c r="H33" s="34" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -6739,7 +6701,7 @@
         <v>53</v>
       </c>
       <c r="I38" s="44" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -7241,7 +7203,7 @@
     </row>
     <row r="66" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="F66" s="8"/>
     </row>
@@ -7266,18 +7228,18 @@
         <v>280</v>
       </c>
       <c r="I67" s="33" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="B68" s="47" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="C68" s="47" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="D68" s="47">
         <v>2</v>
@@ -7290,18 +7252,18 @@
         <v>168</v>
       </c>
       <c r="I68" s="47" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="B69" s="47" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="C69" s="47" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="D69" s="47">
         <v>1</v>
@@ -7314,18 +7276,18 @@
         <v>54</v>
       </c>
       <c r="I69" s="47" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="F71" s="8"/>
     </row>
     <row r="72" spans="1:10" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="33" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="C72" s="49"/>
       <c r="E72" s="36"/>
@@ -7334,7 +7296,7 @@
     </row>
     <row r="73" spans="1:10" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="C73" s="49"/>
       <c r="E73" s="36"/>
@@ -7359,13 +7321,13 @@
     </row>
     <row r="76" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="54" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="B76" s="54" t="s">
         <v>164</v>
       </c>
       <c r="C76" s="54" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="D76" s="54">
         <v>1</v>
@@ -7383,13 +7345,13 @@
     </row>
     <row r="77" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="54" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="B77" s="54" t="s">
         <v>164</v>
       </c>
       <c r="C77" s="54" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="D77" s="54">
         <v>1</v>
@@ -7404,13 +7366,13 @@
     </row>
     <row r="78" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="54" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="B78" s="54" t="s">
         <v>164</v>
       </c>
       <c r="C78" s="54" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="D78" s="54">
         <v>1</v>
@@ -7428,13 +7390,13 @@
     </row>
     <row r="79" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="54" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="B79" s="54" t="s">
         <v>164</v>
       </c>
       <c r="C79" s="54" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="D79" s="54">
         <v>1</v>
@@ -7449,13 +7411,13 @@
     </row>
     <row r="80" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="54" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
       <c r="B80" s="54" t="s">
         <v>164</v>
       </c>
       <c r="C80" s="54" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="D80" s="54">
         <v>1</v>
@@ -7470,13 +7432,13 @@
     </row>
     <row r="81" spans="1:6" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="54" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="B81" s="54" t="s">
         <v>164</v>
       </c>
       <c r="C81" s="54" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="D81" s="54">
         <v>1</v>
@@ -7491,13 +7453,13 @@
     </row>
     <row r="82" spans="1:6" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="54" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="B82" s="54" t="s">
         <v>164</v>
       </c>
       <c r="C82" s="54" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="D82" s="54">
         <v>1</v>
@@ -7512,13 +7474,13 @@
     </row>
     <row r="83" spans="1:6" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="54" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="B83" s="54" t="s">
         <v>164</v>
       </c>
       <c r="C83" s="54" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="D83" s="54">
         <v>1</v>

</xml_diff>

<commit_message>
add Thorlabs shopping cart file for Excitation Arms
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D53B10-C54F-4192-9CCA-6DBC2632C84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83326EA-B7E0-47D2-9D7F-DC10B6688ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5352" yWindow="5784" windowWidth="34368" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4728" yWindow="7632" windowWidth="34368" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="548">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -662,6 +662,9 @@
     <t>SM1 Lens Tube, 1.00" Thread Depth, One Retaining Ring Included</t>
   </si>
   <si>
+    <t>Adapter with External C-Mount Threads and Internal SM1 Threads, 4.4 mm Spacer</t>
+  </si>
+  <si>
     <t>BA1S/M</t>
   </si>
   <si>
@@ -681,9 +684,6 @@
   </si>
   <si>
     <t>Ø12.7 mm Post Holder, Spring-Loaded Hex-Locking Thumbscrew, L=75 mm</t>
-  </si>
-  <si>
-    <t>XRN25P</t>
   </si>
   <si>
     <t>Compact 25 mm Travel Linear Translation Stage, Side Micrometer, 1/4"-20 Taps</t>
@@ -1643,9 +1643,6 @@
     <t>54-774</t>
   </si>
   <si>
-    <t>Adapter with External C-Mount Threads and Internal SM1 Threads, 4.1 mm Spacer</t>
-  </si>
-  <si>
     <t>Modified: BNC cables need to be soldered: see https://github.com/mesoSPIM/mesoSPIM-hardware-documentation/wiki/mesoSPIM_preparing_ETL_drivers</t>
   </si>
   <si>
@@ -1740,6 +1737,12 @@
   </si>
   <si>
     <t>Rods that hold the excitation objectives in 60-mm cage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM1A9 </t>
+  </si>
+  <si>
+    <t>XRN25P/M</t>
   </si>
 </sst>
 </file>
@@ -2507,7 +2510,7 @@
   <dimension ref="A1:J176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3356,7 +3359,7 @@
         <v>61</v>
       </c>
       <c r="C41" s="51" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D41" s="51">
         <v>2</v>
@@ -3371,7 +3374,7 @@
         <v>39</v>
       </c>
       <c r="H41" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3428,7 +3431,7 @@
         <v>40</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3489,13 +3492,13 @@
     </row>
     <row r="46" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="24" t="s">
-        <v>300</v>
+        <v>546</v>
       </c>
       <c r="B46" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>518</v>
+        <v>209</v>
       </c>
       <c r="D46" s="23">
         <v>2</v>
@@ -3511,7 +3514,7 @@
         <v>39</v>
       </c>
       <c r="H46" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -3538,10 +3541,10 @@
         <v>39</v>
       </c>
       <c r="H47" s="51" t="s">
+        <v>520</v>
+      </c>
+      <c r="I47" s="51" t="s">
         <v>521</v>
-      </c>
-      <c r="I47" s="51" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3568,7 +3571,7 @@
         <v>39</v>
       </c>
       <c r="H48" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3658,7 +3661,7 @@
         <v>222</v>
       </c>
       <c r="I51" s="23" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3685,7 +3688,7 @@
         <v>39</v>
       </c>
       <c r="H52" s="23" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I52" s="23" t="s">
         <v>430</v>
@@ -3715,21 +3718,21 @@
         <v>39</v>
       </c>
       <c r="H53" s="23" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I53" s="23" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
+        <v>539</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="24" t="s">
         <v>540</v>
-      </c>
-      <c r="B54" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>541</v>
       </c>
       <c r="D54" s="23">
         <v>2</v>
@@ -3748,28 +3751,28 @@
         <v>226</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
+        <v>541</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="24" t="s">
         <v>542</v>
       </c>
-      <c r="B55" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C55" s="24" t="s">
-        <v>543</v>
-      </c>
       <c r="D55" s="23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E55" s="81">
         <v>7</v>
       </c>
       <c r="F55" s="82">
         <f>E55*D55</f>
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G55" s="23" t="s">
         <v>39</v>
@@ -3778,28 +3781,28 @@
         <v>226</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B56" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D56" s="23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E56" s="81">
         <v>5</v>
       </c>
       <c r="F56" s="82">
         <f>E56*D56</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G56" s="23" t="s">
         <v>39</v>
@@ -3808,7 +3811,7 @@
         <v>226</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3816,7 +3819,7 @@
         <v>91863</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>47</v>
@@ -3838,7 +3841,7 @@
         <v>206</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3868,7 +3871,7 @@
         <v>226</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3898,7 +3901,7 @@
         <v>226</v>
       </c>
       <c r="I59" s="58" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J59" s="99"/>
     </row>
@@ -3959,18 +3962,18 @@
         <v>226</v>
       </c>
       <c r="I61" s="27" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="24" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B62" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D62" s="23">
         <v>4</v>
@@ -3986,21 +3989,21 @@
         <v>39</v>
       </c>
       <c r="H62" s="23" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I62" s="23" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B63" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D63" s="23">
         <v>2</v>
@@ -4021,13 +4024,13 @@
     </row>
     <row r="64" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B64" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D64" s="23">
         <v>4</v>
@@ -4043,21 +4046,21 @@
         <v>39</v>
       </c>
       <c r="H64" s="23" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I64" s="23" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
+        <v>528</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C65" s="24" t="s">
         <v>529</v>
-      </c>
-      <c r="B65" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C65" s="24" t="s">
-        <v>530</v>
       </c>
       <c r="D65" s="23">
         <v>2</v>
@@ -4078,13 +4081,13 @@
     </row>
     <row r="66" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B66" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C66" s="24" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D66" s="23">
         <v>2</v>
@@ -4103,12 +4106,12 @@
         <v>226</v>
       </c>
       <c r="I66" s="23" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="25" t="s">
-        <v>216</v>
+        <v>547</v>
       </c>
       <c r="B67" s="23" t="s">
         <v>61</v>
@@ -4133,7 +4136,7 @@
         <v>221</v>
       </c>
       <c r="I67" s="26" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4163,7 +4166,7 @@
         <v>221</v>
       </c>
       <c r="I68" s="26" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -4223,7 +4226,7 @@
         <v>223</v>
       </c>
       <c r="I70" s="27" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4253,7 +4256,7 @@
         <v>223</v>
       </c>
       <c r="I71" s="58" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -5894,7 +5897,7 @@
       </c>
       <c r="F153" s="66">
         <f>SUM(F3:F151)</f>
-        <v>94565.501499199992</v>
+        <v>94589.501499199992</v>
       </c>
       <c r="G153" s="3" t="s">
         <v>488</v>

</xml_diff>

<commit_message>
update part numbers Thorlabs
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F5B9BE-C9DD-4A4F-8A44-D53E0177D7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B661C5FE-DFE0-4B94-96FE-0F8FF4FBE580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="5496" windowWidth="34368" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2525,8 +2525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3948,33 +3948,33 @@
       </c>
       <c r="J60" s="99"/>
     </row>
-    <row r="61" spans="1:10" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="59" t="s">
+    <row r="61" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="24" t="s">
         <v>227</v>
       </c>
-      <c r="B61" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" s="59" t="s">
+      <c r="B61" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="D61" s="58">
-        <v>0</v>
-      </c>
-      <c r="E61" s="87">
+      <c r="D61" s="23">
+        <v>2</v>
+      </c>
+      <c r="E61" s="81">
         <v>92</v>
       </c>
-      <c r="F61" s="88">
+      <c r="F61" s="82">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G61" s="60" t="s">
+        <v>184</v>
+      </c>
+      <c r="G61" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="H61" s="58" t="s">
+      <c r="H61" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="I61" s="58" t="s">
+      <c r="I61" s="23" t="s">
         <v>467</v>
       </c>
     </row>
@@ -5940,7 +5940,7 @@
       </c>
       <c r="F154" s="66">
         <f>SUM(F3:F152)</f>
-        <v>95317.501499199992</v>
+        <v>95501.501499199992</v>
       </c>
       <c r="G154" s="3" t="s">
         <v>488</v>

</xml_diff>

<commit_message>
update parts list and LCP blank plate name
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B661C5FE-DFE0-4B94-96FE-0F8FF4FBE580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F10AAF-BD5D-4367-99D6-86260C6B6701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="5496" windowWidth="34368" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="550">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -572,9 +572,6 @@
     <t>Power Cord, 220V, 10A (plug country-specific)</t>
   </si>
   <si>
-    <t>Chassis to mount the signal generation card</t>
-  </si>
-  <si>
     <t>NI PCIe-8361, 1 Port MXI-Express Interface</t>
   </si>
   <si>
@@ -717,12 +714,6 @@
   </si>
   <si>
     <t>SM2NFM</t>
-  </si>
-  <si>
-    <t>LCP06/M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60 mm Cage Plate with Ø2" Double-Bore Optic Mount, M4 Tap </t>
   </si>
   <si>
     <t>Adapter with External SM2 Threads and Nikon Female F-Mount Ring</t>
@@ -1574,9 +1565,6 @@
     <t>Includes switching module between 2 laser ports, controlled by TTL signal. The 405nm is NOT included!</t>
   </si>
   <si>
-    <t>Connects the Chassis to the PC. Can be replaced with more modern two-port PCIe-8362 for a higher price.</t>
-  </si>
-  <si>
     <t>The signal generation card, 8 analog and 8 digital channels. Potentially replaceable with two NI-PCIe-6323 cards (and no chassis), but this needs testing and possibly software changes.</t>
   </si>
   <si>
@@ -1755,6 +1743,12 @@
   </si>
   <si>
     <t>Microscope base</t>
+  </si>
+  <si>
+    <t>Chassis to mount the signal generation card.  Alternative: low-cost NI PXI-1033 from second-hand market.</t>
+  </si>
+  <si>
+    <t>Connects the Chassis to the PC. NI-PCIe-8361 is officially discontinued by NI. Alternative: a two-port PCIe-8362 for a higher price.</t>
   </si>
 </sst>
 </file>
@@ -2021,7 +2015,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -2128,9 +2122,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -2525,8 +2516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2546,7 +2537,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="93" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="E1" s="94"/>
       <c r="F1" s="94"/>
@@ -2565,10 +2556,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="70" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="F2" s="70" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -2608,7 +2599,7 @@
         <v>12350</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>173</v>
@@ -2655,7 +2646,7 @@
         <v>39</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2673,7 +2664,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D10" s="54">
         <v>0</v>
@@ -2686,10 +2677,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="54" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I10" s="54" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2713,10 +2704,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="54" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I11" s="44" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2740,7 +2731,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="44" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H12" s="44" t="s">
         <v>13</v>
@@ -2748,13 +2739,13 @@
     </row>
     <row r="13" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D13" s="44">
         <v>1</v>
@@ -2767,10 +2758,10 @@
         <v>160</v>
       </c>
       <c r="G13" s="54" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I13" s="44" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2794,13 +2785,13 @@
         <v>0</v>
       </c>
       <c r="G14" s="44" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H14" s="44" t="s">
         <v>13</v>
       </c>
       <c r="I14" s="44" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2824,10 +2815,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="54" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I15" s="44" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2851,21 +2842,21 @@
         <v>0</v>
       </c>
       <c r="G16" s="54" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I16" s="44" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B17" s="44" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D17" s="44">
         <v>0</v>
@@ -2878,10 +2869,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="54" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I17" s="44" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2905,10 +2896,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="54" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I18" s="54" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2932,21 +2923,21 @@
         <v>0</v>
       </c>
       <c r="G19" s="54" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="I19" s="54" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -2959,7 +2950,7 @@
         <v>19965</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -2991,10 +2982,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="54" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="I22" s="54" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -3018,21 +3009,21 @@
         <v>0</v>
       </c>
       <c r="G23" s="54" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="I23" s="54" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -3045,7 +3036,7 @@
         <v>6900</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3054,13 +3045,13 @@
     </row>
     <row r="26" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="51" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B26" s="51" t="s">
         <v>61</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="D26" s="51">
         <v>4</v>
@@ -3073,28 +3064,28 @@
         <v>108</v>
       </c>
       <c r="G26" s="51" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I26" s="51" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E27" s="72"/>
       <c r="F27" s="72"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D28" s="3">
         <v>2</v>
@@ -3107,21 +3098,21 @@
         <v>140</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D29" s="3">
         <v>6</v>
@@ -3134,21 +3125,21 @@
         <v>216</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -3161,21 +3152,21 @@
         <v>43</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
@@ -3188,21 +3179,21 @@
         <v>29</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
@@ -3215,21 +3206,21 @@
         <v>195</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D33" s="3">
         <v>1</v>
@@ -3242,7 +3233,7 @@
         <v>10</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="12" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3254,7 +3245,7 @@
     </row>
     <row r="35" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E35" s="80"/>
       <c r="F35" s="80"/>
@@ -3267,7 +3258,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="71" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F36" s="71">
         <v>0</v>
@@ -3275,36 +3266,36 @@
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E37" s="72"/>
       <c r="F37" s="72"/>
     </row>
     <row r="38" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="101" t="s">
-        <v>550</v>
+      <c r="A38" s="100" t="s">
+        <v>546</v>
       </c>
       <c r="B38" s="50" t="s">
         <v>61</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="D38" s="50">
         <v>1</v>
       </c>
-      <c r="E38" s="100">
+      <c r="E38" s="99">
         <v>728</v>
       </c>
-      <c r="F38" s="100">
+      <c r="F38" s="99">
         <f>D38*E38</f>
         <v>728</v>
       </c>
       <c r="G38" s="50" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="I38" s="50" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3315,7 +3306,7 @@
         <v>61</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D39" s="23">
         <v>2</v>
@@ -3331,21 +3322,21 @@
         <v>39</v>
       </c>
       <c r="H39" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="24" t="s">
         <v>197</v>
-      </c>
-      <c r="B40" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="24" t="s">
-        <v>198</v>
       </c>
       <c r="D40" s="23">
         <v>2</v>
@@ -3361,10 +3352,10 @@
         <v>39</v>
       </c>
       <c r="H40" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="I40" s="23" t="s">
         <v>199</v>
-      </c>
-      <c r="I40" s="23" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3391,18 +3382,18 @@
         <v>39</v>
       </c>
       <c r="H41" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="51" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B42" s="51" t="s">
         <v>61</v>
       </c>
       <c r="C42" s="51" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D42" s="51">
         <v>2</v>
@@ -3417,7 +3408,7 @@
         <v>39</v>
       </c>
       <c r="H42" s="23" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3425,10 +3416,10 @@
         <v>38</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D43" s="3">
         <v>2</v>
@@ -3452,7 +3443,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>42</v>
@@ -3474,15 +3465,15 @@
         <v>40</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>45</v>
@@ -3511,7 +3502,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>44</v>
@@ -3535,13 +3526,13 @@
     </row>
     <row r="47" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="B47" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D47" s="23">
         <v>2</v>
@@ -3557,7 +3548,7 @@
         <v>39</v>
       </c>
       <c r="H47" s="23" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -3584,21 +3575,21 @@
         <v>39</v>
       </c>
       <c r="H48" s="51" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="I48" s="51" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="24" t="s">
         <v>207</v>
-      </c>
-      <c r="B49" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C49" s="24" t="s">
-        <v>208</v>
       </c>
       <c r="D49" s="23">
         <v>2</v>
@@ -3614,18 +3605,18 @@
         <v>39</v>
       </c>
       <c r="H49" s="23" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="B50" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="24" t="s">
         <v>201</v>
-      </c>
-      <c r="B50" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>202</v>
       </c>
       <c r="D50" s="23">
         <v>4</v>
@@ -3634,28 +3625,28 @@
         <v>189</v>
       </c>
       <c r="F50" s="82">
-        <f>E50*D50</f>
+        <f t="shared" ref="F50:F57" si="4">E50*D50</f>
         <v>756</v>
       </c>
       <c r="G50" s="23" t="s">
         <v>39</v>
       </c>
       <c r="H50" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I50" s="23" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="B51" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="24" t="s">
         <v>204</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>205</v>
       </c>
       <c r="D51" s="23">
         <v>4</v>
@@ -3664,28 +3655,28 @@
         <v>110</v>
       </c>
       <c r="F51" s="82">
-        <f>E51*D51</f>
+        <f t="shared" si="4"/>
         <v>440</v>
       </c>
       <c r="G51" s="23" t="s">
         <v>39</v>
       </c>
       <c r="H51" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I51" s="23" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="B52" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="24" t="s">
         <v>193</v>
-      </c>
-      <c r="B52" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>194</v>
       </c>
       <c r="D52" s="23">
         <v>8</v>
@@ -3694,17 +3685,17 @@
         <v>16</v>
       </c>
       <c r="F52" s="82">
-        <f>E52*D52</f>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="G52" s="23" t="s">
         <v>39</v>
       </c>
       <c r="H52" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I52" s="23" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3715,7 +3706,7 @@
         <v>61</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D53" s="23">
         <v>4</v>
@@ -3724,28 +3715,28 @@
         <v>104</v>
       </c>
       <c r="F53" s="82">
-        <f>E53*D53</f>
+        <f t="shared" si="4"/>
         <v>416</v>
       </c>
       <c r="G53" s="51" t="s">
         <v>39</v>
       </c>
       <c r="H53" s="23" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="I53" s="23" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B54" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D54" s="23">
         <v>2</v>
@@ -3754,28 +3745,28 @@
         <v>41</v>
       </c>
       <c r="F54" s="82">
-        <f>E54*D54</f>
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
       <c r="G54" s="23" t="s">
         <v>39</v>
       </c>
       <c r="H54" s="23" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="B55" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="D55" s="23">
         <v>2</v>
@@ -3784,28 +3775,28 @@
         <v>17</v>
       </c>
       <c r="F55" s="82">
-        <f>E55*D55</f>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="G55" s="23" t="s">
         <v>39</v>
       </c>
       <c r="H55" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B56" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="D56" s="23">
         <v>4</v>
@@ -3814,28 +3805,28 @@
         <v>7</v>
       </c>
       <c r="F56" s="82">
-        <f>E56*D56</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="G56" s="23" t="s">
         <v>39</v>
       </c>
       <c r="H56" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B57" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="D57" s="23">
         <v>4</v>
@@ -3844,17 +3835,17 @@
         <v>5</v>
       </c>
       <c r="F57" s="82">
-        <f>E57*D57</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G57" s="23" t="s">
         <v>39</v>
       </c>
       <c r="H57" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I57" s="23" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3862,7 +3853,7 @@
         <v>91863</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>47</v>
@@ -3874,28 +3865,28 @@
         <v>400</v>
       </c>
       <c r="F58" s="78">
-        <f t="shared" ref="F58:F78" si="4">E58*D58</f>
+        <f t="shared" ref="F58:F78" si="5">E58*D58</f>
         <v>800</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>39</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C59" s="92" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D59" s="4">
         <v>2</v>
@@ -3904,59 +3895,59 @@
         <v>300</v>
       </c>
       <c r="F59" s="78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>600</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>39</v>
       </c>
       <c r="H59" s="27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="98" t="s">
-        <v>228</v>
+      <c r="A60" s="59" t="s">
+        <v>438</v>
       </c>
       <c r="B60" s="58" t="s">
         <v>61</v>
       </c>
       <c r="C60" s="59" t="s">
-        <v>229</v>
+        <v>433</v>
       </c>
       <c r="D60" s="58">
         <v>0</v>
       </c>
       <c r="E60" s="87">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F60" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G60" s="60" t="s">
         <v>39</v>
       </c>
       <c r="H60" s="58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I60" s="58" t="s">
-        <v>535</v>
-      </c>
-      <c r="J60" s="99"/>
+        <v>531</v>
+      </c>
+      <c r="J60" s="98"/>
     </row>
     <row r="61" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" s="24" t="s">
         <v>227</v>
-      </c>
-      <c r="B61" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" s="24" t="s">
-        <v>230</v>
       </c>
       <c r="D61" s="23">
         <v>2</v>
@@ -3965,28 +3956,28 @@
         <v>92</v>
       </c>
       <c r="F61" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>184</v>
       </c>
       <c r="G61" s="51" t="s">
         <v>39</v>
       </c>
       <c r="H61" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="31" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B62" s="27" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C62" s="97" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D62" s="27">
         <v>2</v>
@@ -3995,28 +3986,28 @@
         <v>1</v>
       </c>
       <c r="F62" s="84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>39</v>
       </c>
       <c r="H62" s="27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I62" s="27" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="B63" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D63" s="23">
         <v>4</v>
@@ -4032,21 +4023,21 @@
         <v>39</v>
       </c>
       <c r="H63" s="23" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="I63" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" s="24" t="s">
         <v>215</v>
-      </c>
-      <c r="B64" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C64" s="24" t="s">
-        <v>216</v>
       </c>
       <c r="D64" s="23">
         <v>2</v>
@@ -4055,25 +4046,25 @@
         <v>8</v>
       </c>
       <c r="F64" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H64" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C65" s="24" t="s">
         <v>213</v>
-      </c>
-      <c r="B65" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C65" s="24" t="s">
-        <v>214</v>
       </c>
       <c r="D65" s="23">
         <v>4</v>
@@ -4082,28 +4073,28 @@
         <v>5</v>
       </c>
       <c r="F65" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H65" s="23" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="I65" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="B66" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C66" s="24" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D66" s="23">
         <v>2</v>
@@ -4112,25 +4103,25 @@
         <v>5</v>
       </c>
       <c r="F66" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H66" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="B67" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67" s="24" t="s">
         <v>210</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C67" s="24" t="s">
-        <v>211</v>
       </c>
       <c r="D67" s="23">
         <v>2</v>
@@ -4146,21 +4137,21 @@
         <v>39</v>
       </c>
       <c r="H67" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I67" s="23" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="B68" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D68" s="26">
         <v>2</v>
@@ -4169,28 +4160,28 @@
         <v>398</v>
       </c>
       <c r="F68" s="86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>796</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H68" s="26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I68" s="26" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="62" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B69" s="27" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D69" s="26">
         <v>2</v>
@@ -4199,28 +4190,28 @@
         <v>150</v>
       </c>
       <c r="F69" s="86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>300</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H69" s="26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I69" s="26" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="B70" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C70" s="25" t="s">
         <v>218</v>
-      </c>
-      <c r="B70" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C70" s="25" t="s">
-        <v>219</v>
       </c>
       <c r="D70" s="26">
         <v>2</v>
@@ -4229,28 +4220,28 @@
         <v>30</v>
       </c>
       <c r="F70" s="86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H70" s="26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I70" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="31" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B71" s="27" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D71" s="27">
         <v>2</v>
@@ -4259,28 +4250,28 @@
         <v>300</v>
       </c>
       <c r="F71" s="84">
-        <f t="shared" ref="F71" si="5">E71*D71</f>
+        <f t="shared" ref="F71" si="6">E71*D71</f>
         <v>600</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>39</v>
       </c>
       <c r="H71" s="27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I71" s="27" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B72" s="58" t="s">
         <v>61</v>
       </c>
       <c r="C72" s="59" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D72" s="58">
         <v>0</v>
@@ -4289,28 +4280,28 @@
         <v>36</v>
       </c>
       <c r="F72" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G72" s="60" t="s">
         <v>39</v>
       </c>
       <c r="H72" s="58" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I72" s="58" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B73" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D73" s="23">
         <v>2</v>
@@ -4319,28 +4310,28 @@
         <v>2104</v>
       </c>
       <c r="F73" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4208</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H73" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I73" s="23" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B74" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D74" s="23">
         <v>2</v>
@@ -4349,25 +4340,25 @@
         <v>82</v>
       </c>
       <c r="F74" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>164</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H74" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="30" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B75" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D75" s="23">
         <v>1</v>
@@ -4376,28 +4367,28 @@
         <v>520</v>
       </c>
       <c r="F75" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>520</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H75" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I75" s="23" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="61" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B76" s="58" t="s">
         <v>61</v>
       </c>
       <c r="C76" s="59" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D76" s="58">
         <v>0</v>
@@ -4406,28 +4397,28 @@
         <v>390</v>
       </c>
       <c r="F76" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G76" s="60" t="s">
         <v>39</v>
       </c>
       <c r="H76" s="58" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I76" s="58" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="31" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B77" s="27" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D77" s="23">
         <v>14</v>
@@ -4436,28 +4427,28 @@
         <v>20</v>
       </c>
       <c r="F77" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>280</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H77" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I77" s="27" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="31" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C78" s="24" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D78" s="23">
         <v>1</v>
@@ -4466,22 +4457,22 @@
         <v>10</v>
       </c>
       <c r="F78" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H78" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I78" s="23" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E79" s="72"/>
       <c r="F79" s="72"/>
@@ -4502,18 +4493,18 @@
       <c r="E80" s="81"/>
       <c r="F80" s="82"/>
       <c r="I80" s="23" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="81" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B81" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C81" s="24" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D81" s="23">
         <v>1</v>
@@ -4528,13 +4519,13 @@
     </row>
     <row r="82" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="28" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B82" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C82" s="24" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D82" s="23">
         <v>2</v>
@@ -4563,32 +4554,32 @@
       <c r="E83" s="81"/>
       <c r="F83" s="82"/>
       <c r="I83" s="23" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="84" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="E84" s="72"/>
       <c r="F84" s="72"/>
     </row>
     <row r="85" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E85" s="72"/>
       <c r="F85" s="72"/>
     </row>
     <row r="86" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C86" s="67" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D86" s="3">
         <v>1</v>
@@ -4601,19 +4592,19 @@
         <v>200</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="J86" s="4"/>
     </row>
     <row r="87" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D87" s="4">
         <v>5</v>
@@ -4626,18 +4617,18 @@
         <v>5</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="51" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D88" s="3">
         <v>1</v>
@@ -4650,18 +4641,18 @@
         <v>26</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D89" s="3">
         <v>1</v>
@@ -4674,18 +4665,18 @@
         <v>37</v>
       </c>
       <c r="I89" s="51" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="90" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="51" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B90" s="51" t="s">
         <v>61</v>
       </c>
       <c r="C90" s="51" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D90" s="51">
         <v>2</v>
@@ -4698,7 +4689,7 @@
         <v>48</v>
       </c>
       <c r="I90" s="23" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="91" spans="1:10" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4717,13 +4708,13 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D93" s="3">
         <v>1</v>
@@ -4744,20 +4735,20 @@
     </row>
     <row r="94" spans="1:10" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A94" s="17" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E94" s="90"/>
       <c r="F94" s="90"/>
     </row>
     <row r="95" spans="1:10" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="21" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B95" s="20" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C95" s="95" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D95" s="20">
         <v>1</v>
@@ -4766,25 +4757,25 @@
         <v>900</v>
       </c>
       <c r="F95" s="91">
-        <f t="shared" ref="F95:F101" si="6">E95*D95</f>
+        <f t="shared" ref="F95:F101" si="7">E95*D95</f>
         <v>900</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I95" s="20" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="22" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B96" s="20" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C96" s="96" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="D96" s="3">
         <v>1</v>
@@ -4793,7 +4784,7 @@
         <v>767</v>
       </c>
       <c r="F96" s="91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>767</v>
       </c>
       <c r="G96" s="3" t="s">
@@ -4801,18 +4792,18 @@
       </c>
       <c r="H96" s="20"/>
       <c r="I96" s="3" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="22" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B97" s="20" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C97" s="96" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D97" s="3">
         <v>0</v>
@@ -4821,7 +4812,7 @@
         <v>1540</v>
       </c>
       <c r="F97" s="91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G97" s="3" t="s">
@@ -4829,18 +4820,18 @@
       </c>
       <c r="H97" s="20"/>
       <c r="I97" s="3" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B98" s="20" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C98" s="96" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D98" s="3">
         <v>1</v>
@@ -4849,7 +4840,7 @@
         <v>877</v>
       </c>
       <c r="F98" s="91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>877</v>
       </c>
       <c r="G98" s="3" t="s">
@@ -4857,18 +4848,18 @@
       </c>
       <c r="H98" s="20"/>
       <c r="I98" s="3" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="51" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B99" s="20" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C99" s="96" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D99" s="51">
         <v>0</v>
@@ -4877,7 +4868,7 @@
         <v>4700</v>
       </c>
       <c r="F99" s="91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G99" s="51" t="s">
@@ -4885,18 +4876,18 @@
       </c>
       <c r="H99" s="20"/>
       <c r="I99" s="51" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="51" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B100" s="20" t="s">
         <v>61</v>
       </c>
       <c r="C100" s="51" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="D100" s="51">
         <v>1</v>
@@ -4905,7 +4896,7 @@
         <v>20</v>
       </c>
       <c r="F100" s="91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="G100" s="51" t="s">
@@ -4913,18 +4904,18 @@
       </c>
       <c r="H100" s="20"/>
       <c r="I100" s="51" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="B101" s="20" t="s">
         <v>61</v>
       </c>
       <c r="C101" s="32" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="D101" s="3">
         <v>1</v>
@@ -4933,7 +4924,7 @@
         <v>25</v>
       </c>
       <c r="F101" s="91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
       <c r="G101" s="3" t="s">
@@ -4941,25 +4932,25 @@
       </c>
       <c r="H101" s="20"/>
       <c r="I101" s="51" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A102" s="17" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E102" s="90"/>
       <c r="F102" s="90"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B103" s="20" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C103" s="68" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D103" s="3">
         <v>1</v>
@@ -4968,25 +4959,25 @@
         <v>752</v>
       </c>
       <c r="F103" s="71">
-        <f t="shared" ref="F103:F107" si="7">D103*E103</f>
+        <f t="shared" ref="F103:F107" si="8">D103*E103</f>
         <v>752</v>
       </c>
       <c r="G103" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B104" s="64" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D104" s="4">
         <v>1</v>
@@ -4995,25 +4986,25 @@
         <v>1</v>
       </c>
       <c r="F104" s="78">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G104" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I104" s="4" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B105" s="20" t="s">
         <v>61</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D105" s="3">
         <v>1</v>
@@ -5022,25 +5013,25 @@
         <v>65</v>
       </c>
       <c r="F105" s="71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>65</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B106" s="20" t="s">
         <v>61</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D106" s="3">
         <v>1</v>
@@ -5049,25 +5040,25 @@
         <v>32</v>
       </c>
       <c r="F106" s="71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>32</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B107" s="20" t="s">
         <v>61</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D107" s="3">
         <v>1</v>
@@ -5076,14 +5067,14 @@
         <v>112</v>
       </c>
       <c r="F107" s="71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>112</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5110,25 +5101,25 @@
         <v>3582</v>
       </c>
       <c r="F109" s="71">
-        <f t="shared" ref="F109:F121" si="8">E109*D109</f>
+        <f t="shared" ref="F109:F121" si="9">E109*D109</f>
         <v>3582</v>
       </c>
       <c r="G109" s="3" t="s">
         <v>51</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D110" s="3">
         <v>1</v>
@@ -5137,25 +5128,25 @@
         <v>1630</v>
       </c>
       <c r="F110" s="71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1630</v>
       </c>
       <c r="G110" s="3" t="s">
         <v>51</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>179</v>
+        <v>548</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D111" s="3">
         <v>1</v>
@@ -5164,25 +5155,25 @@
         <v>886</v>
       </c>
       <c r="F111" s="71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>886</v>
       </c>
       <c r="G111" s="3" t="s">
         <v>51</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>495</v>
+        <v>549</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D112" s="3">
         <v>1</v>
@@ -5191,14 +5182,14 @@
         <v>163</v>
       </c>
       <c r="F112" s="71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>163</v>
       </c>
       <c r="G112" s="3" t="s">
         <v>51</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -5218,7 +5209,7 @@
         <v>11</v>
       </c>
       <c r="F113" s="71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="G113" s="3" t="s">
@@ -5242,7 +5233,7 @@
         <v>520</v>
       </c>
       <c r="F114" s="71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>520</v>
       </c>
       <c r="G114" s="3" t="s">
@@ -5251,13 +5242,13 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D115" s="3">
         <v>1</v>
@@ -5266,7 +5257,7 @@
         <v>193</v>
       </c>
       <c r="F115" s="71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>193</v>
       </c>
       <c r="G115" s="3" t="s">
@@ -5275,13 +5266,13 @@
     </row>
     <row r="116" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="23" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B116" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C116" s="23" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D116" s="23">
         <v>10</v>
@@ -5290,25 +5281,25 @@
         <v>12</v>
       </c>
       <c r="F116" s="82">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>120</v>
       </c>
       <c r="G116" s="23" t="s">
         <v>51</v>
       </c>
       <c r="I116" s="23" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="23" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B117" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C117" s="23" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D117" s="23">
         <v>1</v>
@@ -5317,14 +5308,14 @@
         <v>14</v>
       </c>
       <c r="F117" s="82">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="G117" s="23" t="s">
         <v>51</v>
       </c>
       <c r="I117" s="23" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -5344,7 +5335,7 @@
         <v>15.25</v>
       </c>
       <c r="F118" s="71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>61</v>
       </c>
       <c r="G118" s="23" t="s">
@@ -5368,7 +5359,7 @@
         <v>16.5</v>
       </c>
       <c r="F119" s="71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>165</v>
       </c>
       <c r="G119" s="23" t="s">
@@ -5392,7 +5383,7 @@
         <v>24</v>
       </c>
       <c r="F120" s="71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>240</v>
       </c>
       <c r="G120" s="23" t="s">
@@ -5416,7 +5407,7 @@
         <v>24</v>
       </c>
       <c r="F121" s="71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>144</v>
       </c>
       <c r="G121" s="23" t="s">
@@ -5456,7 +5447,7 @@
         <v>16.5</v>
       </c>
       <c r="F126" s="71">
-        <f t="shared" ref="F126:F141" si="9">E126*D126</f>
+        <f t="shared" ref="F126:F141" si="10">E126*D126</f>
         <v>66</v>
       </c>
       <c r="I126" s="3" t="s">
@@ -5480,7 +5471,7 @@
         <v>85.1</v>
       </c>
       <c r="F127" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>85.1</v>
       </c>
     </row>
@@ -5501,7 +5492,7 @@
         <v>32</v>
       </c>
       <c r="F128" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="I128" s="3" t="s">
@@ -5525,7 +5516,7 @@
         <v>51.58</v>
       </c>
       <c r="F129" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>103.16</v>
       </c>
     </row>
@@ -5546,7 +5537,7 @@
         <v>60</v>
       </c>
       <c r="F130" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>60</v>
       </c>
       <c r="I130" s="3" t="s">
@@ -5570,7 +5561,7 @@
         <v>136.47999999999999</v>
       </c>
       <c r="F131" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>136.47999999999999</v>
       </c>
     </row>
@@ -5591,7 +5582,7 @@
         <v>136.47999999999999</v>
       </c>
       <c r="F132" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>136.47999999999999</v>
       </c>
     </row>
@@ -5612,7 +5603,7 @@
         <v>60.95</v>
       </c>
       <c r="F133" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>60.95</v>
       </c>
     </row>
@@ -5633,7 +5624,7 @@
         <v>119.416</v>
       </c>
       <c r="F134" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>119.416</v>
       </c>
     </row>
@@ -5654,7 +5645,7 @@
         <v>105.8</v>
       </c>
       <c r="F135" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>105.8</v>
       </c>
     </row>
@@ -5675,19 +5666,19 @@
         <v>119.6</v>
       </c>
       <c r="F136" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>239.2</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D137" s="3">
         <v>1</v>
@@ -5696,7 +5687,7 @@
         <v>100</v>
       </c>
       <c r="F137" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
     </row>
@@ -5717,7 +5708,7 @@
         <v>92</v>
       </c>
       <c r="F138" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>184</v>
       </c>
     </row>
@@ -5738,7 +5729,7 @@
         <v>96.23</v>
       </c>
       <c r="F139" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>96.23</v>
       </c>
     </row>
@@ -5759,7 +5750,7 @@
         <v>102.44</v>
       </c>
       <c r="F140" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>102.44</v>
       </c>
     </row>
@@ -5780,7 +5771,7 @@
         <v>28</v>
       </c>
       <c r="F141" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>56</v>
       </c>
     </row>
@@ -5816,7 +5807,7 @@
         <v>161</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E146" s="72"/>
       <c r="F146" s="72"/>
@@ -5824,7 +5815,7 @@
     <row r="147" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="51"/>
       <c r="B147" s="51" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C147" s="53" t="s">
         <v>160</v>
@@ -5840,13 +5831,13 @@
         <v>160</v>
       </c>
       <c r="G147" s="51" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H147" s="51" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="I147" s="51" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="J147" s="53"/>
     </row>
@@ -5855,7 +5846,7 @@
         <v>162</v>
       </c>
       <c r="C148" s="51" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D148" s="51">
         <v>2</v>
@@ -5868,7 +5859,7 @@
         <v>662</v>
       </c>
       <c r="G148" s="51" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="149" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -5876,7 +5867,7 @@
         <v>162</v>
       </c>
       <c r="C149" s="51" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D149" s="51">
         <v>4</v>
@@ -5889,7 +5880,7 @@
         <v>100</v>
       </c>
       <c r="G149" s="51" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="150" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -5897,7 +5888,7 @@
         <v>162</v>
       </c>
       <c r="C150" s="51" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D150" s="51">
         <v>4</v>
@@ -5910,7 +5901,7 @@
         <v>112</v>
       </c>
       <c r="G150" s="51" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="151" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -5918,7 +5909,7 @@
         <v>162</v>
       </c>
       <c r="C151" s="51" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D151" s="51">
         <v>6</v>
@@ -5931,19 +5922,19 @@
         <v>729</v>
       </c>
       <c r="G151" s="51" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="154" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E154" s="66" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="F154" s="66">
         <f>SUM(F3:F152)</f>
         <v>95501.501499199992</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="156" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -5952,138 +5943,138 @@
     </row>
     <row r="158" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A158" s="65" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="159" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="4" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B160" s="3">
         <v>14</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B161" s="3">
         <v>2</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B162" s="3">
         <v>2</v>
       </c>
       <c r="C162" s="51" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B163" s="3">
         <v>2</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A166" s="65" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B168" s="3">
         <v>2</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A169" s="3" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B169" s="3">
         <v>5</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B170" s="3">
         <v>1</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A173" s="65" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A174" s="4" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="51" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B175" s="3">
         <v>5</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -6094,18 +6085,18 @@
         <v>3</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -6200,7 +6191,7 @@
         <v>7400</v>
       </c>
       <c r="I3" s="44" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6221,15 +6212,15 @@
         <v>20000</v>
       </c>
       <c r="I4" s="44" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D5" s="33">
         <v>1</v>
@@ -6241,13 +6232,13 @@
         <v>50000</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -6270,27 +6261,27 @@
         <v>25000</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:9" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D12" s="33">
         <v>1</v>
@@ -6306,21 +6297,21 @@
         <v>13</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D13" s="33">
         <v>1</v>
@@ -6336,21 +6327,21 @@
         <v>13</v>
       </c>
       <c r="H13" s="33" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="I13" s="33" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>61</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D14" s="33">
         <v>1</v>
@@ -6366,21 +6357,21 @@
         <v>13</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="I14" s="33" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>61</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D15" s="33">
         <v>1</v>
@@ -6396,21 +6387,21 @@
         <v>13</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="I15" s="33" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D16" s="34">
         <v>1</v>
@@ -6426,32 +6417,32 @@
         <v>13</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="I16" s="34" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:10" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="51" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C19" s="51" t="s">
         <v>14</v>
@@ -6476,13 +6467,13 @@
     </row>
     <row r="20" spans="1:10" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="51" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D20" s="51">
         <v>1</v>
@@ -6504,13 +6495,13 @@
     </row>
     <row r="21" spans="1:10" s="51" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="51" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B21" s="51" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21" s="51" t="s">
         <v>275</v>
-      </c>
-      <c r="C21" s="51" t="s">
-        <v>278</v>
       </c>
       <c r="D21" s="51">
         <v>1</v>
@@ -6531,13 +6522,13 @@
     </row>
     <row r="22" spans="1:10" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="51" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D22" s="51">
         <v>1</v>
@@ -6545,32 +6536,32 @@
       <c r="E22" s="52"/>
       <c r="F22" s="52"/>
       <c r="I22" s="23" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" s="42" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
     </row>
     <row r="26" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D26" s="34">
         <v>2</v>
@@ -6586,21 +6577,21 @@
         <v>39</v>
       </c>
       <c r="H26" s="34" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I26" s="34" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D27" s="34">
         <v>2</v>
@@ -6616,21 +6607,21 @@
         <v>39</v>
       </c>
       <c r="H27" s="34" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I27" s="34" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D28" s="34">
         <v>8</v>
@@ -6646,21 +6637,21 @@
         <v>39</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I28" s="34" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B29" s="34" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D29" s="34">
         <v>6</v>
@@ -6676,18 +6667,18 @@
         <v>39</v>
       </c>
       <c r="H29" s="34" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D30" s="34">
         <v>2</v>
@@ -6703,21 +6694,21 @@
         <v>39</v>
       </c>
       <c r="H30" s="34" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I30" s="34" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D31" s="34">
         <v>1</v>
@@ -6733,21 +6724,21 @@
         <v>39</v>
       </c>
       <c r="H31" s="34" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I31" s="34" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D32" s="34">
         <v>1</v>
@@ -6763,21 +6754,21 @@
         <v>39</v>
       </c>
       <c r="H32" s="34" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I32" s="34" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="37" t="s">
         <v>224</v>
-      </c>
-      <c r="B33" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>225</v>
       </c>
       <c r="D33" s="34">
         <v>2</v>
@@ -6793,7 +6784,7 @@
         <v>39</v>
       </c>
       <c r="H33" s="34" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -6827,7 +6818,7 @@
         <v>51</v>
       </c>
       <c r="I38" s="44" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -7329,7 +7320,7 @@
     </row>
     <row r="66" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F66" s="8"/>
     </row>
@@ -7354,18 +7345,18 @@
         <v>280</v>
       </c>
       <c r="I67" s="33" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B68" s="47" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C68" s="47" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D68" s="47">
         <v>2</v>
@@ -7378,18 +7369,18 @@
         <v>168</v>
       </c>
       <c r="I68" s="47" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B69" s="47" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C69" s="47" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D69" s="47">
         <v>1</v>
@@ -7402,18 +7393,18 @@
         <v>54</v>
       </c>
       <c r="I69" s="47" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F71" s="8"/>
     </row>
     <row r="72" spans="1:10" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="33" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C72" s="49"/>
       <c r="E72" s="36"/>
@@ -7422,7 +7413,7 @@
     </row>
     <row r="73" spans="1:10" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C73" s="49"/>
       <c r="E73" s="36"/>
@@ -7440,20 +7431,20 @@
         <v>161</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
     </row>
     <row r="76" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="54" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B76" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C76" s="54" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D76" s="54">
         <v>1</v>
@@ -7471,13 +7462,13 @@
     </row>
     <row r="77" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="54" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B77" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C77" s="54" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D77" s="54">
         <v>1</v>
@@ -7492,13 +7483,13 @@
     </row>
     <row r="78" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="54" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B78" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C78" s="54" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D78" s="54">
         <v>1</v>
@@ -7516,13 +7507,13 @@
     </row>
     <row r="79" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="54" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B79" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C79" s="54" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D79" s="54">
         <v>1</v>
@@ -7537,13 +7528,13 @@
     </row>
     <row r="80" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="54" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B80" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C80" s="54" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D80" s="54">
         <v>1</v>
@@ -7558,13 +7549,13 @@
     </row>
     <row r="81" spans="1:6" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="54" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B81" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C81" s="54" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D81" s="54">
         <v>1</v>
@@ -7579,13 +7570,13 @@
     </row>
     <row r="82" spans="1:6" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="54" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B82" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C82" s="54" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D82" s="54">
         <v>1</v>
@@ -7600,13 +7591,13 @@
     </row>
     <row r="83" spans="1:6" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="54" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B83" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C83" s="54" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D83" s="54">
         <v>1</v>

</xml_diff>

<commit_message>
add exploded view to Wiki
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F10AAF-BD5D-4367-99D6-86260C6B6701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651385D5-BEB2-4129-849D-80DB34070363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="5496" windowWidth="34368" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18996" yWindow="6156" windowWidth="34368" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="552">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -963,9 +963,6 @@
   </si>
   <si>
     <t>Galvo heat sink assembled from sheets, each galvo requires 7 sheets</t>
-  </si>
-  <si>
-    <t>HeatSink-sheet-H2mm.pdf</t>
   </si>
   <si>
     <t>Claser-cut or water-jet cut from 2-mm Aluminum. See folder /custom-parts/galvo-assembly/15mm-galvo(Thorlabs-QS15)-mount/</t>
@@ -1370,12 +1367,6 @@
     <t>60 mm Blank Cage Plate, M4 Tap (supersedes obsolete LCP03)</t>
   </si>
   <si>
-    <t>Nikon objective mount using Thorlabs LCP06/M 60 mm Cage Plate with Ø2" Double-Bore Optic Mount</t>
-  </si>
-  <si>
-    <t>LCP06M-Nikon-modified.ipt</t>
-  </si>
-  <si>
     <t>Modified 60 mm Blank Cage Plate</t>
   </si>
   <si>
@@ -1749,6 +1740,21 @@
   </si>
   <si>
     <t>Connects the Chassis to the PC. NI-PCIe-8361 is officially discontinued by NI. Alternative: a two-port PCIe-8362 for a higher price.</t>
+  </si>
+  <si>
+    <t>Side covers of the galvo assembly</t>
+  </si>
+  <si>
+    <t>60 mm Blank Cage Plate, M4 Tap</t>
+  </si>
+  <si>
+    <t>Nikon objective mount using Thorlabs LCP31/M 60 mm Blank Cage Plate</t>
+  </si>
+  <si>
+    <t>LCP31M-Nikon-modified</t>
+  </si>
+  <si>
+    <t>HeatSink-sheet-H2mm</t>
   </si>
 </sst>
 </file>
@@ -2514,10 +2520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J177"/>
+  <dimension ref="A1:J178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2537,7 +2543,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="93" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="E1" s="94"/>
       <c r="F1" s="94"/>
@@ -2556,10 +2562,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="70" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="F2" s="70" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -2646,7 +2652,7 @@
         <v>39</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2664,7 +2670,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D10" s="54">
         <v>0</v>
@@ -2739,13 +2745,13 @@
     </row>
     <row r="13" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D13" s="44">
         <v>1</v>
@@ -2761,7 +2767,7 @@
         <v>238</v>
       </c>
       <c r="I13" s="44" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2850,13 +2856,13 @@
     </row>
     <row r="17" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B17" s="44" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D17" s="44">
         <v>0</v>
@@ -2872,7 +2878,7 @@
         <v>238</v>
       </c>
       <c r="I17" s="44" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2931,13 +2937,13 @@
     </row>
     <row r="20" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -2950,7 +2956,7 @@
         <v>19965</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3017,13 +3023,13 @@
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -3036,7 +3042,7 @@
         <v>6900</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3045,13 +3051,13 @@
     </row>
     <row r="26" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="51" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B26" s="51" t="s">
         <v>61</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D26" s="51">
         <v>4</v>
@@ -3067,7 +3073,7 @@
         <v>238</v>
       </c>
       <c r="I26" s="51" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3245,7 +3251,7 @@
     </row>
     <row r="35" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E35" s="80"/>
       <c r="F35" s="80"/>
@@ -3273,13 +3279,13 @@
     </row>
     <row r="38" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="100" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B38" s="50" t="s">
         <v>61</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D38" s="50">
         <v>1</v>
@@ -3292,10 +3298,10 @@
         <v>728</v>
       </c>
       <c r="G38" s="50" t="s">
+        <v>541</v>
+      </c>
+      <c r="I38" s="50" t="s">
         <v>544</v>
-      </c>
-      <c r="I38" s="50" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3393,7 +3399,7 @@
         <v>61</v>
       </c>
       <c r="C42" s="51" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D42" s="51">
         <v>2</v>
@@ -3408,7 +3414,7 @@
         <v>39</v>
       </c>
       <c r="H42" s="23" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3416,10 +3422,10 @@
         <v>38</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D43" s="3">
         <v>2</v>
@@ -3443,7 +3449,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>42</v>
@@ -3465,7 +3471,7 @@
         <v>40</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3502,7 +3508,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>44</v>
@@ -3526,7 +3532,7 @@
     </row>
     <row r="47" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B47" s="23" t="s">
         <v>61</v>
@@ -3548,7 +3554,7 @@
         <v>39</v>
       </c>
       <c r="H47" s="23" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -3575,10 +3581,10 @@
         <v>39</v>
       </c>
       <c r="H48" s="51" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="I48" s="51" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3605,7 +3611,7 @@
         <v>39</v>
       </c>
       <c r="H49" s="23" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3695,7 +3701,7 @@
         <v>221</v>
       </c>
       <c r="I52" s="23" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3706,7 +3712,7 @@
         <v>61</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D53" s="23">
         <v>4</v>
@@ -3722,10 +3728,10 @@
         <v>39</v>
       </c>
       <c r="H53" s="23" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="I53" s="23" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3752,21 +3758,21 @@
         <v>39</v>
       </c>
       <c r="H54" s="23" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B55" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D55" s="23">
         <v>2</v>
@@ -3785,18 +3791,18 @@
         <v>225</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B56" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D56" s="23">
         <v>4</v>
@@ -3815,18 +3821,18 @@
         <v>225</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B57" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D57" s="23">
         <v>4</v>
@@ -3845,7 +3851,7 @@
         <v>225</v>
       </c>
       <c r="I57" s="23" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3853,7 +3859,7 @@
         <v>91863</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>47</v>
@@ -3865,7 +3871,7 @@
         <v>400</v>
       </c>
       <c r="F58" s="78">
-        <f t="shared" ref="F58:F78" si="5">E58*D58</f>
+        <f t="shared" ref="F58:F79" si="5">E58*D58</f>
         <v>800</v>
       </c>
       <c r="G58" s="4" t="s">
@@ -3875,18 +3881,18 @@
         <v>205</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>435</v>
+        <v>550</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C59" s="92" t="s">
-        <v>434</v>
+        <v>549</v>
       </c>
       <c r="D59" s="4">
         <v>2</v>
@@ -3905,18 +3911,18 @@
         <v>225</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="59" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B60" s="58" t="s">
         <v>61</v>
       </c>
       <c r="C60" s="59" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D60" s="58">
         <v>0</v>
@@ -3935,7 +3941,7 @@
         <v>225</v>
       </c>
       <c r="I60" s="58" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="J60" s="98"/>
     </row>
@@ -3966,7 +3972,7 @@
         <v>225</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3996,18 +4002,18 @@
         <v>225</v>
       </c>
       <c r="I62" s="27" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B63" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D63" s="23">
         <v>4</v>
@@ -4023,7 +4029,7 @@
         <v>39</v>
       </c>
       <c r="H63" s="23" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="I63" s="23" t="s">
         <v>211</v>
@@ -4080,7 +4086,7 @@
         <v>39</v>
       </c>
       <c r="H65" s="23" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="I65" s="23" t="s">
         <v>211</v>
@@ -4088,13 +4094,13 @@
     </row>
     <row r="66" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B66" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C66" s="24" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D66" s="23">
         <v>2</v>
@@ -4140,12 +4146,12 @@
         <v>225</v>
       </c>
       <c r="I67" s="23" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B68" s="23" t="s">
         <v>61</v>
@@ -4170,15 +4176,15 @@
         <v>220</v>
       </c>
       <c r="I68" s="26" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="62" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B69" s="27" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C69" s="25" t="s">
         <v>299</v>
@@ -4200,7 +4206,7 @@
         <v>220</v>
       </c>
       <c r="I69" s="26" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -4235,13 +4241,13 @@
     </row>
     <row r="71" spans="1:9" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="31" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B71" s="27" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D71" s="27">
         <v>2</v>
@@ -4260,18 +4266,18 @@
         <v>222</v>
       </c>
       <c r="I71" s="27" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="24" t="s">
-        <v>438</v>
+      <c r="A72" s="59" t="s">
+        <v>435</v>
       </c>
       <c r="B72" s="58" t="s">
         <v>61</v>
       </c>
       <c r="C72" s="59" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D72" s="58">
         <v>0</v>
@@ -4290,614 +4296,616 @@
         <v>222</v>
       </c>
       <c r="I72" s="58" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
-        <v>279</v>
+        <v>435</v>
       </c>
       <c r="B73" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>280</v>
+        <v>548</v>
       </c>
       <c r="D73" s="23">
         <v>2</v>
       </c>
       <c r="E73" s="81">
+        <v>36</v>
+      </c>
+      <c r="F73" s="82">
+        <f t="shared" ref="F73" si="7">E73*D73</f>
+        <v>72</v>
+      </c>
+      <c r="G73" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="H73" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="I73" s="23" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="24" t="s">
+        <v>279</v>
+      </c>
+      <c r="B74" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C74" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="D74" s="23">
+        <v>2</v>
+      </c>
+      <c r="E74" s="81">
         <v>2104</v>
       </c>
-      <c r="F73" s="82">
+      <c r="F74" s="82">
         <f t="shared" si="5"/>
         <v>4208</v>
       </c>
-      <c r="G73" s="3" t="s">
+      <c r="G74" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H73" s="23" t="s">
+      <c r="H74" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="I73" s="23" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="24" t="s">
+      <c r="I74" s="23" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="B74" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C74" s="24" t="s">
+      <c r="B75" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C75" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="D74" s="23">
+      <c r="D75" s="23">
         <v>2</v>
       </c>
-      <c r="E74" s="81">
+      <c r="E75" s="81">
         <v>82</v>
       </c>
-      <c r="F74" s="82">
+      <c r="F75" s="82">
         <f t="shared" si="5"/>
         <v>164</v>
       </c>
-      <c r="G74" s="3" t="s">
+      <c r="G75" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H74" s="23" t="s">
+      <c r="H75" s="23" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="75" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="30" t="s">
-        <v>455</v>
-      </c>
-      <c r="B75" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C75" s="24" t="s">
-        <v>456</v>
-      </c>
-      <c r="D75" s="23">
-        <v>1</v>
-      </c>
-      <c r="E75" s="81">
+    <row r="76" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="30" t="s">
+        <v>452</v>
+      </c>
+      <c r="B76" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C76" s="24" t="s">
+        <v>453</v>
+      </c>
+      <c r="D76" s="23">
+        <v>1</v>
+      </c>
+      <c r="E76" s="81">
         <v>520</v>
       </c>
-      <c r="F75" s="82">
+      <c r="F76" s="82">
         <f t="shared" si="5"/>
         <v>520</v>
       </c>
-      <c r="G75" s="3" t="s">
+      <c r="G76" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H75" s="23" t="s">
+      <c r="H76" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="I75" s="23" t="s">
+      <c r="I76" s="23" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="76" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="61" t="s">
-        <v>311</v>
-      </c>
-      <c r="B76" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C76" s="59" t="s">
+    <row r="77" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="B77" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C77" s="59" t="s">
         <v>283</v>
       </c>
-      <c r="D76" s="58">
+      <c r="D77" s="58">
         <v>0</v>
       </c>
-      <c r="E76" s="87">
+      <c r="E77" s="87">
         <v>390</v>
       </c>
-      <c r="F76" s="88">
+      <c r="F77" s="88">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G76" s="60" t="s">
+      <c r="G77" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="H76" s="58" t="s">
+      <c r="H77" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="I76" s="58" t="s">
+      <c r="I77" s="58" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="77" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="31" t="s">
-        <v>306</v>
-      </c>
-      <c r="B77" s="27" t="s">
-        <v>458</v>
-      </c>
-      <c r="C77" s="24" t="s">
+    <row r="78" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="31" t="s">
+        <v>551</v>
+      </c>
+      <c r="B78" s="27" t="s">
+        <v>455</v>
+      </c>
+      <c r="C78" s="24" t="s">
         <v>305</v>
       </c>
-      <c r="D77" s="23">
+      <c r="D78" s="23">
         <v>14</v>
       </c>
-      <c r="E77" s="81">
+      <c r="E78" s="81">
         <v>20</v>
       </c>
-      <c r="F77" s="82">
+      <c r="F78" s="82">
         <f t="shared" si="5"/>
         <v>280</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="G78" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H77" s="23" t="s">
+      <c r="H78" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="I77" s="27" t="s">
+      <c r="I78" s="27" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="31" t="s">
+        <v>308</v>
+      </c>
+      <c r="B79" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="C79" s="24" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="31" t="s">
-        <v>309</v>
-      </c>
-      <c r="B78" s="23" t="s">
-        <v>272</v>
-      </c>
-      <c r="C78" s="24" t="s">
-        <v>308</v>
-      </c>
-      <c r="D78" s="23">
-        <v>1</v>
-      </c>
-      <c r="E78" s="81">
+      <c r="D79" s="23">
+        <v>1</v>
+      </c>
+      <c r="E79" s="81">
         <v>10</v>
       </c>
-      <c r="F78" s="82">
+      <c r="F79" s="82">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="G78" s="3" t="s">
+      <c r="G79" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H78" s="23" t="s">
+      <c r="H79" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="I78" s="23" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="5" t="s">
+      <c r="I79" s="23" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A80" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E79" s="72"/>
-      <c r="F79" s="72"/>
-    </row>
-    <row r="80" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B80" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C80" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D80" s="23">
-        <v>1</v>
-      </c>
-      <c r="E80" s="81"/>
-      <c r="F80" s="82"/>
-      <c r="I80" s="23" t="s">
-        <v>250</v>
-      </c>
+      <c r="E80" s="72"/>
+      <c r="F80" s="72"/>
     </row>
     <row r="81" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D81" s="23">
+        <v>1</v>
+      </c>
+      <c r="E81" s="81"/>
+      <c r="F81" s="82"/>
+      <c r="I81" s="23" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="B81" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C81" s="24" t="s">
+      <c r="B82" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C82" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="D81" s="23">
-        <v>1</v>
-      </c>
-      <c r="E81" s="81">
+      <c r="D82" s="23">
+        <v>1</v>
+      </c>
+      <c r="E82" s="81">
         <v>63</v>
-      </c>
-      <c r="F81" s="82">
-        <f>D81*E81</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="B82" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C82" s="24" t="s">
-        <v>249</v>
-      </c>
-      <c r="D82" s="23">
-        <v>2</v>
-      </c>
-      <c r="E82" s="81">
-        <v>69</v>
       </c>
       <c r="F82" s="82">
         <f>D82*E82</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="B83" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C83" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="D83" s="23">
+        <v>2</v>
+      </c>
+      <c r="E83" s="81">
+        <v>69</v>
+      </c>
+      <c r="F83" s="82">
+        <f>D83*E83</f>
         <v>138</v>
       </c>
     </row>
-    <row r="83" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="23" t="s">
+    <row r="84" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B83" s="23" t="s">
+      <c r="B84" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C83" s="23" t="s">
+      <c r="C84" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D83" s="23">
-        <v>1</v>
-      </c>
-      <c r="E83" s="81"/>
-      <c r="F83" s="82"/>
-      <c r="I83" s="23" t="s">
+      <c r="D84" s="23">
+        <v>1</v>
+      </c>
+      <c r="E84" s="81"/>
+      <c r="F84" s="82"/>
+      <c r="I84" s="23" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="84" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="E84" s="72"/>
-      <c r="F84" s="72"/>
-    </row>
-    <row r="85" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
-        <v>409</v>
+    <row r="85" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A85" s="5" t="s">
+        <v>407</v>
       </c>
       <c r="E85" s="72"/>
       <c r="F85" s="72"/>
     </row>
-    <row r="86" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="3" t="s">
+    <row r="86" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="E86" s="72"/>
+      <c r="F86" s="72"/>
+    </row>
+    <row r="87" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B87" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="C87" s="67" t="s">
+        <v>409</v>
+      </c>
+      <c r="D87" s="3">
+        <v>1</v>
+      </c>
+      <c r="E87" s="71">
+        <v>200</v>
+      </c>
+      <c r="F87" s="71">
+        <f>E87*D87</f>
+        <v>200</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J87" s="4"/>
+    </row>
+    <row r="88" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="C88" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="C86" s="67" t="s">
-        <v>410</v>
-      </c>
-      <c r="D86" s="3">
-        <v>1</v>
-      </c>
-      <c r="E86" s="71">
-        <v>200</v>
-      </c>
-      <c r="F86" s="71">
-        <f>E86*D86</f>
-        <v>200</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="J86" s="4"/>
-    </row>
-    <row r="87" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="C87" s="4" t="s">
+      <c r="D88" s="4">
+        <v>5</v>
+      </c>
+      <c r="E88" s="78">
+        <v>1</v>
+      </c>
+      <c r="F88" s="78">
+        <f>E88*D88</f>
+        <v>5</v>
+      </c>
+      <c r="I88" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="D87" s="4">
-        <v>5</v>
-      </c>
-      <c r="E87" s="78">
-        <v>1</v>
-      </c>
-      <c r="F87" s="78">
-        <f>E87*D87</f>
-        <v>5</v>
-      </c>
-      <c r="I87" s="4" t="s">
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="51" t="s">
+        <v>416</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="51" t="s">
-        <v>417</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="D88" s="3">
-        <v>1</v>
-      </c>
-      <c r="E88" s="71">
+      <c r="D89" s="3">
+        <v>1</v>
+      </c>
+      <c r="E89" s="71">
         <v>26</v>
-      </c>
-      <c r="F88" s="71">
-        <f>E88*D88</f>
-        <v>26</v>
-      </c>
-      <c r="I88" s="3" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="D89" s="3">
-        <v>1</v>
-      </c>
-      <c r="E89" s="71">
-        <v>37</v>
       </c>
       <c r="F89" s="71">
         <f>E89*D89</f>
+        <v>26</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D90" s="3">
+        <v>1</v>
+      </c>
+      <c r="E90" s="71">
         <v>37</v>
-      </c>
-      <c r="I89" s="51" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="51" t="s">
-        <v>344</v>
-      </c>
-      <c r="B90" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="C90" s="51" t="s">
-        <v>343</v>
-      </c>
-      <c r="D90" s="51">
-        <v>2</v>
-      </c>
-      <c r="E90" s="71">
-        <v>24</v>
       </c>
       <c r="F90" s="71">
         <f>E90*D90</f>
+        <v>37</v>
+      </c>
+      <c r="I90" s="51" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="51" t="s">
+        <v>343</v>
+      </c>
+      <c r="B91" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C91" s="51" t="s">
+        <v>342</v>
+      </c>
+      <c r="D91" s="51">
+        <v>2</v>
+      </c>
+      <c r="E91" s="71">
+        <v>24</v>
+      </c>
+      <c r="F91" s="71">
+        <f>E91*D91</f>
         <v>48</v>
       </c>
-      <c r="I90" s="23" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="56" t="s">
+      <c r="I91" s="23" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="56" t="s">
         <v>167</v>
-      </c>
-      <c r="E91" s="89"/>
-      <c r="F91" s="89"/>
-    </row>
-    <row r="92" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="15" t="s">
-        <v>168</v>
       </c>
       <c r="E92" s="89"/>
       <c r="F92" s="89"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="B93" s="3" t="s">
+    <row r="93" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E93" s="89"/>
+      <c r="F93" s="89"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C93" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="D93" s="3">
-        <v>1</v>
-      </c>
-      <c r="E93" s="71">
+      <c r="C94" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D94" s="3">
+        <v>1</v>
+      </c>
+      <c r="E94" s="71">
         <v>625</v>
       </c>
-      <c r="F93" s="71">
-        <f>E93*D93</f>
+      <c r="F94" s="71">
+        <f>E94*D94</f>
         <v>625</v>
       </c>
-      <c r="G93" s="3" t="s">
+      <c r="G94" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I93" s="3" t="s">
+      <c r="I94" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="94" spans="1:10" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A94" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="E94" s="90"/>
-      <c r="F94" s="90"/>
-    </row>
-    <row r="95" spans="1:10" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="21" t="s">
-        <v>493</v>
-      </c>
-      <c r="B95" s="20" t="s">
-        <v>324</v>
-      </c>
-      <c r="C95" s="95" t="s">
-        <v>494</v>
-      </c>
-      <c r="D95" s="20">
-        <v>1</v>
-      </c>
-      <c r="E95" s="91">
+    <row r="95" spans="1:10" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A95" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="E95" s="90"/>
+      <c r="F95" s="90"/>
+    </row>
+    <row r="96" spans="1:10" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="21" t="s">
+        <v>490</v>
+      </c>
+      <c r="B96" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="C96" s="95" t="s">
+        <v>491</v>
+      </c>
+      <c r="D96" s="20">
+        <v>1</v>
+      </c>
+      <c r="E96" s="91">
         <v>900</v>
       </c>
-      <c r="F95" s="91">
-        <f t="shared" ref="F95:F101" si="7">E95*D95</f>
+      <c r="F96" s="91">
+        <f t="shared" ref="F96:F102" si="8">E96*D96</f>
         <v>900</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I95" s="20" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="22" t="s">
-        <v>497</v>
-      </c>
-      <c r="B96" s="20" t="s">
-        <v>324</v>
-      </c>
-      <c r="C96" s="96" t="s">
-        <v>495</v>
-      </c>
-      <c r="D96" s="3">
-        <v>1</v>
-      </c>
-      <c r="E96" s="71">
-        <v>767</v>
-      </c>
-      <c r="F96" s="91">
-        <f t="shared" si="7"/>
-        <v>767</v>
       </c>
       <c r="G96" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H96" s="20"/>
-      <c r="I96" s="3" t="s">
-        <v>502</v>
+      <c r="I96" s="20" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="22" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B97" s="20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C97" s="96" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D97" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E97" s="71">
-        <v>1540</v>
+        <v>767</v>
       </c>
       <c r="F97" s="91">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>767</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H97" s="20"/>
       <c r="I97" s="3" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="3" t="s">
-        <v>500</v>
+      <c r="A98" s="22" t="s">
+        <v>495</v>
       </c>
       <c r="B98" s="20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C98" s="96" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="D98" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98" s="71">
-        <v>877</v>
+        <v>1540</v>
       </c>
       <c r="F98" s="91">
-        <f t="shared" si="7"/>
-        <v>877</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H98" s="20"/>
       <c r="I98" s="3" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="51" t="s">
-        <v>501</v>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="3" t="s">
+        <v>497</v>
       </c>
       <c r="B99" s="20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C99" s="96" t="s">
-        <v>425</v>
-      </c>
-      <c r="D99" s="51">
+        <v>496</v>
+      </c>
+      <c r="D99" s="3">
+        <v>1</v>
+      </c>
+      <c r="E99" s="71">
+        <v>877</v>
+      </c>
+      <c r="F99" s="91">
+        <f t="shared" si="8"/>
+        <v>877</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H99" s="20"/>
+      <c r="I99" s="3" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="51" t="s">
+        <v>498</v>
+      </c>
+      <c r="B100" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="C100" s="96" t="s">
+        <v>424</v>
+      </c>
+      <c r="D100" s="51">
         <v>0</v>
       </c>
-      <c r="E99" s="71">
+      <c r="E100" s="71">
         <v>4700</v>
       </c>
-      <c r="F99" s="91">
-        <f t="shared" si="7"/>
+      <c r="F100" s="91">
+        <f t="shared" si="8"/>
         <v>0</v>
-      </c>
-      <c r="G99" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="H99" s="20"/>
-      <c r="I99" s="51" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="51" t="s">
-        <v>504</v>
-      </c>
-      <c r="B100" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C100" s="51" t="s">
-        <v>505</v>
-      </c>
-      <c r="D100" s="51">
-        <v>1</v>
-      </c>
-      <c r="E100" s="71">
-        <v>20</v>
-      </c>
-      <c r="F100" s="91">
-        <f t="shared" si="7"/>
-        <v>20</v>
       </c>
       <c r="G100" s="51" t="s">
         <v>13</v>
@@ -4907,334 +4915,338 @@
         <v>508</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
-        <v>506</v>
+    <row r="101" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="51" t="s">
+        <v>501</v>
       </c>
       <c r="B101" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C101" s="32" t="s">
-        <v>507</v>
-      </c>
-      <c r="D101" s="3">
+      <c r="C101" s="51" t="s">
+        <v>502</v>
+      </c>
+      <c r="D101" s="51">
         <v>1</v>
       </c>
       <c r="E101" s="71">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F101" s="91">
-        <f t="shared" si="7"/>
-        <v>25</v>
-      </c>
-      <c r="G101" s="3" t="s">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="G101" s="51" t="s">
         <v>13</v>
       </c>
       <c r="H101" s="20"/>
       <c r="I101" s="51" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A102" s="17" t="s">
-        <v>354</v>
-      </c>
-      <c r="E102" s="90"/>
-      <c r="F102" s="90"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
-        <v>513</v>
-      </c>
-      <c r="B103" s="20" t="s">
-        <v>324</v>
-      </c>
-      <c r="C103" s="68" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C102" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="D102" s="3">
+        <v>1</v>
+      </c>
+      <c r="E102" s="71">
+        <v>25</v>
+      </c>
+      <c r="F102" s="91">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H102" s="20"/>
+      <c r="I102" s="51" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A103" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="E103" s="90"/>
+      <c r="F103" s="90"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="B104" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="C104" s="68" t="s">
+        <v>355</v>
+      </c>
+      <c r="D104" s="3">
+        <v>1</v>
+      </c>
+      <c r="E104" s="71">
+        <v>752</v>
+      </c>
+      <c r="F104" s="71">
+        <f t="shared" ref="F104:F108" si="9">D104*E104</f>
+        <v>752</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I104" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="D103" s="3">
-        <v>1</v>
-      </c>
-      <c r="E103" s="71">
-        <v>752</v>
-      </c>
-      <c r="F103" s="71">
-        <f t="shared" ref="F103:F107" si="8">D103*E103</f>
-        <v>752</v>
-      </c>
-      <c r="G103" s="3" t="s">
+    </row>
+    <row r="105" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B105" s="64" t="s">
+        <v>228</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="D105" s="4">
+        <v>1</v>
+      </c>
+      <c r="E105" s="78">
+        <v>1</v>
+      </c>
+      <c r="F105" s="78">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="G105" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I103" s="3" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="B104" s="64" t="s">
-        <v>228</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="D104" s="4">
-        <v>1</v>
-      </c>
-      <c r="E104" s="78">
-        <v>1</v>
-      </c>
-      <c r="F104" s="78">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="G104" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I104" s="4" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="B105" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="D105" s="3">
-        <v>1</v>
-      </c>
-      <c r="E105" s="71">
-        <v>65</v>
-      </c>
-      <c r="F105" s="71">
-        <f t="shared" si="8"/>
-        <v>65</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I105" s="3" t="s">
-        <v>362</v>
+      <c r="I105" s="4" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B106" s="20" t="s">
         <v>61</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D106" s="3">
         <v>1</v>
       </c>
       <c r="E106" s="71">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="F106" s="71">
-        <f t="shared" si="8"/>
-        <v>32</v>
+        <f t="shared" si="9"/>
+        <v>65</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>347</v>
+        <v>362</v>
       </c>
       <c r="B107" s="20" t="s">
         <v>61</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>348</v>
+        <v>363</v>
       </c>
       <c r="D107" s="3">
         <v>1</v>
       </c>
       <c r="E107" s="71">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="F107" s="71">
-        <f t="shared" si="8"/>
-        <v>112</v>
+        <f t="shared" si="9"/>
+        <v>32</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A108" s="5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B108" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="D108" s="3">
+        <v>1</v>
+      </c>
+      <c r="E108" s="71">
+        <v>112</v>
+      </c>
+      <c r="F108" s="71">
+        <f t="shared" si="9"/>
+        <v>112</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A109" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E108" s="72"/>
-      <c r="F108" s="72"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D109" s="3">
-        <v>1</v>
-      </c>
-      <c r="E109" s="71">
-        <v>3582</v>
-      </c>
-      <c r="F109" s="71">
-        <f t="shared" ref="F109:F121" si="9">E109*D109</f>
-        <v>3582</v>
-      </c>
-      <c r="G109" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I109" s="3" t="s">
-        <v>492</v>
-      </c>
+      <c r="E109" s="72"/>
+      <c r="F109" s="72"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>181</v>
+        <v>57</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>183</v>
+        <v>58</v>
       </c>
       <c r="D110" s="3">
         <v>1</v>
       </c>
       <c r="E110" s="71">
-        <v>1630</v>
+        <v>3582</v>
       </c>
       <c r="F110" s="71">
-        <f t="shared" si="9"/>
-        <v>1630</v>
+        <f t="shared" ref="F110:F122" si="10">E110*D110</f>
+        <v>3582</v>
       </c>
       <c r="G110" s="3" t="s">
         <v>51</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>548</v>
+        <v>489</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D111" s="3">
         <v>1</v>
       </c>
       <c r="E111" s="71">
-        <v>886</v>
+        <v>1630</v>
       </c>
       <c r="F111" s="71">
-        <f t="shared" si="9"/>
-        <v>886</v>
+        <f t="shared" si="10"/>
+        <v>1630</v>
       </c>
       <c r="G111" s="3" t="s">
         <v>51</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D112" s="3">
         <v>1</v>
       </c>
       <c r="E112" s="71">
-        <v>163</v>
+        <v>886</v>
       </c>
       <c r="F112" s="71">
-        <f t="shared" si="9"/>
-        <v>163</v>
+        <f t="shared" si="10"/>
+        <v>886</v>
       </c>
       <c r="G112" s="3" t="s">
         <v>51</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>185</v>
+        <v>546</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>52</v>
+        <v>184</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D113" s="3">
         <v>1</v>
       </c>
       <c r="E113" s="71">
-        <v>11</v>
+        <v>163</v>
       </c>
       <c r="F113" s="71">
-        <f t="shared" si="9"/>
-        <v>11</v>
+        <f t="shared" si="10"/>
+        <v>163</v>
       </c>
       <c r="G113" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="I113" s="3" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>56</v>
+        <v>178</v>
       </c>
       <c r="D114" s="3">
         <v>1</v>
       </c>
       <c r="E114" s="71">
-        <v>520</v>
+        <v>11</v>
       </c>
       <c r="F114" s="71">
-        <f t="shared" si="9"/>
-        <v>520</v>
+        <f t="shared" si="10"/>
+        <v>11</v>
       </c>
       <c r="G114" s="3" t="s">
         <v>51</v>
@@ -5242,125 +5254,125 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>187</v>
+        <v>55</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>186</v>
+        <v>56</v>
       </c>
       <c r="D115" s="3">
         <v>1</v>
       </c>
       <c r="E115" s="71">
-        <v>193</v>
+        <v>520</v>
       </c>
       <c r="F115" s="71">
-        <f t="shared" si="9"/>
-        <v>193</v>
+        <f t="shared" si="10"/>
+        <v>520</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="116" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="B116" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C116" s="23" t="s">
-        <v>292</v>
-      </c>
-      <c r="D116" s="23">
-        <v>10</v>
-      </c>
-      <c r="E116" s="82">
-        <v>12</v>
-      </c>
-      <c r="F116" s="82">
-        <f t="shared" si="9"/>
-        <v>120</v>
-      </c>
-      <c r="G116" s="23" t="s">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D116" s="3">
+        <v>1</v>
+      </c>
+      <c r="E116" s="71">
+        <v>193</v>
+      </c>
+      <c r="F116" s="71">
+        <f t="shared" si="10"/>
+        <v>193</v>
+      </c>
+      <c r="G116" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="I116" s="23" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="23" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B117" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C117" s="23" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D117" s="23">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E117" s="82">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F117" s="82">
-        <f t="shared" si="9"/>
-        <v>14</v>
+        <f t="shared" si="10"/>
+        <v>120</v>
       </c>
       <c r="G117" s="23" t="s">
         <v>51</v>
       </c>
       <c r="I117" s="23" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D118" s="3">
-        <v>4</v>
-      </c>
-      <c r="E118" s="71">
-        <v>15.25</v>
-      </c>
-      <c r="F118" s="71">
-        <f t="shared" si="9"/>
-        <v>61</v>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="B118" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C118" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="D118" s="23">
+        <v>1</v>
+      </c>
+      <c r="E118" s="82">
+        <v>14</v>
+      </c>
+      <c r="F118" s="82">
+        <f t="shared" si="10"/>
+        <v>14</v>
       </c>
       <c r="G118" s="23" t="s">
         <v>51</v>
       </c>
+      <c r="I118" s="23" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D119" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E119" s="71">
-        <v>16.5</v>
+        <v>15.25</v>
       </c>
       <c r="F119" s="71">
-        <f t="shared" si="9"/>
-        <v>165</v>
+        <f t="shared" si="10"/>
+        <v>61</v>
       </c>
       <c r="G119" s="23" t="s">
         <v>51</v>
@@ -5368,23 +5380,23 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D120" s="3">
         <v>10</v>
       </c>
       <c r="E120" s="71">
-        <v>24</v>
+        <v>16.5</v>
       </c>
       <c r="F120" s="71">
-        <f t="shared" si="9"/>
-        <v>240</v>
+        <f t="shared" si="10"/>
+        <v>165</v>
       </c>
       <c r="G120" s="23" t="s">
         <v>51</v>
@@ -5392,177 +5404,180 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D121" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E121" s="71">
         <v>24</v>
       </c>
       <c r="F121" s="71">
-        <f t="shared" si="9"/>
-        <v>144</v>
+        <f t="shared" si="10"/>
+        <v>240</v>
       </c>
       <c r="G121" s="23" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="122" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E122" s="82"/>
-      <c r="F122" s="82"/>
-    </row>
-    <row r="124" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A124" s="10"/>
-      <c r="B124" s="10"/>
-      <c r="C124" s="9"/>
-    </row>
-    <row r="125" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="7" t="s">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D122" s="3">
+        <v>6</v>
+      </c>
+      <c r="E122" s="71">
+        <v>24</v>
+      </c>
+      <c r="F122" s="71">
+        <f t="shared" si="10"/>
+        <v>144</v>
+      </c>
+      <c r="G122" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E123" s="82"/>
+      <c r="F123" s="82"/>
+    </row>
+    <row r="125" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A125" s="10"/>
+      <c r="B125" s="10"/>
+      <c r="C125" s="9"/>
+    </row>
+    <row r="126" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A126" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E125" s="72"/>
-      <c r="F125" s="72"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D126" s="3">
-        <v>4</v>
-      </c>
-      <c r="E126" s="71">
-        <v>16.5</v>
-      </c>
-      <c r="F126" s="71">
-        <f t="shared" ref="F126:F141" si="10">E126*D126</f>
-        <v>66</v>
-      </c>
-      <c r="I126" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="E126" s="72"/>
+      <c r="F126" s="72"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D127" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E127" s="71">
-        <v>85.1</v>
+        <v>16.5</v>
       </c>
       <c r="F127" s="71">
-        <f t="shared" si="10"/>
-        <v>85.1</v>
+        <f t="shared" ref="F127:F142" si="11">E127*D127</f>
+        <v>66</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D128" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E128" s="71">
-        <v>32</v>
+        <v>85.1</v>
       </c>
       <c r="F128" s="71">
-        <f t="shared" si="10"/>
-        <v>64</v>
-      </c>
-      <c r="I128" s="3" t="s">
-        <v>131</v>
+        <f t="shared" si="11"/>
+        <v>85.1</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D129" s="3">
         <v>2</v>
       </c>
       <c r="E129" s="71">
-        <v>51.58</v>
+        <v>32</v>
       </c>
       <c r="F129" s="71">
-        <f t="shared" si="10"/>
-        <v>103.16</v>
+        <f t="shared" si="11"/>
+        <v>64</v>
+      </c>
+      <c r="I129" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D130" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E130" s="71">
-        <v>60</v>
+        <v>51.58</v>
       </c>
       <c r="F130" s="71">
-        <f t="shared" si="10"/>
-        <v>60</v>
-      </c>
-      <c r="I130" s="3" t="s">
-        <v>136</v>
+        <f t="shared" si="11"/>
+        <v>103.16</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D131" s="3">
         <v>1</v>
       </c>
       <c r="E131" s="71">
-        <v>136.47999999999999</v>
+        <v>60</v>
       </c>
       <c r="F131" s="71">
-        <f t="shared" si="10"/>
-        <v>136.47999999999999</v>
+        <f t="shared" si="11"/>
+        <v>60</v>
+      </c>
+      <c r="I131" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -5573,7 +5588,7 @@
         <v>61</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D132" s="3">
         <v>1</v>
@@ -5582,305 +5597,305 @@
         <v>136.47999999999999</v>
       </c>
       <c r="F132" s="71">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>136.47999999999999</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D133" s="3">
         <v>1</v>
       </c>
       <c r="E133" s="71">
-        <v>60.95</v>
+        <v>136.47999999999999</v>
       </c>
       <c r="F133" s="71">
-        <f t="shared" si="10"/>
-        <v>60.95</v>
+        <f t="shared" si="11"/>
+        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D134" s="3">
         <v>1</v>
       </c>
       <c r="E134" s="71">
-        <v>119.416</v>
+        <v>60.95</v>
       </c>
       <c r="F134" s="71">
-        <f t="shared" si="10"/>
-        <v>119.416</v>
+        <f t="shared" si="11"/>
+        <v>60.95</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D135" s="3">
         <v>1</v>
       </c>
       <c r="E135" s="71">
-        <v>105.8</v>
+        <v>119.416</v>
       </c>
       <c r="F135" s="71">
-        <f t="shared" si="10"/>
-        <v>105.8</v>
+        <f t="shared" si="11"/>
+        <v>119.416</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D136" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E136" s="71">
-        <v>119.6</v>
+        <v>105.8</v>
       </c>
       <c r="F136" s="71">
-        <f t="shared" si="10"/>
-        <v>239.2</v>
+        <f t="shared" si="11"/>
+        <v>105.8</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>300</v>
+        <v>146</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>301</v>
+        <v>147</v>
       </c>
       <c r="D137" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E137" s="71">
-        <v>100</v>
+        <v>119.6</v>
       </c>
       <c r="F137" s="71">
-        <f t="shared" si="10"/>
-        <v>100</v>
+        <f t="shared" si="11"/>
+        <v>239.2</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>148</v>
+        <v>300</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>149</v>
+        <v>301</v>
       </c>
       <c r="D138" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E138" s="71">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F138" s="71">
-        <f t="shared" si="10"/>
-        <v>184</v>
+        <f t="shared" si="11"/>
+        <v>100</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D139" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E139" s="71">
-        <v>96.23</v>
+        <v>92</v>
       </c>
       <c r="F139" s="71">
-        <f t="shared" si="10"/>
-        <v>96.23</v>
+        <f t="shared" si="11"/>
+        <v>184</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D140" s="3">
         <v>1</v>
       </c>
       <c r="E140" s="71">
-        <v>102.44</v>
+        <v>96.23</v>
       </c>
       <c r="F140" s="71">
-        <f t="shared" si="10"/>
-        <v>102.44</v>
+        <f t="shared" si="11"/>
+        <v>96.23</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D141" s="3">
+        <v>1</v>
+      </c>
+      <c r="E141" s="71">
+        <v>102.44</v>
+      </c>
+      <c r="F141" s="71">
+        <f t="shared" si="11"/>
+        <v>102.44</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B141" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C141" s="3" t="s">
+      <c r="B142" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C142" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D141" s="3">
+      <c r="D142" s="3">
         <v>2</v>
       </c>
-      <c r="E141" s="71">
+      <c r="E142" s="71">
         <v>28</v>
       </c>
-      <c r="F141" s="71">
-        <f t="shared" si="10"/>
+      <c r="F142" s="71">
+        <f t="shared" si="11"/>
         <v>56</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C142" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D142" s="3">
-        <v>4</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C143" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D143" s="3">
-        <v>1</v>
-      </c>
-      <c r="I143" s="3" t="s">
-        <v>158</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C144" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D144" s="3">
+        <v>1</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C145" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D144" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="7" t="s">
+      <c r="D145" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A147" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B146" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="E146" s="72"/>
-      <c r="F146" s="72"/>
-    </row>
-    <row r="147" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="51"/>
-      <c r="B147" s="51" t="s">
-        <v>443</v>
-      </c>
-      <c r="C147" s="53" t="s">
+      <c r="B147" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E147" s="72"/>
+      <c r="F147" s="72"/>
+    </row>
+    <row r="148" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="51"/>
+      <c r="B148" s="51" t="s">
+        <v>440</v>
+      </c>
+      <c r="C148" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="D147" s="51">
+      <c r="D148" s="51">
         <v>4</v>
       </c>
-      <c r="E147" s="71">
+      <c r="E148" s="71">
         <v>40</v>
-      </c>
-      <c r="F147" s="71">
-        <f>E147*D147</f>
-        <v>160</v>
-      </c>
-      <c r="G147" s="51" t="s">
-        <v>441</v>
-      </c>
-      <c r="H147" s="51" t="s">
-        <v>442</v>
-      </c>
-      <c r="I147" s="51" t="s">
-        <v>440</v>
-      </c>
-      <c r="J147" s="53"/>
-    </row>
-    <row r="148" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B148" s="51" t="s">
-        <v>162</v>
-      </c>
-      <c r="C148" s="51" t="s">
-        <v>352</v>
-      </c>
-      <c r="D148" s="51">
-        <v>2</v>
-      </c>
-      <c r="E148" s="71">
-        <v>331</v>
       </c>
       <c r="F148" s="71">
         <f>E148*D148</f>
-        <v>662</v>
+        <v>160</v>
       </c>
       <c r="G148" s="51" t="s">
-        <v>444</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="H148" s="51" t="s">
+        <v>439</v>
+      </c>
+      <c r="I148" s="51" t="s">
+        <v>437</v>
+      </c>
+      <c r="J148" s="53"/>
     </row>
     <row r="149" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B149" s="51" t="s">
         <v>162</v>
       </c>
       <c r="C149" s="51" t="s">
-        <v>287</v>
+        <v>351</v>
       </c>
       <c r="D149" s="51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E149" s="71">
-        <v>25</v>
+        <v>331</v>
       </c>
       <c r="F149" s="71">
         <f>E149*D149</f>
-        <v>100</v>
+        <v>662</v>
       </c>
       <c r="G149" s="51" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="150" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -5888,20 +5903,20 @@
         <v>162</v>
       </c>
       <c r="C150" s="51" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D150" s="51">
         <v>4</v>
       </c>
       <c r="E150" s="71">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F150" s="71">
         <f>E150*D150</f>
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G150" s="51" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="151" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -5909,206 +5924,227 @@
         <v>162</v>
       </c>
       <c r="C151" s="51" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D151" s="51">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E151" s="71">
-        <v>121.5</v>
+        <v>28</v>
       </c>
       <c r="F151" s="71">
         <f>E151*D151</f>
+        <v>112</v>
+      </c>
+      <c r="G151" s="51" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C152" s="51" t="s">
+        <v>289</v>
+      </c>
+      <c r="D152" s="51">
+        <v>6</v>
+      </c>
+      <c r="E152" s="71">
+        <v>121.5</v>
+      </c>
+      <c r="F152" s="71">
+        <f>E152*D152</f>
         <v>729</v>
       </c>
-      <c r="G151" s="51" t="s">
+      <c r="G152" s="51" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E155" s="66" t="s">
+        <v>470</v>
+      </c>
+      <c r="F155" s="66">
+        <f>SUM(F3:F153)</f>
+        <v>95573.501499199992</v>
+      </c>
+      <c r="G155" s="3" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E157" s="71"/>
+      <c r="F157" s="71"/>
+    </row>
+    <row r="159" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A159" s="65" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A160" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C160" s="4" t="s">
         <v>444</v>
-      </c>
-    </row>
-    <row r="154" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E154" s="66" t="s">
-        <v>473</v>
-      </c>
-      <c r="F154" s="66">
-        <f>SUM(F3:F152)</f>
-        <v>95501.501499199992</v>
-      </c>
-      <c r="G154" s="3" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E156" s="71"/>
-      <c r="F156" s="71"/>
-    </row>
-    <row r="158" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A158" s="65" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="159" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A159" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="B159" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="C159" s="4" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A160" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="B160" s="3">
-        <v>14</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B161" s="3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="B162" s="3">
         <v>2</v>
       </c>
-      <c r="C162" s="51" t="s">
-        <v>460</v>
+      <c r="C162" s="3" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B163" s="3">
         <v>2</v>
       </c>
-      <c r="C163" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A166" s="65" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A167" s="4" t="s">
+      <c r="C163" s="51" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B167" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="C167" s="4" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
+      <c r="B164" s="3">
+        <v>2</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A167" s="65" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A168" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C168" s="4" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="B169" s="3">
+        <v>2</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A170" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B170" s="3">
+        <v>5</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B171" s="3">
+        <v>1</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A174" s="65" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A175" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="51" t="s">
         <v>462</v>
       </c>
-      <c r="B168" s="3">
-        <v>2</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A169" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="B169" s="3">
+      <c r="B176" s="3">
         <v>5</v>
       </c>
-      <c r="C169" s="3" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="B170" s="3">
-        <v>1</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A173" s="65" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A174" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="B174" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="C174" s="4" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="51" t="s">
-        <v>465</v>
-      </c>
-      <c r="B175" s="3">
-        <v>5</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B176" s="3">
-        <v>3</v>
-      </c>
       <c r="C176" s="3" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="B177" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B177" s="3">
+        <v>3</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="B178" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="C177" s="3" t="s">
-        <v>472</v>
+      <c r="C178" s="3" t="s">
+        <v>469</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C95" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C96" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C97" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C98" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C103" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C86" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C99" r:id="rId7" xr:uid="{3002EF90-377A-4FAD-A836-B22D0D243A96}"/>
+    <hyperlink ref="C96" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C97" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C98" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C99" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C104" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C87" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C100" r:id="rId7" xr:uid="{3002EF90-377A-4FAD-A836-B22D0D243A96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
@@ -6191,7 +6227,7 @@
         <v>7400</v>
       </c>
       <c r="I3" s="44" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6217,10 +6253,10 @@
     </row>
     <row r="5" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
+        <v>386</v>
+      </c>
+      <c r="C5" s="33" t="s">
         <v>387</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>388</v>
       </c>
       <c r="D5" s="33">
         <v>1</v>
@@ -6232,13 +6268,13 @@
         <v>50000</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -6261,27 +6297,27 @@
         <v>25000</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:9" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D12" s="33">
         <v>1</v>
@@ -6297,21 +6333,21 @@
         <v>13</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D13" s="33">
         <v>1</v>
@@ -6327,21 +6363,21 @@
         <v>13</v>
       </c>
       <c r="H13" s="33" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I13" s="33" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>61</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D14" s="33">
         <v>1</v>
@@ -6357,21 +6393,21 @@
         <v>13</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I14" s="33" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>61</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D15" s="33">
         <v>1</v>
@@ -6387,10 +6423,10 @@
         <v>13</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I15" s="33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6417,22 +6453,22 @@
         <v>13</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I16" s="34" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -6541,27 +6577,27 @@
     </row>
     <row r="24" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" s="42" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
     </row>
     <row r="26" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B26" s="34" t="s">
         <v>228</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D26" s="34">
         <v>2</v>
@@ -6577,21 +6613,21 @@
         <v>39</v>
       </c>
       <c r="H26" s="34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I26" s="34" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B27" s="34" t="s">
         <v>272</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D27" s="34">
         <v>2</v>
@@ -6607,10 +6643,10 @@
         <v>39</v>
       </c>
       <c r="H27" s="34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I27" s="34" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6618,10 +6654,10 @@
         <v>298</v>
       </c>
       <c r="B28" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="C28" s="37" t="s">
         <v>326</v>
-      </c>
-      <c r="C28" s="37" t="s">
-        <v>327</v>
       </c>
       <c r="D28" s="34">
         <v>8</v>
@@ -6637,21 +6673,21 @@
         <v>39</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I28" s="34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B29" s="34" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D29" s="34">
         <v>6</v>
@@ -6667,18 +6703,18 @@
         <v>39</v>
       </c>
       <c r="H29" s="34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B30" s="34" t="s">
         <v>228</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D30" s="34">
         <v>2</v>
@@ -6694,21 +6730,21 @@
         <v>39</v>
       </c>
       <c r="H30" s="34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I30" s="34" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B31" s="34" t="s">
         <v>272</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D31" s="34">
         <v>1</v>
@@ -6724,21 +6760,21 @@
         <v>39</v>
       </c>
       <c r="H31" s="34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I31" s="34" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B32" s="34" t="s">
         <v>272</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D32" s="34">
         <v>1</v>
@@ -6754,10 +6790,10 @@
         <v>39</v>
       </c>
       <c r="H32" s="34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I32" s="34" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6784,7 +6820,7 @@
         <v>39</v>
       </c>
       <c r="H33" s="34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -6818,7 +6854,7 @@
         <v>51</v>
       </c>
       <c r="I38" s="44" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -7320,7 +7356,7 @@
     </row>
     <row r="66" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F66" s="8"/>
     </row>
@@ -7345,18 +7381,18 @@
         <v>280</v>
       </c>
       <c r="I67" s="33" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>373</v>
+      </c>
+      <c r="B68" s="47" t="s">
         <v>374</v>
       </c>
-      <c r="B68" s="47" t="s">
+      <c r="C68" s="47" t="s">
         <v>375</v>
-      </c>
-      <c r="C68" s="47" t="s">
-        <v>376</v>
       </c>
       <c r="D68" s="47">
         <v>2</v>
@@ -7369,18 +7405,18 @@
         <v>168</v>
       </c>
       <c r="I68" s="47" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B69" s="47" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C69" s="47" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D69" s="47">
         <v>1</v>
@@ -7393,18 +7429,18 @@
         <v>54</v>
       </c>
       <c r="I69" s="47" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F71" s="8"/>
     </row>
     <row r="72" spans="1:10" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="33" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C72" s="49"/>
       <c r="E72" s="36"/>
@@ -7413,7 +7449,7 @@
     </row>
     <row r="73" spans="1:10" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C73" s="49"/>
       <c r="E73" s="36"/>
@@ -7431,20 +7467,20 @@
         <v>161</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
     </row>
     <row r="76" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="54" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B76" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C76" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D76" s="54">
         <v>1</v>
@@ -7462,13 +7498,13 @@
     </row>
     <row r="77" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="54" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B77" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C77" s="54" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D77" s="54">
         <v>1</v>
@@ -7483,13 +7519,13 @@
     </row>
     <row r="78" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="54" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B78" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C78" s="54" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D78" s="54">
         <v>1</v>
@@ -7507,13 +7543,13 @@
     </row>
     <row r="79" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="54" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B79" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C79" s="54" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D79" s="54">
         <v>1</v>
@@ -7528,13 +7564,13 @@
     </row>
     <row r="80" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="54" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B80" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C80" s="54" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D80" s="54">
         <v>1</v>
@@ -7549,13 +7585,13 @@
     </row>
     <row r="81" spans="1:6" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="54" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B81" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C81" s="54" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D81" s="54">
         <v>1</v>
@@ -7570,13 +7606,13 @@
     </row>
     <row r="82" spans="1:6" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="54" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B82" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C82" s="54" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D82" s="54">
         <v>1</v>
@@ -7591,13 +7627,13 @@
     </row>
     <row r="83" spans="1:6" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="54" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B83" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C83" s="54" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D83" s="54">
         <v>1</v>

</xml_diff>

<commit_message>
remove and rename obsolete Thorlabs cage plate.
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651385D5-BEB2-4129-849D-80DB34070363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0180F988-F2D5-4563-9AAD-26206043CA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18996" yWindow="6156" windowWidth="34368" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16308" yWindow="4500" windowWidth="34368" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="556">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -1376,9 +1376,6 @@
     <t>LCP31/M</t>
   </si>
   <si>
-    <t>QS15-mount-modified-Thorlabs-CagePlate-LCP03.ipt</t>
-  </si>
-  <si>
     <t>One for each planned immersion cuvette mount / imaging medium</t>
   </si>
   <si>
@@ -1679,9 +1676,6 @@
     </r>
   </si>
   <si>
-    <t>Included in ASI bundle. If DIY, needs modification (machining), see  /custom-parts/galvo-assembly/15mm-galvo(Thorlabs-QS15)-mount/</t>
-  </si>
-  <si>
     <t>The part is offered by ASI as "mesoS-13 GALVO MOUNT" in the bundle. If DIY, see files in  /custom-parts/galvo-assembly/15mm-galvo(Thorlabs-QS15)-mount/</t>
   </si>
   <si>
@@ -1755,6 +1749,24 @@
   </si>
   <si>
     <t>HeatSink-sheet-H2mm</t>
+  </si>
+  <si>
+    <t>LCP33B</t>
+  </si>
+  <si>
+    <t>60 mm Cage Mounting Bracket</t>
+  </si>
+  <si>
+    <t>Bracket to attach the galvo mount to the 60 mm cage</t>
+  </si>
+  <si>
+    <t>QS15-mount-modified-Thorlabs-LCP31</t>
+  </si>
+  <si>
+    <t>Stock material for the galvo mount. Included in ASI bundle. If DIY, needs modification (machining), see  /custom-parts/galvo-assembly/15mm-galvo(Thorlabs-QS15)-mount/</t>
+  </si>
+  <si>
+    <t>Use your country code for correct plug and voltage.</t>
   </si>
 </sst>
 </file>
@@ -2520,10 +2532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J178"/>
+  <dimension ref="A1:J179"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+      <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2543,7 +2555,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="93" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E1" s="94"/>
       <c r="F1" s="94"/>
@@ -2562,10 +2574,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="70" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F2" s="70" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -2652,7 +2664,7 @@
         <v>39</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2748,7 +2760,7 @@
         <v>333</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C13" s="44" t="s">
         <v>431</v>
@@ -2767,7 +2779,7 @@
         <v>238</v>
       </c>
       <c r="I13" s="44" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2937,13 +2949,13 @@
     </row>
     <row r="20" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -2956,7 +2968,7 @@
         <v>19965</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3023,13 +3035,13 @@
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -3042,7 +3054,7 @@
         <v>6900</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3051,13 +3063,13 @@
     </row>
     <row r="26" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="51" t="s">
+        <v>472</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="51" t="s">
         <v>473</v>
-      </c>
-      <c r="B26" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="51" t="s">
-        <v>474</v>
       </c>
       <c r="D26" s="51">
         <v>4</v>
@@ -3073,7 +3085,7 @@
         <v>238</v>
       </c>
       <c r="I26" s="51" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3279,13 +3291,13 @@
     </row>
     <row r="38" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="100" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B38" s="50" t="s">
         <v>61</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D38" s="50">
         <v>1</v>
@@ -3298,10 +3310,10 @@
         <v>728</v>
       </c>
       <c r="G38" s="50" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="I38" s="50" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3399,7 +3411,7 @@
         <v>61</v>
       </c>
       <c r="C42" s="51" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D42" s="51">
         <v>2</v>
@@ -3414,7 +3426,7 @@
         <v>39</v>
       </c>
       <c r="H42" s="23" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3425,7 +3437,7 @@
         <v>323</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D43" s="3">
         <v>2</v>
@@ -3471,7 +3483,7 @@
         <v>40</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3532,7 +3544,7 @@
     </row>
     <row r="47" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B47" s="23" t="s">
         <v>61</v>
@@ -3554,7 +3566,7 @@
         <v>39</v>
       </c>
       <c r="H47" s="23" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -3581,10 +3593,10 @@
         <v>39</v>
       </c>
       <c r="H48" s="51" t="s">
+        <v>512</v>
+      </c>
+      <c r="I48" s="51" t="s">
         <v>513</v>
-      </c>
-      <c r="I48" s="51" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3611,7 +3623,7 @@
         <v>39</v>
       </c>
       <c r="H49" s="23" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3701,7 +3713,7 @@
         <v>221</v>
       </c>
       <c r="I52" s="23" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3728,7 +3740,7 @@
         <v>39</v>
       </c>
       <c r="H53" s="23" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I53" s="23" t="s">
         <v>426</v>
@@ -3758,21 +3770,21 @@
         <v>39</v>
       </c>
       <c r="H54" s="23" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B55" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D55" s="23">
         <v>2</v>
@@ -3791,18 +3803,18 @@
         <v>225</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B56" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D56" s="23">
         <v>4</v>
@@ -3821,18 +3833,18 @@
         <v>225</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B57" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D57" s="23">
         <v>4</v>
@@ -3851,7 +3863,7 @@
         <v>225</v>
       </c>
       <c r="I57" s="23" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3859,7 +3871,7 @@
         <v>91863</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>47</v>
@@ -3871,7 +3883,7 @@
         <v>400</v>
       </c>
       <c r="F58" s="78">
-        <f t="shared" ref="F58:F79" si="5">E58*D58</f>
+        <f t="shared" ref="F58:F80" si="5">E58*D58</f>
         <v>800</v>
       </c>
       <c r="G58" s="4" t="s">
@@ -3881,18 +3893,18 @@
         <v>205</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C59" s="92" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D59" s="4">
         <v>2</v>
@@ -3911,7 +3923,7 @@
         <v>225</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3941,7 +3953,7 @@
         <v>225</v>
       </c>
       <c r="I60" s="58" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="J60" s="98"/>
     </row>
@@ -3972,7 +3984,7 @@
         <v>225</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4002,18 +4014,18 @@
         <v>225</v>
       </c>
       <c r="I62" s="27" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B63" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D63" s="23">
         <v>4</v>
@@ -4029,7 +4041,7 @@
         <v>39</v>
       </c>
       <c r="H63" s="23" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I63" s="23" t="s">
         <v>211</v>
@@ -4086,7 +4098,7 @@
         <v>39</v>
       </c>
       <c r="H65" s="23" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I65" s="23" t="s">
         <v>211</v>
@@ -4094,13 +4106,13 @@
     </row>
     <row r="66" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
+        <v>520</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C66" s="24" t="s">
         <v>521</v>
-      </c>
-      <c r="B66" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C66" s="24" t="s">
-        <v>522</v>
       </c>
       <c r="D66" s="23">
         <v>2</v>
@@ -4146,12 +4158,12 @@
         <v>225</v>
       </c>
       <c r="I67" s="23" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B68" s="23" t="s">
         <v>61</v>
@@ -4176,15 +4188,15 @@
         <v>220</v>
       </c>
       <c r="I68" s="26" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="62" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B69" s="27" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C69" s="25" t="s">
         <v>299</v>
@@ -4206,7 +4218,7 @@
         <v>220</v>
       </c>
       <c r="I69" s="26" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -4241,10 +4253,10 @@
     </row>
     <row r="71" spans="1:9" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="31" t="s">
-        <v>436</v>
+        <v>553</v>
       </c>
       <c r="B71" s="27" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C71" s="31" t="s">
         <v>433</v>
@@ -4266,7 +4278,7 @@
         <v>222</v>
       </c>
       <c r="I71" s="27" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4296,28 +4308,28 @@
         <v>222</v>
       </c>
       <c r="I72" s="58" t="s">
-        <v>526</v>
+        <v>554</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
-        <v>435</v>
+        <v>550</v>
       </c>
       <c r="B73" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="D73" s="23">
         <v>2</v>
       </c>
       <c r="E73" s="81">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F73" s="82">
-        <f t="shared" ref="F73" si="7">E73*D73</f>
-        <v>72</v>
+        <f t="shared" si="5"/>
+        <v>64</v>
       </c>
       <c r="G73" s="51" t="s">
         <v>39</v>
@@ -4326,1077 +4338,1086 @@
         <v>222</v>
       </c>
       <c r="I73" s="23" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
-        <v>279</v>
+        <v>435</v>
       </c>
       <c r="B74" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>280</v>
+        <v>546</v>
       </c>
       <c r="D74" s="23">
         <v>2</v>
       </c>
       <c r="E74" s="81">
+        <v>36</v>
+      </c>
+      <c r="F74" s="82">
+        <f t="shared" ref="F74" si="7">E74*D74</f>
+        <v>72</v>
+      </c>
+      <c r="G74" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="H74" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="I74" s="23" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="24" t="s">
+        <v>279</v>
+      </c>
+      <c r="B75" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C75" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="D75" s="23">
+        <v>2</v>
+      </c>
+      <c r="E75" s="81">
         <v>2104</v>
       </c>
-      <c r="F74" s="82">
+      <c r="F75" s="82">
         <f t="shared" si="5"/>
         <v>4208</v>
       </c>
-      <c r="G74" s="3" t="s">
+      <c r="G75" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H74" s="23" t="s">
+      <c r="H75" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="I74" s="23" t="s">
+      <c r="I75" s="23" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="75" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="24" t="s">
+    <row r="76" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="B75" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C75" s="24" t="s">
+      <c r="B76" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C76" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="D75" s="23">
+      <c r="D76" s="23">
         <v>2</v>
       </c>
-      <c r="E75" s="81">
+      <c r="E76" s="81">
         <v>82</v>
       </c>
-      <c r="F75" s="82">
+      <c r="F76" s="82">
         <f t="shared" si="5"/>
         <v>164</v>
       </c>
-      <c r="G75" s="3" t="s">
+      <c r="G76" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H75" s="23" t="s">
+      <c r="H76" s="23" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="30" t="s">
+      <c r="I76" s="23" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="30" t="s">
+        <v>451</v>
+      </c>
+      <c r="B77" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C77" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B76" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C76" s="24" t="s">
-        <v>453</v>
-      </c>
-      <c r="D76" s="23">
-        <v>1</v>
-      </c>
-      <c r="E76" s="81">
+      <c r="D77" s="23">
+        <v>1</v>
+      </c>
+      <c r="E77" s="81">
         <v>520</v>
       </c>
-      <c r="F76" s="82">
+      <c r="F77" s="82">
         <f t="shared" si="5"/>
         <v>520</v>
       </c>
-      <c r="G76" s="3" t="s">
+      <c r="G77" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H76" s="23" t="s">
+      <c r="H77" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="I76" s="23" t="s">
+      <c r="I77" s="23" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="77" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="61" t="s">
+    <row r="78" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="61" t="s">
         <v>310</v>
       </c>
-      <c r="B77" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C77" s="59" t="s">
+      <c r="B78" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C78" s="59" t="s">
         <v>283</v>
       </c>
-      <c r="D77" s="58">
+      <c r="D78" s="58">
         <v>0</v>
       </c>
-      <c r="E77" s="87">
+      <c r="E78" s="87">
         <v>390</v>
       </c>
-      <c r="F77" s="88">
+      <c r="F78" s="88">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G77" s="60" t="s">
+      <c r="G78" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="H77" s="58" t="s">
+      <c r="H78" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="I77" s="58" t="s">
+      <c r="I78" s="58" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="78" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="31" t="s">
-        <v>551</v>
-      </c>
-      <c r="B78" s="27" t="s">
-        <v>455</v>
-      </c>
-      <c r="C78" s="24" t="s">
+    <row r="79" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="31" t="s">
+        <v>549</v>
+      </c>
+      <c r="B79" s="27" t="s">
+        <v>454</v>
+      </c>
+      <c r="C79" s="24" t="s">
         <v>305</v>
       </c>
-      <c r="D78" s="23">
+      <c r="D79" s="23">
         <v>14</v>
       </c>
-      <c r="E78" s="81">
+      <c r="E79" s="81">
         <v>20</v>
       </c>
-      <c r="F78" s="82">
+      <c r="F79" s="82">
         <f t="shared" si="5"/>
         <v>280</v>
       </c>
-      <c r="G78" s="3" t="s">
+      <c r="G79" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H78" s="23" t="s">
+      <c r="H79" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="I78" s="27" t="s">
+      <c r="I79" s="27" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="79" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="31" t="s">
+    <row r="80" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="B79" s="23" t="s">
+      <c r="B80" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="C79" s="24" t="s">
+      <c r="C80" s="24" t="s">
         <v>307</v>
       </c>
-      <c r="D79" s="23">
-        <v>1</v>
-      </c>
-      <c r="E79" s="81">
+      <c r="D80" s="23">
+        <v>1</v>
+      </c>
+      <c r="E80" s="81">
         <v>10</v>
       </c>
-      <c r="F79" s="82">
+      <c r="F80" s="82">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="G79" s="3" t="s">
+      <c r="G80" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H79" s="23" t="s">
+      <c r="H80" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="I79" s="23" t="s">
+      <c r="I80" s="23" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="80" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="5" t="s">
+    <row r="81" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E80" s="72"/>
-      <c r="F80" s="72"/>
-    </row>
-    <row r="81" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B81" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C81" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D81" s="23">
-        <v>1</v>
-      </c>
-      <c r="E81" s="81"/>
-      <c r="F81" s="82"/>
-      <c r="I81" s="23" t="s">
-        <v>250</v>
-      </c>
+      <c r="E81" s="72"/>
+      <c r="F81" s="72"/>
     </row>
     <row r="82" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D82" s="23">
+        <v>1</v>
+      </c>
+      <c r="E82" s="81"/>
+      <c r="F82" s="82"/>
+      <c r="I82" s="23" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="B82" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C82" s="24" t="s">
+      <c r="B83" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C83" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="D82" s="23">
-        <v>1</v>
-      </c>
-      <c r="E82" s="81">
+      <c r="D83" s="23">
+        <v>1</v>
+      </c>
+      <c r="E83" s="81">
         <v>63</v>
-      </c>
-      <c r="F82" s="82">
-        <f>D82*E82</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="B83" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C83" s="24" t="s">
-        <v>249</v>
-      </c>
-      <c r="D83" s="23">
-        <v>2</v>
-      </c>
-      <c r="E83" s="81">
-        <v>69</v>
       </c>
       <c r="F83" s="82">
         <f>D83*E83</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="B84" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C84" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="D84" s="23">
+        <v>2</v>
+      </c>
+      <c r="E84" s="81">
+        <v>69</v>
+      </c>
+      <c r="F84" s="82">
+        <f>D84*E84</f>
         <v>138</v>
       </c>
     </row>
-    <row r="84" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="23" t="s">
+    <row r="85" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B84" s="23" t="s">
+      <c r="B85" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C84" s="23" t="s">
+      <c r="C85" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D84" s="23">
-        <v>1</v>
-      </c>
-      <c r="E84" s="81"/>
-      <c r="F84" s="82"/>
-      <c r="I84" s="23" t="s">
+      <c r="D85" s="23">
+        <v>1</v>
+      </c>
+      <c r="E85" s="81"/>
+      <c r="F85" s="82"/>
+      <c r="I85" s="23" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="85" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="5" t="s">
+    <row r="86" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A86" s="5" t="s">
         <v>407</v>
-      </c>
-      <c r="E85" s="72"/>
-      <c r="F85" s="72"/>
-    </row>
-    <row r="86" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
-        <v>408</v>
       </c>
       <c r="E86" s="72"/>
       <c r="F86" s="72"/>
     </row>
-    <row r="87" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
+    <row r="87" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="E87" s="72"/>
+      <c r="F87" s="72"/>
+    </row>
+    <row r="88" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="C87" s="67" t="s">
+      <c r="C88" s="67" t="s">
         <v>409</v>
       </c>
-      <c r="D87" s="3">
-        <v>1</v>
-      </c>
-      <c r="E87" s="71">
+      <c r="D88" s="3">
+        <v>1</v>
+      </c>
+      <c r="E88" s="71">
         <v>200</v>
       </c>
-      <c r="F87" s="71">
-        <f>E87*D87</f>
+      <c r="F88" s="71">
+        <f>E88*D88</f>
         <v>200</v>
       </c>
-      <c r="I87" s="3" t="s">
+      <c r="I88" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="J87" s="4"/>
-    </row>
-    <row r="88" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="4" t="s">
-        <v>462</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>472</v>
-      </c>
-      <c r="C88" s="4" t="s">
+      <c r="J88" s="4"/>
+    </row>
+    <row r="89" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="C89" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <v>5</v>
       </c>
-      <c r="E88" s="78">
-        <v>1</v>
-      </c>
-      <c r="F88" s="78">
-        <f>E88*D88</f>
+      <c r="E89" s="78">
+        <v>1</v>
+      </c>
+      <c r="F89" s="78">
+        <f>E89*D89</f>
         <v>5</v>
       </c>
-      <c r="I88" s="4" t="s">
+      <c r="I89" s="4" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="51" t="s">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="51" t="s">
         <v>416</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C89" s="3" t="s">
+      <c r="B90" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="D89" s="3">
-        <v>1</v>
-      </c>
-      <c r="E89" s="71">
+      <c r="D90" s="3">
+        <v>1</v>
+      </c>
+      <c r="E90" s="71">
         <v>26</v>
-      </c>
-      <c r="F89" s="71">
-        <f>E89*D89</f>
-        <v>26</v>
-      </c>
-      <c r="I89" s="3" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="D90" s="3">
-        <v>1</v>
-      </c>
-      <c r="E90" s="71">
-        <v>37</v>
       </c>
       <c r="F90" s="71">
         <f>E90*D90</f>
+        <v>26</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D91" s="3">
+        <v>1</v>
+      </c>
+      <c r="E91" s="71">
         <v>37</v>
-      </c>
-      <c r="I90" s="51" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="51" t="s">
-        <v>343</v>
-      </c>
-      <c r="B91" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="C91" s="51" t="s">
-        <v>342</v>
-      </c>
-      <c r="D91" s="51">
-        <v>2</v>
-      </c>
-      <c r="E91" s="71">
-        <v>24</v>
       </c>
       <c r="F91" s="71">
         <f>E91*D91</f>
+        <v>37</v>
+      </c>
+      <c r="I91" s="51" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="51" t="s">
+        <v>343</v>
+      </c>
+      <c r="B92" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C92" s="51" t="s">
+        <v>342</v>
+      </c>
+      <c r="D92" s="51">
+        <v>2</v>
+      </c>
+      <c r="E92" s="71">
+        <v>24</v>
+      </c>
+      <c r="F92" s="71">
+        <f>E92*D92</f>
         <v>48</v>
       </c>
-      <c r="I91" s="23" t="s">
+      <c r="I92" s="23" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="92" spans="1:10" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="56" t="s">
+    <row r="93" spans="1:10" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="56" t="s">
         <v>167</v>
-      </c>
-      <c r="E92" s="89"/>
-      <c r="F92" s="89"/>
-    </row>
-    <row r="93" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="15" t="s">
-        <v>168</v>
       </c>
       <c r="E93" s="89"/>
       <c r="F93" s="89"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
+    <row r="94" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E94" s="89"/>
+      <c r="F94" s="89"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B95" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="D94" s="3">
-        <v>1</v>
-      </c>
-      <c r="E94" s="71">
+      <c r="D95" s="3">
+        <v>1</v>
+      </c>
+      <c r="E95" s="71">
         <v>625</v>
       </c>
-      <c r="F94" s="71">
-        <f>E94*D94</f>
+      <c r="F95" s="71">
+        <f>E95*D95</f>
         <v>625</v>
       </c>
-      <c r="G94" s="3" t="s">
+      <c r="G95" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I94" s="3" t="s">
+      <c r="I95" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="95" spans="1:10" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A95" s="17" t="s">
+    <row r="96" spans="1:10" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A96" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="E95" s="90"/>
-      <c r="F95" s="90"/>
-    </row>
-    <row r="96" spans="1:10" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="21" t="s">
-        <v>490</v>
-      </c>
-      <c r="B96" s="20" t="s">
-        <v>323</v>
-      </c>
-      <c r="C96" s="95" t="s">
-        <v>491</v>
-      </c>
-      <c r="D96" s="20">
-        <v>1</v>
-      </c>
-      <c r="E96" s="91">
-        <v>900</v>
-      </c>
-      <c r="F96" s="91">
-        <f t="shared" ref="F96:F102" si="8">E96*D96</f>
-        <v>900</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I96" s="20" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="22" t="s">
-        <v>494</v>
+      <c r="E96" s="90"/>
+      <c r="F96" s="90"/>
+    </row>
+    <row r="97" spans="1:9" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="21" t="s">
+        <v>489</v>
       </c>
       <c r="B97" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="C97" s="96" t="s">
-        <v>492</v>
-      </c>
-      <c r="D97" s="3">
-        <v>1</v>
-      </c>
-      <c r="E97" s="71">
+      <c r="C97" s="95" t="s">
+        <v>490</v>
+      </c>
+      <c r="D97" s="20">
+        <v>1</v>
+      </c>
+      <c r="E97" s="91">
+        <v>900</v>
+      </c>
+      <c r="F97" s="91">
+        <f t="shared" ref="F97:F103" si="8">E97*D97</f>
+        <v>900</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I97" s="20" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="22" t="s">
+        <v>493</v>
+      </c>
+      <c r="B98" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="C98" s="96" t="s">
+        <v>491</v>
+      </c>
+      <c r="D98" s="3">
+        <v>1</v>
+      </c>
+      <c r="E98" s="71">
         <v>767</v>
       </c>
-      <c r="F97" s="91">
+      <c r="F98" s="91">
         <f t="shared" si="8"/>
         <v>767</v>
       </c>
-      <c r="G97" s="3" t="s">
+      <c r="G98" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H97" s="20"/>
-      <c r="I97" s="3" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="22" t="s">
-        <v>495</v>
-      </c>
-      <c r="B98" s="20" t="s">
+      <c r="H98" s="20"/>
+      <c r="I98" s="3" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="22" t="s">
+        <v>494</v>
+      </c>
+      <c r="B99" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="C98" s="96" t="s">
-        <v>493</v>
-      </c>
-      <c r="D98" s="3">
+      <c r="C99" s="96" t="s">
+        <v>492</v>
+      </c>
+      <c r="D99" s="3">
         <v>0</v>
       </c>
-      <c r="E98" s="71">
+      <c r="E99" s="71">
         <v>1540</v>
       </c>
-      <c r="F98" s="91">
+      <c r="F99" s="91">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G98" s="3" t="s">
+      <c r="G99" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H98" s="20"/>
-      <c r="I98" s="3" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="B99" s="20" t="s">
+      <c r="H99" s="20"/>
+      <c r="I99" s="3" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="B100" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="C99" s="96" t="s">
-        <v>496</v>
-      </c>
-      <c r="D99" s="3">
-        <v>1</v>
-      </c>
-      <c r="E99" s="71">
+      <c r="C100" s="96" t="s">
+        <v>495</v>
+      </c>
+      <c r="D100" s="3">
+        <v>1</v>
+      </c>
+      <c r="E100" s="71">
         <v>877</v>
       </c>
-      <c r="F99" s="91">
+      <c r="F100" s="91">
         <f t="shared" si="8"/>
         <v>877</v>
       </c>
-      <c r="G99" s="3" t="s">
+      <c r="G100" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H99" s="20"/>
-      <c r="I99" s="3" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="51" t="s">
+      <c r="H100" s="20"/>
+      <c r="I100" s="3" t="s">
         <v>498</v>
       </c>
-      <c r="B100" s="20" t="s">
+    </row>
+    <row r="101" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="51" t="s">
+        <v>497</v>
+      </c>
+      <c r="B101" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="C100" s="96" t="s">
+      <c r="C101" s="96" t="s">
         <v>424</v>
       </c>
-      <c r="D100" s="51">
+      <c r="D101" s="51">
         <v>0</v>
       </c>
-      <c r="E100" s="71">
+      <c r="E101" s="71">
         <v>4700</v>
       </c>
-      <c r="F100" s="91">
+      <c r="F101" s="91">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G100" s="51" t="s">
+      <c r="G101" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="H100" s="20"/>
-      <c r="I100" s="51" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="51" t="s">
+      <c r="H101" s="20"/>
+      <c r="I101" s="51" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="51" t="s">
+        <v>500</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C102" s="51" t="s">
         <v>501</v>
       </c>
-      <c r="B101" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C101" s="51" t="s">
-        <v>502</v>
-      </c>
-      <c r="D101" s="51">
-        <v>1</v>
-      </c>
-      <c r="E101" s="71">
+      <c r="D102" s="51">
+        <v>1</v>
+      </c>
+      <c r="E102" s="71">
         <v>20</v>
       </c>
-      <c r="F101" s="91">
+      <c r="F102" s="91">
         <f t="shared" si="8"/>
         <v>20</v>
       </c>
-      <c r="G101" s="51" t="s">
+      <c r="G102" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="H101" s="20"/>
-      <c r="I101" s="51" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
+      <c r="H102" s="20"/>
+      <c r="I102" s="51" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C103" s="32" t="s">
         <v>503</v>
       </c>
-      <c r="B102" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C102" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="D102" s="3">
-        <v>1</v>
-      </c>
-      <c r="E102" s="71">
+      <c r="D103" s="3">
+        <v>1</v>
+      </c>
+      <c r="E103" s="71">
         <v>25</v>
       </c>
-      <c r="F102" s="91">
+      <c r="F103" s="91">
         <f t="shared" si="8"/>
         <v>25</v>
       </c>
-      <c r="G102" s="3" t="s">
+      <c r="G103" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H102" s="20"/>
-      <c r="I102" s="51" t="s">
+      <c r="H103" s="20"/>
+      <c r="I103" s="51" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A104" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="E104" s="90"/>
+      <c r="F104" s="90"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="B105" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="C105" s="68" t="s">
+        <v>355</v>
+      </c>
+      <c r="D105" s="3">
+        <v>1</v>
+      </c>
+      <c r="E105" s="71">
+        <v>752</v>
+      </c>
+      <c r="F105" s="71">
+        <f t="shared" ref="F105:F109" si="9">D105*E105</f>
+        <v>752</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B106" s="64" t="s">
+        <v>228</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="D106" s="4">
+        <v>1</v>
+      </c>
+      <c r="E106" s="78">
+        <v>1</v>
+      </c>
+      <c r="F106" s="78">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I106" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="103" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A103" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="E103" s="90"/>
-      <c r="F103" s="90"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
-        <v>510</v>
-      </c>
-      <c r="B104" s="20" t="s">
-        <v>323</v>
-      </c>
-      <c r="C104" s="68" t="s">
-        <v>355</v>
-      </c>
-      <c r="D104" s="3">
-        <v>1</v>
-      </c>
-      <c r="E104" s="71">
-        <v>752</v>
-      </c>
-      <c r="F104" s="71">
-        <f t="shared" ref="F104:F108" si="9">D104*E104</f>
-        <v>752</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I104" s="3" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="B105" s="64" t="s">
-        <v>228</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="D105" s="4">
-        <v>1</v>
-      </c>
-      <c r="E105" s="78">
-        <v>1</v>
-      </c>
-      <c r="F105" s="78">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="G105" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I105" s="4" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="B106" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C106" s="3" t="s">
+      <c r="B107" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="D106" s="3">
-        <v>1</v>
-      </c>
-      <c r="E106" s="71">
+      <c r="D107" s="3">
+        <v>1</v>
+      </c>
+      <c r="E107" s="71">
         <v>65</v>
       </c>
-      <c r="F106" s="71">
+      <c r="F107" s="71">
         <f t="shared" si="9"/>
         <v>65</v>
       </c>
-      <c r="G106" s="3" t="s">
+      <c r="G107" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I106" s="3" t="s">
+      <c r="I107" s="3" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="B107" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C107" s="3" t="s">
+      <c r="B108" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C108" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="D107" s="3">
-        <v>1</v>
-      </c>
-      <c r="E107" s="71">
+      <c r="D108" s="3">
+        <v>1</v>
+      </c>
+      <c r="E108" s="71">
         <v>32</v>
       </c>
-      <c r="F107" s="71">
+      <c r="F108" s="71">
         <f t="shared" si="9"/>
         <v>32</v>
       </c>
-      <c r="G107" s="3" t="s">
+      <c r="G108" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I107" s="3" t="s">
+      <c r="I108" s="3" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="B108" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C108" s="3" t="s">
+      <c r="B109" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="D108" s="3">
-        <v>1</v>
-      </c>
-      <c r="E108" s="71">
+      <c r="D109" s="3">
+        <v>1</v>
+      </c>
+      <c r="E109" s="71">
         <v>112</v>
       </c>
-      <c r="F108" s="71">
+      <c r="F109" s="71">
         <f t="shared" si="9"/>
         <v>112</v>
       </c>
-      <c r="G108" s="3" t="s">
+      <c r="G109" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I108" s="3" t="s">
+      <c r="I109" s="3" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="109" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A109" s="5" t="s">
+    <row r="110" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A110" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E109" s="72"/>
-      <c r="F109" s="72"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D110" s="3">
-        <v>1</v>
-      </c>
-      <c r="E110" s="71">
-        <v>3582</v>
-      </c>
-      <c r="F110" s="71">
-        <f t="shared" ref="F110:F122" si="10">E110*D110</f>
-        <v>3582</v>
-      </c>
-      <c r="G110" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I110" s="3" t="s">
-        <v>489</v>
-      </c>
+      <c r="E110" s="72"/>
+      <c r="F110" s="72"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>181</v>
+        <v>57</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C111" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D111" s="3">
+        <v>1</v>
+      </c>
+      <c r="E111" s="71">
+        <v>3582</v>
+      </c>
+      <c r="F111" s="71">
+        <f t="shared" ref="F111:F123" si="10">E111*D111</f>
+        <v>3582</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C112" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D111" s="3">
-        <v>1</v>
-      </c>
-      <c r="E111" s="71">
+      <c r="D112" s="3">
+        <v>1</v>
+      </c>
+      <c r="E112" s="71">
         <v>1630</v>
       </c>
-      <c r="F111" s="71">
+      <c r="F112" s="71">
         <f t="shared" si="10"/>
         <v>1630</v>
       </c>
-      <c r="G111" s="3" t="s">
+      <c r="G112" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I111" s="3" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
+      <c r="I112" s="3" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B113" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C113" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D112" s="3">
-        <v>1</v>
-      </c>
-      <c r="E112" s="71">
+      <c r="D113" s="3">
+        <v>1</v>
+      </c>
+      <c r="E113" s="71">
         <v>886</v>
       </c>
-      <c r="F112" s="71">
+      <c r="F113" s="71">
         <f t="shared" si="10"/>
         <v>886</v>
       </c>
-      <c r="G112" s="3" t="s">
+      <c r="G113" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I112" s="3" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
+      <c r="I113" s="3" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B114" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="C114" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D113" s="3">
-        <v>1</v>
-      </c>
-      <c r="E113" s="71">
+      <c r="D114" s="3">
+        <v>1</v>
+      </c>
+      <c r="E114" s="71">
         <v>163</v>
       </c>
-      <c r="F113" s="71">
+      <c r="F114" s="71">
         <f t="shared" si="10"/>
         <v>163</v>
       </c>
-      <c r="G113" s="3" t="s">
+      <c r="G114" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I113" s="3" t="s">
+      <c r="I114" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B115" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C115" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D114" s="3">
-        <v>1</v>
-      </c>
-      <c r="E114" s="71">
+      <c r="D115" s="3">
+        <v>1</v>
+      </c>
+      <c r="E115" s="71">
         <v>11</v>
       </c>
-      <c r="F114" s="71">
+      <c r="F115" s="71">
         <f t="shared" si="10"/>
         <v>11</v>
       </c>
-      <c r="G114" s="3" t="s">
+      <c r="G115" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B116" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C116" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D115" s="3">
-        <v>1</v>
-      </c>
-      <c r="E115" s="71">
+      <c r="D116" s="3">
+        <v>1</v>
+      </c>
+      <c r="E116" s="71">
         <v>520</v>
       </c>
-      <c r="F115" s="71">
+      <c r="F116" s="71">
         <f t="shared" si="10"/>
         <v>520</v>
       </c>
-      <c r="G115" s="3" t="s">
+      <c r="G116" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B117" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C117" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D116" s="3">
-        <v>1</v>
-      </c>
-      <c r="E116" s="71">
+      <c r="D117" s="3">
+        <v>1</v>
+      </c>
+      <c r="E117" s="71">
         <v>193</v>
       </c>
-      <c r="F116" s="71">
+      <c r="F117" s="71">
         <f t="shared" si="10"/>
         <v>193</v>
       </c>
-      <c r="G116" s="3" t="s">
+      <c r="G117" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="117" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="23" t="s">
+    <row r="118" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="B117" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C117" s="23" t="s">
+      <c r="B118" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C118" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="D117" s="23">
+      <c r="D118" s="23">
         <v>10</v>
       </c>
-      <c r="E117" s="82">
+      <c r="E118" s="82">
         <v>12</v>
       </c>
-      <c r="F117" s="82">
+      <c r="F118" s="82">
         <f t="shared" si="10"/>
         <v>120</v>
       </c>
-      <c r="G117" s="23" t="s">
+      <c r="G118" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="I117" s="23" t="s">
+      <c r="I118" s="23" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="118" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="23" t="s">
+    <row r="119" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="B118" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C118" s="23" t="s">
+      <c r="B119" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C119" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="D118" s="23">
-        <v>1</v>
-      </c>
-      <c r="E118" s="82">
+      <c r="D119" s="23">
+        <v>1</v>
+      </c>
+      <c r="E119" s="82">
         <v>14</v>
       </c>
-      <c r="F118" s="82">
+      <c r="F119" s="82">
         <f t="shared" si="10"/>
         <v>14</v>
       </c>
-      <c r="G118" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="I118" s="23" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D119" s="3">
-        <v>4</v>
-      </c>
-      <c r="E119" s="71">
-        <v>15.25</v>
-      </c>
-      <c r="F119" s="71">
-        <f t="shared" si="10"/>
-        <v>61</v>
-      </c>
       <c r="G119" s="23" t="s">
         <v>51</v>
       </c>
+      <c r="I119" s="23" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D120" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E120" s="71">
-        <v>16.5</v>
+        <v>15.25</v>
       </c>
       <c r="F120" s="71">
         <f t="shared" si="10"/>
-        <v>165</v>
+        <v>61</v>
       </c>
       <c r="G120" s="23" t="s">
         <v>51</v>
@@ -5404,23 +5425,23 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D121" s="3">
         <v>10</v>
       </c>
       <c r="E121" s="71">
-        <v>24</v>
+        <v>16.5</v>
       </c>
       <c r="F121" s="71">
         <f t="shared" si="10"/>
-        <v>240</v>
+        <v>165</v>
       </c>
       <c r="G121" s="23" t="s">
         <v>51</v>
@@ -5428,177 +5449,180 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D122" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E122" s="71">
         <v>24</v>
       </c>
       <c r="F122" s="71">
         <f t="shared" si="10"/>
-        <v>144</v>
+        <v>240</v>
       </c>
       <c r="G122" s="23" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="123" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E123" s="82"/>
-      <c r="F123" s="82"/>
-    </row>
-    <row r="125" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="10"/>
-      <c r="B125" s="10"/>
-      <c r="C125" s="9"/>
-    </row>
-    <row r="126" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="7" t="s">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D123" s="3">
+        <v>6</v>
+      </c>
+      <c r="E123" s="71">
+        <v>24</v>
+      </c>
+      <c r="F123" s="71">
+        <f t="shared" si="10"/>
+        <v>144</v>
+      </c>
+      <c r="G123" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E124" s="82"/>
+      <c r="F124" s="82"/>
+    </row>
+    <row r="126" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A126" s="10"/>
+      <c r="B126" s="10"/>
+      <c r="C126" s="9"/>
+    </row>
+    <row r="127" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A127" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E126" s="72"/>
-      <c r="F126" s="72"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D127" s="3">
-        <v>4</v>
-      </c>
-      <c r="E127" s="71">
-        <v>16.5</v>
-      </c>
-      <c r="F127" s="71">
-        <f t="shared" ref="F127:F142" si="11">E127*D127</f>
-        <v>66</v>
-      </c>
-      <c r="I127" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="E127" s="72"/>
+      <c r="F127" s="72"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D128" s="3">
+        <v>4</v>
+      </c>
+      <c r="E128" s="71">
+        <v>16.5</v>
+      </c>
+      <c r="F128" s="71">
+        <f t="shared" ref="F128:F143" si="11">E128*D128</f>
+        <v>66</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B128" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C128" s="3" t="s">
+      <c r="B129" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D128" s="3">
-        <v>1</v>
-      </c>
-      <c r="E128" s="71">
+      <c r="D129" s="3">
+        <v>1</v>
+      </c>
+      <c r="E129" s="71">
         <v>85.1</v>
       </c>
-      <c r="F128" s="71">
+      <c r="F129" s="71">
         <f t="shared" si="11"/>
         <v>85.1</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="s">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B129" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C129" s="3" t="s">
+      <c r="B130" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C130" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D129" s="3">
+      <c r="D130" s="3">
         <v>2</v>
       </c>
-      <c r="E129" s="71">
+      <c r="E130" s="71">
         <v>32</v>
       </c>
-      <c r="F129" s="71">
+      <c r="F130" s="71">
         <f t="shared" si="11"/>
         <v>64</v>
       </c>
-      <c r="I129" s="3" t="s">
+      <c r="I130" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="3" t="s">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B130" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C130" s="3" t="s">
+      <c r="B131" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C131" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D130" s="3">
+      <c r="D131" s="3">
         <v>2</v>
       </c>
-      <c r="E130" s="71">
+      <c r="E131" s="71">
         <v>51.58</v>
       </c>
-      <c r="F130" s="71">
+      <c r="F131" s="71">
         <f t="shared" si="11"/>
         <v>103.16</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B131" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C131" s="3" t="s">
+      <c r="B132" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C132" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D131" s="3">
-        <v>1</v>
-      </c>
-      <c r="E131" s="71">
+      <c r="D132" s="3">
+        <v>1</v>
+      </c>
+      <c r="E132" s="71">
         <v>60</v>
       </c>
-      <c r="F131" s="71">
+      <c r="F132" s="71">
         <f t="shared" si="11"/>
         <v>60</v>
       </c>
-      <c r="I131" s="3" t="s">
+      <c r="I132" s="3" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D132" s="3">
-        <v>1</v>
-      </c>
-      <c r="E132" s="71">
-        <v>136.47999999999999</v>
-      </c>
-      <c r="F132" s="71">
-        <f t="shared" si="11"/>
-        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -5609,7 +5633,7 @@
         <v>61</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D133" s="3">
         <v>1</v>
@@ -5624,299 +5648,299 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D134" s="3">
         <v>1</v>
       </c>
       <c r="E134" s="71">
-        <v>60.95</v>
+        <v>136.47999999999999</v>
       </c>
       <c r="F134" s="71">
         <f t="shared" si="11"/>
-        <v>60.95</v>
+        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D135" s="3">
         <v>1</v>
       </c>
       <c r="E135" s="71">
-        <v>119.416</v>
+        <v>60.95</v>
       </c>
       <c r="F135" s="71">
         <f t="shared" si="11"/>
-        <v>119.416</v>
+        <v>60.95</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D136" s="3">
         <v>1</v>
       </c>
       <c r="E136" s="71">
-        <v>105.8</v>
+        <v>119.416</v>
       </c>
       <c r="F136" s="71">
         <f t="shared" si="11"/>
-        <v>105.8</v>
+        <v>119.416</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D137" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E137" s="71">
-        <v>119.6</v>
+        <v>105.8</v>
       </c>
       <c r="F137" s="71">
         <f t="shared" si="11"/>
-        <v>239.2</v>
+        <v>105.8</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>300</v>
+        <v>146</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>301</v>
+        <v>147</v>
       </c>
       <c r="D138" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E138" s="71">
-        <v>100</v>
+        <v>119.6</v>
       </c>
       <c r="F138" s="71">
         <f t="shared" si="11"/>
-        <v>100</v>
+        <v>239.2</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>148</v>
+        <v>300</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>149</v>
+        <v>301</v>
       </c>
       <c r="D139" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E139" s="71">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F139" s="71">
         <f t="shared" si="11"/>
-        <v>184</v>
+        <v>100</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D140" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E140" s="71">
-        <v>96.23</v>
+        <v>92</v>
       </c>
       <c r="F140" s="71">
         <f t="shared" si="11"/>
-        <v>96.23</v>
+        <v>184</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D141" s="3">
         <v>1</v>
       </c>
       <c r="E141" s="71">
-        <v>102.44</v>
+        <v>96.23</v>
       </c>
       <c r="F141" s="71">
         <f t="shared" si="11"/>
-        <v>102.44</v>
+        <v>96.23</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D142" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E142" s="71">
-        <v>28</v>
+        <v>102.44</v>
       </c>
       <c r="F142" s="71">
         <f t="shared" si="11"/>
+        <v>102.44</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D143" s="3">
+        <v>2</v>
+      </c>
+      <c r="E143" s="71">
+        <v>28</v>
+      </c>
+      <c r="F143" s="71">
+        <f t="shared" si="11"/>
         <v>56</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C143" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D143" s="3">
-        <v>4</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C144" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D144" s="3">
-        <v>1</v>
-      </c>
-      <c r="I144" s="3" t="s">
-        <v>158</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C145" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D145" s="3">
+        <v>1</v>
+      </c>
+      <c r="I145" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C146" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D145" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A147" s="7" t="s">
+      <c r="D146" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A148" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B147" s="6" t="s">
+      <c r="B148" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="E147" s="72"/>
-      <c r="F147" s="72"/>
-    </row>
-    <row r="148" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="51"/>
-      <c r="B148" s="51" t="s">
-        <v>440</v>
-      </c>
-      <c r="C148" s="53" t="s">
+      <c r="E148" s="72"/>
+      <c r="F148" s="72"/>
+    </row>
+    <row r="149" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="51"/>
+      <c r="B149" s="51" t="s">
+        <v>439</v>
+      </c>
+      <c r="C149" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="D148" s="51">
+      <c r="D149" s="51">
         <v>4</v>
       </c>
-      <c r="E148" s="71">
+      <c r="E149" s="71">
         <v>40</v>
-      </c>
-      <c r="F148" s="71">
-        <f>E148*D148</f>
-        <v>160</v>
-      </c>
-      <c r="G148" s="51" t="s">
-        <v>438</v>
-      </c>
-      <c r="H148" s="51" t="s">
-        <v>439</v>
-      </c>
-      <c r="I148" s="51" t="s">
-        <v>437</v>
-      </c>
-      <c r="J148" s="53"/>
-    </row>
-    <row r="149" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="51" t="s">
-        <v>162</v>
-      </c>
-      <c r="C149" s="51" t="s">
-        <v>351</v>
-      </c>
-      <c r="D149" s="51">
-        <v>2</v>
-      </c>
-      <c r="E149" s="71">
-        <v>331</v>
       </c>
       <c r="F149" s="71">
         <f>E149*D149</f>
-        <v>662</v>
+        <v>160</v>
       </c>
       <c r="G149" s="51" t="s">
-        <v>441</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="H149" s="51" t="s">
+        <v>438</v>
+      </c>
+      <c r="I149" s="51" t="s">
+        <v>436</v>
+      </c>
+      <c r="J149" s="53"/>
     </row>
     <row r="150" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B150" s="51" t="s">
         <v>162</v>
       </c>
       <c r="C150" s="51" t="s">
-        <v>287</v>
+        <v>351</v>
       </c>
       <c r="D150" s="51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E150" s="71">
-        <v>25</v>
+        <v>331</v>
       </c>
       <c r="F150" s="71">
         <f>E150*D150</f>
-        <v>100</v>
+        <v>662</v>
       </c>
       <c r="G150" s="51" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="151" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -5924,20 +5948,20 @@
         <v>162</v>
       </c>
       <c r="C151" s="51" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D151" s="51">
         <v>4</v>
       </c>
       <c r="E151" s="71">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F151" s="71">
         <f>E151*D151</f>
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G151" s="51" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="152" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -5945,206 +5969,227 @@
         <v>162</v>
       </c>
       <c r="C152" s="51" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D152" s="51">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E152" s="71">
-        <v>121.5</v>
+        <v>28</v>
       </c>
       <c r="F152" s="71">
         <f>E152*D152</f>
+        <v>112</v>
+      </c>
+      <c r="G152" s="51" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C153" s="51" t="s">
+        <v>289</v>
+      </c>
+      <c r="D153" s="51">
+        <v>6</v>
+      </c>
+      <c r="E153" s="71">
+        <v>121.5</v>
+      </c>
+      <c r="F153" s="71">
+        <f>E153*D153</f>
         <v>729</v>
       </c>
-      <c r="G152" s="51" t="s">
+      <c r="G153" s="51" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E156" s="66" t="s">
+        <v>469</v>
+      </c>
+      <c r="F156" s="66">
+        <f>SUM(F3:F154)</f>
+        <v>95637.501499199992</v>
+      </c>
+      <c r="G156" s="3" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E158" s="71"/>
+      <c r="F158" s="71"/>
+    </row>
+    <row r="160" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A160" s="65" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A161" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B161" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E155" s="66" t="s">
-        <v>470</v>
-      </c>
-      <c r="F155" s="66">
-        <f>SUM(F3:F153)</f>
-        <v>95573.501499199992</v>
-      </c>
-      <c r="G155" s="3" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="157" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E157" s="71"/>
-      <c r="F157" s="71"/>
-    </row>
-    <row r="159" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A159" s="65" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A160" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="B160" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="C160" s="4" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
+      <c r="C161" s="4" t="s">
         <v>443</v>
-      </c>
-      <c r="B161" s="3">
-        <v>14</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B162" s="3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B163" s="3">
         <v>2</v>
       </c>
-      <c r="C163" s="51" t="s">
-        <v>457</v>
+      <c r="C163" s="3" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B164" s="3">
         <v>2</v>
       </c>
-      <c r="C164" s="3" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A167" s="65" t="s">
+      <c r="C164" s="51" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="B165" s="3">
+        <v>2</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A168" s="65" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A169" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A168" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="B168" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="C168" s="4" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" s="3" t="s">
+      <c r="B170" s="3">
+        <v>2</v>
+      </c>
+      <c r="C170" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="B169" s="3">
-        <v>2</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A170" s="3" t="s">
+    </row>
+    <row r="171" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A171" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="B170" s="3">
+      <c r="B171" s="3">
         <v>5</v>
       </c>
-      <c r="C170" s="3" t="s">
+      <c r="C171" s="3" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B172" s="3">
+        <v>1</v>
+      </c>
+      <c r="C172" s="3" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="B171" s="3">
-        <v>1</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A174" s="65" t="s">
+    <row r="175" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A175" s="65" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A176" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="C176" s="4" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="51" t="s">
+        <v>461</v>
+      </c>
+      <c r="B177" s="3">
+        <v>5</v>
+      </c>
+      <c r="C177" s="3" t="s">
         <v>463</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A175" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="B175" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="C175" s="4" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="51" t="s">
-        <v>462</v>
-      </c>
-      <c r="B176" s="3">
-        <v>5</v>
-      </c>
-      <c r="C176" s="3" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B177" s="3">
-        <v>3</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B178" s="3">
+        <v>3</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C179" s="3" t="s">
         <v>468</v>
-      </c>
-      <c r="B178" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>469</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C96" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C97" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C98" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C99" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C104" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C87" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C100" r:id="rId7" xr:uid="{3002EF90-377A-4FAD-A836-B22D0D243A96}"/>
+    <hyperlink ref="C97" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C98" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C99" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C100" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C105" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C88" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C101" r:id="rId7" xr:uid="{3002EF90-377A-4FAD-A836-B22D0D243A96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>

</xml_diff>

<commit_message>
add PCIe-8363 to the list
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0180F988-F2D5-4563-9AAD-26206043CA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65432376-D079-40AE-BDC7-D67E546D9F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16308" yWindow="4500" windowWidth="34368" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10884" yWindow="4620" windowWidth="34368" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -572,9 +572,6 @@
     <t>Power Cord, 220V, 10A (plug country-specific)</t>
   </si>
   <si>
-    <t>NI PCIe-8361, 1 Port MXI-Express Interface</t>
-  </si>
-  <si>
     <t>779504-01</t>
   </si>
   <si>
@@ -1733,9 +1730,6 @@
     <t>Chassis to mount the signal generation card.  Alternative: low-cost NI PXI-1033 from second-hand market.</t>
   </si>
   <si>
-    <t>Connects the Chassis to the PC. NI-PCIe-8361 is officially discontinued by NI. Alternative: a two-port PCIe-8362 for a higher price.</t>
-  </si>
-  <si>
     <t>Side covers of the galvo assembly</t>
   </si>
   <si>
@@ -1767,6 +1761,12 @@
   </si>
   <si>
     <t>Use your country code for correct plug and voltage.</t>
+  </si>
+  <si>
+    <t>NI PCIe-8363, 1 Port MXI-Express Interface</t>
+  </si>
+  <si>
+    <t>Connects the Chassis to the PC. Alternative: a two-port PCIe-8362,  or a discontinued PCIe-8361.</t>
   </si>
 </sst>
 </file>
@@ -2534,8 +2534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I77" sqref="I77"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E114" sqref="E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2555,7 +2555,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="93" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E1" s="94"/>
       <c r="F1" s="94"/>
@@ -2574,10 +2574,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="70" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F2" s="70" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -2617,7 +2617,7 @@
         <v>12350</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>173</v>
@@ -2664,7 +2664,7 @@
         <v>39</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2682,7 +2682,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D10" s="54">
         <v>0</v>
@@ -2695,10 +2695,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="54" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I10" s="54" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2722,10 +2722,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="54" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I11" s="44" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2749,7 +2749,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H12" s="44" t="s">
         <v>13</v>
@@ -2757,13 +2757,13 @@
     </row>
     <row r="13" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D13" s="44">
         <v>1</v>
@@ -2776,10 +2776,10 @@
         <v>160</v>
       </c>
       <c r="G13" s="54" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I13" s="44" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2803,13 +2803,13 @@
         <v>0</v>
       </c>
       <c r="G14" s="44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H14" s="44" t="s">
         <v>13</v>
       </c>
       <c r="I14" s="44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2833,10 +2833,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="54" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I15" s="44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2860,21 +2860,21 @@
         <v>0</v>
       </c>
       <c r="G16" s="54" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I16" s="44" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B17" s="44" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D17" s="44">
         <v>0</v>
@@ -2887,10 +2887,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="54" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I17" s="44" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2914,10 +2914,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="54" t="s">
+        <v>237</v>
+      </c>
+      <c r="I18" s="54" t="s">
         <v>238</v>
-      </c>
-      <c r="I18" s="54" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2941,21 +2941,21 @@
         <v>0</v>
       </c>
       <c r="G19" s="54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I19" s="54" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -2968,7 +2968,7 @@
         <v>19965</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3000,10 +3000,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="54" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I22" s="54" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -3027,21 +3027,21 @@
         <v>0</v>
       </c>
       <c r="G23" s="54" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I23" s="54" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -3054,7 +3054,7 @@
         <v>6900</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3063,13 +3063,13 @@
     </row>
     <row r="26" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="51" t="s">
+        <v>471</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="51" t="s">
         <v>472</v>
-      </c>
-      <c r="B26" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="51" t="s">
-        <v>473</v>
       </c>
       <c r="D26" s="51">
         <v>4</v>
@@ -3082,28 +3082,28 @@
         <v>108</v>
       </c>
       <c r="G26" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I26" s="51" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E27" s="72"/>
       <c r="F27" s="72"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="D28" s="3">
         <v>2</v>
@@ -3116,21 +3116,21 @@
         <v>140</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>255</v>
       </c>
       <c r="D29" s="3">
         <v>6</v>
@@ -3143,21 +3143,21 @@
         <v>216</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -3170,21 +3170,21 @@
         <v>43</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
+        <v>260</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>262</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
@@ -3197,21 +3197,21 @@
         <v>29</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="C32" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>266</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
@@ -3224,21 +3224,21 @@
         <v>195</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D33" s="3">
         <v>1</v>
@@ -3251,7 +3251,7 @@
         <v>10</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="12" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3263,7 +3263,7 @@
     </row>
     <row r="35" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E35" s="80"/>
       <c r="F35" s="80"/>
@@ -3276,7 +3276,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="71" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F36" s="71">
         <v>0</v>
@@ -3284,20 +3284,20 @@
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E37" s="72"/>
       <c r="F37" s="72"/>
     </row>
     <row r="38" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="100" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B38" s="50" t="s">
         <v>61</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D38" s="50">
         <v>1</v>
@@ -3310,10 +3310,10 @@
         <v>728</v>
       </c>
       <c r="G38" s="50" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I38" s="50" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3324,7 +3324,7 @@
         <v>61</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D39" s="23">
         <v>2</v>
@@ -3340,21 +3340,21 @@
         <v>39</v>
       </c>
       <c r="H39" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="24" t="s">
         <v>196</v>
-      </c>
-      <c r="B40" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="24" t="s">
-        <v>197</v>
       </c>
       <c r="D40" s="23">
         <v>2</v>
@@ -3370,10 +3370,10 @@
         <v>39</v>
       </c>
       <c r="H40" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="I40" s="23" t="s">
         <v>198</v>
-      </c>
-      <c r="I40" s="23" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3400,18 +3400,18 @@
         <v>39</v>
       </c>
       <c r="H41" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="51" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B42" s="51" t="s">
         <v>61</v>
       </c>
       <c r="C42" s="51" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D42" s="51">
         <v>2</v>
@@ -3426,7 +3426,7 @@
         <v>39</v>
       </c>
       <c r="H42" s="23" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3434,10 +3434,10 @@
         <v>38</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D43" s="3">
         <v>2</v>
@@ -3461,7 +3461,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>42</v>
@@ -3483,15 +3483,15 @@
         <v>40</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>45</v>
@@ -3520,7 +3520,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>44</v>
@@ -3544,13 +3544,13 @@
     </row>
     <row r="47" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B47" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D47" s="23">
         <v>2</v>
@@ -3566,7 +3566,7 @@
         <v>39</v>
       </c>
       <c r="H47" s="23" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -3593,21 +3593,21 @@
         <v>39</v>
       </c>
       <c r="H48" s="51" t="s">
+        <v>511</v>
+      </c>
+      <c r="I48" s="51" t="s">
         <v>512</v>
-      </c>
-      <c r="I48" s="51" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="24" t="s">
         <v>206</v>
-      </c>
-      <c r="B49" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C49" s="24" t="s">
-        <v>207</v>
       </c>
       <c r="D49" s="23">
         <v>2</v>
@@ -3623,18 +3623,18 @@
         <v>39</v>
       </c>
       <c r="H49" s="23" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="B50" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="24" t="s">
         <v>200</v>
-      </c>
-      <c r="B50" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>201</v>
       </c>
       <c r="D50" s="23">
         <v>4</v>
@@ -3650,21 +3650,21 @@
         <v>39</v>
       </c>
       <c r="H50" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I50" s="23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="B51" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="24" t="s">
         <v>203</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>204</v>
       </c>
       <c r="D51" s="23">
         <v>4</v>
@@ -3680,21 +3680,21 @@
         <v>39</v>
       </c>
       <c r="H51" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I51" s="23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="B52" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="24" t="s">
         <v>192</v>
-      </c>
-      <c r="B52" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>193</v>
       </c>
       <c r="D52" s="23">
         <v>8</v>
@@ -3710,10 +3710,10 @@
         <v>39</v>
       </c>
       <c r="H52" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I52" s="23" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -3724,7 +3724,7 @@
         <v>61</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D53" s="23">
         <v>4</v>
@@ -3740,21 +3740,21 @@
         <v>39</v>
       </c>
       <c r="H53" s="23" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I53" s="23" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B54" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D54" s="23">
         <v>2</v>
@@ -3770,21 +3770,21 @@
         <v>39</v>
       </c>
       <c r="H54" s="23" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
+        <v>529</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="24" t="s">
         <v>530</v>
-      </c>
-      <c r="B55" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C55" s="24" t="s">
-        <v>531</v>
       </c>
       <c r="D55" s="23">
         <v>2</v>
@@ -3800,21 +3800,21 @@
         <v>39</v>
       </c>
       <c r="H55" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
+        <v>531</v>
+      </c>
+      <c r="B56" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="24" t="s">
         <v>532</v>
-      </c>
-      <c r="B56" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C56" s="24" t="s">
-        <v>533</v>
       </c>
       <c r="D56" s="23">
         <v>4</v>
@@ -3830,21 +3830,21 @@
         <v>39</v>
       </c>
       <c r="H56" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B57" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D57" s="23">
         <v>4</v>
@@ -3860,10 +3860,10 @@
         <v>39</v>
       </c>
       <c r="H57" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I57" s="23" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3871,7 +3871,7 @@
         <v>91863</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>47</v>
@@ -3890,21 +3890,21 @@
         <v>39</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C59" s="92" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D59" s="4">
         <v>2</v>
@@ -3920,21 +3920,21 @@
         <v>39</v>
       </c>
       <c r="H59" s="27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="59" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B60" s="58" t="s">
         <v>61</v>
       </c>
       <c r="C60" s="59" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D60" s="58">
         <v>0</v>
@@ -3950,22 +3950,22 @@
         <v>39</v>
       </c>
       <c r="H60" s="58" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I60" s="58" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J60" s="98"/>
     </row>
     <row r="61" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" s="24" t="s">
         <v>226</v>
-      </c>
-      <c r="B61" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" s="24" t="s">
-        <v>227</v>
       </c>
       <c r="D61" s="23">
         <v>2</v>
@@ -3981,21 +3981,21 @@
         <v>39</v>
       </c>
       <c r="H61" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B62" s="27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C62" s="97" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D62" s="27">
         <v>2</v>
@@ -4011,21 +4011,21 @@
         <v>39</v>
       </c>
       <c r="H62" s="27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I62" s="27" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B63" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D63" s="23">
         <v>4</v>
@@ -4041,21 +4041,21 @@
         <v>39</v>
       </c>
       <c r="H63" s="23" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I63" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" s="24" t="s">
         <v>214</v>
-      </c>
-      <c r="B64" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C64" s="24" t="s">
-        <v>215</v>
       </c>
       <c r="D64" s="23">
         <v>2</v>
@@ -4071,18 +4071,18 @@
         <v>39</v>
       </c>
       <c r="H64" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C65" s="24" t="s">
         <v>212</v>
-      </c>
-      <c r="B65" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C65" s="24" t="s">
-        <v>213</v>
       </c>
       <c r="D65" s="23">
         <v>4</v>
@@ -4098,21 +4098,21 @@
         <v>39</v>
       </c>
       <c r="H65" s="23" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I65" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
+        <v>519</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C66" s="24" t="s">
         <v>520</v>
-      </c>
-      <c r="B66" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C66" s="24" t="s">
-        <v>521</v>
       </c>
       <c r="D66" s="23">
         <v>2</v>
@@ -4128,18 +4128,18 @@
         <v>39</v>
       </c>
       <c r="H66" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="B67" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67" s="24" t="s">
         <v>209</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C67" s="24" t="s">
-        <v>210</v>
       </c>
       <c r="D67" s="23">
         <v>2</v>
@@ -4155,21 +4155,21 @@
         <v>39</v>
       </c>
       <c r="H67" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I67" s="23" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B68" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D68" s="26">
         <v>2</v>
@@ -4185,21 +4185,21 @@
         <v>39</v>
       </c>
       <c r="H68" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I68" s="26" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="62" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B69" s="27" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D69" s="26">
         <v>2</v>
@@ -4215,21 +4215,21 @@
         <v>39</v>
       </c>
       <c r="H69" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I69" s="26" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="B70" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C70" s="25" t="s">
         <v>217</v>
-      </c>
-      <c r="B70" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C70" s="25" t="s">
-        <v>218</v>
       </c>
       <c r="D70" s="26">
         <v>2</v>
@@ -4245,21 +4245,21 @@
         <v>39</v>
       </c>
       <c r="H70" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I70" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="31" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B71" s="27" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D71" s="27">
         <v>2</v>
@@ -4275,21 +4275,21 @@
         <v>39</v>
       </c>
       <c r="H71" s="27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I71" s="27" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="59" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B72" s="58" t="s">
         <v>61</v>
       </c>
       <c r="C72" s="59" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D72" s="58">
         <v>0</v>
@@ -4305,21 +4305,21 @@
         <v>39</v>
       </c>
       <c r="H72" s="58" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I72" s="58" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B73" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D73" s="23">
         <v>2</v>
@@ -4335,21 +4335,21 @@
         <v>39</v>
       </c>
       <c r="H73" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I73" s="23" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B74" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D74" s="23">
         <v>2</v>
@@ -4365,21 +4365,21 @@
         <v>39</v>
       </c>
       <c r="H74" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I74" s="23" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="B75" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C75" s="24" t="s">
         <v>279</v>
-      </c>
-      <c r="B75" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C75" s="24" t="s">
-        <v>280</v>
       </c>
       <c r="D75" s="23">
         <v>2</v>
@@ -4395,21 +4395,21 @@
         <v>39</v>
       </c>
       <c r="H75" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I75" s="23" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="B76" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C76" s="24" t="s">
         <v>281</v>
-      </c>
-      <c r="B76" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C76" s="24" t="s">
-        <v>282</v>
       </c>
       <c r="D76" s="23">
         <v>2</v>
@@ -4425,21 +4425,21 @@
         <v>39</v>
       </c>
       <c r="H76" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I76" s="23" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="30" t="s">
+        <v>450</v>
+      </c>
+      <c r="B77" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C77" s="24" t="s">
         <v>451</v>
-      </c>
-      <c r="B77" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C77" s="24" t="s">
-        <v>452</v>
       </c>
       <c r="D77" s="23">
         <v>1</v>
@@ -4455,21 +4455,21 @@
         <v>39</v>
       </c>
       <c r="H77" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I77" s="23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="58" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="61" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B78" s="58" t="s">
         <v>61</v>
       </c>
       <c r="C78" s="59" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D78" s="58">
         <v>0</v>
@@ -4485,21 +4485,21 @@
         <v>39</v>
       </c>
       <c r="H78" s="58" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I78" s="58" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="31" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D79" s="23">
         <v>14</v>
@@ -4515,21 +4515,21 @@
         <v>39</v>
       </c>
       <c r="H79" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I79" s="27" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="80" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="31" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C80" s="24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D80" s="23">
         <v>1</v>
@@ -4545,15 +4545,15 @@
         <v>39</v>
       </c>
       <c r="H80" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I80" s="23" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="81" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E81" s="72"/>
       <c r="F81" s="72"/>
@@ -4574,18 +4574,18 @@
       <c r="E82" s="81"/>
       <c r="F82" s="82"/>
       <c r="I82" s="23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="B83" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C83" s="24" t="s">
         <v>243</v>
-      </c>
-      <c r="B83" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C83" s="24" t="s">
-        <v>244</v>
       </c>
       <c r="D83" s="23">
         <v>1</v>
@@ -4600,13 +4600,13 @@
     </row>
     <row r="84" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="B84" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C84" s="24" t="s">
         <v>248</v>
-      </c>
-      <c r="B84" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C84" s="24" t="s">
-        <v>249</v>
       </c>
       <c r="D84" s="23">
         <v>2</v>
@@ -4635,32 +4635,32 @@
       <c r="E85" s="81"/>
       <c r="F85" s="82"/>
       <c r="I85" s="23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="86" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E86" s="72"/>
       <c r="F86" s="72"/>
     </row>
     <row r="87" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E87" s="72"/>
       <c r="F87" s="72"/>
     </row>
     <row r="88" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="B88" s="3" t="s">
-        <v>412</v>
-      </c>
       <c r="C88" s="67" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D88" s="3">
         <v>1</v>
@@ -4673,19 +4673,19 @@
         <v>200</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J88" s="4"/>
     </row>
     <row r="89" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D89" s="4">
         <v>5</v>
@@ -4698,18 +4698,18 @@
         <v>5</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="51" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D90" s="3">
         <v>1</v>
@@ -4722,18 +4722,18 @@
         <v>26</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>418</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>419</v>
       </c>
       <c r="D91" s="3">
         <v>1</v>
@@ -4746,18 +4746,18 @@
         <v>37</v>
       </c>
       <c r="I91" s="51" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="92" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="51" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B92" s="51" t="s">
         <v>61</v>
       </c>
       <c r="C92" s="51" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D92" s="51">
         <v>2</v>
@@ -4770,7 +4770,7 @@
         <v>48</v>
       </c>
       <c r="I92" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="93" spans="1:10" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4789,13 +4789,13 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D95" s="3">
         <v>1</v>
@@ -4816,20 +4816,20 @@
     </row>
     <row r="96" spans="1:10" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A96" s="17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E96" s="90"/>
       <c r="F96" s="90"/>
     </row>
     <row r="97" spans="1:9" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="21" t="s">
+        <v>488</v>
+      </c>
+      <c r="B97" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="C97" s="95" t="s">
         <v>489</v>
-      </c>
-      <c r="B97" s="20" t="s">
-        <v>323</v>
-      </c>
-      <c r="C97" s="95" t="s">
-        <v>490</v>
       </c>
       <c r="D97" s="20">
         <v>1</v>
@@ -4845,18 +4845,18 @@
         <v>13</v>
       </c>
       <c r="I97" s="20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="22" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B98" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C98" s="96" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D98" s="3">
         <v>1</v>
@@ -4873,18 +4873,18 @@
       </c>
       <c r="H98" s="20"/>
       <c r="I98" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="22" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B99" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C99" s="96" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D99" s="3">
         <v>0</v>
@@ -4901,18 +4901,18 @@
       </c>
       <c r="H99" s="20"/>
       <c r="I99" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B100" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C100" s="96" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D100" s="3">
         <v>1</v>
@@ -4929,18 +4929,18 @@
       </c>
       <c r="H100" s="20"/>
       <c r="I100" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="51" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B101" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C101" s="96" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D101" s="51">
         <v>0</v>
@@ -4957,18 +4957,18 @@
       </c>
       <c r="H101" s="20"/>
       <c r="I101" s="51" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="51" t="s">
+        <v>499</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C102" s="51" t="s">
         <v>500</v>
-      </c>
-      <c r="B102" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C102" s="51" t="s">
-        <v>501</v>
       </c>
       <c r="D102" s="51">
         <v>1</v>
@@ -4985,18 +4985,18 @@
       </c>
       <c r="H102" s="20"/>
       <c r="I102" s="51" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C103" s="32" t="s">
         <v>502</v>
-      </c>
-      <c r="B103" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C103" s="32" t="s">
-        <v>503</v>
       </c>
       <c r="D103" s="3">
         <v>1</v>
@@ -5013,25 +5013,25 @@
       </c>
       <c r="H103" s="20"/>
       <c r="I103" s="51" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A104" s="17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E104" s="90"/>
       <c r="F104" s="90"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B105" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C105" s="68" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D105" s="3">
         <v>1</v>
@@ -5047,18 +5047,18 @@
         <v>13</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B106" s="64" t="s">
+        <v>227</v>
+      </c>
+      <c r="C106" s="4" t="s">
         <v>357</v>
-      </c>
-      <c r="B106" s="64" t="s">
-        <v>228</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>358</v>
       </c>
       <c r="D106" s="4">
         <v>1</v>
@@ -5074,18 +5074,18 @@
         <v>13</v>
       </c>
       <c r="I106" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B107" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>359</v>
-      </c>
-      <c r="B107" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>360</v>
       </c>
       <c r="D107" s="3">
         <v>1</v>
@@ -5101,18 +5101,18 @@
         <v>13</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B108" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C108" s="3" t="s">
         <v>362</v>
-      </c>
-      <c r="B108" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>363</v>
       </c>
       <c r="D108" s="3">
         <v>1</v>
@@ -5128,18 +5128,18 @@
         <v>13</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>346</v>
-      </c>
-      <c r="B109" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>347</v>
       </c>
       <c r="D109" s="3">
         <v>1</v>
@@ -5155,7 +5155,7 @@
         <v>13</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5189,18 +5189,18 @@
         <v>51</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D112" s="3">
         <v>1</v>
@@ -5216,45 +5216,45 @@
         <v>51</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>179</v>
+        <v>554</v>
       </c>
       <c r="D113" s="3">
         <v>1</v>
       </c>
       <c r="E113" s="71">
-        <v>886</v>
+        <v>900</v>
       </c>
       <c r="F113" s="71">
         <f t="shared" si="10"/>
-        <v>886</v>
+        <v>900</v>
       </c>
       <c r="G113" s="3" t="s">
         <v>51</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>544</v>
+        <v>555</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D114" s="3">
         <v>1</v>
@@ -5270,7 +5270,7 @@
         <v>51</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -5323,13 +5323,13 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D117" s="3">
         <v>1</v>
@@ -5347,13 +5347,13 @@
     </row>
     <row r="118" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="B118" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C118" s="23" t="s">
         <v>291</v>
-      </c>
-      <c r="B118" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C118" s="23" t="s">
-        <v>292</v>
       </c>
       <c r="D118" s="23">
         <v>10</v>
@@ -5369,18 +5369,18 @@
         <v>51</v>
       </c>
       <c r="I118" s="23" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="119" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="B119" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C119" s="23" t="s">
         <v>293</v>
-      </c>
-      <c r="B119" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C119" s="23" t="s">
-        <v>294</v>
       </c>
       <c r="D119" s="23">
         <v>1</v>
@@ -5396,7 +5396,7 @@
         <v>51</v>
       </c>
       <c r="I119" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -5753,13 +5753,13 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C139" s="3" t="s">
         <v>300</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>301</v>
       </c>
       <c r="D139" s="3">
         <v>1</v>
@@ -5888,7 +5888,7 @@
         <v>161</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E148" s="72"/>
       <c r="F148" s="72"/>
@@ -5896,7 +5896,7 @@
     <row r="149" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="51"/>
       <c r="B149" s="51" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C149" s="53" t="s">
         <v>160</v>
@@ -5912,13 +5912,13 @@
         <v>160</v>
       </c>
       <c r="G149" s="51" t="s">
+        <v>436</v>
+      </c>
+      <c r="H149" s="51" t="s">
         <v>437</v>
       </c>
-      <c r="H149" s="51" t="s">
-        <v>438</v>
-      </c>
       <c r="I149" s="51" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J149" s="53"/>
     </row>
@@ -5927,7 +5927,7 @@
         <v>162</v>
       </c>
       <c r="C150" s="51" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D150" s="51">
         <v>2</v>
@@ -5940,7 +5940,7 @@
         <v>662</v>
       </c>
       <c r="G150" s="51" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="151" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -5948,7 +5948,7 @@
         <v>162</v>
       </c>
       <c r="C151" s="51" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D151" s="51">
         <v>4</v>
@@ -5961,7 +5961,7 @@
         <v>100</v>
       </c>
       <c r="G151" s="51" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="152" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -5969,7 +5969,7 @@
         <v>162</v>
       </c>
       <c r="C152" s="51" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D152" s="51">
         <v>4</v>
@@ -5982,7 +5982,7 @@
         <v>112</v>
       </c>
       <c r="G152" s="51" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="153" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -5990,7 +5990,7 @@
         <v>162</v>
       </c>
       <c r="C153" s="51" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D153" s="51">
         <v>6</v>
@@ -6003,19 +6003,19 @@
         <v>729</v>
       </c>
       <c r="G153" s="51" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="156" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E156" s="66" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F156" s="66">
         <f>SUM(F3:F154)</f>
-        <v>95637.501499199992</v>
+        <v>95651.501499199992</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="158" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -6024,138 +6024,138 @@
     </row>
     <row r="160" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A160" s="65" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A161" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B162" s="3">
         <v>14</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B163" s="3">
         <v>2</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B164" s="3">
         <v>2</v>
       </c>
       <c r="C164" s="51" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B165" s="3">
         <v>2</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A168" s="65" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B170" s="3">
         <v>2</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B171" s="3">
         <v>5</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B172" s="3">
         <v>1</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A175" s="65" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="51" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B177" s="3">
         <v>5</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -6166,18 +6166,18 @@
         <v>3</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C179" s="3" t="s">
         <v>467</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="C179" s="3" t="s">
-        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -6272,7 +6272,7 @@
         <v>7400</v>
       </c>
       <c r="I3" s="44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6293,15 +6293,15 @@
         <v>20000</v>
       </c>
       <c r="I4" s="44" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" s="33" t="s">
         <v>386</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>387</v>
       </c>
       <c r="D5" s="33">
         <v>1</v>
@@ -6313,13 +6313,13 @@
         <v>50000</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -6342,27 +6342,27 @@
         <v>25000</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:9" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D12" s="33">
         <v>1</v>
@@ -6378,21 +6378,21 @@
         <v>13</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D13" s="33">
         <v>1</v>
@@ -6408,21 +6408,21 @@
         <v>13</v>
       </c>
       <c r="H13" s="33" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I13" s="33" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>61</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D14" s="33">
         <v>1</v>
@@ -6438,21 +6438,21 @@
         <v>13</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I14" s="33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>61</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D15" s="33">
         <v>1</v>
@@ -6468,21 +6468,21 @@
         <v>13</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I15" s="33" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
+        <v>245</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="C16" s="37" t="s">
         <v>246</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>245</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>247</v>
       </c>
       <c r="D16" s="34">
         <v>1</v>
@@ -6498,32 +6498,32 @@
         <v>13</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I16" s="34" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:10" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="51" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C19" s="51" t="s">
         <v>14</v>
@@ -6548,13 +6548,13 @@
     </row>
     <row r="20" spans="1:10" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="51" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D20" s="51">
         <v>1</v>
@@ -6576,13 +6576,13 @@
     </row>
     <row r="21" spans="1:10" s="51" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D21" s="51">
         <v>1</v>
@@ -6603,13 +6603,13 @@
     </row>
     <row r="22" spans="1:10" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="51" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D22" s="51">
         <v>1</v>
@@ -6617,32 +6617,32 @@
       <c r="E22" s="52"/>
       <c r="F22" s="52"/>
       <c r="I22" s="23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" s="42" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
     </row>
     <row r="26" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
+        <v>311</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="C26" s="37" t="s">
         <v>312</v>
-      </c>
-      <c r="B26" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>313</v>
       </c>
       <c r="D26" s="34">
         <v>2</v>
@@ -6658,21 +6658,21 @@
         <v>39</v>
       </c>
       <c r="H26" s="34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I26" s="34" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D27" s="34">
         <v>2</v>
@@ -6688,21 +6688,21 @@
         <v>39</v>
       </c>
       <c r="H27" s="34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I27" s="34" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B28" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="C28" s="37" t="s">
         <v>325</v>
-      </c>
-      <c r="C28" s="37" t="s">
-        <v>326</v>
       </c>
       <c r="D28" s="34">
         <v>8</v>
@@ -6718,21 +6718,21 @@
         <v>39</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I28" s="34" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B29" s="34" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D29" s="34">
         <v>6</v>
@@ -6748,18 +6748,18 @@
         <v>39</v>
       </c>
       <c r="H29" s="34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
+        <v>329</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="C30" s="37" t="s">
         <v>330</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="C30" s="37" t="s">
-        <v>331</v>
       </c>
       <c r="D30" s="34">
         <v>2</v>
@@ -6775,21 +6775,21 @@
         <v>39</v>
       </c>
       <c r="H30" s="34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I30" s="34" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D31" s="34">
         <v>1</v>
@@ -6805,21 +6805,21 @@
         <v>39</v>
       </c>
       <c r="H31" s="34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I31" s="34" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D32" s="34">
         <v>1</v>
@@ -6835,21 +6835,21 @@
         <v>39</v>
       </c>
       <c r="H32" s="34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I32" s="34" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="34" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="37" t="s">
         <v>223</v>
-      </c>
-      <c r="B33" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>224</v>
       </c>
       <c r="D33" s="34">
         <v>2</v>
@@ -6865,7 +6865,7 @@
         <v>39</v>
       </c>
       <c r="H33" s="34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -6899,7 +6899,7 @@
         <v>51</v>
       </c>
       <c r="I38" s="44" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -7401,7 +7401,7 @@
     </row>
     <row r="66" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F66" s="8"/>
     </row>
@@ -7426,18 +7426,18 @@
         <v>280</v>
       </c>
       <c r="I67" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>372</v>
+      </c>
+      <c r="B68" s="47" t="s">
         <v>373</v>
       </c>
-      <c r="B68" s="47" t="s">
+      <c r="C68" s="47" t="s">
         <v>374</v>
-      </c>
-      <c r="C68" s="47" t="s">
-        <v>375</v>
       </c>
       <c r="D68" s="47">
         <v>2</v>
@@ -7450,18 +7450,18 @@
         <v>168</v>
       </c>
       <c r="I68" s="47" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B69" s="47" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C69" s="47" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D69" s="47">
         <v>1</v>
@@ -7474,18 +7474,18 @@
         <v>54</v>
       </c>
       <c r="I69" s="47" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F71" s="8"/>
     </row>
     <row r="72" spans="1:10" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C72" s="49"/>
       <c r="E72" s="36"/>
@@ -7494,7 +7494,7 @@
     </row>
     <row r="73" spans="1:10" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C73" s="49"/>
       <c r="E73" s="36"/>
@@ -7512,20 +7512,20 @@
         <v>161</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
     </row>
     <row r="76" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="54" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B76" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C76" s="54" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D76" s="54">
         <v>1</v>
@@ -7543,13 +7543,13 @@
     </row>
     <row r="77" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="54" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B77" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C77" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D77" s="54">
         <v>1</v>
@@ -7564,13 +7564,13 @@
     </row>
     <row r="78" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="54" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B78" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C78" s="54" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D78" s="54">
         <v>1</v>
@@ -7588,13 +7588,13 @@
     </row>
     <row r="79" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="54" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B79" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C79" s="54" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D79" s="54">
         <v>1</v>
@@ -7609,13 +7609,13 @@
     </row>
     <row r="80" spans="1:10" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="54" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B80" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C80" s="54" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D80" s="54">
         <v>1</v>
@@ -7630,13 +7630,13 @@
     </row>
     <row r="81" spans="1:6" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="54" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B81" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C81" s="54" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D81" s="54">
         <v>1</v>
@@ -7651,13 +7651,13 @@
     </row>
     <row r="82" spans="1:6" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="54" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B82" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C82" s="54" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D82" s="54">
         <v>1</v>
@@ -7672,13 +7672,13 @@
     </row>
     <row r="83" spans="1:6" s="54" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="54" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B83" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C83" s="54" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D83" s="54">
         <v>1</v>

</xml_diff>

<commit_message>
add CBLS3P - Command and Power Cables for QS15/20 Scanning Galvanometer Systems and GPS011 Series Power Supply
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265063D6-FBB1-4484-9F44-013EDDEAD329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4EC0AC-3312-4407-BF78-0C2DC9F94E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="4704" windowWidth="34368" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7788" yWindow="3552" windowWidth="30120" windowHeight="17568" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="566">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -1788,6 +1788,15 @@
   </si>
   <si>
     <t>A 2-piece mount for SM2 tubes</t>
+  </si>
+  <si>
+    <t>CBLS3P</t>
+  </si>
+  <si>
+    <t>CBLS3P - Command and Power Cables for QS15/20 Scanning Galvanometer Systems and GPS011 Series Power Supply</t>
+  </si>
+  <si>
+    <t>Kit cables with correct connectors for the GPS011 power supply</t>
   </si>
 </sst>
 </file>
@@ -2054,7 +2063,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -2166,6 +2175,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Excel Built-in Heading 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2553,10 +2563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J182"/>
+  <dimension ref="A1:J183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3904,7 +3914,7 @@
         <v>400</v>
       </c>
       <c r="F58" s="78">
-        <f t="shared" ref="F58:F80" si="5">E58*D58</f>
+        <f t="shared" ref="F58:F81" si="5">E58*D58</f>
         <v>800</v>
       </c>
       <c r="G58" s="4" t="s">
@@ -4512,433 +4522,435 @@
         <v>303</v>
       </c>
     </row>
-    <row r="79" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="31" t="s">
+    <row r="79" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="30" t="s">
+        <v>563</v>
+      </c>
+      <c r="B79" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C79" s="30" t="s">
+        <v>564</v>
+      </c>
+      <c r="D79" s="20">
+        <v>2</v>
+      </c>
+      <c r="E79" s="101">
+        <v>148</v>
+      </c>
+      <c r="F79" s="91">
+        <f t="shared" si="5"/>
+        <v>296</v>
+      </c>
+      <c r="G79" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="H79" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="I79" s="20" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="31" t="s">
         <v>547</v>
       </c>
-      <c r="B79" s="27" t="s">
+      <c r="B80" s="27" t="s">
         <v>453</v>
       </c>
-      <c r="C79" s="24" t="s">
+      <c r="C80" s="24" t="s">
         <v>304</v>
       </c>
-      <c r="D79" s="23">
+      <c r="D80" s="23">
         <v>14</v>
       </c>
-      <c r="E79" s="81">
+      <c r="E80" s="81">
         <v>20</v>
       </c>
-      <c r="F79" s="82">
+      <c r="F80" s="82">
         <f t="shared" si="5"/>
         <v>280</v>
       </c>
-      <c r="G79" s="3" t="s">
+      <c r="G80" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H79" s="23" t="s">
+      <c r="H80" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="I79" s="27" t="s">
+      <c r="I80" s="27" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="80" spans="1:9" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="31" t="s">
+    <row r="81" spans="1:10" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="31" t="s">
         <v>307</v>
       </c>
-      <c r="B80" s="23" t="s">
+      <c r="B81" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="C80" s="24" t="s">
+      <c r="C81" s="24" t="s">
         <v>306</v>
       </c>
-      <c r="D80" s="23">
-        <v>1</v>
-      </c>
-      <c r="E80" s="81">
+      <c r="D81" s="23">
+        <v>1</v>
+      </c>
+      <c r="E81" s="81">
         <v>10</v>
       </c>
-      <c r="F80" s="82">
+      <c r="F81" s="82">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="G80" s="3" t="s">
+      <c r="G81" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H80" s="23" t="s">
+      <c r="H81" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="I80" s="23" t="s">
+      <c r="I81" s="23" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="5" t="s">
+    <row r="82" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A82" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="E81" s="72"/>
-      <c r="F81" s="72"/>
-    </row>
-    <row r="82" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B82" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C82" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D82" s="23">
-        <v>1</v>
-      </c>
-      <c r="E82" s="81"/>
-      <c r="F82" s="82"/>
-      <c r="I82" s="23" t="s">
-        <v>249</v>
-      </c>
+      <c r="E82" s="72"/>
+      <c r="F82" s="72"/>
     </row>
     <row r="83" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B83" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D83" s="23">
+        <v>1</v>
+      </c>
+      <c r="E83" s="81"/>
+      <c r="F83" s="82"/>
+      <c r="I83" s="23" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="B83" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C83" s="24" t="s">
+      <c r="B84" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C84" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="D83" s="23">
-        <v>1</v>
-      </c>
-      <c r="E83" s="81">
+      <c r="D84" s="23">
+        <v>1</v>
+      </c>
+      <c r="E84" s="81">
         <v>63</v>
-      </c>
-      <c r="F83" s="82">
-        <f>D83*E83</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="B84" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C84" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="D84" s="23">
-        <v>2</v>
-      </c>
-      <c r="E84" s="81">
-        <v>69</v>
       </c>
       <c r="F84" s="82">
         <f>D84*E84</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="B85" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C85" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="D85" s="23">
+        <v>2</v>
+      </c>
+      <c r="E85" s="81">
+        <v>69</v>
+      </c>
+      <c r="F85" s="82">
+        <f>D85*E85</f>
         <v>138</v>
       </c>
     </row>
-    <row r="85" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="23" t="s">
+    <row r="86" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B85" s="23" t="s">
+      <c r="B86" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C85" s="23" t="s">
+      <c r="C86" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D85" s="23">
-        <v>1</v>
-      </c>
-      <c r="E85" s="81"/>
-      <c r="F85" s="82"/>
-      <c r="I85" s="23" t="s">
+      <c r="D86" s="23">
+        <v>1</v>
+      </c>
+      <c r="E86" s="81"/>
+      <c r="F86" s="82"/>
+      <c r="I86" s="23" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="86" spans="1:10" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="27" t="s">
+    <row r="87" spans="1:10" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="27" t="s">
         <v>558</v>
       </c>
-      <c r="B86" s="27" t="s">
+      <c r="B87" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="C86" s="27" t="s">
+      <c r="C87" s="27" t="s">
         <v>559</v>
       </c>
-      <c r="D86" s="27">
-        <v>1</v>
-      </c>
-      <c r="E86" s="83">
-        <v>1</v>
-      </c>
-      <c r="F86" s="84">
-        <v>1</v>
-      </c>
-      <c r="I86" s="4" t="s">
+      <c r="D87" s="27">
+        <v>1</v>
+      </c>
+      <c r="E87" s="83">
+        <v>1</v>
+      </c>
+      <c r="F87" s="84">
+        <v>1</v>
+      </c>
+      <c r="I87" s="4" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="87" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="5" t="s">
+    <row r="88" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A88" s="5" t="s">
         <v>406</v>
-      </c>
-      <c r="E87" s="72"/>
-      <c r="F87" s="72"/>
-    </row>
-    <row r="88" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
-        <v>407</v>
       </c>
       <c r="E88" s="72"/>
       <c r="F88" s="72"/>
     </row>
-    <row r="89" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="3" t="s">
+    <row r="89" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="E89" s="72"/>
+      <c r="F89" s="72"/>
+    </row>
+    <row r="90" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="C89" s="67" t="s">
+      <c r="C90" s="67" t="s">
         <v>408</v>
       </c>
-      <c r="D89" s="3">
-        <v>1</v>
-      </c>
-      <c r="E89" s="71">
+      <c r="D90" s="3">
+        <v>1</v>
+      </c>
+      <c r="E90" s="71">
         <v>200</v>
       </c>
-      <c r="F89" s="71">
-        <f>E89*D89</f>
+      <c r="F90" s="71">
+        <f>E90*D90</f>
         <v>200</v>
       </c>
-      <c r="I89" s="3" t="s">
+      <c r="I90" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="J89" s="4"/>
-    </row>
-    <row r="90" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="4" t="s">
+      <c r="J90" s="4"/>
+    </row>
+    <row r="91" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>470</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C91" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D91" s="4">
         <v>5</v>
       </c>
-      <c r="E90" s="78">
-        <v>1</v>
-      </c>
-      <c r="F90" s="78">
-        <f>E90*D90</f>
+      <c r="E91" s="78">
+        <v>1</v>
+      </c>
+      <c r="F91" s="78">
+        <f>E91*D91</f>
         <v>5</v>
       </c>
-      <c r="I90" s="4" t="s">
+      <c r="I91" s="4" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="51" t="s">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="51" t="s">
         <v>415</v>
       </c>
-      <c r="B91" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C91" s="3" t="s">
+      <c r="B92" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C92" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="D91" s="3">
-        <v>1</v>
-      </c>
-      <c r="E91" s="71">
+      <c r="D92" s="3">
+        <v>1</v>
+      </c>
+      <c r="E92" s="71">
         <v>26</v>
-      </c>
-      <c r="F91" s="71">
-        <f>E91*D91</f>
-        <v>26</v>
-      </c>
-      <c r="I91" s="3" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="D92" s="3">
-        <v>1</v>
-      </c>
-      <c r="E92" s="71">
-        <v>37</v>
       </c>
       <c r="F92" s="71">
         <f>E92*D92</f>
+        <v>26</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D93" s="3">
+        <v>1</v>
+      </c>
+      <c r="E93" s="71">
         <v>37</v>
-      </c>
-      <c r="I92" s="51" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="51" t="s">
-        <v>342</v>
-      </c>
-      <c r="B93" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="C93" s="51" t="s">
-        <v>341</v>
-      </c>
-      <c r="D93" s="51">
-        <v>2</v>
-      </c>
-      <c r="E93" s="71">
-        <v>24</v>
       </c>
       <c r="F93" s="71">
         <f>E93*D93</f>
+        <v>37</v>
+      </c>
+      <c r="I93" s="51" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="51" t="s">
+        <v>342</v>
+      </c>
+      <c r="B94" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C94" s="51" t="s">
+        <v>341</v>
+      </c>
+      <c r="D94" s="51">
+        <v>2</v>
+      </c>
+      <c r="E94" s="71">
+        <v>24</v>
+      </c>
+      <c r="F94" s="71">
+        <f>E94*D94</f>
         <v>48</v>
       </c>
-      <c r="I93" s="23" t="s">
+      <c r="I94" s="23" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="94" spans="1:10" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="56" t="s">
+    <row r="95" spans="1:10" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="56" t="s">
         <v>167</v>
-      </c>
-      <c r="E94" s="89"/>
-      <c r="F94" s="89"/>
-    </row>
-    <row r="95" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="15" t="s">
-        <v>168</v>
       </c>
       <c r="E95" s="89"/>
       <c r="F95" s="89"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
+    <row r="96" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E96" s="89"/>
+      <c r="F96" s="89"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B97" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="D96" s="3">
-        <v>1</v>
-      </c>
-      <c r="E96" s="71">
+      <c r="D97" s="3">
+        <v>1</v>
+      </c>
+      <c r="E97" s="71">
         <v>625</v>
       </c>
-      <c r="F96" s="71">
-        <f>E96*D96</f>
+      <c r="F97" s="71">
+        <f>E97*D97</f>
         <v>625</v>
       </c>
-      <c r="G96" s="3" t="s">
+      <c r="G97" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I96" s="3" t="s">
+      <c r="I97" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="97" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A97" s="17" t="s">
+    <row r="98" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A98" s="17" t="s">
         <v>351</v>
       </c>
-      <c r="E97" s="90"/>
-      <c r="F97" s="90"/>
-    </row>
-    <row r="98" spans="1:9" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="21" t="s">
+      <c r="E98" s="90"/>
+      <c r="F98" s="90"/>
+    </row>
+    <row r="99" spans="1:9" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="21" t="s">
         <v>488</v>
-      </c>
-      <c r="B98" s="20" t="s">
-        <v>322</v>
-      </c>
-      <c r="C98" s="95" t="s">
-        <v>489</v>
-      </c>
-      <c r="D98" s="20">
-        <v>1</v>
-      </c>
-      <c r="E98" s="91">
-        <v>900</v>
-      </c>
-      <c r="F98" s="91">
-        <f t="shared" ref="F98:F104" si="8">E98*D98</f>
-        <v>900</v>
-      </c>
-      <c r="G98" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I98" s="20" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="22" t="s">
-        <v>492</v>
       </c>
       <c r="B99" s="20" t="s">
         <v>322</v>
       </c>
-      <c r="C99" s="96" t="s">
+      <c r="C99" s="95" t="s">
+        <v>489</v>
+      </c>
+      <c r="D99" s="20">
+        <v>1</v>
+      </c>
+      <c r="E99" s="91">
+        <v>900</v>
+      </c>
+      <c r="F99" s="91">
+        <f t="shared" ref="F99:F105" si="8">E99*D99</f>
+        <v>900</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I99" s="20" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="22" t="s">
+        <v>492</v>
+      </c>
+      <c r="B100" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="C100" s="96" t="s">
         <v>490</v>
       </c>
-      <c r="D99" s="3">
-        <v>1</v>
-      </c>
-      <c r="E99" s="71">
+      <c r="D100" s="3">
+        <v>1</v>
+      </c>
+      <c r="E100" s="71">
         <v>767</v>
       </c>
-      <c r="F99" s="91">
+      <c r="F100" s="91">
         <f t="shared" si="8"/>
         <v>767</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H99" s="20"/>
-      <c r="I99" s="3" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="22" t="s">
-        <v>493</v>
-      </c>
-      <c r="B100" s="20" t="s">
-        <v>322</v>
-      </c>
-      <c r="C100" s="96" t="s">
-        <v>491</v>
-      </c>
-      <c r="D100" s="3">
-        <v>0</v>
-      </c>
-      <c r="E100" s="71">
-        <v>1540</v>
-      </c>
-      <c r="F100" s="91">
-        <f t="shared" si="8"/>
-        <v>0</v>
       </c>
       <c r="G100" s="3" t="s">
         <v>13</v>
@@ -4949,24 +4961,24 @@
       </c>
     </row>
     <row r="101" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A101" s="3" t="s">
-        <v>495</v>
+      <c r="A101" s="22" t="s">
+        <v>493</v>
       </c>
       <c r="B101" s="20" t="s">
         <v>322</v>
       </c>
       <c r="C101" s="96" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D101" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101" s="71">
-        <v>877</v>
+        <v>1540</v>
       </c>
       <c r="F101" s="91">
         <f t="shared" si="8"/>
-        <v>877</v>
+        <v>0</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>13</v>
@@ -4976,543 +4988,547 @@
         <v>497</v>
       </c>
     </row>
-    <row r="102" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="51" t="s">
-        <v>496</v>
+    <row r="102" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="3" t="s">
+        <v>495</v>
       </c>
       <c r="B102" s="20" t="s">
         <v>322</v>
       </c>
       <c r="C102" s="96" t="s">
-        <v>423</v>
-      </c>
-      <c r="D102" s="51">
-        <v>0</v>
+        <v>494</v>
+      </c>
+      <c r="D102" s="3">
+        <v>1</v>
       </c>
       <c r="E102" s="71">
-        <v>4700</v>
+        <v>877</v>
       </c>
       <c r="F102" s="91">
         <f t="shared" si="8"/>
+        <v>877</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H102" s="20"/>
+      <c r="I102" s="3" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A103" s="51" t="s">
+        <v>496</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="C103" s="96" t="s">
+        <v>423</v>
+      </c>
+      <c r="D103" s="51">
         <v>0</v>
       </c>
-      <c r="G102" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="H102" s="20"/>
-      <c r="I102" s="51" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="51" t="s">
-        <v>499</v>
-      </c>
-      <c r="B103" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C103" s="51" t="s">
-        <v>500</v>
-      </c>
-      <c r="D103" s="51">
-        <v>1</v>
-      </c>
       <c r="E103" s="71">
-        <v>20</v>
+        <v>4700</v>
       </c>
       <c r="F103" s="91">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G103" s="51" t="s">
         <v>13</v>
       </c>
       <c r="H103" s="20"/>
       <c r="I103" s="51" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
-        <v>501</v>
+        <v>506</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="51" t="s">
+        <v>499</v>
       </c>
       <c r="B104" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C104" s="32" t="s">
-        <v>502</v>
-      </c>
-      <c r="D104" s="3">
+      <c r="C104" s="51" t="s">
+        <v>500</v>
+      </c>
+      <c r="D104" s="51">
         <v>1</v>
       </c>
       <c r="E104" s="71">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F104" s="91">
         <f t="shared" si="8"/>
-        <v>25</v>
-      </c>
-      <c r="G104" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G104" s="51" t="s">
         <v>13</v>
       </c>
       <c r="H104" s="20"/>
       <c r="I104" s="51" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="B105" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C105" s="32" t="s">
+        <v>502</v>
+      </c>
+      <c r="D105" s="3">
+        <v>1</v>
+      </c>
+      <c r="E105" s="71">
+        <v>25</v>
+      </c>
+      <c r="F105" s="91">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H105" s="20"/>
+      <c r="I105" s="51" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="105" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A105" s="17" t="s">
+    <row r="106" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A106" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="E105" s="90"/>
-      <c r="F105" s="90"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
+      <c r="E106" s="90"/>
+      <c r="F106" s="90"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="B106" s="20" t="s">
+      <c r="B107" s="20" t="s">
         <v>322</v>
       </c>
-      <c r="C106" s="68" t="s">
+      <c r="C107" s="68" t="s">
         <v>354</v>
       </c>
-      <c r="D106" s="3">
-        <v>1</v>
-      </c>
-      <c r="E106" s="71">
+      <c r="D107" s="3">
+        <v>1</v>
+      </c>
+      <c r="E107" s="71">
         <v>752</v>
       </c>
-      <c r="F106" s="71">
-        <f t="shared" ref="F106:F111" si="9">D106*E106</f>
+      <c r="F107" s="71">
+        <f t="shared" ref="F107:F112" si="9">D107*E107</f>
         <v>752</v>
       </c>
-      <c r="G106" s="3" t="s">
+      <c r="G107" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I106" s="3" t="s">
+      <c r="I107" s="3" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="107" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
+    <row r="108" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="B107" s="64" t="s">
+      <c r="B108" s="64" t="s">
         <v>227</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="C108" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="D107" s="4">
-        <v>1</v>
-      </c>
-      <c r="E107" s="78">
-        <v>1</v>
-      </c>
-      <c r="F107" s="78">
+      <c r="D108" s="4">
+        <v>1</v>
+      </c>
+      <c r="E108" s="78">
+        <v>1</v>
+      </c>
+      <c r="F108" s="78">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="G107" s="4" t="s">
+      <c r="G108" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I107" s="4" t="s">
+      <c r="I108" s="4" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="B108" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C108" s="3" t="s">
+      <c r="B109" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="D108" s="3">
-        <v>1</v>
-      </c>
-      <c r="E108" s="71">
+      <c r="D109" s="3">
+        <v>1</v>
+      </c>
+      <c r="E109" s="71">
         <v>65</v>
       </c>
-      <c r="F108" s="71">
+      <c r="F109" s="71">
         <f t="shared" si="9"/>
         <v>65</v>
       </c>
-      <c r="G108" s="3" t="s">
+      <c r="G109" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I108" s="3" t="s">
+      <c r="I109" s="3" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="B109" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C109" s="3" t="s">
+      <c r="B110" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C110" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="D109" s="3">
-        <v>1</v>
-      </c>
-      <c r="E109" s="71">
+      <c r="D110" s="3">
+        <v>1</v>
+      </c>
+      <c r="E110" s="71">
         <v>32</v>
       </c>
-      <c r="F109" s="71">
+      <c r="F110" s="71">
         <f t="shared" si="9"/>
         <v>32</v>
       </c>
-      <c r="G109" s="3" t="s">
+      <c r="G110" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I109" s="3" t="s">
+      <c r="I110" s="3" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="B110" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C110" s="3" t="s">
+      <c r="B111" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C111" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="D110" s="3">
-        <v>1</v>
-      </c>
-      <c r="E110" s="71">
+      <c r="D111" s="3">
+        <v>1</v>
+      </c>
+      <c r="E111" s="71">
         <v>112</v>
       </c>
-      <c r="F110" s="71">
+      <c r="F111" s="71">
         <f t="shared" si="9"/>
         <v>112</v>
       </c>
-      <c r="G110" s="3" t="s">
+      <c r="G111" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I110" s="3" t="s">
+      <c r="I111" s="3" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="111" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="4" t="s">
+    <row r="112" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="4" t="s">
         <v>561</v>
       </c>
-      <c r="B111" s="64" t="s">
+      <c r="B112" s="64" t="s">
         <v>227</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="C112" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="D111" s="4">
-        <v>1</v>
-      </c>
-      <c r="E111" s="78">
+      <c r="D112" s="4">
+        <v>1</v>
+      </c>
+      <c r="E112" s="78">
         <v>2</v>
       </c>
-      <c r="F111" s="78">
+      <c r="F112" s="78">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="G111" s="4" t="s">
+      <c r="G112" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I111" s="4" t="s">
+      <c r="I112" s="4" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="112" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A112" s="5" t="s">
+    <row r="113" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A113" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E112" s="72"/>
-      <c r="F112" s="72"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D113" s="3">
-        <v>1</v>
-      </c>
-      <c r="E113" s="71">
-        <v>3582</v>
-      </c>
-      <c r="F113" s="71">
-        <f t="shared" ref="F113:F125" si="10">E113*D113</f>
-        <v>3582</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I113" s="3" t="s">
-        <v>487</v>
-      </c>
+      <c r="E113" s="72"/>
+      <c r="F113" s="72"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>180</v>
+        <v>57</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C114" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D114" s="3">
+        <v>1</v>
+      </c>
+      <c r="E114" s="71">
+        <v>3582</v>
+      </c>
+      <c r="F114" s="71">
+        <f t="shared" ref="F114:F126" si="10">E114*D114</f>
+        <v>3582</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D114" s="3">
-        <v>1</v>
-      </c>
-      <c r="E114" s="71">
+      <c r="D115" s="3">
+        <v>1</v>
+      </c>
+      <c r="E115" s="71">
         <v>1630</v>
       </c>
-      <c r="F114" s="71">
+      <c r="F115" s="71">
         <f t="shared" si="10"/>
         <v>1630</v>
       </c>
-      <c r="G114" s="3" t="s">
+      <c r="G115" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I114" s="3" t="s">
+      <c r="I115" s="3" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B116" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C116" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="D115" s="3">
-        <v>1</v>
-      </c>
-      <c r="E115" s="71">
+      <c r="D116" s="3">
+        <v>1</v>
+      </c>
+      <c r="E116" s="71">
         <v>900</v>
       </c>
-      <c r="F115" s="71">
+      <c r="F116" s="71">
         <f t="shared" si="10"/>
         <v>900</v>
       </c>
-      <c r="G115" s="3" t="s">
+      <c r="G116" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I115" s="3" t="s">
+      <c r="I116" s="3" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B117" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C117" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D116" s="3">
-        <v>1</v>
-      </c>
-      <c r="E116" s="71">
+      <c r="D117" s="3">
+        <v>1</v>
+      </c>
+      <c r="E117" s="71">
         <v>163</v>
       </c>
-      <c r="F116" s="71">
+      <c r="F117" s="71">
         <f t="shared" si="10"/>
         <v>163</v>
       </c>
-      <c r="G116" s="3" t="s">
+      <c r="G117" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I116" s="3" t="s">
+      <c r="I117" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B118" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C118" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D117" s="3">
-        <v>1</v>
-      </c>
-      <c r="E117" s="71">
+      <c r="D118" s="3">
+        <v>1</v>
+      </c>
+      <c r="E118" s="71">
         <v>11</v>
       </c>
-      <c r="F117" s="71">
+      <c r="F118" s="71">
         <f t="shared" si="10"/>
         <v>11</v>
       </c>
-      <c r="G117" s="3" t="s">
+      <c r="G118" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B119" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C119" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D118" s="3">
-        <v>1</v>
-      </c>
-      <c r="E118" s="71">
+      <c r="D119" s="3">
+        <v>1</v>
+      </c>
+      <c r="E119" s="71">
         <v>520</v>
       </c>
-      <c r="F118" s="71">
+      <c r="F119" s="71">
         <f t="shared" si="10"/>
         <v>520</v>
       </c>
-      <c r="G118" s="3" t="s">
+      <c r="G119" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B120" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C120" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D119" s="3">
-        <v>1</v>
-      </c>
-      <c r="E119" s="71">
+      <c r="D120" s="3">
+        <v>1</v>
+      </c>
+      <c r="E120" s="71">
         <v>193</v>
       </c>
-      <c r="F119" s="71">
+      <c r="F120" s="71">
         <f t="shared" si="10"/>
         <v>193</v>
       </c>
-      <c r="G119" s="3" t="s">
+      <c r="G120" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="120" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="23" t="s">
+    <row r="121" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="23" t="s">
         <v>290</v>
       </c>
-      <c r="B120" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C120" s="23" t="s">
+      <c r="B121" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C121" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="D120" s="23">
+      <c r="D121" s="23">
         <v>10</v>
       </c>
-      <c r="E120" s="82">
+      <c r="E121" s="82">
         <v>12</v>
       </c>
-      <c r="F120" s="82">
+      <c r="F121" s="82">
         <f t="shared" si="10"/>
         <v>120</v>
       </c>
-      <c r="G120" s="23" t="s">
+      <c r="G121" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="I120" s="23" t="s">
+      <c r="I121" s="23" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="121" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="23" t="s">
+    <row r="122" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="B121" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C121" s="23" t="s">
+      <c r="B122" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C122" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="D121" s="23">
-        <v>1</v>
-      </c>
-      <c r="E121" s="82">
+      <c r="D122" s="23">
+        <v>1</v>
+      </c>
+      <c r="E122" s="82">
         <v>14</v>
       </c>
-      <c r="F121" s="82">
+      <c r="F122" s="82">
         <f t="shared" si="10"/>
         <v>14</v>
       </c>
-      <c r="G121" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="I121" s="23" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D122" s="3">
-        <v>4</v>
-      </c>
-      <c r="E122" s="71">
-        <v>15.25</v>
-      </c>
-      <c r="F122" s="71">
-        <f t="shared" si="10"/>
-        <v>61</v>
-      </c>
       <c r="G122" s="23" t="s">
         <v>51</v>
       </c>
+      <c r="I122" s="23" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D123" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E123" s="71">
-        <v>16.5</v>
+        <v>15.25</v>
       </c>
       <c r="F123" s="71">
         <f t="shared" si="10"/>
-        <v>165</v>
+        <v>61</v>
       </c>
       <c r="G123" s="23" t="s">
         <v>51</v>
@@ -5520,23 +5536,23 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D124" s="3">
         <v>10</v>
       </c>
       <c r="E124" s="71">
-        <v>24</v>
+        <v>16.5</v>
       </c>
       <c r="F124" s="71">
         <f t="shared" si="10"/>
-        <v>240</v>
+        <v>165</v>
       </c>
       <c r="G124" s="23" t="s">
         <v>51</v>
@@ -5544,177 +5560,180 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D125" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E125" s="71">
         <v>24</v>
       </c>
       <c r="F125" s="71">
         <f t="shared" si="10"/>
-        <v>144</v>
+        <v>240</v>
       </c>
       <c r="G125" s="23" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E126" s="82"/>
-      <c r="F126" s="82"/>
-    </row>
-    <row r="128" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A128" s="10"/>
-      <c r="B128" s="10"/>
-      <c r="C128" s="9"/>
-    </row>
-    <row r="129" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="7" t="s">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D126" s="3">
+        <v>6</v>
+      </c>
+      <c r="E126" s="71">
+        <v>24</v>
+      </c>
+      <c r="F126" s="71">
+        <f t="shared" si="10"/>
+        <v>144</v>
+      </c>
+      <c r="G126" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E127" s="82"/>
+      <c r="F127" s="82"/>
+    </row>
+    <row r="129" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A129" s="10"/>
+      <c r="B129" s="10"/>
+      <c r="C129" s="9"/>
+    </row>
+    <row r="130" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E129" s="72"/>
-      <c r="F129" s="72"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D130" s="3">
-        <v>4</v>
-      </c>
-      <c r="E130" s="71">
-        <v>16.5</v>
-      </c>
-      <c r="F130" s="71">
-        <f t="shared" ref="F130:F145" si="11">E130*D130</f>
-        <v>66</v>
-      </c>
-      <c r="I130" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="E130" s="72"/>
+      <c r="F130" s="72"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D131" s="3">
+        <v>4</v>
+      </c>
+      <c r="E131" s="71">
+        <v>16.5</v>
+      </c>
+      <c r="F131" s="71">
+        <f t="shared" ref="F131:F146" si="11">E131*D131</f>
+        <v>66</v>
+      </c>
+      <c r="I131" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B131" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C131" s="3" t="s">
+      <c r="B132" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C132" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D131" s="3">
-        <v>1</v>
-      </c>
-      <c r="E131" s="71">
+      <c r="D132" s="3">
+        <v>1</v>
+      </c>
+      <c r="E132" s="71">
         <v>85.1</v>
       </c>
-      <c r="F131" s="71">
+      <c r="F132" s="71">
         <f t="shared" si="11"/>
         <v>85.1</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="s">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B132" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C132" s="3" t="s">
+      <c r="B133" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C133" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D132" s="3">
+      <c r="D133" s="3">
         <v>2</v>
       </c>
-      <c r="E132" s="71">
+      <c r="E133" s="71">
         <v>32</v>
       </c>
-      <c r="F132" s="71">
+      <c r="F133" s="71">
         <f t="shared" si="11"/>
         <v>64</v>
       </c>
-      <c r="I132" s="3" t="s">
+      <c r="I133" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="3" t="s">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B133" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C133" s="3" t="s">
+      <c r="B134" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C134" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D133" s="3">
+      <c r="D134" s="3">
         <v>2</v>
       </c>
-      <c r="E133" s="71">
+      <c r="E134" s="71">
         <v>51.58</v>
       </c>
-      <c r="F133" s="71">
+      <c r="F134" s="71">
         <f t="shared" si="11"/>
         <v>103.16</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="3" t="s">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B134" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C134" s="3" t="s">
+      <c r="B135" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C135" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D134" s="3">
-        <v>1</v>
-      </c>
-      <c r="E134" s="71">
+      <c r="D135" s="3">
+        <v>1</v>
+      </c>
+      <c r="E135" s="71">
         <v>60</v>
       </c>
-      <c r="F134" s="71">
+      <c r="F135" s="71">
         <f t="shared" si="11"/>
         <v>60</v>
       </c>
-      <c r="I134" s="3" t="s">
+      <c r="I135" s="3" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A135" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D135" s="3">
-        <v>1</v>
-      </c>
-      <c r="E135" s="71">
-        <v>136.47999999999999</v>
-      </c>
-      <c r="F135" s="71">
-        <f t="shared" si="11"/>
-        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -5725,7 +5744,7 @@
         <v>61</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D136" s="3">
         <v>1</v>
@@ -5740,296 +5759,296 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D137" s="3">
         <v>1</v>
       </c>
       <c r="E137" s="71">
-        <v>60.95</v>
+        <v>136.47999999999999</v>
       </c>
       <c r="F137" s="71">
         <f t="shared" si="11"/>
-        <v>60.95</v>
+        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D138" s="3">
         <v>1</v>
       </c>
       <c r="E138" s="71">
-        <v>119.416</v>
+        <v>60.95</v>
       </c>
       <c r="F138" s="71">
         <f t="shared" si="11"/>
-        <v>119.416</v>
+        <v>60.95</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D139" s="3">
         <v>1</v>
       </c>
       <c r="E139" s="71">
-        <v>105.8</v>
+        <v>119.416</v>
       </c>
       <c r="F139" s="71">
         <f t="shared" si="11"/>
-        <v>105.8</v>
+        <v>119.416</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D140" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E140" s="71">
-        <v>119.6</v>
+        <v>105.8</v>
       </c>
       <c r="F140" s="71">
         <f t="shared" si="11"/>
-        <v>239.2</v>
+        <v>105.8</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>299</v>
+        <v>146</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>300</v>
+        <v>147</v>
       </c>
       <c r="D141" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E141" s="71">
-        <v>100</v>
+        <v>119.6</v>
       </c>
       <c r="F141" s="71">
         <f t="shared" si="11"/>
-        <v>100</v>
+        <v>239.2</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>148</v>
+        <v>299</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>149</v>
+        <v>300</v>
       </c>
       <c r="D142" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E142" s="71">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F142" s="71">
         <f t="shared" si="11"/>
-        <v>184</v>
+        <v>100</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D143" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E143" s="71">
-        <v>96.23</v>
+        <v>92</v>
       </c>
       <c r="F143" s="71">
         <f t="shared" si="11"/>
-        <v>96.23</v>
+        <v>184</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D144" s="3">
         <v>1</v>
       </c>
       <c r="E144" s="71">
-        <v>102.44</v>
+        <v>96.23</v>
       </c>
       <c r="F144" s="71">
         <f t="shared" si="11"/>
-        <v>102.44</v>
+        <v>96.23</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D145" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E145" s="71">
-        <v>28</v>
+        <v>102.44</v>
       </c>
       <c r="F145" s="71">
         <f t="shared" si="11"/>
+        <v>102.44</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D146" s="3">
+        <v>2</v>
+      </c>
+      <c r="E146" s="71">
+        <v>28</v>
+      </c>
+      <c r="F146" s="71">
+        <f t="shared" si="11"/>
         <v>56</v>
-      </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C146" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D146" s="3">
-        <v>4</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C147" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D147" s="3">
-        <v>1</v>
-      </c>
-      <c r="I147" s="3" t="s">
-        <v>158</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C148" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D148" s="3">
+        <v>1</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C149" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D148" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A150" s="7" t="s">
+      <c r="D149" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A151" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B150" s="6" t="s">
+      <c r="B151" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="E150" s="72"/>
-      <c r="F150" s="72"/>
-    </row>
-    <row r="151" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="51"/>
-      <c r="B151" s="51" t="s">
+      <c r="E151" s="72"/>
+      <c r="F151" s="72"/>
+    </row>
+    <row r="152" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="51"/>
+      <c r="B152" s="51" t="s">
         <v>438</v>
       </c>
-      <c r="C151" s="53" t="s">
+      <c r="C152" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="D151" s="51">
+      <c r="D152" s="51">
         <v>4</v>
       </c>
-      <c r="E151" s="71">
+      <c r="E152" s="71">
         <v>40</v>
-      </c>
-      <c r="F151" s="71">
-        <f>E151*D151</f>
-        <v>160</v>
-      </c>
-      <c r="G151" s="51" t="s">
-        <v>436</v>
-      </c>
-      <c r="H151" s="51" t="s">
-        <v>437</v>
-      </c>
-      <c r="I151" s="51" t="s">
-        <v>435</v>
-      </c>
-      <c r="J151" s="53"/>
-    </row>
-    <row r="152" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B152" s="51" t="s">
-        <v>162</v>
-      </c>
-      <c r="C152" s="51" t="s">
-        <v>350</v>
-      </c>
-      <c r="D152" s="51">
-        <v>2</v>
-      </c>
-      <c r="E152" s="71">
-        <v>331</v>
       </c>
       <c r="F152" s="71">
         <f>E152*D152</f>
-        <v>662</v>
+        <v>160</v>
       </c>
       <c r="G152" s="51" t="s">
-        <v>439</v>
-      </c>
+        <v>436</v>
+      </c>
+      <c r="H152" s="51" t="s">
+        <v>437</v>
+      </c>
+      <c r="I152" s="51" t="s">
+        <v>435</v>
+      </c>
+      <c r="J152" s="53"/>
     </row>
     <row r="153" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B153" s="51" t="s">
         <v>162</v>
       </c>
       <c r="C153" s="51" t="s">
-        <v>286</v>
+        <v>350</v>
       </c>
       <c r="D153" s="51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E153" s="71">
-        <v>25</v>
+        <v>331</v>
       </c>
       <c r="F153" s="71">
         <f>E153*D153</f>
-        <v>100</v>
+        <v>662</v>
       </c>
       <c r="G153" s="51" t="s">
         <v>439</v>
@@ -6040,17 +6059,17 @@
         <v>162</v>
       </c>
       <c r="C154" s="51" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D154" s="51">
         <v>4</v>
       </c>
       <c r="E154" s="71">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F154" s="71">
         <f>E154*D154</f>
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G154" s="51" t="s">
         <v>439</v>
@@ -6061,230 +6080,251 @@
         <v>162</v>
       </c>
       <c r="C155" s="51" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D155" s="51">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E155" s="71">
-        <v>121.5</v>
+        <v>28</v>
       </c>
       <c r="F155" s="71">
         <f>E155*D155</f>
-        <v>729</v>
+        <v>112</v>
       </c>
       <c r="G155" s="51" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E158" s="66" t="s">
+    <row r="156" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C156" s="51" t="s">
+        <v>288</v>
+      </c>
+      <c r="D156" s="51">
+        <v>6</v>
+      </c>
+      <c r="E156" s="71">
+        <v>121.5</v>
+      </c>
+      <c r="F156" s="71">
+        <f>E156*D156</f>
+        <v>729</v>
+      </c>
+      <c r="G156" s="51" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E159" s="66" t="s">
         <v>468</v>
       </c>
-      <c r="F158" s="66">
-        <f>SUM(F3:F156)</f>
-        <v>95654.501499199992</v>
-      </c>
-      <c r="G158" s="3" t="s">
+      <c r="F159" s="66">
+        <f>SUM(F3:F157)</f>
+        <v>95950.501499199992</v>
+      </c>
+      <c r="G159" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="160" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E160" s="71"/>
-      <c r="F160" s="71"/>
-    </row>
-    <row r="162" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A162" s="65" t="s">
+    <row r="161" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E161" s="71"/>
+      <c r="F161" s="71"/>
+    </row>
+    <row r="163" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A163" s="65" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A163" s="4" t="s">
+    <row r="164" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A164" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="B163" s="4" t="s">
+      <c r="B164" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="C163" s="4" t="s">
+      <c r="C164" s="4" t="s">
         <v>442</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="B164" s="3">
-        <v>14</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B165" s="3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B166" s="3">
         <v>2</v>
       </c>
-      <c r="C166" s="51" t="s">
-        <v>455</v>
+      <c r="C166" s="3" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B167" s="3">
         <v>2</v>
       </c>
-      <c r="C167" s="3" t="s">
+      <c r="C167" s="51" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="B168" s="3">
+        <v>2</v>
+      </c>
+      <c r="C168" s="3" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A170" s="65" t="s">
+    <row r="171" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A171" s="65" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A171" s="4" t="s">
+    <row r="172" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A172" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="B172" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="C171" s="4" t="s">
+      <c r="C172" s="4" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A172" s="3" t="s">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="B172" s="3">
+      <c r="B173" s="3">
         <v>2</v>
       </c>
-      <c r="C172" s="3" t="s">
+      <c r="C173" s="3" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A173" s="3" t="s">
+    <row r="174" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A174" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="B173" s="3">
+      <c r="B174" s="3">
         <v>5</v>
       </c>
-      <c r="C173" s="3" t="s">
+      <c r="C174" s="3" t="s">
         <v>463</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A174" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="B174" s="3">
-        <v>1</v>
-      </c>
-      <c r="C174" s="3" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B175" s="3">
+        <v>1</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="B175" s="3">
-        <v>1</v>
-      </c>
-      <c r="C175" s="3" t="s">
+      <c r="B176" s="3">
+        <v>1</v>
+      </c>
+      <c r="C176" s="3" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="176" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="51" t="s">
+    <row r="177" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="51" t="s">
         <v>561</v>
       </c>
-      <c r="B176" s="51">
-        <v>1</v>
-      </c>
-      <c r="C176" s="51" t="s">
+      <c r="B177" s="51">
+        <v>1</v>
+      </c>
+      <c r="C177" s="51" t="s">
         <v>562</v>
       </c>
-      <c r="E176" s="71"/>
-      <c r="F176" s="71"/>
-    </row>
-    <row r="178" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A178" s="65" t="s">
+      <c r="E177" s="71"/>
+      <c r="F177" s="71"/>
+    </row>
+    <row r="179" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A179" s="65" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A179" s="4" t="s">
+    <row r="180" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A180" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="B180" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="C179" s="4" t="s">
+      <c r="C180" s="4" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" s="51" t="s">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" s="51" t="s">
         <v>460</v>
       </c>
-      <c r="B180" s="3">
+      <c r="B181" s="3">
         <v>5</v>
       </c>
-      <c r="C180" s="3" t="s">
+      <c r="C181" s="3" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" s="3" t="s">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B181" s="3">
+      <c r="B182" s="3">
         <v>3</v>
       </c>
-      <c r="C181" s="3" t="s">
+      <c r="C182" s="3" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" s="3" t="s">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="B182" s="3" t="s">
+      <c r="B183" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="C182" s="3" t="s">
+      <c r="C183" s="3" t="s">
         <v>467</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C98" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C99" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C100" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C101" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C106" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C89" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C102" r:id="rId7" xr:uid="{3002EF90-377A-4FAD-A836-B22D0D243A96}"/>
+    <hyperlink ref="C99" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C100" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C101" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C102" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C107" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C90" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C103" r:id="rId7" xr:uid="{3002EF90-377A-4FAD-A836-B22D0D243A96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>

</xml_diff>

<commit_message>
added Ø45.0 mm Sorbothane Feet to the shopping cart
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C99DE20-761A-4156-ADA3-57C25FC9CCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDD7649-C414-486F-858D-B26994D78468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4452" yWindow="4656" windowWidth="35112" windowHeight="16824" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5244" yWindow="4884" windowWidth="27516" windowHeight="16824" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="578">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -1823,6 +1823,15 @@
   </si>
   <si>
     <t>QuadLine Emission ZET405/488/561/640m, in 25 mm diameter</t>
+  </si>
+  <si>
+    <t>AV6/M</t>
+  </si>
+  <si>
+    <t>Ø45.0 mm Sorbothane Feet, Internal M6 Mounting Thread, 4 Pieces</t>
+  </si>
+  <si>
+    <t>Attached to the bottom of the PBG52522 Breadboard</t>
   </si>
 </sst>
 </file>
@@ -2576,10 +2585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J186"/>
+  <dimension ref="A1:J187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E157" sqref="E157"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3358,116 +3367,112 @@
         <v>524</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="D39" s="3">
-        <v>2</v>
-      </c>
-      <c r="E39" s="59">
-        <v>31</v>
-      </c>
-      <c r="F39" s="57">
-        <f t="shared" ref="F39:F44" si="2">E39*D39</f>
-        <v>62</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H39" s="79" t="s">
-        <v>193</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>557</v>
+    <row r="39" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="77" t="s">
+        <v>575</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="41" t="s">
+        <v>576</v>
+      </c>
+      <c r="D39" s="41">
+        <v>1</v>
+      </c>
+      <c r="E39" s="76">
+        <v>33</v>
+      </c>
+      <c r="F39" s="76">
+        <v>33</v>
+      </c>
+      <c r="G39" s="41" t="s">
+        <v>521</v>
+      </c>
+      <c r="I39" s="41" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>191</v>
+        <v>67</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D40" s="3">
         <v>2</v>
       </c>
       <c r="E40" s="59">
+        <v>31</v>
+      </c>
+      <c r="F40" s="57">
+        <f t="shared" ref="F40:F45" si="2">E40*D40</f>
+        <v>62</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H40" s="79" t="s">
+        <v>193</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D41" s="3">
+        <v>2</v>
+      </c>
+      <c r="E41" s="59">
         <v>99</v>
       </c>
-      <c r="F40" s="57">
+      <c r="F41" s="57">
         <f t="shared" si="2"/>
         <v>198</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G41" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H40" s="79" t="s">
+      <c r="H41" s="79" t="s">
         <v>193</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="I41" s="3" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="B42" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D42" s="3">
         <v>2</v>
       </c>
-      <c r="E41" s="57">
+      <c r="E42" s="57">
         <v>17</v>
       </c>
-      <c r="F41" s="57">
+      <c r="F42" s="57">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="G41" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H41" s="79" t="s">
-        <v>193</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>549</v>
-      </c>
-      <c r="D42" s="3">
-        <v>2</v>
-      </c>
-      <c r="E42" s="57">
-        <v>12</v>
-      </c>
-      <c r="F42" s="57">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
       <c r="G42" s="3" t="s">
         <v>38</v>
       </c>
@@ -3475,18 +3480,18 @@
         <v>193</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D43" s="3">
         <v>2</v>
@@ -3505,28 +3510,28 @@
         <v>193</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>200</v>
+        <v>550</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D44" s="3">
         <v>2</v>
       </c>
       <c r="E44" s="57">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F44" s="57">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>38</v>
@@ -3535,194 +3540,197 @@
         <v>193</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>290</v>
+        <v>200</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>498</v>
+        <v>552</v>
       </c>
       <c r="D45" s="3">
         <v>2</v>
       </c>
       <c r="E45" s="57">
-        <v>18.412749600000001</v>
+        <v>14</v>
       </c>
       <c r="F45" s="57">
-        <v>36.825499200000003</v>
+        <f t="shared" si="2"/>
+        <v>28</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H45" s="3" t="s">
-        <v>499</v>
+      <c r="H45" s="79" t="s">
+        <v>193</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>37</v>
+        <v>290</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>315</v>
+        <v>59</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="D46" s="3">
         <v>2</v>
       </c>
       <c r="E46" s="57">
-        <v>935</v>
+        <v>18.412749600000001</v>
       </c>
       <c r="F46" s="57">
-        <f t="shared" ref="F46:F52" si="3">E46*D46</f>
-        <v>1870</v>
+        <v>36.825499200000003</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>38</v>
       </c>
       <c r="H46" s="3" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="D47" s="3">
+        <v>2</v>
+      </c>
+      <c r="E47" s="57">
+        <v>935</v>
+      </c>
+      <c r="F47" s="57">
+        <f t="shared" ref="F47:F53" si="3">E47*D47</f>
+        <v>1870</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+    <row r="48" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D48" s="4">
         <v>2</v>
       </c>
-      <c r="E47" s="60">
+      <c r="E48" s="60">
         <v>365</v>
       </c>
-      <c r="F47" s="60">
+      <c r="F48" s="60">
         <f t="shared" si="3"/>
         <v>730</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="G48" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="H48" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="I48" s="4" t="s">
         <v>497</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" s="3">
-        <v>1</v>
-      </c>
-      <c r="E48" s="57">
-        <v>30</v>
-      </c>
-      <c r="F48" s="57">
-        <v>30</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="3">
+        <v>1</v>
+      </c>
+      <c r="E49" s="57">
+        <v>30</v>
+      </c>
+      <c r="F49" s="57">
+        <v>30</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D50" s="3">
         <v>2</v>
       </c>
-      <c r="E49" s="57">
+      <c r="E50" s="57">
         <v>90</v>
       </c>
-      <c r="F49" s="57">
+      <c r="F50" s="57">
         <f t="shared" si="3"/>
         <v>180</v>
       </c>
-      <c r="G49" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
-        <v>519</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="D50" s="3">
-        <v>2</v>
-      </c>
-      <c r="E50" s="59">
-        <v>18</v>
-      </c>
-      <c r="F50" s="57">
-        <f>E50*D50</f>
-        <v>36</v>
-      </c>
       <c r="G50" s="3" t="s">
         <v>38</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>499</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>74</v>
+      <c r="A51" s="9" t="s">
+        <v>519</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>75</v>
+      <c r="C51" s="9" t="s">
+        <v>202</v>
       </c>
       <c r="D51" s="3">
         <v>2</v>
       </c>
-      <c r="E51" s="57">
-        <v>21.21</v>
+      <c r="E51" s="59">
+        <v>18</v>
       </c>
       <c r="F51" s="57">
-        <f t="shared" ref="F51" si="4">E51*D51</f>
-        <v>42.42</v>
+        <f>E51*D51</f>
+        <v>36</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>38</v>
@@ -3730,772 +3738,769 @@
       <c r="H51" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="I51" s="3" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>200</v>
+      <c r="A52" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C52" s="9" t="s">
-        <v>201</v>
+      <c r="C52" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="D52" s="3">
         <v>2</v>
       </c>
-      <c r="E52" s="59">
+      <c r="E52" s="57">
+        <v>21.21</v>
+      </c>
+      <c r="F52" s="57">
+        <f t="shared" ref="F52" si="4">E52*D52</f>
+        <v>42.42</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D53" s="3">
+        <v>2</v>
+      </c>
+      <c r="E53" s="59">
         <v>13</v>
       </c>
-      <c r="F52" s="57">
+      <c r="F53" s="57">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="G52" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="D53" s="3">
-        <v>4</v>
-      </c>
-      <c r="E53" s="59">
-        <v>189</v>
-      </c>
-      <c r="F53" s="57">
-        <f t="shared" ref="F53:F60" si="5">E53*D53</f>
-        <v>756</v>
-      </c>
       <c r="G53" s="3" t="s">
         <v>38</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="I53" s="3" t="s">
-        <v>289</v>
+        <v>499</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D54" s="3">
         <v>4</v>
       </c>
       <c r="E54" s="59">
+        <v>189</v>
+      </c>
+      <c r="F54" s="57">
+        <f t="shared" ref="F54:F61" si="5">E54*D54</f>
+        <v>756</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D55" s="3">
+        <v>4</v>
+      </c>
+      <c r="E55" s="59">
         <v>110</v>
       </c>
-      <c r="F54" s="57">
+      <c r="F55" s="57">
         <f t="shared" si="5"/>
         <v>440</v>
       </c>
-      <c r="G54" s="3" t="s">
+      <c r="G55" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="H55" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="I54" s="3" t="s">
+      <c r="I55" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" s="9" t="s">
+      <c r="B56" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D56" s="3">
         <v>8</v>
       </c>
-      <c r="E55" s="59">
+      <c r="E56" s="59">
         <v>16</v>
       </c>
-      <c r="F55" s="57">
+      <c r="F56" s="57">
         <f t="shared" si="5"/>
         <v>128</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="G56" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="H56" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="I55" s="3" t="s">
+      <c r="I56" s="3" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" s="9" t="s">
+      <c r="B57" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D57" s="3">
         <v>4</v>
       </c>
-      <c r="E56" s="59">
+      <c r="E57" s="59">
         <v>104</v>
       </c>
-      <c r="F56" s="57">
+      <c r="F57" s="57">
         <f t="shared" si="5"/>
         <v>416</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G57" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="H57" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="I56" s="3" t="s">
+      <c r="I57" s="3" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C57" s="9" t="s">
+      <c r="B58" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D58" s="3">
         <v>2</v>
       </c>
-      <c r="E57" s="59">
+      <c r="E58" s="59">
         <v>41</v>
       </c>
-      <c r="F57" s="57">
+      <c r="F58" s="57">
         <f t="shared" si="5"/>
         <v>82</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G58" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H57" s="3" t="s">
+      <c r="H58" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="I57" s="3" t="s">
+      <c r="I58" s="3" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
         <v>512</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C58" s="9" t="s">
+      <c r="B59" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>513</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D59" s="3">
         <v>2</v>
       </c>
-      <c r="E58" s="59">
+      <c r="E59" s="59">
         <v>17</v>
       </c>
-      <c r="F58" s="57">
+      <c r="F59" s="57">
         <f t="shared" si="5"/>
         <v>34</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="G59" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H58" s="3" t="s">
+      <c r="H59" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="I58" s="3" t="s">
+      <c r="I59" s="3" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>514</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="9" t="s">
+      <c r="B60" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>515</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D60" s="3">
         <v>4</v>
       </c>
-      <c r="E59" s="59">
+      <c r="E60" s="59">
         <v>7</v>
       </c>
-      <c r="F59" s="57">
+      <c r="F60" s="57">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="G59" s="3" t="s">
+      <c r="G60" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H59" s="3" t="s">
+      <c r="H60" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="I59" s="3" t="s">
+      <c r="I60" s="3" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>517</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="9" t="s">
+      <c r="B61" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>516</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D61" s="3">
         <v>4</v>
       </c>
-      <c r="E60" s="59">
+      <c r="E61" s="59">
         <v>5</v>
       </c>
-      <c r="F60" s="57">
+      <c r="F61" s="57">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="H61" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="I60" s="3" t="s">
+      <c r="I61" s="3" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="49">
+    <row r="62" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="49">
         <v>91863</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C62" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="D61" s="4">
-        <v>2</v>
-      </c>
-      <c r="E61" s="60">
-        <v>400</v>
-      </c>
-      <c r="F61" s="60">
-        <f t="shared" ref="F61:F84" si="6">E61*D61</f>
-        <v>800</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
-        <v>567</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>560</v>
-      </c>
-      <c r="C62" s="50" t="s">
-        <v>528</v>
       </c>
       <c r="D62" s="4">
         <v>2</v>
       </c>
       <c r="E62" s="60">
+        <v>400</v>
+      </c>
+      <c r="F62" s="60">
+        <f t="shared" ref="F62:F85" si="6">E62*D62</f>
+        <v>800</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="C63" s="50" t="s">
+        <v>528</v>
+      </c>
+      <c r="D63" s="4">
+        <v>2</v>
+      </c>
+      <c r="E63" s="60">
         <v>300</v>
       </c>
-      <c r="F62" s="60">
+      <c r="F63" s="60">
         <f t="shared" si="6"/>
         <v>600</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="G63" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H62" s="4" t="s">
+      <c r="H63" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="I62" s="4" t="s">
+      <c r="I63" s="4" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="46" t="s">
+    <row r="64" spans="1:10" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="46" t="s">
         <v>424</v>
       </c>
-      <c r="B63" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="C63" s="46" t="s">
+      <c r="B64" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="D63" s="45">
+      <c r="D64" s="45">
         <v>0</v>
       </c>
-      <c r="E63" s="65">
+      <c r="E64" s="65">
         <v>36</v>
       </c>
-      <c r="F63" s="66">
+      <c r="F64" s="66">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G63" s="45" t="s">
+      <c r="G64" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="H63" s="45" t="s">
+      <c r="H64" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="I63" s="45" t="s">
+      <c r="I64" s="45" t="s">
         <v>509</v>
       </c>
-      <c r="J63" s="75"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
+      <c r="J64" s="75"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C64" s="9" t="s">
+      <c r="B65" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C65" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D65" s="3">
         <v>2</v>
       </c>
-      <c r="E64" s="59">
+      <c r="E65" s="59">
         <v>92</v>
       </c>
-      <c r="F64" s="57">
+      <c r="F65" s="57">
         <f t="shared" si="6"/>
         <v>184</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="G65" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="H65" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="I64" s="3" t="s">
+      <c r="I65" s="3" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="10" t="s">
+    <row r="66" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="C65" s="74" t="s">
+      <c r="C66" s="74" t="s">
         <v>264</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <v>2</v>
       </c>
-      <c r="E65" s="62">
-        <v>1</v>
-      </c>
-      <c r="F65" s="60">
+      <c r="E66" s="62">
+        <v>1</v>
+      </c>
+      <c r="F66" s="60">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="G65" s="4" t="s">
+      <c r="G66" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H65" s="4" t="s">
+      <c r="H66" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="I65" s="4" t="s">
+      <c r="I66" s="4" t="s">
         <v>505</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
-        <v>503</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>502</v>
-      </c>
-      <c r="D66" s="3">
-        <v>4</v>
-      </c>
-      <c r="E66" s="59">
-        <v>7</v>
-      </c>
-      <c r="F66" s="57">
-        <f>E66*D66</f>
-        <v>28</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="I66" s="3" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
+        <v>503</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="D67" s="3">
+        <v>4</v>
+      </c>
+      <c r="E67" s="59">
+        <v>7</v>
+      </c>
+      <c r="F67" s="57">
+        <f>E67*D67</f>
+        <v>28</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C67" s="9" t="s">
+      <c r="B68" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D68" s="3">
         <v>2</v>
       </c>
-      <c r="E67" s="59">
+      <c r="E68" s="59">
         <v>8</v>
       </c>
-      <c r="F67" s="57">
+      <c r="F68" s="57">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="G67" s="3" t="s">
+      <c r="G68" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H67" s="3" t="s">
+      <c r="H68" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C68" s="9" t="s">
+      <c r="B69" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D69" s="3">
         <v>4</v>
       </c>
-      <c r="E68" s="59">
+      <c r="E69" s="59">
         <v>5</v>
       </c>
-      <c r="F68" s="57">
+      <c r="F69" s="57">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="G68" s="3" t="s">
+      <c r="G69" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="H69" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="I68" s="3" t="s">
+      <c r="I69" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
         <v>506</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C69" s="9" t="s">
+      <c r="B70" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>507</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D70" s="3">
         <v>2</v>
       </c>
-      <c r="E69" s="59">
+      <c r="E70" s="59">
         <v>5</v>
       </c>
-      <c r="F69" s="57">
+      <c r="F70" s="57">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="G69" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="D70" s="3">
-        <v>2</v>
-      </c>
-      <c r="E70" s="59">
-        <v>5</v>
-      </c>
-      <c r="F70" s="57">
-        <f>E70*D70</f>
-        <v>10</v>
-      </c>
       <c r="G70" s="3" t="s">
         <v>38</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="I70" s="3" t="s">
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D71" s="3">
+        <v>2</v>
+      </c>
+      <c r="E71" s="59">
+        <v>5</v>
+      </c>
+      <c r="F71" s="57">
+        <f>E71*D71</f>
+        <v>10</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="I71" s="3" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="23" t="s">
+    <row r="72" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="23" t="s">
         <v>520</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C71" s="23" t="s">
+      <c r="B72" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C72" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="D71" s="24">
+      <c r="D72" s="24">
         <v>2</v>
       </c>
-      <c r="E71" s="63">
+      <c r="E72" s="63">
         <v>398</v>
       </c>
-      <c r="F71" s="64">
+      <c r="F72" s="64">
         <f t="shared" si="6"/>
         <v>796</v>
       </c>
-      <c r="G71" s="3" t="s">
+      <c r="G72" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H71" s="24" t="s">
+      <c r="H72" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="I71" s="24" t="s">
+      <c r="I72" s="24" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="72" spans="1:9" s="80" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="48" t="s">
+    <row r="73" spans="1:9" s="80" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="48" t="s">
         <v>565</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="C72" s="48" t="s">
+      <c r="C73" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="D72" s="80">
+      <c r="D73" s="80">
         <v>2</v>
       </c>
-      <c r="E72" s="81">
+      <c r="E73" s="81">
         <v>150</v>
       </c>
-      <c r="F72" s="82">
+      <c r="F73" s="82">
         <f t="shared" si="6"/>
         <v>300</v>
       </c>
-      <c r="G72" s="4" t="s">
+      <c r="G73" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H72" s="80" t="s">
+      <c r="H73" s="80" t="s">
         <v>214</v>
       </c>
-      <c r="I72" s="80" t="s">
+      <c r="I73" s="80" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="s">
+    <row r="74" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C73" s="23" t="s">
+      <c r="B74" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C74" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="D73" s="24">
+      <c r="D74" s="24">
         <v>2</v>
       </c>
-      <c r="E73" s="63">
+      <c r="E74" s="63">
         <v>30</v>
       </c>
-      <c r="F73" s="64">
+      <c r="F74" s="64">
         <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="G73" s="3" t="s">
+      <c r="G74" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H73" s="24" t="s">
+      <c r="H74" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="I73" s="24" t="s">
+      <c r="I74" s="24" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="74" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="10" t="s">
+    <row r="75" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="10" t="s">
         <v>564</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C75" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D75" s="4">
         <v>2</v>
       </c>
-      <c r="E74" s="62">
+      <c r="E75" s="62">
         <v>300</v>
       </c>
-      <c r="F74" s="60">
-        <f t="shared" ref="F74" si="7">E74*D74</f>
+      <c r="F75" s="60">
+        <f t="shared" ref="F75" si="7">E75*D75</f>
         <v>600</v>
       </c>
-      <c r="G74" s="4" t="s">
+      <c r="G75" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H74" s="4" t="s">
+      <c r="H75" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="I74" s="4" t="s">
+      <c r="I75" s="4" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="75" spans="1:9" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="46" t="s">
+    <row r="76" spans="1:9" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="46" t="s">
         <v>424</v>
       </c>
-      <c r="B75" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="C75" s="46" t="s">
+      <c r="B76" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C76" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="D75" s="45">
+      <c r="D76" s="45">
         <v>0</v>
       </c>
-      <c r="E75" s="65">
+      <c r="E76" s="65">
         <v>36</v>
       </c>
-      <c r="F75" s="66">
+      <c r="F76" s="66">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G75" s="45" t="s">
+      <c r="G76" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="H75" s="45" t="s">
+      <c r="H76" s="45" t="s">
         <v>216</v>
       </c>
-      <c r="I75" s="45" t="s">
+      <c r="I76" s="45" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
         <v>529</v>
       </c>
-      <c r="B76" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C76" s="9" t="s">
+      <c r="B77" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D77" s="3">
         <v>2</v>
       </c>
-      <c r="E76" s="59">
+      <c r="E77" s="59">
         <v>32</v>
       </c>
-      <c r="F76" s="57">
+      <c r="F77" s="57">
         <f t="shared" si="6"/>
         <v>64</v>
       </c>
-      <c r="G76" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H76" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="I76" s="3" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="9" t="s">
-        <v>424</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>527</v>
-      </c>
-      <c r="D77" s="3">
-        <v>2</v>
-      </c>
-      <c r="E77" s="59">
-        <v>36</v>
-      </c>
-      <c r="F77" s="57">
-        <f t="shared" ref="F77" si="8">E77*D77</f>
-        <v>72</v>
-      </c>
       <c r="G77" s="3" t="s">
         <v>38</v>
       </c>
@@ -4503,584 +4508,586 @@
         <v>216</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>526</v>
+        <v>531</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>272</v>
+        <v>424</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>273</v>
+        <v>527</v>
       </c>
       <c r="D78" s="3">
         <v>2</v>
       </c>
       <c r="E78" s="59">
+        <v>36</v>
+      </c>
+      <c r="F78" s="57">
+        <f t="shared" ref="F78" si="8">E78*D78</f>
+        <v>72</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D79" s="3">
+        <v>2</v>
+      </c>
+      <c r="E79" s="59">
         <v>2104</v>
       </c>
-      <c r="F78" s="57">
+      <c r="F79" s="57">
         <f t="shared" si="6"/>
         <v>4208</v>
       </c>
-      <c r="G78" s="3" t="s">
+      <c r="G79" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H78" s="3" t="s">
+      <c r="H79" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="I78" s="3" t="s">
+      <c r="I79" s="3" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="9" t="s">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="B79" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C79" s="9" t="s">
+      <c r="B80" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="D79" s="3">
+      <c r="D80" s="3">
         <v>2</v>
       </c>
-      <c r="E79" s="59">
+      <c r="E80" s="59">
         <v>82</v>
       </c>
-      <c r="F79" s="57">
+      <c r="F80" s="57">
         <f t="shared" si="6"/>
         <v>164</v>
       </c>
-      <c r="G79" s="3" t="s">
+      <c r="G80" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H79" s="3" t="s">
+      <c r="H80" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="I79" s="3" t="s">
+      <c r="I80" s="3" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="27" t="s">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="27" t="s">
         <v>439</v>
       </c>
-      <c r="B80" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C80" s="9" t="s">
+      <c r="B81" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>440</v>
       </c>
-      <c r="D80" s="3">
-        <v>1</v>
-      </c>
-      <c r="E80" s="59">
+      <c r="D81" s="3">
+        <v>1</v>
+      </c>
+      <c r="E81" s="59">
         <v>520</v>
       </c>
-      <c r="F80" s="57">
+      <c r="F81" s="57">
         <f t="shared" si="6"/>
         <v>520</v>
       </c>
-      <c r="G80" s="3" t="s">
+      <c r="G81" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H80" s="3" t="s">
+      <c r="H81" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="I80" s="3" t="s">
+      <c r="I81" s="3" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="47" t="s">
+    <row r="82" spans="1:10" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="47" t="s">
         <v>302</v>
       </c>
-      <c r="B81" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="C81" s="46" t="s">
+      <c r="B82" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C82" s="46" t="s">
         <v>276</v>
       </c>
-      <c r="D81" s="45">
+      <c r="D82" s="45">
         <v>0</v>
       </c>
-      <c r="E81" s="65">
+      <c r="E82" s="65">
         <v>390</v>
       </c>
-      <c r="F81" s="66">
+      <c r="F82" s="66">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G81" s="45" t="s">
+      <c r="G82" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="H81" s="45" t="s">
+      <c r="H82" s="45" t="s">
         <v>216</v>
       </c>
-      <c r="I81" s="45" t="s">
+      <c r="I82" s="45" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="27" t="s">
+    <row r="83" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="27" t="s">
         <v>543</v>
       </c>
-      <c r="B82" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C82" s="27" t="s">
+      <c r="B83" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C83" s="27" t="s">
         <v>544</v>
       </c>
-      <c r="D82" s="20">
+      <c r="D83" s="20">
         <v>2</v>
       </c>
-      <c r="E82" s="78">
+      <c r="E83" s="78">
         <v>148</v>
       </c>
-      <c r="F82" s="69">
+      <c r="F83" s="69">
         <f t="shared" si="6"/>
         <v>296</v>
       </c>
-      <c r="G82" s="20" t="s">
+      <c r="G83" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="H82" s="20" t="s">
+      <c r="H83" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="I82" s="20" t="s">
+      <c r="I83" s="20" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="10" t="s">
+    <row r="84" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="10" t="s">
         <v>562</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="C83" s="9" t="s">
+      <c r="C84" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="D83" s="3">
+      <c r="D84" s="3">
         <v>14</v>
       </c>
-      <c r="E83" s="59">
+      <c r="E84" s="59">
         <v>20</v>
       </c>
-      <c r="F83" s="57">
+      <c r="F84" s="57">
         <f t="shared" si="6"/>
         <v>280</v>
       </c>
-      <c r="G83" s="3" t="s">
+      <c r="G84" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H83" s="3" t="s">
+      <c r="H84" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="I83" s="4" t="s">
+      <c r="I84" s="4" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="10" t="s">
+    <row r="85" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="C84" s="9" t="s">
+      <c r="C85" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="D84" s="3">
-        <v>1</v>
-      </c>
-      <c r="E84" s="59">
+      <c r="D85" s="3">
+        <v>1</v>
+      </c>
+      <c r="E85" s="59">
         <v>10</v>
       </c>
-      <c r="F84" s="57">
+      <c r="F85" s="57">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="G84" s="3" t="s">
+      <c r="G85" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H84" s="3" t="s">
+      <c r="H85" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="I84" s="3" t="s">
+      <c r="I85" s="3" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="85" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="5" t="s">
+    <row r="86" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A86" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="E85" s="58"/>
-      <c r="F85" s="58"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D86" s="3">
-        <v>1</v>
-      </c>
-      <c r="E86" s="59"/>
-      <c r="I86" s="3" t="s">
-        <v>243</v>
-      </c>
+      <c r="E86" s="58"/>
+      <c r="F86" s="58"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D87" s="3">
+        <v>1</v>
+      </c>
+      <c r="E87" s="59"/>
+      <c r="I87" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="B87" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C87" s="9" t="s">
+      <c r="B88" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C88" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="D87" s="3">
-        <v>1</v>
-      </c>
-      <c r="E87" s="59">
+      <c r="D88" s="3">
+        <v>1</v>
+      </c>
+      <c r="E88" s="59">
         <v>63</v>
-      </c>
-      <c r="F87" s="57">
-        <f>D87*E87</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="D88" s="3">
-        <v>2</v>
-      </c>
-      <c r="E88" s="59">
-        <v>69</v>
       </c>
       <c r="F88" s="57">
         <f>D88*E88</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D89" s="3">
+        <v>2</v>
+      </c>
+      <c r="E89" s="59">
+        <v>69</v>
+      </c>
+      <c r="F89" s="57">
+        <f>D89*E89</f>
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D89" s="3">
-        <v>1</v>
-      </c>
-      <c r="E89" s="59"/>
-      <c r="I89" s="3" t="s">
+      <c r="D90" s="3">
+        <v>1</v>
+      </c>
+      <c r="E90" s="59"/>
+      <c r="I90" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="90" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="4" t="s">
+    <row r="91" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C91" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="D90" s="4">
-        <v>1</v>
-      </c>
-      <c r="E90" s="62">
-        <v>1</v>
-      </c>
-      <c r="F90" s="60">
-        <v>1</v>
-      </c>
-      <c r="I90" s="4" t="s">
+      <c r="D91" s="4">
+        <v>1</v>
+      </c>
+      <c r="E91" s="62">
+        <v>1</v>
+      </c>
+      <c r="F91" s="60">
+        <v>1</v>
+      </c>
+      <c r="I91" s="4" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="91" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A91" s="5" t="s">
+    <row r="92" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A92" s="5" t="s">
         <v>397</v>
-      </c>
-      <c r="E91" s="58"/>
-      <c r="F91" s="58"/>
-    </row>
-    <row r="92" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
-        <v>398</v>
       </c>
       <c r="E92" s="58"/>
       <c r="F92" s="58"/>
     </row>
-    <row r="93" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="3" t="s">
+    <row r="93" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="E93" s="58"/>
+      <c r="F93" s="58"/>
+    </row>
+    <row r="94" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B94" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="C93" s="53" t="s">
+      <c r="C94" s="53" t="s">
         <v>399</v>
       </c>
-      <c r="D93" s="3">
-        <v>1</v>
-      </c>
-      <c r="E93" s="57">
+      <c r="D94" s="3">
+        <v>1</v>
+      </c>
+      <c r="E94" s="57">
         <v>200</v>
       </c>
-      <c r="F93" s="57">
-        <f>E93*D93</f>
+      <c r="F94" s="57">
+        <f>E94*D94</f>
         <v>200</v>
       </c>
-      <c r="I93" s="3" t="s">
+      <c r="I94" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="J93" s="4"/>
-    </row>
-    <row r="94" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="4" t="s">
+      <c r="J94" s="4"/>
+    </row>
+    <row r="95" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="4" t="s">
         <v>448</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>458</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C95" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <v>5</v>
       </c>
-      <c r="E94" s="60">
-        <v>1</v>
-      </c>
-      <c r="F94" s="60">
-        <f>E94*D94</f>
+      <c r="E95" s="60">
+        <v>1</v>
+      </c>
+      <c r="F95" s="60">
+        <f>E95*D95</f>
         <v>5</v>
       </c>
-      <c r="I94" s="4" t="s">
+      <c r="I95" s="4" t="s">
         <v>404</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="D95" s="3">
-        <v>1</v>
-      </c>
-      <c r="E95" s="57">
-        <v>26</v>
-      </c>
-      <c r="F95" s="57">
-        <f>E95*D95</f>
-        <v>26</v>
-      </c>
-      <c r="I95" s="3" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D96" s="3">
         <v>1</v>
       </c>
       <c r="E96" s="57">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F96" s="57">
         <f>E96*D96</f>
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>457</v>
+        <v>407</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>335</v>
+        <v>408</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>334</v>
+        <v>409</v>
       </c>
       <c r="D97" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E97" s="57">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="F97" s="57">
         <f>E97*D97</f>
+        <v>37</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D98" s="3">
+        <v>2</v>
+      </c>
+      <c r="E98" s="57">
+        <v>24</v>
+      </c>
+      <c r="F98" s="57">
+        <f>E98*D98</f>
         <v>48</v>
       </c>
-      <c r="I97" s="3" t="s">
+      <c r="I98" s="3" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="98" spans="1:9" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="43" t="s">
+    <row r="99" spans="1:9" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="43" t="s">
         <v>165</v>
-      </c>
-      <c r="E98" s="67"/>
-      <c r="F98" s="67"/>
-    </row>
-    <row r="99" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="15" t="s">
-        <v>572</v>
       </c>
       <c r="E99" s="67"/>
       <c r="F99" s="67"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
+    <row r="100" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="15" t="s">
+        <v>572</v>
+      </c>
+      <c r="E100" s="67"/>
+      <c r="F100" s="67"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B101" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="C100" s="3" t="s">
+      <c r="C101" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="D100" s="3">
-        <v>1</v>
-      </c>
-      <c r="E100" s="57">
+      <c r="D101" s="3">
+        <v>1</v>
+      </c>
+      <c r="E101" s="57">
         <v>625</v>
       </c>
-      <c r="F100" s="57">
-        <f>E100*D100</f>
+      <c r="F101" s="57">
+        <f>E101*D101</f>
         <v>625</v>
       </c>
-      <c r="G100" s="3" t="s">
+      <c r="G101" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I100" s="3" t="s">
+      <c r="I101" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="101" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A101" s="17" t="s">
+    <row r="102" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A102" s="17" t="s">
         <v>342</v>
       </c>
-      <c r="E101" s="68"/>
-      <c r="F101" s="68"/>
-    </row>
-    <row r="102" spans="1:9" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="21" t="s">
+      <c r="E102" s="68"/>
+      <c r="F102" s="68"/>
+    </row>
+    <row r="103" spans="1:9" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A103" s="21" t="s">
         <v>476</v>
-      </c>
-      <c r="B102" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="C102" s="72" t="s">
-        <v>477</v>
-      </c>
-      <c r="D102" s="20">
-        <v>1</v>
-      </c>
-      <c r="E102" s="69">
-        <v>900</v>
-      </c>
-      <c r="F102" s="69">
-        <f t="shared" ref="F102:F108" si="9">E102*D102</f>
-        <v>900</v>
-      </c>
-      <c r="G102" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I102" s="20" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A103" s="22" t="s">
-        <v>480</v>
       </c>
       <c r="B103" s="20" t="s">
         <v>315</v>
       </c>
-      <c r="C103" s="73" t="s">
+      <c r="C103" s="72" t="s">
+        <v>477</v>
+      </c>
+      <c r="D103" s="20">
+        <v>1</v>
+      </c>
+      <c r="E103" s="69">
+        <v>900</v>
+      </c>
+      <c r="F103" s="69">
+        <f t="shared" ref="F103:F109" si="9">E103*D103</f>
+        <v>900</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I103" s="20" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A104" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="B104" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="C104" s="73" t="s">
         <v>478</v>
       </c>
-      <c r="D103" s="3">
-        <v>1</v>
-      </c>
-      <c r="E103" s="57">
+      <c r="D104" s="3">
+        <v>1</v>
+      </c>
+      <c r="E104" s="57">
         <v>767</v>
       </c>
-      <c r="F103" s="69">
+      <c r="F104" s="69">
         <f t="shared" si="9"/>
         <v>767</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H103" s="20"/>
-      <c r="I103" s="3" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="22" t="s">
-        <v>481</v>
-      </c>
-      <c r="B104" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="C104" s="73" t="s">
-        <v>479</v>
-      </c>
-      <c r="D104" s="3">
-        <v>0</v>
-      </c>
-      <c r="E104" s="57">
-        <v>1540</v>
-      </c>
-      <c r="F104" s="69">
-        <f t="shared" si="9"/>
-        <v>0</v>
       </c>
       <c r="G104" s="3" t="s">
         <v>13</v>
@@ -5091,24 +5098,24 @@
       </c>
     </row>
     <row r="105" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="3" t="s">
-        <v>483</v>
+      <c r="A105" s="22" t="s">
+        <v>481</v>
       </c>
       <c r="B105" s="20" t="s">
         <v>315</v>
       </c>
       <c r="C105" s="73" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D105" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E105" s="57">
-        <v>877</v>
+        <v>1540</v>
       </c>
       <c r="F105" s="69">
         <f t="shared" si="9"/>
-        <v>877</v>
+        <v>0</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>13</v>
@@ -5120,739 +5127,746 @@
     </row>
     <row r="106" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B106" s="20" t="s">
         <v>315</v>
       </c>
       <c r="C106" s="73" t="s">
-        <v>413</v>
+        <v>482</v>
       </c>
       <c r="D106" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E106" s="57">
-        <v>4700</v>
+        <v>877</v>
       </c>
       <c r="F106" s="69">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>877</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H106" s="20"/>
       <c r="I106" s="3" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B107" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>488</v>
+        <v>315</v>
+      </c>
+      <c r="C107" s="73" t="s">
+        <v>413</v>
       </c>
       <c r="D107" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E107" s="57">
-        <v>20</v>
+        <v>4700</v>
       </c>
       <c r="F107" s="69">
         <f t="shared" si="9"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H107" s="20"/>
       <c r="I107" s="3" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B108" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C108" s="28" t="s">
-        <v>490</v>
+      <c r="C108" s="3" t="s">
+        <v>488</v>
       </c>
       <c r="D108" s="3">
         <v>1</v>
       </c>
       <c r="E108" s="57">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F108" s="69">
         <f t="shared" si="9"/>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H108" s="20"/>
       <c r="I108" s="3" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C109" s="28" t="s">
+        <v>490</v>
+      </c>
+      <c r="D109" s="3">
+        <v>1</v>
+      </c>
+      <c r="E109" s="57">
+        <v>25</v>
+      </c>
+      <c r="F109" s="69">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H109" s="20"/>
+      <c r="I109" s="3" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="109" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A109" s="17" t="s">
+    <row r="110" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A110" s="17" t="s">
         <v>343</v>
       </c>
-      <c r="E109" s="68"/>
-      <c r="F109" s="68"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
+      <c r="E110" s="68"/>
+      <c r="F110" s="68"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="B110" s="20" t="s">
+      <c r="B111" s="20" t="s">
         <v>315</v>
       </c>
-      <c r="C110" s="54" t="s">
+      <c r="C111" s="54" t="s">
         <v>345</v>
       </c>
-      <c r="D110" s="3">
-        <v>1</v>
-      </c>
-      <c r="E110" s="57">
+      <c r="D111" s="3">
+        <v>1</v>
+      </c>
+      <c r="E111" s="57">
         <v>752</v>
       </c>
-      <c r="F110" s="57">
-        <f t="shared" ref="F110:F115" si="10">D110*E110</f>
+      <c r="F111" s="57">
+        <f t="shared" ref="F111:F116" si="10">D111*E111</f>
         <v>752</v>
       </c>
-      <c r="G110" s="3" t="s">
+      <c r="G111" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I110" s="3" t="s">
+      <c r="I111" s="3" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="111" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="4" t="s">
+    <row r="112" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="B111" s="50" t="s">
+      <c r="B112" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="C112" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="D111" s="4">
-        <v>1</v>
-      </c>
-      <c r="E111" s="60">
-        <v>1</v>
-      </c>
-      <c r="F111" s="60">
+      <c r="D112" s="4">
+        <v>1</v>
+      </c>
+      <c r="E112" s="60">
+        <v>1</v>
+      </c>
+      <c r="F112" s="60">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="G111" s="4" t="s">
+      <c r="G112" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I111" s="4" t="s">
+      <c r="I112" s="4" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B112" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C112" s="3" t="s">
+      <c r="B113" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="D112" s="3">
-        <v>1</v>
-      </c>
-      <c r="E112" s="57">
+      <c r="D113" s="3">
+        <v>1</v>
+      </c>
+      <c r="E113" s="57">
         <v>65</v>
       </c>
-      <c r="F112" s="57">
+      <c r="F113" s="57">
         <f t="shared" si="10"/>
         <v>65</v>
       </c>
-      <c r="G112" s="3" t="s">
+      <c r="G113" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I112" s="3" t="s">
+      <c r="I113" s="3" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="B113" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C113" s="3" t="s">
+      <c r="B114" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="D113" s="3">
-        <v>1</v>
-      </c>
-      <c r="E113" s="57">
+      <c r="D114" s="3">
+        <v>1</v>
+      </c>
+      <c r="E114" s="57">
         <v>32</v>
       </c>
-      <c r="F113" s="57">
+      <c r="F114" s="57">
         <f t="shared" si="10"/>
         <v>32</v>
       </c>
-      <c r="G113" s="3" t="s">
+      <c r="G114" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I113" s="3" t="s">
+      <c r="I114" s="3" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="B114" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C114" s="3" t="s">
+      <c r="B115" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="D114" s="3">
-        <v>1</v>
-      </c>
-      <c r="E114" s="57">
+      <c r="D115" s="3">
+        <v>1</v>
+      </c>
+      <c r="E115" s="57">
         <v>112</v>
       </c>
-      <c r="F114" s="57">
+      <c r="F115" s="57">
         <f t="shared" si="10"/>
         <v>112</v>
       </c>
-      <c r="G114" s="3" t="s">
+      <c r="G115" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I114" s="3" t="s">
+      <c r="I115" s="3" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="115" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="4" t="s">
+    <row r="116" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="B115" s="50" t="s">
+      <c r="B116" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="C115" s="4" t="s">
+      <c r="C116" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="D115" s="4">
-        <v>1</v>
-      </c>
-      <c r="E115" s="60">
+      <c r="D116" s="4">
+        <v>1</v>
+      </c>
+      <c r="E116" s="60">
         <v>2</v>
       </c>
-      <c r="F115" s="60">
+      <c r="F116" s="60">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="G115" s="4" t="s">
+      <c r="G116" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I115" s="4" t="s">
+      <c r="I116" s="4" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="116" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A116" s="5" t="s">
+    <row r="117" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A117" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E116" s="58"/>
-      <c r="F116" s="58"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D117" s="3">
-        <v>1</v>
-      </c>
-      <c r="E117" s="57">
-        <v>3582</v>
-      </c>
-      <c r="F117" s="57">
-        <f t="shared" ref="F117:F129" si="11">E117*D117</f>
-        <v>3582</v>
-      </c>
-      <c r="G117" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I117" s="3" t="s">
-        <v>475</v>
-      </c>
+      <c r="E117" s="58"/>
+      <c r="F117" s="58"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>177</v>
+        <v>55</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C118" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D118" s="3">
+        <v>1</v>
+      </c>
+      <c r="E118" s="57">
+        <v>3582</v>
+      </c>
+      <c r="F118" s="57">
+        <f t="shared" ref="F118:F130" si="11">E118*D118</f>
+        <v>3582</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C119" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D118" s="3">
-        <v>1</v>
-      </c>
-      <c r="E118" s="57">
+      <c r="D119" s="3">
+        <v>1</v>
+      </c>
+      <c r="E119" s="57">
         <v>1630</v>
       </c>
-      <c r="F118" s="57">
+      <c r="F119" s="57">
         <f t="shared" si="11"/>
         <v>1630</v>
       </c>
-      <c r="G118" s="3" t="s">
+      <c r="G119" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I118" s="3" t="s">
+      <c r="I119" s="3" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B120" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C120" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="D119" s="3">
-        <v>1</v>
-      </c>
-      <c r="E119" s="57">
+      <c r="D120" s="3">
+        <v>1</v>
+      </c>
+      <c r="E120" s="57">
         <v>900</v>
       </c>
-      <c r="F119" s="57">
+      <c r="F120" s="57">
         <f t="shared" si="11"/>
         <v>900</v>
       </c>
-      <c r="G119" s="3" t="s">
+      <c r="G120" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I119" s="3" t="s">
+      <c r="I120" s="3" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B121" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C120" s="3" t="s">
+      <c r="C121" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D120" s="3">
-        <v>1</v>
-      </c>
-      <c r="E120" s="57">
+      <c r="D121" s="3">
+        <v>1</v>
+      </c>
+      <c r="E121" s="57">
         <v>163</v>
       </c>
-      <c r="F120" s="57">
+      <c r="F121" s="57">
         <f t="shared" si="11"/>
         <v>163</v>
       </c>
-      <c r="G120" s="3" t="s">
+      <c r="G121" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I120" s="3" t="s">
+      <c r="I121" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B122" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C121" s="3" t="s">
+      <c r="C122" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D121" s="3">
-        <v>1</v>
-      </c>
-      <c r="E121" s="57">
+      <c r="D122" s="3">
+        <v>1</v>
+      </c>
+      <c r="E122" s="57">
         <v>11</v>
       </c>
-      <c r="F121" s="57">
+      <c r="F122" s="57">
         <f t="shared" si="11"/>
         <v>11</v>
       </c>
-      <c r="G121" s="3" t="s">
+      <c r="G122" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="3" t="s">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B123" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C122" s="3" t="s">
+      <c r="C123" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D122" s="3">
-        <v>1</v>
-      </c>
-      <c r="E122" s="57">
+      <c r="D123" s="3">
+        <v>1</v>
+      </c>
+      <c r="E123" s="57">
         <v>520</v>
       </c>
-      <c r="F122" s="57">
+      <c r="F123" s="57">
         <f t="shared" si="11"/>
         <v>520</v>
       </c>
-      <c r="G122" s="3" t="s">
+      <c r="G123" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B124" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C123" s="3" t="s">
+      <c r="C124" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D123" s="3">
-        <v>1</v>
-      </c>
-      <c r="E123" s="57">
+      <c r="D124" s="3">
+        <v>1</v>
+      </c>
+      <c r="E124" s="57">
         <v>193</v>
       </c>
-      <c r="F123" s="57">
+      <c r="F124" s="57">
         <f t="shared" si="11"/>
         <v>193</v>
       </c>
-      <c r="G123" s="3" t="s">
+      <c r="G124" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B124" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C124" s="3" t="s">
+      <c r="B125" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D124" s="3">
+      <c r="D125" s="3">
         <v>10</v>
       </c>
-      <c r="E124" s="57">
+      <c r="E125" s="57">
         <v>12</v>
       </c>
-      <c r="F124" s="57">
+      <c r="F125" s="57">
         <f t="shared" si="11"/>
         <v>120</v>
       </c>
-      <c r="G124" s="3" t="s">
+      <c r="G125" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I124" s="3" t="s">
+      <c r="I125" s="3" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="3" t="s">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B125" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C125" s="3" t="s">
+      <c r="B126" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C126" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="D125" s="3">
-        <v>1</v>
-      </c>
-      <c r="E125" s="57">
+      <c r="D126" s="3">
+        <v>1</v>
+      </c>
+      <c r="E126" s="57">
         <v>14</v>
       </c>
-      <c r="F125" s="57">
+      <c r="F126" s="57">
         <f t="shared" si="11"/>
         <v>14</v>
       </c>
-      <c r="G125" s="3" t="s">
+      <c r="G126" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I125" s="3" t="s">
+      <c r="I126" s="3" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="s">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B126" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C126" s="3" t="s">
+      <c r="B127" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C127" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D126" s="3">
+      <c r="D127" s="3">
         <v>4</v>
       </c>
-      <c r="E126" s="57">
+      <c r="E127" s="57">
         <v>15.25</v>
       </c>
-      <c r="F126" s="57">
+      <c r="F127" s="57">
         <f t="shared" si="11"/>
         <v>61</v>
       </c>
-      <c r="G126" s="3" t="s">
+      <c r="G127" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="3" t="s">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B127" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C127" s="3" t="s">
+      <c r="B128" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C128" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D127" s="3">
+      <c r="D128" s="3">
         <v>10</v>
       </c>
-      <c r="E127" s="57">
+      <c r="E128" s="57">
         <v>16.5</v>
       </c>
-      <c r="F127" s="57">
+      <c r="F128" s="57">
         <f t="shared" si="11"/>
         <v>165</v>
       </c>
-      <c r="G127" s="3" t="s">
+      <c r="G128" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" s="3" t="s">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B128" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C128" s="3" t="s">
+      <c r="B129" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D128" s="3">
+      <c r="D129" s="3">
         <v>10</v>
       </c>
-      <c r="E128" s="57">
+      <c r="E129" s="57">
         <v>24</v>
       </c>
-      <c r="F128" s="57">
+      <c r="F129" s="57">
         <f t="shared" si="11"/>
         <v>240</v>
       </c>
-      <c r="G128" s="3" t="s">
+      <c r="G129" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="s">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B129" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C129" s="3" t="s">
+      <c r="B130" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C130" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D129" s="3">
+      <c r="D130" s="3">
         <v>6</v>
       </c>
-      <c r="E129" s="57">
+      <c r="E130" s="57">
         <v>24</v>
       </c>
-      <c r="F129" s="57">
+      <c r="F130" s="57">
         <f t="shared" si="11"/>
         <v>144</v>
       </c>
-      <c r="G129" s="3" t="s">
+      <c r="G130" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A132" s="10"/>
-      <c r="B132" s="10"/>
-      <c r="C132" s="9"/>
-    </row>
-    <row r="133" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A133" s="7" t="s">
+    <row r="133" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A133" s="10"/>
+      <c r="B133" s="10"/>
+      <c r="C133" s="9"/>
+    </row>
+    <row r="134" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A134" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E133" s="58"/>
-      <c r="F133" s="58"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D134" s="3">
-        <v>4</v>
-      </c>
-      <c r="E134" s="57">
-        <v>16.5</v>
-      </c>
-      <c r="F134" s="57">
-        <f t="shared" ref="F134:F149" si="12">E134*D134</f>
-        <v>66</v>
-      </c>
-      <c r="I134" s="3" t="s">
-        <v>114</v>
-      </c>
+      <c r="E134" s="58"/>
+      <c r="F134" s="58"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D135" s="3">
+        <v>4</v>
+      </c>
+      <c r="E135" s="57">
+        <v>16.5</v>
+      </c>
+      <c r="F135" s="57">
+        <f t="shared" ref="F135:F150" si="12">E135*D135</f>
+        <v>66</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B135" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C135" s="3" t="s">
+      <c r="B136" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C136" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D135" s="3">
-        <v>1</v>
-      </c>
-      <c r="E135" s="57">
+      <c r="D136" s="3">
+        <v>1</v>
+      </c>
+      <c r="E136" s="57">
         <v>85.1</v>
       </c>
-      <c r="F135" s="57">
+      <c r="F136" s="57">
         <f t="shared" si="12"/>
         <v>85.1</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" s="3" t="s">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B136" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C136" s="3" t="s">
+      <c r="B137" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C137" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D136" s="3">
+      <c r="D137" s="3">
         <v>2</v>
       </c>
-      <c r="E136" s="57">
+      <c r="E137" s="57">
         <v>32</v>
       </c>
-      <c r="F136" s="57">
+      <c r="F137" s="57">
         <f t="shared" si="12"/>
         <v>64</v>
       </c>
-      <c r="I136" s="3" t="s">
+      <c r="I137" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B137" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C137" s="3" t="s">
+      <c r="B138" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C138" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D137" s="3">
+      <c r="D138" s="3">
         <v>2</v>
       </c>
-      <c r="E137" s="57">
+      <c r="E138" s="57">
         <v>51.58</v>
       </c>
-      <c r="F137" s="57">
+      <c r="F138" s="57">
         <f t="shared" si="12"/>
         <v>103.16</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="3" t="s">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B138" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C138" s="3" t="s">
+      <c r="B139" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C139" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D138" s="3">
-        <v>1</v>
-      </c>
-      <c r="E138" s="57">
+      <c r="D139" s="3">
+        <v>1</v>
+      </c>
+      <c r="E139" s="57">
         <v>60</v>
       </c>
-      <c r="F138" s="57">
+      <c r="F139" s="57">
         <f t="shared" si="12"/>
         <v>60</v>
       </c>
-      <c r="I138" s="3" t="s">
+      <c r="I139" s="3" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A139" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D139" s="3">
-        <v>1</v>
-      </c>
-      <c r="E139" s="57">
-        <v>136.47999999999999</v>
-      </c>
-      <c r="F139" s="57">
-        <f t="shared" si="12"/>
-        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -5863,7 +5877,7 @@
         <v>59</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D140" s="3">
         <v>1</v>
@@ -5878,296 +5892,296 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D141" s="3">
         <v>1</v>
       </c>
       <c r="E141" s="57">
-        <v>60.95</v>
+        <v>136.47999999999999</v>
       </c>
       <c r="F141" s="57">
         <f t="shared" si="12"/>
-        <v>60.95</v>
+        <v>136.47999999999999</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D142" s="3">
         <v>1</v>
       </c>
       <c r="E142" s="57">
-        <v>119.416</v>
+        <v>60.95</v>
       </c>
       <c r="F142" s="57">
         <f t="shared" si="12"/>
-        <v>119.416</v>
+        <v>60.95</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D143" s="3">
         <v>1</v>
       </c>
       <c r="E143" s="57">
-        <v>105.8</v>
+        <v>119.416</v>
       </c>
       <c r="F143" s="57">
         <f t="shared" si="12"/>
-        <v>105.8</v>
+        <v>119.416</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D144" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E144" s="57">
-        <v>119.6</v>
+        <v>105.8</v>
       </c>
       <c r="F144" s="57">
         <f t="shared" si="12"/>
-        <v>239.2</v>
+        <v>105.8</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>293</v>
+        <v>144</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>294</v>
+        <v>145</v>
       </c>
       <c r="D145" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E145" s="57">
-        <v>100</v>
+        <v>119.6</v>
       </c>
       <c r="F145" s="57">
         <f t="shared" si="12"/>
-        <v>100</v>
+        <v>239.2</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>146</v>
+        <v>293</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>147</v>
+        <v>294</v>
       </c>
       <c r="D146" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E146" s="57">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F146" s="57">
         <f t="shared" si="12"/>
-        <v>184</v>
+        <v>100</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D147" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E147" s="57">
-        <v>96.23</v>
+        <v>92</v>
       </c>
       <c r="F147" s="57">
         <f t="shared" si="12"/>
-        <v>96.23</v>
+        <v>184</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D148" s="3">
         <v>1</v>
       </c>
       <c r="E148" s="57">
-        <v>102.44</v>
+        <v>96.23</v>
       </c>
       <c r="F148" s="57">
         <f t="shared" si="12"/>
-        <v>102.44</v>
+        <v>96.23</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D149" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E149" s="57">
-        <v>28</v>
+        <v>102.44</v>
       </c>
       <c r="F149" s="57">
         <f t="shared" si="12"/>
+        <v>102.44</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D150" s="3">
+        <v>2</v>
+      </c>
+      <c r="E150" s="57">
+        <v>28</v>
+      </c>
+      <c r="F150" s="57">
+        <f t="shared" si="12"/>
         <v>56</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C150" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D150" s="3">
-        <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C151" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D151" s="3">
-        <v>1</v>
-      </c>
-      <c r="I151" s="3" t="s">
-        <v>156</v>
+        <v>4</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C152" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D152" s="3">
+        <v>1</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C153" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D152" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A154" s="7" t="s">
+      <c r="D153" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A155" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B154" s="6" t="s">
+      <c r="B155" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="E154" s="58"/>
-      <c r="F154" s="58"/>
-    </row>
-    <row r="155" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="3"/>
-      <c r="B155" s="3" t="s">
+      <c r="E155" s="58"/>
+      <c r="F155" s="58"/>
+    </row>
+    <row r="156" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="3"/>
+      <c r="B156" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="C155" s="20" t="s">
+      <c r="C156" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="D155" s="3">
+      <c r="D156" s="3">
         <v>4</v>
       </c>
-      <c r="E155" s="57">
+      <c r="E156" s="57">
         <v>40</v>
-      </c>
-      <c r="F155" s="57">
-        <f>E155*D155</f>
-        <v>160</v>
-      </c>
-      <c r="G155" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="H155" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="I155" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="J155" s="20"/>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B156" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C156" s="3" t="s">
-        <v>558</v>
-      </c>
-      <c r="D156" s="3">
-        <v>2</v>
-      </c>
-      <c r="E156" s="57">
-        <v>515</v>
       </c>
       <c r="F156" s="57">
         <f>E156*D156</f>
-        <v>1030</v>
+        <v>160</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>429</v>
-      </c>
+        <v>426</v>
+      </c>
+      <c r="H156" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="I156" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="J156" s="20"/>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B157" s="3" t="s">
         <v>160</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>280</v>
+        <v>558</v>
       </c>
       <c r="D157" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E157" s="57">
-        <v>25</v>
+        <v>515</v>
       </c>
       <c r="F157" s="57">
         <f>E157*D157</f>
-        <v>100</v>
+        <v>1030</v>
       </c>
       <c r="G157" s="3" t="s">
         <v>429</v>
@@ -6178,17 +6192,17 @@
         <v>160</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D158" s="3">
         <v>4</v>
       </c>
       <c r="E158" s="57">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F158" s="57">
         <f>E158*D158</f>
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G158" s="3" t="s">
         <v>429</v>
@@ -6199,224 +6213,245 @@
         <v>160</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D159" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E159" s="57">
-        <v>121.5</v>
+        <v>28</v>
       </c>
       <c r="F159" s="57">
         <f>E159*D159</f>
-        <v>729</v>
+        <v>112</v>
       </c>
       <c r="G159" s="3" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E162" s="52" t="s">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B160" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D160" s="3">
+        <v>6</v>
+      </c>
+      <c r="E160" s="57">
+        <v>121.5</v>
+      </c>
+      <c r="F160" s="57">
+        <f>E160*D160</f>
+        <v>729</v>
+      </c>
+      <c r="G160" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E163" s="52" t="s">
         <v>456</v>
       </c>
-      <c r="F162" s="52">
-        <f>SUM(F3:F160)</f>
-        <v>96394.501499199992</v>
-      </c>
-      <c r="G162" s="3" t="s">
+      <c r="F163" s="52">
+        <f>SUM(F3:F161)</f>
+        <v>96427.501499199992</v>
+      </c>
+      <c r="G163" s="3" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A166" s="51" t="s">
+    <row r="167" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A167" s="51" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A167" s="4" t="s">
+    <row r="168" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A168" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="B168" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="C167" s="4" t="s">
+      <c r="C168" s="4" t="s">
         <v>432</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="B168" s="3">
-        <v>14</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B169" s="3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B170" s="3">
         <v>2</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B171" s="3">
         <v>2</v>
       </c>
       <c r="C171" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="B172" s="3">
+        <v>2</v>
+      </c>
+      <c r="C172" s="3" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A174" s="51" t="s">
+    <row r="175" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A175" s="51" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A175" s="4" t="s">
+    <row r="176" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A176" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="B175" s="4" t="s">
+      <c r="B176" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="C175" s="4" t="s">
+      <c r="C176" s="4" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A176" s="3" t="s">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="B176" s="3">
+      <c r="B177" s="3">
         <v>2</v>
       </c>
-      <c r="C176" s="3" t="s">
+      <c r="C177" s="3" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A177" s="3" t="s">
+    <row r="178" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A178" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="B177" s="3">
+      <c r="B178" s="3">
         <v>5</v>
       </c>
-      <c r="C177" s="3" t="s">
+      <c r="C178" s="3" t="s">
         <v>451</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="B178" s="3">
-        <v>1</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>538</v>
+        <v>347</v>
       </c>
       <c r="B179" s="3">
         <v>1</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>540</v>
+        <v>452</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="B180" s="3">
+        <v>1</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="3" t="s">
         <v>541</v>
       </c>
-      <c r="B180" s="3">
-        <v>1</v>
-      </c>
-      <c r="C180" s="3" t="s">
+      <c r="B181" s="3">
+        <v>1</v>
+      </c>
+      <c r="C181" s="3" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A182" s="51" t="s">
+    <row r="183" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A183" s="51" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A183" s="4" t="s">
+    <row r="184" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A184" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="B184" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="C183" s="4" t="s">
+      <c r="C184" s="4" t="s">
         <v>432</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="B184" s="3">
-        <v>5</v>
-      </c>
-      <c r="C184" s="3" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>158</v>
+        <v>448</v>
       </c>
       <c r="B185" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B186" s="3">
+        <v>3</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="B186" s="3" t="s">
+      <c r="B187" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C186" s="3" t="s">
+      <c r="C187" s="3" t="s">
         <v>455</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C102" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C103" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C104" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C105" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C110" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C93" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C106" r:id="rId7" xr:uid="{3002EF90-377A-4FAD-A836-B22D0D243A96}"/>
+    <hyperlink ref="C103" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C104" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C105" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C106" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C111" r:id="rId5" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C94" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C107" r:id="rId7" xr:uid="{3002EF90-377A-4FAD-A836-B22D0D243A96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>

</xml_diff>

<commit_message>
update to smaller-diameter sorbothane feet (AV4/M)
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDD7649-C414-486F-858D-B26994D78468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA47E053-F848-47D7-995F-8953060D519C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5244" yWindow="4884" windowWidth="27516" windowHeight="16824" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1825,13 +1825,13 @@
     <t>QuadLine Emission ZET405/488/561/640m, in 25 mm diameter</t>
   </si>
   <si>
-    <t>AV6/M</t>
-  </si>
-  <si>
     <t>Ø45.0 mm Sorbothane Feet, Internal M6 Mounting Thread, 4 Pieces</t>
   </si>
   <si>
-    <t>Attached to the bottom of the PBG52522 Breadboard</t>
+    <t>AV4/M</t>
+  </si>
+  <si>
+    <t>Attached to the bottom of the PBG52522 Breadboard. Based on Benchtop weight 25 kg on breadboard (including BB).</t>
   </si>
 </sst>
 </file>
@@ -2588,7 +2588,7 @@
   <dimension ref="A1:J187"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3369,13 +3369,13 @@
     </row>
     <row r="39" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="77" t="s">
+        <v>576</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="41" t="s">
         <v>575</v>
-      </c>
-      <c r="B39" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="41" t="s">
-        <v>576</v>
       </c>
       <c r="D39" s="41">
         <v>1</v>

</xml_diff>

<commit_message>
add interferometer and oscilloscope
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753D2A68-E29D-4F6E-B4DE-376E2A420FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D033BF81-6D37-44DE-8F17-462795583352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5952" yWindow="5628" windowWidth="32148" windowHeight="16824" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4932" yWindow="3468" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="592">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -363,9 +363,6 @@
   </si>
   <si>
     <t>Thread adapter female M8/ male M6 thread reduction for Fisso</t>
-  </si>
-  <si>
-    <t>General lab supplies</t>
   </si>
   <si>
     <t>LAB-16</t>
@@ -1832,6 +1829,51 @@
   </si>
   <si>
     <t>All stage parts above offered by ASI (Jon Daniels &lt;jon@asiimaging.com&gt;)</t>
+  </si>
+  <si>
+    <t>General lab and optics supplies</t>
+  </si>
+  <si>
+    <t>Shearing Interferometer with a 10-25.4 mm Beam Diameter Shear Plate</t>
+  </si>
+  <si>
+    <t>30 mm Cage System Adapter for Shearing Interferometers with Diffuser Viewing Screen</t>
+  </si>
+  <si>
+    <t>accessory</t>
+  </si>
+  <si>
+    <t>SM1 (1.035"-40) Coupler, External Threads, 0.5" Long, Two Locking Rings</t>
+  </si>
+  <si>
+    <t>Interferometer for beam collimation</t>
+  </si>
+  <si>
+    <t>30 mm Cage Alignment Plate with Ø0.9 mm Hole</t>
+  </si>
+  <si>
+    <t>60 mm Cage Alignment Plate with Ø1 mm Hole</t>
+  </si>
+  <si>
+    <t>Beam alignment</t>
+  </si>
+  <si>
+    <t>60 mm Cage Fluorescent Alignment Plate, Ø1 mm Hole, Orange</t>
+  </si>
+  <si>
+    <t>LCPA2</t>
+  </si>
+  <si>
+    <t>Basic 2-ch oscilloscope for signal troubleshooting</t>
+  </si>
+  <si>
+    <t>Tektronix</t>
+  </si>
+  <si>
+    <t>2 Channel Digital Storage Oscilloscope</t>
+  </si>
+  <si>
+    <t>TBS1000C</t>
   </si>
 </sst>
 </file>
@@ -2585,10 +2627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J187"/>
+  <dimension ref="A1:J196"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2608,7 +2650,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E1" s="71"/>
       <c r="F1" s="71"/>
@@ -2627,10 +2669,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -2670,10 +2712,10 @@
         <v>12350</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2684,24 +2726,24 @@
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E6" s="58"/>
       <c r="F6" s="58"/>
     </row>
     <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E7" s="58"/>
       <c r="F7" s="58"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
@@ -2717,7 +2759,7 @@
         <v>38</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2735,7 +2777,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D10" s="29">
         <v>0</v>
@@ -2748,10 +2790,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2775,10 +2817,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2802,7 +2844,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H12" s="29" t="s">
         <v>13</v>
@@ -2810,13 +2852,13 @@
     </row>
     <row r="13" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D13" s="29">
         <v>1</v>
@@ -2829,10 +2871,10 @@
         <v>160</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2856,13 +2898,13 @@
         <v>0</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H14" s="29" t="s">
         <v>13</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2886,10 +2928,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I15" s="29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2913,21 +2955,21 @@
         <v>0</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I16" s="29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D17" s="29">
         <v>0</v>
@@ -2940,10 +2982,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I17" s="29" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2967,10 +3009,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="I18" s="29" t="s">
         <v>231</v>
-      </c>
-      <c r="I18" s="29" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2994,21 +3036,21 @@
         <v>0</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -3021,7 +3063,7 @@
         <v>19965</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -3038,7 +3080,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D22" s="29">
         <v>0</v>
@@ -3051,10 +3093,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -3078,21 +3120,21 @@
         <v>0</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -3105,7 +3147,7 @@
         <v>6900</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3114,13 +3156,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>459</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>460</v>
       </c>
       <c r="D26" s="3">
         <v>4</v>
@@ -3133,28 +3175,28 @@
         <v>108</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E27" s="58"/>
       <c r="F27" s="58"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="D28" s="3">
         <v>2</v>
@@ -3167,21 +3209,21 @@
         <v>140</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>248</v>
       </c>
       <c r="D29" s="3">
         <v>6</v>
@@ -3194,21 +3236,21 @@
         <v>216</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -3221,21 +3263,21 @@
         <v>43</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>255</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
@@ -3248,21 +3290,21 @@
         <v>29</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="C32" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
@@ -3275,21 +3317,21 @@
         <v>195</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D33" s="3">
         <v>1</v>
@@ -3302,7 +3344,7 @@
         <v>10</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="12" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3314,20 +3356,20 @@
     </row>
     <row r="35" spans="1:9" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E35" s="61"/>
       <c r="F35" s="61"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C36" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D36" s="3">
         <v>1</v>
       </c>
       <c r="E36" s="57" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F36" s="57">
         <v>0</v>
@@ -3335,20 +3377,20 @@
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E37" s="58"/>
       <c r="F37" s="58"/>
     </row>
     <row r="38" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="77" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B38" s="41" t="s">
         <v>59</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D38" s="41">
         <v>1</v>
@@ -3361,21 +3403,21 @@
         <v>728</v>
       </c>
       <c r="G38" s="41" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I38" s="41" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="77" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B39" s="41" t="s">
         <v>59</v>
       </c>
       <c r="C39" s="41" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D39" s="41">
         <v>1</v>
@@ -3387,10 +3429,10 @@
         <v>33</v>
       </c>
       <c r="G39" s="41" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I39" s="41" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3401,7 +3443,7 @@
         <v>59</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D40" s="3">
         <v>2</v>
@@ -3417,21 +3459,21 @@
         <v>38</v>
       </c>
       <c r="H40" s="79" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>191</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>192</v>
       </c>
       <c r="D41" s="3">
         <v>2</v>
@@ -3447,10 +3489,10 @@
         <v>38</v>
       </c>
       <c r="H41" s="79" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3477,21 +3519,21 @@
         <v>38</v>
       </c>
       <c r="H42" s="79" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>547</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>548</v>
       </c>
       <c r="D43" s="3">
         <v>2</v>
@@ -3507,21 +3549,21 @@
         <v>38</v>
       </c>
       <c r="H43" s="79" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>549</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>550</v>
       </c>
       <c r="D44" s="3">
         <v>2</v>
@@ -3537,21 +3579,21 @@
         <v>38</v>
       </c>
       <c r="H44" s="79" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D45" s="3">
         <v>2</v>
@@ -3567,21 +3609,21 @@
         <v>38</v>
       </c>
       <c r="H45" s="79" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D46" s="3">
         <v>2</v>
@@ -3596,7 +3638,7 @@
         <v>38</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3604,10 +3646,10 @@
         <v>37</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D47" s="3">
         <v>2</v>
@@ -3631,7 +3673,7 @@
         <v>40</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>41</v>
@@ -3653,15 +3695,15 @@
         <v>39</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>44</v>
@@ -3690,7 +3732,7 @@
         <v>42</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>43</v>
@@ -3714,13 +3756,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D51" s="3">
         <v>2</v>
@@ -3736,7 +3778,7 @@
         <v>38</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3763,21 +3805,21 @@
         <v>38</v>
       </c>
       <c r="H52" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="I52" s="3" t="s">
         <v>498</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>200</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>201</v>
       </c>
       <c r="D53" s="3">
         <v>2</v>
@@ -3793,18 +3835,18 @@
         <v>38</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>195</v>
       </c>
       <c r="D54" s="3">
         <v>4</v>
@@ -3820,21 +3862,21 @@
         <v>38</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>197</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>198</v>
       </c>
       <c r="D55" s="3">
         <v>4</v>
@@ -3850,21 +3892,21 @@
         <v>38</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>187</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>188</v>
       </c>
       <c r="D56" s="3">
         <v>8</v>
@@ -3880,10 +3922,10 @@
         <v>38</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -3894,7 +3936,7 @@
         <v>59</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D57" s="3">
         <v>4</v>
@@ -3910,21 +3952,21 @@
         <v>38</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D58" s="3">
         <v>2</v>
@@ -3940,21 +3982,21 @@
         <v>38</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>511</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>512</v>
       </c>
       <c r="D59" s="3">
         <v>2</v>
@@ -3970,21 +4012,21 @@
         <v>38</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
+        <v>512</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>513</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>514</v>
       </c>
       <c r="D60" s="3">
         <v>4</v>
@@ -4000,21 +4042,21 @@
         <v>38</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D61" s="3">
         <v>4</v>
@@ -4030,10 +4072,10 @@
         <v>38</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4041,7 +4083,7 @@
         <v>91863</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>46</v>
@@ -4060,21 +4102,21 @@
         <v>38</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C63" s="50" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D63" s="4">
         <v>2</v>
@@ -4090,21 +4132,21 @@
         <v>38</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="46" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B64" s="45" t="s">
         <v>59</v>
       </c>
       <c r="C64" s="46" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D64" s="45">
         <v>0</v>
@@ -4120,22 +4162,22 @@
         <v>38</v>
       </c>
       <c r="H64" s="45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I64" s="45" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="J64" s="75"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D65" s="3">
         <v>2</v>
@@ -4151,21 +4193,21 @@
         <v>38</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C66" s="74" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D66" s="4">
         <v>2</v>
@@ -4181,21 +4223,21 @@
         <v>38</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D67" s="3">
         <v>4</v>
@@ -4211,21 +4253,21 @@
         <v>38</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>208</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>209</v>
       </c>
       <c r="D68" s="3">
         <v>2</v>
@@ -4241,18 +4283,18 @@
         <v>38</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>206</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>207</v>
       </c>
       <c r="D69" s="3">
         <v>4</v>
@@ -4268,21 +4310,21 @@
         <v>38</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>505</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>506</v>
       </c>
       <c r="D70" s="3">
         <v>2</v>
@@ -4298,18 +4340,18 @@
         <v>38</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>203</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>204</v>
       </c>
       <c r="D71" s="3">
         <v>2</v>
@@ -4325,21 +4367,21 @@
         <v>38</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="23" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D72" s="24">
         <v>2</v>
@@ -4355,21 +4397,21 @@
         <v>38</v>
       </c>
       <c r="H72" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="80" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="48" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C73" s="48" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D73" s="80">
         <v>2</v>
@@ -4385,21 +4427,21 @@
         <v>38</v>
       </c>
       <c r="H73" s="80" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I73" s="80" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C74" s="23" t="s">
         <v>211</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C74" s="23" t="s">
-        <v>212</v>
       </c>
       <c r="D74" s="24">
         <v>2</v>
@@ -4415,21 +4457,21 @@
         <v>38</v>
       </c>
       <c r="H74" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I74" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D75" s="4">
         <v>2</v>
@@ -4445,21 +4487,21 @@
         <v>38</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="46" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B76" s="45" t="s">
         <v>59</v>
       </c>
       <c r="C76" s="46" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D76" s="45">
         <v>0</v>
@@ -4475,21 +4517,21 @@
         <v>38</v>
       </c>
       <c r="H76" s="45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I76" s="45" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
+        <v>527</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>528</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>529</v>
       </c>
       <c r="D77" s="3">
         <v>2</v>
@@ -4505,21 +4547,21 @@
         <v>38</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D78" s="3">
         <v>2</v>
@@ -4535,21 +4577,21 @@
         <v>38</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>273</v>
       </c>
       <c r="D79" s="3">
         <v>2</v>
@@ -4565,21 +4607,21 @@
         <v>38</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>274</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>275</v>
       </c>
       <c r="D80" s="3">
         <v>2</v>
@@ -4595,21 +4637,21 @@
         <v>38</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="27" t="s">
+        <v>438</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>439</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>440</v>
       </c>
       <c r="D81" s="3">
         <v>1</v>
@@ -4625,21 +4667,21 @@
         <v>38</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="82" spans="1:10" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B82" s="45" t="s">
         <v>59</v>
       </c>
       <c r="C82" s="46" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D82" s="45">
         <v>0</v>
@@ -4655,21 +4697,21 @@
         <v>38</v>
       </c>
       <c r="H82" s="45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I82" s="45" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="83" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="27" t="s">
+        <v>541</v>
+      </c>
+      <c r="B83" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C83" s="27" t="s">
         <v>542</v>
-      </c>
-      <c r="B83" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C83" s="27" t="s">
-        <v>543</v>
       </c>
       <c r="D83" s="20">
         <v>2</v>
@@ -4685,21 +4727,21 @@
         <v>38</v>
       </c>
       <c r="H83" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I83" s="20" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="10" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D84" s="3">
         <v>14</v>
@@ -4715,21 +4757,21 @@
         <v>38</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D85" s="3">
         <v>1</v>
@@ -4745,15 +4787,15 @@
         <v>38</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="86" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E86" s="58"/>
       <c r="F86" s="58"/>
@@ -4773,18 +4815,18 @@
       </c>
       <c r="E87" s="59"/>
       <c r="I87" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C88" s="9" t="s">
         <v>236</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>237</v>
       </c>
       <c r="D88" s="3">
         <v>1</v>
@@ -4799,13 +4841,13 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C89" s="9" t="s">
         <v>241</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>242</v>
       </c>
       <c r="D89" s="3">
         <v>2</v>
@@ -4833,19 +4875,19 @@
       </c>
       <c r="E90" s="59"/>
       <c r="I90" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="91" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C91" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="B91" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>538</v>
-      </c>
       <c r="D91" s="4">
         <v>1</v>
       </c>
@@ -4856,32 +4898,32 @@
         <v>1</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="92" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E92" s="58"/>
       <c r="F92" s="58"/>
     </row>
     <row r="93" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E93" s="58"/>
       <c r="F93" s="58"/>
     </row>
     <row r="94" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="B94" s="3" t="s">
-        <v>402</v>
-      </c>
       <c r="C94" s="53" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D94" s="3">
         <v>1</v>
@@ -4894,19 +4936,19 @@
         <v>200</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J94" s="4"/>
     </row>
     <row r="95" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D95" s="4">
         <v>5</v>
@@ -4919,18 +4961,18 @@
         <v>5</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D96" s="3">
         <v>1</v>
@@ -4943,18 +4985,18 @@
         <v>26</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C97" s="3" t="s">
         <v>408</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>409</v>
       </c>
       <c r="D97" s="3">
         <v>1</v>
@@ -4967,18 +5009,18 @@
         <v>37</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D98" s="3">
         <v>2</v>
@@ -4991,32 +5033,32 @@
         <v>48</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E99" s="67"/>
       <c r="F99" s="67"/>
     </row>
     <row r="100" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E100" s="67"/>
       <c r="F100" s="67"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B101" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>572</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>573</v>
       </c>
       <c r="D101" s="3">
         <v>1</v>
@@ -5032,25 +5074,25 @@
         <v>13</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A102" s="17" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E102" s="68"/>
       <c r="F102" s="68"/>
     </row>
     <row r="103" spans="1:9" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="21" t="s">
+        <v>474</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="C103" s="72" t="s">
         <v>475</v>
-      </c>
-      <c r="B103" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="C103" s="72" t="s">
-        <v>476</v>
       </c>
       <c r="D103" s="20">
         <v>1</v>
@@ -5066,18 +5108,18 @@
         <v>13</v>
       </c>
       <c r="I103" s="20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="22" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B104" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C104" s="73" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D104" s="3">
         <v>1</v>
@@ -5094,18 +5136,18 @@
       </c>
       <c r="H104" s="20"/>
       <c r="I104" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="22" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B105" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C105" s="73" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D105" s="3">
         <v>0</v>
@@ -5122,18 +5164,18 @@
       </c>
       <c r="H105" s="20"/>
       <c r="I105" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B106" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C106" s="73" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D106" s="3">
         <v>1</v>
@@ -5150,18 +5192,18 @@
       </c>
       <c r="H106" s="20"/>
       <c r="I106" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B107" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C107" s="73" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D107" s="3">
         <v>0</v>
@@ -5178,18 +5220,18 @@
       </c>
       <c r="H107" s="20"/>
       <c r="I107" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="B108" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C108" s="3" t="s">
         <v>486</v>
-      </c>
-      <c r="B108" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>487</v>
       </c>
       <c r="D108" s="3">
         <v>1</v>
@@ -5206,18 +5248,18 @@
       </c>
       <c r="H108" s="20"/>
       <c r="I108" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C109" s="28" t="s">
         <v>488</v>
-      </c>
-      <c r="B109" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C109" s="28" t="s">
-        <v>489</v>
       </c>
       <c r="D109" s="3">
         <v>1</v>
@@ -5234,25 +5276,25 @@
       </c>
       <c r="H109" s="20"/>
       <c r="I109" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A110" s="17" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E110" s="68"/>
       <c r="F110" s="68"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B111" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C111" s="54" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D111" s="3">
         <v>1</v>
@@ -5268,18 +5310,18 @@
         <v>13</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="B112" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="C112" s="4" t="s">
         <v>347</v>
-      </c>
-      <c r="B112" s="50" t="s">
-        <v>221</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>348</v>
       </c>
       <c r="D112" s="4">
         <v>1</v>
@@ -5295,18 +5337,18 @@
         <v>13</v>
       </c>
       <c r="I112" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B113" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="B113" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>350</v>
       </c>
       <c r="D113" s="3">
         <v>1</v>
@@ -5322,18 +5364,18 @@
         <v>13</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B114" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>352</v>
-      </c>
-      <c r="B114" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>353</v>
       </c>
       <c r="D114" s="3">
         <v>1</v>
@@ -5349,18 +5391,18 @@
         <v>13</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B115" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>338</v>
-      </c>
-      <c r="B115" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>339</v>
       </c>
       <c r="D115" s="3">
         <v>1</v>
@@ -5376,18 +5418,18 @@
         <v>13</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="116" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B116" s="50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D116" s="4">
         <v>1</v>
@@ -5403,7 +5445,7 @@
         <v>13</v>
       </c>
       <c r="I116" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5437,18 +5479,18 @@
         <v>49</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D119" s="3">
         <v>1</v>
@@ -5464,18 +5506,18 @@
         <v>49</v>
       </c>
       <c r="I119" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D120" s="3">
         <v>1</v>
@@ -5491,18 +5533,18 @@
         <v>49</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D121" s="3">
         <v>1</v>
@@ -5518,7 +5560,7 @@
         <v>49</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -5529,7 +5571,7 @@
         <v>48</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D122" s="3">
         <v>1</v>
@@ -5571,13 +5613,13 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D124" s="3">
         <v>1</v>
@@ -5595,13 +5637,13 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>285</v>
       </c>
       <c r="D125" s="3">
         <v>10</v>
@@ -5617,18 +5659,18 @@
         <v>49</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C126" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>287</v>
       </c>
       <c r="D126" s="3">
         <v>1</v>
@@ -5644,18 +5686,18 @@
         <v>49</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C127" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="D127" s="3">
         <v>4</v>
@@ -5673,13 +5715,13 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C128" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="D128" s="3">
         <v>10</v>
@@ -5697,13 +5739,13 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="D129" s="3">
         <v>10</v>
@@ -5721,13 +5763,13 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D130" s="3">
         <v>6</v>
@@ -5750,20 +5792,20 @@
     </row>
     <row r="134" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="7" t="s">
-        <v>110</v>
+        <v>577</v>
       </c>
       <c r="E134" s="58"/>
       <c r="F134" s="58"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B135" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B135" s="3" t="s">
+      <c r="C135" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="D135" s="3">
         <v>4</v>
@@ -5772,22 +5814,22 @@
         <v>16.5</v>
       </c>
       <c r="F135" s="57">
-        <f t="shared" ref="F135:F150" si="12">E135*D135</f>
+        <f t="shared" ref="F135:F159" si="12">E135*D135</f>
         <v>66</v>
       </c>
       <c r="I135" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C136" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="D136" s="3">
         <v>1</v>
@@ -5802,13 +5844,13 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C137" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C137" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="D137" s="3">
         <v>2</v>
@@ -5821,18 +5863,18 @@
         <v>64</v>
       </c>
       <c r="I137" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C138" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C138" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="D138" s="3">
         <v>2</v>
@@ -5847,13 +5889,13 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C139" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="D139" s="3">
         <v>1</v>
@@ -5866,18 +5908,18 @@
         <v>60</v>
       </c>
       <c r="I139" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C140" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="D140" s="3">
         <v>1</v>
@@ -5892,13 +5934,13 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D141" s="3">
         <v>1</v>
@@ -5913,13 +5955,13 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C142" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="D142" s="3">
         <v>1</v>
@@ -5934,13 +5976,13 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C143" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="D143" s="3">
         <v>1</v>
@@ -5955,13 +5997,13 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C144" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="D144" s="3">
         <v>1</v>
@@ -5974,15 +6016,15 @@
         <v>105.8</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C145" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="D145" s="3">
         <v>2</v>
@@ -5995,15 +6037,15 @@
         <v>239.2</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C146" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C146" s="3" t="s">
-        <v>294</v>
       </c>
       <c r="D146" s="3">
         <v>1</v>
@@ -6016,15 +6058,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C147" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="D147" s="3">
         <v>2</v>
@@ -6037,15 +6079,15 @@
         <v>184</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C148" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="D148" s="3">
         <v>1</v>
@@ -6058,15 +6100,15 @@
         <v>96.23</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C149" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="D149" s="3">
         <v>1</v>
@@ -6079,15 +6121,15 @@
         <v>102.44</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C150" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="B150" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="D150" s="3">
         <v>2</v>
@@ -6100,346 +6142,562 @@
         <v>56</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="C151" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="D151" s="3">
+        <v>1</v>
+      </c>
+      <c r="E151" s="57">
+        <v>490</v>
+      </c>
+      <c r="F151" s="57">
+        <f t="shared" si="12"/>
+        <v>490</v>
+      </c>
+      <c r="I151" s="3" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A152" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B152" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C152" s="29" t="s">
+        <v>579</v>
+      </c>
+      <c r="D152" s="29">
+        <v>1</v>
+      </c>
+      <c r="E152" s="44">
+        <v>77</v>
+      </c>
+      <c r="F152" s="44">
+        <f t="shared" si="12"/>
+        <v>77</v>
+      </c>
+      <c r="I152" s="29" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A153" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B153" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C153" s="29" t="s">
+        <v>581</v>
+      </c>
+      <c r="D153" s="29">
+        <v>1</v>
+      </c>
+      <c r="E153" s="44">
+        <v>20</v>
+      </c>
+      <c r="F153" s="44">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="I153" s="29" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A154" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B154" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C154" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D154" s="29">
+        <v>1</v>
+      </c>
+      <c r="E154" s="44">
+        <v>177</v>
+      </c>
+      <c r="F154" s="44">
+        <f t="shared" si="12"/>
+        <v>177</v>
+      </c>
+      <c r="I154" s="29" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="D155" s="3">
+        <v>2</v>
+      </c>
+      <c r="E155" s="57">
+        <v>13</v>
+      </c>
+      <c r="F155" s="57">
+        <f t="shared" si="12"/>
+        <v>26</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="D156" s="3">
+        <v>2</v>
+      </c>
+      <c r="E156" s="57">
+        <v>19</v>
+      </c>
+      <c r="F156" s="57">
+        <f t="shared" si="12"/>
+        <v>38</v>
+      </c>
+      <c r="I156" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="D157" s="3">
+        <v>1</v>
+      </c>
+      <c r="E157" s="57">
+        <v>12</v>
+      </c>
+      <c r="F157" s="57">
+        <f t="shared" si="12"/>
+        <v>12</v>
+      </c>
+      <c r="I157" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D158" s="3">
+        <v>2</v>
+      </c>
+      <c r="E158" s="57">
+        <v>35</v>
+      </c>
+      <c r="F158" s="57">
+        <f t="shared" si="12"/>
+        <v>70</v>
+      </c>
+      <c r="I158" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="D159" s="3">
+        <v>0</v>
+      </c>
+      <c r="E159" s="57">
+        <v>520</v>
+      </c>
+      <c r="F159" s="57">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I159" s="3" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C160" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D160" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C161" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D151" s="3">
+      <c r="D161" s="3">
+        <v>1</v>
+      </c>
+      <c r="I161" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C162" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D162" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A164" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B164" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="E164" s="58"/>
+      <c r="F164" s="58"/>
+    </row>
+    <row r="165" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="3"/>
+      <c r="B165" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="C165" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D165" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C152" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D152" s="3">
-        <v>1</v>
-      </c>
-      <c r="I152" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C153" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D153" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A155" s="7" t="s">
+      <c r="E165" s="57">
+        <v>40</v>
+      </c>
+      <c r="F165" s="57">
+        <f>E165*D165</f>
+        <v>160</v>
+      </c>
+      <c r="G165" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="H165" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="I165" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="J165" s="20"/>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B166" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B155" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="E155" s="58"/>
-      <c r="F155" s="58"/>
-    </row>
-    <row r="156" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="3"/>
-      <c r="B156" s="3" t="s">
+      <c r="C166" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D166" s="3">
+        <v>2</v>
+      </c>
+      <c r="E166" s="57">
+        <v>515</v>
+      </c>
+      <c r="F166" s="57">
+        <f>E166*D166</f>
+        <v>1030</v>
+      </c>
+      <c r="G166" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="C156" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="D156" s="3">
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B167" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D167" s="3">
         <v>4</v>
       </c>
-      <c r="E156" s="57">
-        <v>40</v>
-      </c>
-      <c r="F156" s="57">
-        <f>E156*D156</f>
-        <v>160</v>
-      </c>
-      <c r="G156" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="H156" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="I156" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="J156" s="20"/>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B157" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>557</v>
-      </c>
-      <c r="D157" s="3">
-        <v>2</v>
-      </c>
-      <c r="E157" s="57">
-        <v>515</v>
-      </c>
-      <c r="F157" s="57">
-        <f>E157*D157</f>
-        <v>1030</v>
-      </c>
-      <c r="G157" s="3" t="s">
+      <c r="E167" s="57">
+        <v>25</v>
+      </c>
+      <c r="F167" s="57">
+        <f>E167*D167</f>
+        <v>100</v>
+      </c>
+      <c r="G167" s="3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B168" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="D168" s="3">
+        <v>4</v>
+      </c>
+      <c r="E168" s="57">
+        <v>28</v>
+      </c>
+      <c r="F168" s="57">
+        <f>E168*D168</f>
+        <v>112</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B169" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D169" s="3">
+        <v>6</v>
+      </c>
+      <c r="E169" s="57">
+        <v>121.5</v>
+      </c>
+      <c r="F169" s="57">
+        <f>E169*D169</f>
+        <v>729</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E172" s="52" t="s">
+        <v>455</v>
+      </c>
+      <c r="F172" s="52">
+        <f>SUM(F3:F170)</f>
+        <v>97337.501499199992</v>
+      </c>
+      <c r="G172" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A176" s="51" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A177" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="B177" s="4" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B158" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="D158" s="3">
-        <v>4</v>
-      </c>
-      <c r="E158" s="57">
-        <v>25</v>
-      </c>
-      <c r="F158" s="57">
-        <f>E158*D158</f>
-        <v>100</v>
-      </c>
-      <c r="G158" s="3" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B159" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="D159" s="3">
-        <v>4</v>
-      </c>
-      <c r="E159" s="57">
-        <v>28</v>
-      </c>
-      <c r="F159" s="57">
-        <f>E159*D159</f>
-        <v>112</v>
-      </c>
-      <c r="G159" s="3" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B160" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="D160" s="3">
-        <v>6</v>
-      </c>
-      <c r="E160" s="57">
-        <v>121.5</v>
-      </c>
-      <c r="F160" s="57">
-        <f>E160*D160</f>
-        <v>729</v>
-      </c>
-      <c r="G160" s="3" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E163" s="52" t="s">
-        <v>456</v>
-      </c>
-      <c r="F163" s="52">
-        <f>SUM(F3:F161)</f>
-        <v>96427.501499199992</v>
-      </c>
-      <c r="G163" s="3" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A167" s="51" t="s">
+      <c r="C177" s="4" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B178" s="3">
+        <v>14</v>
+      </c>
+      <c r="C178" s="3" t="s">
         <v>441</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A168" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="B168" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="C168" s="4" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A169" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="B169" s="3">
-        <v>14</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A170" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="B170" s="3">
-        <v>2</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A171" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="B171" s="3">
-        <v>2</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A172" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="B172" s="3">
-        <v>2</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A175" s="51" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A176" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="B176" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="C176" s="4" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="B177" s="3">
-        <v>2</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A178" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="B178" s="3">
-        <v>5</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>347</v>
+        <v>432</v>
       </c>
       <c r="B179" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>537</v>
+        <v>435</v>
       </c>
       <c r="B180" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>539</v>
+        <v>442</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>540</v>
+        <v>436</v>
       </c>
       <c r="B181" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A183" s="51" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A184" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="B184" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="C184" s="4" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="B185" s="3">
-        <v>5</v>
-      </c>
-      <c r="C185" s="3" t="s">
-        <v>450</v>
+        <v>437</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A184" s="51" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A185" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="C185" s="4" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>158</v>
+        <v>444</v>
       </c>
       <c r="B186" s="3">
+        <v>2</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A187" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B187" s="3">
+        <v>5</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B188" s="3">
+        <v>1</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="B189" s="3">
+        <v>1</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="B190" s="3">
+        <v>1</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A192" s="51" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A193" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="B193" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="C193" s="4" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="B194" s="3">
+        <v>5</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B195" s="3">
         <v>3</v>
       </c>
-      <c r="C186" s="3" t="s">
+      <c r="C195" s="3" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="3" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" s="3" t="s">
+      <c r="B196" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C196" s="3" t="s">
         <v>454</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="C187" s="3" t="s">
-        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -6508,7 +6766,7 @@
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -6518,7 +6776,7 @@
         <v>1008062</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C3" s="29" t="s">
         <v>16</v>
@@ -6534,15 +6792,15 @@
         <v>7400</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D4" s="29">
         <v>1</v>
@@ -6555,15 +6813,15 @@
         <v>20000</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
+        <v>375</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>376</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>377</v>
       </c>
       <c r="D5" s="29">
         <v>1</v>
@@ -6575,23 +6833,23 @@
         <v>50000</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B8" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>168</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>169</v>
       </c>
       <c r="D8" s="29">
         <v>1</v>
@@ -6604,27 +6862,27 @@
         <v>25000</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:9" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D12" s="29">
         <v>1</v>
@@ -6640,21 +6898,21 @@
         <v>13</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D13" s="29">
         <v>1</v>
@@ -6670,21 +6928,21 @@
         <v>13</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D14" s="29">
         <v>1</v>
@@ -6700,21 +6958,21 @@
         <v>13</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D15" s="29">
         <v>1</v>
@@ -6730,21 +6988,21 @@
         <v>13</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I15" s="29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="C16" s="33" t="s">
         <v>239</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>238</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>240</v>
       </c>
       <c r="D16" s="30">
         <v>1</v>
@@ -6760,32 +7018,32 @@
         <v>13</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I16" s="30" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:10" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>14</v>
@@ -6810,13 +7068,13 @@
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
@@ -6838,13 +7096,13 @@
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
@@ -6865,13 +7123,13 @@
     </row>
     <row r="22" spans="1:10" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
@@ -6879,32 +7137,32 @@
       <c r="E22" s="42"/>
       <c r="F22" s="42"/>
       <c r="I22" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" s="38" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E25" s="39"/>
       <c r="F25" s="39"/>
     </row>
     <row r="26" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
+        <v>303</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="C26" s="33" t="s">
         <v>304</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>305</v>
       </c>
       <c r="D26" s="30">
         <v>2</v>
@@ -6920,21 +7178,21 @@
         <v>38</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I26" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D27" s="30">
         <v>2</v>
@@ -6950,21 +7208,21 @@
         <v>38</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I27" s="30" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B28" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="C28" s="33" t="s">
         <v>317</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>318</v>
       </c>
       <c r="D28" s="30">
         <v>8</v>
@@ -6980,21 +7238,21 @@
         <v>38</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I28" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B29" s="30" t="s">
         <v>59</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D29" s="30">
         <v>6</v>
@@ -7010,18 +7268,18 @@
         <v>38</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="C30" s="33" t="s">
         <v>322</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>323</v>
       </c>
       <c r="D30" s="30">
         <v>2</v>
@@ -7037,21 +7295,21 @@
         <v>38</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I30" s="30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D31" s="30">
         <v>1</v>
@@ -7067,21 +7325,21 @@
         <v>38</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I31" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D32" s="30">
         <v>1</v>
@@ -7097,21 +7355,21 @@
         <v>38</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I32" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="33" t="s">
         <v>217</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>218</v>
       </c>
       <c r="D33" s="30">
         <v>2</v>
@@ -7127,7 +7385,7 @@
         <v>38</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7161,7 +7419,7 @@
         <v>49</v>
       </c>
       <c r="I38" s="29" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -7663,19 +7921,19 @@
     </row>
     <row r="66" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F66" s="8"/>
     </row>
     <row r="67" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B67" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="B67" s="29" t="s">
+      <c r="C67" s="29" t="s">
         <v>116</v>
-      </c>
-      <c r="C67" s="29" t="s">
-        <v>117</v>
       </c>
       <c r="D67" s="29">
         <v>2</v>
@@ -7688,18 +7946,18 @@
         <v>280</v>
       </c>
       <c r="I67" s="29" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>362</v>
+      </c>
+      <c r="B68" s="29" t="s">
         <v>363</v>
       </c>
-      <c r="B68" s="29" t="s">
+      <c r="C68" s="29" t="s">
         <v>364</v>
-      </c>
-      <c r="C68" s="29" t="s">
-        <v>365</v>
       </c>
       <c r="D68" s="29">
         <v>2</v>
@@ -7712,18 +7970,18 @@
         <v>168</v>
       </c>
       <c r="I68" s="29" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B69" s="29" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C69" s="29" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D69" s="29">
         <v>1</v>
@@ -7736,18 +7994,18 @@
         <v>54</v>
       </c>
       <c r="I69" s="29" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F71" s="8"/>
     </row>
     <row r="72" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C72" s="30"/>
       <c r="E72" s="32"/>
@@ -7756,7 +8014,7 @@
     </row>
     <row r="73" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C73" s="30"/>
       <c r="E73" s="32"/>
@@ -7771,23 +8029,23 @@
     </row>
     <row r="75" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
     </row>
     <row r="76" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="B76" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C76" s="29" t="s">
         <v>379</v>
-      </c>
-      <c r="B76" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="C76" s="29" t="s">
-        <v>380</v>
       </c>
       <c r="D76" s="29">
         <v>1</v>
@@ -7800,18 +8058,18 @@
         <v>518.5</v>
       </c>
       <c r="I76" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="77" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="29" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B77" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C77" s="29" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D77" s="29">
         <v>1</v>
@@ -7826,13 +8084,13 @@
     </row>
     <row r="78" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="29" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B78" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C78" s="29" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D78" s="29">
         <v>1</v>
@@ -7845,18 +8103,18 @@
         <v>816</v>
       </c>
       <c r="I78" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="29" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B79" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C79" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D79" s="29">
         <v>1</v>
@@ -7871,13 +8129,13 @@
     </row>
     <row r="80" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="29" t="s">
+        <v>392</v>
+      </c>
+      <c r="B80" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C80" s="29" t="s">
         <v>393</v>
-      </c>
-      <c r="B80" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="C80" s="29" t="s">
-        <v>394</v>
       </c>
       <c r="D80" s="29">
         <v>1</v>
@@ -7892,13 +8150,13 @@
     </row>
     <row r="81" spans="1:6" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="29" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B81" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C81" s="29" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D81" s="29">
         <v>1</v>
@@ -7913,13 +8171,13 @@
     </row>
     <row r="82" spans="1:6" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="29" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B82" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C82" s="29" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D82" s="29">
         <v>1</v>
@@ -7934,13 +8192,13 @@
     </row>
     <row r="83" spans="1:6" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="29" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B83" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C83" s="29" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D83" s="29">
         <v>1</v>

</xml_diff>

<commit_message>
fix: 3D printing instructions for laser cover.
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D033BF81-6D37-44DE-8F17-462795583352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7669BD5-E95D-4C80-AB7D-555A9E5B1C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4932" yWindow="3468" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -863,9 +863,6 @@
     <t>±15 V Power Supply for BLINK &amp; QS, SS, SP, &amp; XG Series Galvo Scanners</t>
   </si>
   <si>
-    <t>Cage60mm-2sides-InnerD75mm-L75mm.stl</t>
-  </si>
-  <si>
     <r>
       <t>See folder</t>
     </r>
@@ -1598,9 +1595,6 @@
     <t>The 1:1 relay from ETL to galvo</t>
   </si>
   <si>
-    <t>See files files in folder /custom-parts/laser-safety/</t>
-  </si>
-  <si>
     <t>TR50/M</t>
   </si>
   <si>
@@ -1874,6 +1868,12 @@
   </si>
   <si>
     <t>TBS1000C</t>
+  </si>
+  <si>
+    <t>Cage60mm-2sides-InnerD75mm-L100mm.stl</t>
+  </si>
+  <si>
+    <t>When printing, the Z-dimension of the model must be rescaled by 75%, so it's height is 75 instead of 100mm. See the STL file in folder /custom-parts/laser-safety/Universal-cage60mm-L100mm</t>
   </si>
 </sst>
 </file>
@@ -2629,8 +2629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2650,7 +2650,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E1" s="71"/>
       <c r="F1" s="71"/>
@@ -2669,10 +2669,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -2759,7 +2759,7 @@
         <v>38</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2777,7 +2777,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D10" s="29">
         <v>0</v>
@@ -2852,13 +2852,13 @@
     </row>
     <row r="13" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D13" s="29">
         <v>1</v>
@@ -2874,7 +2874,7 @@
         <v>230</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2963,13 +2963,13 @@
     </row>
     <row r="17" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D17" s="29">
         <v>0</v>
@@ -2985,7 +2985,7 @@
         <v>230</v>
       </c>
       <c r="I17" s="29" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -3044,13 +3044,13 @@
     </row>
     <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -3063,7 +3063,7 @@
         <v>19965</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -3128,13 +3128,13 @@
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -3147,7 +3147,7 @@
         <v>6900</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3156,13 +3156,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>458</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>459</v>
       </c>
       <c r="D26" s="3">
         <v>4</v>
@@ -3178,7 +3178,7 @@
         <v>230</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3356,20 +3356,20 @@
     </row>
     <row r="35" spans="1:9" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E35" s="61"/>
       <c r="F35" s="61"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C36" s="3" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D36" s="3">
         <v>1</v>
       </c>
       <c r="E36" s="57" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F36" s="57">
         <v>0</v>
@@ -3384,13 +3384,13 @@
     </row>
     <row r="38" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="77" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B38" s="41" t="s">
         <v>59</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D38" s="41">
         <v>1</v>
@@ -3403,21 +3403,21 @@
         <v>728</v>
       </c>
       <c r="G38" s="41" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="I38" s="41" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="77" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B39" s="41" t="s">
         <v>59</v>
       </c>
       <c r="C39" s="41" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D39" s="41">
         <v>1</v>
@@ -3429,10 +3429,10 @@
         <v>33</v>
       </c>
       <c r="G39" s="41" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="I39" s="41" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3462,7 +3462,7 @@
         <v>192</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3492,7 +3492,7 @@
         <v>192</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3522,18 +3522,18 @@
         <v>192</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D43" s="3">
         <v>2</v>
@@ -3552,18 +3552,18 @@
         <v>192</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D44" s="3">
         <v>2</v>
@@ -3582,7 +3582,7 @@
         <v>192</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3593,7 +3593,7 @@
         <v>59</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D45" s="3">
         <v>2</v>
@@ -3612,18 +3612,18 @@
         <v>192</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D46" s="3">
         <v>2</v>
@@ -3638,7 +3638,7 @@
         <v>38</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3646,10 +3646,10 @@
         <v>37</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D47" s="3">
         <v>2</v>
@@ -3673,7 +3673,7 @@
         <v>40</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>41</v>
@@ -3695,12 +3695,12 @@
         <v>39</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>183</v>
@@ -3732,7 +3732,7 @@
         <v>42</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>43</v>
@@ -3756,7 +3756,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>59</v>
@@ -3778,7 +3778,7 @@
         <v>38</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3805,10 +3805,10 @@
         <v>38</v>
       </c>
       <c r="H52" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="I52" s="3" t="s">
         <v>497</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -3835,7 +3835,7 @@
         <v>38</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -3865,7 +3865,7 @@
         <v>195</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3895,7 +3895,7 @@
         <v>195</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -3925,7 +3925,7 @@
         <v>214</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -3936,7 +3936,7 @@
         <v>59</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D57" s="3">
         <v>4</v>
@@ -3952,10 +3952,10 @@
         <v>38</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -3982,21 +3982,21 @@
         <v>38</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D59" s="3">
         <v>2</v>
@@ -4015,18 +4015,18 @@
         <v>218</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D60" s="3">
         <v>4</v>
@@ -4045,18 +4045,18 @@
         <v>218</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D61" s="3">
         <v>4</v>
@@ -4075,7 +4075,7 @@
         <v>218</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4083,7 +4083,7 @@
         <v>91863</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>46</v>
@@ -4105,18 +4105,18 @@
         <v>198</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C63" s="50" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D63" s="4">
         <v>2</v>
@@ -4135,18 +4135,18 @@
         <v>218</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="46" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B64" s="45" t="s">
         <v>59</v>
       </c>
       <c r="C64" s="46" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D64" s="45">
         <v>0</v>
@@ -4165,13 +4165,13 @@
         <v>218</v>
       </c>
       <c r="I64" s="45" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="J64" s="75"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>59</v>
@@ -4196,12 +4196,12 @@
         <v>218</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
-        <v>276</v>
+        <v>590</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>220</v>
@@ -4226,18 +4226,18 @@
         <v>218</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>503</v>
+        <v>591</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D67" s="3">
         <v>4</v>
@@ -4253,7 +4253,7 @@
         <v>38</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I67" s="3" t="s">
         <v>204</v>
@@ -4310,7 +4310,7 @@
         <v>38</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I69" s="3" t="s">
         <v>204</v>
@@ -4318,13 +4318,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D70" s="3">
         <v>2</v>
@@ -4370,12 +4370,12 @@
         <v>218</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="23" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>59</v>
@@ -4400,18 +4400,18 @@
         <v>213</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="80" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="48" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C73" s="48" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D73" s="80">
         <v>2</v>
@@ -4430,7 +4430,7 @@
         <v>213</v>
       </c>
       <c r="I73" s="80" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -4465,13 +4465,13 @@
     </row>
     <row r="75" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D75" s="4">
         <v>2</v>
@@ -4490,18 +4490,18 @@
         <v>215</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="46" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B76" s="45" t="s">
         <v>59</v>
       </c>
       <c r="C76" s="46" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D76" s="45">
         <v>0</v>
@@ -4520,18 +4520,18 @@
         <v>215</v>
       </c>
       <c r="I76" s="45" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D77" s="3">
         <v>2</v>
@@ -4550,18 +4550,18 @@
         <v>215</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D78" s="3">
         <v>2</v>
@@ -4580,7 +4580,7 @@
         <v>215</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -4610,7 +4610,7 @@
         <v>215</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -4640,18 +4640,18 @@
         <v>215</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="27" t="s">
+        <v>437</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>438</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>439</v>
       </c>
       <c r="D81" s="3">
         <v>1</v>
@@ -4670,12 +4670,12 @@
         <v>215</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="82" spans="1:10" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B82" s="45" t="s">
         <v>59</v>
@@ -4700,18 +4700,18 @@
         <v>215</v>
       </c>
       <c r="I82" s="45" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="27" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B83" s="20" t="s">
         <v>59</v>
       </c>
       <c r="C83" s="27" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D83" s="20">
         <v>2</v>
@@ -4730,18 +4730,18 @@
         <v>215</v>
       </c>
       <c r="I83" s="20" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="10" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D84" s="3">
         <v>14</v>
@@ -4760,18 +4760,18 @@
         <v>215</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>264</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D85" s="3">
         <v>1</v>
@@ -4790,7 +4790,7 @@
         <v>215</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="86" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4880,13 +4880,13 @@
     </row>
     <row r="91" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>220</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D91" s="4">
         <v>1</v>
@@ -4898,32 +4898,32 @@
         <v>1</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="92" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E92" s="58"/>
       <c r="F92" s="58"/>
     </row>
     <row r="93" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E93" s="58"/>
       <c r="F93" s="58"/>
     </row>
     <row r="94" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="B94" s="3" t="s">
-        <v>401</v>
-      </c>
       <c r="C94" s="53" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D94" s="3">
         <v>1</v>
@@ -4936,19 +4936,19 @@
         <v>200</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J94" s="4"/>
     </row>
     <row r="95" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D95" s="4">
         <v>5</v>
@@ -4961,18 +4961,18 @@
         <v>5</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D96" s="3">
         <v>1</v>
@@ -4985,18 +4985,18 @@
         <v>26</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C97" s="3" t="s">
         <v>407</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>408</v>
       </c>
       <c r="D97" s="3">
         <v>1</v>
@@ -5009,18 +5009,18 @@
         <v>37</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D98" s="3">
         <v>2</v>
@@ -5033,7 +5033,7 @@
         <v>48</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -5045,20 +5045,20 @@
     </row>
     <row r="100" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="E100" s="67"/>
       <c r="F100" s="67"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D101" s="3">
         <v>1</v>
@@ -5079,20 +5079,20 @@
     </row>
     <row r="102" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A102" s="17" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E102" s="68"/>
       <c r="F102" s="68"/>
     </row>
     <row r="103" spans="1:9" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="21" t="s">
+        <v>473</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="C103" s="72" t="s">
         <v>474</v>
-      </c>
-      <c r="B103" s="20" t="s">
-        <v>314</v>
-      </c>
-      <c r="C103" s="72" t="s">
-        <v>475</v>
       </c>
       <c r="D103" s="20">
         <v>1</v>
@@ -5108,18 +5108,18 @@
         <v>13</v>
       </c>
       <c r="I103" s="20" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="22" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B104" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C104" s="73" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D104" s="3">
         <v>1</v>
@@ -5136,18 +5136,18 @@
       </c>
       <c r="H104" s="20"/>
       <c r="I104" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="22" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B105" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C105" s="73" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D105" s="3">
         <v>0</v>
@@ -5164,18 +5164,18 @@
       </c>
       <c r="H105" s="20"/>
       <c r="I105" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B106" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C106" s="73" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D106" s="3">
         <v>1</v>
@@ -5192,18 +5192,18 @@
       </c>
       <c r="H106" s="20"/>
       <c r="I106" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B107" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C107" s="73" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D107" s="3">
         <v>0</v>
@@ -5220,18 +5220,18 @@
       </c>
       <c r="H107" s="20"/>
       <c r="I107" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="B108" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C108" s="3" t="s">
         <v>485</v>
-      </c>
-      <c r="B108" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>486</v>
       </c>
       <c r="D108" s="3">
         <v>1</v>
@@ -5248,18 +5248,18 @@
       </c>
       <c r="H108" s="20"/>
       <c r="I108" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C109" s="28" t="s">
         <v>487</v>
-      </c>
-      <c r="B109" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C109" s="28" t="s">
-        <v>488</v>
       </c>
       <c r="D109" s="3">
         <v>1</v>
@@ -5276,25 +5276,25 @@
       </c>
       <c r="H109" s="20"/>
       <c r="I109" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A110" s="17" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E110" s="68"/>
       <c r="F110" s="68"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B111" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C111" s="54" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D111" s="3">
         <v>1</v>
@@ -5310,18 +5310,18 @@
         <v>13</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B112" s="50" t="s">
         <v>220</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D112" s="4">
         <v>1</v>
@@ -5337,18 +5337,18 @@
         <v>13</v>
       </c>
       <c r="I112" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B113" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>348</v>
-      </c>
-      <c r="B113" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>349</v>
       </c>
       <c r="D113" s="3">
         <v>1</v>
@@ -5364,18 +5364,18 @@
         <v>13</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B114" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="B114" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>352</v>
       </c>
       <c r="D114" s="3">
         <v>1</v>
@@ -5391,18 +5391,18 @@
         <v>13</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B115" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>337</v>
-      </c>
-      <c r="B115" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>338</v>
       </c>
       <c r="D115" s="3">
         <v>1</v>
@@ -5418,18 +5418,18 @@
         <v>13</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="116" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B116" s="50" t="s">
         <v>220</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D116" s="4">
         <v>1</v>
@@ -5445,7 +5445,7 @@
         <v>13</v>
       </c>
       <c r="I116" s="4" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5479,7 +5479,7 @@
         <v>49</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -5506,7 +5506,7 @@
         <v>49</v>
       </c>
       <c r="I119" s="3" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -5517,7 +5517,7 @@
         <v>48</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D120" s="3">
         <v>1</v>
@@ -5533,7 +5533,7 @@
         <v>49</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -5637,13 +5637,13 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>283</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>284</v>
       </c>
       <c r="D125" s="3">
         <v>10</v>
@@ -5659,18 +5659,18 @@
         <v>49</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C126" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>286</v>
       </c>
       <c r="D126" s="3">
         <v>1</v>
@@ -5686,7 +5686,7 @@
         <v>49</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -5792,7 +5792,7 @@
     </row>
     <row r="134" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="7" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E134" s="58"/>
       <c r="F134" s="58"/>
@@ -6039,13 +6039,13 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C146" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C146" s="3" t="s">
-        <v>293</v>
       </c>
       <c r="D146" s="3">
         <v>1</v>
@@ -6150,7 +6150,7 @@
         <v>59</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D151" s="3">
         <v>1</v>
@@ -6163,7 +6163,7 @@
         <v>490</v>
       </c>
       <c r="I151" s="3" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="152" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6174,7 +6174,7 @@
         <v>59</v>
       </c>
       <c r="C152" s="29" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D152" s="29">
         <v>1</v>
@@ -6187,7 +6187,7 @@
         <v>77</v>
       </c>
       <c r="I152" s="29" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="153" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6198,7 +6198,7 @@
         <v>59</v>
       </c>
       <c r="C153" s="29" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D153" s="29">
         <v>1</v>
@@ -6211,7 +6211,7 @@
         <v>20</v>
       </c>
       <c r="I153" s="29" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="154" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6235,7 +6235,7 @@
         <v>177</v>
       </c>
       <c r="I154" s="29" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -6246,7 +6246,7 @@
         <v>59</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D155" s="3">
         <v>2</v>
@@ -6259,7 +6259,7 @@
         <v>26</v>
       </c>
       <c r="I155" s="3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -6270,7 +6270,7 @@
         <v>59</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="D156" s="3">
         <v>2</v>
@@ -6283,18 +6283,18 @@
         <v>38</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D157" s="3">
         <v>1</v>
@@ -6307,7 +6307,7 @@
         <v>12</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -6331,18 +6331,18 @@
         <v>70</v>
       </c>
       <c r="I158" s="3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D159" s="3">
         <v>0</v>
@@ -6355,7 +6355,7 @@
         <v>0</v>
       </c>
       <c r="I159" s="3" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -6390,7 +6390,7 @@
         <v>158</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E164" s="58"/>
       <c r="F164" s="58"/>
@@ -6398,7 +6398,7 @@
     <row r="165" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
       <c r="B165" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C165" s="20" t="s">
         <v>157</v>
@@ -6414,13 +6414,13 @@
         <v>160</v>
       </c>
       <c r="G165" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="H165" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="H165" s="3" t="s">
-        <v>426</v>
-      </c>
       <c r="I165" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J165" s="20"/>
     </row>
@@ -6429,7 +6429,7 @@
         <v>159</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D166" s="3">
         <v>2</v>
@@ -6442,7 +6442,7 @@
         <v>1030</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
@@ -6450,7 +6450,7 @@
         <v>159</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D167" s="3">
         <v>4</v>
@@ -6463,7 +6463,7 @@
         <v>100</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
@@ -6471,7 +6471,7 @@
         <v>159</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D168" s="3">
         <v>4</v>
@@ -6484,7 +6484,7 @@
         <v>112</v>
       </c>
       <c r="G168" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
@@ -6492,7 +6492,7 @@
         <v>159</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D169" s="3">
         <v>6</v>
@@ -6505,177 +6505,177 @@
         <v>729</v>
       </c>
       <c r="G169" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="172" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E172" s="52" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F172" s="52">
         <f>SUM(F3:F170)</f>
         <v>97337.501499199992</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="176" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A176" s="51" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A177" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B178" s="3">
         <v>14</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B179" s="3">
         <v>2</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B180" s="3">
         <v>2</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B181" s="3">
         <v>2</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A184" s="51" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A185" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B186" s="3">
         <v>2</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A187" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B187" s="3">
         <v>5</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B188" s="3">
         <v>1</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="B189" s="3">
+        <v>1</v>
+      </c>
+      <c r="C189" s="3" t="s">
         <v>536</v>
-      </c>
-      <c r="B189" s="3">
-        <v>1</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B190" s="3">
         <v>1</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A192" s="51" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A193" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B194" s="3">
         <v>5</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -6686,18 +6686,18 @@
         <v>3</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C196" s="3" t="s">
         <v>453</v>
-      </c>
-      <c r="B196" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C196" s="3" t="s">
-        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -6792,7 +6792,7 @@
         <v>7400</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6813,15 +6813,15 @@
         <v>20000</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
+        <v>374</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>375</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>376</v>
       </c>
       <c r="D5" s="29">
         <v>1</v>
@@ -6833,13 +6833,13 @@
         <v>50000</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -6862,27 +6862,27 @@
         <v>25000</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:9" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D12" s="29">
         <v>1</v>
@@ -6898,21 +6898,21 @@
         <v>13</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D13" s="29">
         <v>1</v>
@@ -6928,21 +6928,21 @@
         <v>13</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D14" s="29">
         <v>1</v>
@@ -6958,21 +6958,21 @@
         <v>13</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D15" s="29">
         <v>1</v>
@@ -6988,10 +6988,10 @@
         <v>13</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I15" s="29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -7018,22 +7018,22 @@
         <v>13</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I16" s="30" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -7123,7 +7123,7 @@
     </row>
     <row r="22" spans="1:10" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>220</v>
@@ -7137,32 +7137,32 @@
       <c r="E22" s="42"/>
       <c r="F22" s="42"/>
       <c r="I22" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" s="38" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E25" s="39"/>
       <c r="F25" s="39"/>
     </row>
     <row r="26" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B26" s="30" t="s">
         <v>220</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D26" s="30">
         <v>2</v>
@@ -7178,21 +7178,21 @@
         <v>38</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I26" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>264</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D27" s="30">
         <v>2</v>
@@ -7208,21 +7208,21 @@
         <v>38</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I27" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B28" s="30" t="s">
+        <v>315</v>
+      </c>
+      <c r="C28" s="33" t="s">
         <v>316</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>317</v>
       </c>
       <c r="D28" s="30">
         <v>8</v>
@@ -7238,21 +7238,21 @@
         <v>38</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I28" s="30" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B29" s="30" t="s">
         <v>59</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D29" s="30">
         <v>6</v>
@@ -7268,18 +7268,18 @@
         <v>38</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B30" s="30" t="s">
         <v>220</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D30" s="30">
         <v>2</v>
@@ -7295,21 +7295,21 @@
         <v>38</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I30" s="30" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B31" s="30" t="s">
         <v>264</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D31" s="30">
         <v>1</v>
@@ -7325,21 +7325,21 @@
         <v>38</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I31" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B32" s="30" t="s">
         <v>264</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D32" s="30">
         <v>1</v>
@@ -7355,10 +7355,10 @@
         <v>38</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I32" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -7385,7 +7385,7 @@
         <v>38</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7419,7 +7419,7 @@
         <v>49</v>
       </c>
       <c r="I38" s="29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -7921,7 +7921,7 @@
     </row>
     <row r="66" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F66" s="8"/>
     </row>
@@ -7946,18 +7946,18 @@
         <v>280</v>
       </c>
       <c r="I67" s="29" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>361</v>
+      </c>
+      <c r="B68" s="29" t="s">
         <v>362</v>
       </c>
-      <c r="B68" s="29" t="s">
+      <c r="C68" s="29" t="s">
         <v>363</v>
-      </c>
-      <c r="C68" s="29" t="s">
-        <v>364</v>
       </c>
       <c r="D68" s="29">
         <v>2</v>
@@ -7970,18 +7970,18 @@
         <v>168</v>
       </c>
       <c r="I68" s="29" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B69" s="29" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C69" s="29" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D69" s="29">
         <v>1</v>
@@ -7994,18 +7994,18 @@
         <v>54</v>
       </c>
       <c r="I69" s="29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F71" s="8"/>
     </row>
     <row r="72" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C72" s="30"/>
       <c r="E72" s="32"/>
@@ -8014,7 +8014,7 @@
     </row>
     <row r="73" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C73" s="30"/>
       <c r="E73" s="32"/>
@@ -8032,20 +8032,20 @@
         <v>158</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
     </row>
     <row r="76" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="29" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B76" s="29" t="s">
         <v>159</v>
       </c>
       <c r="C76" s="29" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D76" s="29">
         <v>1</v>
@@ -8063,13 +8063,13 @@
     </row>
     <row r="77" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="29" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B77" s="29" t="s">
         <v>159</v>
       </c>
       <c r="C77" s="29" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D77" s="29">
         <v>1</v>
@@ -8084,13 +8084,13 @@
     </row>
     <row r="78" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="29" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B78" s="29" t="s">
         <v>159</v>
       </c>
       <c r="C78" s="29" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D78" s="29">
         <v>1</v>
@@ -8108,13 +8108,13 @@
     </row>
     <row r="79" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B79" s="29" t="s">
         <v>159</v>
       </c>
       <c r="C79" s="29" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D79" s="29">
         <v>1</v>
@@ -8129,13 +8129,13 @@
     </row>
     <row r="80" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="29" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B80" s="29" t="s">
         <v>159</v>
       </c>
       <c r="C80" s="29" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D80" s="29">
         <v>1</v>
@@ -8150,13 +8150,13 @@
     </row>
     <row r="81" spans="1:6" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="29" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B81" s="29" t="s">
         <v>159</v>
       </c>
       <c r="C81" s="29" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D81" s="29">
         <v>1</v>
@@ -8171,13 +8171,13 @@
     </row>
     <row r="82" spans="1:6" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="29" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B82" s="29" t="s">
         <v>159</v>
       </c>
       <c r="C82" s="29" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D82" s="29">
         <v>1</v>
@@ -8192,13 +8192,13 @@
     </row>
     <row r="83" spans="1:6" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="29" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B83" s="29" t="s">
         <v>159</v>
       </c>
       <c r="C83" s="29" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D83" s="29">
         <v>1</v>

</xml_diff>

<commit_message>
update PCIe slot specs
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8808DB6E-A603-4103-9C17-1CE3AF0C6108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8A3E6C-A54F-47F4-B3DD-4F33E71A98E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2952" yWindow="4152" windowWidth="37116" windowHeight="20412" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5040" yWindow="900" windowWidth="39372" windowHeight="21276" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1787,8 +1787,83 @@
     <t>SM2NFMA or (discontinued) SM2NFM</t>
   </si>
   <si>
+    <t>Imaging Workstation with a large screen</t>
+  </si>
+  <si>
+    <t>Filters have to be selected according to lasers &amp; needs (flurescent markers and dyes used). The single quadband is a MINIMALIST choice</t>
+  </si>
+  <si>
+    <t>Chroma (distributors: AHF in Germany, or europe@chroma.com in the rest of EU)</t>
+  </si>
+  <si>
+    <t>QuadLine Emission ZET405/488/561/640m, in 25 mm diameter</t>
+  </si>
+  <si>
+    <t>Ø45.0 mm Sorbothane Feet, Internal M6 Mounting Thread, 4 Pieces</t>
+  </si>
+  <si>
+    <t>AV4/M</t>
+  </si>
+  <si>
+    <t>Attached to the bottom of the PBG52522 Breadboard. Based on Benchtop weight 25 kg on breadboard (including BB).</t>
+  </si>
+  <si>
+    <t>All stage parts above offered by ASI (Jon Daniels &lt;jon@asiimaging.com&gt;)</t>
+  </si>
+  <si>
+    <t>General lab and optics supplies</t>
+  </si>
+  <si>
+    <t>Shearing Interferometer with a 10-25.4 mm Beam Diameter Shear Plate</t>
+  </si>
+  <si>
+    <t>30 mm Cage System Adapter for Shearing Interferometers with Diffuser Viewing Screen</t>
+  </si>
+  <si>
+    <t>accessory</t>
+  </si>
+  <si>
+    <t>SM1 (1.035"-40) Coupler, External Threads, 0.5" Long, Two Locking Rings</t>
+  </si>
+  <si>
+    <t>Interferometer for beam collimation</t>
+  </si>
+  <si>
+    <t>30 mm Cage Alignment Plate with Ø0.9 mm Hole</t>
+  </si>
+  <si>
+    <t>60 mm Cage Alignment Plate with Ø1 mm Hole</t>
+  </si>
+  <si>
+    <t>Beam alignment</t>
+  </si>
+  <si>
+    <t>60 mm Cage Fluorescent Alignment Plate, Ø1 mm Hole, Orange</t>
+  </si>
+  <si>
+    <t>LCPA2</t>
+  </si>
+  <si>
+    <t>Basic 2-ch oscilloscope for signal troubleshooting</t>
+  </si>
+  <si>
+    <t>Tektronix</t>
+  </si>
+  <si>
+    <t>2 Channel Digital Storage Oscilloscope</t>
+  </si>
+  <si>
+    <t>TBS1000C</t>
+  </si>
+  <si>
+    <t>Cage60mm-2sides-InnerD75mm-L100mm.stl</t>
+  </si>
+  <si>
+    <t>When printing, the Z-dimension of the model must be rescaled by 75%, so it's height is 75 instead of 100mm. See the STL file in folder /custom-parts/laser-safety/Universal-cage60mm-L100mm</t>
+  </si>
+  <si>
     <r>
-      <t>Recommendations: at least 64 GB RAM, 2 TB SSD drive, 2 PCIex8 slots.</t>
+      <t>Recommendations: at least 64 GB RAM, 2 TB SSD drive, one PCIe x1 (or higher) and one PCIe x4 (or higher) slot.</t>
     </r>
     <r>
       <rPr>
@@ -1799,81 +1874,6 @@
       </rPr>
       <t xml:space="preserve"> Ideally: 256 GB RAM and 8 TB SSD drive.</t>
     </r>
-  </si>
-  <si>
-    <t>Imaging Workstation with a large screen</t>
-  </si>
-  <si>
-    <t>Filters have to be selected according to lasers &amp; needs (flurescent markers and dyes used). The single quadband is a MINIMALIST choice</t>
-  </si>
-  <si>
-    <t>Chroma (distributors: AHF in Germany, or europe@chroma.com in the rest of EU)</t>
-  </si>
-  <si>
-    <t>QuadLine Emission ZET405/488/561/640m, in 25 mm diameter</t>
-  </si>
-  <si>
-    <t>Ø45.0 mm Sorbothane Feet, Internal M6 Mounting Thread, 4 Pieces</t>
-  </si>
-  <si>
-    <t>AV4/M</t>
-  </si>
-  <si>
-    <t>Attached to the bottom of the PBG52522 Breadboard. Based on Benchtop weight 25 kg on breadboard (including BB).</t>
-  </si>
-  <si>
-    <t>All stage parts above offered by ASI (Jon Daniels &lt;jon@asiimaging.com&gt;)</t>
-  </si>
-  <si>
-    <t>General lab and optics supplies</t>
-  </si>
-  <si>
-    <t>Shearing Interferometer with a 10-25.4 mm Beam Diameter Shear Plate</t>
-  </si>
-  <si>
-    <t>30 mm Cage System Adapter for Shearing Interferometers with Diffuser Viewing Screen</t>
-  </si>
-  <si>
-    <t>accessory</t>
-  </si>
-  <si>
-    <t>SM1 (1.035"-40) Coupler, External Threads, 0.5" Long, Two Locking Rings</t>
-  </si>
-  <si>
-    <t>Interferometer for beam collimation</t>
-  </si>
-  <si>
-    <t>30 mm Cage Alignment Plate with Ø0.9 mm Hole</t>
-  </si>
-  <si>
-    <t>60 mm Cage Alignment Plate with Ø1 mm Hole</t>
-  </si>
-  <si>
-    <t>Beam alignment</t>
-  </si>
-  <si>
-    <t>60 mm Cage Fluorescent Alignment Plate, Ø1 mm Hole, Orange</t>
-  </si>
-  <si>
-    <t>LCPA2</t>
-  </si>
-  <si>
-    <t>Basic 2-ch oscilloscope for signal troubleshooting</t>
-  </si>
-  <si>
-    <t>Tektronix</t>
-  </si>
-  <si>
-    <t>2 Channel Digital Storage Oscilloscope</t>
-  </si>
-  <si>
-    <t>TBS1000C</t>
-  </si>
-  <si>
-    <t>Cage60mm-2sides-InnerD75mm-L100mm.stl</t>
-  </si>
-  <si>
-    <t>When printing, the Z-dimension of the model must be rescaled by 75%, so it's height is 75 instead of 100mm. See the STL file in folder /custom-parts/laser-safety/Universal-cage60mm-L100mm</t>
   </si>
 </sst>
 </file>
@@ -2629,8 +2629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3050,7 +3050,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -3356,14 +3356,14 @@
     </row>
     <row r="35" spans="1:9" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>566</v>
+        <v>591</v>
       </c>
       <c r="E35" s="61"/>
       <c r="F35" s="61"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C36" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D36" s="3">
         <v>1</v>
@@ -3411,13 +3411,13 @@
     </row>
     <row r="39" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="77" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B39" s="41" t="s">
         <v>59</v>
       </c>
       <c r="C39" s="41" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D39" s="41">
         <v>1</v>
@@ -3432,7 +3432,7 @@
         <v>517</v>
       </c>
       <c r="I39" s="41" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -4201,7 +4201,7 @@
     </row>
     <row r="66" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>220</v>
@@ -4226,7 +4226,7 @@
         <v>218</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -5045,7 +5045,7 @@
     </row>
     <row r="100" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E100" s="67"/>
       <c r="F100" s="67"/>
@@ -5055,10 +5055,10 @@
         <v>339</v>
       </c>
       <c r="B101" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>569</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>570</v>
       </c>
       <c r="D101" s="3">
         <v>1</v>
@@ -5792,7 +5792,7 @@
     </row>
     <row r="134" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="7" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E134" s="58"/>
       <c r="F134" s="58"/>
@@ -6150,7 +6150,7 @@
         <v>59</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D151" s="3">
         <v>1</v>
@@ -6163,7 +6163,7 @@
         <v>490</v>
       </c>
       <c r="I151" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="152" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6174,7 +6174,7 @@
         <v>59</v>
       </c>
       <c r="C152" s="29" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D152" s="29">
         <v>1</v>
@@ -6187,7 +6187,7 @@
         <v>77</v>
       </c>
       <c r="I152" s="29" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="153" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6198,7 +6198,7 @@
         <v>59</v>
       </c>
       <c r="C153" s="29" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D153" s="29">
         <v>1</v>
@@ -6211,7 +6211,7 @@
         <v>20</v>
       </c>
       <c r="I153" s="29" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="154" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6235,7 +6235,7 @@
         <v>177</v>
       </c>
       <c r="I154" s="29" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -6246,7 +6246,7 @@
         <v>59</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D155" s="3">
         <v>2</v>
@@ -6259,7 +6259,7 @@
         <v>26</v>
       </c>
       <c r="I155" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -6270,7 +6270,7 @@
         <v>59</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D156" s="3">
         <v>2</v>
@@ -6283,18 +6283,18 @@
         <v>38</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D157" s="3">
         <v>1</v>
@@ -6307,7 +6307,7 @@
         <v>12</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -6331,18 +6331,18 @@
         <v>70</v>
       </c>
       <c r="I158" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B159" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="C159" s="3" t="s">
         <v>587</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>588</v>
       </c>
       <c r="D159" s="3">
         <v>0</v>
@@ -6355,7 +6355,7 @@
         <v>0</v>
       </c>
       <c r="I159" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed Thorlabs BNC cable part number and PCIe-8363 card number
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736574BC-0572-4E73-8987-7C73CADA934F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FAFCEC-3D29-49F6-88A0-711E7C6CFF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11112" yWindow="3528" windowWidth="32304" windowHeight="21276" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11472" yWindow="6768" windowWidth="31464" windowHeight="16752" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="588">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -540,9 +540,6 @@
   </si>
   <si>
     <t>Power Cord, 220V, 10A (plug country-specific)</t>
-  </si>
-  <si>
-    <t>779504-01</t>
   </si>
   <si>
     <t>781163-01</t>
@@ -1856,6 +1853,15 @@
   </si>
   <si>
     <t>Includes switching module between 2 laser ports, controlled by TTL signal. The 405nm is NOT included! A four-laser version is ~35k.</t>
+  </si>
+  <si>
+    <t>HW-KIT6</t>
+  </si>
+  <si>
+    <t>2249-C-12</t>
+  </si>
+  <si>
+    <t>788814-01</t>
   </si>
 </sst>
 </file>
@@ -2618,8 +2624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J195"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J109" sqref="J109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2639,7 +2645,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E1" s="70"/>
       <c r="F1" s="70"/>
@@ -2658,10 +2664,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="55" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F2" s="55" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -2701,10 +2707,10 @@
         <v>15000</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2748,7 +2754,7 @@
         <v>38</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2766,7 +2772,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D10" s="29">
         <v>0</v>
@@ -2779,10 +2785,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2806,10 +2812,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2833,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H12" s="29" t="s">
         <v>13</v>
@@ -2841,13 +2847,13 @@
     </row>
     <row r="13" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D13" s="29">
         <v>1</v>
@@ -2860,10 +2866,10 @@
         <v>160</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2887,13 +2893,13 @@
         <v>0</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H14" s="29" t="s">
         <v>13</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2917,10 +2923,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I15" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2944,21 +2950,21 @@
         <v>0</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I16" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D17" s="29">
         <v>0</v>
@@ -2971,10 +2977,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I17" s="29" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -2998,10 +3004,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="I18" s="29" t="s">
         <v>224</v>
-      </c>
-      <c r="I18" s="29" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -3025,21 +3031,21 @@
         <v>0</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -3052,7 +3058,7 @@
         <v>19965</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -3082,10 +3088,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -3109,21 +3115,21 @@
         <v>0</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -3136,7 +3142,7 @@
         <v>6900</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3145,13 +3151,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>447</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>448</v>
       </c>
       <c r="D26" s="3">
         <v>4</v>
@@ -3164,28 +3170,28 @@
         <v>108</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>237</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>238</v>
       </c>
       <c r="D28" s="3">
         <v>2</v>
@@ -3198,21 +3204,21 @@
         <v>140</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="D29" s="3">
         <v>6</v>
@@ -3225,21 +3231,21 @@
         <v>216</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -3252,21 +3258,21 @@
         <v>43</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>248</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
@@ -3279,21 +3285,21 @@
         <v>29</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="C32" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
@@ -3306,21 +3312,21 @@
         <v>195</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D33" s="3">
         <v>1</v>
@@ -3333,7 +3339,7 @@
         <v>10</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="12" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3345,20 +3351,20 @@
     </row>
     <row r="35" spans="1:9" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E35" s="60"/>
       <c r="F35" s="60"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C36" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D36" s="3">
         <v>1</v>
       </c>
       <c r="E36" s="56" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F36" s="56">
         <v>0</v>
@@ -3366,20 +3372,20 @@
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E37" s="57"/>
       <c r="F37" s="57"/>
     </row>
     <row r="38" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="76" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B38" s="41" t="s">
         <v>58</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D38" s="41">
         <v>1</v>
@@ -3392,21 +3398,21 @@
         <v>728</v>
       </c>
       <c r="G38" s="41" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I38" s="41" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="76" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B39" s="41" t="s">
         <v>58</v>
       </c>
       <c r="C39" s="41" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D39" s="41">
         <v>1</v>
@@ -3418,10 +3424,10 @@
         <v>33</v>
       </c>
       <c r="G39" s="41" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I39" s="41" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3432,7 +3438,7 @@
         <v>58</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D40" s="3">
         <v>2</v>
@@ -3448,21 +3454,21 @@
         <v>38</v>
       </c>
       <c r="H40" s="78" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>184</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>185</v>
       </c>
       <c r="D41" s="3">
         <v>2</v>
@@ -3478,10 +3484,10 @@
         <v>38</v>
       </c>
       <c r="H41" s="78" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3508,21 +3514,21 @@
         <v>38</v>
       </c>
       <c r="H42" s="78" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>533</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>534</v>
       </c>
       <c r="D43" s="3">
         <v>2</v>
@@ -3538,21 +3544,21 @@
         <v>38</v>
       </c>
       <c r="H43" s="78" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>535</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>536</v>
       </c>
       <c r="D44" s="3">
         <v>2</v>
@@ -3568,21 +3574,21 @@
         <v>38</v>
       </c>
       <c r="H44" s="78" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D45" s="3">
         <v>2</v>
@@ -3598,21 +3604,21 @@
         <v>38</v>
       </c>
       <c r="H45" s="78" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D46" s="3">
         <v>2</v>
@@ -3627,7 +3633,7 @@
         <v>38</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3635,10 +3641,10 @@
         <v>37</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D47" s="3">
         <v>2</v>
@@ -3662,7 +3668,7 @@
         <v>40</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>41</v>
@@ -3684,18 +3690,18 @@
         <v>39</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D49" s="3">
         <v>1</v>
@@ -3722,7 +3728,7 @@
         <v>42</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>43</v>
@@ -3746,13 +3752,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D51" s="3">
         <v>2</v>
@@ -3768,7 +3774,7 @@
         <v>38</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3795,21 +3801,21 @@
         <v>38</v>
       </c>
       <c r="H52" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="I52" s="3" t="s">
         <v>485</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>194</v>
       </c>
       <c r="D53" s="3">
         <v>2</v>
@@ -3825,18 +3831,18 @@
         <v>38</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>187</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>188</v>
       </c>
       <c r="D54" s="3">
         <v>4</v>
@@ -3852,21 +3858,21 @@
         <v>38</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>190</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>191</v>
       </c>
       <c r="D55" s="3">
         <v>4</v>
@@ -3882,21 +3888,21 @@
         <v>38</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>181</v>
       </c>
       <c r="D56" s="3">
         <v>8</v>
@@ -3912,10 +3918,10 @@
         <v>38</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -3926,7 +3932,7 @@
         <v>58</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D57" s="3">
         <v>4</v>
@@ -3942,21 +3948,21 @@
         <v>38</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D58" s="3">
         <v>2</v>
@@ -3972,21 +3978,21 @@
         <v>38</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
+        <v>496</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>497</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>498</v>
       </c>
       <c r="D59" s="3">
         <v>2</v>
@@ -4002,21 +4008,21 @@
         <v>38</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>499</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>500</v>
       </c>
       <c r="D60" s="3">
         <v>4</v>
@@ -4032,21 +4038,21 @@
         <v>38</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D61" s="3">
         <v>4</v>
@@ -4062,10 +4068,10 @@
         <v>38</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4073,7 +4079,7 @@
         <v>91863</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>45</v>
@@ -4092,21 +4098,21 @@
         <v>38</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C63" s="49" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D63" s="4">
         <v>2</v>
@@ -4122,21 +4128,21 @@
         <v>38</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="46" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B64" s="45" t="s">
         <v>58</v>
       </c>
       <c r="C64" s="46" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D64" s="45">
         <v>0</v>
@@ -4152,22 +4158,22 @@
         <v>38</v>
       </c>
       <c r="H64" s="45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I64" s="45" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J64" s="74"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D65" s="3">
         <v>2</v>
@@ -4183,21 +4189,21 @@
         <v>38</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C66" s="73" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D66" s="4">
         <v>2</v>
@@ -4213,21 +4219,21 @@
         <v>38</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D67" s="3">
         <v>4</v>
@@ -4243,21 +4249,21 @@
         <v>38</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>201</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>202</v>
       </c>
       <c r="D68" s="3">
         <v>2</v>
@@ -4273,18 +4279,18 @@
         <v>38</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>199</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>200</v>
       </c>
       <c r="D69" s="3">
         <v>4</v>
@@ -4300,21 +4306,21 @@
         <v>38</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>491</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>492</v>
       </c>
       <c r="D70" s="3">
         <v>2</v>
@@ -4330,18 +4336,18 @@
         <v>38</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>196</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>197</v>
       </c>
       <c r="D71" s="3">
         <v>2</v>
@@ -4357,21 +4363,21 @@
         <v>38</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="23" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D72" s="24">
         <v>2</v>
@@ -4387,21 +4393,21 @@
         <v>38</v>
       </c>
       <c r="H72" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="79" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="47" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C73" s="47" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D73" s="79">
         <v>2</v>
@@ -4417,21 +4423,21 @@
         <v>38</v>
       </c>
       <c r="H73" s="79" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I73" s="79" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C74" s="23" t="s">
         <v>204</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C74" s="23" t="s">
-        <v>205</v>
       </c>
       <c r="D74" s="24">
         <v>2</v>
@@ -4447,21 +4453,21 @@
         <v>38</v>
       </c>
       <c r="H74" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I74" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D75" s="4">
         <v>2</v>
@@ -4477,21 +4483,21 @@
         <v>38</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="46" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B76" s="45" t="s">
         <v>58</v>
       </c>
       <c r="C76" s="46" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D76" s="45">
         <v>0</v>
@@ -4507,21 +4513,21 @@
         <v>38</v>
       </c>
       <c r="H76" s="45" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I76" s="45" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>514</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>515</v>
       </c>
       <c r="D77" s="3">
         <v>2</v>
@@ -4537,21 +4543,21 @@
         <v>38</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C78" s="82" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D78" s="3">
         <v>2</v>
@@ -4567,21 +4573,21 @@
         <v>38</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>265</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>266</v>
       </c>
       <c r="D79" s="3">
         <v>2</v>
@@ -4597,21 +4603,21 @@
         <v>38</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>267</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>268</v>
       </c>
       <c r="D80" s="3">
         <v>2</v>
@@ -4627,21 +4633,21 @@
         <v>38</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="27" t="s">
+        <v>426</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>427</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>428</v>
       </c>
       <c r="D81" s="3">
         <v>1</v>
@@ -4657,21 +4663,21 @@
         <v>38</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="82" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="27" t="s">
+        <v>527</v>
+      </c>
+      <c r="B82" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C82" s="27" t="s">
         <v>528</v>
-      </c>
-      <c r="B82" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C82" s="27" t="s">
-        <v>529</v>
       </c>
       <c r="D82" s="20">
         <v>2</v>
@@ -4687,21 +4693,21 @@
         <v>38</v>
       </c>
       <c r="H82" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I82" s="20" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="10" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D83" s="3">
         <v>14</v>
@@ -4717,21 +4723,21 @@
         <v>38</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D84" s="3">
         <v>1</v>
@@ -4747,15 +4753,15 @@
         <v>38</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="85" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E85" s="57"/>
       <c r="F85" s="57"/>
@@ -4775,18 +4781,18 @@
       </c>
       <c r="E86" s="58"/>
       <c r="I86" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C87" s="9" t="s">
         <v>229</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C87" s="9" t="s">
-        <v>230</v>
       </c>
       <c r="D87" s="3">
         <v>1</v>
@@ -4801,13 +4807,13 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C88" s="9" t="s">
         <v>234</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>235</v>
       </c>
       <c r="D88" s="3">
         <v>2</v>
@@ -4835,19 +4841,19 @@
       </c>
       <c r="E89" s="58"/>
       <c r="I89" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="90" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C90" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="B90" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>524</v>
-      </c>
       <c r="D90" s="4">
         <v>1</v>
       </c>
@@ -4858,32 +4864,32 @@
         <v>1</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="91" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E91" s="57"/>
       <c r="F91" s="57"/>
     </row>
     <row r="92" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E92" s="57"/>
       <c r="F92" s="57"/>
     </row>
     <row r="93" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="B93" s="3" t="s">
-        <v>390</v>
-      </c>
       <c r="C93" s="52" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D93" s="3">
         <v>1</v>
@@ -4896,19 +4902,19 @@
         <v>200</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J93" s="4"/>
     </row>
     <row r="94" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D94" s="4">
         <v>5</v>
@@ -4921,18 +4927,18 @@
         <v>5</v>
       </c>
       <c r="I94" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D95" s="3">
         <v>1</v>
@@ -4945,18 +4951,18 @@
         <v>26</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C96" s="3" t="s">
         <v>396</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>397</v>
       </c>
       <c r="D96" s="3">
         <v>1</v>
@@ -4969,18 +4975,18 @@
         <v>37</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D97" s="3">
         <v>2</v>
@@ -4993,7 +4999,7 @@
         <v>48</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="98" spans="1:9" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -5005,20 +5011,20 @@
     </row>
     <row r="99" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E99" s="66"/>
       <c r="F99" s="66"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B100" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>557</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>558</v>
       </c>
       <c r="D100" s="3">
         <v>1</v>
@@ -5039,20 +5045,20 @@
     </row>
     <row r="101" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A101" s="17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E101" s="67"/>
       <c r="F101" s="67"/>
     </row>
     <row r="102" spans="1:9" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="21" t="s">
+        <v>461</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="C102" s="71" t="s">
         <v>462</v>
-      </c>
-      <c r="B102" s="20" t="s">
-        <v>304</v>
-      </c>
-      <c r="C102" s="71" t="s">
-        <v>463</v>
       </c>
       <c r="D102" s="20">
         <v>1</v>
@@ -5068,18 +5074,18 @@
         <v>13</v>
       </c>
       <c r="I102" s="20" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="22" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B103" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C103" s="72" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D103" s="3">
         <v>1</v>
@@ -5096,18 +5102,18 @@
       </c>
       <c r="H103" s="20"/>
       <c r="I103" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="22" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B104" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C104" s="72" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D104" s="3">
         <v>0</v>
@@ -5124,18 +5130,18 @@
       </c>
       <c r="H104" s="20"/>
       <c r="I104" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B105" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C105" s="72" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D105" s="3">
         <v>1</v>
@@ -5152,18 +5158,18 @@
       </c>
       <c r="H105" s="20"/>
       <c r="I105" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B106" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C106" s="72" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D106" s="3">
         <v>0</v>
@@ -5180,18 +5186,18 @@
       </c>
       <c r="H106" s="20"/>
       <c r="I106" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="B107" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>473</v>
-      </c>
-      <c r="B107" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>474</v>
       </c>
       <c r="D107" s="3">
         <v>1</v>
@@ -5208,18 +5214,18 @@
       </c>
       <c r="H107" s="20"/>
       <c r="I107" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B108" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C108" s="28" t="s">
         <v>475</v>
-      </c>
-      <c r="B108" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C108" s="28" t="s">
-        <v>476</v>
       </c>
       <c r="D108" s="3">
         <v>1</v>
@@ -5236,25 +5242,25 @@
       </c>
       <c r="H108" s="20"/>
       <c r="I108" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A109" s="17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E109" s="67"/>
       <c r="F109" s="67"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B110" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C110" s="53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D110" s="3">
         <v>1</v>
@@ -5270,18 +5276,18 @@
         <v>13</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="111" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B111" s="49" t="s">
+        <v>213</v>
+      </c>
+      <c r="C111" s="4" t="s">
         <v>336</v>
-      </c>
-      <c r="B111" s="49" t="s">
-        <v>214</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>337</v>
       </c>
       <c r="D111" s="4">
         <v>1</v>
@@ -5297,18 +5303,18 @@
         <v>13</v>
       </c>
       <c r="I111" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B112" s="20" t="s">
         <v>58</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D112" s="3">
         <v>1</v>
@@ -5324,18 +5330,18 @@
         <v>13</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B113" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="B113" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>341</v>
       </c>
       <c r="D113" s="3">
         <v>1</v>
@@ -5351,18 +5357,18 @@
         <v>13</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B114" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="B114" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>328</v>
       </c>
       <c r="D114" s="3">
         <v>1</v>
@@ -5378,18 +5384,18 @@
         <v>13</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B115" s="49" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D115" s="4">
         <v>1</v>
@@ -5405,7 +5411,7 @@
         <v>13</v>
       </c>
       <c r="I115" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="116" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5439,18 +5445,18 @@
         <v>48</v>
       </c>
       <c r="I117" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D118" s="3">
         <v>1</v>
@@ -5466,18 +5472,18 @@
         <v>48</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>169</v>
+        <v>587</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D119" s="3">
         <v>1</v>
@@ -5493,18 +5499,18 @@
         <v>48</v>
       </c>
       <c r="I119" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D120" s="3">
         <v>1</v>
@@ -5520,7 +5526,7 @@
         <v>48</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -5573,13 +5579,13 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D123" s="3">
         <v>1</v>
@@ -5597,13 +5603,13 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C124" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>276</v>
       </c>
       <c r="D124" s="3">
         <v>10</v>
@@ -5619,18 +5625,18 @@
         <v>48</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="D125" s="3">
         <v>1</v>
@@ -5646,12 +5652,12 @@
         <v>48</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>114</v>
+        <v>586</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>58</v>
@@ -5752,20 +5758,20 @@
     </row>
     <row r="133" spans="1:9" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="7" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E133" s="57"/>
       <c r="F133" s="57"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D134" s="3">
         <v>2</v>
@@ -5870,7 +5876,7 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>129</v>
+        <v>585</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>58</v>
@@ -5996,13 +6002,13 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C145" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>285</v>
       </c>
       <c r="D145" s="3">
         <v>1</v>
@@ -6107,7 +6113,7 @@
         <v>58</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D150" s="3">
         <v>1</v>
@@ -6120,7 +6126,7 @@
         <v>490</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="151" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6131,7 +6137,7 @@
         <v>58</v>
       </c>
       <c r="C151" s="29" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D151" s="29">
         <v>1</v>
@@ -6144,7 +6150,7 @@
         <v>77</v>
       </c>
       <c r="I151" s="29" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="152" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6155,7 +6161,7 @@
         <v>58</v>
       </c>
       <c r="C152" s="29" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D152" s="29">
         <v>1</v>
@@ -6168,7 +6174,7 @@
         <v>20</v>
       </c>
       <c r="I152" s="29" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="153" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6192,7 +6198,7 @@
         <v>177</v>
       </c>
       <c r="I153" s="29" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -6203,7 +6209,7 @@
         <v>58</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D154" s="3">
         <v>2</v>
@@ -6216,7 +6222,7 @@
         <v>26</v>
       </c>
       <c r="I154" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -6227,7 +6233,7 @@
         <v>58</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D155" s="3">
         <v>2</v>
@@ -6240,18 +6246,18 @@
         <v>38</v>
       </c>
       <c r="I155" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D156" s="3">
         <v>1</v>
@@ -6264,7 +6270,7 @@
         <v>12</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -6288,18 +6294,18 @@
         <v>70</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B158" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="C158" s="3" t="s">
         <v>574</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>575</v>
       </c>
       <c r="D158" s="3">
         <v>0</v>
@@ -6312,7 +6318,7 @@
         <v>0</v>
       </c>
       <c r="I158" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -6347,7 +6353,7 @@
         <v>153</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E163" s="57"/>
       <c r="F163" s="57"/>
@@ -6355,7 +6361,7 @@
     <row r="164" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
       <c r="B164" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C164" s="20" t="s">
         <v>152</v>
@@ -6371,13 +6377,13 @@
         <v>160</v>
       </c>
       <c r="G164" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="H164" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="H164" s="3" t="s">
-        <v>415</v>
-      </c>
       <c r="I164" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J164" s="20"/>
     </row>
@@ -6386,7 +6392,7 @@
         <v>154</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D165" s="3">
         <v>2</v>
@@ -6399,7 +6405,7 @@
         <v>1030</v>
       </c>
       <c r="G165" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
@@ -6407,7 +6413,7 @@
         <v>154</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D166" s="3">
         <v>4</v>
@@ -6420,7 +6426,7 @@
         <v>100</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
@@ -6428,7 +6434,7 @@
         <v>154</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D167" s="3">
         <v>4</v>
@@ -6441,7 +6447,7 @@
         <v>112</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
@@ -6449,7 +6455,7 @@
         <v>154</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D168" s="3">
         <v>6</v>
@@ -6462,177 +6468,177 @@
         <v>729</v>
       </c>
       <c r="G168" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="171" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E171" s="51" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F171" s="51">
         <f>SUM(F3:F169)</f>
         <v>102749.50149919999</v>
       </c>
       <c r="G171" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="175" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A175" s="50" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="176" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B177" s="3">
         <v>14</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B178" s="3">
         <v>2</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B179" s="3">
         <v>2</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B180" s="3">
         <v>2</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A183" s="50" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A184" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B185" s="3">
         <v>2</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A186" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B186" s="3">
         <v>5</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B187" s="3">
         <v>1</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B188" s="3">
         <v>1</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="B189" s="3">
+        <v>1</v>
+      </c>
+      <c r="C189" s="3" t="s">
         <v>526</v>
-      </c>
-      <c r="B189" s="3">
-        <v>1</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A191" s="50" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A192" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B193" s="3">
         <v>5</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -6643,18 +6649,18 @@
         <v>3</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C195" s="3" t="s">
         <v>442</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -6749,7 +6755,7 @@
         <v>7400</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -6770,15 +6776,15 @@
         <v>20000</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
+        <v>363</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>364</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>365</v>
       </c>
       <c r="D5" s="29">
         <v>1</v>
@@ -6790,13 +6796,13 @@
         <v>50000</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -6819,27 +6825,27 @@
         <v>25000</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:9" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D12" s="29">
         <v>1</v>
@@ -6855,21 +6861,21 @@
         <v>13</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D13" s="29">
         <v>1</v>
@@ -6885,21 +6891,21 @@
         <v>13</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>58</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D14" s="29">
         <v>1</v>
@@ -6915,21 +6921,21 @@
         <v>13</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D15" s="29">
         <v>1</v>
@@ -6945,21 +6951,21 @@
         <v>13</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I15" s="29" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
+        <v>231</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="C16" s="33" t="s">
         <v>232</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>231</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>233</v>
       </c>
       <c r="D16" s="30">
         <v>1</v>
@@ -6975,32 +6981,32 @@
         <v>13</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I16" s="30" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:10" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>14</v>
@@ -7025,13 +7031,13 @@
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
@@ -7053,13 +7059,13 @@
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
@@ -7080,13 +7086,13 @@
     </row>
     <row r="22" spans="1:10" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
@@ -7094,32 +7100,32 @@
       <c r="E22" s="42"/>
       <c r="F22" s="42"/>
       <c r="I22" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" s="38" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E25" s="39"/>
       <c r="F25" s="39"/>
     </row>
     <row r="26" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="C26" s="33" t="s">
         <v>293</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>214</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>294</v>
       </c>
       <c r="D26" s="30">
         <v>2</v>
@@ -7135,21 +7141,21 @@
         <v>38</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I26" s="30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D27" s="30">
         <v>2</v>
@@ -7165,21 +7171,21 @@
         <v>38</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I27" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B28" s="30" t="s">
+        <v>305</v>
+      </c>
+      <c r="C28" s="33" t="s">
         <v>306</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>307</v>
       </c>
       <c r="D28" s="30">
         <v>8</v>
@@ -7195,21 +7201,21 @@
         <v>38</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I28" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B29" s="30" t="s">
         <v>58</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D29" s="30">
         <v>6</v>
@@ -7225,18 +7231,18 @@
         <v>38</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="C30" s="33" t="s">
         <v>311</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>214</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>312</v>
       </c>
       <c r="D30" s="30">
         <v>2</v>
@@ -7252,21 +7258,21 @@
         <v>38</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I30" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D31" s="30">
         <v>1</v>
@@ -7282,21 +7288,21 @@
         <v>38</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I31" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D32" s="30">
         <v>1</v>
@@ -7312,21 +7318,21 @@
         <v>38</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I32" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="30" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="33" t="s">
         <v>210</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>211</v>
       </c>
       <c r="D33" s="30">
         <v>2</v>
@@ -7342,7 +7348,7 @@
         <v>38</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7376,7 +7382,7 @@
         <v>48</v>
       </c>
       <c r="I38" s="29" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -7878,7 +7884,7 @@
     </row>
     <row r="66" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F66" s="8"/>
     </row>
@@ -7903,18 +7909,18 @@
         <v>280</v>
       </c>
       <c r="I67" s="29" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>350</v>
+      </c>
+      <c r="B68" s="29" t="s">
         <v>351</v>
       </c>
-      <c r="B68" s="29" t="s">
+      <c r="C68" s="29" t="s">
         <v>352</v>
-      </c>
-      <c r="C68" s="29" t="s">
-        <v>353</v>
       </c>
       <c r="D68" s="29">
         <v>2</v>
@@ -7927,18 +7933,18 @@
         <v>168</v>
       </c>
       <c r="I68" s="29" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B69" s="29" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C69" s="29" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D69" s="29">
         <v>1</v>
@@ -7951,18 +7957,18 @@
         <v>54</v>
       </c>
       <c r="I69" s="29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F71" s="8"/>
     </row>
     <row r="72" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C72" s="30"/>
       <c r="E72" s="32"/>
@@ -7971,7 +7977,7 @@
     </row>
     <row r="73" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C73" s="30"/>
       <c r="E73" s="32"/>
@@ -7989,20 +7995,20 @@
         <v>153</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
     </row>
     <row r="76" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="29" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B76" s="29" t="s">
         <v>154</v>
       </c>
       <c r="C76" s="29" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D76" s="29">
         <v>1</v>
@@ -8020,13 +8026,13 @@
     </row>
     <row r="77" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B77" s="29" t="s">
         <v>154</v>
       </c>
       <c r="C77" s="29" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D77" s="29">
         <v>1</v>
@@ -8041,13 +8047,13 @@
     </row>
     <row r="78" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B78" s="29" t="s">
         <v>154</v>
       </c>
       <c r="C78" s="29" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D78" s="29">
         <v>1</v>
@@ -8065,13 +8071,13 @@
     </row>
     <row r="79" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="29" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B79" s="29" t="s">
         <v>154</v>
       </c>
       <c r="C79" s="29" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D79" s="29">
         <v>1</v>
@@ -8086,13 +8092,13 @@
     </row>
     <row r="80" spans="1:10" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="29" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B80" s="29" t="s">
         <v>154</v>
       </c>
       <c r="C80" s="29" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D80" s="29">
         <v>1</v>
@@ -8107,13 +8113,13 @@
     </row>
     <row r="81" spans="1:6" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="29" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B81" s="29" t="s">
         <v>154</v>
       </c>
       <c r="C81" s="29" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D81" s="29">
         <v>1</v>
@@ -8128,13 +8134,13 @@
     </row>
     <row r="82" spans="1:6" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="29" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B82" s="29" t="s">
         <v>154</v>
       </c>
       <c r="C82" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D82" s="29">
         <v>1</v>
@@ -8149,13 +8155,13 @@
     </row>
     <row r="83" spans="1:6" s="29" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="29" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B83" s="29" t="s">
         <v>154</v>
       </c>
       <c r="C83" s="29" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D83" s="29">
         <v>1</v>

</xml_diff>

<commit_message>
add TR200/M posts for excitation alignment
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FAFCEC-3D29-49F6-88A0-711E7C6CFF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B51EAB-9437-478E-B075-B612F30AD8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11472" yWindow="6768" windowWidth="31464" windowHeight="16752" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6888" yWindow="3360" windowWidth="34560" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="591">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -1862,6 +1862,15 @@
   </si>
   <si>
     <t>788814-01</t>
+  </si>
+  <si>
+    <t>TR200/M</t>
+  </si>
+  <si>
+    <t>Ø12.7 mm Optical Post, SS, M4 Setscrew, M6 Tap, L = 200 mm</t>
+  </si>
+  <si>
+    <t>Excitation cage alignment jig, see details at https://github.com/mesoSPIM/benchtop-hardware/wiki/Excitation_alignment</t>
   </si>
 </sst>
 </file>
@@ -2622,10 +2631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J195"/>
+  <dimension ref="A1:J196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J109" sqref="J109"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A158" sqref="A158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5780,7 +5789,7 @@
         <v>25</v>
       </c>
       <c r="F134" s="56">
-        <f t="shared" ref="F134:F158" si="12">E134*D134</f>
+        <f t="shared" ref="F134:F159" si="12">E134*D134</f>
         <v>50</v>
       </c>
     </row>
@@ -6299,131 +6308,134 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>575</v>
+        <v>588</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>573</v>
+        <v>58</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>574</v>
+        <v>589</v>
       </c>
       <c r="D158" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E158" s="56">
-        <v>520</v>
+        <v>9</v>
       </c>
       <c r="F158" s="56">
         <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+      <c r="I158" s="3" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="D159" s="3">
         <v>0</v>
       </c>
-      <c r="I158" s="3" t="s">
+      <c r="E159" s="56">
+        <v>520</v>
+      </c>
+      <c r="F159" s="56">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I159" s="3" t="s">
         <v>582</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C159" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D159" s="3">
-        <v>4</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C160" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D160" s="3">
-        <v>1</v>
-      </c>
-      <c r="I160" s="3" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C161" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D161" s="3">
+        <v>1</v>
+      </c>
+      <c r="I161" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C162" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D161" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A163" s="7" t="s">
+      <c r="D162" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A164" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B163" s="6" t="s">
+      <c r="B164" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="E163" s="57"/>
-      <c r="F163" s="57"/>
-    </row>
-    <row r="164" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="3"/>
-      <c r="B164" s="3" t="s">
+      <c r="E164" s="57"/>
+      <c r="F164" s="57"/>
+    </row>
+    <row r="165" spans="1:10" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="3"/>
+      <c r="B165" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="C164" s="20" t="s">
+      <c r="C165" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="D164" s="3">
+      <c r="D165" s="3">
         <v>4</v>
       </c>
-      <c r="E164" s="56">
+      <c r="E165" s="56">
         <v>40</v>
-      </c>
-      <c r="F164" s="56">
-        <f>E164*D164</f>
-        <v>160</v>
-      </c>
-      <c r="G164" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="H164" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="I164" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="J164" s="20"/>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B165" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>542</v>
-      </c>
-      <c r="D165" s="3">
-        <v>2</v>
-      </c>
-      <c r="E165" s="56">
-        <v>515</v>
       </c>
       <c r="F165" s="56">
         <f>E165*D165</f>
-        <v>1030</v>
+        <v>160</v>
       </c>
       <c r="G165" s="3" t="s">
-        <v>416</v>
-      </c>
+        <v>413</v>
+      </c>
+      <c r="H165" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I165" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="J165" s="20"/>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B166" s="3" t="s">
         <v>154</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>270</v>
+        <v>542</v>
       </c>
       <c r="D166" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E166" s="56">
-        <v>25</v>
+        <v>515</v>
       </c>
       <c r="F166" s="56">
         <f>E166*D166</f>
-        <v>100</v>
+        <v>1030</v>
       </c>
       <c r="G166" s="3" t="s">
         <v>416</v>
@@ -6434,17 +6446,17 @@
         <v>154</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D167" s="3">
         <v>4</v>
       </c>
       <c r="E167" s="56">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F167" s="56">
         <f>E167*D167</f>
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G167" s="3" t="s">
         <v>416</v>
@@ -6455,211 +6467,232 @@
         <v>154</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D168" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E168" s="56">
-        <v>121.5</v>
+        <v>28</v>
       </c>
       <c r="F168" s="56">
         <f>E168*D168</f>
-        <v>729</v>
+        <v>112</v>
       </c>
       <c r="G168" s="3" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="171" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E171" s="51" t="s">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B169" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D169" s="3">
+        <v>6</v>
+      </c>
+      <c r="E169" s="56">
+        <v>121.5</v>
+      </c>
+      <c r="F169" s="56">
+        <f>E169*D169</f>
+        <v>729</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E172" s="51" t="s">
         <v>443</v>
       </c>
-      <c r="F171" s="51">
-        <f>SUM(F3:F169)</f>
-        <v>102749.50149919999</v>
-      </c>
-      <c r="G171" s="3" t="s">
+      <c r="F172" s="51">
+        <f>SUM(F3:F170)</f>
+        <v>102767.50149919999</v>
+      </c>
+      <c r="G172" s="3" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A175" s="50" t="s">
+    <row r="176" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A176" s="50" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="176" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A176" s="4" t="s">
+    <row r="177" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A177" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B177" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="C176" s="4" t="s">
+      <c r="C177" s="4" t="s">
         <v>419</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="B177" s="3">
-        <v>14</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B178" s="3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1